<commit_message>
Updated some level completion achievements to use Lum and cage data so they trigger in level and don't rely on a level ID
</commit_message>
<xml_diff>
--- a/Rayman 2.xlsx
+++ b/Rayman 2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Areas" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1215" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1330" uniqueCount="84">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -172,6 +172,12 @@
     <t xml:space="preserve">Bayou</t>
   </si>
   <si>
+    <t xml:space="preserve">788764</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BayouArea2</t>
+  </si>
+  <si>
     <t xml:space="preserve">Index</t>
   </si>
   <si>
@@ -235,16 +241,25 @@
     <t xml:space="preserve">0x224994</t>
   </si>
   <si>
-    <t xml:space="preserve">0x224a36</t>
+    <t xml:space="preserve">0x224995</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x224996</t>
   </si>
   <si>
     <t xml:space="preserve">0x224997</t>
   </si>
   <si>
-    <t xml:space="preserve">0x224996</t>
+    <t xml:space="preserve">0x224998</t>
   </si>
   <si>
-    <t xml:space="preserve">0x224998</t>
+    <t xml:space="preserve">0x224999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x22499a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x224a36</t>
   </si>
   <si>
     <t xml:space="preserve">Level ID</t>
@@ -257,6 +272,9 @@
   </si>
   <si>
     <t xml:space="preserve">0x2249f2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x2249f3</t>
   </si>
 </sst>
 </file>
@@ -375,12 +393,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -462,20 +480,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G1015"/>
+  <dimension ref="A1:H1015"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="bottomLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.76953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.02"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -497,6 +516,10 @@
       <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="H1" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT(E2:E1000)</f>
+        <v>0x784BFC: { "id": 0x784BFC, "areaName": "Menu", "displayName": "Main Menu", "levelName": "Menu" },0x789668: { "id": 0x789668, "areaName": "Intro", "displayName": "somewhere in the Glade of Dreams…", "levelName": "None" },0x778C74: { "id": 0x778C74, "areaName": "BuccaneerBrig", "displayName": "in the Buccaneer’s brig", "levelName": "None" },0x78D424: { "id": 0x78D424, "areaName": "WoodsOfLight", "displayName": "in the Woods of Light", "levelName": "Woods of Light" },0x790570: { "id": 0x790570, "areaName": "HallOfDoors", "displayName": "in the Hall of Doors", "levelName": "Hall of Doors" },0x7875A8: { "id": 0x7875A8, "areaName": "FairyGladeArea1", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x78A320: { "id": 0x78A320, "areaName": "FairyGladeArea2", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x7A1BD8: { "id": 0x7A1BD8, "areaName": "FairyGladeArea3", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x77BFFC: { "id": 0x77BFFC, "areaName": "FairyGladeArea4", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x771B74: { "id": 0x771B74, "areaName": "FairyGladeArea5", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x74AAA8: { "id": 0x74AAA8, "areaName": "Results", "displayName": "viewing level results…", "levelName": "None" },0x788708: { "id": 0x788708, "areaName": "MarshesArea1", "displayName": "in the Marshes of Awakening", "levelName": "Marshes of Awakening" },0x7786E8: { "id": 0x7786E8, "areaName": "MarshesArea2", "displayName": "in the Marshes of Awakening", "levelName": "Marshes of Awakening" },0x790598: { "id": 0x790598, "areaName": "BayouArea1", "displayName": "in the Bayou", "levelName": "Bayou" },0x788764: { "id": 0x788764, "areaName": "BayouArea2", "displayName": "in the Bayou", "levelName": "Bayou" },</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
@@ -515,10 +538,6 @@
         <f aca="false">_xlfn.CONCAT("0x", A2,": { ""id"": ","0x", A2,", ""areaName"": """,B2,""", ""displayName"": """,C2,""", ""levelName"": """,D2,""" },")</f>
         <v>0x784BFC: { "id": 0x784BFC, "areaName": "Menu", "displayName": "Main Menu", "levelName": "Menu" },</v>
       </c>
-      <c r="G2" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT(E2:E1000)</f>
-        <v>0x784BFC: { "id": 0x784BFC, "areaName": "Menu", "displayName": "Main Menu", "levelName": "Menu" },0x789668: { "id": 0x789668, "areaName": "Intro", "displayName": "somewhere in the Glade of Dreams…", "levelName": "None" },0x778C74: { "id": 0x778C74, "areaName": "BuccaneerBrig", "displayName": "in the Buccaneer’s brig", "levelName": "None" },0x78D424: { "id": 0x78D424, "areaName": "WoodsOfLight", "displayName": "in the Woods of Light", "levelName": "Woods of Light" },0x790570: { "id": 0x790570, "areaName": "HallOfDoors", "displayName": "in the Hall of Doors", "levelName": "Hall of Doors" },0x7875A8: { "id": 0x7875A8, "areaName": "FairyGladeArea1", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x78A320: { "id": 0x78A320, "areaName": "FairyGladeArea2", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x7A1BD8: { "id": 0x7A1BD8, "areaName": "FairyGladeArea3", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x77BFFC: { "id": 0x77BFFC, "areaName": "FairyGladeArea4", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x771B74: { "id": 0x771B74, "areaName": "FairyGladeArea5", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x74AAA8: { "id": 0x74AAA8, "areaName": "Results", "displayName": "viewing level results…", "levelName": "None" },0x788708: { "id": 0x788708, "areaName": "MarshesArea1", "displayName": "in the Marshes of Awakening", "levelName": "Marshes of Awakening" },0x7786E8: { "id": 0x7786E8, "areaName": "MarshesArea2", "displayName": "in the Marshes of Awakening", "levelName": "Marshes of Awakening" },0x790598: { "id": 0x790598, "areaName": "BayouArea1", "displayName": "in the Bayou", "levelName": "Bayou" },</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
@@ -755,7 +774,22 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D16" s="4"/>
+      <c r="A16" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("0x", A16,": { ""id"": ","0x", A16,", ""areaName"": """,B16,""", ""displayName"": """,C16,""", ""levelName"": """,D16,""" },")</f>
+        <v>0x788764: { "id": 0x788764, "areaName": "BayouArea2", "displayName": "in the Bayou", "levelName": "Bayou" },</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D17" s="4"/>
@@ -3781,10 +3815,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="bottomLeft" activeCell="L2" activeCellId="0" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.21"/>
@@ -3796,22 +3830,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>4</v>
@@ -3887,11 +3921,11 @@
       </c>
       <c r="E4" s="0" t="n">
         <f aca="false">COUNTIFS(Lums!C3:C1002, "=" &amp; B4)</f>
-        <v>897</v>
+        <v>858</v>
       </c>
       <c r="F4" s="0" t="n">
         <f aca="false">COUNTIFS(Cages!C3:C83, "=" &amp; B4)</f>
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="G4" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A4,": { ""id"": ",A4,", ""name"": """,B4,""", ""lums"": ",C4,", ""cages"": ",D4," },")</f>
@@ -3968,11 +4002,11 @@
       </c>
       <c r="E7" s="0" t="n">
         <f aca="false">COUNTIFS(Lums!C6:C1005, "=" &amp; B7)</f>
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="F7" s="0" t="n">
         <f aca="false">COUNTIFS(Cages!C6:C86, "=" &amp; B7)</f>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="G7" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A7,": { ""id"": ",A7,", ""name"": """,B7,""", ""lums"": ",C7,", ""cages"": ",D7," },")</f>
@@ -4018,7 +4052,7 @@
       </c>
       <c r="F9" s="0" t="n">
         <f aca="false">COUNTIFS(Cages!C8:C88, "=" &amp; B9)</f>
-        <v>74</v>
+        <v>7</v>
       </c>
       <c r="G9" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A9,": { ""id"": ",A9,", ""name"": """,B9,""", ""lums"": ",C9,", ""cages"": ",D9," },")</f>
@@ -4037,7 +4071,7 @@
       </c>
       <c r="F10" s="0" t="n">
         <f aca="false">COUNTIFS(Cages!C9:C89, "=" &amp; B10)</f>
-        <v>75</v>
+        <v>8</v>
       </c>
       <c r="G10" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A10,": { ""id"": ",A10,", ""name"": """,B10,""", ""lums"": ",C10,", ""cages"": ",D10," },")</f>
@@ -4056,7 +4090,7 @@
       </c>
       <c r="F11" s="0" t="n">
         <f aca="false">COUNTIFS(Cages!C10:C90, "=" &amp; B11)</f>
-        <v>76</v>
+        <v>9</v>
       </c>
       <c r="G11" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A11,": { ""id"": ",A11,", ""name"": """,B11,""", ""lums"": ",C11,", ""cages"": ",D11," },")</f>
@@ -4075,7 +4109,7 @@
       </c>
       <c r="F12" s="0" t="n">
         <f aca="false">COUNTIFS(Cages!C11:C91, "=" &amp; B12)</f>
-        <v>77</v>
+        <v>10</v>
       </c>
       <c r="G12" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A12,": { ""id"": ",A12,", ""name"": """,B12,""", ""lums"": ",C12,", ""cages"": ",D12," },")</f>
@@ -4094,7 +4128,7 @@
       </c>
       <c r="F13" s="0" t="n">
         <f aca="false">COUNTIFS(Cages!C12:C92, "=" &amp; B13)</f>
-        <v>78</v>
+        <v>11</v>
       </c>
       <c r="G13" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A13,": { ""id"": ",A13,", ""name"": """,B13,""", ""lums"": ",C13,", ""cages"": ",D13," },")</f>
@@ -4113,7 +4147,7 @@
       </c>
       <c r="F14" s="0" t="n">
         <f aca="false">COUNTIFS(Cages!C13:C93, "=" &amp; B14)</f>
-        <v>79</v>
+        <v>12</v>
       </c>
       <c r="G14" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A14,": { ""id"": ",A14,", ""name"": """,B14,""", ""lums"": ",C14,", ""cages"": ",D14," },")</f>
@@ -4132,7 +4166,7 @@
       </c>
       <c r="F15" s="0" t="n">
         <f aca="false">COUNTIFS(Cages!C14:C94, "=" &amp; B15)</f>
-        <v>80</v>
+        <v>13</v>
       </c>
       <c r="G15" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A15,": { ""id"": ",A15,", ""name"": """,B15,""", ""lums"": ",C15,", ""cages"": ",D15," },")</f>
@@ -4151,7 +4185,7 @@
       </c>
       <c r="F16" s="0" t="n">
         <f aca="false">COUNTIFS(Cages!C15:C95, "=" &amp; B16)</f>
-        <v>81</v>
+        <v>14</v>
       </c>
       <c r="G16" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A16,": { ""id"": ",A16,", ""name"": """,B16,""", ""lums"": ",C16,", ""cages"": ",D16," },")</f>
@@ -4170,7 +4204,7 @@
       </c>
       <c r="F17" s="0" t="n">
         <f aca="false">COUNTIFS(Cages!C16:C96, "=" &amp; B17)</f>
-        <v>81</v>
+        <v>15</v>
       </c>
       <c r="G17" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A17,": { ""id"": ",A17,", ""name"": """,B17,""", ""lums"": ",C17,", ""cages"": ",D17," },")</f>
@@ -4189,7 +4223,7 @@
       </c>
       <c r="F18" s="0" t="n">
         <f aca="false">COUNTIFS(Cages!C17:C97, "=" &amp; B18)</f>
-        <v>81</v>
+        <v>16</v>
       </c>
       <c r="G18" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A18,": { ""id"": ",A18,", ""name"": """,B18,""", ""lums"": ",C18,", ""cages"": ",D18," },")</f>
@@ -4208,7 +4242,7 @@
       </c>
       <c r="F19" s="0" t="n">
         <f aca="false">COUNTIFS(Cages!C18:C98, "=" &amp; B19)</f>
-        <v>81</v>
+        <v>17</v>
       </c>
       <c r="G19" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A19,": { ""id"": ",A19,", ""name"": """,B19,""", ""lums"": ",C19,", ""cages"": ",D19," },")</f>
@@ -4227,7 +4261,7 @@
       </c>
       <c r="F20" s="0" t="n">
         <f aca="false">COUNTIFS(Cages!C19:C99, "=" &amp; B20)</f>
-        <v>81</v>
+        <v>18</v>
       </c>
       <c r="G20" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A20,": { ""id"": ",A20,", ""name"": """,B20,""", ""lums"": ",C20,", ""cages"": ",D20," },")</f>
@@ -4246,7 +4280,7 @@
       </c>
       <c r="F21" s="0" t="n">
         <f aca="false">COUNTIFS(Cages!C20:C100, "=" &amp; B21)</f>
-        <v>81</v>
+        <v>19</v>
       </c>
       <c r="G21" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A21,": { ""id"": ",A21,", ""name"": """,B21,""", ""lums"": ",C21,", ""cages"": ",D21," },")</f>
@@ -4265,7 +4299,7 @@
       </c>
       <c r="F22" s="0" t="n">
         <f aca="false">COUNTIFS(Cages!C21:C101, "=" &amp; B22)</f>
-        <v>81</v>
+        <v>20</v>
       </c>
       <c r="G22" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A22,": { ""id"": ",A22,", ""name"": """,B22,""", ""lums"": ",C22,", ""cages"": ",D22," },")</f>
@@ -7476,15 +7510,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G1001"/>
+  <dimension ref="A1:H1001"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A124" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F110" activeCellId="0" sqref="F110"/>
+      <selection pane="bottomLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.93"/>
@@ -7493,10 +7527,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>3</v>
@@ -7507,10 +7541,14 @@
       <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="H1" s="5" t="str">
+        <f aca="false">_xlfn.CONCAT(D2:D1001)</f>
+        <v>1: { "levelId": 2, "mem": bit0(0x224988),"good": 1},2: { "levelId": 2, "mem": bit1(0x224988),"good": 1},3: { "levelId": 2, "mem": bit2(0x224988),"good": 1},4: { "levelId": 2, "mem": bit3(0x224988),"good": 1},5: { "levelId": 2, "mem": bit4(0x224988),"good": 1},6: { "levelId": 2, "mem": bit5(0x224988),"good": 1},7: { "levelId": 2, "mem": bit6(0x224988),"good": 1},8: { "levelId": 2, "mem": bit7(0x224988),"good": 1},9: { "levelId": 2, "mem": bit2(0x224989),"good": 1},10: { "levelId": 2, "mem": bit1(0x22498a),"good": 1},11: { "levelId": 2, "mem": bit2(0x22498a),"good": 1},12: { "levelId": 2, "mem": bit3(0x22498a),"good": 1},13: { "levelId": 2, "mem": bit4(0x22498a),"good": 1},14: { "levelId": 2, "mem": bit5(0x22498a),"good": 1},15: { "levelId": 2, "mem": bit6(0x22498a),"good": 1},16: { "levelId": 2, "mem": bit7(0x22498a),"good": 1},17: { "levelId": 2, "mem": bit5(0x22498b),"good": 1},18: { "levelId": 2, "mem": bit6(0x22498b),"good": 1},19: { "levelId": 2, "mem": bit7(0x22498b),"good": 1},20: { "levelId": 2, "mem": bit0(0x22498c),"good": 1},21: { "levelId": 2, "mem": bit1(0x22498c),"good": 1},22: { "levelId": 2, "mem": bit2(0x22498c),"good": 1},23: { "levelId": 2, "mem": bit3(0x22498c),"good": 1},24: { "levelId": 2, "mem": bit4(0x22498c),"good": 1},25: { "levelId": 2, "mem": bit5(0x22498c),"good": 1},26: { "levelId": 2, "mem": bit6(0x22498c),"good": 1},27: { "levelId": 2, "mem": bit7(0x22498c),"good": 1},28: { "levelId": 2, "mem": bit0(0x22498d),"good": 1},29: { "levelId": 2, "mem": bit1(0x22498d),"good": 1},30: { "levelId": 2, "mem": bit2(0x22498d),"good": 1},31: { "levelId": 2, "mem": bit3(0x22498d),"good": 1},32: { "levelId": 2, "mem": bit4(0x22498d),"good": 1},33: { "levelId": 2, "mem": bit5(0x22498d),"good": 1},34: { "levelId": 2, "mem": bit6(0x22498d),"good": 1},35: { "levelId": 2, "mem": bit7(0x22498d),"good": 1},36: { "levelId": 2, "mem": bit0(0x22498e),"good": 1},37: { "levelId": 2, "mem": bit1(0x22498e),"good": 1},38: { "levelId": 5, "mem": bit2(0x22498e),"good": 1},39: { "levelId": 5, "mem": bit3(0x22498e),"good": 1},40: { "levelId": 5, "mem": bit4(0x22498e),"good": 1},41: { "levelId": 5, "mem": bit5(0x22498e),"good": 1},42: { "levelId": 5, "mem": bit6(0x22498e),"good": 1},43: { "levelId": 5, "mem": bit7(0x22498e),"good": 1},44: { "levelId": 5, "mem": bit0(0x22498f),"good": 1},45: { "levelId": 5, "mem": bit1(0x22498f),"good": 1},46: { "levelId": 5, "mem": bit2(0x22498f),"good": 1},47: { "levelId": 5, "mem": bit3(0x22498f),"good": 1},48: { "levelId": 5, "mem": bit4(0x22498f),"good": 1},49: { "levelId": 5, "mem": bit5(0x22498f),"good": 1},50: { "levelId": 5, "mem": bit6(0x22498f),"good": 1},51: { "levelId": 5, "mem": bit7(0x22498f),"good": 1},52: { "levelId": 5, "mem": bit0(0x224990),"good": 1},53: { "levelId": 5, "mem": bit1(0x224990),"good": 1},54: { "levelId": 5, "mem": bit2(0x224990),"good": 1},55: { "levelId": 5, "mem": bit3(0x224990),"good": 1},56: { "levelId": 5, "mem": bit4(0x224990),"good": 1},57: { "levelId": 5, "mem": bit5(0x224990),"good": 1},58: { "levelId": 5, "mem": bit6(0x224990),"good": 1},59: { "levelId": 5, "mem": bit7(0x224990),"good": 1},60: { "levelId": 5, "mem": bit0(0x224991),"good": 1},61: { "levelId": 5, "mem": bit1(0x224991),"good": 1},62: { "levelId": 5, "mem": bit2(0x224991),"good": 1},63: { "levelId": 5, "mem": bit3(0x224991),"good": 1},64: { "levelId": 5, "mem": bit4(0x224991),"good": 1},65: { "levelId": 5, "mem": bit5(0x224991),"good": 1},66: { "levelId": 5, "mem": bit6(0x224991),"good": 1},67: { "levelId": 5, "mem": bit7(0x224991),"good": 1},68: { "levelId": 5, "mem": bit0(0x224992),"good": 1},69: { "levelId": 5, "mem": bit1(0x224992),"good": 1},70: { "levelId": 5, "mem": bit2(0x224992),"good": 1},71: { "levelId": 5, "mem": bit3(0x224992),"good": 1},72: { "levelId": 5, "mem": bit4(0x224992),"good": 1},73: { "levelId": 5, "mem": bit5(0x224992),"good": 1},74: { "levelId": 5, "mem": bit6(0x224992),"good": 1},75: { "levelId": 5, "mem": bit7(0x224992),"good": 1},76: { "levelId": 5, "mem": bit0(0x224993),"good": 1},77: { "levelId": 5, "mem": bit1(0x224993),"good": 1},78: { "levelId": 5, "mem": bit2(0x224993),"good": 1},79: { "levelId": 5, "mem": bit3(0x224993),"good": 1},80: { "levelId": 5, "mem": bit4(0x224993),"good": 1},81: { "levelId": 5, "mem": bit5(0x224993),"good": 1},82: { "levelId": 5, "mem": bit6(0x224993),"good": 1},83: { "levelId": 5, "mem": bit7(0x224993),"good": 1},84: { "levelId": 5, "mem": bit0(0x224994),"good": 1},85: { "levelId": 5, "mem": bit1(0x224994),"good": 1},86: { "levelId": 5, "mem": bit2(0x224994),"good": 1},87: { "levelId": 5, "mem": bit3(0x224994),"good": 1},88: { "levelId": 6, "mem": bit4(0x224994),"good": 1},89: { "levelId": 6, "mem": bit5(0x224994),"good": 1},90: { "levelId": 6, "mem": bit6(0x224994),"good": 1},91: { "levelId": 6, "mem": bit7(0x224994),"good": 1},92: { "levelId": 6, "mem": bit0(0x224995),"good": 1},93: { "levelId": 6, "mem": bit1(0x224995),"good": 1},94: { "levelId": 6, "mem": bit2(0x224995),"good": 1},95: { "levelId": 6, "mem": bit3(0x224995),"good": 1},96: { "levelId": 6, "mem": bit4(0x224995),"good": 1},97: { "levelId": 6, "mem": bit5(0x224995),"good": 1},98: { "levelId": 6, "mem": bit6(0x224995),"good": 1},99: { "levelId": 6, "mem": bit7(0x224995),"good": 1},100: { "levelId": 6, "mem": bit0(0x224996),"good": 1},101: { "levelId": 6, "mem": bit1(0x224996),"good": 1},102: { "levelId": 6, "mem": bit2(0x224996),"good": 1},103: { "levelId": 6, "mem": bit3(0x224996),"good": 1},104: { "levelId": 6, "mem": bit4(0x224996),"good": 1},105: { "levelId": 6, "mem": bit5(0x224996),"good": 1},106: { "levelId": 6, "mem": bit6(0x224996),"good": 1},107: { "levelId": 6, "mem": bit7(0x224996),"good": 1},108: { "levelId": 6, "mem": bit0(0x224997),"good": 1},109: { "levelId": 6, "mem": bit1(0x224997),"good": 1},110: { "levelId": 6, "mem": bit2(0x224997),"good": 1},111: { "levelId": 6, "mem": bit3(0x224997),"good": 1},112: { "levelId": 6, "mem": bit4(0x224997),"good": 1},113: { "levelId": 6, "mem": bit5(0x224997),"good": 1},114: { "levelId": 6, "mem": bit6(0x224997),"good": 1},115: { "levelId": 6, "mem": bit7(0x224997),"good": 1},116: { "levelId": 6, "mem": bit0(0x224998),"good": 1},117: { "levelId": 6, "mem": bit1(0x224998),"good": 1},118: { "levelId": 6, "mem": bit2(0x224998),"good": 1},119: { "levelId": 6, "mem": bit3(0x224998),"good": 1},120: { "levelId": 6, "mem": bit4(0x224998),"good": 1},121: { "levelId": 6, "mem": bit5(0x224998),"good": 1},122: { "levelId": 6, "mem": bit6(0x224998),"good": 1},123: { "levelId": 6, "mem": bit0(0x224999),"good": 1},124: { "levelId": 6, "mem": bit1(0x224999),"good": 1},125: { "levelId": 6, "mem": bit2(0x224999),"good": 1},126: { "levelId": 6, "mem": bit3(0x224999),"good": 1},127: { "levelId": 6, "mem": bit4(0x224999),"good": 1},128: { "levelId": 6, "mem": bit5(0x224999),"good": 1},129: { "levelId": 6, "mem": bit6(0x224999),"good": 1},130: { "levelId": 6, "mem": bit7(0x224999),"good": 1},131: { "levelId": 6, "mem": bit0(0x22499a),"good": 1},132: { "levelId": 6, "mem": bit1(0x22499a),"good": 1},133: { "levelId": 6, "mem": bit2(0x22499a),"good": 1},134: { "levelId": 6, "mem": bit3(0x22499a),"good": 1},135: { "levelId": 6, "mem": bit4(0x22499a),"good": 1},136: { "levelId": 6, "mem": bit5(0x22499a),"good": 1},137: { "levelId": 1, "mem": bit3(0x224a36),"good": 1},138: { "levelId": 1, "mem": bit4(0x224a36),"good": 1},139: { "levelId": 1, "mem": bit5(0x224a36),"good": 1},140: { "levelId": 1, "mem": bit6(0x224a36),"good": 1},141: { "levelId": 1, "mem": bit7(0x224a36),"good": 1},142: { "levelId": 6, "mem": bit7(0x224998),"good": 1},143: { "levelId": 3, "good": 0},144: { "levelId": 3, "good": 0},145: { "levelId": 3, "good": 0},146: { "levelId": 3, "good": 0},147: { "levelId": 3, "good": 0},148: { "levelId": 3, "good": 0},149: { "levelId": 3, "good": 0},150: { "levelId": 3, "good": 0},151: { "levelId": 3, "good": 0},152: { "levelId": 3, "good": 0},153: { "levelId": 3, "good": 0},154: { "levelId": 3, "good": 0},155: { "levelId": 3, "good": 0},156: { "levelId": 3, "good": 0},157: { "levelId": 3, "good": 0},158: { "levelId": 3, "good": 0},159: { "levelId": 3, "good": 0},160: { "levelId": 3, "good": 0},161: { "levelId": 3, "good": 0},162: { "levelId": 3, "good": 0},163: { "levelId": 3, "good": 0},164: { "levelId": 3, "good": 0},165: { "levelId": 3, "good": 0},166: { "levelId": 3, "good": 0},167: { "levelId": 3, "good": 0},168: { "levelId": 3, "good": 0},169: { "levelId": 3, "good": 0},170: { "levelId": 3, "good": 0},171: { "levelId": 3, "good": 0},172: { "levelId": 3, "good": 0},173: { "levelId": 3, "good": 0},174: { "levelId": 3, "good": 0},175: { "levelId": 3, "good": 0},176: { "levelId": 3, "good": 0},177: { "levelId": 3, "good": 0},178: { "levelId": 3, "good": 0},179: { "levelId": 3, "good": 0},180: { "levelId": 3, "good": 0},181: { "levelId": 3, "good": 0},182: { "levelId": 3, "good": 0},183: { "levelId": 3, "good": 0},184: { "levelId": 3, "good": 0},185: { "levelId": 3, "good": 0},186: { "levelId": 3, "good": 0},187: { "levelId": 3, "good": 0},188: { "levelId": 3, "good": 0},189: { "levelId": 3, "good": 0},190: { "levelId": 3, "good": 0},191: { "levelId": 3, "good": 0},192: { "levelId": 3, "good": 0},193: { "levelId": 3, "good": 0},194: { "levelId": 3, "good": 0},195: { "levelId": 3, "good": 0},196: { "levelId": 3, "good": 0},197: { "levelId": 3, "good": 0},198: { "levelId": 3, "good": 0},199: { "levelId": 3, "good": 0},200: { "levelId": 3, "good": 0},201: { "levelId": 3, "good": 0},202: { "levelId": 3, "good": 0},203: { "levelId": 3, "good": 0},204: { "levelId": 3, "good": 0},205: { "levelId": 3, "good": 0},206: { "levelId": 3, "good": 0},207: { "levelId": 3, "good": 0},208: { "levelId": 3, "good": 0},209: { "levelId": 3, "good": 0},210: { "levelId": 3, "good": 0},211: { "levelId": 3, "good": 0},212: { "levelId": 3, "good": 0},213: { "levelId": 3, "good": 0},214: { "levelId": 3, "good": 0},215: { "levelId": 3, "good": 0},216: { "levelId": 3, "good": 0},217: { "levelId": 3, "good": 0},218: { "levelId": 3, "good": 0},219: { "levelId": 3, "good": 0},220: { "levelId": 3, "good": 0},221: { "levelId": 3, "good": 0},222: { "levelId": 3, "good": 0},223: { "levelId": 3, "good": 0},224: { "levelId": 3, "good": 0},225: { "levelId": 3, "good": 0},226: { "levelId": 3, "good": 0},227: { "levelId": 3, "good": 0},228: { "levelId": 3, "good": 0},229: { "levelId": 3, "good": 0},230: { "levelId": 3, "good": 0},231: { "levelId": 3, "good": 0},232: { "levelId": 3, "good": 0},233: { "levelId": 3, "good": 0},234: { "levelId": 3, "good": 0},235: { "levelId": 3, "good": 0},236: { "levelId": 3, "good": 0},237: { "levelId": 3, "good": 0},238: { "levelId": 3, "good": 0},239: { "levelId": 3, "good": 0},240: { "levelId": 3, "good": 0},241: { "levelId": 3, "good": 0},242: { "levelId": 3, "good": 0},243: { "levelId": 3, "good": 0},244: { "levelId": 3, "good": 0},245: { "levelId": 3, "good": 0},246: { "levelId": 3, "good": 0},247: { "levelId": 3, "good": 0},248: { "levelId": 3, "good": 0},249: { "levelId": 3, "good": 0},250: { "levelId": 3, "good": 0},251: { "levelId": 3, "good": 0},252: { "levelId": 3, "good": 0},253: { "levelId": 3, "good": 0},254: { "levelId": 3, "good": 0},255: { "levelId": 3, "good": 0},256: { "levelId": 3, "good": 0},257: { "levelId": 3, "good": 0},258: { "levelId": 3, "good": 0},259: { "levelId": 3, "good": 0},260: { "levelId": 3, "good": 0},261: { "levelId": 3, "good": 0},262: { "levelId": 3, "good": 0},263: { "levelId": 3, "good": 0},264: { "levelId": 3, "good": 0},265: { "levelId": 3, "good": 0},266: { "levelId": 3, "good": 0},267: { "levelId": 3, "good": 0},268: { "levelId": 3, "good": 0},269: { "levelId": 3, "good": 0},270: { "levelId": 3, "good": 0},271: { "levelId": 3, "good": 0},272: { "levelId": 3, "good": 0},273: { "levelId": 3, "good": 0},274: { "levelId": 3, "good": 0},275: { "levelId": 3, "good": 0},276: { "levelId": 3, "good": 0},277: { "levelId": 3, "good": 0},278: { "levelId": 3, "good": 0},279: { "levelId": 3, "good": 0},280: { "levelId": 3, "good": 0},281: { "levelId": 3, "good": 0},282: { "levelId": 3, "good": 0},283: { "levelId": 3, "good": 0},284: { "levelId": 3, "good": 0},285: { "levelId": 3, "good": 0},286: { "levelId": 3, "good": 0},287: { "levelId": 3, "good": 0},288: { "levelId": 3, "good": 0},289: { "levelId": 3, "good": 0},290: { "levelId": 3, "good": 0},291: { "levelId": 3, "good": 0},292: { "levelId": 3, "good": 0},293: { "levelId": 3, "good": 0},294: { "levelId": 3, "good": 0},295: { "levelId": 3, "good": 0},296: { "levelId": 3, "good": 0},297: { "levelId": 3, "good": 0},298: { "levelId": 3, "good": 0},299: { "levelId": 3, "good": 0},300: { "levelId": 3, "good": 0},301: { "levelId": 3, "good": 0},302: { "levelId": 3, "good": 0},303: { "levelId": 3, "good": 0},304: { "levelId": 3, "good": 0},305: { "levelId": 3, "good": 0},306: { "levelId": 3, "good": 0},307: { "levelId": 3, "good": 0},308: { "levelId": 3, "good": 0},309: { "levelId": 3, "good": 0},310: { "levelId": 3, "good": 0},311: { "levelId": 3, "good": 0},312: { "levelId": 3, "good": 0},313: { "levelId": 3, "good": 0},314: { "levelId": 3, "good": 0},315: { "levelId": 3, "good": 0},316: { "levelId": 3, "good": 0},317: { "levelId": 3, "good": 0},318: { "levelId": 3, "good": 0},319: { "levelId": 3, "good": 0},320: { "levelId": 3, "good": 0},321: { "levelId": 3, "good": 0},322: { "levelId": 3, "good": 0},323: { "levelId": 3, "good": 0},324: { "levelId": 3, "good": 0},325: { "levelId": 3, "good": 0},326: { "levelId": 3, "good": 0},327: { "levelId": 3, "good": 0},328: { "levelId": 3, "good": 0},329: { "levelId": 3, "good": 0},330: { "levelId": 3, "good": 0},331: { "levelId": 3, "good": 0},332: { "levelId": 3, "good": 0},333: { "levelId": 3, "good": 0},334: { "levelId": 3, "good": 0},335: { "levelId": 3, "good": 0},336: { "levelId": 3, "good": 0},337: { "levelId": 3, "good": 0},338: { "levelId": 3, "good": 0},339: { "levelId": 3, "good": 0},340: { "levelId": 3, "good": 0},341: { "levelId": 3, "good": 0},342: { "levelId": 3, "good": 0},343: { "levelId": 3, "good": 0},344: { "levelId": 3, "good": 0},345: { "levelId": 3, "good": 0},346: { "levelId": 3, "good": 0},347: { "levelId": 3, "good": 0},348: { "levelId": 3, "good": 0},349: { "levelId": 3, "good": 0},350: { "levelId": 3, "good": 0},351: { "levelId": 3, "good": 0},352: { "levelId": 3, "good": 0},353: { "levelId": 3, "good": 0},354: { "levelId": 3, "good": 0},355: { "levelId": 3, "good": 0},356: { "levelId": 3, "good": 0},357: { "levelId": 3, "good": 0},358: { "levelId": 3, "good": 0},359: { "levelId": 3, "good": 0},360: { "levelId": 3, "good": 0},361: { "levelId": 3, "good": 0},362: { "levelId": 3, "good": 0},363: { "levelId": 3, "good": 0},364: { "levelId": 3, "good": 0},365: { "levelId": 3, "good": 0},366: { "levelId": 3, "good": 0},367: { "levelId": 3, "good": 0},368: { "levelId": 3, "good": 0},369: { "levelId": 3, "good": 0},370: { "levelId": 3, "good": 0},371: { "levelId": 3, "good": 0},372: { "levelId": 3, "good": 0},373: { "levelId": 3, "good": 0},374: { "levelId": 3, "good": 0},375: { "levelId": 3, "good": 0},376: { "levelId": 3, "good": 0},377: { "levelId": 3, "good": 0},378: { "levelId": 3, "good": 0},379: { "levelId": 3, "good": 0},380: { "levelId": 3, "good": 0},381: { "levelId": 3, "good": 0},382: { "levelId": 3, "good": 0},383: { "levelId": 3, "good": 0},384: { "levelId": 3, "good": 0},385: { "levelId": 3, "good": 0},386: { "levelId": 3, "good": 0},387: { "levelId": 3, "good": 0},388: { "levelId": 3, "good": 0},389: { "levelId": 3, "good": 0},390: { "levelId": 3, "good": 0},391: { "levelId": 3, "good": 0},392: { "levelId": 3, "good": 0},393: { "levelId": 3, "good": 0},394: { "levelId": 3, "good": 0},395: { "levelId": 3, "good": 0},396: { "levelId": 3, "good": 0},397: { "levelId": 3, "good": 0},398: { "levelId": 3, "good": 0},399: { "levelId": 3, "good": 0},400: { "levelId": 3, "good": 0},401: { "levelId": 3, "good": 0},402: { "levelId": 3, "good": 0},403: { "levelId": 3, "good": 0},404: { "levelId": 3, "good": 0},405: { "levelId": 3, "good": 0},406: { "levelId": 3, "good": 0},407: { "levelId": 3, "good": 0},408: { "levelId": 3, "good": 0},409: { "levelId": 3, "good": 0},410: { "levelId": 3, "good": 0},411: { "levelId": 3, "good": 0},412: { "levelId": 3, "good": 0},413: { "levelId": 3, "good": 0},414: { "levelId": 3, "good": 0},415: { "levelId": 3, "good": 0},416: { "levelId": 3, "good": 0},417: { "levelId": 3, "good": 0},418: { "levelId": 3, "good": 0},419: { "levelId": 3, "good": 0},420: { "levelId": 3, "good": 0},421: { "levelId": 3, "good": 0},422: { "levelId": 3, "good": 0},423: { "levelId": 3, "good": 0},424: { "levelId": 3, "good": 0},425: { "levelId": 3, "good": 0},426: { "levelId": 3, "good": 0},427: { "levelId": 3, "good": 0},428: { "levelId": 3, "good": 0},429: { "levelId": 3, "good": 0},430: { "levelId": 3, "good": 0},431: { "levelId": 3, "good": 0},432: { "levelId": 3, "good": 0},433: { "levelId": 3, "good": 0},434: { "levelId": 3, "good": 0},435: { "levelId": 3, "good": 0},436: { "levelId": 3, "good": 0},437: { "levelId": 3, "good": 0},438: { "levelId": 3, "good": 0},439: { "levelId": 3, "good": 0},440: { "levelId": 3, "good": 0},441: { "levelId": 3, "good": 0},442: { "levelId": 3, "good": 0},443: { "levelId": 3, "good": 0},444: { "levelId": 3, "good": 0},445: { "levelId": 3, "good": 0},446: { "levelId": 3, "good": 0},447: { "levelId": 3, "good": 0},448: { "levelId": 3, "good": 0},449: { "levelId": 3, "good": 0},450: { "levelId": 3, "good": 0},451: { "levelId": 3, "good": 0},452: { "levelId": 3, "good": 0},453: { "levelId": 3, "good": 0},454: { "levelId": 3, "good": 0},455: { "levelId": 3, "good": 0},456: { "levelId": 3, "good": 0},457: { "levelId": 3, "good": 0},458: { "levelId": 3, "good": 0},459: { "levelId": 3, "good": 0},460: { "levelId": 3, "good": 0},461: { "levelId": 3, "good": 0},462: { "levelId": 3, "good": 0},463: { "levelId": 3, "good": 0},464: { "levelId": 3, "good": 0},465: { "levelId": 3, "good": 0},466: { "levelId": 3, "good": 0},467: { "levelId": 3, "good": 0},468: { "levelId": 3, "good": 0},469: { "levelId": 3, "good": 0},470: { "levelId": 3, "good": 0},471: { "levelId": 3, "good": 0},472: { "levelId": 3, "good": 0},473: { "levelId": 3, "good": 0},474: { "levelId": 3, "good": 0},475: { "levelId": 3, "good": 0},476: { "levelId": 3, "good": 0},477: { "levelId": 3, "good": 0},478: { "levelId": 3, "good": 0},479: { "levelId": 3, "good": 0},480: { "levelId": 3, "good": 0},481: { "levelId": 3, "good": 0},482: { "levelId": 3, "good": 0},483: { "levelId": 3, "good": 0},484: { "levelId": 3, "good": 0},485: { "levelId": 3, "good": 0},486: { "levelId": 3, "good": 0},487: { "levelId": 3, "good": 0},488: { "levelId": 3, "good": 0},489: { "levelId": 3, "good": 0},490: { "levelId": 3, "good": 0},491: { "levelId": 3, "good": 0},492: { "levelId": 3, "good": 0},493: { "levelId": 3, "good": 0},494: { "levelId": 3, "good": 0},495: { "levelId": 3, "good": 0},496: { "levelId": 3, "good": 0},497: { "levelId": 3, "good": 0},498: { "levelId": 3, "good": 0},499: { "levelId": 3, "good": 0},500: { "levelId": 3, "good": 0},501: { "levelId": 3, "good": 0},502: { "levelId": 3, "good": 0},503: { "levelId": 3, "good": 0},504: { "levelId": 3, "good": 0},505: { "levelId": 3, "good": 0},506: { "levelId": 3, "good": 0},507: { "levelId": 3, "good": 0},508: { "levelId": 3, "good": 0},509: { "levelId": 3, "good": 0},510: { "levelId": 3, "good": 0},511: { "levelId": 3, "good": 0},512: { "levelId": 3, "good": 0},513: { "levelId": 3, "good": 0},514: { "levelId": 3, "good": 0},515: { "levelId": 3, "good": 0},516: { "levelId": 3, "good": 0},517: { "levelId": 3, "good": 0},518: { "levelId": 3, "good": 0},519: { "levelId": 3, "good": 0},520: { "levelId": 3, "good": 0},521: { "levelId": 3, "good": 0},522: { "levelId": 3, "good": 0},523: { "levelId": 3, "good": 0},524: { "levelId": 3, "good": 0},525: { "levelId": 3, "good": 0},526: { "levelId": 3, "good": 0},527: { "levelId": 3, "good": 0},528: { "levelId": 3, "good": 0},529: { "levelId": 3, "good": 0},530: { "levelId": 3, "good": 0},531: { "levelId": 3, "good": 0},532: { "levelId": 3, "good": 0},533: { "levelId": 3, "good": 0},534: { "levelId": 3, "good": 0},535: { "levelId": 3, "good": 0},536: { "levelId": 3, "good": 0},537: { "levelId": 3, "good": 0},538: { "levelId": 3, "good": 0},539: { "levelId": 3, "good": 0},540: { "levelId": 3, "good": 0},541: { "levelId": 3, "good": 0},542: { "levelId": 3, "good": 0},543: { "levelId": 3, "good": 0},544: { "levelId": 3, "good": 0},545: { "levelId": 3, "good": 0},546: { "levelId": 3, "good": 0},547: { "levelId": 3, "good": 0},548: { "levelId": 3, "good": 0},549: { "levelId": 3, "good": 0},550: { "levelId": 3, "good": 0},551: { "levelId": 3, "good": 0},552: { "levelId": 3, "good": 0},553: { "levelId": 3, "good": 0},554: { "levelId": 3, "good": 0},555: { "levelId": 3, "good": 0},556: { "levelId": 3, "good": 0},557: { "levelId": 3, "good": 0},558: { "levelId": 3, "good": 0},559: { "levelId": 3, "good": 0},560: { "levelId": 3, "good": 0},561: { "levelId": 3, "good": 0},562: { "levelId": 3, "good": 0},563: { "levelId": 3, "good": 0},564: { "levelId": 3, "good": 0},565: { "levelId": 3, "good": 0},566: { "levelId": 3, "good": 0},567: { "levelId": 3, "good": 0},568: { "levelId": 3, "good": 0},569: { "levelId": 3, "good": 0},570: { "levelId": 3, "good": 0},571: { "levelId": 3, "good": 0},572: { "levelId": 3, "good": 0},573: { "levelId": 3, "good": 0},574: { "levelId": 3, "good": 0},575: { "levelId": 3, "good": 0},576: { "levelId": 3, "good": 0},577: { "levelId": 3, "good": 0},578: { "levelId": 3, "good": 0},579: { "levelId": 3, "good": 0},580: { "levelId": 3, "good": 0},581: { "levelId": 3, "good": 0},582: { "levelId": 3, "good": 0},583: { "levelId": 3, "good": 0},584: { "levelId": 3, "good": 0},585: { "levelId": 3, "good": 0},586: { "levelId": 3, "good": 0},587: { "levelId": 3, "good": 0},588: { "levelId": 3, "good": 0},589: { "levelId": 3, "good": 0},590: { "levelId": 3, "good": 0},591: { "levelId": 3, "good": 0},592: { "levelId": 3, "good": 0},593: { "levelId": 3, "good": 0},594: { "levelId": 3, "good": 0},595: { "levelId": 3, "good": 0},596: { "levelId": 3, "good": 0},597: { "levelId": 3, "good": 0},598: { "levelId": 3, "good": 0},599: { "levelId": 3, "good": 0},600: { "levelId": 3, "good": 0},601: { "levelId": 3, "good": 0},602: { "levelId": 3, "good": 0},603: { "levelId": 3, "good": 0},604: { "levelId": 3, "good": 0},605: { "levelId": 3, "good": 0},606: { "levelId": 3, "good": 0},607: { "levelId": 3, "good": 0},608: { "levelId": 3, "good": 0},609: { "levelId": 3, "good": 0},610: { "levelId": 3, "good": 0},611: { "levelId": 3, "good": 0},612: { "levelId": 3, "good": 0},613: { "levelId": 3, "good": 0},614: { "levelId": 3, "good": 0},615: { "levelId": 3, "good": 0},616: { "levelId": 3, "good": 0},617: { "levelId": 3, "good": 0},618: { "levelId": 3, "good": 0},619: { "levelId": 3, "good": 0},620: { "levelId": 3, "good": 0},621: { "levelId": 3, "good": 0},622: { "levelId": 3, "good": 0},623: { "levelId": 3, "good": 0},624: { "levelId": 3, "good": 0},625: { "levelId": 3, "good": 0},626: { "levelId": 3, "good": 0},627: { "levelId": 3, "good": 0},628: { "levelId": 3, "good": 0},629: { "levelId": 3, "good": 0},630: { "levelId": 3, "good": 0},631: { "levelId": 3, "good": 0},632: { "levelId": 3, "good": 0},633: { "levelId": 3, "good": 0},634: { "levelId": 3, "good": 0},635: { "levelId": 3, "good": 0},636: { "levelId": 3, "good": 0},637: { "levelId": 3, "good": 0},638: { "levelId": 3, "good": 0},639: { "levelId": 3, "good": 0},640: { "levelId": 3, "good": 0},641: { "levelId": 3, "good": 0},642: { "levelId": 3, "good": 0},643: { "levelId": 3, "good": 0},644: { "levelId": 3, "good": 0},645: { "levelId": 3, "good": 0},646: { "levelId": 3, "good": 0},647: { "levelId": 3, "good": 0},648: { "levelId": 3, "good": 0},649: { "levelId": 3, "good": 0},650: { "levelId": 3, "good": 0},651: { "levelId": 3, "good": 0},652: { "levelId": 3, "good": 0},653: { "levelId": 3, "good": 0},654: { "levelId": 3, "good": 0},655: { "levelId": 3, "good": 0},656: { "levelId": 3, "good": 0},657: { "levelId": 3, "good": 0},658: { "levelId": 3, "good": 0},659: { "levelId": 3, "good": 0},660: { "levelId": 3, "good": 0},661: { "levelId": 3, "good": 0},662: { "levelId": 3, "good": 0},663: { "levelId": 3, "good": 0},664: { "levelId": 3, "good": 0},665: { "levelId": 3, "good": 0},666: { "levelId": 3, "good": 0},667: { "levelId": 3, "good": 0},668: { "levelId": 3, "good": 0},669: { "levelId": 3, "good": 0},670: { "levelId": 3, "good": 0},671: { "levelId": 3, "good": 0},672: { "levelId": 3, "good": 0},673: { "levelId": 3, "good": 0},674: { "levelId": 3, "good": 0},675: { "levelId": 3, "good": 0},676: { "levelId": 3, "good": 0},677: { "levelId": 3, "good": 0},678: { "levelId": 3, "good": 0},679: { "levelId": 3, "good": 0},680: { "levelId": 3, "good": 0},681: { "levelId": 3, "good": 0},682: { "levelId": 3, "good": 0},683: { "levelId": 3, "good": 0},684: { "levelId": 3, "good": 0},685: { "levelId": 3, "good": 0},686: { "levelId": 3, "good": 0},687: { "levelId": 3, "good": 0},688: { "levelId": 3, "good": 0},689: { "levelId": 3, "good": 0},690: { "levelId": 3, "good": 0},691: { "levelId": 3, "good": 0},692: { "levelId": 3, "good": 0},693: { "levelId": 3, "good": 0},694: { "levelId": 3, "good": 0},695: { "levelId": 3, "good": 0},696: { "levelId": 3, "good": 0},697: { "levelId": 3, "good": 0},698: { "levelId": 3, "good": 0},699: { "levelId": 3, "good": 0},700: { "levelId": 3, "good": 0},701: { "levelId": 3, "good": 0},702: { "levelId": 3, "good": 0},703: { "levelId": 3, "good": 0},704: { "levelId": 3, "good": 0},705: { "levelId": 3, "good": 0},706: { "levelId": 3, "good": 0},707: { "levelId": 3, "good": 0},708: { "levelId": 3, "good": 0},709: { "levelId": 3, "good": 0},710: { "levelId": 3, "good": 0},711: { "levelId": 3, "good": 0},712: { "levelId": 3, "good": 0},713: { "levelId": 3, "good": 0},714: { "levelId": 3, "good": 0},715: { "levelId": 3, "good": 0},716: { "levelId": 3, "good": 0},717: { "levelId": 3, "good": 0},718: { "levelId": 3, "good": 0},719: { "levelId": 3, "good": 0},720: { "levelId": 3, "good": 0},721: { "levelId": 3, "good": 0},722: { "levelId": 3, "good": 0},723: { "levelId": 3, "good": 0},724: { "levelId": 3, "good": 0},725: { "levelId": 3, "good": 0},726: { "levelId": 3, "good": 0},727: { "levelId": 3, "good": 0},728: { "levelId": 3, "good": 0},729: { "levelId": 3, "good": 0},730: { "levelId": 3, "good": 0},731: { "levelId": 3, "good": 0},732: { "levelId": 3, "good": 0},733: { "levelId": 3, "good": 0},734: { "levelId": 3, "good": 0},735: { "levelId": 3, "good": 0},736: { "levelId": 3, "good": 0},737: { "levelId": 3, "good": 0},738: { "levelId": 3, "good": 0},739: { "levelId": 3, "good": 0},740: { "levelId": 3, "good": 0},741: { "levelId": 3, "good": 0},742: { "levelId": 3, "good": 0},743: { "levelId": 3, "good": 0},744: { "levelId": 3, "good": 0},745: { "levelId": 3, "good": 0},746: { "levelId": 3, "good": 0},747: { "levelId": 3, "good": 0},748: { "levelId": 3, "good": 0},749: { "levelId": 3, "good": 0},750: { "levelId": 3, "good": 0},751: { "levelId": 3, "good": 0},752: { "levelId": 3, "good": 0},753: { "levelId": 3, "good": 0},754: { "levelId": 3, "good": 0},755: { "levelId": 3, "good": 0},756: { "levelId": 3, "good": 0},757: { "levelId": 3, "good": 0},758: { "levelId": 3, "good": 0},759: { "levelId": 3, "good": 0},760: { "levelId": 3, "good": 0},761: { "levelId": 3, "good": 0},762: { "levelId": 3, "good": 0},763: { "levelId": 3, "good": 0},764: { "levelId": 3, "good": 0},765: { "levelId": 3, "good": 0},766: { "levelId": 3, "good": 0},767: { "levelId": 3, "good": 0},768: { "levelId": 3, "good": 0},769: { "levelId": 3, "good": 0},770: { "levelId": 3, "good": 0},771: { "levelId": 3, "good": 0},772: { "levelId": 3, "good": 0},773: { "levelId": 3, "good": 0},774: { "levelId": 3, "good": 0},775: { "levelId": 3, "good": 0},776: { "levelId": 3, "good": 0},777: { "levelId": 3, "good": 0},778: { "levelId": 3, "good": 0},779: { "levelId": 3, "good": 0},780: { "levelId": 3, "good": 0},781: { "levelId": 3, "good": 0},782: { "levelId": 3, "good": 0},783: { "levelId": 3, "good": 0},784: { "levelId": 3, "good": 0},785: { "levelId": 3, "good": 0},786: { "levelId": 3, "good": 0},787: { "levelId": 3, "good": 0},788: { "levelId": 3, "good": 0},789: { "levelId": 3, "good": 0},790: { "levelId": 3, "good": 0},791: { "levelId": 3, "good": 0},792: { "levelId": 3, "good": 0},793: { "levelId": 3, "good": 0},794: { "levelId": 3, "good": 0},795: { "levelId": 3, "good": 0},796: { "levelId": 3, "good": 0},797: { "levelId": 3, "good": 0},798: { "levelId": 3, "good": 0},799: { "levelId": 3, "good": 0},800: { "levelId": 3, "good": 0},801: { "levelId": 3, "good": 0},802: { "levelId": 3, "good": 0},803: { "levelId": 3, "good": 0},804: { "levelId": 3, "good": 0},805: { "levelId": 3, "good": 0},806: { "levelId": 3, "good": 0},807: { "levelId": 3, "good": 0},808: { "levelId": 3, "good": 0},809: { "levelId": 3, "good": 0},810: { "levelId": 3, "good": 0},811: { "levelId": 3, "good": 0},812: { "levelId": 3, "good": 0},813: { "levelId": 3, "good": 0},814: { "levelId": 3, "good": 0},815: { "levelId": 3, "good": 0},816: { "levelId": 3, "good": 0},817: { "levelId": 3, "good": 0},818: { "levelId": 3, "good": 0},819: { "levelId": 3, "good": 0},820: { "levelId": 3, "good": 0},821: { "levelId": 3, "good": 0},822: { "levelId": 3, "good": 0},823: { "levelId": 3, "good": 0},824: { "levelId": 3, "good": 0},825: { "levelId": 3, "good": 0},826: { "levelId": 3, "good": 0},827: { "levelId": 3, "good": 0},828: { "levelId": 3, "good": 0},829: { "levelId": 3, "good": 0},830: { "levelId": 3, "good": 0},831: { "levelId": 3, "good": 0},832: { "levelId": 3, "good": 0},833: { "levelId": 3, "good": 0},834: { "levelId": 3, "good": 0},835: { "levelId": 3, "good": 0},836: { "levelId": 3, "good": 0},837: { "levelId": 3, "good": 0},838: { "levelId": 3, "good": 0},839: { "levelId": 3, "good": 0},840: { "levelId": 3, "good": 0},841: { "levelId": 3, "good": 0},842: { "levelId": 3, "good": 0},843: { "levelId": 3, "good": 0},844: { "levelId": 3, "good": 0},845: { "levelId": 3, "good": 0},846: { "levelId": 3, "good": 0},847: { "levelId": 3, "good": 0},848: { "levelId": 3, "good": 0},849: { "levelId": 3, "good": 0},850: { "levelId": 3, "good": 0},851: { "levelId": 3, "good": 0},852: { "levelId": 3, "good": 0},853: { "levelId": 3, "good": 0},854: { "levelId": 3, "good": 0},855: { "levelId": 3, "good": 0},856: { "levelId": 3, "good": 0},857: { "levelId": 3, "good": 0},858: { "levelId": 3, "good": 0},859: { "levelId": 3, "good": 0},860: { "levelId": 3, "good": 0},861: { "levelId": 3, "good": 0},862: { "levelId": 3, "good": 0},863: { "levelId": 3, "good": 0},864: { "levelId": 3, "good": 0},865: { "levelId": 3, "good": 0},866: { "levelId": 3, "good": 0},867: { "levelId": 3, "good": 0},868: { "levelId": 3, "good": 0},869: { "levelId": 3, "good": 0},870: { "levelId": 3, "good": 0},871: { "levelId": 3, "good": 0},872: { "levelId": 3, "good": 0},873: { "levelId": 3, "good": 0},874: { "levelId": 3, "good": 0},875: { "levelId": 3, "good": 0},876: { "levelId": 3, "good": 0},877: { "levelId": 3, "good": 0},878: { "levelId": 3, "good": 0},879: { "levelId": 3, "good": 0},880: { "levelId": 3, "good": 0},881: { "levelId": 3, "good": 0},882: { "levelId": 3, "good": 0},883: { "levelId": 3, "good": 0},884: { "levelId": 3, "good": 0},885: { "levelId": 3, "good": 0},886: { "levelId": 3, "good": 0},887: { "levelId": 3, "good": 0},888: { "levelId": 3, "good": 0},889: { "levelId": 3, "good": 0},890: { "levelId": 3, "good": 0},891: { "levelId": 3, "good": 0},892: { "levelId": 3, "good": 0},893: { "levelId": 3, "good": 0},894: { "levelId": 3, "good": 0},895: { "levelId": 3, "good": 0},896: { "levelId": 3, "good": 0},897: { "levelId": 3, "good": 0},898: { "levelId": 3, "good": 0},899: { "levelId": 3, "good": 0},900: { "levelId": 3, "good": 0},901: { "levelId": 3, "good": 0},902: { "levelId": 3, "good": 0},903: { "levelId": 3, "good": 0},904: { "levelId": 3, "good": 0},905: { "levelId": 3, "good": 0},906: { "levelId": 3, "good": 0},907: { "levelId": 3, "good": 0},908: { "levelId": 3, "good": 0},909: { "levelId": 3, "good": 0},910: { "levelId": 3, "good": 0},911: { "levelId": 3, "good": 0},912: { "levelId": 3, "good": 0},913: { "levelId": 3, "good": 0},914: { "levelId": 3, "good": 0},915: { "levelId": 3, "good": 0},916: { "levelId": 3, "good": 0},917: { "levelId": 3, "good": 0},918: { "levelId": 3, "good": 0},919: { "levelId": 3, "good": 0},920: { "levelId": 3, "good": 0},921: { "levelId": 3, "good": 0},922: { "levelId": 3, "good": 0},923: { "levelId": 3, "good": 0},924: { "levelId": 3, "good": 0},925: { "levelId": 3, "good": 0},926: { "levelId": 3, "good": 0},927: { "levelId": 3, "good": 0},928: { "levelId": 3, "good": 0},929: { "levelId": 3, "good": 0},930: { "levelId": 3, "good": 0},931: { "levelId": 3, "good": 0},932: { "levelId": 3, "good": 0},933: { "levelId": 3, "good": 0},934: { "levelId": 3, "good": 0},935: { "levelId": 3, "good": 0},936: { "levelId": 3, "good": 0},937: { "levelId": 3, "good": 0},938: { "levelId": 3, "good": 0},939: { "levelId": 3, "good": 0},940: { "levelId": 3, "good": 0},941: { "levelId": 3, "good": 0},942: { "levelId": 3, "good": 0},943: { "levelId": 3, "good": 0},944: { "levelId": 3, "good": 0},945: { "levelId": 3, "good": 0},946: { "levelId": 3, "good": 0},947: { "levelId": 3, "good": 0},948: { "levelId": 3, "good": 0},949: { "levelId": 3, "good": 0},950: { "levelId": 3, "good": 0},951: { "levelId": 3, "good": 0},952: { "levelId": 3, "good": 0},953: { "levelId": 3, "good": 0},954: { "levelId": 3, "good": 0},955: { "levelId": 3, "good": 0},956: { "levelId": 3, "good": 0},957: { "levelId": 3, "good": 0},958: { "levelId": 3, "good": 0},959: { "levelId": 3, "good": 0},960: { "levelId": 3, "good": 0},961: { "levelId": 3, "good": 0},962: { "levelId": 3, "good": 0},963: { "levelId": 3, "good": 0},964: { "levelId": 3, "good": 0},965: { "levelId": 3, "good": 0},966: { "levelId": 3, "good": 0},967: { "levelId": 3, "good": 0},968: { "levelId": 3, "good": 0},969: { "levelId": 3, "good": 0},970: { "levelId": 3, "good": 0},971: { "levelId": 3, "good": 0},972: { "levelId": 3, "good": 0},973: { "levelId": 3, "good": 0},974: { "levelId": 3, "good": 0},975: { "levelId": 3, "good": 0},976: { "levelId": 3, "good": 0},977: { "levelId": 3, "good": 0},978: { "levelId": 3, "good": 0},979: { "levelId": 3, "good": 0},980: { "levelId": 3, "good": 0},981: { "levelId": 3, "good": 0},982: { "levelId": 3, "good": 0},983: { "levelId": 3, "good": 0},984: { "levelId": 3, "good": 0},985: { "levelId": 3, "good": 0},986: { "levelId": 3, "good": 0},987: { "levelId": 3, "good": 0},988: { "levelId": 3, "good": 0},989: { "levelId": 3, "good": 0},990: { "levelId": 3, "good": 0},991: { "levelId": 3, "good": 0},992: { "levelId": 3, "good": 0},993: { "levelId": 3, "good": 0},994: { "levelId": 3, "good": 0},995: { "levelId": 3, "good": 0},996: { "levelId": 3, "good": 0},997: { "levelId": 3, "good": 0},998: { "levelId": 3, "good": 0},999: { "levelId": 3, "good": 0},1000: { "levelId": 3, "good": 0},</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>57</v>
+      <c r="A2" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0</v>
@@ -7522,14 +7560,10 @@
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C2, Levels!B:B, 0), 1, 1)),", ",IF(A2 &lt;&gt; "", """mem"": bit" &amp; B2 &amp; "(" &amp; A2 &amp; "),", ""),"""good"": ",IF(A2 &lt;&gt; "", 1, 0),"},")</f>
         <v>1: { "levelId": 2, "mem": bit0(0x224988),"good": 1},</v>
       </c>
-      <c r="G2" s="6" t="str">
-        <f aca="false">_xlfn.CONCAT(D2:D1001)</f>
-        <v>1: { "levelId": 2, "mem": bit0(0x224988),"good": 1},2: { "levelId": 2, "mem": bit1(0x224988),"good": 1},3: { "levelId": 2, "mem": bit2(0x224988),"good": 1},4: { "levelId": 2, "mem": bit3(0x224988),"good": 1},5: { "levelId": 2, "mem": bit4(0x224988),"good": 1},6: { "levelId": 2, "mem": bit5(0x224988),"good": 1},7: { "levelId": 2, "mem": bit6(0x224988),"good": 1},8: { "levelId": 2, "mem": bit7(0x224988),"good": 1},9: { "levelId": 2, "mem": bit2(0x224989),"good": 1},10: { "levelId": 2, "mem": bit1(0x22498a),"good": 1},11: { "levelId": 2, "mem": bit2(0x22498a),"good": 1},12: { "levelId": 2, "mem": bit3(0x22498a),"good": 1},13: { "levelId": 2, "mem": bit4(0x22498a),"good": 1},14: { "levelId": 2, "mem": bit5(0x22498a),"good": 1},15: { "levelId": 2, "mem": bit6(0x22498a),"good": 1},16: { "levelId": 2, "mem": bit7(0x22498a),"good": 1},17: { "levelId": 2, "mem": bit5(0x22498b),"good": 1},18: { "levelId": 2, "mem": bit6(0x22498b),"good": 1},19: { "levelId": 2, "mem": bit7(0x22498b),"good": 1},20: { "levelId": 2, "mem": bit0(0x22498c),"good": 1},21: { "levelId": 2, "mem": bit1(0x22498c),"good": 1},22: { "levelId": 2, "mem": bit2(0x22498c),"good": 1},23: { "levelId": 2, "mem": bit3(0x22498c),"good": 1},24: { "levelId": 2, "mem": bit4(0x22498c),"good": 1},25: { "levelId": 2, "mem": bit5(0x22498c),"good": 1},26: { "levelId": 2, "mem": bit6(0x22498c),"good": 1},27: { "levelId": 2, "mem": bit7(0x22498c),"good": 1},28: { "levelId": 2, "mem": bit0(0x22498d),"good": 1},29: { "levelId": 2, "mem": bit1(0x22498d),"good": 1},30: { "levelId": 2, "mem": bit2(0x22498d),"good": 1},31: { "levelId": 2, "mem": bit3(0x22498d),"good": 1},32: { "levelId": 2, "mem": bit4(0x22498d),"good": 1},33: { "levelId": 2, "mem": bit5(0x22498d),"good": 1},34: { "levelId": 2, "mem": bit6(0x22498d),"good": 1},35: { "levelId": 2, "mem": bit7(0x22498d),"good": 1},36: { "levelId": 2, "mem": bit0(0x22498e),"good": 1},37: { "levelId": 2, "mem": bit1(0x22498e),"good": 1},38: { "levelId": 5, "mem": bit2(0x22498e),"good": 1},39: { "levelId": 5, "mem": bit3(0x22498e),"good": 1},40: { "levelId": 5, "mem": bit4(0x22498e),"good": 1},41: { "levelId": 5, "mem": bit5(0x22498e),"good": 1},42: { "levelId": 5, "mem": bit6(0x22498e),"good": 1},43: { "levelId": 5, "mem": bit7(0x22498e),"good": 1},44: { "levelId": 5, "mem": bit0(0x22498f),"good": 1},45: { "levelId": 5, "mem": bit1(0x22498f),"good": 1},46: { "levelId": 5, "mem": bit2(0x22498f),"good": 1},47: { "levelId": 5, "mem": bit3(0x22498f),"good": 1},48: { "levelId": 5, "mem": bit4(0x22498f),"good": 1},49: { "levelId": 5, "mem": bit5(0x22498f),"good": 1},50: { "levelId": 5, "mem": bit6(0x22498f),"good": 1},51: { "levelId": 5, "mem": bit7(0x22498f),"good": 1},52: { "levelId": 5, "mem": bit0(0x224990),"good": 1},53: { "levelId": 5, "mem": bit1(0x224990),"good": 1},54: { "levelId": 5, "mem": bit2(0x224990),"good": 1},55: { "levelId": 5, "mem": bit3(0x224990),"good": 1},56: { "levelId": 5, "mem": bit4(0x224990),"good": 1},57: { "levelId": 5, "mem": bit5(0x224990),"good": 1},58: { "levelId": 5, "mem": bit6(0x224990),"good": 1},59: { "levelId": 5, "mem": bit7(0x224990),"good": 1},60: { "levelId": 5, "mem": bit0(0x224991),"good": 1},61: { "levelId": 5, "mem": bit1(0x224991),"good": 1},62: { "levelId": 5, "mem": bit2(0x224991),"good": 1},63: { "levelId": 5, "mem": bit3(0x224991),"good": 1},64: { "levelId": 5, "mem": bit4(0x224991),"good": 1},65: { "levelId": 5, "mem": bit5(0x224991),"good": 1},66: { "levelId": 5, "mem": bit6(0x224991),"good": 1},67: { "levelId": 5, "mem": bit7(0x224991),"good": 1},68: { "levelId": 5, "mem": bit0(0x224992),"good": 1},69: { "levelId": 5, "mem": bit1(0x224992),"good": 1},70: { "levelId": 5, "mem": bit2(0x224992),"good": 1},71: { "levelId": 5, "mem": bit3(0x224992),"good": 1},72: { "levelId": 5, "mem": bit4(0x224992),"good": 1},73: { "levelId": 5, "mem": bit5(0x224992),"good": 1},74: { "levelId": 5, "mem": bit6(0x224992),"good": 1},75: { "levelId": 5, "mem": bit7(0x224992),"good": 1},76: { "levelId": 5, "mem": bit0(0x224993),"good": 1},77: { "levelId": 5, "mem": bit1(0x224993),"good": 1},78: { "levelId": 5, "mem": bit2(0x224993),"good": 1},79: { "levelId": 5, "mem": bit3(0x224993),"good": 1},80: { "levelId": 5, "mem": bit4(0x224993),"good": 1},81: { "levelId": 5, "mem": bit5(0x224993),"good": 1},82: { "levelId": 5, "mem": bit6(0x224993),"good": 1},83: { "levelId": 5, "mem": bit7(0x224993),"good": 1},84: { "levelId": 5, "mem": bit0(0x224994),"good": 1},85: { "levelId": 5, "mem": bit1(0x224994),"good": 1},86: { "levelId": 5, "mem": bit2(0x224994),"good": 1},87: { "levelId": 5, "mem": bit3(0x224994),"good": 1},88: { "levelId": 1, "mem": bit3(0x224a36),"good": 1},89: { "levelId": 1, "mem": bit4(0x224a36),"good": 1},90: { "levelId": 1, "mem": bit5(0x224a36),"good": 1},91: { "levelId": 1, "mem": bit6(0x224a36),"good": 1},92: { "levelId": 1, "mem": bit7(0x224a36),"good": 1},93: { "levelId": 6, "mem": bit1(0x224997),"good": 1},94: { "levelId": 6, "mem": bit2(0x224997),"good": 1},95: { "levelId": 6, "mem": bit4(0x224994),"good": 1},96: { "levelId": 6, "mem": bit5(0x224994),"good": 1},97: { "levelId": 6, "mem": bit6(0x224994),"good": 1},98: { "levelId": 6, "mem": bit7(0x224996),"good": 1},99: { "levelId": 6, "mem": bit0(0x224997),"good": 1},100: { "levelId": 6, "mem": bit7(0x224997),"good": 1},101: { "levelId": 6, "mem": bit0(0x224998),"good": 1},102: { "levelId": 6, "mem": bit1(0x224998),"good": 1},103: { "levelId": 6, "mem": bit2(0x224998),"good": 1},104: { "levelId": 3, "good": 0},105: { "levelId": 3, "good": 0},106: { "levelId": 3, "good": 0},107: { "levelId": 3, "good": 0},108: { "levelId": 3, "good": 0},109: { "levelId": 3, "good": 0},110: { "levelId": 3, "good": 0},111: { "levelId": 3, "good": 0},112: { "levelId": 3, "good": 0},113: { "levelId": 3, "good": 0},114: { "levelId": 3, "good": 0},115: { "levelId": 3, "good": 0},116: { "levelId": 3, "good": 0},117: { "levelId": 3, "good": 0},118: { "levelId": 3, "good": 0},119: { "levelId": 3, "good": 0},120: { "levelId": 3, "good": 0},121: { "levelId": 3, "good": 0},122: { "levelId": 3, "good": 0},123: { "levelId": 3, "good": 0},124: { "levelId": 3, "good": 0},125: { "levelId": 3, "good": 0},126: { "levelId": 3, "good": 0},127: { "levelId": 3, "good": 0},128: { "levelId": 3, "good": 0},129: { "levelId": 3, "good": 0},130: { "levelId": 3, "good": 0},131: { "levelId": 3, "good": 0},132: { "levelId": 3, "good": 0},133: { "levelId": 3, "good": 0},134: { "levelId": 3, "good": 0},135: { "levelId": 3, "good": 0},136: { "levelId": 3, "good": 0},137: { "levelId": 3, "good": 0},138: { "levelId": 3, "good": 0},139: { "levelId": 3, "good": 0},140: { "levelId": 3, "good": 0},141: { "levelId": 3, "good": 0},142: { "levelId": 3, "good": 0},143: { "levelId": 3, "good": 0},144: { "levelId": 3, "good": 0},145: { "levelId": 3, "good": 0},146: { "levelId": 3, "good": 0},147: { "levelId": 3, "good": 0},148: { "levelId": 3, "good": 0},149: { "levelId": 3, "good": 0},150: { "levelId": 3, "good": 0},151: { "levelId": 3, "good": 0},152: { "levelId": 3, "good": 0},153: { "levelId": 3, "good": 0},154: { "levelId": 3, "good": 0},155: { "levelId": 3, "good": 0},156: { "levelId": 3, "good": 0},157: { "levelId": 3, "good": 0},158: { "levelId": 3, "good": 0},159: { "levelId": 3, "good": 0},160: { "levelId": 3, "good": 0},161: { "levelId": 3, "good": 0},162: { "levelId": 3, "good": 0},163: { "levelId": 3, "good": 0},164: { "levelId": 3, "good": 0},165: { "levelId": 3, "good": 0},166: { "levelId": 3, "good": 0},167: { "levelId": 3, "good": 0},168: { "levelId": 3, "good": 0},169: { "levelId": 3, "good": 0},170: { "levelId": 3, "good": 0},171: { "levelId": 3, "good": 0},172: { "levelId": 3, "good": 0},173: { "levelId": 3, "good": 0},174: { "levelId": 3, "good": 0},175: { "levelId": 3, "good": 0},176: { "levelId": 3, "good": 0},177: { "levelId": 3, "good": 0},178: { "levelId": 3, "good": 0},179: { "levelId": 3, "good": 0},180: { "levelId": 3, "good": 0},181: { "levelId": 3, "good": 0},182: { "levelId": 3, "good": 0},183: { "levelId": 3, "good": 0},184: { "levelId": 3, "good": 0},185: { "levelId": 3, "good": 0},186: { "levelId": 3, "good": 0},187: { "levelId": 3, "good": 0},188: { "levelId": 3, "good": 0},189: { "levelId": 3, "good": 0},190: { "levelId": 3, "good": 0},191: { "levelId": 3, "good": 0},192: { "levelId": 3, "good": 0},193: { "levelId": 3, "good": 0},194: { "levelId": 3, "good": 0},195: { "levelId": 3, "good": 0},196: { "levelId": 3, "good": 0},197: { "levelId": 3, "good": 0},198: { "levelId": 3, "good": 0},199: { "levelId": 3, "good": 0},200: { "levelId": 3, "good": 0},201: { "levelId": 3, "good": 0},202: { "levelId": 3, "good": 0},203: { "levelId": 3, "good": 0},204: { "levelId": 3, "good": 0},205: { "levelId": 3, "good": 0},206: { "levelId": 3, "good": 0},207: { "levelId": 3, "good": 0},208: { "levelId": 3, "good": 0},209: { "levelId": 3, "good": 0},210: { "levelId": 3, "good": 0},211: { "levelId": 3, "good": 0},212: { "levelId": 3, "good": 0},213: { "levelId": 3, "good": 0},214: { "levelId": 3, "good": 0},215: { "levelId": 3, "good": 0},216: { "levelId": 3, "good": 0},217: { "levelId": 3, "good": 0},218: { "levelId": 3, "good": 0},219: { "levelId": 3, "good": 0},220: { "levelId": 3, "good": 0},221: { "levelId": 3, "good": 0},222: { "levelId": 3, "good": 0},223: { "levelId": 3, "good": 0},224: { "levelId": 3, "good": 0},225: { "levelId": 3, "good": 0},226: { "levelId": 3, "good": 0},227: { "levelId": 3, "good": 0},228: { "levelId": 3, "good": 0},229: { "levelId": 3, "good": 0},230: { "levelId": 3, "good": 0},231: { "levelId": 3, "good": 0},232: { "levelId": 3, "good": 0},233: { "levelId": 3, "good": 0},234: { "levelId": 3, "good": 0},235: { "levelId": 3, "good": 0},236: { "levelId": 3, "good": 0},237: { "levelId": 3, "good": 0},238: { "levelId": 3, "good": 0},239: { "levelId": 3, "good": 0},240: { "levelId": 3, "good": 0},241: { "levelId": 3, "good": 0},242: { "levelId": 3, "good": 0},243: { "levelId": 3, "good": 0},244: { "levelId": 3, "good": 0},245: { "levelId": 3, "good": 0},246: { "levelId": 3, "good": 0},247: { "levelId": 3, "good": 0},248: { "levelId": 3, "good": 0},249: { "levelId": 3, "good": 0},250: { "levelId": 3, "good": 0},251: { "levelId": 3, "good": 0},252: { "levelId": 3, "good": 0},253: { "levelId": 3, "good": 0},254: { "levelId": 3, "good": 0},255: { "levelId": 3, "good": 0},256: { "levelId": 3, "good": 0},257: { "levelId": 3, "good": 0},258: { "levelId": 3, "good": 0},259: { "levelId": 3, "good": 0},260: { "levelId": 3, "good": 0},261: { "levelId": 3, "good": 0},262: { "levelId": 3, "good": 0},263: { "levelId": 3, "good": 0},264: { "levelId": 3, "good": 0},265: { "levelId": 3, "good": 0},266: { "levelId": 3, "good": 0},267: { "levelId": 3, "good": 0},268: { "levelId": 3, "good": 0},269: { "levelId": 3, "good": 0},270: { "levelId": 3, "good": 0},271: { "levelId": 3, "good": 0},272: { "levelId": 3, "good": 0},273: { "levelId": 3, "good": 0},274: { "levelId": 3, "good": 0},275: { "levelId": 3, "good": 0},276: { "levelId": 3, "good": 0},277: { "levelId": 3, "good": 0},278: { "levelId": 3, "good": 0},279: { "levelId": 3, "good": 0},280: { "levelId": 3, "good": 0},281: { "levelId": 3, "good": 0},282: { "levelId": 3, "good": 0},283: { "levelId": 3, "good": 0},284: { "levelId": 3, "good": 0},285: { "levelId": 3, "good": 0},286: { "levelId": 3, "good": 0},287: { "levelId": 3, "good": 0},288: { "levelId": 3, "good": 0},289: { "levelId": 3, "good": 0},290: { "levelId": 3, "good": 0},291: { "levelId": 3, "good": 0},292: { "levelId": 3, "good": 0},293: { "levelId": 3, "good": 0},294: { "levelId": 3, "good": 0},295: { "levelId": 3, "good": 0},296: { "levelId": 3, "good": 0},297: { "levelId": 3, "good": 0},298: { "levelId": 3, "good": 0},299: { "levelId": 3, "good": 0},300: { "levelId": 3, "good": 0},301: { "levelId": 3, "good": 0},302: { "levelId": 3, "good": 0},303: { "levelId": 3, "good": 0},304: { "levelId": 3, "good": 0},305: { "levelId": 3, "good": 0},306: { "levelId": 3, "good": 0},307: { "levelId": 3, "good": 0},308: { "levelId": 3, "good": 0},309: { "levelId": 3, "good": 0},310: { "levelId": 3, "good": 0},311: { "levelId": 3, "good": 0},312: { "levelId": 3, "good": 0},313: { "levelId": 3, "good": 0},314: { "levelId": 3, "good": 0},315: { "levelId": 3, "good": 0},316: { "levelId": 3, "good": 0},317: { "levelId": 3, "good": 0},318: { "levelId": 3, "good": 0},319: { "levelId": 3, "good": 0},320: { "levelId": 3, "good": 0},321: { "levelId": 3, "good": 0},322: { "levelId": 3, "good": 0},323: { "levelId": 3, "good": 0},324: { "levelId": 3, "good": 0},325: { "levelId": 3, "good": 0},326: { "levelId": 3, "good": 0},327: { "levelId": 3, "good": 0},328: { "levelId": 3, "good": 0},329: { "levelId": 3, "good": 0},330: { "levelId": 3, "good": 0},331: { "levelId": 3, "good": 0},332: { "levelId": 3, "good": 0},333: { "levelId": 3, "good": 0},334: { "levelId": 3, "good": 0},335: { "levelId": 3, "good": 0},336: { "levelId": 3, "good": 0},337: { "levelId": 3, "good": 0},338: { "levelId": 3, "good": 0},339: { "levelId": 3, "good": 0},340: { "levelId": 3, "good": 0},341: { "levelId": 3, "good": 0},342: { "levelId": 3, "good": 0},343: { "levelId": 3, "good": 0},344: { "levelId": 3, "good": 0},345: { "levelId": 3, "good": 0},346: { "levelId": 3, "good": 0},347: { "levelId": 3, "good": 0},348: { "levelId": 3, "good": 0},349: { "levelId": 3, "good": 0},350: { "levelId": 3, "good": 0},351: { "levelId": 3, "good": 0},352: { "levelId": 3, "good": 0},353: { "levelId": 3, "good": 0},354: { "levelId": 3, "good": 0},355: { "levelId": 3, "good": 0},356: { "levelId": 3, "good": 0},357: { "levelId": 3, "good": 0},358: { "levelId": 3, "good": 0},359: { "levelId": 3, "good": 0},360: { "levelId": 3, "good": 0},361: { "levelId": 3, "good": 0},362: { "levelId": 3, "good": 0},363: { "levelId": 3, "good": 0},364: { "levelId": 3, "good": 0},365: { "levelId": 3, "good": 0},366: { "levelId": 3, "good": 0},367: { "levelId": 3, "good": 0},368: { "levelId": 3, "good": 0},369: { "levelId": 3, "good": 0},370: { "levelId": 3, "good": 0},371: { "levelId": 3, "good": 0},372: { "levelId": 3, "good": 0},373: { "levelId": 3, "good": 0},374: { "levelId": 3, "good": 0},375: { "levelId": 3, "good": 0},376: { "levelId": 3, "good": 0},377: { "levelId": 3, "good": 0},378: { "levelId": 3, "good": 0},379: { "levelId": 3, "good": 0},380: { "levelId": 3, "good": 0},381: { "levelId": 3, "good": 0},382: { "levelId": 3, "good": 0},383: { "levelId": 3, "good": 0},384: { "levelId": 3, "good": 0},385: { "levelId": 3, "good": 0},386: { "levelId": 3, "good": 0},387: { "levelId": 3, "good": 0},388: { "levelId": 3, "good": 0},389: { "levelId": 3, "good": 0},390: { "levelId": 3, "good": 0},391: { "levelId": 3, "good": 0},392: { "levelId": 3, "good": 0},393: { "levelId": 3, "good": 0},394: { "levelId": 3, "good": 0},395: { "levelId": 3, "good": 0},396: { "levelId": 3, "good": 0},397: { "levelId": 3, "good": 0},398: { "levelId": 3, "good": 0},399: { "levelId": 3, "good": 0},400: { "levelId": 3, "good": 0},401: { "levelId": 3, "good": 0},402: { "levelId": 3, "good": 0},403: { "levelId": 3, "good": 0},404: { "levelId": 3, "good": 0},405: { "levelId": 3, "good": 0},406: { "levelId": 3, "good": 0},407: { "levelId": 3, "good": 0},408: { "levelId": 3, "good": 0},409: { "levelId": 3, "good": 0},410: { "levelId": 3, "good": 0},411: { "levelId": 3, "good": 0},412: { "levelId": 3, "good": 0},413: { "levelId": 3, "good": 0},414: { "levelId": 3, "good": 0},415: { "levelId": 3, "good": 0},416: { "levelId": 3, "good": 0},417: { "levelId": 3, "good": 0},418: { "levelId": 3, "good": 0},419: { "levelId": 3, "good": 0},420: { "levelId": 3, "good": 0},421: { "levelId": 3, "good": 0},422: { "levelId": 3, "good": 0},423: { "levelId": 3, "good": 0},424: { "levelId": 3, "good": 0},425: { "levelId": 3, "good": 0},426: { "levelId": 3, "good": 0},427: { "levelId": 3, "good": 0},428: { "levelId": 3, "good": 0},429: { "levelId": 3, "good": 0},430: { "levelId": 3, "good": 0},431: { "levelId": 3, "good": 0},432: { "levelId": 3, "good": 0},433: { "levelId": 3, "good": 0},434: { "levelId": 3, "good": 0},435: { "levelId": 3, "good": 0},436: { "levelId": 3, "good": 0},437: { "levelId": 3, "good": 0},438: { "levelId": 3, "good": 0},439: { "levelId": 3, "good": 0},440: { "levelId": 3, "good": 0},441: { "levelId": 3, "good": 0},442: { "levelId": 3, "good": 0},443: { "levelId": 3, "good": 0},444: { "levelId": 3, "good": 0},445: { "levelId": 3, "good": 0},446: { "levelId": 3, "good": 0},447: { "levelId": 3, "good": 0},448: { "levelId": 3, "good": 0},449: { "levelId": 3, "good": 0},450: { "levelId": 3, "good": 0},451: { "levelId": 3, "good": 0},452: { "levelId": 3, "good": 0},453: { "levelId": 3, "good": 0},454: { "levelId": 3, "good": 0},455: { "levelId": 3, "good": 0},456: { "levelId": 3, "good": 0},457: { "levelId": 3, "good": 0},458: { "levelId": 3, "good": 0},459: { "levelId": 3, "good": 0},460: { "levelId": 3, "good": 0},461: { "levelId": 3, "good": 0},462: { "levelId": 3, "good": 0},463: { "levelId": 3, "good": 0},464: { "levelId": 3, "good": 0},465: { "levelId": 3, "good": 0},466: { "levelId": 3, "good": 0},467: { "levelId": 3, "good": 0},468: { "levelId": 3, "good": 0},469: { "levelId": 3, "good": 0},470: { "levelId": 3, "good": 0},471: { "levelId": 3, "good": 0},472: { "levelId": 3, "good": 0},473: { "levelId": 3, "good": 0},474: { "levelId": 3, "good": 0},475: { "levelId": 3, "good": 0},476: { "levelId": 3, "good": 0},477: { "levelId": 3, "good": 0},478: { "levelId": 3, "good": 0},479: { "levelId": 3, "good": 0},480: { "levelId": 3, "good": 0},481: { "levelId": 3, "good": 0},482: { "levelId": 3, "good": 0},483: { "levelId": 3, "good": 0},484: { "levelId": 3, "good": 0},485: { "levelId": 3, "good": 0},486: { "levelId": 3, "good": 0},487: { "levelId": 3, "good": 0},488: { "levelId": 3, "good": 0},489: { "levelId": 3, "good": 0},490: { "levelId": 3, "good": 0},491: { "levelId": 3, "good": 0},492: { "levelId": 3, "good": 0},493: { "levelId": 3, "good": 0},494: { "levelId": 3, "good": 0},495: { "levelId": 3, "good": 0},496: { "levelId": 3, "good": 0},497: { "levelId": 3, "good": 0},498: { "levelId": 3, "good": 0},499: { "levelId": 3, "good": 0},500: { "levelId": 3, "good": 0},501: { "levelId": 3, "good": 0},502: { "levelId": 3, "good": 0},503: { "levelId": 3, "good": 0},504: { "levelId": 3, "good": 0},505: { "levelId": 3, "good": 0},506: { "levelId": 3, "good": 0},507: { "levelId": 3, "good": 0},508: { "levelId": 3, "good": 0},509: { "levelId": 3, "good": 0},510: { "levelId": 3, "good": 0},511: { "levelId": 3, "good": 0},512: { "levelId": 3, "good": 0},513: { "levelId": 3, "good": 0},514: { "levelId": 3, "good": 0},515: { "levelId": 3, "good": 0},516: { "levelId": 3, "good": 0},517: { "levelId": 3, "good": 0},518: { "levelId": 3, "good": 0},519: { "levelId": 3, "good": 0},520: { "levelId": 3, "good": 0},521: { "levelId": 3, "good": 0},522: { "levelId": 3, "good": 0},523: { "levelId": 3, "good": 0},524: { "levelId": 3, "good": 0},525: { "levelId": 3, "good": 0},526: { "levelId": 3, "good": 0},527: { "levelId": 3, "good": 0},528: { "levelId": 3, "good": 0},529: { "levelId": 3, "good": 0},530: { "levelId": 3, "good": 0},531: { "levelId": 3, "good": 0},532: { "levelId": 3, "good": 0},533: { "levelId": 3, "good": 0},534: { "levelId": 3, "good": 0},535: { "levelId": 3, "good": 0},536: { "levelId": 3, "good": 0},537: { "levelId": 3, "good": 0},538: { "levelId": 3, "good": 0},539: { "levelId": 3, "good": 0},540: { "levelId": 3, "good": 0},541: { "levelId": 3, "good": 0},542: { "levelId": 3, "good": 0},543: { "levelId": 3, "good": 0},544: { "levelId": 3, "good": 0},545: { "levelId": 3, "good": 0},546: { "levelId": 3, "good": 0},547: { "levelId": 3, "good": 0},548: { "levelId": 3, "good": 0},549: { "levelId": 3, "good": 0},550: { "levelId": 3, "good": 0},551: { "levelId": 3, "good": 0},552: { "levelId": 3, "good": 0},553: { "levelId": 3, "good": 0},554: { "levelId": 3, "good": 0},555: { "levelId": 3, "good": 0},556: { "levelId": 3, "good": 0},557: { "levelId": 3, "good": 0},558: { "levelId": 3, "good": 0},559: { "levelId": 3, "good": 0},560: { "levelId": 3, "good": 0},561: { "levelId": 3, "good": 0},562: { "levelId": 3, "good": 0},563: { "levelId": 3, "good": 0},564: { "levelId": 3, "good": 0},565: { "levelId": 3, "good": 0},566: { "levelId": 3, "good": 0},567: { "levelId": 3, "good": 0},568: { "levelId": 3, "good": 0},569: { "levelId": 3, "good": 0},570: { "levelId": 3, "good": 0},571: { "levelId": 3, "good": 0},572: { "levelId": 3, "good": 0},573: { "levelId": 3, "good": 0},574: { "levelId": 3, "good": 0},575: { "levelId": 3, "good": 0},576: { "levelId": 3, "good": 0},577: { "levelId": 3, "good": 0},578: { "levelId": 3, "good": 0},579: { "levelId": 3, "good": 0},580: { "levelId": 3, "good": 0},581: { "levelId": 3, "good": 0},582: { "levelId": 3, "good": 0},583: { "levelId": 3, "good": 0},584: { "levelId": 3, "good": 0},585: { "levelId": 3, "good": 0},586: { "levelId": 3, "good": 0},587: { "levelId": 3, "good": 0},588: { "levelId": 3, "good": 0},589: { "levelId": 3, "good": 0},590: { "levelId": 3, "good": 0},591: { "levelId": 3, "good": 0},592: { "levelId": 3, "good": 0},593: { "levelId": 3, "good": 0},594: { "levelId": 3, "good": 0},595: { "levelId": 3, "good": 0},596: { "levelId": 3, "good": 0},597: { "levelId": 3, "good": 0},598: { "levelId": 3, "good": 0},599: { "levelId": 3, "good": 0},600: { "levelId": 3, "good": 0},601: { "levelId": 3, "good": 0},602: { "levelId": 3, "good": 0},603: { "levelId": 3, "good": 0},604: { "levelId": 3, "good": 0},605: { "levelId": 3, "good": 0},606: { "levelId": 3, "good": 0},607: { "levelId": 3, "good": 0},608: { "levelId": 3, "good": 0},609: { "levelId": 3, "good": 0},610: { "levelId": 3, "good": 0},611: { "levelId": 3, "good": 0},612: { "levelId": 3, "good": 0},613: { "levelId": 3, "good": 0},614: { "levelId": 3, "good": 0},615: { "levelId": 3, "good": 0},616: { "levelId": 3, "good": 0},617: { "levelId": 3, "good": 0},618: { "levelId": 3, "good": 0},619: { "levelId": 3, "good": 0},620: { "levelId": 3, "good": 0},621: { "levelId": 3, "good": 0},622: { "levelId": 3, "good": 0},623: { "levelId": 3, "good": 0},624: { "levelId": 3, "good": 0},625: { "levelId": 3, "good": 0},626: { "levelId": 3, "good": 0},627: { "levelId": 3, "good": 0},628: { "levelId": 3, "good": 0},629: { "levelId": 3, "good": 0},630: { "levelId": 3, "good": 0},631: { "levelId": 3, "good": 0},632: { "levelId": 3, "good": 0},633: { "levelId": 3, "good": 0},634: { "levelId": 3, "good": 0},635: { "levelId": 3, "good": 0},636: { "levelId": 3, "good": 0},637: { "levelId": 3, "good": 0},638: { "levelId": 3, "good": 0},639: { "levelId": 3, "good": 0},640: { "levelId": 3, "good": 0},641: { "levelId": 3, "good": 0},642: { "levelId": 3, "good": 0},643: { "levelId": 3, "good": 0},644: { "levelId": 3, "good": 0},645: { "levelId": 3, "good": 0},646: { "levelId": 3, "good": 0},647: { "levelId": 3, "good": 0},648: { "levelId": 3, "good": 0},649: { "levelId": 3, "good": 0},650: { "levelId": 3, "good": 0},651: { "levelId": 3, "good": 0},652: { "levelId": 3, "good": 0},653: { "levelId": 3, "good": 0},654: { "levelId": 3, "good": 0},655: { "levelId": 3, "good": 0},656: { "levelId": 3, "good": 0},657: { "levelId": 3, "good": 0},658: { "levelId": 3, "good": 0},659: { "levelId": 3, "good": 0},660: { "levelId": 3, "good": 0},661: { "levelId": 3, "good": 0},662: { "levelId": 3, "good": 0},663: { "levelId": 3, "good": 0},664: { "levelId": 3, "good": 0},665: { "levelId": 3, "good": 0},666: { "levelId": 3, "good": 0},667: { "levelId": 3, "good": 0},668: { "levelId": 3, "good": 0},669: { "levelId": 3, "good": 0},670: { "levelId": 3, "good": 0},671: { "levelId": 3, "good": 0},672: { "levelId": 3, "good": 0},673: { "levelId": 3, "good": 0},674: { "levelId": 3, "good": 0},675: { "levelId": 3, "good": 0},676: { "levelId": 3, "good": 0},677: { "levelId": 3, "good": 0},678: { "levelId": 3, "good": 0},679: { "levelId": 3, "good": 0},680: { "levelId": 3, "good": 0},681: { "levelId": 3, "good": 0},682: { "levelId": 3, "good": 0},683: { "levelId": 3, "good": 0},684: { "levelId": 3, "good": 0},685: { "levelId": 3, "good": 0},686: { "levelId": 3, "good": 0},687: { "levelId": 3, "good": 0},688: { "levelId": 3, "good": 0},689: { "levelId": 3, "good": 0},690: { "levelId": 3, "good": 0},691: { "levelId": 3, "good": 0},692: { "levelId": 3, "good": 0},693: { "levelId": 3, "good": 0},694: { "levelId": 3, "good": 0},695: { "levelId": 3, "good": 0},696: { "levelId": 3, "good": 0},697: { "levelId": 3, "good": 0},698: { "levelId": 3, "good": 0},699: { "levelId": 3, "good": 0},700: { "levelId": 3, "good": 0},701: { "levelId": 3, "good": 0},702: { "levelId": 3, "good": 0},703: { "levelId": 3, "good": 0},704: { "levelId": 3, "good": 0},705: { "levelId": 3, "good": 0},706: { "levelId": 3, "good": 0},707: { "levelId": 3, "good": 0},708: { "levelId": 3, "good": 0},709: { "levelId": 3, "good": 0},710: { "levelId": 3, "good": 0},711: { "levelId": 3, "good": 0},712: { "levelId": 3, "good": 0},713: { "levelId": 3, "good": 0},714: { "levelId": 3, "good": 0},715: { "levelId": 3, "good": 0},716: { "levelId": 3, "good": 0},717: { "levelId": 3, "good": 0},718: { "levelId": 3, "good": 0},719: { "levelId": 3, "good": 0},720: { "levelId": 3, "good": 0},721: { "levelId": 3, "good": 0},722: { "levelId": 3, "good": 0},723: { "levelId": 3, "good": 0},724: { "levelId": 3, "good": 0},725: { "levelId": 3, "good": 0},726: { "levelId": 3, "good": 0},727: { "levelId": 3, "good": 0},728: { "levelId": 3, "good": 0},729: { "levelId": 3, "good": 0},730: { "levelId": 3, "good": 0},731: { "levelId": 3, "good": 0},732: { "levelId": 3, "good": 0},733: { "levelId": 3, "good": 0},734: { "levelId": 3, "good": 0},735: { "levelId": 3, "good": 0},736: { "levelId": 3, "good": 0},737: { "levelId": 3, "good": 0},738: { "levelId": 3, "good": 0},739: { "levelId": 3, "good": 0},740: { "levelId": 3, "good": 0},741: { "levelId": 3, "good": 0},742: { "levelId": 3, "good": 0},743: { "levelId": 3, "good": 0},744: { "levelId": 3, "good": 0},745: { "levelId": 3, "good": 0},746: { "levelId": 3, "good": 0},747: { "levelId": 3, "good": 0},748: { "levelId": 3, "good": 0},749: { "levelId": 3, "good": 0},750: { "levelId": 3, "good": 0},751: { "levelId": 3, "good": 0},752: { "levelId": 3, "good": 0},753: { "levelId": 3, "good": 0},754: { "levelId": 3, "good": 0},755: { "levelId": 3, "good": 0},756: { "levelId": 3, "good": 0},757: { "levelId": 3, "good": 0},758: { "levelId": 3, "good": 0},759: { "levelId": 3, "good": 0},760: { "levelId": 3, "good": 0},761: { "levelId": 3, "good": 0},762: { "levelId": 3, "good": 0},763: { "levelId": 3, "good": 0},764: { "levelId": 3, "good": 0},765: { "levelId": 3, "good": 0},766: { "levelId": 3, "good": 0},767: { "levelId": 3, "good": 0},768: { "levelId": 3, "good": 0},769: { "levelId": 3, "good": 0},770: { "levelId": 3, "good": 0},771: { "levelId": 3, "good": 0},772: { "levelId": 3, "good": 0},773: { "levelId": 3, "good": 0},774: { "levelId": 3, "good": 0},775: { "levelId": 3, "good": 0},776: { "levelId": 3, "good": 0},777: { "levelId": 3, "good": 0},778: { "levelId": 3, "good": 0},779: { "levelId": 3, "good": 0},780: { "levelId": 3, "good": 0},781: { "levelId": 3, "good": 0},782: { "levelId": 3, "good": 0},783: { "levelId": 3, "good": 0},784: { "levelId": 3, "good": 0},785: { "levelId": 3, "good": 0},786: { "levelId": 3, "good": 0},787: { "levelId": 3, "good": 0},788: { "levelId": 3, "good": 0},789: { "levelId": 3, "good": 0},790: { "levelId": 3, "good": 0},791: { "levelId": 3, "good": 0},792: { "levelId": 3, "good": 0},793: { "levelId": 3, "good": 0},794: { "levelId": 3, "good": 0},795: { "levelId": 3, "good": 0},796: { "levelId": 3, "good": 0},797: { "levelId": 3, "good": 0},798: { "levelId": 3, "good": 0},799: { "levelId": 3, "good": 0},800: { "levelId": 3, "good": 0},801: { "levelId": 3, "good": 0},802: { "levelId": 3, "good": 0},803: { "levelId": 3, "good": 0},804: { "levelId": 3, "good": 0},805: { "levelId": 3, "good": 0},806: { "levelId": 3, "good": 0},807: { "levelId": 3, "good": 0},808: { "levelId": 3, "good": 0},809: { "levelId": 3, "good": 0},810: { "levelId": 3, "good": 0},811: { "levelId": 3, "good": 0},812: { "levelId": 3, "good": 0},813: { "levelId": 3, "good": 0},814: { "levelId": 3, "good": 0},815: { "levelId": 3, "good": 0},816: { "levelId": 3, "good": 0},817: { "levelId": 3, "good": 0},818: { "levelId": 3, "good": 0},819: { "levelId": 3, "good": 0},820: { "levelId": 3, "good": 0},821: { "levelId": 3, "good": 0},822: { "levelId": 3, "good": 0},823: { "levelId": 3, "good": 0},824: { "levelId": 3, "good": 0},825: { "levelId": 3, "good": 0},826: { "levelId": 3, "good": 0},827: { "levelId": 3, "good": 0},828: { "levelId": 3, "good": 0},829: { "levelId": 3, "good": 0},830: { "levelId": 3, "good": 0},831: { "levelId": 3, "good": 0},832: { "levelId": 3, "good": 0},833: { "levelId": 3, "good": 0},834: { "levelId": 3, "good": 0},835: { "levelId": 3, "good": 0},836: { "levelId": 3, "good": 0},837: { "levelId": 3, "good": 0},838: { "levelId": 3, "good": 0},839: { "levelId": 3, "good": 0},840: { "levelId": 3, "good": 0},841: { "levelId": 3, "good": 0},842: { "levelId": 3, "good": 0},843: { "levelId": 3, "good": 0},844: { "levelId": 3, "good": 0},845: { "levelId": 3, "good": 0},846: { "levelId": 3, "good": 0},847: { "levelId": 3, "good": 0},848: { "levelId": 3, "good": 0},849: { "levelId": 3, "good": 0},850: { "levelId": 3, "good": 0},851: { "levelId": 3, "good": 0},852: { "levelId": 3, "good": 0},853: { "levelId": 3, "good": 0},854: { "levelId": 3, "good": 0},855: { "levelId": 3, "good": 0},856: { "levelId": 3, "good": 0},857: { "levelId": 3, "good": 0},858: { "levelId": 3, "good": 0},859: { "levelId": 3, "good": 0},860: { "levelId": 3, "good": 0},861: { "levelId": 3, "good": 0},862: { "levelId": 3, "good": 0},863: { "levelId": 3, "good": 0},864: { "levelId": 3, "good": 0},865: { "levelId": 3, "good": 0},866: { "levelId": 3, "good": 0},867: { "levelId": 3, "good": 0},868: { "levelId": 3, "good": 0},869: { "levelId": 3, "good": 0},870: { "levelId": 3, "good": 0},871: { "levelId": 3, "good": 0},872: { "levelId": 3, "good": 0},873: { "levelId": 3, "good": 0},874: { "levelId": 3, "good": 0},875: { "levelId": 3, "good": 0},876: { "levelId": 3, "good": 0},877: { "levelId": 3, "good": 0},878: { "levelId": 3, "good": 0},879: { "levelId": 3, "good": 0},880: { "levelId": 3, "good": 0},881: { "levelId": 3, "good": 0},882: { "levelId": 3, "good": 0},883: { "levelId": 3, "good": 0},884: { "levelId": 3, "good": 0},885: { "levelId": 3, "good": 0},886: { "levelId": 3, "good": 0},887: { "levelId": 3, "good": 0},888: { "levelId": 3, "good": 0},889: { "levelId": 3, "good": 0},890: { "levelId": 3, "good": 0},891: { "levelId": 3, "good": 0},892: { "levelId": 3, "good": 0},893: { "levelId": 3, "good": 0},894: { "levelId": 3, "good": 0},895: { "levelId": 3, "good": 0},896: { "levelId": 3, "good": 0},897: { "levelId": 3, "good": 0},898: { "levelId": 3, "good": 0},899: { "levelId": 3, "good": 0},900: { "levelId": 3, "good": 0},901: { "levelId": 3, "good": 0},902: { "levelId": 3, "good": 0},903: { "levelId": 3, "good": 0},904: { "levelId": 3, "good": 0},905: { "levelId": 3, "good": 0},906: { "levelId": 3, "good": 0},907: { "levelId": 3, "good": 0},908: { "levelId": 3, "good": 0},909: { "levelId": 3, "good": 0},910: { "levelId": 3, "good": 0},911: { "levelId": 3, "good": 0},912: { "levelId": 3, "good": 0},913: { "levelId": 3, "good": 0},914: { "levelId": 3, "good": 0},915: { "levelId": 3, "good": 0},916: { "levelId": 3, "good": 0},917: { "levelId": 3, "good": 0},918: { "levelId": 3, "good": 0},919: { "levelId": 3, "good": 0},920: { "levelId": 3, "good": 0},921: { "levelId": 3, "good": 0},922: { "levelId": 3, "good": 0},923: { "levelId": 3, "good": 0},924: { "levelId": 3, "good": 0},925: { "levelId": 3, "good": 0},926: { "levelId": 3, "good": 0},927: { "levelId": 3, "good": 0},928: { "levelId": 3, "good": 0},929: { "levelId": 3, "good": 0},930: { "levelId": 3, "good": 0},931: { "levelId": 3, "good": 0},932: { "levelId": 3, "good": 0},933: { "levelId": 3, "good": 0},934: { "levelId": 3, "good": 0},935: { "levelId": 3, "good": 0},936: { "levelId": 3, "good": 0},937: { "levelId": 3, "good": 0},938: { "levelId": 3, "good": 0},939: { "levelId": 3, "good": 0},940: { "levelId": 3, "good": 0},941: { "levelId": 3, "good": 0},942: { "levelId": 3, "good": 0},943: { "levelId": 3, "good": 0},944: { "levelId": 3, "good": 0},945: { "levelId": 3, "good": 0},946: { "levelId": 3, "good": 0},947: { "levelId": 3, "good": 0},948: { "levelId": 3, "good": 0},949: { "levelId": 3, "good": 0},950: { "levelId": 3, "good": 0},951: { "levelId": 3, "good": 0},952: { "levelId": 3, "good": 0},953: { "levelId": 3, "good": 0},954: { "levelId": 3, "good": 0},955: { "levelId": 3, "good": 0},956: { "levelId": 3, "good": 0},957: { "levelId": 3, "good": 0},958: { "levelId": 3, "good": 0},959: { "levelId": 3, "good": 0},960: { "levelId": 3, "good": 0},961: { "levelId": 3, "good": 0},962: { "levelId": 3, "good": 0},963: { "levelId": 3, "good": 0},964: { "levelId": 3, "good": 0},965: { "levelId": 3, "good": 0},966: { "levelId": 3, "good": 0},967: { "levelId": 3, "good": 0},968: { "levelId": 3, "good": 0},969: { "levelId": 3, "good": 0},970: { "levelId": 3, "good": 0},971: { "levelId": 3, "good": 0},972: { "levelId": 3, "good": 0},973: { "levelId": 3, "good": 0},974: { "levelId": 3, "good": 0},975: { "levelId": 3, "good": 0},976: { "levelId": 3, "good": 0},977: { "levelId": 3, "good": 0},978: { "levelId": 3, "good": 0},979: { "levelId": 3, "good": 0},980: { "levelId": 3, "good": 0},981: { "levelId": 3, "good": 0},982: { "levelId": 3, "good": 0},983: { "levelId": 3, "good": 0},984: { "levelId": 3, "good": 0},985: { "levelId": 3, "good": 0},986: { "levelId": 3, "good": 0},987: { "levelId": 3, "good": 0},988: { "levelId": 3, "good": 0},989: { "levelId": 3, "good": 0},990: { "levelId": 3, "good": 0},991: { "levelId": 3, "good": 0},992: { "levelId": 3, "good": 0},993: { "levelId": 3, "good": 0},994: { "levelId": 3, "good": 0},995: { "levelId": 3, "good": 0},996: { "levelId": 3, "good": 0},997: { "levelId": 3, "good": 0},998: { "levelId": 3, "good": 0},999: { "levelId": 3, "good": 0},1000: { "levelId": 3, "good": 0},</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
-        <v>57</v>
+      <c r="A3" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1</v>
@@ -7541,11 +7575,11 @@
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C3, Levels!B:B, 0), 1, 1)),", ",IF(A3 &lt;&gt; "", """mem"": bit" &amp; B3 &amp; "(" &amp; A3 &amp; "),", ""),"""good"": ",IF(A3 &lt;&gt; "", 1, 0),"},")</f>
         <v>2: { "levelId": 2, "mem": bit1(0x224988),"good": 1},</v>
       </c>
-      <c r="E3" s="6"/>
+      <c r="E3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
-        <v>57</v>
+      <c r="A4" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>2</v>
@@ -7557,11 +7591,11 @@
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C4, Levels!B:B, 0), 1, 1)),", ",IF(A4 &lt;&gt; "", """mem"": bit" &amp; B4 &amp; "(" &amp; A4 &amp; "),", ""),"""good"": ",IF(A4 &lt;&gt; "", 1, 0),"},")</f>
         <v>3: { "levelId": 2, "mem": bit2(0x224988),"good": 1},</v>
       </c>
-      <c r="E4" s="6"/>
+      <c r="E4" s="5"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
-        <v>57</v>
+      <c r="A5" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>3</v>
@@ -7573,11 +7607,11 @@
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C5, Levels!B:B, 0), 1, 1)),", ",IF(A5 &lt;&gt; "", """mem"": bit" &amp; B5 &amp; "(" &amp; A5 &amp; "),", ""),"""good"": ",IF(A5 &lt;&gt; "", 1, 0),"},")</f>
         <v>4: { "levelId": 2, "mem": bit3(0x224988),"good": 1},</v>
       </c>
-      <c r="E5" s="6"/>
+      <c r="E5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
-        <v>57</v>
+      <c r="A6" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>4</v>
@@ -7589,11 +7623,11 @@
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C6, Levels!B:B, 0), 1, 1)),", ",IF(A6 &lt;&gt; "", """mem"": bit" &amp; B6 &amp; "(" &amp; A6 &amp; "),", ""),"""good"": ",IF(A6 &lt;&gt; "", 1, 0),"},")</f>
         <v>5: { "levelId": 2, "mem": bit4(0x224988),"good": 1},</v>
       </c>
-      <c r="E6" s="6"/>
+      <c r="E6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
-        <v>57</v>
+      <c r="A7" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>5</v>
@@ -7605,11 +7639,11 @@
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C7, Levels!B:B, 0), 1, 1)),", ",IF(A7 &lt;&gt; "", """mem"": bit" &amp; B7 &amp; "(" &amp; A7 &amp; "),", ""),"""good"": ",IF(A7 &lt;&gt; "", 1, 0),"},")</f>
         <v>6: { "levelId": 2, "mem": bit5(0x224988),"good": 1},</v>
       </c>
-      <c r="E7" s="6"/>
+      <c r="E7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
-        <v>57</v>
+      <c r="A8" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>6</v>
@@ -7621,11 +7655,11 @@
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C8, Levels!B:B, 0), 1, 1)),", ",IF(A8 &lt;&gt; "", """mem"": bit" &amp; B8 &amp; "(" &amp; A8 &amp; "),", ""),"""good"": ",IF(A8 &lt;&gt; "", 1, 0),"},")</f>
         <v>7: { "levelId": 2, "mem": bit6(0x224988),"good": 1},</v>
       </c>
-      <c r="E8" s="6"/>
+      <c r="E8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="s">
-        <v>57</v>
+      <c r="A9" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>7</v>
@@ -7637,11 +7671,11 @@
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C9, Levels!B:B, 0), 1, 1)),", ",IF(A9 &lt;&gt; "", """mem"": bit" &amp; B9 &amp; "(" &amp; A9 &amp; "),", ""),"""good"": ",IF(A9 &lt;&gt; "", 1, 0),"},")</f>
         <v>8: { "levelId": 2, "mem": bit7(0x224988),"good": 1},</v>
       </c>
-      <c r="E9" s="6"/>
+      <c r="E9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="s">
-        <v>58</v>
+      <c r="A10" s="6" t="s">
+        <v>60</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>2</v>
@@ -7655,8 +7689,8 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="s">
-        <v>59</v>
+      <c r="A11" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>1</v>
@@ -7670,8 +7704,8 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="s">
-        <v>59</v>
+      <c r="A12" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>2</v>
@@ -7685,8 +7719,8 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="s">
-        <v>59</v>
+      <c r="A13" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>3</v>
@@ -7700,8 +7734,8 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5" t="s">
-        <v>59</v>
+      <c r="A14" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>4</v>
@@ -7715,8 +7749,8 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5" t="s">
-        <v>59</v>
+      <c r="A15" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>5</v>
@@ -7730,8 +7764,8 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5" t="s">
-        <v>59</v>
+      <c r="A16" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>6</v>
@@ -7745,8 +7779,8 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="5" t="s">
-        <v>59</v>
+      <c r="A17" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>7</v>
@@ -7760,8 +7794,8 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5" t="s">
-        <v>60</v>
+      <c r="A18" s="6" t="s">
+        <v>62</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>5</v>
@@ -7775,8 +7809,8 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="5" t="s">
-        <v>60</v>
+      <c r="A19" s="6" t="s">
+        <v>62</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>6</v>
@@ -7790,8 +7824,8 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="5" t="s">
-        <v>60</v>
+      <c r="A20" s="6" t="s">
+        <v>62</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>7</v>
@@ -7805,8 +7839,8 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="5" t="s">
-        <v>61</v>
+      <c r="A21" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>0</v>
@@ -7820,8 +7854,8 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="5" t="s">
-        <v>61</v>
+      <c r="A22" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>1</v>
@@ -7835,8 +7869,8 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="5" t="s">
-        <v>61</v>
+      <c r="A23" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>2</v>
@@ -7850,8 +7884,8 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="5" t="s">
-        <v>61</v>
+      <c r="A24" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>3</v>
@@ -7865,8 +7899,8 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="5" t="s">
-        <v>61</v>
+      <c r="A25" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>4</v>
@@ -7880,8 +7914,8 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="5" t="s">
-        <v>61</v>
+      <c r="A26" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>5</v>
@@ -7895,8 +7929,8 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="5" t="s">
-        <v>61</v>
+      <c r="A27" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>6</v>
@@ -7910,8 +7944,8 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="5" t="s">
-        <v>61</v>
+      <c r="A28" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>7</v>
@@ -7925,8 +7959,8 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="5" t="s">
-        <v>62</v>
+      <c r="A29" s="6" t="s">
+        <v>64</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>0</v>
@@ -7940,8 +7974,8 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="5" t="s">
-        <v>62</v>
+      <c r="A30" s="6" t="s">
+        <v>64</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>1</v>
@@ -7955,8 +7989,8 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="5" t="s">
-        <v>62</v>
+      <c r="A31" s="6" t="s">
+        <v>64</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>2</v>
@@ -7970,8 +8004,8 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="5" t="s">
-        <v>62</v>
+      <c r="A32" s="6" t="s">
+        <v>64</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>3</v>
@@ -7985,8 +8019,8 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="5" t="s">
-        <v>62</v>
+      <c r="A33" s="6" t="s">
+        <v>64</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>4</v>
@@ -8000,8 +8034,8 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="5" t="s">
-        <v>62</v>
+      <c r="A34" s="6" t="s">
+        <v>64</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>5</v>
@@ -8015,8 +8049,8 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="5" t="s">
-        <v>62</v>
+      <c r="A35" s="6" t="s">
+        <v>64</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>6</v>
@@ -8030,8 +8064,8 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="5" t="s">
-        <v>62</v>
+      <c r="A36" s="6" t="s">
+        <v>64</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>7</v>
@@ -8045,8 +8079,8 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="5" t="s">
-        <v>63</v>
+      <c r="A37" s="6" t="s">
+        <v>65</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>0</v>
@@ -8060,8 +8094,8 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="5" t="s">
-        <v>63</v>
+      <c r="A38" s="6" t="s">
+        <v>65</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>1</v>
@@ -8076,7 +8110,7 @@
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>2</v>
@@ -8091,7 +8125,7 @@
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>3</v>
@@ -8106,7 +8140,7 @@
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>4</v>
@@ -8121,7 +8155,7 @@
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>5</v>
@@ -8136,7 +8170,7 @@
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>6</v>
@@ -8151,7 +8185,7 @@
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B44" s="0" t="n">
         <v>7</v>
@@ -8166,7 +8200,7 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B45" s="0" t="n">
         <v>0</v>
@@ -8181,7 +8215,7 @@
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B46" s="0" t="n">
         <v>1</v>
@@ -8196,7 +8230,7 @@
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B47" s="0" t="n">
         <v>2</v>
@@ -8211,7 +8245,7 @@
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B48" s="0" t="n">
         <v>3</v>
@@ -8226,7 +8260,7 @@
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B49" s="0" t="n">
         <v>4</v>
@@ -8241,7 +8275,7 @@
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B50" s="0" t="n">
         <v>5</v>
@@ -8256,7 +8290,7 @@
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B51" s="0" t="n">
         <v>6</v>
@@ -8271,7 +8305,7 @@
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B52" s="0" t="n">
         <v>7</v>
@@ -8286,7 +8320,7 @@
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B53" s="0" t="n">
         <v>0</v>
@@ -8301,7 +8335,7 @@
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B54" s="0" t="n">
         <v>1</v>
@@ -8316,7 +8350,7 @@
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B55" s="0" t="n">
         <v>2</v>
@@ -8331,7 +8365,7 @@
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B56" s="0" t="n">
         <v>3</v>
@@ -8346,7 +8380,7 @@
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B57" s="0" t="n">
         <v>4</v>
@@ -8361,7 +8395,7 @@
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B58" s="0" t="n">
         <v>5</v>
@@ -8376,7 +8410,7 @@
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B59" s="0" t="n">
         <v>6</v>
@@ -8391,7 +8425,7 @@
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B60" s="0" t="n">
         <v>7</v>
@@ -8406,7 +8440,7 @@
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B61" s="0" t="n">
         <v>0</v>
@@ -8421,7 +8455,7 @@
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B62" s="0" t="n">
         <v>1</v>
@@ -8436,7 +8470,7 @@
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B63" s="0" t="n">
         <v>2</v>
@@ -8451,7 +8485,7 @@
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B64" s="0" t="n">
         <v>3</v>
@@ -8466,7 +8500,7 @@
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B65" s="0" t="n">
         <v>4</v>
@@ -8481,7 +8515,7 @@
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B66" s="0" t="n">
         <v>5</v>
@@ -8496,7 +8530,7 @@
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B67" s="0" t="n">
         <v>6</v>
@@ -8511,7 +8545,7 @@
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B68" s="0" t="n">
         <v>7</v>
@@ -8526,7 +8560,7 @@
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B69" s="0" t="n">
         <v>0</v>
@@ -8541,7 +8575,7 @@
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B70" s="0" t="n">
         <v>1</v>
@@ -8556,7 +8590,7 @@
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B71" s="0" t="n">
         <v>2</v>
@@ -8571,7 +8605,7 @@
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B72" s="0" t="n">
         <v>3</v>
@@ -8586,7 +8620,7 @@
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B73" s="0" t="n">
         <v>4</v>
@@ -8601,7 +8635,7 @@
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B74" s="0" t="n">
         <v>5</v>
@@ -8616,7 +8650,7 @@
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B75" s="0" t="n">
         <v>6</v>
@@ -8631,7 +8665,7 @@
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B76" s="0" t="n">
         <v>7</v>
@@ -8646,7 +8680,7 @@
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B77" s="0" t="n">
         <v>0</v>
@@ -8661,7 +8695,7 @@
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B78" s="0" t="n">
         <v>1</v>
@@ -8676,7 +8710,7 @@
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B79" s="0" t="n">
         <v>2</v>
@@ -8691,7 +8725,7 @@
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B80" s="0" t="n">
         <v>3</v>
@@ -8706,7 +8740,7 @@
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B81" s="0" t="n">
         <v>4</v>
@@ -8721,7 +8755,7 @@
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B82" s="0" t="n">
         <v>5</v>
@@ -8736,7 +8770,7 @@
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B83" s="0" t="n">
         <v>6</v>
@@ -8751,7 +8785,7 @@
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B84" s="0" t="n">
         <v>7</v>
@@ -8765,8 +8799,8 @@
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="5" t="s">
-        <v>69</v>
+      <c r="A85" s="6" t="s">
+        <v>71</v>
       </c>
       <c r="B85" s="0" t="n">
         <v>0</v>
@@ -8780,8 +8814,8 @@
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="5" t="s">
-        <v>69</v>
+      <c r="A86" s="6" t="s">
+        <v>71</v>
       </c>
       <c r="B86" s="0" t="n">
         <v>1</v>
@@ -8795,8 +8829,8 @@
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="5" t="s">
-        <v>69</v>
+      <c r="A87" s="6" t="s">
+        <v>71</v>
       </c>
       <c r="B87" s="0" t="n">
         <v>2</v>
@@ -8810,8 +8844,8 @@
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="5" t="s">
-        <v>69</v>
+      <c r="A88" s="6" t="s">
+        <v>71</v>
       </c>
       <c r="B88" s="0" t="n">
         <v>3</v>
@@ -8825,83 +8859,83 @@
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="5" t="s">
-        <v>70</v>
+      <c r="A89" s="0" t="s">
+        <v>71</v>
       </c>
       <c r="B89" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="D89" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C89, Levels!B:B, 0), 1, 1)),", ",IF(A89 &lt;&gt; "", """mem"": bit" &amp; B89 &amp; "(" &amp; A89 &amp; "),", ""),"""good"": ",IF(A89 &lt;&gt; "", 1, 0),"},")</f>
-        <v>88: { "levelId": 1, "mem": bit3(0x224a36),"good": 1},</v>
+        <v>88: { "levelId": 6, "mem": bit4(0x224994),"good": 1},</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B90" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="D90" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C90, Levels!B:B, 0), 1, 1)),", ",IF(A90 &lt;&gt; "", """mem"": bit" &amp; B90 &amp; "(" &amp; A90 &amp; "),", ""),"""good"": ",IF(A90 &lt;&gt; "", 1, 0),"},")</f>
-        <v>89: { "levelId": 1, "mem": bit4(0x224a36),"good": 1},</v>
+        <v>89: { "levelId": 6, "mem": bit5(0x224994),"good": 1},</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B91" s="0" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="D91" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C91, Levels!B:B, 0), 1, 1)),", ",IF(A91 &lt;&gt; "", """mem"": bit" &amp; B91 &amp; "(" &amp; A91 &amp; "),", ""),"""good"": ",IF(A91 &lt;&gt; "", 1, 0),"},")</f>
-        <v>90: { "levelId": 1, "mem": bit5(0x224a36),"good": 1},</v>
+        <v>90: { "levelId": 6, "mem": bit6(0x224994),"good": 1},</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B92" s="0" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="D92" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C92, Levels!B:B, 0), 1, 1)),", ",IF(A92 &lt;&gt; "", """mem"": bit" &amp; B92 &amp; "(" &amp; A92 &amp; "),", ""),"""good"": ",IF(A92 &lt;&gt; "", 1, 0),"},")</f>
-        <v>91: { "levelId": 1, "mem": bit6(0x224a36),"good": 1},</v>
+        <v>91: { "levelId": 6, "mem": bit7(0x224994),"good": 1},</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B93" s="0" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="D93" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C93, Levels!B:B, 0), 1, 1)),", ",IF(A93 &lt;&gt; "", """mem"": bit" &amp; B93 &amp; "(" &amp; A93 &amp; "),", ""),"""good"": ",IF(A93 &lt;&gt; "", 1, 0),"},")</f>
-        <v>92: { "levelId": 1, "mem": bit7(0x224a36),"good": 1},</v>
+        <v>92: { "levelId": 6, "mem": bit0(0x224995),"good": 1},</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B94" s="0" t="n">
         <v>1</v>
@@ -8911,12 +8945,12 @@
       </c>
       <c r="D94" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C94, Levels!B:B, 0), 1, 1)),", ",IF(A94 &lt;&gt; "", """mem"": bit" &amp; B94 &amp; "(" &amp; A94 &amp; "),", ""),"""good"": ",IF(A94 &lt;&gt; "", 1, 0),"},")</f>
-        <v>93: { "levelId": 6, "mem": bit1(0x224997),"good": 1},</v>
+        <v>93: { "levelId": 6, "mem": bit1(0x224995),"good": 1},</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B95" s="0" t="n">
         <v>2</v>
@@ -8926,52 +8960,52 @@
       </c>
       <c r="D95" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C95, Levels!B:B, 0), 1, 1)),", ",IF(A95 &lt;&gt; "", """mem"": bit" &amp; B95 &amp; "(" &amp; A95 &amp; "),", ""),"""good"": ",IF(A95 &lt;&gt; "", 1, 0),"},")</f>
-        <v>94: { "levelId": 6, "mem": bit2(0x224997),"good": 1},</v>
+        <v>94: { "levelId": 6, "mem": bit2(0x224995),"good": 1},</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B96" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C96" s="4" t="s">
         <v>48</v>
       </c>
       <c r="D96" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C96, Levels!B:B, 0), 1, 1)),", ",IF(A96 &lt;&gt; "", """mem"": bit" &amp; B96 &amp; "(" &amp; A96 &amp; "),", ""),"""good"": ",IF(A96 &lt;&gt; "", 1, 0),"},")</f>
-        <v>95: { "levelId": 6, "mem": bit4(0x224994),"good": 1},</v>
+        <v>95: { "levelId": 6, "mem": bit3(0x224995),"good": 1},</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B97" s="0" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C97" s="4" t="s">
         <v>48</v>
       </c>
       <c r="D97" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C97, Levels!B:B, 0), 1, 1)),", ",IF(A97 &lt;&gt; "", """mem"": bit" &amp; B97 &amp; "(" &amp; A97 &amp; "),", ""),"""good"": ",IF(A97 &lt;&gt; "", 1, 0),"},")</f>
-        <v>96: { "levelId": 6, "mem": bit5(0x224994),"good": 1},</v>
+        <v>96: { "levelId": 6, "mem": bit4(0x224995),"good": 1},</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B98" s="0" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C98" s="4" t="s">
         <v>48</v>
       </c>
       <c r="D98" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C98, Levels!B:B, 0), 1, 1)),", ",IF(A98 &lt;&gt; "", """mem"": bit" &amp; B98 &amp; "(" &amp; A98 &amp; "),", ""),"""good"": ",IF(A98 &lt;&gt; "", 1, 0),"},")</f>
-        <v>97: { "levelId": 6, "mem": bit6(0x224994),"good": 1},</v>
+        <v>97: { "levelId": 6, "mem": bit5(0x224995),"good": 1},</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8979,44 +9013,44 @@
         <v>72</v>
       </c>
       <c r="B99" s="0" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C99" s="4" t="s">
         <v>48</v>
       </c>
       <c r="D99" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C99, Levels!B:B, 0), 1, 1)),", ",IF(A99 &lt;&gt; "", """mem"": bit" &amp; B99 &amp; "(" &amp; A99 &amp; "),", ""),"""good"": ",IF(A99 &lt;&gt; "", 1, 0),"},")</f>
-        <v>98: { "levelId": 6, "mem": bit7(0x224996),"good": 1},</v>
+        <v>98: { "levelId": 6, "mem": bit6(0x224995),"good": 1},</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B100" s="0" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C100" s="4" t="s">
         <v>48</v>
       </c>
       <c r="D100" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C100, Levels!B:B, 0), 1, 1)),", ",IF(A100 &lt;&gt; "", """mem"": bit" &amp; B100 &amp; "(" &amp; A100 &amp; "),", ""),"""good"": ",IF(A100 &lt;&gt; "", 1, 0),"},")</f>
-        <v>99: { "levelId": 6, "mem": bit0(0x224997),"good": 1},</v>
+        <v>99: { "levelId": 6, "mem": bit7(0x224995),"good": 1},</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B101" s="0" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C101" s="4" t="s">
         <v>48</v>
       </c>
       <c r="D101" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C101, Levels!B:B, 0), 1, 1)),", ",IF(A101 &lt;&gt; "", """mem"": bit" &amp; B101 &amp; "(" &amp; A101 &amp; "),", ""),"""good"": ",IF(A101 &lt;&gt; "", 1, 0),"},")</f>
-        <v>100: { "levelId": 6, "mem": bit7(0x224997),"good": 1},</v>
+        <v>100: { "levelId": 6, "mem": bit0(0x224996),"good": 1},</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9024,14 +9058,14 @@
         <v>73</v>
       </c>
       <c r="B102" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C102" s="4" t="s">
         <v>48</v>
       </c>
       <c r="D102" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C102, Levels!B:B, 0), 1, 1)),", ",IF(A102 &lt;&gt; "", """mem"": bit" &amp; B102 &amp; "(" &amp; A102 &amp; "),", ""),"""good"": ",IF(A102 &lt;&gt; "", 1, 0),"},")</f>
-        <v>101: { "levelId": 6, "mem": bit0(0x224998),"good": 1},</v>
+        <v>101: { "levelId": 6, "mem": bit1(0x224996),"good": 1},</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9039,14 +9073,14 @@
         <v>73</v>
       </c>
       <c r="B103" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C103" s="4" t="s">
         <v>48</v>
       </c>
       <c r="D103" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C103, Levels!B:B, 0), 1, 1)),", ",IF(A103 &lt;&gt; "", """mem"": bit" &amp; B103 &amp; "(" &amp; A103 &amp; "),", ""),"""good"": ",IF(A103 &lt;&gt; "", 1, 0),"},")</f>
-        <v>102: { "levelId": 6, "mem": bit1(0x224998),"good": 1},</v>
+        <v>102: { "levelId": 6, "mem": bit2(0x224996),"good": 1},</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9054,365 +9088,599 @@
         <v>73</v>
       </c>
       <c r="B104" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C104" s="4" t="s">
         <v>48</v>
       </c>
       <c r="D104" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C104, Levels!B:B, 0), 1, 1)),", ",IF(A104 &lt;&gt; "", """mem"": bit" &amp; B104 &amp; "(" &amp; A104 &amp; "),", ""),"""good"": ",IF(A104 &lt;&gt; "", 1, 0),"},")</f>
-        <v>103: { "levelId": 6, "mem": bit2(0x224998),"good": 1},</v>
+        <v>103: { "levelId": 6, "mem": bit3(0x224996),"good": 1},</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="B105" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="C105" s="4" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="D105" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C105, Levels!B:B, 0), 1, 1)),", ",IF(A105 &lt;&gt; "", """mem"": bit" &amp; B105 &amp; "(" &amp; A105 &amp; "),", ""),"""good"": ",IF(A105 &lt;&gt; "", 1, 0),"},")</f>
-        <v>104: { "levelId": 3, "good": 0},</v>
+        <v>104: { "levelId": 6, "mem": bit4(0x224996),"good": 1},</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="B106" s="0" t="n">
+        <v>5</v>
+      </c>
       <c r="C106" s="4" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="D106" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C106, Levels!B:B, 0), 1, 1)),", ",IF(A106 &lt;&gt; "", """mem"": bit" &amp; B106 &amp; "(" &amp; A106 &amp; "),", ""),"""good"": ",IF(A106 &lt;&gt; "", 1, 0),"},")</f>
-        <v>105: { "levelId": 3, "good": 0},</v>
+        <v>105: { "levelId": 6, "mem": bit5(0x224996),"good": 1},</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="B107" s="0" t="n">
+        <v>6</v>
+      </c>
       <c r="C107" s="4" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="D107" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C107, Levels!B:B, 0), 1, 1)),", ",IF(A107 &lt;&gt; "", """mem"": bit" &amp; B107 &amp; "(" &amp; A107 &amp; "),", ""),"""good"": ",IF(A107 &lt;&gt; "", 1, 0),"},")</f>
-        <v>106: { "levelId": 3, "good": 0},</v>
+        <v>106: { "levelId": 6, "mem": bit6(0x224996),"good": 1},</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="B108" s="0" t="n">
+        <v>7</v>
+      </c>
       <c r="C108" s="4" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="D108" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C108, Levels!B:B, 0), 1, 1)),", ",IF(A108 &lt;&gt; "", """mem"": bit" &amp; B108 &amp; "(" &amp; A108 &amp; "),", ""),"""good"": ",IF(A108 &lt;&gt; "", 1, 0),"},")</f>
-        <v>107: { "levelId": 3, "good": 0},</v>
+        <v>107: { "levelId": 6, "mem": bit7(0x224996),"good": 1},</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B109" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="C109" s="4" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="D109" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C109, Levels!B:B, 0), 1, 1)),", ",IF(A109 &lt;&gt; "", """mem"": bit" &amp; B109 &amp; "(" &amp; A109 &amp; "),", ""),"""good"": ",IF(A109 &lt;&gt; "", 1, 0),"},")</f>
-        <v>108: { "levelId": 3, "good": 0},</v>
+        <v>108: { "levelId": 6, "mem": bit0(0x224997),"good": 1},</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B110" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="C110" s="4" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="D110" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C110, Levels!B:B, 0), 1, 1)),", ",IF(A110 &lt;&gt; "", """mem"": bit" &amp; B110 &amp; "(" &amp; A110 &amp; "),", ""),"""good"": ",IF(A110 &lt;&gt; "", 1, 0),"},")</f>
-        <v>109: { "levelId": 3, "good": 0},</v>
+        <v>109: { "levelId": 6, "mem": bit1(0x224997),"good": 1},</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B111" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="C111" s="4" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="D111" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C111, Levels!B:B, 0), 1, 1)),", ",IF(A111 &lt;&gt; "", """mem"": bit" &amp; B111 &amp; "(" &amp; A111 &amp; "),", ""),"""good"": ",IF(A111 &lt;&gt; "", 1, 0),"},")</f>
-        <v>110: { "levelId": 3, "good": 0},</v>
+        <v>110: { "levelId": 6, "mem": bit2(0x224997),"good": 1},</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B112" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="C112" s="4" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="D112" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C112, Levels!B:B, 0), 1, 1)),", ",IF(A112 &lt;&gt; "", """mem"": bit" &amp; B112 &amp; "(" &amp; A112 &amp; "),", ""),"""good"": ",IF(A112 &lt;&gt; "", 1, 0),"},")</f>
-        <v>111: { "levelId": 3, "good": 0},</v>
+        <v>111: { "levelId": 6, "mem": bit3(0x224997),"good": 1},</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B113" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="C113" s="4" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="D113" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C113, Levels!B:B, 0), 1, 1)),", ",IF(A113 &lt;&gt; "", """mem"": bit" &amp; B113 &amp; "(" &amp; A113 &amp; "),", ""),"""good"": ",IF(A113 &lt;&gt; "", 1, 0),"},")</f>
-        <v>112: { "levelId": 3, "good": 0},</v>
+        <v>112: { "levelId": 6, "mem": bit4(0x224997),"good": 1},</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B114" s="0" t="n">
+        <v>5</v>
+      </c>
       <c r="C114" s="4" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="D114" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C114, Levels!B:B, 0), 1, 1)),", ",IF(A114 &lt;&gt; "", """mem"": bit" &amp; B114 &amp; "(" &amp; A114 &amp; "),", ""),"""good"": ",IF(A114 &lt;&gt; "", 1, 0),"},")</f>
-        <v>113: { "levelId": 3, "good": 0},</v>
+        <v>113: { "levelId": 6, "mem": bit5(0x224997),"good": 1},</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B115" s="0" t="n">
+        <v>6</v>
+      </c>
       <c r="C115" s="4" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="D115" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C115, Levels!B:B, 0), 1, 1)),", ",IF(A115 &lt;&gt; "", """mem"": bit" &amp; B115 &amp; "(" &amp; A115 &amp; "),", ""),"""good"": ",IF(A115 &lt;&gt; "", 1, 0),"},")</f>
-        <v>114: { "levelId": 3, "good": 0},</v>
+        <v>114: { "levelId": 6, "mem": bit6(0x224997),"good": 1},</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B116" s="0" t="n">
+        <v>7</v>
+      </c>
       <c r="C116" s="4" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="D116" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C116, Levels!B:B, 0), 1, 1)),", ",IF(A116 &lt;&gt; "", """mem"": bit" &amp; B116 &amp; "(" &amp; A116 &amp; "),", ""),"""good"": ",IF(A116 &lt;&gt; "", 1, 0),"},")</f>
-        <v>115: { "levelId": 3, "good": 0},</v>
+        <v>115: { "levelId": 6, "mem": bit7(0x224997),"good": 1},</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B117" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="C117" s="4" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="D117" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C117, Levels!B:B, 0), 1, 1)),", ",IF(A117 &lt;&gt; "", """mem"": bit" &amp; B117 &amp; "(" &amp; A117 &amp; "),", ""),"""good"": ",IF(A117 &lt;&gt; "", 1, 0),"},")</f>
-        <v>116: { "levelId": 3, "good": 0},</v>
+        <v>116: { "levelId": 6, "mem": bit0(0x224998),"good": 1},</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B118" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="C118" s="4" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="D118" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C118, Levels!B:B, 0), 1, 1)),", ",IF(A118 &lt;&gt; "", """mem"": bit" &amp; B118 &amp; "(" &amp; A118 &amp; "),", ""),"""good"": ",IF(A118 &lt;&gt; "", 1, 0),"},")</f>
-        <v>117: { "levelId": 3, "good": 0},</v>
+        <v>117: { "levelId": 6, "mem": bit1(0x224998),"good": 1},</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B119" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="C119" s="4" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="D119" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C119, Levels!B:B, 0), 1, 1)),", ",IF(A119 &lt;&gt; "", """mem"": bit" &amp; B119 &amp; "(" &amp; A119 &amp; "),", ""),"""good"": ",IF(A119 &lt;&gt; "", 1, 0),"},")</f>
-        <v>118: { "levelId": 3, "good": 0},</v>
+        <v>118: { "levelId": 6, "mem": bit2(0x224998),"good": 1},</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B120" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="C120" s="4" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="D120" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C120, Levels!B:B, 0), 1, 1)),", ",IF(A120 &lt;&gt; "", """mem"": bit" &amp; B120 &amp; "(" &amp; A120 &amp; "),", ""),"""good"": ",IF(A120 &lt;&gt; "", 1, 0),"},")</f>
-        <v>119: { "levelId": 3, "good": 0},</v>
+        <v>119: { "levelId": 6, "mem": bit3(0x224998),"good": 1},</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B121" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="C121" s="4" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="D121" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C121, Levels!B:B, 0), 1, 1)),", ",IF(A121 &lt;&gt; "", """mem"": bit" &amp; B121 &amp; "(" &amp; A121 &amp; "),", ""),"""good"": ",IF(A121 &lt;&gt; "", 1, 0),"},")</f>
-        <v>120: { "levelId": 3, "good": 0},</v>
+        <v>120: { "levelId": 6, "mem": bit4(0x224998),"good": 1},</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B122" s="0" t="n">
+        <v>5</v>
+      </c>
       <c r="C122" s="4" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="D122" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C122, Levels!B:B, 0), 1, 1)),", ",IF(A122 &lt;&gt; "", """mem"": bit" &amp; B122 &amp; "(" &amp; A122 &amp; "),", ""),"""good"": ",IF(A122 &lt;&gt; "", 1, 0),"},")</f>
-        <v>121: { "levelId": 3, "good": 0},</v>
+        <v>121: { "levelId": 6, "mem": bit5(0x224998),"good": 1},</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B123" s="0" t="n">
+        <v>6</v>
+      </c>
       <c r="C123" s="4" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="D123" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C123, Levels!B:B, 0), 1, 1)),", ",IF(A123 &lt;&gt; "", """mem"": bit" &amp; B123 &amp; "(" &amp; A123 &amp; "),", ""),"""good"": ",IF(A123 &lt;&gt; "", 1, 0),"},")</f>
-        <v>122: { "levelId": 3, "good": 0},</v>
+        <v>122: { "levelId": 6, "mem": bit6(0x224998),"good": 1},</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="B124" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="C124" s="4" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="D124" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C124, Levels!B:B, 0), 1, 1)),", ",IF(A124 &lt;&gt; "", """mem"": bit" &amp; B124 &amp; "(" &amp; A124 &amp; "),", ""),"""good"": ",IF(A124 &lt;&gt; "", 1, 0),"},")</f>
-        <v>123: { "levelId": 3, "good": 0},</v>
+        <v>123: { "levelId": 6, "mem": bit0(0x224999),"good": 1},</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="B125" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="C125" s="4" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="D125" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C125, Levels!B:B, 0), 1, 1)),", ",IF(A125 &lt;&gt; "", """mem"": bit" &amp; B125 &amp; "(" &amp; A125 &amp; "),", ""),"""good"": ",IF(A125 &lt;&gt; "", 1, 0),"},")</f>
-        <v>124: { "levelId": 3, "good": 0},</v>
+        <v>124: { "levelId": 6, "mem": bit1(0x224999),"good": 1},</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="B126" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="C126" s="4" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="D126" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C126, Levels!B:B, 0), 1, 1)),", ",IF(A126 &lt;&gt; "", """mem"": bit" &amp; B126 &amp; "(" &amp; A126 &amp; "),", ""),"""good"": ",IF(A126 &lt;&gt; "", 1, 0),"},")</f>
-        <v>125: { "levelId": 3, "good": 0},</v>
+        <v>125: { "levelId": 6, "mem": bit2(0x224999),"good": 1},</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="B127" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="C127" s="4" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="D127" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C127, Levels!B:B, 0), 1, 1)),", ",IF(A127 &lt;&gt; "", """mem"": bit" &amp; B127 &amp; "(" &amp; A127 &amp; "),", ""),"""good"": ",IF(A127 &lt;&gt; "", 1, 0),"},")</f>
-        <v>126: { "levelId": 3, "good": 0},</v>
+        <v>126: { "levelId": 6, "mem": bit3(0x224999),"good": 1},</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="B128" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="C128" s="4" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="D128" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C128, Levels!B:B, 0), 1, 1)),", ",IF(A128 &lt;&gt; "", """mem"": bit" &amp; B128 &amp; "(" &amp; A128 &amp; "),", ""),"""good"": ",IF(A128 &lt;&gt; "", 1, 0),"},")</f>
-        <v>127: { "levelId": 3, "good": 0},</v>
+        <v>127: { "levelId": 6, "mem": bit4(0x224999),"good": 1},</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="B129" s="0" t="n">
+        <v>5</v>
+      </c>
       <c r="C129" s="4" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="D129" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C129, Levels!B:B, 0), 1, 1)),", ",IF(A129 &lt;&gt; "", """mem"": bit" &amp; B129 &amp; "(" &amp; A129 &amp; "),", ""),"""good"": ",IF(A129 &lt;&gt; "", 1, 0),"},")</f>
-        <v>128: { "levelId": 3, "good": 0},</v>
+        <v>128: { "levelId": 6, "mem": bit5(0x224999),"good": 1},</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="B130" s="0" t="n">
+        <v>6</v>
+      </c>
       <c r="C130" s="4" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="D130" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C130, Levels!B:B, 0), 1, 1)),", ",IF(A130 &lt;&gt; "", """mem"": bit" &amp; B130 &amp; "(" &amp; A130 &amp; "),", ""),"""good"": ",IF(A130 &lt;&gt; "", 1, 0),"},")</f>
-        <v>129: { "levelId": 3, "good": 0},</v>
+        <v>129: { "levelId": 6, "mem": bit6(0x224999),"good": 1},</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="B131" s="0" t="n">
+        <v>7</v>
+      </c>
       <c r="C131" s="4" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="D131" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C131, Levels!B:B, 0), 1, 1)),", ",IF(A131 &lt;&gt; "", """mem"": bit" &amp; B131 &amp; "(" &amp; A131 &amp; "),", ""),"""good"": ",IF(A131 &lt;&gt; "", 1, 0),"},")</f>
-        <v>130: { "levelId": 3, "good": 0},</v>
+        <v>130: { "levelId": 6, "mem": bit7(0x224999),"good": 1},</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="B132" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="C132" s="4" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="D132" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C132, Levels!B:B, 0), 1, 1)),", ",IF(A132 &lt;&gt; "", """mem"": bit" &amp; B132 &amp; "(" &amp; A132 &amp; "),", ""),"""good"": ",IF(A132 &lt;&gt; "", 1, 0),"},")</f>
-        <v>131: { "levelId": 3, "good": 0},</v>
+        <v>131: { "levelId": 6, "mem": bit0(0x22499a),"good": 1},</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="B133" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="C133" s="4" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="D133" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C133, Levels!B:B, 0), 1, 1)),", ",IF(A133 &lt;&gt; "", """mem"": bit" &amp; B133 &amp; "(" &amp; A133 &amp; "),", ""),"""good"": ",IF(A133 &lt;&gt; "", 1, 0),"},")</f>
-        <v>132: { "levelId": 3, "good": 0},</v>
+        <v>132: { "levelId": 6, "mem": bit1(0x22499a),"good": 1},</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="B134" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="C134" s="4" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="D134" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C134, Levels!B:B, 0), 1, 1)),", ",IF(A134 &lt;&gt; "", """mem"": bit" &amp; B134 &amp; "(" &amp; A134 &amp; "),", ""),"""good"": ",IF(A134 &lt;&gt; "", 1, 0),"},")</f>
-        <v>133: { "levelId": 3, "good": 0},</v>
+        <v>133: { "levelId": 6, "mem": bit2(0x22499a),"good": 1},</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="B135" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="C135" s="4" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="D135" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C135, Levels!B:B, 0), 1, 1)),", ",IF(A135 &lt;&gt; "", """mem"": bit" &amp; B135 &amp; "(" &amp; A135 &amp; "),", ""),"""good"": ",IF(A135 &lt;&gt; "", 1, 0),"},")</f>
-        <v>134: { "levelId": 3, "good": 0},</v>
+        <v>134: { "levelId": 6, "mem": bit3(0x22499a),"good": 1},</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="B136" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="C136" s="4" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="D136" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C136, Levels!B:B, 0), 1, 1)),", ",IF(A136 &lt;&gt; "", """mem"": bit" &amp; B136 &amp; "(" &amp; A136 &amp; "),", ""),"""good"": ",IF(A136 &lt;&gt; "", 1, 0),"},")</f>
-        <v>135: { "levelId": 3, "good": 0},</v>
+        <v>135: { "levelId": 6, "mem": bit4(0x22499a),"good": 1},</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="B137" s="0" t="n">
+        <v>5</v>
+      </c>
       <c r="C137" s="4" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="D137" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C137, Levels!B:B, 0), 1, 1)),", ",IF(A137 &lt;&gt; "", """mem"": bit" &amp; B137 &amp; "(" &amp; A137 &amp; "),", ""),"""good"": ",IF(A137 &lt;&gt; "", 1, 0),"},")</f>
-        <v>136: { "levelId": 3, "good": 0},</v>
+        <v>136: { "levelId": 6, "mem": bit5(0x22499a),"good": 1},</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B138" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="C138" s="4" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D138" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C138, Levels!B:B, 0), 1, 1)),", ",IF(A138 &lt;&gt; "", """mem"": bit" &amp; B138 &amp; "(" &amp; A138 &amp; "),", ""),"""good"": ",IF(A138 &lt;&gt; "", 1, 0),"},")</f>
-        <v>137: { "levelId": 3, "good": 0},</v>
+        <v>137: { "levelId": 1, "mem": bit3(0x224a36),"good": 1},</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="B139" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="C139" s="4" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D139" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C139, Levels!B:B, 0), 1, 1)),", ",IF(A139 &lt;&gt; "", """mem"": bit" &amp; B139 &amp; "(" &amp; A139 &amp; "),", ""),"""good"": ",IF(A139 &lt;&gt; "", 1, 0),"},")</f>
-        <v>138: { "levelId": 3, "good": 0},</v>
+        <v>138: { "levelId": 1, "mem": bit4(0x224a36),"good": 1},</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="B140" s="0" t="n">
+        <v>5</v>
+      </c>
       <c r="C140" s="4" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D140" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C140, Levels!B:B, 0), 1, 1)),", ",IF(A140 &lt;&gt; "", """mem"": bit" &amp; B140 &amp; "(" &amp; A140 &amp; "),", ""),"""good"": ",IF(A140 &lt;&gt; "", 1, 0),"},")</f>
-        <v>139: { "levelId": 3, "good": 0},</v>
+        <v>139: { "levelId": 1, "mem": bit5(0x224a36),"good": 1},</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="B141" s="0" t="n">
+        <v>6</v>
+      </c>
       <c r="C141" s="4" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D141" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C141, Levels!B:B, 0), 1, 1)),", ",IF(A141 &lt;&gt; "", """mem"": bit" &amp; B141 &amp; "(" &amp; A141 &amp; "),", ""),"""good"": ",IF(A141 &lt;&gt; "", 1, 0),"},")</f>
-        <v>140: { "levelId": 3, "good": 0},</v>
+        <v>140: { "levelId": 1, "mem": bit6(0x224a36),"good": 1},</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="B142" s="0" t="n">
+        <v>7</v>
+      </c>
       <c r="C142" s="4" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D142" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C142, Levels!B:B, 0), 1, 1)),", ",IF(A142 &lt;&gt; "", """mem"": bit" &amp; B142 &amp; "(" &amp; A142 &amp; "),", ""),"""good"": ",IF(A142 &lt;&gt; "", 1, 0),"},")</f>
-        <v>141: { "levelId": 3, "good": 0},</v>
+        <v>141: { "levelId": 1, "mem": bit7(0x224a36),"good": 1},</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B143" s="0" t="n">
+        <v>7</v>
+      </c>
       <c r="C143" s="4" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="D143" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C143, Levels!B:B, 0), 1, 1)),", ",IF(A143 &lt;&gt; "", """mem"": bit" &amp; B143 &amp; "(" &amp; A143 &amp; "),", ""),"""good"": ",IF(A143 &lt;&gt; "", 1, 0),"},")</f>
-        <v>142: { "levelId": 3, "good": 0},</v>
+        <v>142: { "levelId": 6, "mem": bit7(0x224998),"good": 1},</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17164,26 +17432,26 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="B2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+      <selection pane="bottomLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="25.84"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>4</v>
@@ -17194,7 +17462,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>7</v>
@@ -17203,17 +17471,17 @@
         <v>19</v>
       </c>
       <c r="D2" s="0" t="str">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C2, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A2 &lt;&gt; "", "bit" &amp; B2 &amp; "(" &amp; A2 &amp; ")", ""),"},")</f>
-        <v>1: { "levelId": 1, "mem": bit7(0x2249f0)},</v>
-      </c>
-      <c r="G2" s="0" t="e">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C2, Levels!B:B, 0), 1, 1)),", ",IF(A2 &lt;&gt; "", """mem"": bit" &amp; B2 &amp; "(" &amp; A2 &amp; "),", ""),"""good"": ",IF(A2 &lt;&gt; "", 1, 0),"},")</f>
+        <v>1: { "levelId": 1, "mem": bit7(0x2249f0),"good": 1},</v>
+      </c>
+      <c r="G2" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D2:D81)</f>
-        <v>#N/A</v>
+        <v>1: { "levelId": 1, "mem": bit7(0x2249f0),"good": 1},2: { "levelId": 2, "mem": bit0(0x2249f1),"good": 1},3: { "levelId": 2, "mem": bit1(0x2249f1),"good": 1},4: { "levelId": 2, "mem": bit5(0x2249f1),"good": 1},5: { "levelId": 2, "mem": bit6(0x2249f1),"good": 1},6: { "levelId": 1, "mem": bit7(0x2249f1),"good": 1},7: { "levelId": 5, "mem": bit0(0x2249f2),"good": 1},8: { "levelId": 5, "mem": bit1(0x2249f2),"good": 1},9: { "levelId": 5, "mem": bit2(0x2249f2),"good": 1},10: { "levelId": 5, "mem": bit3(0x2249f2),"good": 1},11: { "levelId": 5, "mem": bit4(0x2249f2),"good": 1},12: { "levelId": 6, "mem": bit5(0x2249f2),"good": 1},13: { "levelId": 6, "mem": bit7(0x2249f2),"good": 1},14: { "levelId": 6, "mem": bit1(0x2249f3),"good": 1},15: { "levelId": 6, "mem": bit6(0x2249f2),"good": 1},16: { "levelId": 6, "mem": bit0(0x2249f3),"good": 1},17: { "levelId": 6, "mem": bit3(0x2249f3),"good": 1},18: { "levelId": 6, "mem": bit2(0x2249f3),"good": 1},19: { "levelId": 3, "good": 0},20: { "levelId": 3, "good": 0},21: { "levelId": 3, "good": 0},22: { "levelId": 3, "good": 0},23: { "levelId": 3, "good": 0},24: { "levelId": 3, "good": 0},25: { "levelId": 3, "good": 0},26: { "levelId": 3, "good": 0},27: { "levelId": 3, "good": 0},28: { "levelId": 3, "good": 0},29: { "levelId": 3, "good": 0},30: { "levelId": 3, "good": 0},31: { "levelId": 3, "good": 0},32: { "levelId": 3, "good": 0},33: { "levelId": 3, "good": 0},34: { "levelId": 3, "good": 0},35: { "levelId": 3, "good": 0},36: { "levelId": 3, "good": 0},37: { "levelId": 3, "good": 0},38: { "levelId": 3, "good": 0},39: { "levelId": 3, "good": 0},40: { "levelId": 3, "good": 0},41: { "levelId": 3, "good": 0},42: { "levelId": 3, "good": 0},43: { "levelId": 3, "good": 0},44: { "levelId": 3, "good": 0},45: { "levelId": 3, "good": 0},46: { "levelId": 3, "good": 0},47: { "levelId": 3, "good": 0},48: { "levelId": 3, "good": 0},49: { "levelId": 3, "good": 0},50: { "levelId": 3, "good": 0},51: { "levelId": 3, "good": 0},52: { "levelId": 3, "good": 0},53: { "levelId": 3, "good": 0},54: { "levelId": 3, "good": 0},55: { "levelId": 3, "good": 0},56: { "levelId": 3, "good": 0},57: { "levelId": 3, "good": 0},58: { "levelId": 3, "good": 0},59: { "levelId": 3, "good": 0},60: { "levelId": 3, "good": 0},61: { "levelId": 3, "good": 0},62: { "levelId": 3, "good": 0},63: { "levelId": 3, "good": 0},64: { "levelId": 3, "good": 0},65: { "levelId": 3, "good": 0},66: { "levelId": 3, "good": 0},67: { "levelId": 3, "good": 0},68: { "levelId": 3, "good": 0},69: { "levelId": 3, "good": 0},70: { "levelId": 3, "good": 0},71: { "levelId": 3, "good": 0},72: { "levelId": 3, "good": 0},73: { "levelId": 3, "good": 0},74: { "levelId": 3, "good": 0},75: { "levelId": 3, "good": 0},76: { "levelId": 3, "good": 0},77: { "levelId": 3, "good": 0},78: { "levelId": 3, "good": 0},79: { "levelId": 3, "good": 0},80: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
-        <v>76</v>
+      <c r="A3" s="6" t="s">
+        <v>81</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0</v>
@@ -17222,13 +17490,13 @@
         <v>27</v>
       </c>
       <c r="D3" s="0" t="str">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C3, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A3 &lt;&gt; "", "bit" &amp; B3 &amp; "(" &amp; A3 &amp; ")", ""),"},")</f>
-        <v>2: { "levelId": 2, "mem": bit0(0x2249f1)},</v>
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C3, Levels!B:B, 0), 1, 1)),", ",IF(A3 &lt;&gt; "", """mem"": bit" &amp; B3 &amp; "(" &amp; A3 &amp; "),", ""),"""good"": ",IF(A3 &lt;&gt; "", 1, 0),"},")</f>
+        <v>2: { "levelId": 2, "mem": bit0(0x2249f1),"good": 1},</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
-        <v>76</v>
+      <c r="A4" s="6" t="s">
+        <v>81</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>1</v>
@@ -17237,13 +17505,13 @@
         <v>27</v>
       </c>
       <c r="D4" s="0" t="str">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C4, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A4 &lt;&gt; "", "bit" &amp; B4 &amp; "(" &amp; A4 &amp; ")", ""),"},")</f>
-        <v>3: { "levelId": 2, "mem": bit1(0x2249f1)},</v>
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C4, Levels!B:B, 0), 1, 1)),", ",IF(A4 &lt;&gt; "", """mem"": bit" &amp; B4 &amp; "(" &amp; A4 &amp; "),", ""),"""good"": ",IF(A4 &lt;&gt; "", 1, 0),"},")</f>
+        <v>3: { "levelId": 2, "mem": bit1(0x2249f1),"good": 1},</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
-        <v>76</v>
+      <c r="A5" s="6" t="s">
+        <v>81</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>5</v>
@@ -17252,13 +17520,13 @@
         <v>27</v>
       </c>
       <c r="D5" s="0" t="str">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C5, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A5 &lt;&gt; "", "bit" &amp; B5 &amp; "(" &amp; A5 &amp; ")", ""),"},")</f>
-        <v>4: { "levelId": 2, "mem": bit5(0x2249f1)},</v>
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C5, Levels!B:B, 0), 1, 1)),", ",IF(A5 &lt;&gt; "", """mem"": bit" &amp; B5 &amp; "(" &amp; A5 &amp; "),", ""),"""good"": ",IF(A5 &lt;&gt; "", 1, 0),"},")</f>
+        <v>4: { "levelId": 2, "mem": bit5(0x2249f1),"good": 1},</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
-        <v>76</v>
+      <c r="A6" s="6" t="s">
+        <v>81</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>6</v>
@@ -17267,13 +17535,13 @@
         <v>27</v>
       </c>
       <c r="D6" s="0" t="str">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C6, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A6 &lt;&gt; "", "bit" &amp; B6 &amp; "(" &amp; A6 &amp; ")", ""),"},")</f>
-        <v>5: { "levelId": 2, "mem": bit6(0x2249f1)},</v>
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C6, Levels!B:B, 0), 1, 1)),", ",IF(A6 &lt;&gt; "", """mem"": bit" &amp; B6 &amp; "(" &amp; A6 &amp; "),", ""),"""good"": ",IF(A6 &lt;&gt; "", 1, 0),"},")</f>
+        <v>5: { "levelId": 2, "mem": bit6(0x2249f1),"good": 1},</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
-        <v>76</v>
+      <c r="A7" s="6" t="s">
+        <v>81</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>7</v>
@@ -17282,13 +17550,13 @@
         <v>19</v>
       </c>
       <c r="D7" s="0" t="str">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C7, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A7 &lt;&gt; "", "bit" &amp; B7 &amp; "(" &amp; A7 &amp; ")", ""),"},")</f>
-        <v>6: { "levelId": 1, "mem": bit7(0x2249f1)},</v>
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C7, Levels!B:B, 0), 1, 1)),", ",IF(A7 &lt;&gt; "", """mem"": bit" &amp; B7 &amp; "(" &amp; A7 &amp; "),", ""),"""good"": ",IF(A7 &lt;&gt; "", 1, 0),"},")</f>
+        <v>6: { "levelId": 1, "mem": bit7(0x2249f1),"good": 1},</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>0</v>
@@ -17297,13 +17565,13 @@
         <v>42</v>
       </c>
       <c r="D8" s="0" t="str">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C8, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A8 &lt;&gt; "", "bit" &amp; B8 &amp; "(" &amp; A8 &amp; ")", ""),"},")</f>
-        <v>7: { "levelId": 5, "mem": bit0(0x2249f2)},</v>
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C8, Levels!B:B, 0), 1, 1)),", ",IF(A8 &lt;&gt; "", """mem"": bit" &amp; B8 &amp; "(" &amp; A8 &amp; "),", ""),"""good"": ",IF(A8 &lt;&gt; "", 1, 0),"},")</f>
+        <v>7: { "levelId": 5, "mem": bit0(0x2249f2),"good": 1},</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>1</v>
@@ -17312,13 +17580,13 @@
         <v>42</v>
       </c>
       <c r="D9" s="0" t="str">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C9, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A9 &lt;&gt; "", "bit" &amp; B9 &amp; "(" &amp; A9 &amp; ")", ""),"},")</f>
-        <v>8: { "levelId": 5, "mem": bit1(0x2249f2)},</v>
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C9, Levels!B:B, 0), 1, 1)),", ",IF(A9 &lt;&gt; "", """mem"": bit" &amp; B9 &amp; "(" &amp; A9 &amp; "),", ""),"""good"": ",IF(A9 &lt;&gt; "", 1, 0),"},")</f>
+        <v>8: { "levelId": 5, "mem": bit1(0x2249f2),"good": 1},</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>2</v>
@@ -17327,13 +17595,13 @@
         <v>42</v>
       </c>
       <c r="D10" s="0" t="str">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C10, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A10 &lt;&gt; "", "bit" &amp; B10 &amp; "(" &amp; A10 &amp; ")", ""),"},")</f>
-        <v>9: { "levelId": 5, "mem": bit2(0x2249f2)},</v>
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C10, Levels!B:B, 0), 1, 1)),", ",IF(A10 &lt;&gt; "", """mem"": bit" &amp; B10 &amp; "(" &amp; A10 &amp; "),", ""),"""good"": ",IF(A10 &lt;&gt; "", 1, 0),"},")</f>
+        <v>9: { "levelId": 5, "mem": bit2(0x2249f2),"good": 1},</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>3</v>
@@ -17342,13 +17610,13 @@
         <v>42</v>
       </c>
       <c r="D11" s="0" t="str">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C11, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A11 &lt;&gt; "", "bit" &amp; B11 &amp; "(" &amp; A11 &amp; ")", ""),"},")</f>
-        <v>10: { "levelId": 5, "mem": bit3(0x2249f2)},</v>
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C11, Levels!B:B, 0), 1, 1)),", ",IF(A11 &lt;&gt; "", """mem"": bit" &amp; B11 &amp; "(" &amp; A11 &amp; "),", ""),"""good"": ",IF(A11 &lt;&gt; "", 1, 0),"},")</f>
+        <v>10: { "levelId": 5, "mem": bit3(0x2249f2),"good": 1},</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>4</v>
@@ -17357,13 +17625,13 @@
         <v>42</v>
       </c>
       <c r="D12" s="0" t="str">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C12, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A12 &lt;&gt; "", "bit" &amp; B12 &amp; "(" &amp; A12 &amp; ")", ""),"},")</f>
-        <v>11: { "levelId": 5, "mem": bit4(0x2249f2)},</v>
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C12, Levels!B:B, 0), 1, 1)),", ",IF(A12 &lt;&gt; "", """mem"": bit" &amp; B12 &amp; "(" &amp; A12 &amp; "),", ""),"""good"": ",IF(A12 &lt;&gt; "", 1, 0),"},")</f>
+        <v>11: { "levelId": 5, "mem": bit4(0x2249f2),"good": 1},</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>5</v>
@@ -17372,13 +17640,13 @@
         <v>48</v>
       </c>
       <c r="D13" s="0" t="str">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C13, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A13 &lt;&gt; "", "bit" &amp; B13 &amp; "(" &amp; A13 &amp; ")", ""),"},")</f>
-        <v>12: { "levelId": 6, "mem": bit5(0x2249f2)},</v>
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C13, Levels!B:B, 0), 1, 1)),", ",IF(A13 &lt;&gt; "", """mem"": bit" &amp; B13 &amp; "(" &amp; A13 &amp; "),", ""),"""good"": ",IF(A13 &lt;&gt; "", 1, 0),"},")</f>
+        <v>12: { "levelId": 6, "mem": bit5(0x2249f2),"good": 1},</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>7</v>
@@ -17387,477 +17655,641 @@
         <v>48</v>
       </c>
       <c r="D14" s="0" t="str">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C14, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A14 &lt;&gt; "", "bit" &amp; B14 &amp; "(" &amp; A14 &amp; ")", ""),"},")</f>
-        <v>13: { "levelId": 6, "mem": bit7(0x2249f2)},</v>
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C14, Levels!B:B, 0), 1, 1)),", ",IF(A14 &lt;&gt; "", """mem"": bit" &amp; B14 &amp; "(" &amp; A14 &amp; "),", ""),"""good"": ",IF(A14 &lt;&gt; "", 1, 0),"},")</f>
+        <v>13: { "levelId": 6, "mem": bit7(0x2249f2),"good": 1},</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C15" s="4"/>
-      <c r="D15" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C15, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A15 &lt;&gt; "", "bit" &amp; B15 &amp; "(" &amp; A15 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="A15" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C15, Levels!B:B, 0), 1, 1)),", ",IF(A15 &lt;&gt; "", """mem"": bit" &amp; B15 &amp; "(" &amp; A15 &amp; "),", ""),"""good"": ",IF(A15 &lt;&gt; "", 1, 0),"},")</f>
+        <v>14: { "levelId": 6, "mem": bit1(0x2249f3),"good": 1},</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C16" s="4"/>
-      <c r="D16" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C16, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A16 &lt;&gt; "", "bit" &amp; B16 &amp; "(" &amp; A16 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="A16" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C16, Levels!B:B, 0), 1, 1)),", ",IF(A16 &lt;&gt; "", """mem"": bit" &amp; B16 &amp; "(" &amp; A16 &amp; "),", ""),"""good"": ",IF(A16 &lt;&gt; "", 1, 0),"},")</f>
+        <v>15: { "levelId": 6, "mem": bit6(0x2249f2),"good": 1},</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="4"/>
-      <c r="D17" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C17, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A17 &lt;&gt; "", "bit" &amp; B17 &amp; "(" &amp; A17 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="A17" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C17, Levels!B:B, 0), 1, 1)),", ",IF(A17 &lt;&gt; "", """mem"": bit" &amp; B17 &amp; "(" &amp; A17 &amp; "),", ""),"""good"": ",IF(A17 &lt;&gt; "", 1, 0),"},")</f>
+        <v>16: { "levelId": 6, "mem": bit0(0x2249f3),"good": 1},</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="4"/>
-      <c r="D18" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C18, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A18 &lt;&gt; "", "bit" &amp; B18 &amp; "(" &amp; A18 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="A18" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C18, Levels!B:B, 0), 1, 1)),", ",IF(A18 &lt;&gt; "", """mem"": bit" &amp; B18 &amp; "(" &amp; A18 &amp; "),", ""),"""good"": ",IF(A18 &lt;&gt; "", 1, 0),"},")</f>
+        <v>17: { "levelId": 6, "mem": bit3(0x2249f3),"good": 1},</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C19" s="4"/>
-      <c r="D19" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C19, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A19 &lt;&gt; "", "bit" &amp; B19 &amp; "(" &amp; A19 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="A19" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C19, Levels!B:B, 0), 1, 1)),", ",IF(A19 &lt;&gt; "", """mem"": bit" &amp; B19 &amp; "(" &amp; A19 &amp; "),", ""),"""good"": ",IF(A19 &lt;&gt; "", 1, 0),"},")</f>
+        <v>18: { "levelId": 6, "mem": bit2(0x2249f3),"good": 1},</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C20" s="4"/>
-      <c r="D20" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C20, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A20 &lt;&gt; "", "bit" &amp; B20 &amp; "(" &amp; A20 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="C20" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C20, Levels!B:B, 0), 1, 1)),", ",IF(A20 &lt;&gt; "", """mem"": bit" &amp; B20 &amp; "(" &amp; A20 &amp; "),", ""),"""good"": ",IF(A20 &lt;&gt; "", 1, 0),"},")</f>
+        <v>19: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C21" s="4"/>
-      <c r="D21" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C21, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A21 &lt;&gt; "", "bit" &amp; B21 &amp; "(" &amp; A21 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="C21" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C21, Levels!B:B, 0), 1, 1)),", ",IF(A21 &lt;&gt; "", """mem"": bit" &amp; B21 &amp; "(" &amp; A21 &amp; "),", ""),"""good"": ",IF(A21 &lt;&gt; "", 1, 0),"},")</f>
+        <v>20: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C22" s="4"/>
-      <c r="D22" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C22, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A22 &lt;&gt; "", "bit" &amp; B22 &amp; "(" &amp; A22 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="C22" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C22, Levels!B:B, 0), 1, 1)),", ",IF(A22 &lt;&gt; "", """mem"": bit" &amp; B22 &amp; "(" &amp; A22 &amp; "),", ""),"""good"": ",IF(A22 &lt;&gt; "", 1, 0),"},")</f>
+        <v>21: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C23" s="4"/>
-      <c r="D23" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C23, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A23 &lt;&gt; "", "bit" &amp; B23 &amp; "(" &amp; A23 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="C23" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C23, Levels!B:B, 0), 1, 1)),", ",IF(A23 &lt;&gt; "", """mem"": bit" &amp; B23 &amp; "(" &amp; A23 &amp; "),", ""),"""good"": ",IF(A23 &lt;&gt; "", 1, 0),"},")</f>
+        <v>22: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C24" s="4"/>
-      <c r="D24" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C24, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A24 &lt;&gt; "", "bit" &amp; B24 &amp; "(" &amp; A24 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="C24" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C24, Levels!B:B, 0), 1, 1)),", ",IF(A24 &lt;&gt; "", """mem"": bit" &amp; B24 &amp; "(" &amp; A24 &amp; "),", ""),"""good"": ",IF(A24 &lt;&gt; "", 1, 0),"},")</f>
+        <v>23: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C25" s="4"/>
-      <c r="D25" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C25, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A25 &lt;&gt; "", "bit" &amp; B25 &amp; "(" &amp; A25 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="C25" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C25, Levels!B:B, 0), 1, 1)),", ",IF(A25 &lt;&gt; "", """mem"": bit" &amp; B25 &amp; "(" &amp; A25 &amp; "),", ""),"""good"": ",IF(A25 &lt;&gt; "", 1, 0),"},")</f>
+        <v>24: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C26" s="4"/>
-      <c r="D26" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C26, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A26 &lt;&gt; "", "bit" &amp; B26 &amp; "(" &amp; A26 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="C26" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C26, Levels!B:B, 0), 1, 1)),", ",IF(A26 &lt;&gt; "", """mem"": bit" &amp; B26 &amp; "(" &amp; A26 &amp; "),", ""),"""good"": ",IF(A26 &lt;&gt; "", 1, 0),"},")</f>
+        <v>25: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C27" s="4"/>
-      <c r="D27" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C27, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A27 &lt;&gt; "", "bit" &amp; B27 &amp; "(" &amp; A27 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="C27" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C27, Levels!B:B, 0), 1, 1)),", ",IF(A27 &lt;&gt; "", """mem"": bit" &amp; B27 &amp; "(" &amp; A27 &amp; "),", ""),"""good"": ",IF(A27 &lt;&gt; "", 1, 0),"},")</f>
+        <v>26: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C28" s="4"/>
-      <c r="D28" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C28, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A28 &lt;&gt; "", "bit" &amp; B28 &amp; "(" &amp; A28 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="C28" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C28, Levels!B:B, 0), 1, 1)),", ",IF(A28 &lt;&gt; "", """mem"": bit" &amp; B28 &amp; "(" &amp; A28 &amp; "),", ""),"""good"": ",IF(A28 &lt;&gt; "", 1, 0),"},")</f>
+        <v>27: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C29" s="4"/>
-      <c r="D29" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C29, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A29 &lt;&gt; "", "bit" &amp; B29 &amp; "(" &amp; A29 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="C29" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C29, Levels!B:B, 0), 1, 1)),", ",IF(A29 &lt;&gt; "", """mem"": bit" &amp; B29 &amp; "(" &amp; A29 &amp; "),", ""),"""good"": ",IF(A29 &lt;&gt; "", 1, 0),"},")</f>
+        <v>28: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C30" s="4"/>
-      <c r="D30" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C30, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A30 &lt;&gt; "", "bit" &amp; B30 &amp; "(" &amp; A30 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="C30" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D30" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C30, Levels!B:B, 0), 1, 1)),", ",IF(A30 &lt;&gt; "", """mem"": bit" &amp; B30 &amp; "(" &amp; A30 &amp; "),", ""),"""good"": ",IF(A30 &lt;&gt; "", 1, 0),"},")</f>
+        <v>29: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C31" s="4"/>
-      <c r="D31" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C31, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A31 &lt;&gt; "", "bit" &amp; B31 &amp; "(" &amp; A31 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="C31" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D31" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C31, Levels!B:B, 0), 1, 1)),", ",IF(A31 &lt;&gt; "", """mem"": bit" &amp; B31 &amp; "(" &amp; A31 &amp; "),", ""),"""good"": ",IF(A31 &lt;&gt; "", 1, 0),"},")</f>
+        <v>30: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C32" s="4"/>
-      <c r="D32" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C32, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A32 &lt;&gt; "", "bit" &amp; B32 &amp; "(" &amp; A32 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="C32" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D32" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C32, Levels!B:B, 0), 1, 1)),", ",IF(A32 &lt;&gt; "", """mem"": bit" &amp; B32 &amp; "(" &amp; A32 &amp; "),", ""),"""good"": ",IF(A32 &lt;&gt; "", 1, 0),"},")</f>
+        <v>31: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C33" s="4"/>
-      <c r="D33" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C33, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A33 &lt;&gt; "", "bit" &amp; B33 &amp; "(" &amp; A33 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="C33" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D33" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C33, Levels!B:B, 0), 1, 1)),", ",IF(A33 &lt;&gt; "", """mem"": bit" &amp; B33 &amp; "(" &amp; A33 &amp; "),", ""),"""good"": ",IF(A33 &lt;&gt; "", 1, 0),"},")</f>
+        <v>32: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C34" s="4"/>
-      <c r="D34" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C34, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A34 &lt;&gt; "", "bit" &amp; B34 &amp; "(" &amp; A34 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="C34" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D34" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C34, Levels!B:B, 0), 1, 1)),", ",IF(A34 &lt;&gt; "", """mem"": bit" &amp; B34 &amp; "(" &amp; A34 &amp; "),", ""),"""good"": ",IF(A34 &lt;&gt; "", 1, 0),"},")</f>
+        <v>33: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C35" s="4"/>
-      <c r="D35" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C35, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A35 &lt;&gt; "", "bit" &amp; B35 &amp; "(" &amp; A35 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="C35" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D35" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C35, Levels!B:B, 0), 1, 1)),", ",IF(A35 &lt;&gt; "", """mem"": bit" &amp; B35 &amp; "(" &amp; A35 &amp; "),", ""),"""good"": ",IF(A35 &lt;&gt; "", 1, 0),"},")</f>
+        <v>34: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C36" s="4"/>
-      <c r="D36" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C36, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A36 &lt;&gt; "", "bit" &amp; B36 &amp; "(" &amp; A36 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="C36" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D36" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C36, Levels!B:B, 0), 1, 1)),", ",IF(A36 &lt;&gt; "", """mem"": bit" &amp; B36 &amp; "(" &amp; A36 &amp; "),", ""),"""good"": ",IF(A36 &lt;&gt; "", 1, 0),"},")</f>
+        <v>35: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C37" s="4"/>
-      <c r="D37" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C37, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A37 &lt;&gt; "", "bit" &amp; B37 &amp; "(" &amp; A37 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="C37" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D37" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C37, Levels!B:B, 0), 1, 1)),", ",IF(A37 &lt;&gt; "", """mem"": bit" &amp; B37 &amp; "(" &amp; A37 &amp; "),", ""),"""good"": ",IF(A37 &lt;&gt; "", 1, 0),"},")</f>
+        <v>36: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C38" s="4"/>
-      <c r="D38" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C38, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A38 &lt;&gt; "", "bit" &amp; B38 &amp; "(" &amp; A38 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="C38" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D38" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C38, Levels!B:B, 0), 1, 1)),", ",IF(A38 &lt;&gt; "", """mem"": bit" &amp; B38 &amp; "(" &amp; A38 &amp; "),", ""),"""good"": ",IF(A38 &lt;&gt; "", 1, 0),"},")</f>
+        <v>37: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C39" s="4"/>
-      <c r="D39" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C39, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A39 &lt;&gt; "", "bit" &amp; B39 &amp; "(" &amp; A39 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="C39" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D39" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C39, Levels!B:B, 0), 1, 1)),", ",IF(A39 &lt;&gt; "", """mem"": bit" &amp; B39 &amp; "(" &amp; A39 &amp; "),", ""),"""good"": ",IF(A39 &lt;&gt; "", 1, 0),"},")</f>
+        <v>38: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C40" s="4"/>
-      <c r="D40" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C40, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A40 &lt;&gt; "", "bit" &amp; B40 &amp; "(" &amp; A40 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="C40" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D40" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C40, Levels!B:B, 0), 1, 1)),", ",IF(A40 &lt;&gt; "", """mem"": bit" &amp; B40 &amp; "(" &amp; A40 &amp; "),", ""),"""good"": ",IF(A40 &lt;&gt; "", 1, 0),"},")</f>
+        <v>39: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C41" s="4"/>
-      <c r="D41" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C41, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A41 &lt;&gt; "", "bit" &amp; B41 &amp; "(" &amp; A41 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="C41" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D41" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C41, Levels!B:B, 0), 1, 1)),", ",IF(A41 &lt;&gt; "", """mem"": bit" &amp; B41 &amp; "(" &amp; A41 &amp; "),", ""),"""good"": ",IF(A41 &lt;&gt; "", 1, 0),"},")</f>
+        <v>40: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C42" s="4"/>
-      <c r="D42" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C42, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A42 &lt;&gt; "", "bit" &amp; B42 &amp; "(" &amp; A42 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="C42" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D42" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C42, Levels!B:B, 0), 1, 1)),", ",IF(A42 &lt;&gt; "", """mem"": bit" &amp; B42 &amp; "(" &amp; A42 &amp; "),", ""),"""good"": ",IF(A42 &lt;&gt; "", 1, 0),"},")</f>
+        <v>41: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C43" s="4"/>
-      <c r="D43" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C43, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A43 &lt;&gt; "", "bit" &amp; B43 &amp; "(" &amp; A43 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="C43" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D43" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C43, Levels!B:B, 0), 1, 1)),", ",IF(A43 &lt;&gt; "", """mem"": bit" &amp; B43 &amp; "(" &amp; A43 &amp; "),", ""),"""good"": ",IF(A43 &lt;&gt; "", 1, 0),"},")</f>
+        <v>42: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C44" s="4"/>
-      <c r="D44" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C44, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A44 &lt;&gt; "", "bit" &amp; B44 &amp; "(" &amp; A44 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="C44" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D44" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C44, Levels!B:B, 0), 1, 1)),", ",IF(A44 &lt;&gt; "", """mem"": bit" &amp; B44 &amp; "(" &amp; A44 &amp; "),", ""),"""good"": ",IF(A44 &lt;&gt; "", 1, 0),"},")</f>
+        <v>43: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C45" s="4"/>
-      <c r="D45" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C45, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A45 &lt;&gt; "", "bit" &amp; B45 &amp; "(" &amp; A45 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="C45" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D45" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C45, Levels!B:B, 0), 1, 1)),", ",IF(A45 &lt;&gt; "", """mem"": bit" &amp; B45 &amp; "(" &amp; A45 &amp; "),", ""),"""good"": ",IF(A45 &lt;&gt; "", 1, 0),"},")</f>
+        <v>44: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C46" s="4"/>
-      <c r="D46" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C46, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A46 &lt;&gt; "", "bit" &amp; B46 &amp; "(" &amp; A46 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="C46" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D46" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C46, Levels!B:B, 0), 1, 1)),", ",IF(A46 &lt;&gt; "", """mem"": bit" &amp; B46 &amp; "(" &amp; A46 &amp; "),", ""),"""good"": ",IF(A46 &lt;&gt; "", 1, 0),"},")</f>
+        <v>45: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C47" s="4"/>
-      <c r="D47" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C47, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A47 &lt;&gt; "", "bit" &amp; B47 &amp; "(" &amp; A47 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="C47" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D47" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C47, Levels!B:B, 0), 1, 1)),", ",IF(A47 &lt;&gt; "", """mem"": bit" &amp; B47 &amp; "(" &amp; A47 &amp; "),", ""),"""good"": ",IF(A47 &lt;&gt; "", 1, 0),"},")</f>
+        <v>46: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C48" s="4"/>
-      <c r="D48" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C48, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A48 &lt;&gt; "", "bit" &amp; B48 &amp; "(" &amp; A48 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="C48" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D48" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C48, Levels!B:B, 0), 1, 1)),", ",IF(A48 &lt;&gt; "", """mem"": bit" &amp; B48 &amp; "(" &amp; A48 &amp; "),", ""),"""good"": ",IF(A48 &lt;&gt; "", 1, 0),"},")</f>
+        <v>47: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C49" s="4"/>
-      <c r="D49" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C49, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A49 &lt;&gt; "", "bit" &amp; B49 &amp; "(" &amp; A49 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="C49" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D49" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C49, Levels!B:B, 0), 1, 1)),", ",IF(A49 &lt;&gt; "", """mem"": bit" &amp; B49 &amp; "(" &amp; A49 &amp; "),", ""),"""good"": ",IF(A49 &lt;&gt; "", 1, 0),"},")</f>
+        <v>48: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C50" s="4"/>
-      <c r="D50" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C50, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A50 &lt;&gt; "", "bit" &amp; B50 &amp; "(" &amp; A50 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="C50" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D50" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C50, Levels!B:B, 0), 1, 1)),", ",IF(A50 &lt;&gt; "", """mem"": bit" &amp; B50 &amp; "(" &amp; A50 &amp; "),", ""),"""good"": ",IF(A50 &lt;&gt; "", 1, 0),"},")</f>
+        <v>49: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C51" s="4"/>
-      <c r="D51" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C51, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A51 &lt;&gt; "", "bit" &amp; B51 &amp; "(" &amp; A51 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="C51" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D51" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C51, Levels!B:B, 0), 1, 1)),", ",IF(A51 &lt;&gt; "", """mem"": bit" &amp; B51 &amp; "(" &amp; A51 &amp; "),", ""),"""good"": ",IF(A51 &lt;&gt; "", 1, 0),"},")</f>
+        <v>50: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C52" s="4"/>
-      <c r="D52" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C52, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A52 &lt;&gt; "", "bit" &amp; B52 &amp; "(" &amp; A52 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="C52" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D52" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C52, Levels!B:B, 0), 1, 1)),", ",IF(A52 &lt;&gt; "", """mem"": bit" &amp; B52 &amp; "(" &amp; A52 &amp; "),", ""),"""good"": ",IF(A52 &lt;&gt; "", 1, 0),"},")</f>
+        <v>51: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C53" s="4"/>
-      <c r="D53" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C53, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A53 &lt;&gt; "", "bit" &amp; B53 &amp; "(" &amp; A53 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="C53" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D53" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C53, Levels!B:B, 0), 1, 1)),", ",IF(A53 &lt;&gt; "", """mem"": bit" &amp; B53 &amp; "(" &amp; A53 &amp; "),", ""),"""good"": ",IF(A53 &lt;&gt; "", 1, 0),"},")</f>
+        <v>52: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C54" s="4"/>
-      <c r="D54" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C54, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A54 &lt;&gt; "", "bit" &amp; B54 &amp; "(" &amp; A54 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="C54" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D54" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C54, Levels!B:B, 0), 1, 1)),", ",IF(A54 &lt;&gt; "", """mem"": bit" &amp; B54 &amp; "(" &amp; A54 &amp; "),", ""),"""good"": ",IF(A54 &lt;&gt; "", 1, 0),"},")</f>
+        <v>53: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C55" s="4"/>
-      <c r="D55" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C55, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A55 &lt;&gt; "", "bit" &amp; B55 &amp; "(" &amp; A55 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="C55" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D55" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C55, Levels!B:B, 0), 1, 1)),", ",IF(A55 &lt;&gt; "", """mem"": bit" &amp; B55 &amp; "(" &amp; A55 &amp; "),", ""),"""good"": ",IF(A55 &lt;&gt; "", 1, 0),"},")</f>
+        <v>54: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C56" s="4"/>
-      <c r="D56" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C56, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A56 &lt;&gt; "", "bit" &amp; B56 &amp; "(" &amp; A56 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="C56" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D56" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C56, Levels!B:B, 0), 1, 1)),", ",IF(A56 &lt;&gt; "", """mem"": bit" &amp; B56 &amp; "(" &amp; A56 &amp; "),", ""),"""good"": ",IF(A56 &lt;&gt; "", 1, 0),"},")</f>
+        <v>55: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C57" s="4"/>
-      <c r="D57" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C57, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A57 &lt;&gt; "", "bit" &amp; B57 &amp; "(" &amp; A57 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="C57" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D57" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C57, Levels!B:B, 0), 1, 1)),", ",IF(A57 &lt;&gt; "", """mem"": bit" &amp; B57 &amp; "(" &amp; A57 &amp; "),", ""),"""good"": ",IF(A57 &lt;&gt; "", 1, 0),"},")</f>
+        <v>56: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C58" s="4"/>
-      <c r="D58" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C58, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A58 &lt;&gt; "", "bit" &amp; B58 &amp; "(" &amp; A58 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="C58" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D58" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C58, Levels!B:B, 0), 1, 1)),", ",IF(A58 &lt;&gt; "", """mem"": bit" &amp; B58 &amp; "(" &amp; A58 &amp; "),", ""),"""good"": ",IF(A58 &lt;&gt; "", 1, 0),"},")</f>
+        <v>57: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C59" s="4"/>
-      <c r="D59" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C59, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A59 &lt;&gt; "", "bit" &amp; B59 &amp; "(" &amp; A59 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="C59" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D59" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C59, Levels!B:B, 0), 1, 1)),", ",IF(A59 &lt;&gt; "", """mem"": bit" &amp; B59 &amp; "(" &amp; A59 &amp; "),", ""),"""good"": ",IF(A59 &lt;&gt; "", 1, 0),"},")</f>
+        <v>58: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C60" s="4"/>
-      <c r="D60" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C60, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A60 &lt;&gt; "", "bit" &amp; B60 &amp; "(" &amp; A60 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="C60" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D60" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C60, Levels!B:B, 0), 1, 1)),", ",IF(A60 &lt;&gt; "", """mem"": bit" &amp; B60 &amp; "(" &amp; A60 &amp; "),", ""),"""good"": ",IF(A60 &lt;&gt; "", 1, 0),"},")</f>
+        <v>59: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C61" s="4"/>
-      <c r="D61" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C61, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A61 &lt;&gt; "", "bit" &amp; B61 &amp; "(" &amp; A61 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="C61" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D61" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C61, Levels!B:B, 0), 1, 1)),", ",IF(A61 &lt;&gt; "", """mem"": bit" &amp; B61 &amp; "(" &amp; A61 &amp; "),", ""),"""good"": ",IF(A61 &lt;&gt; "", 1, 0),"},")</f>
+        <v>60: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C62" s="4"/>
-      <c r="D62" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C62, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A62 &lt;&gt; "", "bit" &amp; B62 &amp; "(" &amp; A62 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="C62" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D62" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C62, Levels!B:B, 0), 1, 1)),", ",IF(A62 &lt;&gt; "", """mem"": bit" &amp; B62 &amp; "(" &amp; A62 &amp; "),", ""),"""good"": ",IF(A62 &lt;&gt; "", 1, 0),"},")</f>
+        <v>61: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C63" s="4"/>
-      <c r="D63" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C63, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A63 &lt;&gt; "", "bit" &amp; B63 &amp; "(" &amp; A63 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="C63" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D63" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C63, Levels!B:B, 0), 1, 1)),", ",IF(A63 &lt;&gt; "", """mem"": bit" &amp; B63 &amp; "(" &amp; A63 &amp; "),", ""),"""good"": ",IF(A63 &lt;&gt; "", 1, 0),"},")</f>
+        <v>62: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C64" s="4"/>
-      <c r="D64" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C64, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A64 &lt;&gt; "", "bit" &amp; B64 &amp; "(" &amp; A64 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="C64" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D64" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C64, Levels!B:B, 0), 1, 1)),", ",IF(A64 &lt;&gt; "", """mem"": bit" &amp; B64 &amp; "(" &amp; A64 &amp; "),", ""),"""good"": ",IF(A64 &lt;&gt; "", 1, 0),"},")</f>
+        <v>63: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C65" s="4"/>
-      <c r="D65" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C65, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A65 &lt;&gt; "", "bit" &amp; B65 &amp; "(" &amp; A65 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="C65" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D65" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C65, Levels!B:B, 0), 1, 1)),", ",IF(A65 &lt;&gt; "", """mem"": bit" &amp; B65 &amp; "(" &amp; A65 &amp; "),", ""),"""good"": ",IF(A65 &lt;&gt; "", 1, 0),"},")</f>
+        <v>64: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C66" s="4"/>
-      <c r="D66" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C66, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A66 &lt;&gt; "", "bit" &amp; B66 &amp; "(" &amp; A66 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="C66" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D66" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C66, Levels!B:B, 0), 1, 1)),", ",IF(A66 &lt;&gt; "", """mem"": bit" &amp; B66 &amp; "(" &amp; A66 &amp; "),", ""),"""good"": ",IF(A66 &lt;&gt; "", 1, 0),"},")</f>
+        <v>65: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C67" s="4"/>
-      <c r="D67" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C67, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A67 &lt;&gt; "", "bit" &amp; B67 &amp; "(" &amp; A67 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="C67" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D67" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C67, Levels!B:B, 0), 1, 1)),", ",IF(A67 &lt;&gt; "", """mem"": bit" &amp; B67 &amp; "(" &amp; A67 &amp; "),", ""),"""good"": ",IF(A67 &lt;&gt; "", 1, 0),"},")</f>
+        <v>66: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C68" s="4"/>
-      <c r="D68" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C68, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A68 &lt;&gt; "", "bit" &amp; B68 &amp; "(" &amp; A68 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="C68" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D68" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C68, Levels!B:B, 0), 1, 1)),", ",IF(A68 &lt;&gt; "", """mem"": bit" &amp; B68 &amp; "(" &amp; A68 &amp; "),", ""),"""good"": ",IF(A68 &lt;&gt; "", 1, 0),"},")</f>
+        <v>67: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C69" s="4"/>
-      <c r="D69" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C69, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A69 &lt;&gt; "", "bit" &amp; B69 &amp; "(" &amp; A69 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="C69" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D69" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C69, Levels!B:B, 0), 1, 1)),", ",IF(A69 &lt;&gt; "", """mem"": bit" &amp; B69 &amp; "(" &amp; A69 &amp; "),", ""),"""good"": ",IF(A69 &lt;&gt; "", 1, 0),"},")</f>
+        <v>68: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C70" s="4"/>
-      <c r="D70" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C70, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A70 &lt;&gt; "", "bit" &amp; B70 &amp; "(" &amp; A70 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="C70" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D70" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C70, Levels!B:B, 0), 1, 1)),", ",IF(A70 &lt;&gt; "", """mem"": bit" &amp; B70 &amp; "(" &amp; A70 &amp; "),", ""),"""good"": ",IF(A70 &lt;&gt; "", 1, 0),"},")</f>
+        <v>69: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C71" s="4"/>
-      <c r="D71" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C71, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A71 &lt;&gt; "", "bit" &amp; B71 &amp; "(" &amp; A71 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="C71" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D71" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C71, Levels!B:B, 0), 1, 1)),", ",IF(A71 &lt;&gt; "", """mem"": bit" &amp; B71 &amp; "(" &amp; A71 &amp; "),", ""),"""good"": ",IF(A71 &lt;&gt; "", 1, 0),"},")</f>
+        <v>70: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C72" s="4"/>
-      <c r="D72" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C72, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A72 &lt;&gt; "", "bit" &amp; B72 &amp; "(" &amp; A72 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="C72" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D72" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C72, Levels!B:B, 0), 1, 1)),", ",IF(A72 &lt;&gt; "", """mem"": bit" &amp; B72 &amp; "(" &amp; A72 &amp; "),", ""),"""good"": ",IF(A72 &lt;&gt; "", 1, 0),"},")</f>
+        <v>71: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C73" s="4"/>
-      <c r="D73" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C73, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A73 &lt;&gt; "", "bit" &amp; B73 &amp; "(" &amp; A73 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="C73" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D73" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C73, Levels!B:B, 0), 1, 1)),", ",IF(A73 &lt;&gt; "", """mem"": bit" &amp; B73 &amp; "(" &amp; A73 &amp; "),", ""),"""good"": ",IF(A73 &lt;&gt; "", 1, 0),"},")</f>
+        <v>72: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C74" s="4"/>
-      <c r="D74" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C74, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A74 &lt;&gt; "", "bit" &amp; B74 &amp; "(" &amp; A74 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="C74" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D74" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C74, Levels!B:B, 0), 1, 1)),", ",IF(A74 &lt;&gt; "", """mem"": bit" &amp; B74 &amp; "(" &amp; A74 &amp; "),", ""),"""good"": ",IF(A74 &lt;&gt; "", 1, 0),"},")</f>
+        <v>73: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C75" s="4"/>
-      <c r="D75" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C75, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A75 &lt;&gt; "", "bit" &amp; B75 &amp; "(" &amp; A75 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="C75" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D75" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C75, Levels!B:B, 0), 1, 1)),", ",IF(A75 &lt;&gt; "", """mem"": bit" &amp; B75 &amp; "(" &amp; A75 &amp; "),", ""),"""good"": ",IF(A75 &lt;&gt; "", 1, 0),"},")</f>
+        <v>74: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C76" s="4"/>
-      <c r="D76" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C76, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A76 &lt;&gt; "", "bit" &amp; B76 &amp; "(" &amp; A76 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="C76" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D76" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C76, Levels!B:B, 0), 1, 1)),", ",IF(A76 &lt;&gt; "", """mem"": bit" &amp; B76 &amp; "(" &amp; A76 &amp; "),", ""),"""good"": ",IF(A76 &lt;&gt; "", 1, 0),"},")</f>
+        <v>75: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C77" s="4"/>
-      <c r="D77" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C77, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A77 &lt;&gt; "", "bit" &amp; B77 &amp; "(" &amp; A77 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="C77" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D77" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C77, Levels!B:B, 0), 1, 1)),", ",IF(A77 &lt;&gt; "", """mem"": bit" &amp; B77 &amp; "(" &amp; A77 &amp; "),", ""),"""good"": ",IF(A77 &lt;&gt; "", 1, 0),"},")</f>
+        <v>76: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C78" s="4"/>
-      <c r="D78" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C78, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A78 &lt;&gt; "", "bit" &amp; B78 &amp; "(" &amp; A78 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="C78" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D78" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C78, Levels!B:B, 0), 1, 1)),", ",IF(A78 &lt;&gt; "", """mem"": bit" &amp; B78 &amp; "(" &amp; A78 &amp; "),", ""),"""good"": ",IF(A78 &lt;&gt; "", 1, 0),"},")</f>
+        <v>77: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C79" s="4"/>
-      <c r="D79" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C79, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A79 &lt;&gt; "", "bit" &amp; B79 &amp; "(" &amp; A79 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="C79" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D79" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C79, Levels!B:B, 0), 1, 1)),", ",IF(A79 &lt;&gt; "", """mem"": bit" &amp; B79 &amp; "(" &amp; A79 &amp; "),", ""),"""good"": ",IF(A79 &lt;&gt; "", 1, 0),"},")</f>
+        <v>78: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C80" s="4"/>
-      <c r="D80" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C80, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A80 &lt;&gt; "", "bit" &amp; B80 &amp; "(" &amp; A80 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="C80" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D80" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C80, Levels!B:B, 0), 1, 1)),", ",IF(A80 &lt;&gt; "", """mem"": bit" &amp; B80 &amp; "(" &amp; A80 &amp; "),", ""),"""good"": ",IF(A80 &lt;&gt; "", 1, 0),"},")</f>
+        <v>79: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C81" s="4"/>
-      <c r="D81" s="0" t="e">
-        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C81, Levels!B:B, 0), 1, 1)),", ""mem"": ",IF(A81 &lt;&gt; "", "bit" &amp; B81 &amp; "(" &amp; A81 &amp; ")", ""),"},")</f>
-        <v>#N/A</v>
+      <c r="C81" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D81" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C81, Levels!B:B, 0), 1, 1)),", ",IF(A81 &lt;&gt; "", """mem"": bit" &amp; B81 &amp; "(" &amp; A81 &amp; "),", ""),"""good"": ",IF(A81 &lt;&gt; "", 1, 0),"},")</f>
+        <v>80: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Fixed achievements in the Sanctuary of Water and Ice
Working on the bonus stage achievements.
</commit_message>
<xml_diff>
--- a/Rayman 2.xlsx
+++ b/Rayman 2.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1330" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1400" uniqueCount="100">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -178,6 +178,36 @@
     <t xml:space="preserve">BayouArea2</t>
   </si>
   <si>
+    <t xml:space="preserve">7928A4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SoWaIArea1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">in the Sanctuary of Water and Ice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sanctuary of Water and Ice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">774694</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SoWaIArea2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">76F100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Polokus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">in Polokus’s dream</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0</t>
+  </si>
+  <si>
     <t xml:space="preserve">Index</t>
   </si>
   <si>
@@ -260,6 +290,24 @@
   </si>
   <si>
     <t xml:space="preserve">0x224a36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x22499b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x22499c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x22499d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x22499e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x22499f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x2249a0</t>
   </si>
   <si>
     <t xml:space="preserve">Level ID</t>
@@ -485,16 +533,16 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
+      <selection pane="bottomLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.03"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -518,7 +566,7 @@
       </c>
       <c r="H1" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(E2:E1000)</f>
-        <v>0x784BFC: { "id": 0x784BFC, "areaName": "Menu", "displayName": "Main Menu", "levelName": "Menu" },0x789668: { "id": 0x789668, "areaName": "Intro", "displayName": "somewhere in the Glade of Dreams…", "levelName": "None" },0x778C74: { "id": 0x778C74, "areaName": "BuccaneerBrig", "displayName": "in the Buccaneer’s brig", "levelName": "None" },0x78D424: { "id": 0x78D424, "areaName": "WoodsOfLight", "displayName": "in the Woods of Light", "levelName": "Woods of Light" },0x790570: { "id": 0x790570, "areaName": "HallOfDoors", "displayName": "in the Hall of Doors", "levelName": "Hall of Doors" },0x7875A8: { "id": 0x7875A8, "areaName": "FairyGladeArea1", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x78A320: { "id": 0x78A320, "areaName": "FairyGladeArea2", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x7A1BD8: { "id": 0x7A1BD8, "areaName": "FairyGladeArea3", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x77BFFC: { "id": 0x77BFFC, "areaName": "FairyGladeArea4", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x771B74: { "id": 0x771B74, "areaName": "FairyGladeArea5", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x74AAA8: { "id": 0x74AAA8, "areaName": "Results", "displayName": "viewing level results…", "levelName": "None" },0x788708: { "id": 0x788708, "areaName": "MarshesArea1", "displayName": "in the Marshes of Awakening", "levelName": "Marshes of Awakening" },0x7786E8: { "id": 0x7786E8, "areaName": "MarshesArea2", "displayName": "in the Marshes of Awakening", "levelName": "Marshes of Awakening" },0x790598: { "id": 0x790598, "areaName": "BayouArea1", "displayName": "in the Bayou", "levelName": "Bayou" },0x788764: { "id": 0x788764, "areaName": "BayouArea2", "displayName": "in the Bayou", "levelName": "Bayou" },</v>
+        <v>0x784BFC: { "id": 0x784BFC, "areaName": "Menu", "displayName": "Main Menu", "levelName": "Menu" },0x789668: { "id": 0x789668, "areaName": "Intro", "displayName": "somewhere in the Glade of Dreams…", "levelName": "None" },0x778C74: { "id": 0x778C74, "areaName": "BuccaneerBrig", "displayName": "in the Buccaneer’s brig", "levelName": "None" },0x78D424: { "id": 0x78D424, "areaName": "WoodsOfLight", "displayName": "in the Woods of Light", "levelName": "Woods of Light" },0x790570: { "id": 0x790570, "areaName": "HallOfDoors", "displayName": "in the Hall of Doors", "levelName": "Hall of Doors" },0x7875A8: { "id": 0x7875A8, "areaName": "FairyGladeArea1", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x78A320: { "id": 0x78A320, "areaName": "FairyGladeArea2", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x7A1BD8: { "id": 0x7A1BD8, "areaName": "FairyGladeArea3", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x77BFFC: { "id": 0x77BFFC, "areaName": "FairyGladeArea4", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x771B74: { "id": 0x771B74, "areaName": "FairyGladeArea5", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x74AAA8: { "id": 0x74AAA8, "areaName": "Results", "displayName": "viewing level results…", "levelName": "None" },0x788708: { "id": 0x788708, "areaName": "MarshesArea1", "displayName": "in the Marshes of Awakening", "levelName": "Marshes of Awakening" },0x7786E8: { "id": 0x7786E8, "areaName": "MarshesArea2", "displayName": "in the Marshes of Awakening", "levelName": "Marshes of Awakening" },0x790598: { "id": 0x790598, "areaName": "BayouArea1", "displayName": "in the Bayou", "levelName": "Bayou" },0x788764: { "id": 0x788764, "areaName": "BayouArea2", "displayName": "in the Bayou", "levelName": "Bayou" },0x7928A4: { "id": 0x7928A4, "areaName": "SoWaIArea1", "displayName": "in the Sanctuary of Water and Ice", "levelName": "Sanctuary of Water and Ice" },0x774694: { "id": 0x774694, "areaName": "SoWaIArea2", "displayName": "in the Sanctuary of Water and Ice", "levelName": "Sanctuary of Water and Ice" },0x76F100: { "id": 0x76F100, "areaName": "Polokus", "displayName": "in Polokus’s dream", "levelName": "Polokus" },0x0: { "id": 0x0, "areaName": "None", "displayName": "somewhere in the Glade of Dreams…", "levelName": "None" },</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -792,16 +840,76 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D17" s="4"/>
+      <c r="A17" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("0x", A17,": { ""id"": ","0x", A17,", ""areaName"": """,B17,""", ""displayName"": """,C17,""", ""levelName"": """,D17,""" },")</f>
+        <v>0x7928A4: { "id": 0x7928A4, "areaName": "SoWaIArea1", "displayName": "in the Sanctuary of Water and Ice", "levelName": "Sanctuary of Water and Ice" },</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D18" s="4"/>
+      <c r="A18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("0x", A18,": { ""id"": ","0x", A18,", ""areaName"": """,B18,""", ""displayName"": """,C18,""", ""levelName"": """,D18,""" },")</f>
+        <v>0x774694: { "id": 0x774694, "areaName": "SoWaIArea2", "displayName": "in the Sanctuary of Water and Ice", "levelName": "Sanctuary of Water and Ice" },</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D19" s="4"/>
+      <c r="A19" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("0x", A19,": { ""id"": ","0x", A19,", ""areaName"": """,B19,""", ""displayName"": """,C19,""", ""levelName"": """,D19,""" },")</f>
+        <v>0x76F100: { "id": 0x76F100, "areaName": "Polokus", "displayName": "in Polokus’s dream", "levelName": "Polokus" },</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D20" s="4"/>
+      <c r="A20" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("0x", A20,": { ""id"": ","0x", A20,", ""areaName"": """,B20,""", ""displayName"": """,C20,""", ""levelName"": """,D20,""" },")</f>
+        <v>0x0: { "id": 0x0, "areaName": "None", "displayName": "somewhere in the Glade of Dreams…", "levelName": "None" },</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D21" s="4"/>
@@ -3815,10 +3923,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="L2" activeCellId="0" sqref="L2"/>
+      <selection pane="bottomLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.21"/>
@@ -3830,22 +3938,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>4</v>
@@ -3921,11 +4029,11 @@
       </c>
       <c r="E4" s="0" t="n">
         <f aca="false">COUNTIFS(Lums!C3:C1002, "=" &amp; B4)</f>
-        <v>858</v>
+        <v>808</v>
       </c>
       <c r="F4" s="0" t="n">
         <f aca="false">COUNTIFS(Cages!C3:C83, "=" &amp; B4)</f>
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G4" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A4,": { ""id"": ",A4,", ""name"": """,B4,""", ""lums"": ",C4,", ""cages"": ",D4," },")</f>
@@ -4045,18 +4153,26 @@
         <f aca="false">ROW()-1</f>
         <v>8</v>
       </c>
-      <c r="B9" s="4"/>
+      <c r="B9" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="E9" s="0" t="n">
         <f aca="false">COUNTIFS(Lums!C8:C1007, "=" &amp; B9)</f>
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="F9" s="0" t="n">
         <f aca="false">COUNTIFS(Cages!C8:C88, "=" &amp; B9)</f>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G9" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A9,": { ""id"": ",A9,", ""name"": """,B9,""", ""lums"": ",C9,", ""cages"": ",D9," },")</f>
-        <v>8: { "id": 8, "name": "", "lums": , "cages":  },</v>
+        <v>8: { "id": 8, "name": "Sanctuary of Water and Ice", "lums": 50, "cages": 2 },</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4064,18 +4180,26 @@
         <f aca="false">ROW()-1</f>
         <v>9</v>
       </c>
-      <c r="B10" s="4"/>
+      <c r="B10" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="E10" s="0" t="n">
         <f aca="false">COUNTIFS(Lums!C9:C1008, "=" &amp; B10)</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F10" s="0" t="n">
         <f aca="false">COUNTIFS(Cages!C9:C89, "=" &amp; B10)</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G10" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A10,": { ""id"": ",A10,", ""name"": """,B10,""", ""lums"": ",C10,", ""cages"": ",D10," },")</f>
-        <v>9: { "id": 9, "name": "", "lums": , "cages":  },</v>
+        <v>9: { "id": 9, "name": "Polokus", "lums": 0, "cages": 0 },</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7513,12 +7637,12 @@
   <dimension ref="A1:H1001"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A124" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A177" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.93"/>
@@ -7527,10 +7651,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>3</v>
@@ -7543,12 +7667,12 @@
       </c>
       <c r="H1" s="5" t="str">
         <f aca="false">_xlfn.CONCAT(D2:D1001)</f>
-        <v>1: { "levelId": 2, "mem": bit0(0x224988),"good": 1},2: { "levelId": 2, "mem": bit1(0x224988),"good": 1},3: { "levelId": 2, "mem": bit2(0x224988),"good": 1},4: { "levelId": 2, "mem": bit3(0x224988),"good": 1},5: { "levelId": 2, "mem": bit4(0x224988),"good": 1},6: { "levelId": 2, "mem": bit5(0x224988),"good": 1},7: { "levelId": 2, "mem": bit6(0x224988),"good": 1},8: { "levelId": 2, "mem": bit7(0x224988),"good": 1},9: { "levelId": 2, "mem": bit2(0x224989),"good": 1},10: { "levelId": 2, "mem": bit1(0x22498a),"good": 1},11: { "levelId": 2, "mem": bit2(0x22498a),"good": 1},12: { "levelId": 2, "mem": bit3(0x22498a),"good": 1},13: { "levelId": 2, "mem": bit4(0x22498a),"good": 1},14: { "levelId": 2, "mem": bit5(0x22498a),"good": 1},15: { "levelId": 2, "mem": bit6(0x22498a),"good": 1},16: { "levelId": 2, "mem": bit7(0x22498a),"good": 1},17: { "levelId": 2, "mem": bit5(0x22498b),"good": 1},18: { "levelId": 2, "mem": bit6(0x22498b),"good": 1},19: { "levelId": 2, "mem": bit7(0x22498b),"good": 1},20: { "levelId": 2, "mem": bit0(0x22498c),"good": 1},21: { "levelId": 2, "mem": bit1(0x22498c),"good": 1},22: { "levelId": 2, "mem": bit2(0x22498c),"good": 1},23: { "levelId": 2, "mem": bit3(0x22498c),"good": 1},24: { "levelId": 2, "mem": bit4(0x22498c),"good": 1},25: { "levelId": 2, "mem": bit5(0x22498c),"good": 1},26: { "levelId": 2, "mem": bit6(0x22498c),"good": 1},27: { "levelId": 2, "mem": bit7(0x22498c),"good": 1},28: { "levelId": 2, "mem": bit0(0x22498d),"good": 1},29: { "levelId": 2, "mem": bit1(0x22498d),"good": 1},30: { "levelId": 2, "mem": bit2(0x22498d),"good": 1},31: { "levelId": 2, "mem": bit3(0x22498d),"good": 1},32: { "levelId": 2, "mem": bit4(0x22498d),"good": 1},33: { "levelId": 2, "mem": bit5(0x22498d),"good": 1},34: { "levelId": 2, "mem": bit6(0x22498d),"good": 1},35: { "levelId": 2, "mem": bit7(0x22498d),"good": 1},36: { "levelId": 2, "mem": bit0(0x22498e),"good": 1},37: { "levelId": 2, "mem": bit1(0x22498e),"good": 1},38: { "levelId": 5, "mem": bit2(0x22498e),"good": 1},39: { "levelId": 5, "mem": bit3(0x22498e),"good": 1},40: { "levelId": 5, "mem": bit4(0x22498e),"good": 1},41: { "levelId": 5, "mem": bit5(0x22498e),"good": 1},42: { "levelId": 5, "mem": bit6(0x22498e),"good": 1},43: { "levelId": 5, "mem": bit7(0x22498e),"good": 1},44: { "levelId": 5, "mem": bit0(0x22498f),"good": 1},45: { "levelId": 5, "mem": bit1(0x22498f),"good": 1},46: { "levelId": 5, "mem": bit2(0x22498f),"good": 1},47: { "levelId": 5, "mem": bit3(0x22498f),"good": 1},48: { "levelId": 5, "mem": bit4(0x22498f),"good": 1},49: { "levelId": 5, "mem": bit5(0x22498f),"good": 1},50: { "levelId": 5, "mem": bit6(0x22498f),"good": 1},51: { "levelId": 5, "mem": bit7(0x22498f),"good": 1},52: { "levelId": 5, "mem": bit0(0x224990),"good": 1},53: { "levelId": 5, "mem": bit1(0x224990),"good": 1},54: { "levelId": 5, "mem": bit2(0x224990),"good": 1},55: { "levelId": 5, "mem": bit3(0x224990),"good": 1},56: { "levelId": 5, "mem": bit4(0x224990),"good": 1},57: { "levelId": 5, "mem": bit5(0x224990),"good": 1},58: { "levelId": 5, "mem": bit6(0x224990),"good": 1},59: { "levelId": 5, "mem": bit7(0x224990),"good": 1},60: { "levelId": 5, "mem": bit0(0x224991),"good": 1},61: { "levelId": 5, "mem": bit1(0x224991),"good": 1},62: { "levelId": 5, "mem": bit2(0x224991),"good": 1},63: { "levelId": 5, "mem": bit3(0x224991),"good": 1},64: { "levelId": 5, "mem": bit4(0x224991),"good": 1},65: { "levelId": 5, "mem": bit5(0x224991),"good": 1},66: { "levelId": 5, "mem": bit6(0x224991),"good": 1},67: { "levelId": 5, "mem": bit7(0x224991),"good": 1},68: { "levelId": 5, "mem": bit0(0x224992),"good": 1},69: { "levelId": 5, "mem": bit1(0x224992),"good": 1},70: { "levelId": 5, "mem": bit2(0x224992),"good": 1},71: { "levelId": 5, "mem": bit3(0x224992),"good": 1},72: { "levelId": 5, "mem": bit4(0x224992),"good": 1},73: { "levelId": 5, "mem": bit5(0x224992),"good": 1},74: { "levelId": 5, "mem": bit6(0x224992),"good": 1},75: { "levelId": 5, "mem": bit7(0x224992),"good": 1},76: { "levelId": 5, "mem": bit0(0x224993),"good": 1},77: { "levelId": 5, "mem": bit1(0x224993),"good": 1},78: { "levelId": 5, "mem": bit2(0x224993),"good": 1},79: { "levelId": 5, "mem": bit3(0x224993),"good": 1},80: { "levelId": 5, "mem": bit4(0x224993),"good": 1},81: { "levelId": 5, "mem": bit5(0x224993),"good": 1},82: { "levelId": 5, "mem": bit6(0x224993),"good": 1},83: { "levelId": 5, "mem": bit7(0x224993),"good": 1},84: { "levelId": 5, "mem": bit0(0x224994),"good": 1},85: { "levelId": 5, "mem": bit1(0x224994),"good": 1},86: { "levelId": 5, "mem": bit2(0x224994),"good": 1},87: { "levelId": 5, "mem": bit3(0x224994),"good": 1},88: { "levelId": 6, "mem": bit4(0x224994),"good": 1},89: { "levelId": 6, "mem": bit5(0x224994),"good": 1},90: { "levelId": 6, "mem": bit6(0x224994),"good": 1},91: { "levelId": 6, "mem": bit7(0x224994),"good": 1},92: { "levelId": 6, "mem": bit0(0x224995),"good": 1},93: { "levelId": 6, "mem": bit1(0x224995),"good": 1},94: { "levelId": 6, "mem": bit2(0x224995),"good": 1},95: { "levelId": 6, "mem": bit3(0x224995),"good": 1},96: { "levelId": 6, "mem": bit4(0x224995),"good": 1},97: { "levelId": 6, "mem": bit5(0x224995),"good": 1},98: { "levelId": 6, "mem": bit6(0x224995),"good": 1},99: { "levelId": 6, "mem": bit7(0x224995),"good": 1},100: { "levelId": 6, "mem": bit0(0x224996),"good": 1},101: { "levelId": 6, "mem": bit1(0x224996),"good": 1},102: { "levelId": 6, "mem": bit2(0x224996),"good": 1},103: { "levelId": 6, "mem": bit3(0x224996),"good": 1},104: { "levelId": 6, "mem": bit4(0x224996),"good": 1},105: { "levelId": 6, "mem": bit5(0x224996),"good": 1},106: { "levelId": 6, "mem": bit6(0x224996),"good": 1},107: { "levelId": 6, "mem": bit7(0x224996),"good": 1},108: { "levelId": 6, "mem": bit0(0x224997),"good": 1},109: { "levelId": 6, "mem": bit1(0x224997),"good": 1},110: { "levelId": 6, "mem": bit2(0x224997),"good": 1},111: { "levelId": 6, "mem": bit3(0x224997),"good": 1},112: { "levelId": 6, "mem": bit4(0x224997),"good": 1},113: { "levelId": 6, "mem": bit5(0x224997),"good": 1},114: { "levelId": 6, "mem": bit6(0x224997),"good": 1},115: { "levelId": 6, "mem": bit7(0x224997),"good": 1},116: { "levelId": 6, "mem": bit0(0x224998),"good": 1},117: { "levelId": 6, "mem": bit1(0x224998),"good": 1},118: { "levelId": 6, "mem": bit2(0x224998),"good": 1},119: { "levelId": 6, "mem": bit3(0x224998),"good": 1},120: { "levelId": 6, "mem": bit4(0x224998),"good": 1},121: { "levelId": 6, "mem": bit5(0x224998),"good": 1},122: { "levelId": 6, "mem": bit6(0x224998),"good": 1},123: { "levelId": 6, "mem": bit0(0x224999),"good": 1},124: { "levelId": 6, "mem": bit1(0x224999),"good": 1},125: { "levelId": 6, "mem": bit2(0x224999),"good": 1},126: { "levelId": 6, "mem": bit3(0x224999),"good": 1},127: { "levelId": 6, "mem": bit4(0x224999),"good": 1},128: { "levelId": 6, "mem": bit5(0x224999),"good": 1},129: { "levelId": 6, "mem": bit6(0x224999),"good": 1},130: { "levelId": 6, "mem": bit7(0x224999),"good": 1},131: { "levelId": 6, "mem": bit0(0x22499a),"good": 1},132: { "levelId": 6, "mem": bit1(0x22499a),"good": 1},133: { "levelId": 6, "mem": bit2(0x22499a),"good": 1},134: { "levelId": 6, "mem": bit3(0x22499a),"good": 1},135: { "levelId": 6, "mem": bit4(0x22499a),"good": 1},136: { "levelId": 6, "mem": bit5(0x22499a),"good": 1},137: { "levelId": 1, "mem": bit3(0x224a36),"good": 1},138: { "levelId": 1, "mem": bit4(0x224a36),"good": 1},139: { "levelId": 1, "mem": bit5(0x224a36),"good": 1},140: { "levelId": 1, "mem": bit6(0x224a36),"good": 1},141: { "levelId": 1, "mem": bit7(0x224a36),"good": 1},142: { "levelId": 6, "mem": bit7(0x224998),"good": 1},143: { "levelId": 3, "good": 0},144: { "levelId": 3, "good": 0},145: { "levelId": 3, "good": 0},146: { "levelId": 3, "good": 0},147: { "levelId": 3, "good": 0},148: { "levelId": 3, "good": 0},149: { "levelId": 3, "good": 0},150: { "levelId": 3, "good": 0},151: { "levelId": 3, "good": 0},152: { "levelId": 3, "good": 0},153: { "levelId": 3, "good": 0},154: { "levelId": 3, "good": 0},155: { "levelId": 3, "good": 0},156: { "levelId": 3, "good": 0},157: { "levelId": 3, "good": 0},158: { "levelId": 3, "good": 0},159: { "levelId": 3, "good": 0},160: { "levelId": 3, "good": 0},161: { "levelId": 3, "good": 0},162: { "levelId": 3, "good": 0},163: { "levelId": 3, "good": 0},164: { "levelId": 3, "good": 0},165: { "levelId": 3, "good": 0},166: { "levelId": 3, "good": 0},167: { "levelId": 3, "good": 0},168: { "levelId": 3, "good": 0},169: { "levelId": 3, "good": 0},170: { "levelId": 3, "good": 0},171: { "levelId": 3, "good": 0},172: { "levelId": 3, "good": 0},173: { "levelId": 3, "good": 0},174: { "levelId": 3, "good": 0},175: { "levelId": 3, "good": 0},176: { "levelId": 3, "good": 0},177: { "levelId": 3, "good": 0},178: { "levelId": 3, "good": 0},179: { "levelId": 3, "good": 0},180: { "levelId": 3, "good": 0},181: { "levelId": 3, "good": 0},182: { "levelId": 3, "good": 0},183: { "levelId": 3, "good": 0},184: { "levelId": 3, "good": 0},185: { "levelId": 3, "good": 0},186: { "levelId": 3, "good": 0},187: { "levelId": 3, "good": 0},188: { "levelId": 3, "good": 0},189: { "levelId": 3, "good": 0},190: { "levelId": 3, "good": 0},191: { "levelId": 3, "good": 0},192: { "levelId": 3, "good": 0},193: { "levelId": 3, "good": 0},194: { "levelId": 3, "good": 0},195: { "levelId": 3, "good": 0},196: { "levelId": 3, "good": 0},197: { "levelId": 3, "good": 0},198: { "levelId": 3, "good": 0},199: { "levelId": 3, "good": 0},200: { "levelId": 3, "good": 0},201: { "levelId": 3, "good": 0},202: { "levelId": 3, "good": 0},203: { "levelId": 3, "good": 0},204: { "levelId": 3, "good": 0},205: { "levelId": 3, "good": 0},206: { "levelId": 3, "good": 0},207: { "levelId": 3, "good": 0},208: { "levelId": 3, "good": 0},209: { "levelId": 3, "good": 0},210: { "levelId": 3, "good": 0},211: { "levelId": 3, "good": 0},212: { "levelId": 3, "good": 0},213: { "levelId": 3, "good": 0},214: { "levelId": 3, "good": 0},215: { "levelId": 3, "good": 0},216: { "levelId": 3, "good": 0},217: { "levelId": 3, "good": 0},218: { "levelId": 3, "good": 0},219: { "levelId": 3, "good": 0},220: { "levelId": 3, "good": 0},221: { "levelId": 3, "good": 0},222: { "levelId": 3, "good": 0},223: { "levelId": 3, "good": 0},224: { "levelId": 3, "good": 0},225: { "levelId": 3, "good": 0},226: { "levelId": 3, "good": 0},227: { "levelId": 3, "good": 0},228: { "levelId": 3, "good": 0},229: { "levelId": 3, "good": 0},230: { "levelId": 3, "good": 0},231: { "levelId": 3, "good": 0},232: { "levelId": 3, "good": 0},233: { "levelId": 3, "good": 0},234: { "levelId": 3, "good": 0},235: { "levelId": 3, "good": 0},236: { "levelId": 3, "good": 0},237: { "levelId": 3, "good": 0},238: { "levelId": 3, "good": 0},239: { "levelId": 3, "good": 0},240: { "levelId": 3, "good": 0},241: { "levelId": 3, "good": 0},242: { "levelId": 3, "good": 0},243: { "levelId": 3, "good": 0},244: { "levelId": 3, "good": 0},245: { "levelId": 3, "good": 0},246: { "levelId": 3, "good": 0},247: { "levelId": 3, "good": 0},248: { "levelId": 3, "good": 0},249: { "levelId": 3, "good": 0},250: { "levelId": 3, "good": 0},251: { "levelId": 3, "good": 0},252: { "levelId": 3, "good": 0},253: { "levelId": 3, "good": 0},254: { "levelId": 3, "good": 0},255: { "levelId": 3, "good": 0},256: { "levelId": 3, "good": 0},257: { "levelId": 3, "good": 0},258: { "levelId": 3, "good": 0},259: { "levelId": 3, "good": 0},260: { "levelId": 3, "good": 0},261: { "levelId": 3, "good": 0},262: { "levelId": 3, "good": 0},263: { "levelId": 3, "good": 0},264: { "levelId": 3, "good": 0},265: { "levelId": 3, "good": 0},266: { "levelId": 3, "good": 0},267: { "levelId": 3, "good": 0},268: { "levelId": 3, "good": 0},269: { "levelId": 3, "good": 0},270: { "levelId": 3, "good": 0},271: { "levelId": 3, "good": 0},272: { "levelId": 3, "good": 0},273: { "levelId": 3, "good": 0},274: { "levelId": 3, "good": 0},275: { "levelId": 3, "good": 0},276: { "levelId": 3, "good": 0},277: { "levelId": 3, "good": 0},278: { "levelId": 3, "good": 0},279: { "levelId": 3, "good": 0},280: { "levelId": 3, "good": 0},281: { "levelId": 3, "good": 0},282: { "levelId": 3, "good": 0},283: { "levelId": 3, "good": 0},284: { "levelId": 3, "good": 0},285: { "levelId": 3, "good": 0},286: { "levelId": 3, "good": 0},287: { "levelId": 3, "good": 0},288: { "levelId": 3, "good": 0},289: { "levelId": 3, "good": 0},290: { "levelId": 3, "good": 0},291: { "levelId": 3, "good": 0},292: { "levelId": 3, "good": 0},293: { "levelId": 3, "good": 0},294: { "levelId": 3, "good": 0},295: { "levelId": 3, "good": 0},296: { "levelId": 3, "good": 0},297: { "levelId": 3, "good": 0},298: { "levelId": 3, "good": 0},299: { "levelId": 3, "good": 0},300: { "levelId": 3, "good": 0},301: { "levelId": 3, "good": 0},302: { "levelId": 3, "good": 0},303: { "levelId": 3, "good": 0},304: { "levelId": 3, "good": 0},305: { "levelId": 3, "good": 0},306: { "levelId": 3, "good": 0},307: { "levelId": 3, "good": 0},308: { "levelId": 3, "good": 0},309: { "levelId": 3, "good": 0},310: { "levelId": 3, "good": 0},311: { "levelId": 3, "good": 0},312: { "levelId": 3, "good": 0},313: { "levelId": 3, "good": 0},314: { "levelId": 3, "good": 0},315: { "levelId": 3, "good": 0},316: { "levelId": 3, "good": 0},317: { "levelId": 3, "good": 0},318: { "levelId": 3, "good": 0},319: { "levelId": 3, "good": 0},320: { "levelId": 3, "good": 0},321: { "levelId": 3, "good": 0},322: { "levelId": 3, "good": 0},323: { "levelId": 3, "good": 0},324: { "levelId": 3, "good": 0},325: { "levelId": 3, "good": 0},326: { "levelId": 3, "good": 0},327: { "levelId": 3, "good": 0},328: { "levelId": 3, "good": 0},329: { "levelId": 3, "good": 0},330: { "levelId": 3, "good": 0},331: { "levelId": 3, "good": 0},332: { "levelId": 3, "good": 0},333: { "levelId": 3, "good": 0},334: { "levelId": 3, "good": 0},335: { "levelId": 3, "good": 0},336: { "levelId": 3, "good": 0},337: { "levelId": 3, "good": 0},338: { "levelId": 3, "good": 0},339: { "levelId": 3, "good": 0},340: { "levelId": 3, "good": 0},341: { "levelId": 3, "good": 0},342: { "levelId": 3, "good": 0},343: { "levelId": 3, "good": 0},344: { "levelId": 3, "good": 0},345: { "levelId": 3, "good": 0},346: { "levelId": 3, "good": 0},347: { "levelId": 3, "good": 0},348: { "levelId": 3, "good": 0},349: { "levelId": 3, "good": 0},350: { "levelId": 3, "good": 0},351: { "levelId": 3, "good": 0},352: { "levelId": 3, "good": 0},353: { "levelId": 3, "good": 0},354: { "levelId": 3, "good": 0},355: { "levelId": 3, "good": 0},356: { "levelId": 3, "good": 0},357: { "levelId": 3, "good": 0},358: { "levelId": 3, "good": 0},359: { "levelId": 3, "good": 0},360: { "levelId": 3, "good": 0},361: { "levelId": 3, "good": 0},362: { "levelId": 3, "good": 0},363: { "levelId": 3, "good": 0},364: { "levelId": 3, "good": 0},365: { "levelId": 3, "good": 0},366: { "levelId": 3, "good": 0},367: { "levelId": 3, "good": 0},368: { "levelId": 3, "good": 0},369: { "levelId": 3, "good": 0},370: { "levelId": 3, "good": 0},371: { "levelId": 3, "good": 0},372: { "levelId": 3, "good": 0},373: { "levelId": 3, "good": 0},374: { "levelId": 3, "good": 0},375: { "levelId": 3, "good": 0},376: { "levelId": 3, "good": 0},377: { "levelId": 3, "good": 0},378: { "levelId": 3, "good": 0},379: { "levelId": 3, "good": 0},380: { "levelId": 3, "good": 0},381: { "levelId": 3, "good": 0},382: { "levelId": 3, "good": 0},383: { "levelId": 3, "good": 0},384: { "levelId": 3, "good": 0},385: { "levelId": 3, "good": 0},386: { "levelId": 3, "good": 0},387: { "levelId": 3, "good": 0},388: { "levelId": 3, "good": 0},389: { "levelId": 3, "good": 0},390: { "levelId": 3, "good": 0},391: { "levelId": 3, "good": 0},392: { "levelId": 3, "good": 0},393: { "levelId": 3, "good": 0},394: { "levelId": 3, "good": 0},395: { "levelId": 3, "good": 0},396: { "levelId": 3, "good": 0},397: { "levelId": 3, "good": 0},398: { "levelId": 3, "good": 0},399: { "levelId": 3, "good": 0},400: { "levelId": 3, "good": 0},401: { "levelId": 3, "good": 0},402: { "levelId": 3, "good": 0},403: { "levelId": 3, "good": 0},404: { "levelId": 3, "good": 0},405: { "levelId": 3, "good": 0},406: { "levelId": 3, "good": 0},407: { "levelId": 3, "good": 0},408: { "levelId": 3, "good": 0},409: { "levelId": 3, "good": 0},410: { "levelId": 3, "good": 0},411: { "levelId": 3, "good": 0},412: { "levelId": 3, "good": 0},413: { "levelId": 3, "good": 0},414: { "levelId": 3, "good": 0},415: { "levelId": 3, "good": 0},416: { "levelId": 3, "good": 0},417: { "levelId": 3, "good": 0},418: { "levelId": 3, "good": 0},419: { "levelId": 3, "good": 0},420: { "levelId": 3, "good": 0},421: { "levelId": 3, "good": 0},422: { "levelId": 3, "good": 0},423: { "levelId": 3, "good": 0},424: { "levelId": 3, "good": 0},425: { "levelId": 3, "good": 0},426: { "levelId": 3, "good": 0},427: { "levelId": 3, "good": 0},428: { "levelId": 3, "good": 0},429: { "levelId": 3, "good": 0},430: { "levelId": 3, "good": 0},431: { "levelId": 3, "good": 0},432: { "levelId": 3, "good": 0},433: { "levelId": 3, "good": 0},434: { "levelId": 3, "good": 0},435: { "levelId": 3, "good": 0},436: { "levelId": 3, "good": 0},437: { "levelId": 3, "good": 0},438: { "levelId": 3, "good": 0},439: { "levelId": 3, "good": 0},440: { "levelId": 3, "good": 0},441: { "levelId": 3, "good": 0},442: { "levelId": 3, "good": 0},443: { "levelId": 3, "good": 0},444: { "levelId": 3, "good": 0},445: { "levelId": 3, "good": 0},446: { "levelId": 3, "good": 0},447: { "levelId": 3, "good": 0},448: { "levelId": 3, "good": 0},449: { "levelId": 3, "good": 0},450: { "levelId": 3, "good": 0},451: { "levelId": 3, "good": 0},452: { "levelId": 3, "good": 0},453: { "levelId": 3, "good": 0},454: { "levelId": 3, "good": 0},455: { "levelId": 3, "good": 0},456: { "levelId": 3, "good": 0},457: { "levelId": 3, "good": 0},458: { "levelId": 3, "good": 0},459: { "levelId": 3, "good": 0},460: { "levelId": 3, "good": 0},461: { "levelId": 3, "good": 0},462: { "levelId": 3, "good": 0},463: { "levelId": 3, "good": 0},464: { "levelId": 3, "good": 0},465: { "levelId": 3, "good": 0},466: { "levelId": 3, "good": 0},467: { "levelId": 3, "good": 0},468: { "levelId": 3, "good": 0},469: { "levelId": 3, "good": 0},470: { "levelId": 3, "good": 0},471: { "levelId": 3, "good": 0},472: { "levelId": 3, "good": 0},473: { "levelId": 3, "good": 0},474: { "levelId": 3, "good": 0},475: { "levelId": 3, "good": 0},476: { "levelId": 3, "good": 0},477: { "levelId": 3, "good": 0},478: { "levelId": 3, "good": 0},479: { "levelId": 3, "good": 0},480: { "levelId": 3, "good": 0},481: { "levelId": 3, "good": 0},482: { "levelId": 3, "good": 0},483: { "levelId": 3, "good": 0},484: { "levelId": 3, "good": 0},485: { "levelId": 3, "good": 0},486: { "levelId": 3, "good": 0},487: { "levelId": 3, "good": 0},488: { "levelId": 3, "good": 0},489: { "levelId": 3, "good": 0},490: { "levelId": 3, "good": 0},491: { "levelId": 3, "good": 0},492: { "levelId": 3, "good": 0},493: { "levelId": 3, "good": 0},494: { "levelId": 3, "good": 0},495: { "levelId": 3, "good": 0},496: { "levelId": 3, "good": 0},497: { "levelId": 3, "good": 0},498: { "levelId": 3, "good": 0},499: { "levelId": 3, "good": 0},500: { "levelId": 3, "good": 0},501: { "levelId": 3, "good": 0},502: { "levelId": 3, "good": 0},503: { "levelId": 3, "good": 0},504: { "levelId": 3, "good": 0},505: { "levelId": 3, "good": 0},506: { "levelId": 3, "good": 0},507: { "levelId": 3, "good": 0},508: { "levelId": 3, "good": 0},509: { "levelId": 3, "good": 0},510: { "levelId": 3, "good": 0},511: { "levelId": 3, "good": 0},512: { "levelId": 3, "good": 0},513: { "levelId": 3, "good": 0},514: { "levelId": 3, "good": 0},515: { "levelId": 3, "good": 0},516: { "levelId": 3, "good": 0},517: { "levelId": 3, "good": 0},518: { "levelId": 3, "good": 0},519: { "levelId": 3, "good": 0},520: { "levelId": 3, "good": 0},521: { "levelId": 3, "good": 0},522: { "levelId": 3, "good": 0},523: { "levelId": 3, "good": 0},524: { "levelId": 3, "good": 0},525: { "levelId": 3, "good": 0},526: { "levelId": 3, "good": 0},527: { "levelId": 3, "good": 0},528: { "levelId": 3, "good": 0},529: { "levelId": 3, "good": 0},530: { "levelId": 3, "good": 0},531: { "levelId": 3, "good": 0},532: { "levelId": 3, "good": 0},533: { "levelId": 3, "good": 0},534: { "levelId": 3, "good": 0},535: { "levelId": 3, "good": 0},536: { "levelId": 3, "good": 0},537: { "levelId": 3, "good": 0},538: { "levelId": 3, "good": 0},539: { "levelId": 3, "good": 0},540: { "levelId": 3, "good": 0},541: { "levelId": 3, "good": 0},542: { "levelId": 3, "good": 0},543: { "levelId": 3, "good": 0},544: { "levelId": 3, "good": 0},545: { "levelId": 3, "good": 0},546: { "levelId": 3, "good": 0},547: { "levelId": 3, "good": 0},548: { "levelId": 3, "good": 0},549: { "levelId": 3, "good": 0},550: { "levelId": 3, "good": 0},551: { "levelId": 3, "good": 0},552: { "levelId": 3, "good": 0},553: { "levelId": 3, "good": 0},554: { "levelId": 3, "good": 0},555: { "levelId": 3, "good": 0},556: { "levelId": 3, "good": 0},557: { "levelId": 3, "good": 0},558: { "levelId": 3, "good": 0},559: { "levelId": 3, "good": 0},560: { "levelId": 3, "good": 0},561: { "levelId": 3, "good": 0},562: { "levelId": 3, "good": 0},563: { "levelId": 3, "good": 0},564: { "levelId": 3, "good": 0},565: { "levelId": 3, "good": 0},566: { "levelId": 3, "good": 0},567: { "levelId": 3, "good": 0},568: { "levelId": 3, "good": 0},569: { "levelId": 3, "good": 0},570: { "levelId": 3, "good": 0},571: { "levelId": 3, "good": 0},572: { "levelId": 3, "good": 0},573: { "levelId": 3, "good": 0},574: { "levelId": 3, "good": 0},575: { "levelId": 3, "good": 0},576: { "levelId": 3, "good": 0},577: { "levelId": 3, "good": 0},578: { "levelId": 3, "good": 0},579: { "levelId": 3, "good": 0},580: { "levelId": 3, "good": 0},581: { "levelId": 3, "good": 0},582: { "levelId": 3, "good": 0},583: { "levelId": 3, "good": 0},584: { "levelId": 3, "good": 0},585: { "levelId": 3, "good": 0},586: { "levelId": 3, "good": 0},587: { "levelId": 3, "good": 0},588: { "levelId": 3, "good": 0},589: { "levelId": 3, "good": 0},590: { "levelId": 3, "good": 0},591: { "levelId": 3, "good": 0},592: { "levelId": 3, "good": 0},593: { "levelId": 3, "good": 0},594: { "levelId": 3, "good": 0},595: { "levelId": 3, "good": 0},596: { "levelId": 3, "good": 0},597: { "levelId": 3, "good": 0},598: { "levelId": 3, "good": 0},599: { "levelId": 3, "good": 0},600: { "levelId": 3, "good": 0},601: { "levelId": 3, "good": 0},602: { "levelId": 3, "good": 0},603: { "levelId": 3, "good": 0},604: { "levelId": 3, "good": 0},605: { "levelId": 3, "good": 0},606: { "levelId": 3, "good": 0},607: { "levelId": 3, "good": 0},608: { "levelId": 3, "good": 0},609: { "levelId": 3, "good": 0},610: { "levelId": 3, "good": 0},611: { "levelId": 3, "good": 0},612: { "levelId": 3, "good": 0},613: { "levelId": 3, "good": 0},614: { "levelId": 3, "good": 0},615: { "levelId": 3, "good": 0},616: { "levelId": 3, "good": 0},617: { "levelId": 3, "good": 0},618: { "levelId": 3, "good": 0},619: { "levelId": 3, "good": 0},620: { "levelId": 3, "good": 0},621: { "levelId": 3, "good": 0},622: { "levelId": 3, "good": 0},623: { "levelId": 3, "good": 0},624: { "levelId": 3, "good": 0},625: { "levelId": 3, "good": 0},626: { "levelId": 3, "good": 0},627: { "levelId": 3, "good": 0},628: { "levelId": 3, "good": 0},629: { "levelId": 3, "good": 0},630: { "levelId": 3, "good": 0},631: { "levelId": 3, "good": 0},632: { "levelId": 3, "good": 0},633: { "levelId": 3, "good": 0},634: { "levelId": 3, "good": 0},635: { "levelId": 3, "good": 0},636: { "levelId": 3, "good": 0},637: { "levelId": 3, "good": 0},638: { "levelId": 3, "good": 0},639: { "levelId": 3, "good": 0},640: { "levelId": 3, "good": 0},641: { "levelId": 3, "good": 0},642: { "levelId": 3, "good": 0},643: { "levelId": 3, "good": 0},644: { "levelId": 3, "good": 0},645: { "levelId": 3, "good": 0},646: { "levelId": 3, "good": 0},647: { "levelId": 3, "good": 0},648: { "levelId": 3, "good": 0},649: { "levelId": 3, "good": 0},650: { "levelId": 3, "good": 0},651: { "levelId": 3, "good": 0},652: { "levelId": 3, "good": 0},653: { "levelId": 3, "good": 0},654: { "levelId": 3, "good": 0},655: { "levelId": 3, "good": 0},656: { "levelId": 3, "good": 0},657: { "levelId": 3, "good": 0},658: { "levelId": 3, "good": 0},659: { "levelId": 3, "good": 0},660: { "levelId": 3, "good": 0},661: { "levelId": 3, "good": 0},662: { "levelId": 3, "good": 0},663: { "levelId": 3, "good": 0},664: { "levelId": 3, "good": 0},665: { "levelId": 3, "good": 0},666: { "levelId": 3, "good": 0},667: { "levelId": 3, "good": 0},668: { "levelId": 3, "good": 0},669: { "levelId": 3, "good": 0},670: { "levelId": 3, "good": 0},671: { "levelId": 3, "good": 0},672: { "levelId": 3, "good": 0},673: { "levelId": 3, "good": 0},674: { "levelId": 3, "good": 0},675: { "levelId": 3, "good": 0},676: { "levelId": 3, "good": 0},677: { "levelId": 3, "good": 0},678: { "levelId": 3, "good": 0},679: { "levelId": 3, "good": 0},680: { "levelId": 3, "good": 0},681: { "levelId": 3, "good": 0},682: { "levelId": 3, "good": 0},683: { "levelId": 3, "good": 0},684: { "levelId": 3, "good": 0},685: { "levelId": 3, "good": 0},686: { "levelId": 3, "good": 0},687: { "levelId": 3, "good": 0},688: { "levelId": 3, "good": 0},689: { "levelId": 3, "good": 0},690: { "levelId": 3, "good": 0},691: { "levelId": 3, "good": 0},692: { "levelId": 3, "good": 0},693: { "levelId": 3, "good": 0},694: { "levelId": 3, "good": 0},695: { "levelId": 3, "good": 0},696: { "levelId": 3, "good": 0},697: { "levelId": 3, "good": 0},698: { "levelId": 3, "good": 0},699: { "levelId": 3, "good": 0},700: { "levelId": 3, "good": 0},701: { "levelId": 3, "good": 0},702: { "levelId": 3, "good": 0},703: { "levelId": 3, "good": 0},704: { "levelId": 3, "good": 0},705: { "levelId": 3, "good": 0},706: { "levelId": 3, "good": 0},707: { "levelId": 3, "good": 0},708: { "levelId": 3, "good": 0},709: { "levelId": 3, "good": 0},710: { "levelId": 3, "good": 0},711: { "levelId": 3, "good": 0},712: { "levelId": 3, "good": 0},713: { "levelId": 3, "good": 0},714: { "levelId": 3, "good": 0},715: { "levelId": 3, "good": 0},716: { "levelId": 3, "good": 0},717: { "levelId": 3, "good": 0},718: { "levelId": 3, "good": 0},719: { "levelId": 3, "good": 0},720: { "levelId": 3, "good": 0},721: { "levelId": 3, "good": 0},722: { "levelId": 3, "good": 0},723: { "levelId": 3, "good": 0},724: { "levelId": 3, "good": 0},725: { "levelId": 3, "good": 0},726: { "levelId": 3, "good": 0},727: { "levelId": 3, "good": 0},728: { "levelId": 3, "good": 0},729: { "levelId": 3, "good": 0},730: { "levelId": 3, "good": 0},731: { "levelId": 3, "good": 0},732: { "levelId": 3, "good": 0},733: { "levelId": 3, "good": 0},734: { "levelId": 3, "good": 0},735: { "levelId": 3, "good": 0},736: { "levelId": 3, "good": 0},737: { "levelId": 3, "good": 0},738: { "levelId": 3, "good": 0},739: { "levelId": 3, "good": 0},740: { "levelId": 3, "good": 0},741: { "levelId": 3, "good": 0},742: { "levelId": 3, "good": 0},743: { "levelId": 3, "good": 0},744: { "levelId": 3, "good": 0},745: { "levelId": 3, "good": 0},746: { "levelId": 3, "good": 0},747: { "levelId": 3, "good": 0},748: { "levelId": 3, "good": 0},749: { "levelId": 3, "good": 0},750: { "levelId": 3, "good": 0},751: { "levelId": 3, "good": 0},752: { "levelId": 3, "good": 0},753: { "levelId": 3, "good": 0},754: { "levelId": 3, "good": 0},755: { "levelId": 3, "good": 0},756: { "levelId": 3, "good": 0},757: { "levelId": 3, "good": 0},758: { "levelId": 3, "good": 0},759: { "levelId": 3, "good": 0},760: { "levelId": 3, "good": 0},761: { "levelId": 3, "good": 0},762: { "levelId": 3, "good": 0},763: { "levelId": 3, "good": 0},764: { "levelId": 3, "good": 0},765: { "levelId": 3, "good": 0},766: { "levelId": 3, "good": 0},767: { "levelId": 3, "good": 0},768: { "levelId": 3, "good": 0},769: { "levelId": 3, "good": 0},770: { "levelId": 3, "good": 0},771: { "levelId": 3, "good": 0},772: { "levelId": 3, "good": 0},773: { "levelId": 3, "good": 0},774: { "levelId": 3, "good": 0},775: { "levelId": 3, "good": 0},776: { "levelId": 3, "good": 0},777: { "levelId": 3, "good": 0},778: { "levelId": 3, "good": 0},779: { "levelId": 3, "good": 0},780: { "levelId": 3, "good": 0},781: { "levelId": 3, "good": 0},782: { "levelId": 3, "good": 0},783: { "levelId": 3, "good": 0},784: { "levelId": 3, "good": 0},785: { "levelId": 3, "good": 0},786: { "levelId": 3, "good": 0},787: { "levelId": 3, "good": 0},788: { "levelId": 3, "good": 0},789: { "levelId": 3, "good": 0},790: { "levelId": 3, "good": 0},791: { "levelId": 3, "good": 0},792: { "levelId": 3, "good": 0},793: { "levelId": 3, "good": 0},794: { "levelId": 3, "good": 0},795: { "levelId": 3, "good": 0},796: { "levelId": 3, "good": 0},797: { "levelId": 3, "good": 0},798: { "levelId": 3, "good": 0},799: { "levelId": 3, "good": 0},800: { "levelId": 3, "good": 0},801: { "levelId": 3, "good": 0},802: { "levelId": 3, "good": 0},803: { "levelId": 3, "good": 0},804: { "levelId": 3, "good": 0},805: { "levelId": 3, "good": 0},806: { "levelId": 3, "good": 0},807: { "levelId": 3, "good": 0},808: { "levelId": 3, "good": 0},809: { "levelId": 3, "good": 0},810: { "levelId": 3, "good": 0},811: { "levelId": 3, "good": 0},812: { "levelId": 3, "good": 0},813: { "levelId": 3, "good": 0},814: { "levelId": 3, "good": 0},815: { "levelId": 3, "good": 0},816: { "levelId": 3, "good": 0},817: { "levelId": 3, "good": 0},818: { "levelId": 3, "good": 0},819: { "levelId": 3, "good": 0},820: { "levelId": 3, "good": 0},821: { "levelId": 3, "good": 0},822: { "levelId": 3, "good": 0},823: { "levelId": 3, "good": 0},824: { "levelId": 3, "good": 0},825: { "levelId": 3, "good": 0},826: { "levelId": 3, "good": 0},827: { "levelId": 3, "good": 0},828: { "levelId": 3, "good": 0},829: { "levelId": 3, "good": 0},830: { "levelId": 3, "good": 0},831: { "levelId": 3, "good": 0},832: { "levelId": 3, "good": 0},833: { "levelId": 3, "good": 0},834: { "levelId": 3, "good": 0},835: { "levelId": 3, "good": 0},836: { "levelId": 3, "good": 0},837: { "levelId": 3, "good": 0},838: { "levelId": 3, "good": 0},839: { "levelId": 3, "good": 0},840: { "levelId": 3, "good": 0},841: { "levelId": 3, "good": 0},842: { "levelId": 3, "good": 0},843: { "levelId": 3, "good": 0},844: { "levelId": 3, "good": 0},845: { "levelId": 3, "good": 0},846: { "levelId": 3, "good": 0},847: { "levelId": 3, "good": 0},848: { "levelId": 3, "good": 0},849: { "levelId": 3, "good": 0},850: { "levelId": 3, "good": 0},851: { "levelId": 3, "good": 0},852: { "levelId": 3, "good": 0},853: { "levelId": 3, "good": 0},854: { "levelId": 3, "good": 0},855: { "levelId": 3, "good": 0},856: { "levelId": 3, "good": 0},857: { "levelId": 3, "good": 0},858: { "levelId": 3, "good": 0},859: { "levelId": 3, "good": 0},860: { "levelId": 3, "good": 0},861: { "levelId": 3, "good": 0},862: { "levelId": 3, "good": 0},863: { "levelId": 3, "good": 0},864: { "levelId": 3, "good": 0},865: { "levelId": 3, "good": 0},866: { "levelId": 3, "good": 0},867: { "levelId": 3, "good": 0},868: { "levelId": 3, "good": 0},869: { "levelId": 3, "good": 0},870: { "levelId": 3, "good": 0},871: { "levelId": 3, "good": 0},872: { "levelId": 3, "good": 0},873: { "levelId": 3, "good": 0},874: { "levelId": 3, "good": 0},875: { "levelId": 3, "good": 0},876: { "levelId": 3, "good": 0},877: { "levelId": 3, "good": 0},878: { "levelId": 3, "good": 0},879: { "levelId": 3, "good": 0},880: { "levelId": 3, "good": 0},881: { "levelId": 3, "good": 0},882: { "levelId": 3, "good": 0},883: { "levelId": 3, "good": 0},884: { "levelId": 3, "good": 0},885: { "levelId": 3, "good": 0},886: { "levelId": 3, "good": 0},887: { "levelId": 3, "good": 0},888: { "levelId": 3, "good": 0},889: { "levelId": 3, "good": 0},890: { "levelId": 3, "good": 0},891: { "levelId": 3, "good": 0},892: { "levelId": 3, "good": 0},893: { "levelId": 3, "good": 0},894: { "levelId": 3, "good": 0},895: { "levelId": 3, "good": 0},896: { "levelId": 3, "good": 0},897: { "levelId": 3, "good": 0},898: { "levelId": 3, "good": 0},899: { "levelId": 3, "good": 0},900: { "levelId": 3, "good": 0},901: { "levelId": 3, "good": 0},902: { "levelId": 3, "good": 0},903: { "levelId": 3, "good": 0},904: { "levelId": 3, "good": 0},905: { "levelId": 3, "good": 0},906: { "levelId": 3, "good": 0},907: { "levelId": 3, "good": 0},908: { "levelId": 3, "good": 0},909: { "levelId": 3, "good": 0},910: { "levelId": 3, "good": 0},911: { "levelId": 3, "good": 0},912: { "levelId": 3, "good": 0},913: { "levelId": 3, "good": 0},914: { "levelId": 3, "good": 0},915: { "levelId": 3, "good": 0},916: { "levelId": 3, "good": 0},917: { "levelId": 3, "good": 0},918: { "levelId": 3, "good": 0},919: { "levelId": 3, "good": 0},920: { "levelId": 3, "good": 0},921: { "levelId": 3, "good": 0},922: { "levelId": 3, "good": 0},923: { "levelId": 3, "good": 0},924: { "levelId": 3, "good": 0},925: { "levelId": 3, "good": 0},926: { "levelId": 3, "good": 0},927: { "levelId": 3, "good": 0},928: { "levelId": 3, "good": 0},929: { "levelId": 3, "good": 0},930: { "levelId": 3, "good": 0},931: { "levelId": 3, "good": 0},932: { "levelId": 3, "good": 0},933: { "levelId": 3, "good": 0},934: { "levelId": 3, "good": 0},935: { "levelId": 3, "good": 0},936: { "levelId": 3, "good": 0},937: { "levelId": 3, "good": 0},938: { "levelId": 3, "good": 0},939: { "levelId": 3, "good": 0},940: { "levelId": 3, "good": 0},941: { "levelId": 3, "good": 0},942: { "levelId": 3, "good": 0},943: { "levelId": 3, "good": 0},944: { "levelId": 3, "good": 0},945: { "levelId": 3, "good": 0},946: { "levelId": 3, "good": 0},947: { "levelId": 3, "good": 0},948: { "levelId": 3, "good": 0},949: { "levelId": 3, "good": 0},950: { "levelId": 3, "good": 0},951: { "levelId": 3, "good": 0},952: { "levelId": 3, "good": 0},953: { "levelId": 3, "good": 0},954: { "levelId": 3, "good": 0},955: { "levelId": 3, "good": 0},956: { "levelId": 3, "good": 0},957: { "levelId": 3, "good": 0},958: { "levelId": 3, "good": 0},959: { "levelId": 3, "good": 0},960: { "levelId": 3, "good": 0},961: { "levelId": 3, "good": 0},962: { "levelId": 3, "good": 0},963: { "levelId": 3, "good": 0},964: { "levelId": 3, "good": 0},965: { "levelId": 3, "good": 0},966: { "levelId": 3, "good": 0},967: { "levelId": 3, "good": 0},968: { "levelId": 3, "good": 0},969: { "levelId": 3, "good": 0},970: { "levelId": 3, "good": 0},971: { "levelId": 3, "good": 0},972: { "levelId": 3, "good": 0},973: { "levelId": 3, "good": 0},974: { "levelId": 3, "good": 0},975: { "levelId": 3, "good": 0},976: { "levelId": 3, "good": 0},977: { "levelId": 3, "good": 0},978: { "levelId": 3, "good": 0},979: { "levelId": 3, "good": 0},980: { "levelId": 3, "good": 0},981: { "levelId": 3, "good": 0},982: { "levelId": 3, "good": 0},983: { "levelId": 3, "good": 0},984: { "levelId": 3, "good": 0},985: { "levelId": 3, "good": 0},986: { "levelId": 3, "good": 0},987: { "levelId": 3, "good": 0},988: { "levelId": 3, "good": 0},989: { "levelId": 3, "good": 0},990: { "levelId": 3, "good": 0},991: { "levelId": 3, "good": 0},992: { "levelId": 3, "good": 0},993: { "levelId": 3, "good": 0},994: { "levelId": 3, "good": 0},995: { "levelId": 3, "good": 0},996: { "levelId": 3, "good": 0},997: { "levelId": 3, "good": 0},998: { "levelId": 3, "good": 0},999: { "levelId": 3, "good": 0},1000: { "levelId": 3, "good": 0},</v>
+        <v>1: { "levelId": 2, "mem": bit0(0x224988),"good": 1},2: { "levelId": 2, "mem": bit1(0x224988),"good": 1},3: { "levelId": 2, "mem": bit2(0x224988),"good": 1},4: { "levelId": 2, "mem": bit3(0x224988),"good": 1},5: { "levelId": 2, "mem": bit4(0x224988),"good": 1},6: { "levelId": 2, "mem": bit5(0x224988),"good": 1},7: { "levelId": 2, "mem": bit6(0x224988),"good": 1},8: { "levelId": 2, "mem": bit7(0x224988),"good": 1},9: { "levelId": 2, "mem": bit2(0x224989),"good": 1},10: { "levelId": 2, "mem": bit1(0x22498a),"good": 1},11: { "levelId": 2, "mem": bit2(0x22498a),"good": 1},12: { "levelId": 2, "mem": bit3(0x22498a),"good": 1},13: { "levelId": 2, "mem": bit4(0x22498a),"good": 1},14: { "levelId": 2, "mem": bit5(0x22498a),"good": 1},15: { "levelId": 2, "mem": bit6(0x22498a),"good": 1},16: { "levelId": 2, "mem": bit7(0x22498a),"good": 1},17: { "levelId": 2, "mem": bit5(0x22498b),"good": 1},18: { "levelId": 2, "mem": bit6(0x22498b),"good": 1},19: { "levelId": 2, "mem": bit7(0x22498b),"good": 1},20: { "levelId": 2, "mem": bit0(0x22498c),"good": 1},21: { "levelId": 2, "mem": bit1(0x22498c),"good": 1},22: { "levelId": 2, "mem": bit2(0x22498c),"good": 1},23: { "levelId": 2, "mem": bit3(0x22498c),"good": 1},24: { "levelId": 2, "mem": bit4(0x22498c),"good": 1},25: { "levelId": 2, "mem": bit5(0x22498c),"good": 1},26: { "levelId": 2, "mem": bit6(0x22498c),"good": 1},27: { "levelId": 2, "mem": bit7(0x22498c),"good": 1},28: { "levelId": 2, "mem": bit0(0x22498d),"good": 1},29: { "levelId": 2, "mem": bit1(0x22498d),"good": 1},30: { "levelId": 2, "mem": bit2(0x22498d),"good": 1},31: { "levelId": 2, "mem": bit3(0x22498d),"good": 1},32: { "levelId": 2, "mem": bit4(0x22498d),"good": 1},33: { "levelId": 2, "mem": bit5(0x22498d),"good": 1},34: { "levelId": 2, "mem": bit6(0x22498d),"good": 1},35: { "levelId": 2, "mem": bit7(0x22498d),"good": 1},36: { "levelId": 2, "mem": bit0(0x22498e),"good": 1},37: { "levelId": 2, "mem": bit1(0x22498e),"good": 1},38: { "levelId": 5, "mem": bit2(0x22498e),"good": 1},39: { "levelId": 5, "mem": bit3(0x22498e),"good": 1},40: { "levelId": 5, "mem": bit4(0x22498e),"good": 1},41: { "levelId": 5, "mem": bit5(0x22498e),"good": 1},42: { "levelId": 5, "mem": bit6(0x22498e),"good": 1},43: { "levelId": 5, "mem": bit7(0x22498e),"good": 1},44: { "levelId": 5, "mem": bit0(0x22498f),"good": 1},45: { "levelId": 5, "mem": bit1(0x22498f),"good": 1},46: { "levelId": 5, "mem": bit2(0x22498f),"good": 1},47: { "levelId": 5, "mem": bit3(0x22498f),"good": 1},48: { "levelId": 5, "mem": bit4(0x22498f),"good": 1},49: { "levelId": 5, "mem": bit5(0x22498f),"good": 1},50: { "levelId": 5, "mem": bit6(0x22498f),"good": 1},51: { "levelId": 5, "mem": bit7(0x22498f),"good": 1},52: { "levelId": 5, "mem": bit0(0x224990),"good": 1},53: { "levelId": 5, "mem": bit1(0x224990),"good": 1},54: { "levelId": 5, "mem": bit2(0x224990),"good": 1},55: { "levelId": 5, "mem": bit3(0x224990),"good": 1},56: { "levelId": 5, "mem": bit4(0x224990),"good": 1},57: { "levelId": 5, "mem": bit5(0x224990),"good": 1},58: { "levelId": 5, "mem": bit6(0x224990),"good": 1},59: { "levelId": 5, "mem": bit7(0x224990),"good": 1},60: { "levelId": 5, "mem": bit0(0x224991),"good": 1},61: { "levelId": 5, "mem": bit1(0x224991),"good": 1},62: { "levelId": 5, "mem": bit2(0x224991),"good": 1},63: { "levelId": 5, "mem": bit3(0x224991),"good": 1},64: { "levelId": 5, "mem": bit4(0x224991),"good": 1},65: { "levelId": 5, "mem": bit5(0x224991),"good": 1},66: { "levelId": 5, "mem": bit6(0x224991),"good": 1},67: { "levelId": 5, "mem": bit7(0x224991),"good": 1},68: { "levelId": 5, "mem": bit0(0x224992),"good": 1},69: { "levelId": 5, "mem": bit1(0x224992),"good": 1},70: { "levelId": 5, "mem": bit2(0x224992),"good": 1},71: { "levelId": 5, "mem": bit3(0x224992),"good": 1},72: { "levelId": 5, "mem": bit4(0x224992),"good": 1},73: { "levelId": 5, "mem": bit5(0x224992),"good": 1},74: { "levelId": 5, "mem": bit6(0x224992),"good": 1},75: { "levelId": 5, "mem": bit7(0x224992),"good": 1},76: { "levelId": 5, "mem": bit0(0x224993),"good": 1},77: { "levelId": 5, "mem": bit1(0x224993),"good": 1},78: { "levelId": 5, "mem": bit2(0x224993),"good": 1},79: { "levelId": 5, "mem": bit3(0x224993),"good": 1},80: { "levelId": 5, "mem": bit4(0x224993),"good": 1},81: { "levelId": 5, "mem": bit5(0x224993),"good": 1},82: { "levelId": 5, "mem": bit6(0x224993),"good": 1},83: { "levelId": 5, "mem": bit7(0x224993),"good": 1},84: { "levelId": 5, "mem": bit0(0x224994),"good": 1},85: { "levelId": 5, "mem": bit1(0x224994),"good": 1},86: { "levelId": 5, "mem": bit2(0x224994),"good": 1},87: { "levelId": 5, "mem": bit3(0x224994),"good": 1},88: { "levelId": 6, "mem": bit4(0x224994),"good": 1},89: { "levelId": 6, "mem": bit5(0x224994),"good": 1},90: { "levelId": 6, "mem": bit6(0x224994),"good": 1},91: { "levelId": 6, "mem": bit7(0x224994),"good": 1},92: { "levelId": 6, "mem": bit0(0x224995),"good": 1},93: { "levelId": 6, "mem": bit1(0x224995),"good": 1},94: { "levelId": 6, "mem": bit2(0x224995),"good": 1},95: { "levelId": 6, "mem": bit3(0x224995),"good": 1},96: { "levelId": 6, "mem": bit4(0x224995),"good": 1},97: { "levelId": 6, "mem": bit5(0x224995),"good": 1},98: { "levelId": 6, "mem": bit6(0x224995),"good": 1},99: { "levelId": 6, "mem": bit7(0x224995),"good": 1},100: { "levelId": 6, "mem": bit0(0x224996),"good": 1},101: { "levelId": 6, "mem": bit1(0x224996),"good": 1},102: { "levelId": 6, "mem": bit2(0x224996),"good": 1},103: { "levelId": 6, "mem": bit3(0x224996),"good": 1},104: { "levelId": 6, "mem": bit4(0x224996),"good": 1},105: { "levelId": 6, "mem": bit5(0x224996),"good": 1},106: { "levelId": 6, "mem": bit6(0x224996),"good": 1},107: { "levelId": 6, "mem": bit7(0x224996),"good": 1},108: { "levelId": 6, "mem": bit0(0x224997),"good": 1},109: { "levelId": 6, "mem": bit1(0x224997),"good": 1},110: { "levelId": 6, "mem": bit2(0x224997),"good": 1},111: { "levelId": 6, "mem": bit3(0x224997),"good": 1},112: { "levelId": 6, "mem": bit4(0x224997),"good": 1},113: { "levelId": 6, "mem": bit5(0x224997),"good": 1},114: { "levelId": 6, "mem": bit6(0x224997),"good": 1},115: { "levelId": 6, "mem": bit7(0x224997),"good": 1},116: { "levelId": 6, "mem": bit0(0x224998),"good": 1},117: { "levelId": 6, "mem": bit1(0x224998),"good": 1},118: { "levelId": 6, "mem": bit2(0x224998),"good": 1},119: { "levelId": 6, "mem": bit3(0x224998),"good": 1},120: { "levelId": 6, "mem": bit4(0x224998),"good": 1},121: { "levelId": 6, "mem": bit5(0x224998),"good": 1},122: { "levelId": 6, "mem": bit6(0x224998),"good": 1},123: { "levelId": 6, "mem": bit0(0x224999),"good": 1},124: { "levelId": 6, "mem": bit1(0x224999),"good": 1},125: { "levelId": 6, "mem": bit2(0x224999),"good": 1},126: { "levelId": 6, "mem": bit3(0x224999),"good": 1},127: { "levelId": 6, "mem": bit4(0x224999),"good": 1},128: { "levelId": 6, "mem": bit5(0x224999),"good": 1},129: { "levelId": 6, "mem": bit6(0x224999),"good": 1},130: { "levelId": 6, "mem": bit7(0x224999),"good": 1},131: { "levelId": 6, "mem": bit0(0x22499a),"good": 1},132: { "levelId": 6, "mem": bit1(0x22499a),"good": 1},133: { "levelId": 6, "mem": bit2(0x22499a),"good": 1},134: { "levelId": 6, "mem": bit3(0x22499a),"good": 1},135: { "levelId": 6, "mem": bit4(0x22499a),"good": 1},136: { "levelId": 6, "mem": bit5(0x22499a),"good": 1},137: { "levelId": 1, "mem": bit3(0x224a36),"good": 1},138: { "levelId": 1, "mem": bit4(0x224a36),"good": 1},139: { "levelId": 1, "mem": bit5(0x224a36),"good": 1},140: { "levelId": 1, "mem": bit6(0x224a36),"good": 1},141: { "levelId": 1, "mem": bit7(0x224a36),"good": 1},142: { "levelId": 6, "mem": bit7(0x224998),"good": 1},143: { "levelId": 8, "mem": bit3(0x22499b),"good": 1},144: { "levelId": 8, "mem": bit4(0x22499b),"good": 1},145: { "levelId": 8, "mem": bit5(0x22499b),"good": 1},146: { "levelId": 8, "mem": bit5(0x22499c),"good": 1},147: { "levelId": 8, "mem": bit6(0x22499c),"good": 1},148: { "levelId": 8, "mem": bit7(0x22499c),"good": 1},149: { "levelId": 8, "mem": bit0(0x22499d),"good": 1},150: { "levelId": 8, "mem": bit1(0x22499d),"good": 1},151: { "levelId": 8, "mem": bit2(0x22499d),"good": 1},152: { "levelId": 8, "mem": bit3(0x22499d),"good": 1},153: { "levelId": 8, "mem": bit4(0x22499d),"good": 1},154: { "levelId": 8, "mem": bit5(0x22499d),"good": 1},155: { "levelId": 8, "mem": bit6(0x22499d),"good": 1},156: { "levelId": 8, "mem": bit7(0x22499d),"good": 1},157: { "levelId": 8, "mem": bit0(0x22499e),"good": 1},158: { "levelId": 8, "mem": bit1(0x22499e),"good": 1},159: { "levelId": 8, "mem": bit6(0x22499a),"good": 1},160: { "levelId": 8, "mem": bit7(0x22499a),"good": 1},161: { "levelId": 8, "mem": bit0(0x22499b),"good": 1},162: { "levelId": 8, "mem": bit1(0x22499b),"good": 1},163: { "levelId": 8, "mem": bit2(0x22499b),"good": 1},164: { "levelId": 8, "mem": bit6(0x22499b),"good": 1},165: { "levelId": 8, "mem": bit7(0x22499b),"good": 1},166: { "levelId": 8, "mem": bit0(0x22499c),"good": 1},167: { "levelId": 8, "mem": bit1(0x22499c),"good": 1},168: { "levelId": 8, "mem": bit2(0x22499c),"good": 1},169: { "levelId": 8, "mem": bit3(0x22499c),"good": 1},170: { "levelId": 8, "mem": bit4(0x22499c),"good": 1},171: { "levelId": 8, "mem": bit2(0x22499e),"good": 1},172: { "levelId": 8, "mem": bit3(0x22499e),"good": 1},173: { "levelId": 8, "mem": bit4(0x22499e),"good": 1},174: { "levelId": 8, "mem": bit5(0x22499e),"good": 1},175: { "levelId": 8, "mem": bit6(0x22499e),"good": 1},176: { "levelId": 8, "mem": bit7(0x22499e),"good": 1},177: { "levelId": 8, "mem": bit0(0x22499f),"good": 1},178: { "levelId": 8, "mem": bit1(0x22499f),"good": 1},179: { "levelId": 8, "mem": bit2(0x22499f),"good": 1},180: { "levelId": 8, "mem": bit3(0x22499f),"good": 1},181: { "levelId": 8, "mem": bit4(0x22499f),"good": 1},182: { "levelId": 8, "mem": bit5(0x22499f),"good": 1},183: { "levelId": 8, "mem": bit6(0x22499f),"good": 1},184: { "levelId": 8, "mem": bit7(0x22499f),"good": 1},185: { "levelId": 8, "mem": bit0(0x2249a0),"good": 1},186: { "levelId": 8, "mem": bit1(0x2249a0),"good": 1},187: { "levelId": 8, "mem": bit2(0x2249a0),"good": 1},188: { "levelId": 8, "mem": bit3(0x2249a0),"good": 1},189: { "levelId": 8, "mem": bit4(0x2249a0),"good": 1},190: { "levelId": 8, "mem": bit5(0x2249a0),"good": 1},191: { "levelId": 8, "mem": bit6(0x2249a0),"good": 1},192: { "levelId": 8, "mem": bit7(0x2249a0),"good": 1},193: { "levelId": 3, "good": 0},194: { "levelId": 3, "good": 0},195: { "levelId": 3, "good": 0},196: { "levelId": 3, "good": 0},197: { "levelId": 3, "good": 0},198: { "levelId": 3, "good": 0},199: { "levelId": 3, "good": 0},200: { "levelId": 3, "good": 0},201: { "levelId": 3, "good": 0},202: { "levelId": 3, "good": 0},203: { "levelId": 3, "good": 0},204: { "levelId": 3, "good": 0},205: { "levelId": 3, "good": 0},206: { "levelId": 3, "good": 0},207: { "levelId": 3, "good": 0},208: { "levelId": 3, "good": 0},209: { "levelId": 3, "good": 0},210: { "levelId": 3, "good": 0},211: { "levelId": 3, "good": 0},212: { "levelId": 3, "good": 0},213: { "levelId": 3, "good": 0},214: { "levelId": 3, "good": 0},215: { "levelId": 3, "good": 0},216: { "levelId": 3, "good": 0},217: { "levelId": 3, "good": 0},218: { "levelId": 3, "good": 0},219: { "levelId": 3, "good": 0},220: { "levelId": 3, "good": 0},221: { "levelId": 3, "good": 0},222: { "levelId": 3, "good": 0},223: { "levelId": 3, "good": 0},224: { "levelId": 3, "good": 0},225: { "levelId": 3, "good": 0},226: { "levelId": 3, "good": 0},227: { "levelId": 3, "good": 0},228: { "levelId": 3, "good": 0},229: { "levelId": 3, "good": 0},230: { "levelId": 3, "good": 0},231: { "levelId": 3, "good": 0},232: { "levelId": 3, "good": 0},233: { "levelId": 3, "good": 0},234: { "levelId": 3, "good": 0},235: { "levelId": 3, "good": 0},236: { "levelId": 3, "good": 0},237: { "levelId": 3, "good": 0},238: { "levelId": 3, "good": 0},239: { "levelId": 3, "good": 0},240: { "levelId": 3, "good": 0},241: { "levelId": 3, "good": 0},242: { "levelId": 3, "good": 0},243: { "levelId": 3, "good": 0},244: { "levelId": 3, "good": 0},245: { "levelId": 3, "good": 0},246: { "levelId": 3, "good": 0},247: { "levelId": 3, "good": 0},248: { "levelId": 3, "good": 0},249: { "levelId": 3, "good": 0},250: { "levelId": 3, "good": 0},251: { "levelId": 3, "good": 0},252: { "levelId": 3, "good": 0},253: { "levelId": 3, "good": 0},254: { "levelId": 3, "good": 0},255: { "levelId": 3, "good": 0},256: { "levelId": 3, "good": 0},257: { "levelId": 3, "good": 0},258: { "levelId": 3, "good": 0},259: { "levelId": 3, "good": 0},260: { "levelId": 3, "good": 0},261: { "levelId": 3, "good": 0},262: { "levelId": 3, "good": 0},263: { "levelId": 3, "good": 0},264: { "levelId": 3, "good": 0},265: { "levelId": 3, "good": 0},266: { "levelId": 3, "good": 0},267: { "levelId": 3, "good": 0},268: { "levelId": 3, "good": 0},269: { "levelId": 3, "good": 0},270: { "levelId": 3, "good": 0},271: { "levelId": 3, "good": 0},272: { "levelId": 3, "good": 0},273: { "levelId": 3, "good": 0},274: { "levelId": 3, "good": 0},275: { "levelId": 3, "good": 0},276: { "levelId": 3, "good": 0},277: { "levelId": 3, "good": 0},278: { "levelId": 3, "good": 0},279: { "levelId": 3, "good": 0},280: { "levelId": 3, "good": 0},281: { "levelId": 3, "good": 0},282: { "levelId": 3, "good": 0},283: { "levelId": 3, "good": 0},284: { "levelId": 3, "good": 0},285: { "levelId": 3, "good": 0},286: { "levelId": 3, "good": 0},287: { "levelId": 3, "good": 0},288: { "levelId": 3, "good": 0},289: { "levelId": 3, "good": 0},290: { "levelId": 3, "good": 0},291: { "levelId": 3, "good": 0},292: { "levelId": 3, "good": 0},293: { "levelId": 3, "good": 0},294: { "levelId": 3, "good": 0},295: { "levelId": 3, "good": 0},296: { "levelId": 3, "good": 0},297: { "levelId": 3, "good": 0},298: { "levelId": 3, "good": 0},299: { "levelId": 3, "good": 0},300: { "levelId": 3, "good": 0},301: { "levelId": 3, "good": 0},302: { "levelId": 3, "good": 0},303: { "levelId": 3, "good": 0},304: { "levelId": 3, "good": 0},305: { "levelId": 3, "good": 0},306: { "levelId": 3, "good": 0},307: { "levelId": 3, "good": 0},308: { "levelId": 3, "good": 0},309: { "levelId": 3, "good": 0},310: { "levelId": 3, "good": 0},311: { "levelId": 3, "good": 0},312: { "levelId": 3, "good": 0},313: { "levelId": 3, "good": 0},314: { "levelId": 3, "good": 0},315: { "levelId": 3, "good": 0},316: { "levelId": 3, "good": 0},317: { "levelId": 3, "good": 0},318: { "levelId": 3, "good": 0},319: { "levelId": 3, "good": 0},320: { "levelId": 3, "good": 0},321: { "levelId": 3, "good": 0},322: { "levelId": 3, "good": 0},323: { "levelId": 3, "good": 0},324: { "levelId": 3, "good": 0},325: { "levelId": 3, "good": 0},326: { "levelId": 3, "good": 0},327: { "levelId": 3, "good": 0},328: { "levelId": 3, "good": 0},329: { "levelId": 3, "good": 0},330: { "levelId": 3, "good": 0},331: { "levelId": 3, "good": 0},332: { "levelId": 3, "good": 0},333: { "levelId": 3, "good": 0},334: { "levelId": 3, "good": 0},335: { "levelId": 3, "good": 0},336: { "levelId": 3, "good": 0},337: { "levelId": 3, "good": 0},338: { "levelId": 3, "good": 0},339: { "levelId": 3, "good": 0},340: { "levelId": 3, "good": 0},341: { "levelId": 3, "good": 0},342: { "levelId": 3, "good": 0},343: { "levelId": 3, "good": 0},344: { "levelId": 3, "good": 0},345: { "levelId": 3, "good": 0},346: { "levelId": 3, "good": 0},347: { "levelId": 3, "good": 0},348: { "levelId": 3, "good": 0},349: { "levelId": 3, "good": 0},350: { "levelId": 3, "good": 0},351: { "levelId": 3, "good": 0},352: { "levelId": 3, "good": 0},353: { "levelId": 3, "good": 0},354: { "levelId": 3, "good": 0},355: { "levelId": 3, "good": 0},356: { "levelId": 3, "good": 0},357: { "levelId": 3, "good": 0},358: { "levelId": 3, "good": 0},359: { "levelId": 3, "good": 0},360: { "levelId": 3, "good": 0},361: { "levelId": 3, "good": 0},362: { "levelId": 3, "good": 0},363: { "levelId": 3, "good": 0},364: { "levelId": 3, "good": 0},365: { "levelId": 3, "good": 0},366: { "levelId": 3, "good": 0},367: { "levelId": 3, "good": 0},368: { "levelId": 3, "good": 0},369: { "levelId": 3, "good": 0},370: { "levelId": 3, "good": 0},371: { "levelId": 3, "good": 0},372: { "levelId": 3, "good": 0},373: { "levelId": 3, "good": 0},374: { "levelId": 3, "good": 0},375: { "levelId": 3, "good": 0},376: { "levelId": 3, "good": 0},377: { "levelId": 3, "good": 0},378: { "levelId": 3, "good": 0},379: { "levelId": 3, "good": 0},380: { "levelId": 3, "good": 0},381: { "levelId": 3, "good": 0},382: { "levelId": 3, "good": 0},383: { "levelId": 3, "good": 0},384: { "levelId": 3, "good": 0},385: { "levelId": 3, "good": 0},386: { "levelId": 3, "good": 0},387: { "levelId": 3, "good": 0},388: { "levelId": 3, "good": 0},389: { "levelId": 3, "good": 0},390: { "levelId": 3, "good": 0},391: { "levelId": 3, "good": 0},392: { "levelId": 3, "good": 0},393: { "levelId": 3, "good": 0},394: { "levelId": 3, "good": 0},395: { "levelId": 3, "good": 0},396: { "levelId": 3, "good": 0},397: { "levelId": 3, "good": 0},398: { "levelId": 3, "good": 0},399: { "levelId": 3, "good": 0},400: { "levelId": 3, "good": 0},401: { "levelId": 3, "good": 0},402: { "levelId": 3, "good": 0},403: { "levelId": 3, "good": 0},404: { "levelId": 3, "good": 0},405: { "levelId": 3, "good": 0},406: { "levelId": 3, "good": 0},407: { "levelId": 3, "good": 0},408: { "levelId": 3, "good": 0},409: { "levelId": 3, "good": 0},410: { "levelId": 3, "good": 0},411: { "levelId": 3, "good": 0},412: { "levelId": 3, "good": 0},413: { "levelId": 3, "good": 0},414: { "levelId": 3, "good": 0},415: { "levelId": 3, "good": 0},416: { "levelId": 3, "good": 0},417: { "levelId": 3, "good": 0},418: { "levelId": 3, "good": 0},419: { "levelId": 3, "good": 0},420: { "levelId": 3, "good": 0},421: { "levelId": 3, "good": 0},422: { "levelId": 3, "good": 0},423: { "levelId": 3, "good": 0},424: { "levelId": 3, "good": 0},425: { "levelId": 3, "good": 0},426: { "levelId": 3, "good": 0},427: { "levelId": 3, "good": 0},428: { "levelId": 3, "good": 0},429: { "levelId": 3, "good": 0},430: { "levelId": 3, "good": 0},431: { "levelId": 3, "good": 0},432: { "levelId": 3, "good": 0},433: { "levelId": 3, "good": 0},434: { "levelId": 3, "good": 0},435: { "levelId": 3, "good": 0},436: { "levelId": 3, "good": 0},437: { "levelId": 3, "good": 0},438: { "levelId": 3, "good": 0},439: { "levelId": 3, "good": 0},440: { "levelId": 3, "good": 0},441: { "levelId": 3, "good": 0},442: { "levelId": 3, "good": 0},443: { "levelId": 3, "good": 0},444: { "levelId": 3, "good": 0},445: { "levelId": 3, "good": 0},446: { "levelId": 3, "good": 0},447: { "levelId": 3, "good": 0},448: { "levelId": 3, "good": 0},449: { "levelId": 3, "good": 0},450: { "levelId": 3, "good": 0},451: { "levelId": 3, "good": 0},452: { "levelId": 3, "good": 0},453: { "levelId": 3, "good": 0},454: { "levelId": 3, "good": 0},455: { "levelId": 3, "good": 0},456: { "levelId": 3, "good": 0},457: { "levelId": 3, "good": 0},458: { "levelId": 3, "good": 0},459: { "levelId": 3, "good": 0},460: { "levelId": 3, "good": 0},461: { "levelId": 3, "good": 0},462: { "levelId": 3, "good": 0},463: { "levelId": 3, "good": 0},464: { "levelId": 3, "good": 0},465: { "levelId": 3, "good": 0},466: { "levelId": 3, "good": 0},467: { "levelId": 3, "good": 0},468: { "levelId": 3, "good": 0},469: { "levelId": 3, "good": 0},470: { "levelId": 3, "good": 0},471: { "levelId": 3, "good": 0},472: { "levelId": 3, "good": 0},473: { "levelId": 3, "good": 0},474: { "levelId": 3, "good": 0},475: { "levelId": 3, "good": 0},476: { "levelId": 3, "good": 0},477: { "levelId": 3, "good": 0},478: { "levelId": 3, "good": 0},479: { "levelId": 3, "good": 0},480: { "levelId": 3, "good": 0},481: { "levelId": 3, "good": 0},482: { "levelId": 3, "good": 0},483: { "levelId": 3, "good": 0},484: { "levelId": 3, "good": 0},485: { "levelId": 3, "good": 0},486: { "levelId": 3, "good": 0},487: { "levelId": 3, "good": 0},488: { "levelId": 3, "good": 0},489: { "levelId": 3, "good": 0},490: { "levelId": 3, "good": 0},491: { "levelId": 3, "good": 0},492: { "levelId": 3, "good": 0},493: { "levelId": 3, "good": 0},494: { "levelId": 3, "good": 0},495: { "levelId": 3, "good": 0},496: { "levelId": 3, "good": 0},497: { "levelId": 3, "good": 0},498: { "levelId": 3, "good": 0},499: { "levelId": 3, "good": 0},500: { "levelId": 3, "good": 0},501: { "levelId": 3, "good": 0},502: { "levelId": 3, "good": 0},503: { "levelId": 3, "good": 0},504: { "levelId": 3, "good": 0},505: { "levelId": 3, "good": 0},506: { "levelId": 3, "good": 0},507: { "levelId": 3, "good": 0},508: { "levelId": 3, "good": 0},509: { "levelId": 3, "good": 0},510: { "levelId": 3, "good": 0},511: { "levelId": 3, "good": 0},512: { "levelId": 3, "good": 0},513: { "levelId": 3, "good": 0},514: { "levelId": 3, "good": 0},515: { "levelId": 3, "good": 0},516: { "levelId": 3, "good": 0},517: { "levelId": 3, "good": 0},518: { "levelId": 3, "good": 0},519: { "levelId": 3, "good": 0},520: { "levelId": 3, "good": 0},521: { "levelId": 3, "good": 0},522: { "levelId": 3, "good": 0},523: { "levelId": 3, "good": 0},524: { "levelId": 3, "good": 0},525: { "levelId": 3, "good": 0},526: { "levelId": 3, "good": 0},527: { "levelId": 3, "good": 0},528: { "levelId": 3, "good": 0},529: { "levelId": 3, "good": 0},530: { "levelId": 3, "good": 0},531: { "levelId": 3, "good": 0},532: { "levelId": 3, "good": 0},533: { "levelId": 3, "good": 0},534: { "levelId": 3, "good": 0},535: { "levelId": 3, "good": 0},536: { "levelId": 3, "good": 0},537: { "levelId": 3, "good": 0},538: { "levelId": 3, "good": 0},539: { "levelId": 3, "good": 0},540: { "levelId": 3, "good": 0},541: { "levelId": 3, "good": 0},542: { "levelId": 3, "good": 0},543: { "levelId": 3, "good": 0},544: { "levelId": 3, "good": 0},545: { "levelId": 3, "good": 0},546: { "levelId": 3, "good": 0},547: { "levelId": 3, "good": 0},548: { "levelId": 3, "good": 0},549: { "levelId": 3, "good": 0},550: { "levelId": 3, "good": 0},551: { "levelId": 3, "good": 0},552: { "levelId": 3, "good": 0},553: { "levelId": 3, "good": 0},554: { "levelId": 3, "good": 0},555: { "levelId": 3, "good": 0},556: { "levelId": 3, "good": 0},557: { "levelId": 3, "good": 0},558: { "levelId": 3, "good": 0},559: { "levelId": 3, "good": 0},560: { "levelId": 3, "good": 0},561: { "levelId": 3, "good": 0},562: { "levelId": 3, "good": 0},563: { "levelId": 3, "good": 0},564: { "levelId": 3, "good": 0},565: { "levelId": 3, "good": 0},566: { "levelId": 3, "good": 0},567: { "levelId": 3, "good": 0},568: { "levelId": 3, "good": 0},569: { "levelId": 3, "good": 0},570: { "levelId": 3, "good": 0},571: { "levelId": 3, "good": 0},572: { "levelId": 3, "good": 0},573: { "levelId": 3, "good": 0},574: { "levelId": 3, "good": 0},575: { "levelId": 3, "good": 0},576: { "levelId": 3, "good": 0},577: { "levelId": 3, "good": 0},578: { "levelId": 3, "good": 0},579: { "levelId": 3, "good": 0},580: { "levelId": 3, "good": 0},581: { "levelId": 3, "good": 0},582: { "levelId": 3, "good": 0},583: { "levelId": 3, "good": 0},584: { "levelId": 3, "good": 0},585: { "levelId": 3, "good": 0},586: { "levelId": 3, "good": 0},587: { "levelId": 3, "good": 0},588: { "levelId": 3, "good": 0},589: { "levelId": 3, "good": 0},590: { "levelId": 3, "good": 0},591: { "levelId": 3, "good": 0},592: { "levelId": 3, "good": 0},593: { "levelId": 3, "good": 0},594: { "levelId": 3, "good": 0},595: { "levelId": 3, "good": 0},596: { "levelId": 3, "good": 0},597: { "levelId": 3, "good": 0},598: { "levelId": 3, "good": 0},599: { "levelId": 3, "good": 0},600: { "levelId": 3, "good": 0},601: { "levelId": 3, "good": 0},602: { "levelId": 3, "good": 0},603: { "levelId": 3, "good": 0},604: { "levelId": 3, "good": 0},605: { "levelId": 3, "good": 0},606: { "levelId": 3, "good": 0},607: { "levelId": 3, "good": 0},608: { "levelId": 3, "good": 0},609: { "levelId": 3, "good": 0},610: { "levelId": 3, "good": 0},611: { "levelId": 3, "good": 0},612: { "levelId": 3, "good": 0},613: { "levelId": 3, "good": 0},614: { "levelId": 3, "good": 0},615: { "levelId": 3, "good": 0},616: { "levelId": 3, "good": 0},617: { "levelId": 3, "good": 0},618: { "levelId": 3, "good": 0},619: { "levelId": 3, "good": 0},620: { "levelId": 3, "good": 0},621: { "levelId": 3, "good": 0},622: { "levelId": 3, "good": 0},623: { "levelId": 3, "good": 0},624: { "levelId": 3, "good": 0},625: { "levelId": 3, "good": 0},626: { "levelId": 3, "good": 0},627: { "levelId": 3, "good": 0},628: { "levelId": 3, "good": 0},629: { "levelId": 3, "good": 0},630: { "levelId": 3, "good": 0},631: { "levelId": 3, "good": 0},632: { "levelId": 3, "good": 0},633: { "levelId": 3, "good": 0},634: { "levelId": 3, "good": 0},635: { "levelId": 3, "good": 0},636: { "levelId": 3, "good": 0},637: { "levelId": 3, "good": 0},638: { "levelId": 3, "good": 0},639: { "levelId": 3, "good": 0},640: { "levelId": 3, "good": 0},641: { "levelId": 3, "good": 0},642: { "levelId": 3, "good": 0},643: { "levelId": 3, "good": 0},644: { "levelId": 3, "good": 0},645: { "levelId": 3, "good": 0},646: { "levelId": 3, "good": 0},647: { "levelId": 3, "good": 0},648: { "levelId": 3, "good": 0},649: { "levelId": 3, "good": 0},650: { "levelId": 3, "good": 0},651: { "levelId": 3, "good": 0},652: { "levelId": 3, "good": 0},653: { "levelId": 3, "good": 0},654: { "levelId": 3, "good": 0},655: { "levelId": 3, "good": 0},656: { "levelId": 3, "good": 0},657: { "levelId": 3, "good": 0},658: { "levelId": 3, "good": 0},659: { "levelId": 3, "good": 0},660: { "levelId": 3, "good": 0},661: { "levelId": 3, "good": 0},662: { "levelId": 3, "good": 0},663: { "levelId": 3, "good": 0},664: { "levelId": 3, "good": 0},665: { "levelId": 3, "good": 0},666: { "levelId": 3, "good": 0},667: { "levelId": 3, "good": 0},668: { "levelId": 3, "good": 0},669: { "levelId": 3, "good": 0},670: { "levelId": 3, "good": 0},671: { "levelId": 3, "good": 0},672: { "levelId": 3, "good": 0},673: { "levelId": 3, "good": 0},674: { "levelId": 3, "good": 0},675: { "levelId": 3, "good": 0},676: { "levelId": 3, "good": 0},677: { "levelId": 3, "good": 0},678: { "levelId": 3, "good": 0},679: { "levelId": 3, "good": 0},680: { "levelId": 3, "good": 0},681: { "levelId": 3, "good": 0},682: { "levelId": 3, "good": 0},683: { "levelId": 3, "good": 0},684: { "levelId": 3, "good": 0},685: { "levelId": 3, "good": 0},686: { "levelId": 3, "good": 0},687: { "levelId": 3, "good": 0},688: { "levelId": 3, "good": 0},689: { "levelId": 3, "good": 0},690: { "levelId": 3, "good": 0},691: { "levelId": 3, "good": 0},692: { "levelId": 3, "good": 0},693: { "levelId": 3, "good": 0},694: { "levelId": 3, "good": 0},695: { "levelId": 3, "good": 0},696: { "levelId": 3, "good": 0},697: { "levelId": 3, "good": 0},698: { "levelId": 3, "good": 0},699: { "levelId": 3, "good": 0},700: { "levelId": 3, "good": 0},701: { "levelId": 3, "good": 0},702: { "levelId": 3, "good": 0},703: { "levelId": 3, "good": 0},704: { "levelId": 3, "good": 0},705: { "levelId": 3, "good": 0},706: { "levelId": 3, "good": 0},707: { "levelId": 3, "good": 0},708: { "levelId": 3, "good": 0},709: { "levelId": 3, "good": 0},710: { "levelId": 3, "good": 0},711: { "levelId": 3, "good": 0},712: { "levelId": 3, "good": 0},713: { "levelId": 3, "good": 0},714: { "levelId": 3, "good": 0},715: { "levelId": 3, "good": 0},716: { "levelId": 3, "good": 0},717: { "levelId": 3, "good": 0},718: { "levelId": 3, "good": 0},719: { "levelId": 3, "good": 0},720: { "levelId": 3, "good": 0},721: { "levelId": 3, "good": 0},722: { "levelId": 3, "good": 0},723: { "levelId": 3, "good": 0},724: { "levelId": 3, "good": 0},725: { "levelId": 3, "good": 0},726: { "levelId": 3, "good": 0},727: { "levelId": 3, "good": 0},728: { "levelId": 3, "good": 0},729: { "levelId": 3, "good": 0},730: { "levelId": 3, "good": 0},731: { "levelId": 3, "good": 0},732: { "levelId": 3, "good": 0},733: { "levelId": 3, "good": 0},734: { "levelId": 3, "good": 0},735: { "levelId": 3, "good": 0},736: { "levelId": 3, "good": 0},737: { "levelId": 3, "good": 0},738: { "levelId": 3, "good": 0},739: { "levelId": 3, "good": 0},740: { "levelId": 3, "good": 0},741: { "levelId": 3, "good": 0},742: { "levelId": 3, "good": 0},743: { "levelId": 3, "good": 0},744: { "levelId": 3, "good": 0},745: { "levelId": 3, "good": 0},746: { "levelId": 3, "good": 0},747: { "levelId": 3, "good": 0},748: { "levelId": 3, "good": 0},749: { "levelId": 3, "good": 0},750: { "levelId": 3, "good": 0},751: { "levelId": 3, "good": 0},752: { "levelId": 3, "good": 0},753: { "levelId": 3, "good": 0},754: { "levelId": 3, "good": 0},755: { "levelId": 3, "good": 0},756: { "levelId": 3, "good": 0},757: { "levelId": 3, "good": 0},758: { "levelId": 3, "good": 0},759: { "levelId": 3, "good": 0},760: { "levelId": 3, "good": 0},761: { "levelId": 3, "good": 0},762: { "levelId": 3, "good": 0},763: { "levelId": 3, "good": 0},764: { "levelId": 3, "good": 0},765: { "levelId": 3, "good": 0},766: { "levelId": 3, "good": 0},767: { "levelId": 3, "good": 0},768: { "levelId": 3, "good": 0},769: { "levelId": 3, "good": 0},770: { "levelId": 3, "good": 0},771: { "levelId": 3, "good": 0},772: { "levelId": 3, "good": 0},773: { "levelId": 3, "good": 0},774: { "levelId": 3, "good": 0},775: { "levelId": 3, "good": 0},776: { "levelId": 3, "good": 0},777: { "levelId": 3, "good": 0},778: { "levelId": 3, "good": 0},779: { "levelId": 3, "good": 0},780: { "levelId": 3, "good": 0},781: { "levelId": 3, "good": 0},782: { "levelId": 3, "good": 0},783: { "levelId": 3, "good": 0},784: { "levelId": 3, "good": 0},785: { "levelId": 3, "good": 0},786: { "levelId": 3, "good": 0},787: { "levelId": 3, "good": 0},788: { "levelId": 3, "good": 0},789: { "levelId": 3, "good": 0},790: { "levelId": 3, "good": 0},791: { "levelId": 3, "good": 0},792: { "levelId": 3, "good": 0},793: { "levelId": 3, "good": 0},794: { "levelId": 3, "good": 0},795: { "levelId": 3, "good": 0},796: { "levelId": 3, "good": 0},797: { "levelId": 3, "good": 0},798: { "levelId": 3, "good": 0},799: { "levelId": 3, "good": 0},800: { "levelId": 3, "good": 0},801: { "levelId": 3, "good": 0},802: { "levelId": 3, "good": 0},803: { "levelId": 3, "good": 0},804: { "levelId": 3, "good": 0},805: { "levelId": 3, "good": 0},806: { "levelId": 3, "good": 0},807: { "levelId": 3, "good": 0},808: { "levelId": 3, "good": 0},809: { "levelId": 3, "good": 0},810: { "levelId": 3, "good": 0},811: { "levelId": 3, "good": 0},812: { "levelId": 3, "good": 0},813: { "levelId": 3, "good": 0},814: { "levelId": 3, "good": 0},815: { "levelId": 3, "good": 0},816: { "levelId": 3, "good": 0},817: { "levelId": 3, "good": 0},818: { "levelId": 3, "good": 0},819: { "levelId": 3, "good": 0},820: { "levelId": 3, "good": 0},821: { "levelId": 3, "good": 0},822: { "levelId": 3, "good": 0},823: { "levelId": 3, "good": 0},824: { "levelId": 3, "good": 0},825: { "levelId": 3, "good": 0},826: { "levelId": 3, "good": 0},827: { "levelId": 3, "good": 0},828: { "levelId": 3, "good": 0},829: { "levelId": 3, "good": 0},830: { "levelId": 3, "good": 0},831: { "levelId": 3, "good": 0},832: { "levelId": 3, "good": 0},833: { "levelId": 3, "good": 0},834: { "levelId": 3, "good": 0},835: { "levelId": 3, "good": 0},836: { "levelId": 3, "good": 0},837: { "levelId": 3, "good": 0},838: { "levelId": 3, "good": 0},839: { "levelId": 3, "good": 0},840: { "levelId": 3, "good": 0},841: { "levelId": 3, "good": 0},842: { "levelId": 3, "good": 0},843: { "levelId": 3, "good": 0},844: { "levelId": 3, "good": 0},845: { "levelId": 3, "good": 0},846: { "levelId": 3, "good": 0},847: { "levelId": 3, "good": 0},848: { "levelId": 3, "good": 0},849: { "levelId": 3, "good": 0},850: { "levelId": 3, "good": 0},851: { "levelId": 3, "good": 0},852: { "levelId": 3, "good": 0},853: { "levelId": 3, "good": 0},854: { "levelId": 3, "good": 0},855: { "levelId": 3, "good": 0},856: { "levelId": 3, "good": 0},857: { "levelId": 3, "good": 0},858: { "levelId": 3, "good": 0},859: { "levelId": 3, "good": 0},860: { "levelId": 3, "good": 0},861: { "levelId": 3, "good": 0},862: { "levelId": 3, "good": 0},863: { "levelId": 3, "good": 0},864: { "levelId": 3, "good": 0},865: { "levelId": 3, "good": 0},866: { "levelId": 3, "good": 0},867: { "levelId": 3, "good": 0},868: { "levelId": 3, "good": 0},869: { "levelId": 3, "good": 0},870: { "levelId": 3, "good": 0},871: { "levelId": 3, "good": 0},872: { "levelId": 3, "good": 0},873: { "levelId": 3, "good": 0},874: { "levelId": 3, "good": 0},875: { "levelId": 3, "good": 0},876: { "levelId": 3, "good": 0},877: { "levelId": 3, "good": 0},878: { "levelId": 3, "good": 0},879: { "levelId": 3, "good": 0},880: { "levelId": 3, "good": 0},881: { "levelId": 3, "good": 0},882: { "levelId": 3, "good": 0},883: { "levelId": 3, "good": 0},884: { "levelId": 3, "good": 0},885: { "levelId": 3, "good": 0},886: { "levelId": 3, "good": 0},887: { "levelId": 3, "good": 0},888: { "levelId": 3, "good": 0},889: { "levelId": 3, "good": 0},890: { "levelId": 3, "good": 0},891: { "levelId": 3, "good": 0},892: { "levelId": 3, "good": 0},893: { "levelId": 3, "good": 0},894: { "levelId": 3, "good": 0},895: { "levelId": 3, "good": 0},896: { "levelId": 3, "good": 0},897: { "levelId": 3, "good": 0},898: { "levelId": 3, "good": 0},899: { "levelId": 3, "good": 0},900: { "levelId": 3, "good": 0},901: { "levelId": 3, "good": 0},902: { "levelId": 3, "good": 0},903: { "levelId": 3, "good": 0},904: { "levelId": 3, "good": 0},905: { "levelId": 3, "good": 0},906: { "levelId": 3, "good": 0},907: { "levelId": 3, "good": 0},908: { "levelId": 3, "good": 0},909: { "levelId": 3, "good": 0},910: { "levelId": 3, "good": 0},911: { "levelId": 3, "good": 0},912: { "levelId": 3, "good": 0},913: { "levelId": 3, "good": 0},914: { "levelId": 3, "good": 0},915: { "levelId": 3, "good": 0},916: { "levelId": 3, "good": 0},917: { "levelId": 3, "good": 0},918: { "levelId": 3, "good": 0},919: { "levelId": 3, "good": 0},920: { "levelId": 3, "good": 0},921: { "levelId": 3, "good": 0},922: { "levelId": 3, "good": 0},923: { "levelId": 3, "good": 0},924: { "levelId": 3, "good": 0},925: { "levelId": 3, "good": 0},926: { "levelId": 3, "good": 0},927: { "levelId": 3, "good": 0},928: { "levelId": 3, "good": 0},929: { "levelId": 3, "good": 0},930: { "levelId": 3, "good": 0},931: { "levelId": 3, "good": 0},932: { "levelId": 3, "good": 0},933: { "levelId": 3, "good": 0},934: { "levelId": 3, "good": 0},935: { "levelId": 3, "good": 0},936: { "levelId": 3, "good": 0},937: { "levelId": 3, "good": 0},938: { "levelId": 3, "good": 0},939: { "levelId": 3, "good": 0},940: { "levelId": 3, "good": 0},941: { "levelId": 3, "good": 0},942: { "levelId": 3, "good": 0},943: { "levelId": 3, "good": 0},944: { "levelId": 3, "good": 0},945: { "levelId": 3, "good": 0},946: { "levelId": 3, "good": 0},947: { "levelId": 3, "good": 0},948: { "levelId": 3, "good": 0},949: { "levelId": 3, "good": 0},950: { "levelId": 3, "good": 0},951: { "levelId": 3, "good": 0},952: { "levelId": 3, "good": 0},953: { "levelId": 3, "good": 0},954: { "levelId": 3, "good": 0},955: { "levelId": 3, "good": 0},956: { "levelId": 3, "good": 0},957: { "levelId": 3, "good": 0},958: { "levelId": 3, "good": 0},959: { "levelId": 3, "good": 0},960: { "levelId": 3, "good": 0},961: { "levelId": 3, "good": 0},962: { "levelId": 3, "good": 0},963: { "levelId": 3, "good": 0},964: { "levelId": 3, "good": 0},965: { "levelId": 3, "good": 0},966: { "levelId": 3, "good": 0},967: { "levelId": 3, "good": 0},968: { "levelId": 3, "good": 0},969: { "levelId": 3, "good": 0},970: { "levelId": 3, "good": 0},971: { "levelId": 3, "good": 0},972: { "levelId": 3, "good": 0},973: { "levelId": 3, "good": 0},974: { "levelId": 3, "good": 0},975: { "levelId": 3, "good": 0},976: { "levelId": 3, "good": 0},977: { "levelId": 3, "good": 0},978: { "levelId": 3, "good": 0},979: { "levelId": 3, "good": 0},980: { "levelId": 3, "good": 0},981: { "levelId": 3, "good": 0},982: { "levelId": 3, "good": 0},983: { "levelId": 3, "good": 0},984: { "levelId": 3, "good": 0},985: { "levelId": 3, "good": 0},986: { "levelId": 3, "good": 0},987: { "levelId": 3, "good": 0},988: { "levelId": 3, "good": 0},989: { "levelId": 3, "good": 0},990: { "levelId": 3, "good": 0},991: { "levelId": 3, "good": 0},992: { "levelId": 3, "good": 0},993: { "levelId": 3, "good": 0},994: { "levelId": 3, "good": 0},995: { "levelId": 3, "good": 0},996: { "levelId": 3, "good": 0},997: { "levelId": 3, "good": 0},998: { "levelId": 3, "good": 0},999: { "levelId": 3, "good": 0},1000: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0</v>
@@ -7563,7 +7687,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1</v>
@@ -7579,7 +7703,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>2</v>
@@ -7595,7 +7719,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>3</v>
@@ -7611,7 +7735,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>4</v>
@@ -7627,7 +7751,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>5</v>
@@ -7643,7 +7767,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>6</v>
@@ -7659,7 +7783,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>7</v>
@@ -7675,7 +7799,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>2</v>
@@ -7690,7 +7814,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>1</v>
@@ -7705,7 +7829,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>2</v>
@@ -7720,7 +7844,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>3</v>
@@ -7735,7 +7859,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>4</v>
@@ -7750,7 +7874,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>5</v>
@@ -7765,7 +7889,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>6</v>
@@ -7780,7 +7904,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>7</v>
@@ -7795,7 +7919,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>5</v>
@@ -7810,7 +7934,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>6</v>
@@ -7825,7 +7949,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>7</v>
@@ -7840,7 +7964,7 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>0</v>
@@ -7855,7 +7979,7 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="6" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>1</v>
@@ -7870,7 +7994,7 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>2</v>
@@ -7885,7 +8009,7 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>3</v>
@@ -7900,7 +8024,7 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="6" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>4</v>
@@ -7915,7 +8039,7 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="6" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>5</v>
@@ -7930,7 +8054,7 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="6" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>6</v>
@@ -7945,7 +8069,7 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="6" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>7</v>
@@ -7960,7 +8084,7 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="6" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>0</v>
@@ -7975,7 +8099,7 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="6" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>1</v>
@@ -7990,7 +8114,7 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="6" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>2</v>
@@ -8005,7 +8129,7 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="6" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>3</v>
@@ -8020,7 +8144,7 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="6" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>4</v>
@@ -8035,7 +8159,7 @@
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="6" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>5</v>
@@ -8050,7 +8174,7 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="6" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>6</v>
@@ -8065,7 +8189,7 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="6" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>7</v>
@@ -8080,7 +8204,7 @@
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="6" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>0</v>
@@ -8095,7 +8219,7 @@
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="6" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>1</v>
@@ -8110,7 +8234,7 @@
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>2</v>
@@ -8125,7 +8249,7 @@
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>3</v>
@@ -8140,7 +8264,7 @@
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>4</v>
@@ -8155,7 +8279,7 @@
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>5</v>
@@ -8170,7 +8294,7 @@
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>6</v>
@@ -8185,7 +8309,7 @@
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="B44" s="0" t="n">
         <v>7</v>
@@ -8200,7 +8324,7 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="B45" s="0" t="n">
         <v>0</v>
@@ -8215,7 +8339,7 @@
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="B46" s="0" t="n">
         <v>1</v>
@@ -8230,7 +8354,7 @@
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="B47" s="0" t="n">
         <v>2</v>
@@ -8245,7 +8369,7 @@
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="B48" s="0" t="n">
         <v>3</v>
@@ -8260,7 +8384,7 @@
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="B49" s="0" t="n">
         <v>4</v>
@@ -8275,7 +8399,7 @@
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="B50" s="0" t="n">
         <v>5</v>
@@ -8290,7 +8414,7 @@
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="B51" s="0" t="n">
         <v>6</v>
@@ -8305,7 +8429,7 @@
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="B52" s="0" t="n">
         <v>7</v>
@@ -8320,7 +8444,7 @@
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="B53" s="0" t="n">
         <v>0</v>
@@ -8335,7 +8459,7 @@
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="B54" s="0" t="n">
         <v>1</v>
@@ -8350,7 +8474,7 @@
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="B55" s="0" t="n">
         <v>2</v>
@@ -8365,7 +8489,7 @@
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="B56" s="0" t="n">
         <v>3</v>
@@ -8380,7 +8504,7 @@
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="B57" s="0" t="n">
         <v>4</v>
@@ -8395,7 +8519,7 @@
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="B58" s="0" t="n">
         <v>5</v>
@@ -8410,7 +8534,7 @@
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="B59" s="0" t="n">
         <v>6</v>
@@ -8425,7 +8549,7 @@
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="B60" s="0" t="n">
         <v>7</v>
@@ -8440,7 +8564,7 @@
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B61" s="0" t="n">
         <v>0</v>
@@ -8455,7 +8579,7 @@
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B62" s="0" t="n">
         <v>1</v>
@@ -8470,7 +8594,7 @@
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B63" s="0" t="n">
         <v>2</v>
@@ -8485,7 +8609,7 @@
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B64" s="0" t="n">
         <v>3</v>
@@ -8500,7 +8624,7 @@
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B65" s="0" t="n">
         <v>4</v>
@@ -8515,7 +8639,7 @@
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B66" s="0" t="n">
         <v>5</v>
@@ -8530,7 +8654,7 @@
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B67" s="0" t="n">
         <v>6</v>
@@ -8545,7 +8669,7 @@
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B68" s="0" t="n">
         <v>7</v>
@@ -8560,7 +8684,7 @@
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="B69" s="0" t="n">
         <v>0</v>
@@ -8575,7 +8699,7 @@
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="B70" s="0" t="n">
         <v>1</v>
@@ -8590,7 +8714,7 @@
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="B71" s="0" t="n">
         <v>2</v>
@@ -8605,7 +8729,7 @@
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="B72" s="0" t="n">
         <v>3</v>
@@ -8620,7 +8744,7 @@
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="B73" s="0" t="n">
         <v>4</v>
@@ -8635,7 +8759,7 @@
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="B74" s="0" t="n">
         <v>5</v>
@@ -8650,7 +8774,7 @@
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="B75" s="0" t="n">
         <v>6</v>
@@ -8665,7 +8789,7 @@
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="B76" s="0" t="n">
         <v>7</v>
@@ -8680,7 +8804,7 @@
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="B77" s="0" t="n">
         <v>0</v>
@@ -8695,7 +8819,7 @@
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="B78" s="0" t="n">
         <v>1</v>
@@ -8710,7 +8834,7 @@
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="B79" s="0" t="n">
         <v>2</v>
@@ -8725,7 +8849,7 @@
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="B80" s="0" t="n">
         <v>3</v>
@@ -8740,7 +8864,7 @@
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="B81" s="0" t="n">
         <v>4</v>
@@ -8755,7 +8879,7 @@
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="B82" s="0" t="n">
         <v>5</v>
@@ -8770,7 +8894,7 @@
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="B83" s="0" t="n">
         <v>6</v>
@@ -8785,7 +8909,7 @@
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="B84" s="0" t="n">
         <v>7</v>
@@ -8800,7 +8924,7 @@
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="6" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="B85" s="0" t="n">
         <v>0</v>
@@ -8815,7 +8939,7 @@
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="6" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="B86" s="0" t="n">
         <v>1</v>
@@ -8830,7 +8954,7 @@
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="6" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="B87" s="0" t="n">
         <v>2</v>
@@ -8845,7 +8969,7 @@
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="6" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="B88" s="0" t="n">
         <v>3</v>
@@ -8860,7 +8984,7 @@
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="B89" s="0" t="n">
         <v>4</v>
@@ -8875,7 +8999,7 @@
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="B90" s="0" t="n">
         <v>5</v>
@@ -8890,7 +9014,7 @@
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="B91" s="0" t="n">
         <v>6</v>
@@ -8905,7 +9029,7 @@
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="B92" s="0" t="n">
         <v>7</v>
@@ -8920,7 +9044,7 @@
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="B93" s="0" t="n">
         <v>0</v>
@@ -8935,7 +9059,7 @@
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="B94" s="0" t="n">
         <v>1</v>
@@ -8950,7 +9074,7 @@
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="B95" s="0" t="n">
         <v>2</v>
@@ -8965,7 +9089,7 @@
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="B96" s="0" t="n">
         <v>3</v>
@@ -8980,7 +9104,7 @@
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="B97" s="0" t="n">
         <v>4</v>
@@ -8995,7 +9119,7 @@
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="B98" s="0" t="n">
         <v>5</v>
@@ -9010,7 +9134,7 @@
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="B99" s="0" t="n">
         <v>6</v>
@@ -9025,7 +9149,7 @@
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="B100" s="0" t="n">
         <v>7</v>
@@ -9040,7 +9164,7 @@
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="B101" s="0" t="n">
         <v>0</v>
@@ -9055,7 +9179,7 @@
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="B102" s="0" t="n">
         <v>1</v>
@@ -9070,7 +9194,7 @@
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="B103" s="0" t="n">
         <v>2</v>
@@ -9085,7 +9209,7 @@
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="B104" s="0" t="n">
         <v>3</v>
@@ -9100,7 +9224,7 @@
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="B105" s="0" t="n">
         <v>4</v>
@@ -9115,7 +9239,7 @@
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="B106" s="0" t="n">
         <v>5</v>
@@ -9130,7 +9254,7 @@
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="B107" s="0" t="n">
         <v>6</v>
@@ -9145,7 +9269,7 @@
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="B108" s="0" t="n">
         <v>7</v>
@@ -9160,7 +9284,7 @@
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="B109" s="0" t="n">
         <v>0</v>
@@ -9175,7 +9299,7 @@
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="B110" s="0" t="n">
         <v>1</v>
@@ -9190,7 +9314,7 @@
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="B111" s="0" t="n">
         <v>2</v>
@@ -9205,7 +9329,7 @@
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="B112" s="0" t="n">
         <v>3</v>
@@ -9220,7 +9344,7 @@
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="B113" s="0" t="n">
         <v>4</v>
@@ -9235,7 +9359,7 @@
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="B114" s="0" t="n">
         <v>5</v>
@@ -9250,7 +9374,7 @@
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="B115" s="0" t="n">
         <v>6</v>
@@ -9265,7 +9389,7 @@
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="B116" s="0" t="n">
         <v>7</v>
@@ -9280,7 +9404,7 @@
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="B117" s="0" t="n">
         <v>0</v>
@@ -9295,7 +9419,7 @@
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="B118" s="0" t="n">
         <v>1</v>
@@ -9310,7 +9434,7 @@
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="B119" s="0" t="n">
         <v>2</v>
@@ -9325,7 +9449,7 @@
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="B120" s="0" t="n">
         <v>3</v>
@@ -9340,7 +9464,7 @@
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="B121" s="0" t="n">
         <v>4</v>
@@ -9355,7 +9479,7 @@
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="B122" s="0" t="n">
         <v>5</v>
@@ -9370,7 +9494,7 @@
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="B123" s="0" t="n">
         <v>6</v>
@@ -9385,7 +9509,7 @@
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="B124" s="0" t="n">
         <v>0</v>
@@ -9400,7 +9524,7 @@
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="B125" s="0" t="n">
         <v>1</v>
@@ -9415,7 +9539,7 @@
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="B126" s="0" t="n">
         <v>2</v>
@@ -9430,7 +9554,7 @@
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="B127" s="0" t="n">
         <v>3</v>
@@ -9445,7 +9569,7 @@
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="B128" s="0" t="n">
         <v>4</v>
@@ -9460,7 +9584,7 @@
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="B129" s="0" t="n">
         <v>5</v>
@@ -9475,7 +9599,7 @@
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="B130" s="0" t="n">
         <v>6</v>
@@ -9490,7 +9614,7 @@
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="B131" s="0" t="n">
         <v>7</v>
@@ -9505,7 +9629,7 @@
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="B132" s="0" t="n">
         <v>0</v>
@@ -9520,7 +9644,7 @@
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="B133" s="0" t="n">
         <v>1</v>
@@ -9535,7 +9659,7 @@
     </row>
     <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="B134" s="0" t="n">
         <v>2</v>
@@ -9550,7 +9674,7 @@
     </row>
     <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="B135" s="0" t="n">
         <v>3</v>
@@ -9565,7 +9689,7 @@
     </row>
     <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="B136" s="0" t="n">
         <v>4</v>
@@ -9580,7 +9704,7 @@
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="B137" s="0" t="n">
         <v>5</v>
@@ -9595,7 +9719,7 @@
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="6" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="B138" s="0" t="n">
         <v>3</v>
@@ -9610,7 +9734,7 @@
     </row>
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="B139" s="0" t="n">
         <v>4</v>
@@ -9625,7 +9749,7 @@
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="B140" s="0" t="n">
         <v>5</v>
@@ -9640,7 +9764,7 @@
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="B141" s="0" t="n">
         <v>6</v>
@@ -9655,7 +9779,7 @@
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="B142" s="0" t="n">
         <v>7</v>
@@ -9670,7 +9794,7 @@
     </row>
     <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="B143" s="0" t="n">
         <v>7</v>
@@ -9684,453 +9808,753 @@
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="B144" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="C144" s="4" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="D144" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C144, Levels!B:B, 0), 1, 1)),", ",IF(A144 &lt;&gt; "", """mem"": bit" &amp; B144 &amp; "(" &amp; A144 &amp; "),", ""),"""good"": ",IF(A144 &lt;&gt; "", 1, 0),"},")</f>
-        <v>143: { "levelId": 3, "good": 0},</v>
+        <v>143: { "levelId": 8, "mem": bit3(0x22499b),"good": 1},</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="B145" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="C145" s="4" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="D145" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C145, Levels!B:B, 0), 1, 1)),", ",IF(A145 &lt;&gt; "", """mem"": bit" &amp; B145 &amp; "(" &amp; A145 &amp; "),", ""),"""good"": ",IF(A145 &lt;&gt; "", 1, 0),"},")</f>
-        <v>144: { "levelId": 3, "good": 0},</v>
+        <v>144: { "levelId": 8, "mem": bit4(0x22499b),"good": 1},</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="B146" s="0" t="n">
+        <v>5</v>
+      </c>
       <c r="C146" s="4" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="D146" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C146, Levels!B:B, 0), 1, 1)),", ",IF(A146 &lt;&gt; "", """mem"": bit" &amp; B146 &amp; "(" &amp; A146 &amp; "),", ""),"""good"": ",IF(A146 &lt;&gt; "", 1, 0),"},")</f>
-        <v>145: { "levelId": 3, "good": 0},</v>
+        <v>145: { "levelId": 8, "mem": bit5(0x22499b),"good": 1},</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B147" s="0" t="n">
+        <v>5</v>
+      </c>
       <c r="C147" s="4" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="D147" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C147, Levels!B:B, 0), 1, 1)),", ",IF(A147 &lt;&gt; "", """mem"": bit" &amp; B147 &amp; "(" &amp; A147 &amp; "),", ""),"""good"": ",IF(A147 &lt;&gt; "", 1, 0),"},")</f>
-        <v>146: { "levelId": 3, "good": 0},</v>
+        <v>146: { "levelId": 8, "mem": bit5(0x22499c),"good": 1},</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A148" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B148" s="0" t="n">
+        <v>6</v>
+      </c>
       <c r="C148" s="4" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="D148" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C148, Levels!B:B, 0), 1, 1)),", ",IF(A148 &lt;&gt; "", """mem"": bit" &amp; B148 &amp; "(" &amp; A148 &amp; "),", ""),"""good"": ",IF(A148 &lt;&gt; "", 1, 0),"},")</f>
-        <v>147: { "levelId": 3, "good": 0},</v>
+        <v>147: { "levelId": 8, "mem": bit6(0x22499c),"good": 1},</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B149" s="0" t="n">
+        <v>7</v>
+      </c>
       <c r="C149" s="4" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="D149" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C149, Levels!B:B, 0), 1, 1)),", ",IF(A149 &lt;&gt; "", """mem"": bit" &amp; B149 &amp; "(" &amp; A149 &amp; "),", ""),"""good"": ",IF(A149 &lt;&gt; "", 1, 0),"},")</f>
-        <v>148: { "levelId": 3, "good": 0},</v>
+        <v>148: { "levelId": 8, "mem": bit7(0x22499c),"good": 1},</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="B150" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="C150" s="4" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="D150" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C150, Levels!B:B, 0), 1, 1)),", ",IF(A150 &lt;&gt; "", """mem"": bit" &amp; B150 &amp; "(" &amp; A150 &amp; "),", ""),"""good"": ",IF(A150 &lt;&gt; "", 1, 0),"},")</f>
-        <v>149: { "levelId": 3, "good": 0},</v>
+        <v>149: { "levelId": 8, "mem": bit0(0x22499d),"good": 1},</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="B151" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="C151" s="4" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="D151" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C151, Levels!B:B, 0), 1, 1)),", ",IF(A151 &lt;&gt; "", """mem"": bit" &amp; B151 &amp; "(" &amp; A151 &amp; "),", ""),"""good"": ",IF(A151 &lt;&gt; "", 1, 0),"},")</f>
-        <v>150: { "levelId": 3, "good": 0},</v>
+        <v>150: { "levelId": 8, "mem": bit1(0x22499d),"good": 1},</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A152" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="B152" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="C152" s="4" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="D152" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C152, Levels!B:B, 0), 1, 1)),", ",IF(A152 &lt;&gt; "", """mem"": bit" &amp; B152 &amp; "(" &amp; A152 &amp; "),", ""),"""good"": ",IF(A152 &lt;&gt; "", 1, 0),"},")</f>
-        <v>151: { "levelId": 3, "good": 0},</v>
+        <v>151: { "levelId": 8, "mem": bit2(0x22499d),"good": 1},</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="B153" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="C153" s="4" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="D153" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C153, Levels!B:B, 0), 1, 1)),", ",IF(A153 &lt;&gt; "", """mem"": bit" &amp; B153 &amp; "(" &amp; A153 &amp; "),", ""),"""good"": ",IF(A153 &lt;&gt; "", 1, 0),"},")</f>
-        <v>152: { "levelId": 3, "good": 0},</v>
+        <v>152: { "levelId": 8, "mem": bit3(0x22499d),"good": 1},</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="B154" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="C154" s="4" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="D154" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C154, Levels!B:B, 0), 1, 1)),", ",IF(A154 &lt;&gt; "", """mem"": bit" &amp; B154 &amp; "(" &amp; A154 &amp; "),", ""),"""good"": ",IF(A154 &lt;&gt; "", 1, 0),"},")</f>
-        <v>153: { "levelId": 3, "good": 0},</v>
+        <v>153: { "levelId": 8, "mem": bit4(0x22499d),"good": 1},</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="B155" s="0" t="n">
+        <v>5</v>
+      </c>
       <c r="C155" s="4" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="D155" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C155, Levels!B:B, 0), 1, 1)),", ",IF(A155 &lt;&gt; "", """mem"": bit" &amp; B155 &amp; "(" &amp; A155 &amp; "),", ""),"""good"": ",IF(A155 &lt;&gt; "", 1, 0),"},")</f>
-        <v>154: { "levelId": 3, "good": 0},</v>
+        <v>154: { "levelId": 8, "mem": bit5(0x22499d),"good": 1},</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="B156" s="0" t="n">
+        <v>6</v>
+      </c>
       <c r="C156" s="4" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="D156" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C156, Levels!B:B, 0), 1, 1)),", ",IF(A156 &lt;&gt; "", """mem"": bit" &amp; B156 &amp; "(" &amp; A156 &amp; "),", ""),"""good"": ",IF(A156 &lt;&gt; "", 1, 0),"},")</f>
-        <v>155: { "levelId": 3, "good": 0},</v>
+        <v>155: { "levelId": 8, "mem": bit6(0x22499d),"good": 1},</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="B157" s="0" t="n">
+        <v>7</v>
+      </c>
       <c r="C157" s="4" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="D157" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C157, Levels!B:B, 0), 1, 1)),", ",IF(A157 &lt;&gt; "", """mem"": bit" &amp; B157 &amp; "(" &amp; A157 &amp; "),", ""),"""good"": ",IF(A157 &lt;&gt; "", 1, 0),"},")</f>
-        <v>156: { "levelId": 3, "good": 0},</v>
+        <v>156: { "levelId": 8, "mem": bit7(0x22499d),"good": 1},</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="B158" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="C158" s="4" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="D158" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C158, Levels!B:B, 0), 1, 1)),", ",IF(A158 &lt;&gt; "", """mem"": bit" &amp; B158 &amp; "(" &amp; A158 &amp; "),", ""),"""good"": ",IF(A158 &lt;&gt; "", 1, 0),"},")</f>
-        <v>157: { "levelId": 3, "good": 0},</v>
+        <v>157: { "levelId": 8, "mem": bit0(0x22499e),"good": 1},</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="B159" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="C159" s="4" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="D159" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C159, Levels!B:B, 0), 1, 1)),", ",IF(A159 &lt;&gt; "", """mem"": bit" &amp; B159 &amp; "(" &amp; A159 &amp; "),", ""),"""good"": ",IF(A159 &lt;&gt; "", 1, 0),"},")</f>
-        <v>158: { "levelId": 3, "good": 0},</v>
+        <v>158: { "levelId": 8, "mem": bit1(0x22499e),"good": 1},</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="B160" s="0" t="n">
+        <v>6</v>
+      </c>
       <c r="C160" s="4" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="D160" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C160, Levels!B:B, 0), 1, 1)),", ",IF(A160 &lt;&gt; "", """mem"": bit" &amp; B160 &amp; "(" &amp; A160 &amp; "),", ""),"""good"": ",IF(A160 &lt;&gt; "", 1, 0),"},")</f>
-        <v>159: { "levelId": 3, "good": 0},</v>
+        <v>159: { "levelId": 8, "mem": bit6(0x22499a),"good": 1},</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="B161" s="0" t="n">
+        <v>7</v>
+      </c>
       <c r="C161" s="4" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="D161" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C161, Levels!B:B, 0), 1, 1)),", ",IF(A161 &lt;&gt; "", """mem"": bit" &amp; B161 &amp; "(" &amp; A161 &amp; "),", ""),"""good"": ",IF(A161 &lt;&gt; "", 1, 0),"},")</f>
-        <v>160: { "levelId": 3, "good": 0},</v>
+        <v>160: { "levelId": 8, "mem": bit7(0x22499a),"good": 1},</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="B162" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="C162" s="4" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="D162" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C162, Levels!B:B, 0), 1, 1)),", ",IF(A162 &lt;&gt; "", """mem"": bit" &amp; B162 &amp; "(" &amp; A162 &amp; "),", ""),"""good"": ",IF(A162 &lt;&gt; "", 1, 0),"},")</f>
-        <v>161: { "levelId": 3, "good": 0},</v>
+        <v>161: { "levelId": 8, "mem": bit0(0x22499b),"good": 1},</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A163" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="B163" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="C163" s="4" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="D163" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C163, Levels!B:B, 0), 1, 1)),", ",IF(A163 &lt;&gt; "", """mem"": bit" &amp; B163 &amp; "(" &amp; A163 &amp; "),", ""),"""good"": ",IF(A163 &lt;&gt; "", 1, 0),"},")</f>
-        <v>162: { "levelId": 3, "good": 0},</v>
+        <v>162: { "levelId": 8, "mem": bit1(0x22499b),"good": 1},</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="B164" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="C164" s="4" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="D164" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C164, Levels!B:B, 0), 1, 1)),", ",IF(A164 &lt;&gt; "", """mem"": bit" &amp; B164 &amp; "(" &amp; A164 &amp; "),", ""),"""good"": ",IF(A164 &lt;&gt; "", 1, 0),"},")</f>
-        <v>163: { "levelId": 3, "good": 0},</v>
+        <v>163: { "levelId": 8, "mem": bit2(0x22499b),"good": 1},</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A165" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="B165" s="0" t="n">
+        <v>6</v>
+      </c>
       <c r="C165" s="4" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="D165" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C165, Levels!B:B, 0), 1, 1)),", ",IF(A165 &lt;&gt; "", """mem"": bit" &amp; B165 &amp; "(" &amp; A165 &amp; "),", ""),"""good"": ",IF(A165 &lt;&gt; "", 1, 0),"},")</f>
-        <v>164: { "levelId": 3, "good": 0},</v>
+        <v>164: { "levelId": 8, "mem": bit6(0x22499b),"good": 1},</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="B166" s="0" t="n">
+        <v>7</v>
+      </c>
       <c r="C166" s="4" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="D166" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C166, Levels!B:B, 0), 1, 1)),", ",IF(A166 &lt;&gt; "", """mem"": bit" &amp; B166 &amp; "(" &amp; A166 &amp; "),", ""),"""good"": ",IF(A166 &lt;&gt; "", 1, 0),"},")</f>
-        <v>165: { "levelId": 3, "good": 0},</v>
+        <v>165: { "levelId": 8, "mem": bit7(0x22499b),"good": 1},</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B167" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="C167" s="4" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="D167" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C167, Levels!B:B, 0), 1, 1)),", ",IF(A167 &lt;&gt; "", """mem"": bit" &amp; B167 &amp; "(" &amp; A167 &amp; "),", ""),"""good"": ",IF(A167 &lt;&gt; "", 1, 0),"},")</f>
-        <v>166: { "levelId": 3, "good": 0},</v>
+        <v>166: { "levelId": 8, "mem": bit0(0x22499c),"good": 1},</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B168" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="C168" s="4" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="D168" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C168, Levels!B:B, 0), 1, 1)),", ",IF(A168 &lt;&gt; "", """mem"": bit" &amp; B168 &amp; "(" &amp; A168 &amp; "),", ""),"""good"": ",IF(A168 &lt;&gt; "", 1, 0),"},")</f>
-        <v>167: { "levelId": 3, "good": 0},</v>
+        <v>167: { "levelId": 8, "mem": bit1(0x22499c),"good": 1},</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B169" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="C169" s="4" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="D169" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C169, Levels!B:B, 0), 1, 1)),", ",IF(A169 &lt;&gt; "", """mem"": bit" &amp; B169 &amp; "(" &amp; A169 &amp; "),", ""),"""good"": ",IF(A169 &lt;&gt; "", 1, 0),"},")</f>
-        <v>168: { "levelId": 3, "good": 0},</v>
+        <v>168: { "levelId": 8, "mem": bit2(0x22499c),"good": 1},</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B170" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="C170" s="4" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="D170" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C170, Levels!B:B, 0), 1, 1)),", ",IF(A170 &lt;&gt; "", """mem"": bit" &amp; B170 &amp; "(" &amp; A170 &amp; "),", ""),"""good"": ",IF(A170 &lt;&gt; "", 1, 0),"},")</f>
-        <v>169: { "levelId": 3, "good": 0},</v>
+        <v>169: { "levelId": 8, "mem": bit3(0x22499c),"good": 1},</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B171" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="C171" s="4" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="D171" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C171, Levels!B:B, 0), 1, 1)),", ",IF(A171 &lt;&gt; "", """mem"": bit" &amp; B171 &amp; "(" &amp; A171 &amp; "),", ""),"""good"": ",IF(A171 &lt;&gt; "", 1, 0),"},")</f>
-        <v>170: { "levelId": 3, "good": 0},</v>
+        <v>170: { "levelId": 8, "mem": bit4(0x22499c),"good": 1},</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="B172" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="C172" s="4" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="D172" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C172, Levels!B:B, 0), 1, 1)),", ",IF(A172 &lt;&gt; "", """mem"": bit" &amp; B172 &amp; "(" &amp; A172 &amp; "),", ""),"""good"": ",IF(A172 &lt;&gt; "", 1, 0),"},")</f>
-        <v>171: { "levelId": 3, "good": 0},</v>
+        <v>171: { "levelId": 8, "mem": bit2(0x22499e),"good": 1},</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A173" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="B173" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="C173" s="4" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="D173" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C173, Levels!B:B, 0), 1, 1)),", ",IF(A173 &lt;&gt; "", """mem"": bit" &amp; B173 &amp; "(" &amp; A173 &amp; "),", ""),"""good"": ",IF(A173 &lt;&gt; "", 1, 0),"},")</f>
-        <v>172: { "levelId": 3, "good": 0},</v>
+        <v>172: { "levelId": 8, "mem": bit3(0x22499e),"good": 1},</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A174" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="B174" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="C174" s="4" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="D174" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C174, Levels!B:B, 0), 1, 1)),", ",IF(A174 &lt;&gt; "", """mem"": bit" &amp; B174 &amp; "(" &amp; A174 &amp; "),", ""),"""good"": ",IF(A174 &lt;&gt; "", 1, 0),"},")</f>
-        <v>173: { "levelId": 3, "good": 0},</v>
+        <v>173: { "levelId": 8, "mem": bit4(0x22499e),"good": 1},</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="B175" s="0" t="n">
+        <v>5</v>
+      </c>
       <c r="C175" s="4" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="D175" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C175, Levels!B:B, 0), 1, 1)),", ",IF(A175 &lt;&gt; "", """mem"": bit" &amp; B175 &amp; "(" &amp; A175 &amp; "),", ""),"""good"": ",IF(A175 &lt;&gt; "", 1, 0),"},")</f>
-        <v>174: { "levelId": 3, "good": 0},</v>
+        <v>174: { "levelId": 8, "mem": bit5(0x22499e),"good": 1},</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A176" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="B176" s="0" t="n">
+        <v>6</v>
+      </c>
       <c r="C176" s="4" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="D176" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C176, Levels!B:B, 0), 1, 1)),", ",IF(A176 &lt;&gt; "", """mem"": bit" &amp; B176 &amp; "(" &amp; A176 &amp; "),", ""),"""good"": ",IF(A176 &lt;&gt; "", 1, 0),"},")</f>
-        <v>175: { "levelId": 3, "good": 0},</v>
+        <v>175: { "levelId": 8, "mem": bit6(0x22499e),"good": 1},</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="B177" s="0" t="n">
+        <v>7</v>
+      </c>
       <c r="C177" s="4" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="D177" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C177, Levels!B:B, 0), 1, 1)),", ",IF(A177 &lt;&gt; "", """mem"": bit" &amp; B177 &amp; "(" &amp; A177 &amp; "),", ""),"""good"": ",IF(A177 &lt;&gt; "", 1, 0),"},")</f>
-        <v>176: { "levelId": 3, "good": 0},</v>
+        <v>176: { "levelId": 8, "mem": bit7(0x22499e),"good": 1},</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A178" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="B178" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="C178" s="4" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="D178" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C178, Levels!B:B, 0), 1, 1)),", ",IF(A178 &lt;&gt; "", """mem"": bit" &amp; B178 &amp; "(" &amp; A178 &amp; "),", ""),"""good"": ",IF(A178 &lt;&gt; "", 1, 0),"},")</f>
-        <v>177: { "levelId": 3, "good": 0},</v>
+        <v>177: { "levelId": 8, "mem": bit0(0x22499f),"good": 1},</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A179" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="B179" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="C179" s="4" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="D179" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C179, Levels!B:B, 0), 1, 1)),", ",IF(A179 &lt;&gt; "", """mem"": bit" &amp; B179 &amp; "(" &amp; A179 &amp; "),", ""),"""good"": ",IF(A179 &lt;&gt; "", 1, 0),"},")</f>
-        <v>178: { "levelId": 3, "good": 0},</v>
+        <v>178: { "levelId": 8, "mem": bit1(0x22499f),"good": 1},</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A180" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="B180" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="C180" s="4" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="D180" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C180, Levels!B:B, 0), 1, 1)),", ",IF(A180 &lt;&gt; "", """mem"": bit" &amp; B180 &amp; "(" &amp; A180 &amp; "),", ""),"""good"": ",IF(A180 &lt;&gt; "", 1, 0),"},")</f>
-        <v>179: { "levelId": 3, "good": 0},</v>
+        <v>179: { "levelId": 8, "mem": bit2(0x22499f),"good": 1},</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A181" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="B181" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="C181" s="4" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="D181" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C181, Levels!B:B, 0), 1, 1)),", ",IF(A181 &lt;&gt; "", """mem"": bit" &amp; B181 &amp; "(" &amp; A181 &amp; "),", ""),"""good"": ",IF(A181 &lt;&gt; "", 1, 0),"},")</f>
-        <v>180: { "levelId": 3, "good": 0},</v>
+        <v>180: { "levelId": 8, "mem": bit3(0x22499f),"good": 1},</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A182" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="B182" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="C182" s="4" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="D182" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C182, Levels!B:B, 0), 1, 1)),", ",IF(A182 &lt;&gt; "", """mem"": bit" &amp; B182 &amp; "(" &amp; A182 &amp; "),", ""),"""good"": ",IF(A182 &lt;&gt; "", 1, 0),"},")</f>
-        <v>181: { "levelId": 3, "good": 0},</v>
+        <v>181: { "levelId": 8, "mem": bit4(0x22499f),"good": 1},</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A183" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="B183" s="0" t="n">
+        <v>5</v>
+      </c>
       <c r="C183" s="4" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="D183" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C183, Levels!B:B, 0), 1, 1)),", ",IF(A183 &lt;&gt; "", """mem"": bit" &amp; B183 &amp; "(" &amp; A183 &amp; "),", ""),"""good"": ",IF(A183 &lt;&gt; "", 1, 0),"},")</f>
-        <v>182: { "levelId": 3, "good": 0},</v>
+        <v>182: { "levelId": 8, "mem": bit5(0x22499f),"good": 1},</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A184" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="B184" s="0" t="n">
+        <v>6</v>
+      </c>
       <c r="C184" s="4" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="D184" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C184, Levels!B:B, 0), 1, 1)),", ",IF(A184 &lt;&gt; "", """mem"": bit" &amp; B184 &amp; "(" &amp; A184 &amp; "),", ""),"""good"": ",IF(A184 &lt;&gt; "", 1, 0),"},")</f>
-        <v>183: { "levelId": 3, "good": 0},</v>
+        <v>183: { "levelId": 8, "mem": bit6(0x22499f),"good": 1},</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A185" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="B185" s="0" t="n">
+        <v>7</v>
+      </c>
       <c r="C185" s="4" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="D185" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C185, Levels!B:B, 0), 1, 1)),", ",IF(A185 &lt;&gt; "", """mem"": bit" &amp; B185 &amp; "(" &amp; A185 &amp; "),", ""),"""good"": ",IF(A185 &lt;&gt; "", 1, 0),"},")</f>
-        <v>184: { "levelId": 3, "good": 0},</v>
+        <v>184: { "levelId": 8, "mem": bit7(0x22499f),"good": 1},</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A186" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B186" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="C186" s="4" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="D186" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C186, Levels!B:B, 0), 1, 1)),", ",IF(A186 &lt;&gt; "", """mem"": bit" &amp; B186 &amp; "(" &amp; A186 &amp; "),", ""),"""good"": ",IF(A186 &lt;&gt; "", 1, 0),"},")</f>
-        <v>185: { "levelId": 3, "good": 0},</v>
+        <v>185: { "levelId": 8, "mem": bit0(0x2249a0),"good": 1},</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A187" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B187" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="C187" s="4" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="D187" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C187, Levels!B:B, 0), 1, 1)),", ",IF(A187 &lt;&gt; "", """mem"": bit" &amp; B187 &amp; "(" &amp; A187 &amp; "),", ""),"""good"": ",IF(A187 &lt;&gt; "", 1, 0),"},")</f>
-        <v>186: { "levelId": 3, "good": 0},</v>
+        <v>186: { "levelId": 8, "mem": bit1(0x2249a0),"good": 1},</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A188" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B188" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="C188" s="4" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="D188" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C188, Levels!B:B, 0), 1, 1)),", ",IF(A188 &lt;&gt; "", """mem"": bit" &amp; B188 &amp; "(" &amp; A188 &amp; "),", ""),"""good"": ",IF(A188 &lt;&gt; "", 1, 0),"},")</f>
-        <v>187: { "levelId": 3, "good": 0},</v>
+        <v>187: { "levelId": 8, "mem": bit2(0x2249a0),"good": 1},</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A189" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B189" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="C189" s="4" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="D189" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C189, Levels!B:B, 0), 1, 1)),", ",IF(A189 &lt;&gt; "", """mem"": bit" &amp; B189 &amp; "(" &amp; A189 &amp; "),", ""),"""good"": ",IF(A189 &lt;&gt; "", 1, 0),"},")</f>
-        <v>188: { "levelId": 3, "good": 0},</v>
+        <v>188: { "levelId": 8, "mem": bit3(0x2249a0),"good": 1},</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A190" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B190" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="C190" s="4" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="D190" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C190, Levels!B:B, 0), 1, 1)),", ",IF(A190 &lt;&gt; "", """mem"": bit" &amp; B190 &amp; "(" &amp; A190 &amp; "),", ""),"""good"": ",IF(A190 &lt;&gt; "", 1, 0),"},")</f>
-        <v>189: { "levelId": 3, "good": 0},</v>
+        <v>189: { "levelId": 8, "mem": bit4(0x2249a0),"good": 1},</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A191" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B191" s="0" t="n">
+        <v>5</v>
+      </c>
       <c r="C191" s="4" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="D191" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C191, Levels!B:B, 0), 1, 1)),", ",IF(A191 &lt;&gt; "", """mem"": bit" &amp; B191 &amp; "(" &amp; A191 &amp; "),", ""),"""good"": ",IF(A191 &lt;&gt; "", 1, 0),"},")</f>
-        <v>190: { "levelId": 3, "good": 0},</v>
+        <v>190: { "levelId": 8, "mem": bit5(0x2249a0),"good": 1},</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A192" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B192" s="0" t="n">
+        <v>6</v>
+      </c>
       <c r="C192" s="4" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="D192" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C192, Levels!B:B, 0), 1, 1)),", ",IF(A192 &lt;&gt; "", """mem"": bit" &amp; B192 &amp; "(" &amp; A192 &amp; "),", ""),"""good"": ",IF(A192 &lt;&gt; "", 1, 0),"},")</f>
-        <v>191: { "levelId": 3, "good": 0},</v>
+        <v>191: { "levelId": 8, "mem": bit6(0x2249a0),"good": 1},</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A193" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B193" s="0" t="n">
+        <v>7</v>
+      </c>
       <c r="C193" s="4" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="D193" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C193, Levels!B:B, 0), 1, 1)),", ",IF(A193 &lt;&gt; "", """mem"": bit" &amp; B193 &amp; "(" &amp; A193 &amp; "),", ""),"""good"": ",IF(A193 &lt;&gt; "", 1, 0),"},")</f>
-        <v>192: { "levelId": 3, "good": 0},</v>
+        <v>192: { "levelId": 8, "mem": bit7(0x2249a0),"good": 1},</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17432,10 +17856,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="B2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
+      <selection pane="bottomLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.93"/>
@@ -17445,13 +17869,13 @@
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>79</v>
+        <v>95</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>4</v>
@@ -17462,7 +17886,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>7</v>
@@ -17476,12 +17900,12 @@
       </c>
       <c r="G2" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D2:D81)</f>
-        <v>1: { "levelId": 1, "mem": bit7(0x2249f0),"good": 1},2: { "levelId": 2, "mem": bit0(0x2249f1),"good": 1},3: { "levelId": 2, "mem": bit1(0x2249f1),"good": 1},4: { "levelId": 2, "mem": bit5(0x2249f1),"good": 1},5: { "levelId": 2, "mem": bit6(0x2249f1),"good": 1},6: { "levelId": 1, "mem": bit7(0x2249f1),"good": 1},7: { "levelId": 5, "mem": bit0(0x2249f2),"good": 1},8: { "levelId": 5, "mem": bit1(0x2249f2),"good": 1},9: { "levelId": 5, "mem": bit2(0x2249f2),"good": 1},10: { "levelId": 5, "mem": bit3(0x2249f2),"good": 1},11: { "levelId": 5, "mem": bit4(0x2249f2),"good": 1},12: { "levelId": 6, "mem": bit5(0x2249f2),"good": 1},13: { "levelId": 6, "mem": bit7(0x2249f2),"good": 1},14: { "levelId": 6, "mem": bit1(0x2249f3),"good": 1},15: { "levelId": 6, "mem": bit6(0x2249f2),"good": 1},16: { "levelId": 6, "mem": bit0(0x2249f3),"good": 1},17: { "levelId": 6, "mem": bit3(0x2249f3),"good": 1},18: { "levelId": 6, "mem": bit2(0x2249f3),"good": 1},19: { "levelId": 3, "good": 0},20: { "levelId": 3, "good": 0},21: { "levelId": 3, "good": 0},22: { "levelId": 3, "good": 0},23: { "levelId": 3, "good": 0},24: { "levelId": 3, "good": 0},25: { "levelId": 3, "good": 0},26: { "levelId": 3, "good": 0},27: { "levelId": 3, "good": 0},28: { "levelId": 3, "good": 0},29: { "levelId": 3, "good": 0},30: { "levelId": 3, "good": 0},31: { "levelId": 3, "good": 0},32: { "levelId": 3, "good": 0},33: { "levelId": 3, "good": 0},34: { "levelId": 3, "good": 0},35: { "levelId": 3, "good": 0},36: { "levelId": 3, "good": 0},37: { "levelId": 3, "good": 0},38: { "levelId": 3, "good": 0},39: { "levelId": 3, "good": 0},40: { "levelId": 3, "good": 0},41: { "levelId": 3, "good": 0},42: { "levelId": 3, "good": 0},43: { "levelId": 3, "good": 0},44: { "levelId": 3, "good": 0},45: { "levelId": 3, "good": 0},46: { "levelId": 3, "good": 0},47: { "levelId": 3, "good": 0},48: { "levelId": 3, "good": 0},49: { "levelId": 3, "good": 0},50: { "levelId": 3, "good": 0},51: { "levelId": 3, "good": 0},52: { "levelId": 3, "good": 0},53: { "levelId": 3, "good": 0},54: { "levelId": 3, "good": 0},55: { "levelId": 3, "good": 0},56: { "levelId": 3, "good": 0},57: { "levelId": 3, "good": 0},58: { "levelId": 3, "good": 0},59: { "levelId": 3, "good": 0},60: { "levelId": 3, "good": 0},61: { "levelId": 3, "good": 0},62: { "levelId": 3, "good": 0},63: { "levelId": 3, "good": 0},64: { "levelId": 3, "good": 0},65: { "levelId": 3, "good": 0},66: { "levelId": 3, "good": 0},67: { "levelId": 3, "good": 0},68: { "levelId": 3, "good": 0},69: { "levelId": 3, "good": 0},70: { "levelId": 3, "good": 0},71: { "levelId": 3, "good": 0},72: { "levelId": 3, "good": 0},73: { "levelId": 3, "good": 0},74: { "levelId": 3, "good": 0},75: { "levelId": 3, "good": 0},76: { "levelId": 3, "good": 0},77: { "levelId": 3, "good": 0},78: { "levelId": 3, "good": 0},79: { "levelId": 3, "good": 0},80: { "levelId": 3, "good": 0},</v>
+        <v>1: { "levelId": 1, "mem": bit7(0x2249f0),"good": 1},2: { "levelId": 2, "mem": bit0(0x2249f1),"good": 1},3: { "levelId": 2, "mem": bit1(0x2249f1),"good": 1},4: { "levelId": 2, "mem": bit5(0x2249f1),"good": 1},5: { "levelId": 2, "mem": bit6(0x2249f1),"good": 1},6: { "levelId": 1, "mem": bit7(0x2249f1),"good": 1},7: { "levelId": 5, "mem": bit0(0x2249f2),"good": 1},8: { "levelId": 5, "mem": bit1(0x2249f2),"good": 1},9: { "levelId": 5, "mem": bit2(0x2249f2),"good": 1},10: { "levelId": 5, "mem": bit3(0x2249f2),"good": 1},11: { "levelId": 5, "mem": bit4(0x2249f2),"good": 1},12: { "levelId": 6, "mem": bit5(0x2249f2),"good": 1},13: { "levelId": 6, "mem": bit7(0x2249f2),"good": 1},14: { "levelId": 6, "mem": bit1(0x2249f3),"good": 1},15: { "levelId": 6, "mem": bit6(0x2249f2),"good": 1},16: { "levelId": 6, "mem": bit0(0x2249f3),"good": 1},17: { "levelId": 6, "mem": bit3(0x2249f3),"good": 1},18: { "levelId": 6, "mem": bit2(0x2249f3),"good": 1},19: { "levelId": 8, "mem": bit5(0x2249f3),"good": 1},20: { "levelId": 8, "mem": bit4(0x2249f3),"good": 1},21: { "levelId": 3, "good": 0},22: { "levelId": 3, "good": 0},23: { "levelId": 3, "good": 0},24: { "levelId": 3, "good": 0},25: { "levelId": 3, "good": 0},26: { "levelId": 3, "good": 0},27: { "levelId": 3, "good": 0},28: { "levelId": 3, "good": 0},29: { "levelId": 3, "good": 0},30: { "levelId": 3, "good": 0},31: { "levelId": 3, "good": 0},32: { "levelId": 3, "good": 0},33: { "levelId": 3, "good": 0},34: { "levelId": 3, "good": 0},35: { "levelId": 3, "good": 0},36: { "levelId": 3, "good": 0},37: { "levelId": 3, "good": 0},38: { "levelId": 3, "good": 0},39: { "levelId": 3, "good": 0},40: { "levelId": 3, "good": 0},41: { "levelId": 3, "good": 0},42: { "levelId": 3, "good": 0},43: { "levelId": 3, "good": 0},44: { "levelId": 3, "good": 0},45: { "levelId": 3, "good": 0},46: { "levelId": 3, "good": 0},47: { "levelId": 3, "good": 0},48: { "levelId": 3, "good": 0},49: { "levelId": 3, "good": 0},50: { "levelId": 3, "good": 0},51: { "levelId": 3, "good": 0},52: { "levelId": 3, "good": 0},53: { "levelId": 3, "good": 0},54: { "levelId": 3, "good": 0},55: { "levelId": 3, "good": 0},56: { "levelId": 3, "good": 0},57: { "levelId": 3, "good": 0},58: { "levelId": 3, "good": 0},59: { "levelId": 3, "good": 0},60: { "levelId": 3, "good": 0},61: { "levelId": 3, "good": 0},62: { "levelId": 3, "good": 0},63: { "levelId": 3, "good": 0},64: { "levelId": 3, "good": 0},65: { "levelId": 3, "good": 0},66: { "levelId": 3, "good": 0},67: { "levelId": 3, "good": 0},68: { "levelId": 3, "good": 0},69: { "levelId": 3, "good": 0},70: { "levelId": 3, "good": 0},71: { "levelId": 3, "good": 0},72: { "levelId": 3, "good": 0},73: { "levelId": 3, "good": 0},74: { "levelId": 3, "good": 0},75: { "levelId": 3, "good": 0},76: { "levelId": 3, "good": 0},77: { "levelId": 3, "good": 0},78: { "levelId": 3, "good": 0},79: { "levelId": 3, "good": 0},80: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>81</v>
+        <v>97</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0</v>
@@ -17496,7 +17920,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>81</v>
+        <v>97</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>1</v>
@@ -17511,7 +17935,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>81</v>
+        <v>97</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>5</v>
@@ -17526,7 +17950,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>81</v>
+        <v>97</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>6</v>
@@ -17541,7 +17965,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>81</v>
+        <v>97</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>7</v>
@@ -17556,7 +17980,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>0</v>
@@ -17571,7 +17995,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>1</v>
@@ -17586,7 +18010,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>2</v>
@@ -17601,7 +18025,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>3</v>
@@ -17616,7 +18040,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>4</v>
@@ -17631,7 +18055,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>5</v>
@@ -17646,7 +18070,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>7</v>
@@ -17661,7 +18085,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>1</v>
@@ -17676,7 +18100,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>6</v>
@@ -17691,7 +18115,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>0</v>
@@ -17706,7 +18130,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>3</v>
@@ -17721,7 +18145,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>2</v>
@@ -17735,21 +18159,33 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>5</v>
+      </c>
       <c r="C20" s="4" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="D20" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C20, Levels!B:B, 0), 1, 1)),", ",IF(A20 &lt;&gt; "", """mem"": bit" &amp; B20 &amp; "(" &amp; A20 &amp; "),", ""),"""good"": ",IF(A20 &lt;&gt; "", 1, 0),"},")</f>
-        <v>19: { "levelId": 3, "good": 0},</v>
+        <v>19: { "levelId": 8, "mem": bit5(0x2249f3),"good": 1},</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="C21" s="4" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="D21" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C21, Levels!B:B, 0), 1, 1)),", ",IF(A21 &lt;&gt; "", """mem"": bit" &amp; B21 &amp; "(" &amp; A21 &amp; "),", ""),"""good"": ",IF(A21 &lt;&gt; "", 1, 0),"},")</f>
-        <v>20: { "levelId": 3, "good": 0},</v>
+        <v>20: { "levelId": 8, "mem": bit4(0x2249f3),"good": 1},</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Documented additional Lums and Cages from the Menhir Hills and removed a couple of extraneous achievements.
</commit_message>
<xml_diff>
--- a/Rayman 2.xlsx
+++ b/Rayman 2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Areas" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1400" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1438" uniqueCount="115">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -208,6 +208,33 @@
     <t xml:space="preserve">0</t>
   </si>
   <si>
+    <t xml:space="preserve">751974</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bonus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">in the bonus stage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">776C08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MenhirArea1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">in the Menhir Hills</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Menhir Hills</t>
+  </si>
+  <si>
+    <t xml:space="preserve">78FBD8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MenhirArea2</t>
+  </si>
+  <si>
     <t xml:space="preserve">Index</t>
   </si>
   <si>
@@ -310,6 +337,21 @@
     <t xml:space="preserve">0x2249a0</t>
   </si>
   <si>
+    <t xml:space="preserve">0x2249a1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x2249a2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x2249a4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x2249a3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x2249a5</t>
+  </si>
+  <si>
     <t xml:space="preserve">Level ID</t>
   </si>
   <si>
@@ -323,6 +365,9 @@
   </si>
   <si>
     <t xml:space="preserve">0x2249f3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x2249f4</t>
   </si>
 </sst>
 </file>
@@ -530,19 +575,19 @@
   </sheetPr>
   <dimension ref="A1:H1015"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
+      <selection pane="bottomLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.04"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -566,7 +611,7 @@
       </c>
       <c r="H1" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(E2:E1000)</f>
-        <v>0x784BFC: { "id": 0x784BFC, "areaName": "Menu", "displayName": "Main Menu", "levelName": "Menu" },0x789668: { "id": 0x789668, "areaName": "Intro", "displayName": "somewhere in the Glade of Dreams…", "levelName": "None" },0x778C74: { "id": 0x778C74, "areaName": "BuccaneerBrig", "displayName": "in the Buccaneer’s brig", "levelName": "None" },0x78D424: { "id": 0x78D424, "areaName": "WoodsOfLight", "displayName": "in the Woods of Light", "levelName": "Woods of Light" },0x790570: { "id": 0x790570, "areaName": "HallOfDoors", "displayName": "in the Hall of Doors", "levelName": "Hall of Doors" },0x7875A8: { "id": 0x7875A8, "areaName": "FairyGladeArea1", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x78A320: { "id": 0x78A320, "areaName": "FairyGladeArea2", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x7A1BD8: { "id": 0x7A1BD8, "areaName": "FairyGladeArea3", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x77BFFC: { "id": 0x77BFFC, "areaName": "FairyGladeArea4", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x771B74: { "id": 0x771B74, "areaName": "FairyGladeArea5", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x74AAA8: { "id": 0x74AAA8, "areaName": "Results", "displayName": "viewing level results…", "levelName": "None" },0x788708: { "id": 0x788708, "areaName": "MarshesArea1", "displayName": "in the Marshes of Awakening", "levelName": "Marshes of Awakening" },0x7786E8: { "id": 0x7786E8, "areaName": "MarshesArea2", "displayName": "in the Marshes of Awakening", "levelName": "Marshes of Awakening" },0x790598: { "id": 0x790598, "areaName": "BayouArea1", "displayName": "in the Bayou", "levelName": "Bayou" },0x788764: { "id": 0x788764, "areaName": "BayouArea2", "displayName": "in the Bayou", "levelName": "Bayou" },0x7928A4: { "id": 0x7928A4, "areaName": "SoWaIArea1", "displayName": "in the Sanctuary of Water and Ice", "levelName": "Sanctuary of Water and Ice" },0x774694: { "id": 0x774694, "areaName": "SoWaIArea2", "displayName": "in the Sanctuary of Water and Ice", "levelName": "Sanctuary of Water and Ice" },0x76F100: { "id": 0x76F100, "areaName": "Polokus", "displayName": "in Polokus’s dream", "levelName": "Polokus" },0x0: { "id": 0x0, "areaName": "None", "displayName": "somewhere in the Glade of Dreams…", "levelName": "None" },</v>
+        <v>0x784BFC: { "id": 0x784BFC, "areaName": "Menu", "displayName": "Main Menu", "levelName": "Menu" },0x789668: { "id": 0x789668, "areaName": "Intro", "displayName": "somewhere in the Glade of Dreams…", "levelName": "None" },0x778C74: { "id": 0x778C74, "areaName": "BuccaneerBrig", "displayName": "in the Buccaneer’s brig", "levelName": "None" },0x78D424: { "id": 0x78D424, "areaName": "WoodsOfLight", "displayName": "in the Woods of Light", "levelName": "Woods of Light" },0x790570: { "id": 0x790570, "areaName": "HallOfDoors", "displayName": "in the Hall of Doors", "levelName": "Hall of Doors" },0x7875A8: { "id": 0x7875A8, "areaName": "FairyGladeArea1", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x78A320: { "id": 0x78A320, "areaName": "FairyGladeArea2", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x7A1BD8: { "id": 0x7A1BD8, "areaName": "FairyGladeArea3", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x77BFFC: { "id": 0x77BFFC, "areaName": "FairyGladeArea4", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x771B74: { "id": 0x771B74, "areaName": "FairyGladeArea5", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x74AAA8: { "id": 0x74AAA8, "areaName": "Results", "displayName": "viewing level results…", "levelName": "None" },0x788708: { "id": 0x788708, "areaName": "MarshesArea1", "displayName": "in the Marshes of Awakening", "levelName": "Marshes of Awakening" },0x7786E8: { "id": 0x7786E8, "areaName": "MarshesArea2", "displayName": "in the Marshes of Awakening", "levelName": "Marshes of Awakening" },0x790598: { "id": 0x790598, "areaName": "BayouArea1", "displayName": "in the Bayou", "levelName": "Bayou" },0x788764: { "id": 0x788764, "areaName": "BayouArea2", "displayName": "in the Bayou", "levelName": "Bayou" },0x7928A4: { "id": 0x7928A4, "areaName": "SoWaIArea1", "displayName": "in the Sanctuary of Water and Ice", "levelName": "Sanctuary of Water and Ice" },0x774694: { "id": 0x774694, "areaName": "SoWaIArea2", "displayName": "in the Sanctuary of Water and Ice", "levelName": "Sanctuary of Water and Ice" },0x76F100: { "id": 0x76F100, "areaName": "Polokus", "displayName": "in Polokus’s dream", "levelName": "Polokus" },0x0: { "id": 0x0, "areaName": "None", "displayName": "somewhere in the Glade of Dreams…", "levelName": "None" },0x751974: { "id": 0x751974, "areaName": "Bonus", "displayName": "in the bonus stage", "levelName": "None" },0x776C08: { "id": 0x776C08, "areaName": "MenhirArea1", "displayName": "in the Menhir Hills", "levelName": "Menhir Hills" },0x78FBD8: { "id": 0x78FBD8, "areaName": "MenhirArea2", "displayName": "in the Menhir Hills", "levelName": "Menhir Hills" },</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -912,13 +957,58 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D21" s="4"/>
+      <c r="A21" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("0x", A21,": { ""id"": ","0x", A21,", ""areaName"": """,B21,""", ""displayName"": """,C21,""", ""levelName"": """,D21,""" },")</f>
+        <v>0x751974: { "id": 0x751974, "areaName": "Bonus", "displayName": "in the bonus stage", "levelName": "None" },</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D22" s="4"/>
+      <c r="A22" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E22" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("0x", A22,": { ""id"": ","0x", A22,", ""areaName"": """,B22,""", ""displayName"": """,C22,""", ""levelName"": """,D22,""" },")</f>
+        <v>0x776C08: { "id": 0x776C08, "areaName": "MenhirArea1", "displayName": "in the Menhir Hills", "levelName": "Menhir Hills" },</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D23" s="4"/>
+      <c r="A23" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E23" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("0x", A23,": { ""id"": ","0x", A23,", ""areaName"": """,B23,""", ""displayName"": """,C23,""", ""levelName"": """,D23,""" },")</f>
+        <v>0x78FBD8: { "id": 0x78FBD8, "areaName": "MenhirArea2", "displayName": "in the Menhir Hills", "levelName": "Menhir Hills" },</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D24" s="4"/>
@@ -3923,10 +4013,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+      <selection pane="bottomLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.21"/>
@@ -3938,22 +4028,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>4</v>
@@ -4029,11 +4119,11 @@
       </c>
       <c r="E4" s="0" t="n">
         <f aca="false">COUNTIFS(Lums!C3:C1002, "=" &amp; B4)</f>
-        <v>808</v>
+        <v>785</v>
       </c>
       <c r="F4" s="0" t="n">
         <f aca="false">COUNTIFS(Cages!C3:C83, "=" &amp; B4)</f>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G4" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A4,": { ""id"": ",A4,", ""name"": """,B4,""", ""lums"": ",C4,", ""cages"": ",D4," },")</f>
@@ -4207,18 +4297,26 @@
         <f aca="false">ROW()-1</f>
         <v>10</v>
       </c>
-      <c r="B11" s="4"/>
+      <c r="B11" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>8</v>
+      </c>
       <c r="E11" s="0" t="n">
         <f aca="false">COUNTIFS(Lums!C10:C1009, "=" &amp; B11)</f>
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="F11" s="0" t="n">
         <f aca="false">COUNTIFS(Cages!C10:C90, "=" &amp; B11)</f>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="G11" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A11,": { ""id"": ",A11,", ""name"": """,B11,""", ""lums"": ",C11,", ""cages"": ",D11," },")</f>
-        <v>10: { "id": 10, "name": "", "lums": , "cages":  },</v>
+        <v>10: { "id": 10, "name": "Menhir Hills", "lums": 50, "cages": 8 },</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7636,13 +7734,13 @@
   </sheetPr>
   <dimension ref="A1:H1001"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A177" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A190" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+      <selection pane="bottomLeft" activeCell="D216" activeCellId="0" sqref="D216"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.93"/>
@@ -7651,10 +7749,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>3</v>
@@ -7667,12 +7765,12 @@
       </c>
       <c r="H1" s="5" t="str">
         <f aca="false">_xlfn.CONCAT(D2:D1001)</f>
-        <v>1: { "levelId": 2, "mem": bit0(0x224988),"good": 1},2: { "levelId": 2, "mem": bit1(0x224988),"good": 1},3: { "levelId": 2, "mem": bit2(0x224988),"good": 1},4: { "levelId": 2, "mem": bit3(0x224988),"good": 1},5: { "levelId": 2, "mem": bit4(0x224988),"good": 1},6: { "levelId": 2, "mem": bit5(0x224988),"good": 1},7: { "levelId": 2, "mem": bit6(0x224988),"good": 1},8: { "levelId": 2, "mem": bit7(0x224988),"good": 1},9: { "levelId": 2, "mem": bit2(0x224989),"good": 1},10: { "levelId": 2, "mem": bit1(0x22498a),"good": 1},11: { "levelId": 2, "mem": bit2(0x22498a),"good": 1},12: { "levelId": 2, "mem": bit3(0x22498a),"good": 1},13: { "levelId": 2, "mem": bit4(0x22498a),"good": 1},14: { "levelId": 2, "mem": bit5(0x22498a),"good": 1},15: { "levelId": 2, "mem": bit6(0x22498a),"good": 1},16: { "levelId": 2, "mem": bit7(0x22498a),"good": 1},17: { "levelId": 2, "mem": bit5(0x22498b),"good": 1},18: { "levelId": 2, "mem": bit6(0x22498b),"good": 1},19: { "levelId": 2, "mem": bit7(0x22498b),"good": 1},20: { "levelId": 2, "mem": bit0(0x22498c),"good": 1},21: { "levelId": 2, "mem": bit1(0x22498c),"good": 1},22: { "levelId": 2, "mem": bit2(0x22498c),"good": 1},23: { "levelId": 2, "mem": bit3(0x22498c),"good": 1},24: { "levelId": 2, "mem": bit4(0x22498c),"good": 1},25: { "levelId": 2, "mem": bit5(0x22498c),"good": 1},26: { "levelId": 2, "mem": bit6(0x22498c),"good": 1},27: { "levelId": 2, "mem": bit7(0x22498c),"good": 1},28: { "levelId": 2, "mem": bit0(0x22498d),"good": 1},29: { "levelId": 2, "mem": bit1(0x22498d),"good": 1},30: { "levelId": 2, "mem": bit2(0x22498d),"good": 1},31: { "levelId": 2, "mem": bit3(0x22498d),"good": 1},32: { "levelId": 2, "mem": bit4(0x22498d),"good": 1},33: { "levelId": 2, "mem": bit5(0x22498d),"good": 1},34: { "levelId": 2, "mem": bit6(0x22498d),"good": 1},35: { "levelId": 2, "mem": bit7(0x22498d),"good": 1},36: { "levelId": 2, "mem": bit0(0x22498e),"good": 1},37: { "levelId": 2, "mem": bit1(0x22498e),"good": 1},38: { "levelId": 5, "mem": bit2(0x22498e),"good": 1},39: { "levelId": 5, "mem": bit3(0x22498e),"good": 1},40: { "levelId": 5, "mem": bit4(0x22498e),"good": 1},41: { "levelId": 5, "mem": bit5(0x22498e),"good": 1},42: { "levelId": 5, "mem": bit6(0x22498e),"good": 1},43: { "levelId": 5, "mem": bit7(0x22498e),"good": 1},44: { "levelId": 5, "mem": bit0(0x22498f),"good": 1},45: { "levelId": 5, "mem": bit1(0x22498f),"good": 1},46: { "levelId": 5, "mem": bit2(0x22498f),"good": 1},47: { "levelId": 5, "mem": bit3(0x22498f),"good": 1},48: { "levelId": 5, "mem": bit4(0x22498f),"good": 1},49: { "levelId": 5, "mem": bit5(0x22498f),"good": 1},50: { "levelId": 5, "mem": bit6(0x22498f),"good": 1},51: { "levelId": 5, "mem": bit7(0x22498f),"good": 1},52: { "levelId": 5, "mem": bit0(0x224990),"good": 1},53: { "levelId": 5, "mem": bit1(0x224990),"good": 1},54: { "levelId": 5, "mem": bit2(0x224990),"good": 1},55: { "levelId": 5, "mem": bit3(0x224990),"good": 1},56: { "levelId": 5, "mem": bit4(0x224990),"good": 1},57: { "levelId": 5, "mem": bit5(0x224990),"good": 1},58: { "levelId": 5, "mem": bit6(0x224990),"good": 1},59: { "levelId": 5, "mem": bit7(0x224990),"good": 1},60: { "levelId": 5, "mem": bit0(0x224991),"good": 1},61: { "levelId": 5, "mem": bit1(0x224991),"good": 1},62: { "levelId": 5, "mem": bit2(0x224991),"good": 1},63: { "levelId": 5, "mem": bit3(0x224991),"good": 1},64: { "levelId": 5, "mem": bit4(0x224991),"good": 1},65: { "levelId": 5, "mem": bit5(0x224991),"good": 1},66: { "levelId": 5, "mem": bit6(0x224991),"good": 1},67: { "levelId": 5, "mem": bit7(0x224991),"good": 1},68: { "levelId": 5, "mem": bit0(0x224992),"good": 1},69: { "levelId": 5, "mem": bit1(0x224992),"good": 1},70: { "levelId": 5, "mem": bit2(0x224992),"good": 1},71: { "levelId": 5, "mem": bit3(0x224992),"good": 1},72: { "levelId": 5, "mem": bit4(0x224992),"good": 1},73: { "levelId": 5, "mem": bit5(0x224992),"good": 1},74: { "levelId": 5, "mem": bit6(0x224992),"good": 1},75: { "levelId": 5, "mem": bit7(0x224992),"good": 1},76: { "levelId": 5, "mem": bit0(0x224993),"good": 1},77: { "levelId": 5, "mem": bit1(0x224993),"good": 1},78: { "levelId": 5, "mem": bit2(0x224993),"good": 1},79: { "levelId": 5, "mem": bit3(0x224993),"good": 1},80: { "levelId": 5, "mem": bit4(0x224993),"good": 1},81: { "levelId": 5, "mem": bit5(0x224993),"good": 1},82: { "levelId": 5, "mem": bit6(0x224993),"good": 1},83: { "levelId": 5, "mem": bit7(0x224993),"good": 1},84: { "levelId": 5, "mem": bit0(0x224994),"good": 1},85: { "levelId": 5, "mem": bit1(0x224994),"good": 1},86: { "levelId": 5, "mem": bit2(0x224994),"good": 1},87: { "levelId": 5, "mem": bit3(0x224994),"good": 1},88: { "levelId": 6, "mem": bit4(0x224994),"good": 1},89: { "levelId": 6, "mem": bit5(0x224994),"good": 1},90: { "levelId": 6, "mem": bit6(0x224994),"good": 1},91: { "levelId": 6, "mem": bit7(0x224994),"good": 1},92: { "levelId": 6, "mem": bit0(0x224995),"good": 1},93: { "levelId": 6, "mem": bit1(0x224995),"good": 1},94: { "levelId": 6, "mem": bit2(0x224995),"good": 1},95: { "levelId": 6, "mem": bit3(0x224995),"good": 1},96: { "levelId": 6, "mem": bit4(0x224995),"good": 1},97: { "levelId": 6, "mem": bit5(0x224995),"good": 1},98: { "levelId": 6, "mem": bit6(0x224995),"good": 1},99: { "levelId": 6, "mem": bit7(0x224995),"good": 1},100: { "levelId": 6, "mem": bit0(0x224996),"good": 1},101: { "levelId": 6, "mem": bit1(0x224996),"good": 1},102: { "levelId": 6, "mem": bit2(0x224996),"good": 1},103: { "levelId": 6, "mem": bit3(0x224996),"good": 1},104: { "levelId": 6, "mem": bit4(0x224996),"good": 1},105: { "levelId": 6, "mem": bit5(0x224996),"good": 1},106: { "levelId": 6, "mem": bit6(0x224996),"good": 1},107: { "levelId": 6, "mem": bit7(0x224996),"good": 1},108: { "levelId": 6, "mem": bit0(0x224997),"good": 1},109: { "levelId": 6, "mem": bit1(0x224997),"good": 1},110: { "levelId": 6, "mem": bit2(0x224997),"good": 1},111: { "levelId": 6, "mem": bit3(0x224997),"good": 1},112: { "levelId": 6, "mem": bit4(0x224997),"good": 1},113: { "levelId": 6, "mem": bit5(0x224997),"good": 1},114: { "levelId": 6, "mem": bit6(0x224997),"good": 1},115: { "levelId": 6, "mem": bit7(0x224997),"good": 1},116: { "levelId": 6, "mem": bit0(0x224998),"good": 1},117: { "levelId": 6, "mem": bit1(0x224998),"good": 1},118: { "levelId": 6, "mem": bit2(0x224998),"good": 1},119: { "levelId": 6, "mem": bit3(0x224998),"good": 1},120: { "levelId": 6, "mem": bit4(0x224998),"good": 1},121: { "levelId": 6, "mem": bit5(0x224998),"good": 1},122: { "levelId": 6, "mem": bit6(0x224998),"good": 1},123: { "levelId": 6, "mem": bit0(0x224999),"good": 1},124: { "levelId": 6, "mem": bit1(0x224999),"good": 1},125: { "levelId": 6, "mem": bit2(0x224999),"good": 1},126: { "levelId": 6, "mem": bit3(0x224999),"good": 1},127: { "levelId": 6, "mem": bit4(0x224999),"good": 1},128: { "levelId": 6, "mem": bit5(0x224999),"good": 1},129: { "levelId": 6, "mem": bit6(0x224999),"good": 1},130: { "levelId": 6, "mem": bit7(0x224999),"good": 1},131: { "levelId": 6, "mem": bit0(0x22499a),"good": 1},132: { "levelId": 6, "mem": bit1(0x22499a),"good": 1},133: { "levelId": 6, "mem": bit2(0x22499a),"good": 1},134: { "levelId": 6, "mem": bit3(0x22499a),"good": 1},135: { "levelId": 6, "mem": bit4(0x22499a),"good": 1},136: { "levelId": 6, "mem": bit5(0x22499a),"good": 1},137: { "levelId": 1, "mem": bit3(0x224a36),"good": 1},138: { "levelId": 1, "mem": bit4(0x224a36),"good": 1},139: { "levelId": 1, "mem": bit5(0x224a36),"good": 1},140: { "levelId": 1, "mem": bit6(0x224a36),"good": 1},141: { "levelId": 1, "mem": bit7(0x224a36),"good": 1},142: { "levelId": 6, "mem": bit7(0x224998),"good": 1},143: { "levelId": 8, "mem": bit3(0x22499b),"good": 1},144: { "levelId": 8, "mem": bit4(0x22499b),"good": 1},145: { "levelId": 8, "mem": bit5(0x22499b),"good": 1},146: { "levelId": 8, "mem": bit5(0x22499c),"good": 1},147: { "levelId": 8, "mem": bit6(0x22499c),"good": 1},148: { "levelId": 8, "mem": bit7(0x22499c),"good": 1},149: { "levelId": 8, "mem": bit0(0x22499d),"good": 1},150: { "levelId": 8, "mem": bit1(0x22499d),"good": 1},151: { "levelId": 8, "mem": bit2(0x22499d),"good": 1},152: { "levelId": 8, "mem": bit3(0x22499d),"good": 1},153: { "levelId": 8, "mem": bit4(0x22499d),"good": 1},154: { "levelId": 8, "mem": bit5(0x22499d),"good": 1},155: { "levelId": 8, "mem": bit6(0x22499d),"good": 1},156: { "levelId": 8, "mem": bit7(0x22499d),"good": 1},157: { "levelId": 8, "mem": bit0(0x22499e),"good": 1},158: { "levelId": 8, "mem": bit1(0x22499e),"good": 1},159: { "levelId": 8, "mem": bit6(0x22499a),"good": 1},160: { "levelId": 8, "mem": bit7(0x22499a),"good": 1},161: { "levelId": 8, "mem": bit0(0x22499b),"good": 1},162: { "levelId": 8, "mem": bit1(0x22499b),"good": 1},163: { "levelId": 8, "mem": bit2(0x22499b),"good": 1},164: { "levelId": 8, "mem": bit6(0x22499b),"good": 1},165: { "levelId": 8, "mem": bit7(0x22499b),"good": 1},166: { "levelId": 8, "mem": bit0(0x22499c),"good": 1},167: { "levelId": 8, "mem": bit1(0x22499c),"good": 1},168: { "levelId": 8, "mem": bit2(0x22499c),"good": 1},169: { "levelId": 8, "mem": bit3(0x22499c),"good": 1},170: { "levelId": 8, "mem": bit4(0x22499c),"good": 1},171: { "levelId": 8, "mem": bit2(0x22499e),"good": 1},172: { "levelId": 8, "mem": bit3(0x22499e),"good": 1},173: { "levelId": 8, "mem": bit4(0x22499e),"good": 1},174: { "levelId": 8, "mem": bit5(0x22499e),"good": 1},175: { "levelId": 8, "mem": bit6(0x22499e),"good": 1},176: { "levelId": 8, "mem": bit7(0x22499e),"good": 1},177: { "levelId": 8, "mem": bit0(0x22499f),"good": 1},178: { "levelId": 8, "mem": bit1(0x22499f),"good": 1},179: { "levelId": 8, "mem": bit2(0x22499f),"good": 1},180: { "levelId": 8, "mem": bit3(0x22499f),"good": 1},181: { "levelId": 8, "mem": bit4(0x22499f),"good": 1},182: { "levelId": 8, "mem": bit5(0x22499f),"good": 1},183: { "levelId": 8, "mem": bit6(0x22499f),"good": 1},184: { "levelId": 8, "mem": bit7(0x22499f),"good": 1},185: { "levelId": 8, "mem": bit0(0x2249a0),"good": 1},186: { "levelId": 8, "mem": bit1(0x2249a0),"good": 1},187: { "levelId": 8, "mem": bit2(0x2249a0),"good": 1},188: { "levelId": 8, "mem": bit3(0x2249a0),"good": 1},189: { "levelId": 8, "mem": bit4(0x2249a0),"good": 1},190: { "levelId": 8, "mem": bit5(0x2249a0),"good": 1},191: { "levelId": 8, "mem": bit6(0x2249a0),"good": 1},192: { "levelId": 8, "mem": bit7(0x2249a0),"good": 1},193: { "levelId": 3, "good": 0},194: { "levelId": 3, "good": 0},195: { "levelId": 3, "good": 0},196: { "levelId": 3, "good": 0},197: { "levelId": 3, "good": 0},198: { "levelId": 3, "good": 0},199: { "levelId": 3, "good": 0},200: { "levelId": 3, "good": 0},201: { "levelId": 3, "good": 0},202: { "levelId": 3, "good": 0},203: { "levelId": 3, "good": 0},204: { "levelId": 3, "good": 0},205: { "levelId": 3, "good": 0},206: { "levelId": 3, "good": 0},207: { "levelId": 3, "good": 0},208: { "levelId": 3, "good": 0},209: { "levelId": 3, "good": 0},210: { "levelId": 3, "good": 0},211: { "levelId": 3, "good": 0},212: { "levelId": 3, "good": 0},213: { "levelId": 3, "good": 0},214: { "levelId": 3, "good": 0},215: { "levelId": 3, "good": 0},216: { "levelId": 3, "good": 0},217: { "levelId": 3, "good": 0},218: { "levelId": 3, "good": 0},219: { "levelId": 3, "good": 0},220: { "levelId": 3, "good": 0},221: { "levelId": 3, "good": 0},222: { "levelId": 3, "good": 0},223: { "levelId": 3, "good": 0},224: { "levelId": 3, "good": 0},225: { "levelId": 3, "good": 0},226: { "levelId": 3, "good": 0},227: { "levelId": 3, "good": 0},228: { "levelId": 3, "good": 0},229: { "levelId": 3, "good": 0},230: { "levelId": 3, "good": 0},231: { "levelId": 3, "good": 0},232: { "levelId": 3, "good": 0},233: { "levelId": 3, "good": 0},234: { "levelId": 3, "good": 0},235: { "levelId": 3, "good": 0},236: { "levelId": 3, "good": 0},237: { "levelId": 3, "good": 0},238: { "levelId": 3, "good": 0},239: { "levelId": 3, "good": 0},240: { "levelId": 3, "good": 0},241: { "levelId": 3, "good": 0},242: { "levelId": 3, "good": 0},243: { "levelId": 3, "good": 0},244: { "levelId": 3, "good": 0},245: { "levelId": 3, "good": 0},246: { "levelId": 3, "good": 0},247: { "levelId": 3, "good": 0},248: { "levelId": 3, "good": 0},249: { "levelId": 3, "good": 0},250: { "levelId": 3, "good": 0},251: { "levelId": 3, "good": 0},252: { "levelId": 3, "good": 0},253: { "levelId": 3, "good": 0},254: { "levelId": 3, "good": 0},255: { "levelId": 3, "good": 0},256: { "levelId": 3, "good": 0},257: { "levelId": 3, "good": 0},258: { "levelId": 3, "good": 0},259: { "levelId": 3, "good": 0},260: { "levelId": 3, "good": 0},261: { "levelId": 3, "good": 0},262: { "levelId": 3, "good": 0},263: { "levelId": 3, "good": 0},264: { "levelId": 3, "good": 0},265: { "levelId": 3, "good": 0},266: { "levelId": 3, "good": 0},267: { "levelId": 3, "good": 0},268: { "levelId": 3, "good": 0},269: { "levelId": 3, "good": 0},270: { "levelId": 3, "good": 0},271: { "levelId": 3, "good": 0},272: { "levelId": 3, "good": 0},273: { "levelId": 3, "good": 0},274: { "levelId": 3, "good": 0},275: { "levelId": 3, "good": 0},276: { "levelId": 3, "good": 0},277: { "levelId": 3, "good": 0},278: { "levelId": 3, "good": 0},279: { "levelId": 3, "good": 0},280: { "levelId": 3, "good": 0},281: { "levelId": 3, "good": 0},282: { "levelId": 3, "good": 0},283: { "levelId": 3, "good": 0},284: { "levelId": 3, "good": 0},285: { "levelId": 3, "good": 0},286: { "levelId": 3, "good": 0},287: { "levelId": 3, "good": 0},288: { "levelId": 3, "good": 0},289: { "levelId": 3, "good": 0},290: { "levelId": 3, "good": 0},291: { "levelId": 3, "good": 0},292: { "levelId": 3, "good": 0},293: { "levelId": 3, "good": 0},294: { "levelId": 3, "good": 0},295: { "levelId": 3, "good": 0},296: { "levelId": 3, "good": 0},297: { "levelId": 3, "good": 0},298: { "levelId": 3, "good": 0},299: { "levelId": 3, "good": 0},300: { "levelId": 3, "good": 0},301: { "levelId": 3, "good": 0},302: { "levelId": 3, "good": 0},303: { "levelId": 3, "good": 0},304: { "levelId": 3, "good": 0},305: { "levelId": 3, "good": 0},306: { "levelId": 3, "good": 0},307: { "levelId": 3, "good": 0},308: { "levelId": 3, "good": 0},309: { "levelId": 3, "good": 0},310: { "levelId": 3, "good": 0},311: { "levelId": 3, "good": 0},312: { "levelId": 3, "good": 0},313: { "levelId": 3, "good": 0},314: { "levelId": 3, "good": 0},315: { "levelId": 3, "good": 0},316: { "levelId": 3, "good": 0},317: { "levelId": 3, "good": 0},318: { "levelId": 3, "good": 0},319: { "levelId": 3, "good": 0},320: { "levelId": 3, "good": 0},321: { "levelId": 3, "good": 0},322: { "levelId": 3, "good": 0},323: { "levelId": 3, "good": 0},324: { "levelId": 3, "good": 0},325: { "levelId": 3, "good": 0},326: { "levelId": 3, "good": 0},327: { "levelId": 3, "good": 0},328: { "levelId": 3, "good": 0},329: { "levelId": 3, "good": 0},330: { "levelId": 3, "good": 0},331: { "levelId": 3, "good": 0},332: { "levelId": 3, "good": 0},333: { "levelId": 3, "good": 0},334: { "levelId": 3, "good": 0},335: { "levelId": 3, "good": 0},336: { "levelId": 3, "good": 0},337: { "levelId": 3, "good": 0},338: { "levelId": 3, "good": 0},339: { "levelId": 3, "good": 0},340: { "levelId": 3, "good": 0},341: { "levelId": 3, "good": 0},342: { "levelId": 3, "good": 0},343: { "levelId": 3, "good": 0},344: { "levelId": 3, "good": 0},345: { "levelId": 3, "good": 0},346: { "levelId": 3, "good": 0},347: { "levelId": 3, "good": 0},348: { "levelId": 3, "good": 0},349: { "levelId": 3, "good": 0},350: { "levelId": 3, "good": 0},351: { "levelId": 3, "good": 0},352: { "levelId": 3, "good": 0},353: { "levelId": 3, "good": 0},354: { "levelId": 3, "good": 0},355: { "levelId": 3, "good": 0},356: { "levelId": 3, "good": 0},357: { "levelId": 3, "good": 0},358: { "levelId": 3, "good": 0},359: { "levelId": 3, "good": 0},360: { "levelId": 3, "good": 0},361: { "levelId": 3, "good": 0},362: { "levelId": 3, "good": 0},363: { "levelId": 3, "good": 0},364: { "levelId": 3, "good": 0},365: { "levelId": 3, "good": 0},366: { "levelId": 3, "good": 0},367: { "levelId": 3, "good": 0},368: { "levelId": 3, "good": 0},369: { "levelId": 3, "good": 0},370: { "levelId": 3, "good": 0},371: { "levelId": 3, "good": 0},372: { "levelId": 3, "good": 0},373: { "levelId": 3, "good": 0},374: { "levelId": 3, "good": 0},375: { "levelId": 3, "good": 0},376: { "levelId": 3, "good": 0},377: { "levelId": 3, "good": 0},378: { "levelId": 3, "good": 0},379: { "levelId": 3, "good": 0},380: { "levelId": 3, "good": 0},381: { "levelId": 3, "good": 0},382: { "levelId": 3, "good": 0},383: { "levelId": 3, "good": 0},384: { "levelId": 3, "good": 0},385: { "levelId": 3, "good": 0},386: { "levelId": 3, "good": 0},387: { "levelId": 3, "good": 0},388: { "levelId": 3, "good": 0},389: { "levelId": 3, "good": 0},390: { "levelId": 3, "good": 0},391: { "levelId": 3, "good": 0},392: { "levelId": 3, "good": 0},393: { "levelId": 3, "good": 0},394: { "levelId": 3, "good": 0},395: { "levelId": 3, "good": 0},396: { "levelId": 3, "good": 0},397: { "levelId": 3, "good": 0},398: { "levelId": 3, "good": 0},399: { "levelId": 3, "good": 0},400: { "levelId": 3, "good": 0},401: { "levelId": 3, "good": 0},402: { "levelId": 3, "good": 0},403: { "levelId": 3, "good": 0},404: { "levelId": 3, "good": 0},405: { "levelId": 3, "good": 0},406: { "levelId": 3, "good": 0},407: { "levelId": 3, "good": 0},408: { "levelId": 3, "good": 0},409: { "levelId": 3, "good": 0},410: { "levelId": 3, "good": 0},411: { "levelId": 3, "good": 0},412: { "levelId": 3, "good": 0},413: { "levelId": 3, "good": 0},414: { "levelId": 3, "good": 0},415: { "levelId": 3, "good": 0},416: { "levelId": 3, "good": 0},417: { "levelId": 3, "good": 0},418: { "levelId": 3, "good": 0},419: { "levelId": 3, "good": 0},420: { "levelId": 3, "good": 0},421: { "levelId": 3, "good": 0},422: { "levelId": 3, "good": 0},423: { "levelId": 3, "good": 0},424: { "levelId": 3, "good": 0},425: { "levelId": 3, "good": 0},426: { "levelId": 3, "good": 0},427: { "levelId": 3, "good": 0},428: { "levelId": 3, "good": 0},429: { "levelId": 3, "good": 0},430: { "levelId": 3, "good": 0},431: { "levelId": 3, "good": 0},432: { "levelId": 3, "good": 0},433: { "levelId": 3, "good": 0},434: { "levelId": 3, "good": 0},435: { "levelId": 3, "good": 0},436: { "levelId": 3, "good": 0},437: { "levelId": 3, "good": 0},438: { "levelId": 3, "good": 0},439: { "levelId": 3, "good": 0},440: { "levelId": 3, "good": 0},441: { "levelId": 3, "good": 0},442: { "levelId": 3, "good": 0},443: { "levelId": 3, "good": 0},444: { "levelId": 3, "good": 0},445: { "levelId": 3, "good": 0},446: { "levelId": 3, "good": 0},447: { "levelId": 3, "good": 0},448: { "levelId": 3, "good": 0},449: { "levelId": 3, "good": 0},450: { "levelId": 3, "good": 0},451: { "levelId": 3, "good": 0},452: { "levelId": 3, "good": 0},453: { "levelId": 3, "good": 0},454: { "levelId": 3, "good": 0},455: { "levelId": 3, "good": 0},456: { "levelId": 3, "good": 0},457: { "levelId": 3, "good": 0},458: { "levelId": 3, "good": 0},459: { "levelId": 3, "good": 0},460: { "levelId": 3, "good": 0},461: { "levelId": 3, "good": 0},462: { "levelId": 3, "good": 0},463: { "levelId": 3, "good": 0},464: { "levelId": 3, "good": 0},465: { "levelId": 3, "good": 0},466: { "levelId": 3, "good": 0},467: { "levelId": 3, "good": 0},468: { "levelId": 3, "good": 0},469: { "levelId": 3, "good": 0},470: { "levelId": 3, "good": 0},471: { "levelId": 3, "good": 0},472: { "levelId": 3, "good": 0},473: { "levelId": 3, "good": 0},474: { "levelId": 3, "good": 0},475: { "levelId": 3, "good": 0},476: { "levelId": 3, "good": 0},477: { "levelId": 3, "good": 0},478: { "levelId": 3, "good": 0},479: { "levelId": 3, "good": 0},480: { "levelId": 3, "good": 0},481: { "levelId": 3, "good": 0},482: { "levelId": 3, "good": 0},483: { "levelId": 3, "good": 0},484: { "levelId": 3, "good": 0},485: { "levelId": 3, "good": 0},486: { "levelId": 3, "good": 0},487: { "levelId": 3, "good": 0},488: { "levelId": 3, "good": 0},489: { "levelId": 3, "good": 0},490: { "levelId": 3, "good": 0},491: { "levelId": 3, "good": 0},492: { "levelId": 3, "good": 0},493: { "levelId": 3, "good": 0},494: { "levelId": 3, "good": 0},495: { "levelId": 3, "good": 0},496: { "levelId": 3, "good": 0},497: { "levelId": 3, "good": 0},498: { "levelId": 3, "good": 0},499: { "levelId": 3, "good": 0},500: { "levelId": 3, "good": 0},501: { "levelId": 3, "good": 0},502: { "levelId": 3, "good": 0},503: { "levelId": 3, "good": 0},504: { "levelId": 3, "good": 0},505: { "levelId": 3, "good": 0},506: { "levelId": 3, "good": 0},507: { "levelId": 3, "good": 0},508: { "levelId": 3, "good": 0},509: { "levelId": 3, "good": 0},510: { "levelId": 3, "good": 0},511: { "levelId": 3, "good": 0},512: { "levelId": 3, "good": 0},513: { "levelId": 3, "good": 0},514: { "levelId": 3, "good": 0},515: { "levelId": 3, "good": 0},516: { "levelId": 3, "good": 0},517: { "levelId": 3, "good": 0},518: { "levelId": 3, "good": 0},519: { "levelId": 3, "good": 0},520: { "levelId": 3, "good": 0},521: { "levelId": 3, "good": 0},522: { "levelId": 3, "good": 0},523: { "levelId": 3, "good": 0},524: { "levelId": 3, "good": 0},525: { "levelId": 3, "good": 0},526: { "levelId": 3, "good": 0},527: { "levelId": 3, "good": 0},528: { "levelId": 3, "good": 0},529: { "levelId": 3, "good": 0},530: { "levelId": 3, "good": 0},531: { "levelId": 3, "good": 0},532: { "levelId": 3, "good": 0},533: { "levelId": 3, "good": 0},534: { "levelId": 3, "good": 0},535: { "levelId": 3, "good": 0},536: { "levelId": 3, "good": 0},537: { "levelId": 3, "good": 0},538: { "levelId": 3, "good": 0},539: { "levelId": 3, "good": 0},540: { "levelId": 3, "good": 0},541: { "levelId": 3, "good": 0},542: { "levelId": 3, "good": 0},543: { "levelId": 3, "good": 0},544: { "levelId": 3, "good": 0},545: { "levelId": 3, "good": 0},546: { "levelId": 3, "good": 0},547: { "levelId": 3, "good": 0},548: { "levelId": 3, "good": 0},549: { "levelId": 3, "good": 0},550: { "levelId": 3, "good": 0},551: { "levelId": 3, "good": 0},552: { "levelId": 3, "good": 0},553: { "levelId": 3, "good": 0},554: { "levelId": 3, "good": 0},555: { "levelId": 3, "good": 0},556: { "levelId": 3, "good": 0},557: { "levelId": 3, "good": 0},558: { "levelId": 3, "good": 0},559: { "levelId": 3, "good": 0},560: { "levelId": 3, "good": 0},561: { "levelId": 3, "good": 0},562: { "levelId": 3, "good": 0},563: { "levelId": 3, "good": 0},564: { "levelId": 3, "good": 0},565: { "levelId": 3, "good": 0},566: { "levelId": 3, "good": 0},567: { "levelId": 3, "good": 0},568: { "levelId": 3, "good": 0},569: { "levelId": 3, "good": 0},570: { "levelId": 3, "good": 0},571: { "levelId": 3, "good": 0},572: { "levelId": 3, "good": 0},573: { "levelId": 3, "good": 0},574: { "levelId": 3, "good": 0},575: { "levelId": 3, "good": 0},576: { "levelId": 3, "good": 0},577: { "levelId": 3, "good": 0},578: { "levelId": 3, "good": 0},579: { "levelId": 3, "good": 0},580: { "levelId": 3, "good": 0},581: { "levelId": 3, "good": 0},582: { "levelId": 3, "good": 0},583: { "levelId": 3, "good": 0},584: { "levelId": 3, "good": 0},585: { "levelId": 3, "good": 0},586: { "levelId": 3, "good": 0},587: { "levelId": 3, "good": 0},588: { "levelId": 3, "good": 0},589: { "levelId": 3, "good": 0},590: { "levelId": 3, "good": 0},591: { "levelId": 3, "good": 0},592: { "levelId": 3, "good": 0},593: { "levelId": 3, "good": 0},594: { "levelId": 3, "good": 0},595: { "levelId": 3, "good": 0},596: { "levelId": 3, "good": 0},597: { "levelId": 3, "good": 0},598: { "levelId": 3, "good": 0},599: { "levelId": 3, "good": 0},600: { "levelId": 3, "good": 0},601: { "levelId": 3, "good": 0},602: { "levelId": 3, "good": 0},603: { "levelId": 3, "good": 0},604: { "levelId": 3, "good": 0},605: { "levelId": 3, "good": 0},606: { "levelId": 3, "good": 0},607: { "levelId": 3, "good": 0},608: { "levelId": 3, "good": 0},609: { "levelId": 3, "good": 0},610: { "levelId": 3, "good": 0},611: { "levelId": 3, "good": 0},612: { "levelId": 3, "good": 0},613: { "levelId": 3, "good": 0},614: { "levelId": 3, "good": 0},615: { "levelId": 3, "good": 0},616: { "levelId": 3, "good": 0},617: { "levelId": 3, "good": 0},618: { "levelId": 3, "good": 0},619: { "levelId": 3, "good": 0},620: { "levelId": 3, "good": 0},621: { "levelId": 3, "good": 0},622: { "levelId": 3, "good": 0},623: { "levelId": 3, "good": 0},624: { "levelId": 3, "good": 0},625: { "levelId": 3, "good": 0},626: { "levelId": 3, "good": 0},627: { "levelId": 3, "good": 0},628: { "levelId": 3, "good": 0},629: { "levelId": 3, "good": 0},630: { "levelId": 3, "good": 0},631: { "levelId": 3, "good": 0},632: { "levelId": 3, "good": 0},633: { "levelId": 3, "good": 0},634: { "levelId": 3, "good": 0},635: { "levelId": 3, "good": 0},636: { "levelId": 3, "good": 0},637: { "levelId": 3, "good": 0},638: { "levelId": 3, "good": 0},639: { "levelId": 3, "good": 0},640: { "levelId": 3, "good": 0},641: { "levelId": 3, "good": 0},642: { "levelId": 3, "good": 0},643: { "levelId": 3, "good": 0},644: { "levelId": 3, "good": 0},645: { "levelId": 3, "good": 0},646: { "levelId": 3, "good": 0},647: { "levelId": 3, "good": 0},648: { "levelId": 3, "good": 0},649: { "levelId": 3, "good": 0},650: { "levelId": 3, "good": 0},651: { "levelId": 3, "good": 0},652: { "levelId": 3, "good": 0},653: { "levelId": 3, "good": 0},654: { "levelId": 3, "good": 0},655: { "levelId": 3, "good": 0},656: { "levelId": 3, "good": 0},657: { "levelId": 3, "good": 0},658: { "levelId": 3, "good": 0},659: { "levelId": 3, "good": 0},660: { "levelId": 3, "good": 0},661: { "levelId": 3, "good": 0},662: { "levelId": 3, "good": 0},663: { "levelId": 3, "good": 0},664: { "levelId": 3, "good": 0},665: { "levelId": 3, "good": 0},666: { "levelId": 3, "good": 0},667: { "levelId": 3, "good": 0},668: { "levelId": 3, "good": 0},669: { "levelId": 3, "good": 0},670: { "levelId": 3, "good": 0},671: { "levelId": 3, "good": 0},672: { "levelId": 3, "good": 0},673: { "levelId": 3, "good": 0},674: { "levelId": 3, "good": 0},675: { "levelId": 3, "good": 0},676: { "levelId": 3, "good": 0},677: { "levelId": 3, "good": 0},678: { "levelId": 3, "good": 0},679: { "levelId": 3, "good": 0},680: { "levelId": 3, "good": 0},681: { "levelId": 3, "good": 0},682: { "levelId": 3, "good": 0},683: { "levelId": 3, "good": 0},684: { "levelId": 3, "good": 0},685: { "levelId": 3, "good": 0},686: { "levelId": 3, "good": 0},687: { "levelId": 3, "good": 0},688: { "levelId": 3, "good": 0},689: { "levelId": 3, "good": 0},690: { "levelId": 3, "good": 0},691: { "levelId": 3, "good": 0},692: { "levelId": 3, "good": 0},693: { "levelId": 3, "good": 0},694: { "levelId": 3, "good": 0},695: { "levelId": 3, "good": 0},696: { "levelId": 3, "good": 0},697: { "levelId": 3, "good": 0},698: { "levelId": 3, "good": 0},699: { "levelId": 3, "good": 0},700: { "levelId": 3, "good": 0},701: { "levelId": 3, "good": 0},702: { "levelId": 3, "good": 0},703: { "levelId": 3, "good": 0},704: { "levelId": 3, "good": 0},705: { "levelId": 3, "good": 0},706: { "levelId": 3, "good": 0},707: { "levelId": 3, "good": 0},708: { "levelId": 3, "good": 0},709: { "levelId": 3, "good": 0},710: { "levelId": 3, "good": 0},711: { "levelId": 3, "good": 0},712: { "levelId": 3, "good": 0},713: { "levelId": 3, "good": 0},714: { "levelId": 3, "good": 0},715: { "levelId": 3, "good": 0},716: { "levelId": 3, "good": 0},717: { "levelId": 3, "good": 0},718: { "levelId": 3, "good": 0},719: { "levelId": 3, "good": 0},720: { "levelId": 3, "good": 0},721: { "levelId": 3, "good": 0},722: { "levelId": 3, "good": 0},723: { "levelId": 3, "good": 0},724: { "levelId": 3, "good": 0},725: { "levelId": 3, "good": 0},726: { "levelId": 3, "good": 0},727: { "levelId": 3, "good": 0},728: { "levelId": 3, "good": 0},729: { "levelId": 3, "good": 0},730: { "levelId": 3, "good": 0},731: { "levelId": 3, "good": 0},732: { "levelId": 3, "good": 0},733: { "levelId": 3, "good": 0},734: { "levelId": 3, "good": 0},735: { "levelId": 3, "good": 0},736: { "levelId": 3, "good": 0},737: { "levelId": 3, "good": 0},738: { "levelId": 3, "good": 0},739: { "levelId": 3, "good": 0},740: { "levelId": 3, "good": 0},741: { "levelId": 3, "good": 0},742: { "levelId": 3, "good": 0},743: { "levelId": 3, "good": 0},744: { "levelId": 3, "good": 0},745: { "levelId": 3, "good": 0},746: { "levelId": 3, "good": 0},747: { "levelId": 3, "good": 0},748: { "levelId": 3, "good": 0},749: { "levelId": 3, "good": 0},750: { "levelId": 3, "good": 0},751: { "levelId": 3, "good": 0},752: { "levelId": 3, "good": 0},753: { "levelId": 3, "good": 0},754: { "levelId": 3, "good": 0},755: { "levelId": 3, "good": 0},756: { "levelId": 3, "good": 0},757: { "levelId": 3, "good": 0},758: { "levelId": 3, "good": 0},759: { "levelId": 3, "good": 0},760: { "levelId": 3, "good": 0},761: { "levelId": 3, "good": 0},762: { "levelId": 3, "good": 0},763: { "levelId": 3, "good": 0},764: { "levelId": 3, "good": 0},765: { "levelId": 3, "good": 0},766: { "levelId": 3, "good": 0},767: { "levelId": 3, "good": 0},768: { "levelId": 3, "good": 0},769: { "levelId": 3, "good": 0},770: { "levelId": 3, "good": 0},771: { "levelId": 3, "good": 0},772: { "levelId": 3, "good": 0},773: { "levelId": 3, "good": 0},774: { "levelId": 3, "good": 0},775: { "levelId": 3, "good": 0},776: { "levelId": 3, "good": 0},777: { "levelId": 3, "good": 0},778: { "levelId": 3, "good": 0},779: { "levelId": 3, "good": 0},780: { "levelId": 3, "good": 0},781: { "levelId": 3, "good": 0},782: { "levelId": 3, "good": 0},783: { "levelId": 3, "good": 0},784: { "levelId": 3, "good": 0},785: { "levelId": 3, "good": 0},786: { "levelId": 3, "good": 0},787: { "levelId": 3, "good": 0},788: { "levelId": 3, "good": 0},789: { "levelId": 3, "good": 0},790: { "levelId": 3, "good": 0},791: { "levelId": 3, "good": 0},792: { "levelId": 3, "good": 0},793: { "levelId": 3, "good": 0},794: { "levelId": 3, "good": 0},795: { "levelId": 3, "good": 0},796: { "levelId": 3, "good": 0},797: { "levelId": 3, "good": 0},798: { "levelId": 3, "good": 0},799: { "levelId": 3, "good": 0},800: { "levelId": 3, "good": 0},801: { "levelId": 3, "good": 0},802: { "levelId": 3, "good": 0},803: { "levelId": 3, "good": 0},804: { "levelId": 3, "good": 0},805: { "levelId": 3, "good": 0},806: { "levelId": 3, "good": 0},807: { "levelId": 3, "good": 0},808: { "levelId": 3, "good": 0},809: { "levelId": 3, "good": 0},810: { "levelId": 3, "good": 0},811: { "levelId": 3, "good": 0},812: { "levelId": 3, "good": 0},813: { "levelId": 3, "good": 0},814: { "levelId": 3, "good": 0},815: { "levelId": 3, "good": 0},816: { "levelId": 3, "good": 0},817: { "levelId": 3, "good": 0},818: { "levelId": 3, "good": 0},819: { "levelId": 3, "good": 0},820: { "levelId": 3, "good": 0},821: { "levelId": 3, "good": 0},822: { "levelId": 3, "good": 0},823: { "levelId": 3, "good": 0},824: { "levelId": 3, "good": 0},825: { "levelId": 3, "good": 0},826: { "levelId": 3, "good": 0},827: { "levelId": 3, "good": 0},828: { "levelId": 3, "good": 0},829: { "levelId": 3, "good": 0},830: { "levelId": 3, "good": 0},831: { "levelId": 3, "good": 0},832: { "levelId": 3, "good": 0},833: { "levelId": 3, "good": 0},834: { "levelId": 3, "good": 0},835: { "levelId": 3, "good": 0},836: { "levelId": 3, "good": 0},837: { "levelId": 3, "good": 0},838: { "levelId": 3, "good": 0},839: { "levelId": 3, "good": 0},840: { "levelId": 3, "good": 0},841: { "levelId": 3, "good": 0},842: { "levelId": 3, "good": 0},843: { "levelId": 3, "good": 0},844: { "levelId": 3, "good": 0},845: { "levelId": 3, "good": 0},846: { "levelId": 3, "good": 0},847: { "levelId": 3, "good": 0},848: { "levelId": 3, "good": 0},849: { "levelId": 3, "good": 0},850: { "levelId": 3, "good": 0},851: { "levelId": 3, "good": 0},852: { "levelId": 3, "good": 0},853: { "levelId": 3, "good": 0},854: { "levelId": 3, "good": 0},855: { "levelId": 3, "good": 0},856: { "levelId": 3, "good": 0},857: { "levelId": 3, "good": 0},858: { "levelId": 3, "good": 0},859: { "levelId": 3, "good": 0},860: { "levelId": 3, "good": 0},861: { "levelId": 3, "good": 0},862: { "levelId": 3, "good": 0},863: { "levelId": 3, "good": 0},864: { "levelId": 3, "good": 0},865: { "levelId": 3, "good": 0},866: { "levelId": 3, "good": 0},867: { "levelId": 3, "good": 0},868: { "levelId": 3, "good": 0},869: { "levelId": 3, "good": 0},870: { "levelId": 3, "good": 0},871: { "levelId": 3, "good": 0},872: { "levelId": 3, "good": 0},873: { "levelId": 3, "good": 0},874: { "levelId": 3, "good": 0},875: { "levelId": 3, "good": 0},876: { "levelId": 3, "good": 0},877: { "levelId": 3, "good": 0},878: { "levelId": 3, "good": 0},879: { "levelId": 3, "good": 0},880: { "levelId": 3, "good": 0},881: { "levelId": 3, "good": 0},882: { "levelId": 3, "good": 0},883: { "levelId": 3, "good": 0},884: { "levelId": 3, "good": 0},885: { "levelId": 3, "good": 0},886: { "levelId": 3, "good": 0},887: { "levelId": 3, "good": 0},888: { "levelId": 3, "good": 0},889: { "levelId": 3, "good": 0},890: { "levelId": 3, "good": 0},891: { "levelId": 3, "good": 0},892: { "levelId": 3, "good": 0},893: { "levelId": 3, "good": 0},894: { "levelId": 3, "good": 0},895: { "levelId": 3, "good": 0},896: { "levelId": 3, "good": 0},897: { "levelId": 3, "good": 0},898: { "levelId": 3, "good": 0},899: { "levelId": 3, "good": 0},900: { "levelId": 3, "good": 0},901: { "levelId": 3, "good": 0},902: { "levelId": 3, "good": 0},903: { "levelId": 3, "good": 0},904: { "levelId": 3, "good": 0},905: { "levelId": 3, "good": 0},906: { "levelId": 3, "good": 0},907: { "levelId": 3, "good": 0},908: { "levelId": 3, "good": 0},909: { "levelId": 3, "good": 0},910: { "levelId": 3, "good": 0},911: { "levelId": 3, "good": 0},912: { "levelId": 3, "good": 0},913: { "levelId": 3, "good": 0},914: { "levelId": 3, "good": 0},915: { "levelId": 3, "good": 0},916: { "levelId": 3, "good": 0},917: { "levelId": 3, "good": 0},918: { "levelId": 3, "good": 0},919: { "levelId": 3, "good": 0},920: { "levelId": 3, "good": 0},921: { "levelId": 3, "good": 0},922: { "levelId": 3, "good": 0},923: { "levelId": 3, "good": 0},924: { "levelId": 3, "good": 0},925: { "levelId": 3, "good": 0},926: { "levelId": 3, "good": 0},927: { "levelId": 3, "good": 0},928: { "levelId": 3, "good": 0},929: { "levelId": 3, "good": 0},930: { "levelId": 3, "good": 0},931: { "levelId": 3, "good": 0},932: { "levelId": 3, "good": 0},933: { "levelId": 3, "good": 0},934: { "levelId": 3, "good": 0},935: { "levelId": 3, "good": 0},936: { "levelId": 3, "good": 0},937: { "levelId": 3, "good": 0},938: { "levelId": 3, "good": 0},939: { "levelId": 3, "good": 0},940: { "levelId": 3, "good": 0},941: { "levelId": 3, "good": 0},942: { "levelId": 3, "good": 0},943: { "levelId": 3, "good": 0},944: { "levelId": 3, "good": 0},945: { "levelId": 3, "good": 0},946: { "levelId": 3, "good": 0},947: { "levelId": 3, "good": 0},948: { "levelId": 3, "good": 0},949: { "levelId": 3, "good": 0},950: { "levelId": 3, "good": 0},951: { "levelId": 3, "good": 0},952: { "levelId": 3, "good": 0},953: { "levelId": 3, "good": 0},954: { "levelId": 3, "good": 0},955: { "levelId": 3, "good": 0},956: { "levelId": 3, "good": 0},957: { "levelId": 3, "good": 0},958: { "levelId": 3, "good": 0},959: { "levelId": 3, "good": 0},960: { "levelId": 3, "good": 0},961: { "levelId": 3, "good": 0},962: { "levelId": 3, "good": 0},963: { "levelId": 3, "good": 0},964: { "levelId": 3, "good": 0},965: { "levelId": 3, "good": 0},966: { "levelId": 3, "good": 0},967: { "levelId": 3, "good": 0},968: { "levelId": 3, "good": 0},969: { "levelId": 3, "good": 0},970: { "levelId": 3, "good": 0},971: { "levelId": 3, "good": 0},972: { "levelId": 3, "good": 0},973: { "levelId": 3, "good": 0},974: { "levelId": 3, "good": 0},975: { "levelId": 3, "good": 0},976: { "levelId": 3, "good": 0},977: { "levelId": 3, "good": 0},978: { "levelId": 3, "good": 0},979: { "levelId": 3, "good": 0},980: { "levelId": 3, "good": 0},981: { "levelId": 3, "good": 0},982: { "levelId": 3, "good": 0},983: { "levelId": 3, "good": 0},984: { "levelId": 3, "good": 0},985: { "levelId": 3, "good": 0},986: { "levelId": 3, "good": 0},987: { "levelId": 3, "good": 0},988: { "levelId": 3, "good": 0},989: { "levelId": 3, "good": 0},990: { "levelId": 3, "good": 0},991: { "levelId": 3, "good": 0},992: { "levelId": 3, "good": 0},993: { "levelId": 3, "good": 0},994: { "levelId": 3, "good": 0},995: { "levelId": 3, "good": 0},996: { "levelId": 3, "good": 0},997: { "levelId": 3, "good": 0},998: { "levelId": 3, "good": 0},999: { "levelId": 3, "good": 0},1000: { "levelId": 3, "good": 0},</v>
+        <v>1: { "levelId": 2, "mem": bit0(0x224988),"good": 1},2: { "levelId": 2, "mem": bit1(0x224988),"good": 1},3: { "levelId": 2, "mem": bit2(0x224988),"good": 1},4: { "levelId": 2, "mem": bit3(0x224988),"good": 1},5: { "levelId": 2, "mem": bit4(0x224988),"good": 1},6: { "levelId": 2, "mem": bit5(0x224988),"good": 1},7: { "levelId": 2, "mem": bit6(0x224988),"good": 1},8: { "levelId": 2, "mem": bit7(0x224988),"good": 1},9: { "levelId": 2, "mem": bit2(0x224989),"good": 1},10: { "levelId": 2, "mem": bit1(0x22498a),"good": 1},11: { "levelId": 2, "mem": bit2(0x22498a),"good": 1},12: { "levelId": 2, "mem": bit3(0x22498a),"good": 1},13: { "levelId": 2, "mem": bit4(0x22498a),"good": 1},14: { "levelId": 2, "mem": bit5(0x22498a),"good": 1},15: { "levelId": 2, "mem": bit6(0x22498a),"good": 1},16: { "levelId": 2, "mem": bit7(0x22498a),"good": 1},17: { "levelId": 2, "mem": bit5(0x22498b),"good": 1},18: { "levelId": 2, "mem": bit6(0x22498b),"good": 1},19: { "levelId": 2, "mem": bit7(0x22498b),"good": 1},20: { "levelId": 2, "mem": bit0(0x22498c),"good": 1},21: { "levelId": 2, "mem": bit1(0x22498c),"good": 1},22: { "levelId": 2, "mem": bit2(0x22498c),"good": 1},23: { "levelId": 2, "mem": bit3(0x22498c),"good": 1},24: { "levelId": 2, "mem": bit4(0x22498c),"good": 1},25: { "levelId": 2, "mem": bit5(0x22498c),"good": 1},26: { "levelId": 2, "mem": bit6(0x22498c),"good": 1},27: { "levelId": 2, "mem": bit7(0x22498c),"good": 1},28: { "levelId": 2, "mem": bit0(0x22498d),"good": 1},29: { "levelId": 2, "mem": bit1(0x22498d),"good": 1},30: { "levelId": 2, "mem": bit2(0x22498d),"good": 1},31: { "levelId": 2, "mem": bit3(0x22498d),"good": 1},32: { "levelId": 2, "mem": bit4(0x22498d),"good": 1},33: { "levelId": 2, "mem": bit5(0x22498d),"good": 1},34: { "levelId": 2, "mem": bit6(0x22498d),"good": 1},35: { "levelId": 2, "mem": bit7(0x22498d),"good": 1},36: { "levelId": 2, "mem": bit0(0x22498e),"good": 1},37: { "levelId": 2, "mem": bit1(0x22498e),"good": 1},38: { "levelId": 5, "mem": bit2(0x22498e),"good": 1},39: { "levelId": 5, "mem": bit3(0x22498e),"good": 1},40: { "levelId": 5, "mem": bit4(0x22498e),"good": 1},41: { "levelId": 5, "mem": bit5(0x22498e),"good": 1},42: { "levelId": 5, "mem": bit6(0x22498e),"good": 1},43: { "levelId": 5, "mem": bit7(0x22498e),"good": 1},44: { "levelId": 5, "mem": bit0(0x22498f),"good": 1},45: { "levelId": 5, "mem": bit1(0x22498f),"good": 1},46: { "levelId": 5, "mem": bit2(0x22498f),"good": 1},47: { "levelId": 5, "mem": bit3(0x22498f),"good": 1},48: { "levelId": 5, "mem": bit4(0x22498f),"good": 1},49: { "levelId": 5, "mem": bit5(0x22498f),"good": 1},50: { "levelId": 5, "mem": bit6(0x22498f),"good": 1},51: { "levelId": 5, "mem": bit7(0x22498f),"good": 1},52: { "levelId": 5, "mem": bit0(0x224990),"good": 1},53: { "levelId": 5, "mem": bit1(0x224990),"good": 1},54: { "levelId": 5, "mem": bit2(0x224990),"good": 1},55: { "levelId": 5, "mem": bit3(0x224990),"good": 1},56: { "levelId": 5, "mem": bit4(0x224990),"good": 1},57: { "levelId": 5, "mem": bit5(0x224990),"good": 1},58: { "levelId": 5, "mem": bit6(0x224990),"good": 1},59: { "levelId": 5, "mem": bit7(0x224990),"good": 1},60: { "levelId": 5, "mem": bit0(0x224991),"good": 1},61: { "levelId": 5, "mem": bit1(0x224991),"good": 1},62: { "levelId": 5, "mem": bit2(0x224991),"good": 1},63: { "levelId": 5, "mem": bit3(0x224991),"good": 1},64: { "levelId": 5, "mem": bit4(0x224991),"good": 1},65: { "levelId": 5, "mem": bit5(0x224991),"good": 1},66: { "levelId": 5, "mem": bit6(0x224991),"good": 1},67: { "levelId": 5, "mem": bit7(0x224991),"good": 1},68: { "levelId": 5, "mem": bit0(0x224992),"good": 1},69: { "levelId": 5, "mem": bit1(0x224992),"good": 1},70: { "levelId": 5, "mem": bit2(0x224992),"good": 1},71: { "levelId": 5, "mem": bit3(0x224992),"good": 1},72: { "levelId": 5, "mem": bit4(0x224992),"good": 1},73: { "levelId": 5, "mem": bit5(0x224992),"good": 1},74: { "levelId": 5, "mem": bit6(0x224992),"good": 1},75: { "levelId": 5, "mem": bit7(0x224992),"good": 1},76: { "levelId": 5, "mem": bit0(0x224993),"good": 1},77: { "levelId": 5, "mem": bit1(0x224993),"good": 1},78: { "levelId": 5, "mem": bit2(0x224993),"good": 1},79: { "levelId": 5, "mem": bit3(0x224993),"good": 1},80: { "levelId": 5, "mem": bit4(0x224993),"good": 1},81: { "levelId": 5, "mem": bit5(0x224993),"good": 1},82: { "levelId": 5, "mem": bit6(0x224993),"good": 1},83: { "levelId": 5, "mem": bit7(0x224993),"good": 1},84: { "levelId": 5, "mem": bit0(0x224994),"good": 1},85: { "levelId": 5, "mem": bit1(0x224994),"good": 1},86: { "levelId": 5, "mem": bit2(0x224994),"good": 1},87: { "levelId": 5, "mem": bit3(0x224994),"good": 1},88: { "levelId": 6, "mem": bit4(0x224994),"good": 1},89: { "levelId": 6, "mem": bit5(0x224994),"good": 1},90: { "levelId": 6, "mem": bit6(0x224994),"good": 1},91: { "levelId": 6, "mem": bit7(0x224994),"good": 1},92: { "levelId": 6, "mem": bit0(0x224995),"good": 1},93: { "levelId": 6, "mem": bit1(0x224995),"good": 1},94: { "levelId": 6, "mem": bit2(0x224995),"good": 1},95: { "levelId": 6, "mem": bit3(0x224995),"good": 1},96: { "levelId": 6, "mem": bit4(0x224995),"good": 1},97: { "levelId": 6, "mem": bit5(0x224995),"good": 1},98: { "levelId": 6, "mem": bit6(0x224995),"good": 1},99: { "levelId": 6, "mem": bit7(0x224995),"good": 1},100: { "levelId": 6, "mem": bit0(0x224996),"good": 1},101: { "levelId": 6, "mem": bit1(0x224996),"good": 1},102: { "levelId": 6, "mem": bit2(0x224996),"good": 1},103: { "levelId": 6, "mem": bit3(0x224996),"good": 1},104: { "levelId": 6, "mem": bit4(0x224996),"good": 1},105: { "levelId": 6, "mem": bit5(0x224996),"good": 1},106: { "levelId": 6, "mem": bit6(0x224996),"good": 1},107: { "levelId": 6, "mem": bit7(0x224996),"good": 1},108: { "levelId": 6, "mem": bit0(0x224997),"good": 1},109: { "levelId": 6, "mem": bit1(0x224997),"good": 1},110: { "levelId": 6, "mem": bit2(0x224997),"good": 1},111: { "levelId": 6, "mem": bit3(0x224997),"good": 1},112: { "levelId": 6, "mem": bit4(0x224997),"good": 1},113: { "levelId": 6, "mem": bit5(0x224997),"good": 1},114: { "levelId": 6, "mem": bit6(0x224997),"good": 1},115: { "levelId": 6, "mem": bit7(0x224997),"good": 1},116: { "levelId": 6, "mem": bit0(0x224998),"good": 1},117: { "levelId": 6, "mem": bit1(0x224998),"good": 1},118: { "levelId": 6, "mem": bit2(0x224998),"good": 1},119: { "levelId": 6, "mem": bit3(0x224998),"good": 1},120: { "levelId": 6, "mem": bit4(0x224998),"good": 1},121: { "levelId": 6, "mem": bit5(0x224998),"good": 1},122: { "levelId": 6, "mem": bit6(0x224998),"good": 1},123: { "levelId": 6, "mem": bit0(0x224999),"good": 1},124: { "levelId": 6, "mem": bit1(0x224999),"good": 1},125: { "levelId": 6, "mem": bit2(0x224999),"good": 1},126: { "levelId": 6, "mem": bit3(0x224999),"good": 1},127: { "levelId": 6, "mem": bit4(0x224999),"good": 1},128: { "levelId": 6, "mem": bit5(0x224999),"good": 1},129: { "levelId": 6, "mem": bit6(0x224999),"good": 1},130: { "levelId": 6, "mem": bit7(0x224999),"good": 1},131: { "levelId": 6, "mem": bit0(0x22499a),"good": 1},132: { "levelId": 6, "mem": bit1(0x22499a),"good": 1},133: { "levelId": 6, "mem": bit2(0x22499a),"good": 1},134: { "levelId": 6, "mem": bit3(0x22499a),"good": 1},135: { "levelId": 6, "mem": bit4(0x22499a),"good": 1},136: { "levelId": 6, "mem": bit5(0x22499a),"good": 1},137: { "levelId": 1, "mem": bit3(0x224a36),"good": 1},138: { "levelId": 1, "mem": bit4(0x224a36),"good": 1},139: { "levelId": 1, "mem": bit5(0x224a36),"good": 1},140: { "levelId": 1, "mem": bit6(0x224a36),"good": 1},141: { "levelId": 1, "mem": bit7(0x224a36),"good": 1},142: { "levelId": 6, "mem": bit7(0x224998),"good": 1},143: { "levelId": 8, "mem": bit3(0x22499b),"good": 1},144: { "levelId": 8, "mem": bit4(0x22499b),"good": 1},145: { "levelId": 8, "mem": bit5(0x22499b),"good": 1},146: { "levelId": 8, "mem": bit5(0x22499c),"good": 1},147: { "levelId": 8, "mem": bit6(0x22499c),"good": 1},148: { "levelId": 8, "mem": bit7(0x22499c),"good": 1},149: { "levelId": 8, "mem": bit0(0x22499d),"good": 1},150: { "levelId": 8, "mem": bit1(0x22499d),"good": 1},151: { "levelId": 8, "mem": bit2(0x22499d),"good": 1},152: { "levelId": 8, "mem": bit3(0x22499d),"good": 1},153: { "levelId": 8, "mem": bit4(0x22499d),"good": 1},154: { "levelId": 8, "mem": bit5(0x22499d),"good": 1},155: { "levelId": 8, "mem": bit6(0x22499d),"good": 1},156: { "levelId": 8, "mem": bit7(0x22499d),"good": 1},157: { "levelId": 8, "mem": bit0(0x22499e),"good": 1},158: { "levelId": 8, "mem": bit1(0x22499e),"good": 1},159: { "levelId": 8, "mem": bit6(0x22499a),"good": 1},160: { "levelId": 8, "mem": bit7(0x22499a),"good": 1},161: { "levelId": 8, "mem": bit0(0x22499b),"good": 1},162: { "levelId": 8, "mem": bit1(0x22499b),"good": 1},163: { "levelId": 8, "mem": bit2(0x22499b),"good": 1},164: { "levelId": 8, "mem": bit6(0x22499b),"good": 1},165: { "levelId": 8, "mem": bit7(0x22499b),"good": 1},166: { "levelId": 8, "mem": bit0(0x22499c),"good": 1},167: { "levelId": 8, "mem": bit1(0x22499c),"good": 1},168: { "levelId": 8, "mem": bit2(0x22499c),"good": 1},169: { "levelId": 8, "mem": bit3(0x22499c),"good": 1},170: { "levelId": 8, "mem": bit4(0x22499c),"good": 1},171: { "levelId": 8, "mem": bit2(0x22499e),"good": 1},172: { "levelId": 8, "mem": bit3(0x22499e),"good": 1},173: { "levelId": 8, "mem": bit4(0x22499e),"good": 1},174: { "levelId": 8, "mem": bit5(0x22499e),"good": 1},175: { "levelId": 8, "mem": bit6(0x22499e),"good": 1},176: { "levelId": 8, "mem": bit7(0x22499e),"good": 1},177: { "levelId": 8, "mem": bit0(0x22499f),"good": 1},178: { "levelId": 8, "mem": bit1(0x22499f),"good": 1},179: { "levelId": 8, "mem": bit2(0x22499f),"good": 1},180: { "levelId": 8, "mem": bit3(0x22499f),"good": 1},181: { "levelId": 8, "mem": bit4(0x22499f),"good": 1},182: { "levelId": 8, "mem": bit5(0x22499f),"good": 1},183: { "levelId": 8, "mem": bit6(0x22499f),"good": 1},184: { "levelId": 8, "mem": bit7(0x22499f),"good": 1},185: { "levelId": 8, "mem": bit0(0x2249a0),"good": 1},186: { "levelId": 8, "mem": bit1(0x2249a0),"good": 1},187: { "levelId": 8, "mem": bit2(0x2249a0),"good": 1},188: { "levelId": 8, "mem": bit3(0x2249a0),"good": 1},189: { "levelId": 8, "mem": bit4(0x2249a0),"good": 1},190: { "levelId": 8, "mem": bit5(0x2249a0),"good": 1},191: { "levelId": 8, "mem": bit6(0x2249a0),"good": 1},192: { "levelId": 8, "mem": bit7(0x2249a0),"good": 1},193: { "levelId": 10, "mem": bit0(0x2249a1),"good": 1},194: { "levelId": 10, "mem": bit1(0x2249a1),"good": 1},195: { "levelId": 10, "mem": bit2(0x2249a1),"good": 1},196: { "levelId": 10, "mem": bit3(0x2249a1),"good": 1},197: { "levelId": 10, "mem": bit4(0x2249a1),"good": 1},198: { "levelId": 10, "mem": bit2(0x2249a2),"good": 1},199: { "levelId": 10, "mem": bit3(0x2249a2),"good": 1},200: { "levelId": 10, "mem": bit4(0x2249a2),"good": 1},201: { "levelId": 10, "mem": bit5(0x2249a2),"good": 1},202: { "levelId": 10, "mem": bit6(0x2249a2),"good": 1},203: { "levelId": 10, "mem": bit1(0x2249a4),"good": 1},204: { "levelId": 10, "mem": bit5(0x2249a3),"good": 1},205: { "levelId": 10, "mem": bit6(0x2249a3),"good": 1},206: { "levelId": 10, "mem": bit7(0x2249a3),"good": 1},207: { "levelId": 10, "mem": bit0(0x2249a4),"good": 1},208: { "levelId": 10, "mem": bit3(0x2249a4),"good": 1},209: { "levelId": 10, "mem": bit5(0x2249a4),"good": 1},210: { "levelId": 10, "mem": bit6(0x2249a4),"good": 1},211: { "levelId": 10, "mem": bit7(0x2249a4),"good": 1},212: { "levelId": 10, "mem": bit0(0x2249a5),"good": 1},213: { "levelId": 10, "mem": bit1(0x2249a5),"good": 1},214: { "levelId": 10, "mem": bit2(0x2249a5),"good": 1},215: { "levelId": 10, "mem": bit4(0x2249a4),"good": 1},216: { "levelId": 3, "good": 0},217: { "levelId": 3, "good": 0},218: { "levelId": 3, "good": 0},219: { "levelId": 3, "good": 0},220: { "levelId": 3, "good": 0},221: { "levelId": 3, "good": 0},222: { "levelId": 3, "good": 0},223: { "levelId": 3, "good": 0},224: { "levelId": 3, "good": 0},225: { "levelId": 3, "good": 0},226: { "levelId": 3, "good": 0},227: { "levelId": 3, "good": 0},228: { "levelId": 3, "good": 0},229: { "levelId": 3, "good": 0},230: { "levelId": 3, "good": 0},231: { "levelId": 3, "good": 0},232: { "levelId": 3, "good": 0},233: { "levelId": 3, "good": 0},234: { "levelId": 3, "good": 0},235: { "levelId": 3, "good": 0},236: { "levelId": 3, "good": 0},237: { "levelId": 3, "good": 0},238: { "levelId": 3, "good": 0},239: { "levelId": 3, "good": 0},240: { "levelId": 3, "good": 0},241: { "levelId": 3, "good": 0},242: { "levelId": 3, "good": 0},243: { "levelId": 3, "good": 0},244: { "levelId": 3, "good": 0},245: { "levelId": 3, "good": 0},246: { "levelId": 3, "good": 0},247: { "levelId": 3, "good": 0},248: { "levelId": 3, "good": 0},249: { "levelId": 3, "good": 0},250: { "levelId": 3, "good": 0},251: { "levelId": 3, "good": 0},252: { "levelId": 3, "good": 0},253: { "levelId": 3, "good": 0},254: { "levelId": 3, "good": 0},255: { "levelId": 3, "good": 0},256: { "levelId": 3, "good": 0},257: { "levelId": 3, "good": 0},258: { "levelId": 3, "good": 0},259: { "levelId": 3, "good": 0},260: { "levelId": 3, "good": 0},261: { "levelId": 3, "good": 0},262: { "levelId": 3, "good": 0},263: { "levelId": 3, "good": 0},264: { "levelId": 3, "good": 0},265: { "levelId": 3, "good": 0},266: { "levelId": 3, "good": 0},267: { "levelId": 3, "good": 0},268: { "levelId": 3, "good": 0},269: { "levelId": 3, "good": 0},270: { "levelId": 3, "good": 0},271: { "levelId": 3, "good": 0},272: { "levelId": 3, "good": 0},273: { "levelId": 3, "good": 0},274: { "levelId": 3, "good": 0},275: { "levelId": 3, "good": 0},276: { "levelId": 3, "good": 0},277: { "levelId": 3, "good": 0},278: { "levelId": 3, "good": 0},279: { "levelId": 3, "good": 0},280: { "levelId": 3, "good": 0},281: { "levelId": 3, "good": 0},282: { "levelId": 3, "good": 0},283: { "levelId": 3, "good": 0},284: { "levelId": 3, "good": 0},285: { "levelId": 3, "good": 0},286: { "levelId": 3, "good": 0},287: { "levelId": 3, "good": 0},288: { "levelId": 3, "good": 0},289: { "levelId": 3, "good": 0},290: { "levelId": 3, "good": 0},291: { "levelId": 3, "good": 0},292: { "levelId": 3, "good": 0},293: { "levelId": 3, "good": 0},294: { "levelId": 3, "good": 0},295: { "levelId": 3, "good": 0},296: { "levelId": 3, "good": 0},297: { "levelId": 3, "good": 0},298: { "levelId": 3, "good": 0},299: { "levelId": 3, "good": 0},300: { "levelId": 3, "good": 0},301: { "levelId": 3, "good": 0},302: { "levelId": 3, "good": 0},303: { "levelId": 3, "good": 0},304: { "levelId": 3, "good": 0},305: { "levelId": 3, "good": 0},306: { "levelId": 3, "good": 0},307: { "levelId": 3, "good": 0},308: { "levelId": 3, "good": 0},309: { "levelId": 3, "good": 0},310: { "levelId": 3, "good": 0},311: { "levelId": 3, "good": 0},312: { "levelId": 3, "good": 0},313: { "levelId": 3, "good": 0},314: { "levelId": 3, "good": 0},315: { "levelId": 3, "good": 0},316: { "levelId": 3, "good": 0},317: { "levelId": 3, "good": 0},318: { "levelId": 3, "good": 0},319: { "levelId": 3, "good": 0},320: { "levelId": 3, "good": 0},321: { "levelId": 3, "good": 0},322: { "levelId": 3, "good": 0},323: { "levelId": 3, "good": 0},324: { "levelId": 3, "good": 0},325: { "levelId": 3, "good": 0},326: { "levelId": 3, "good": 0},327: { "levelId": 3, "good": 0},328: { "levelId": 3, "good": 0},329: { "levelId": 3, "good": 0},330: { "levelId": 3, "good": 0},331: { "levelId": 3, "good": 0},332: { "levelId": 3, "good": 0},333: { "levelId": 3, "good": 0},334: { "levelId": 3, "good": 0},335: { "levelId": 3, "good": 0},336: { "levelId": 3, "good": 0},337: { "levelId": 3, "good": 0},338: { "levelId": 3, "good": 0},339: { "levelId": 3, "good": 0},340: { "levelId": 3, "good": 0},341: { "levelId": 3, "good": 0},342: { "levelId": 3, "good": 0},343: { "levelId": 3, "good": 0},344: { "levelId": 3, "good": 0},345: { "levelId": 3, "good": 0},346: { "levelId": 3, "good": 0},347: { "levelId": 3, "good": 0},348: { "levelId": 3, "good": 0},349: { "levelId": 3, "good": 0},350: { "levelId": 3, "good": 0},351: { "levelId": 3, "good": 0},352: { "levelId": 3, "good": 0},353: { "levelId": 3, "good": 0},354: { "levelId": 3, "good": 0},355: { "levelId": 3, "good": 0},356: { "levelId": 3, "good": 0},357: { "levelId": 3, "good": 0},358: { "levelId": 3, "good": 0},359: { "levelId": 3, "good": 0},360: { "levelId": 3, "good": 0},361: { "levelId": 3, "good": 0},362: { "levelId": 3, "good": 0},363: { "levelId": 3, "good": 0},364: { "levelId": 3, "good": 0},365: { "levelId": 3, "good": 0},366: { "levelId": 3, "good": 0},367: { "levelId": 3, "good": 0},368: { "levelId": 3, "good": 0},369: { "levelId": 3, "good": 0},370: { "levelId": 3, "good": 0},371: { "levelId": 3, "good": 0},372: { "levelId": 3, "good": 0},373: { "levelId": 3, "good": 0},374: { "levelId": 3, "good": 0},375: { "levelId": 3, "good": 0},376: { "levelId": 3, "good": 0},377: { "levelId": 3, "good": 0},378: { "levelId": 3, "good": 0},379: { "levelId": 3, "good": 0},380: { "levelId": 3, "good": 0},381: { "levelId": 3, "good": 0},382: { "levelId": 3, "good": 0},383: { "levelId": 3, "good": 0},384: { "levelId": 3, "good": 0},385: { "levelId": 3, "good": 0},386: { "levelId": 3, "good": 0},387: { "levelId": 3, "good": 0},388: { "levelId": 3, "good": 0},389: { "levelId": 3, "good": 0},390: { "levelId": 3, "good": 0},391: { "levelId": 3, "good": 0},392: { "levelId": 3, "good": 0},393: { "levelId": 3, "good": 0},394: { "levelId": 3, "good": 0},395: { "levelId": 3, "good": 0},396: { "levelId": 3, "good": 0},397: { "levelId": 3, "good": 0},398: { "levelId": 3, "good": 0},399: { "levelId": 3, "good": 0},400: { "levelId": 3, "good": 0},401: { "levelId": 3, "good": 0},402: { "levelId": 3, "good": 0},403: { "levelId": 3, "good": 0},404: { "levelId": 3, "good": 0},405: { "levelId": 3, "good": 0},406: { "levelId": 3, "good": 0},407: { "levelId": 3, "good": 0},408: { "levelId": 3, "good": 0},409: { "levelId": 3, "good": 0},410: { "levelId": 3, "good": 0},411: { "levelId": 3, "good": 0},412: { "levelId": 3, "good": 0},413: { "levelId": 3, "good": 0},414: { "levelId": 3, "good": 0},415: { "levelId": 3, "good": 0},416: { "levelId": 3, "good": 0},417: { "levelId": 3, "good": 0},418: { "levelId": 3, "good": 0},419: { "levelId": 3, "good": 0},420: { "levelId": 3, "good": 0},421: { "levelId": 3, "good": 0},422: { "levelId": 3, "good": 0},423: { "levelId": 3, "good": 0},424: { "levelId": 3, "good": 0},425: { "levelId": 3, "good": 0},426: { "levelId": 3, "good": 0},427: { "levelId": 3, "good": 0},428: { "levelId": 3, "good": 0},429: { "levelId": 3, "good": 0},430: { "levelId": 3, "good": 0},431: { "levelId": 3, "good": 0},432: { "levelId": 3, "good": 0},433: { "levelId": 3, "good": 0},434: { "levelId": 3, "good": 0},435: { "levelId": 3, "good": 0},436: { "levelId": 3, "good": 0},437: { "levelId": 3, "good": 0},438: { "levelId": 3, "good": 0},439: { "levelId": 3, "good": 0},440: { "levelId": 3, "good": 0},441: { "levelId": 3, "good": 0},442: { "levelId": 3, "good": 0},443: { "levelId": 3, "good": 0},444: { "levelId": 3, "good": 0},445: { "levelId": 3, "good": 0},446: { "levelId": 3, "good": 0},447: { "levelId": 3, "good": 0},448: { "levelId": 3, "good": 0},449: { "levelId": 3, "good": 0},450: { "levelId": 3, "good": 0},451: { "levelId": 3, "good": 0},452: { "levelId": 3, "good": 0},453: { "levelId": 3, "good": 0},454: { "levelId": 3, "good": 0},455: { "levelId": 3, "good": 0},456: { "levelId": 3, "good": 0},457: { "levelId": 3, "good": 0},458: { "levelId": 3, "good": 0},459: { "levelId": 3, "good": 0},460: { "levelId": 3, "good": 0},461: { "levelId": 3, "good": 0},462: { "levelId": 3, "good": 0},463: { "levelId": 3, "good": 0},464: { "levelId": 3, "good": 0},465: { "levelId": 3, "good": 0},466: { "levelId": 3, "good": 0},467: { "levelId": 3, "good": 0},468: { "levelId": 3, "good": 0},469: { "levelId": 3, "good": 0},470: { "levelId": 3, "good": 0},471: { "levelId": 3, "good": 0},472: { "levelId": 3, "good": 0},473: { "levelId": 3, "good": 0},474: { "levelId": 3, "good": 0},475: { "levelId": 3, "good": 0},476: { "levelId": 3, "good": 0},477: { "levelId": 3, "good": 0},478: { "levelId": 3, "good": 0},479: { "levelId": 3, "good": 0},480: { "levelId": 3, "good": 0},481: { "levelId": 3, "good": 0},482: { "levelId": 3, "good": 0},483: { "levelId": 3, "good": 0},484: { "levelId": 3, "good": 0},485: { "levelId": 3, "good": 0},486: { "levelId": 3, "good": 0},487: { "levelId": 3, "good": 0},488: { "levelId": 3, "good": 0},489: { "levelId": 3, "good": 0},490: { "levelId": 3, "good": 0},491: { "levelId": 3, "good": 0},492: { "levelId": 3, "good": 0},493: { "levelId": 3, "good": 0},494: { "levelId": 3, "good": 0},495: { "levelId": 3, "good": 0},496: { "levelId": 3, "good": 0},497: { "levelId": 3, "good": 0},498: { "levelId": 3, "good": 0},499: { "levelId": 3, "good": 0},500: { "levelId": 3, "good": 0},501: { "levelId": 3, "good": 0},502: { "levelId": 3, "good": 0},503: { "levelId": 3, "good": 0},504: { "levelId": 3, "good": 0},505: { "levelId": 3, "good": 0},506: { "levelId": 3, "good": 0},507: { "levelId": 3, "good": 0},508: { "levelId": 3, "good": 0},509: { "levelId": 3, "good": 0},510: { "levelId": 3, "good": 0},511: { "levelId": 3, "good": 0},512: { "levelId": 3, "good": 0},513: { "levelId": 3, "good": 0},514: { "levelId": 3, "good": 0},515: { "levelId": 3, "good": 0},516: { "levelId": 3, "good": 0},517: { "levelId": 3, "good": 0},518: { "levelId": 3, "good": 0},519: { "levelId": 3, "good": 0},520: { "levelId": 3, "good": 0},521: { "levelId": 3, "good": 0},522: { "levelId": 3, "good": 0},523: { "levelId": 3, "good": 0},524: { "levelId": 3, "good": 0},525: { "levelId": 3, "good": 0},526: { "levelId": 3, "good": 0},527: { "levelId": 3, "good": 0},528: { "levelId": 3, "good": 0},529: { "levelId": 3, "good": 0},530: { "levelId": 3, "good": 0},531: { "levelId": 3, "good": 0},532: { "levelId": 3, "good": 0},533: { "levelId": 3, "good": 0},534: { "levelId": 3, "good": 0},535: { "levelId": 3, "good": 0},536: { "levelId": 3, "good": 0},537: { "levelId": 3, "good": 0},538: { "levelId": 3, "good": 0},539: { "levelId": 3, "good": 0},540: { "levelId": 3, "good": 0},541: { "levelId": 3, "good": 0},542: { "levelId": 3, "good": 0},543: { "levelId": 3, "good": 0},544: { "levelId": 3, "good": 0},545: { "levelId": 3, "good": 0},546: { "levelId": 3, "good": 0},547: { "levelId": 3, "good": 0},548: { "levelId": 3, "good": 0},549: { "levelId": 3, "good": 0},550: { "levelId": 3, "good": 0},551: { "levelId": 3, "good": 0},552: { "levelId": 3, "good": 0},553: { "levelId": 3, "good": 0},554: { "levelId": 3, "good": 0},555: { "levelId": 3, "good": 0},556: { "levelId": 3, "good": 0},557: { "levelId": 3, "good": 0},558: { "levelId": 3, "good": 0},559: { "levelId": 3, "good": 0},560: { "levelId": 3, "good": 0},561: { "levelId": 3, "good": 0},562: { "levelId": 3, "good": 0},563: { "levelId": 3, "good": 0},564: { "levelId": 3, "good": 0},565: { "levelId": 3, "good": 0},566: { "levelId": 3, "good": 0},567: { "levelId": 3, "good": 0},568: { "levelId": 3, "good": 0},569: { "levelId": 3, "good": 0},570: { "levelId": 3, "good": 0},571: { "levelId": 3, "good": 0},572: { "levelId": 3, "good": 0},573: { "levelId": 3, "good": 0},574: { "levelId": 3, "good": 0},575: { "levelId": 3, "good": 0},576: { "levelId": 3, "good": 0},577: { "levelId": 3, "good": 0},578: { "levelId": 3, "good": 0},579: { "levelId": 3, "good": 0},580: { "levelId": 3, "good": 0},581: { "levelId": 3, "good": 0},582: { "levelId": 3, "good": 0},583: { "levelId": 3, "good": 0},584: { "levelId": 3, "good": 0},585: { "levelId": 3, "good": 0},586: { "levelId": 3, "good": 0},587: { "levelId": 3, "good": 0},588: { "levelId": 3, "good": 0},589: { "levelId": 3, "good": 0},590: { "levelId": 3, "good": 0},591: { "levelId": 3, "good": 0},592: { "levelId": 3, "good": 0},593: { "levelId": 3, "good": 0},594: { "levelId": 3, "good": 0},595: { "levelId": 3, "good": 0},596: { "levelId": 3, "good": 0},597: { "levelId": 3, "good": 0},598: { "levelId": 3, "good": 0},599: { "levelId": 3, "good": 0},600: { "levelId": 3, "good": 0},601: { "levelId": 3, "good": 0},602: { "levelId": 3, "good": 0},603: { "levelId": 3, "good": 0},604: { "levelId": 3, "good": 0},605: { "levelId": 3, "good": 0},606: { "levelId": 3, "good": 0},607: { "levelId": 3, "good": 0},608: { "levelId": 3, "good": 0},609: { "levelId": 3, "good": 0},610: { "levelId": 3, "good": 0},611: { "levelId": 3, "good": 0},612: { "levelId": 3, "good": 0},613: { "levelId": 3, "good": 0},614: { "levelId": 3, "good": 0},615: { "levelId": 3, "good": 0},616: { "levelId": 3, "good": 0},617: { "levelId": 3, "good": 0},618: { "levelId": 3, "good": 0},619: { "levelId": 3, "good": 0},620: { "levelId": 3, "good": 0},621: { "levelId": 3, "good": 0},622: { "levelId": 3, "good": 0},623: { "levelId": 3, "good": 0},624: { "levelId": 3, "good": 0},625: { "levelId": 3, "good": 0},626: { "levelId": 3, "good": 0},627: { "levelId": 3, "good": 0},628: { "levelId": 3, "good": 0},629: { "levelId": 3, "good": 0},630: { "levelId": 3, "good": 0},631: { "levelId": 3, "good": 0},632: { "levelId": 3, "good": 0},633: { "levelId": 3, "good": 0},634: { "levelId": 3, "good": 0},635: { "levelId": 3, "good": 0},636: { "levelId": 3, "good": 0},637: { "levelId": 3, "good": 0},638: { "levelId": 3, "good": 0},639: { "levelId": 3, "good": 0},640: { "levelId": 3, "good": 0},641: { "levelId": 3, "good": 0},642: { "levelId": 3, "good": 0},643: { "levelId": 3, "good": 0},644: { "levelId": 3, "good": 0},645: { "levelId": 3, "good": 0},646: { "levelId": 3, "good": 0},647: { "levelId": 3, "good": 0},648: { "levelId": 3, "good": 0},649: { "levelId": 3, "good": 0},650: { "levelId": 3, "good": 0},651: { "levelId": 3, "good": 0},652: { "levelId": 3, "good": 0},653: { "levelId": 3, "good": 0},654: { "levelId": 3, "good": 0},655: { "levelId": 3, "good": 0},656: { "levelId": 3, "good": 0},657: { "levelId": 3, "good": 0},658: { "levelId": 3, "good": 0},659: { "levelId": 3, "good": 0},660: { "levelId": 3, "good": 0},661: { "levelId": 3, "good": 0},662: { "levelId": 3, "good": 0},663: { "levelId": 3, "good": 0},664: { "levelId": 3, "good": 0},665: { "levelId": 3, "good": 0},666: { "levelId": 3, "good": 0},667: { "levelId": 3, "good": 0},668: { "levelId": 3, "good": 0},669: { "levelId": 3, "good": 0},670: { "levelId": 3, "good": 0},671: { "levelId": 3, "good": 0},672: { "levelId": 3, "good": 0},673: { "levelId": 3, "good": 0},674: { "levelId": 3, "good": 0},675: { "levelId": 3, "good": 0},676: { "levelId": 3, "good": 0},677: { "levelId": 3, "good": 0},678: { "levelId": 3, "good": 0},679: { "levelId": 3, "good": 0},680: { "levelId": 3, "good": 0},681: { "levelId": 3, "good": 0},682: { "levelId": 3, "good": 0},683: { "levelId": 3, "good": 0},684: { "levelId": 3, "good": 0},685: { "levelId": 3, "good": 0},686: { "levelId": 3, "good": 0},687: { "levelId": 3, "good": 0},688: { "levelId": 3, "good": 0},689: { "levelId": 3, "good": 0},690: { "levelId": 3, "good": 0},691: { "levelId": 3, "good": 0},692: { "levelId": 3, "good": 0},693: { "levelId": 3, "good": 0},694: { "levelId": 3, "good": 0},695: { "levelId": 3, "good": 0},696: { "levelId": 3, "good": 0},697: { "levelId": 3, "good": 0},698: { "levelId": 3, "good": 0},699: { "levelId": 3, "good": 0},700: { "levelId": 3, "good": 0},701: { "levelId": 3, "good": 0},702: { "levelId": 3, "good": 0},703: { "levelId": 3, "good": 0},704: { "levelId": 3, "good": 0},705: { "levelId": 3, "good": 0},706: { "levelId": 3, "good": 0},707: { "levelId": 3, "good": 0},708: { "levelId": 3, "good": 0},709: { "levelId": 3, "good": 0},710: { "levelId": 3, "good": 0},711: { "levelId": 3, "good": 0},712: { "levelId": 3, "good": 0},713: { "levelId": 3, "good": 0},714: { "levelId": 3, "good": 0},715: { "levelId": 3, "good": 0},716: { "levelId": 3, "good": 0},717: { "levelId": 3, "good": 0},718: { "levelId": 3, "good": 0},719: { "levelId": 3, "good": 0},720: { "levelId": 3, "good": 0},721: { "levelId": 3, "good": 0},722: { "levelId": 3, "good": 0},723: { "levelId": 3, "good": 0},724: { "levelId": 3, "good": 0},725: { "levelId": 3, "good": 0},726: { "levelId": 3, "good": 0},727: { "levelId": 3, "good": 0},728: { "levelId": 3, "good": 0},729: { "levelId": 3, "good": 0},730: { "levelId": 3, "good": 0},731: { "levelId": 3, "good": 0},732: { "levelId": 3, "good": 0},733: { "levelId": 3, "good": 0},734: { "levelId": 3, "good": 0},735: { "levelId": 3, "good": 0},736: { "levelId": 3, "good": 0},737: { "levelId": 3, "good": 0},738: { "levelId": 3, "good": 0},739: { "levelId": 3, "good": 0},740: { "levelId": 3, "good": 0},741: { "levelId": 3, "good": 0},742: { "levelId": 3, "good": 0},743: { "levelId": 3, "good": 0},744: { "levelId": 3, "good": 0},745: { "levelId": 3, "good": 0},746: { "levelId": 3, "good": 0},747: { "levelId": 3, "good": 0},748: { "levelId": 3, "good": 0},749: { "levelId": 3, "good": 0},750: { "levelId": 3, "good": 0},751: { "levelId": 3, "good": 0},752: { "levelId": 3, "good": 0},753: { "levelId": 3, "good": 0},754: { "levelId": 3, "good": 0},755: { "levelId": 3, "good": 0},756: { "levelId": 3, "good": 0},757: { "levelId": 3, "good": 0},758: { "levelId": 3, "good": 0},759: { "levelId": 3, "good": 0},760: { "levelId": 3, "good": 0},761: { "levelId": 3, "good": 0},762: { "levelId": 3, "good": 0},763: { "levelId": 3, "good": 0},764: { "levelId": 3, "good": 0},765: { "levelId": 3, "good": 0},766: { "levelId": 3, "good": 0},767: { "levelId": 3, "good": 0},768: { "levelId": 3, "good": 0},769: { "levelId": 3, "good": 0},770: { "levelId": 3, "good": 0},771: { "levelId": 3, "good": 0},772: { "levelId": 3, "good": 0},773: { "levelId": 3, "good": 0},774: { "levelId": 3, "good": 0},775: { "levelId": 3, "good": 0},776: { "levelId": 3, "good": 0},777: { "levelId": 3, "good": 0},778: { "levelId": 3, "good": 0},779: { "levelId": 3, "good": 0},780: { "levelId": 3, "good": 0},781: { "levelId": 3, "good": 0},782: { "levelId": 3, "good": 0},783: { "levelId": 3, "good": 0},784: { "levelId": 3, "good": 0},785: { "levelId": 3, "good": 0},786: { "levelId": 3, "good": 0},787: { "levelId": 3, "good": 0},788: { "levelId": 3, "good": 0},789: { "levelId": 3, "good": 0},790: { "levelId": 3, "good": 0},791: { "levelId": 3, "good": 0},792: { "levelId": 3, "good": 0},793: { "levelId": 3, "good": 0},794: { "levelId": 3, "good": 0},795: { "levelId": 3, "good": 0},796: { "levelId": 3, "good": 0},797: { "levelId": 3, "good": 0},798: { "levelId": 3, "good": 0},799: { "levelId": 3, "good": 0},800: { "levelId": 3, "good": 0},801: { "levelId": 3, "good": 0},802: { "levelId": 3, "good": 0},803: { "levelId": 3, "good": 0},804: { "levelId": 3, "good": 0},805: { "levelId": 3, "good": 0},806: { "levelId": 3, "good": 0},807: { "levelId": 3, "good": 0},808: { "levelId": 3, "good": 0},809: { "levelId": 3, "good": 0},810: { "levelId": 3, "good": 0},811: { "levelId": 3, "good": 0},812: { "levelId": 3, "good": 0},813: { "levelId": 3, "good": 0},814: { "levelId": 3, "good": 0},815: { "levelId": 3, "good": 0},816: { "levelId": 3, "good": 0},817: { "levelId": 3, "good": 0},818: { "levelId": 3, "good": 0},819: { "levelId": 3, "good": 0},820: { "levelId": 3, "good": 0},821: { "levelId": 3, "good": 0},822: { "levelId": 3, "good": 0},823: { "levelId": 3, "good": 0},824: { "levelId": 3, "good": 0},825: { "levelId": 3, "good": 0},826: { "levelId": 3, "good": 0},827: { "levelId": 3, "good": 0},828: { "levelId": 3, "good": 0},829: { "levelId": 3, "good": 0},830: { "levelId": 3, "good": 0},831: { "levelId": 3, "good": 0},832: { "levelId": 3, "good": 0},833: { "levelId": 3, "good": 0},834: { "levelId": 3, "good": 0},835: { "levelId": 3, "good": 0},836: { "levelId": 3, "good": 0},837: { "levelId": 3, "good": 0},838: { "levelId": 3, "good": 0},839: { "levelId": 3, "good": 0},840: { "levelId": 3, "good": 0},841: { "levelId": 3, "good": 0},842: { "levelId": 3, "good": 0},843: { "levelId": 3, "good": 0},844: { "levelId": 3, "good": 0},845: { "levelId": 3, "good": 0},846: { "levelId": 3, "good": 0},847: { "levelId": 3, "good": 0},848: { "levelId": 3, "good": 0},849: { "levelId": 3, "good": 0},850: { "levelId": 3, "good": 0},851: { "levelId": 3, "good": 0},852: { "levelId": 3, "good": 0},853: { "levelId": 3, "good": 0},854: { "levelId": 3, "good": 0},855: { "levelId": 3, "good": 0},856: { "levelId": 3, "good": 0},857: { "levelId": 3, "good": 0},858: { "levelId": 3, "good": 0},859: { "levelId": 3, "good": 0},860: { "levelId": 3, "good": 0},861: { "levelId": 3, "good": 0},862: { "levelId": 3, "good": 0},863: { "levelId": 3, "good": 0},864: { "levelId": 3, "good": 0},865: { "levelId": 3, "good": 0},866: { "levelId": 3, "good": 0},867: { "levelId": 3, "good": 0},868: { "levelId": 3, "good": 0},869: { "levelId": 3, "good": 0},870: { "levelId": 3, "good": 0},871: { "levelId": 3, "good": 0},872: { "levelId": 3, "good": 0},873: { "levelId": 3, "good": 0},874: { "levelId": 3, "good": 0},875: { "levelId": 3, "good": 0},876: { "levelId": 3, "good": 0},877: { "levelId": 3, "good": 0},878: { "levelId": 3, "good": 0},879: { "levelId": 3, "good": 0},880: { "levelId": 3, "good": 0},881: { "levelId": 3, "good": 0},882: { "levelId": 3, "good": 0},883: { "levelId": 3, "good": 0},884: { "levelId": 3, "good": 0},885: { "levelId": 3, "good": 0},886: { "levelId": 3, "good": 0},887: { "levelId": 3, "good": 0},888: { "levelId": 3, "good": 0},889: { "levelId": 3, "good": 0},890: { "levelId": 3, "good": 0},891: { "levelId": 3, "good": 0},892: { "levelId": 3, "good": 0},893: { "levelId": 3, "good": 0},894: { "levelId": 3, "good": 0},895: { "levelId": 3, "good": 0},896: { "levelId": 3, "good": 0},897: { "levelId": 3, "good": 0},898: { "levelId": 3, "good": 0},899: { "levelId": 3, "good": 0},900: { "levelId": 3, "good": 0},901: { "levelId": 3, "good": 0},902: { "levelId": 3, "good": 0},903: { "levelId": 3, "good": 0},904: { "levelId": 3, "good": 0},905: { "levelId": 3, "good": 0},906: { "levelId": 3, "good": 0},907: { "levelId": 3, "good": 0},908: { "levelId": 3, "good": 0},909: { "levelId": 3, "good": 0},910: { "levelId": 3, "good": 0},911: { "levelId": 3, "good": 0},912: { "levelId": 3, "good": 0},913: { "levelId": 3, "good": 0},914: { "levelId": 3, "good": 0},915: { "levelId": 3, "good": 0},916: { "levelId": 3, "good": 0},917: { "levelId": 3, "good": 0},918: { "levelId": 3, "good": 0},919: { "levelId": 3, "good": 0},920: { "levelId": 3, "good": 0},921: { "levelId": 3, "good": 0},922: { "levelId": 3, "good": 0},923: { "levelId": 3, "good": 0},924: { "levelId": 3, "good": 0},925: { "levelId": 3, "good": 0},926: { "levelId": 3, "good": 0},927: { "levelId": 3, "good": 0},928: { "levelId": 3, "good": 0},929: { "levelId": 3, "good": 0},930: { "levelId": 3, "good": 0},931: { "levelId": 3, "good": 0},932: { "levelId": 3, "good": 0},933: { "levelId": 3, "good": 0},934: { "levelId": 3, "good": 0},935: { "levelId": 3, "good": 0},936: { "levelId": 3, "good": 0},937: { "levelId": 3, "good": 0},938: { "levelId": 3, "good": 0},939: { "levelId": 3, "good": 0},940: { "levelId": 3, "good": 0},941: { "levelId": 3, "good": 0},942: { "levelId": 3, "good": 0},943: { "levelId": 3, "good": 0},944: { "levelId": 3, "good": 0},945: { "levelId": 3, "good": 0},946: { "levelId": 3, "good": 0},947: { "levelId": 3, "good": 0},948: { "levelId": 3, "good": 0},949: { "levelId": 3, "good": 0},950: { "levelId": 3, "good": 0},951: { "levelId": 3, "good": 0},952: { "levelId": 3, "good": 0},953: { "levelId": 3, "good": 0},954: { "levelId": 3, "good": 0},955: { "levelId": 3, "good": 0},956: { "levelId": 3, "good": 0},957: { "levelId": 3, "good": 0},958: { "levelId": 3, "good": 0},959: { "levelId": 3, "good": 0},960: { "levelId": 3, "good": 0},961: { "levelId": 3, "good": 0},962: { "levelId": 3, "good": 0},963: { "levelId": 3, "good": 0},964: { "levelId": 3, "good": 0},965: { "levelId": 3, "good": 0},966: { "levelId": 3, "good": 0},967: { "levelId": 3, "good": 0},968: { "levelId": 3, "good": 0},969: { "levelId": 3, "good": 0},970: { "levelId": 3, "good": 0},971: { "levelId": 3, "good": 0},972: { "levelId": 3, "good": 0},973: { "levelId": 3, "good": 0},974: { "levelId": 3, "good": 0},975: { "levelId": 3, "good": 0},976: { "levelId": 3, "good": 0},977: { "levelId": 3, "good": 0},978: { "levelId": 3, "good": 0},979: { "levelId": 3, "good": 0},980: { "levelId": 3, "good": 0},981: { "levelId": 3, "good": 0},982: { "levelId": 3, "good": 0},983: { "levelId": 3, "good": 0},984: { "levelId": 3, "good": 0},985: { "levelId": 3, "good": 0},986: { "levelId": 3, "good": 0},987: { "levelId": 3, "good": 0},988: { "levelId": 3, "good": 0},989: { "levelId": 3, "good": 0},990: { "levelId": 3, "good": 0},991: { "levelId": 3, "good": 0},992: { "levelId": 3, "good": 0},993: { "levelId": 3, "good": 0},994: { "levelId": 3, "good": 0},995: { "levelId": 3, "good": 0},996: { "levelId": 3, "good": 0},997: { "levelId": 3, "good": 0},998: { "levelId": 3, "good": 0},999: { "levelId": 3, "good": 0},1000: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0</v>
@@ -7687,7 +7785,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1</v>
@@ -7703,7 +7801,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>2</v>
@@ -7719,7 +7817,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>3</v>
@@ -7735,7 +7833,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>4</v>
@@ -7751,7 +7849,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>5</v>
@@ -7767,7 +7865,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>6</v>
@@ -7783,7 +7881,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>7</v>
@@ -7799,7 +7897,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>2</v>
@@ -7814,7 +7912,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>1</v>
@@ -7829,7 +7927,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>2</v>
@@ -7844,7 +7942,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>3</v>
@@ -7859,7 +7957,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>4</v>
@@ -7874,7 +7972,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>5</v>
@@ -7889,7 +7987,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>6</v>
@@ -7904,7 +8002,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>7</v>
@@ -7919,7 +8017,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>5</v>
@@ -7934,7 +8032,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>6</v>
@@ -7949,7 +8047,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>7</v>
@@ -7964,7 +8062,7 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>0</v>
@@ -7979,7 +8077,7 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="6" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>1</v>
@@ -7994,7 +8092,7 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>2</v>
@@ -8009,7 +8107,7 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>3</v>
@@ -8024,7 +8122,7 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="6" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>4</v>
@@ -8039,7 +8137,7 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="6" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>5</v>
@@ -8054,7 +8152,7 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="6" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>6</v>
@@ -8069,7 +8167,7 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="6" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>7</v>
@@ -8084,7 +8182,7 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="6" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>0</v>
@@ -8099,7 +8197,7 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="6" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>1</v>
@@ -8114,7 +8212,7 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="6" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>2</v>
@@ -8129,7 +8227,7 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="6" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>3</v>
@@ -8144,7 +8242,7 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="6" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>4</v>
@@ -8159,7 +8257,7 @@
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="6" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>5</v>
@@ -8174,7 +8272,7 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="6" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>6</v>
@@ -8189,7 +8287,7 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="6" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>7</v>
@@ -8204,7 +8302,7 @@
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="6" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>0</v>
@@ -8219,7 +8317,7 @@
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="6" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>1</v>
@@ -8234,7 +8332,7 @@
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>2</v>
@@ -8249,7 +8347,7 @@
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>3</v>
@@ -8264,7 +8362,7 @@
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>4</v>
@@ -8279,7 +8377,7 @@
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>5</v>
@@ -8294,7 +8392,7 @@
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>6</v>
@@ -8309,7 +8407,7 @@
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="B44" s="0" t="n">
         <v>7</v>
@@ -8324,7 +8422,7 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="B45" s="0" t="n">
         <v>0</v>
@@ -8339,7 +8437,7 @@
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="B46" s="0" t="n">
         <v>1</v>
@@ -8354,7 +8452,7 @@
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="B47" s="0" t="n">
         <v>2</v>
@@ -8369,7 +8467,7 @@
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="B48" s="0" t="n">
         <v>3</v>
@@ -8384,7 +8482,7 @@
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="B49" s="0" t="n">
         <v>4</v>
@@ -8399,7 +8497,7 @@
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="B50" s="0" t="n">
         <v>5</v>
@@ -8414,7 +8512,7 @@
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="B51" s="0" t="n">
         <v>6</v>
@@ -8429,7 +8527,7 @@
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="B52" s="0" t="n">
         <v>7</v>
@@ -8444,7 +8542,7 @@
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="B53" s="0" t="n">
         <v>0</v>
@@ -8459,7 +8557,7 @@
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="B54" s="0" t="n">
         <v>1</v>
@@ -8474,7 +8572,7 @@
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="B55" s="0" t="n">
         <v>2</v>
@@ -8489,7 +8587,7 @@
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="B56" s="0" t="n">
         <v>3</v>
@@ -8504,7 +8602,7 @@
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="B57" s="0" t="n">
         <v>4</v>
@@ -8519,7 +8617,7 @@
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="B58" s="0" t="n">
         <v>5</v>
@@ -8534,7 +8632,7 @@
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="B59" s="0" t="n">
         <v>6</v>
@@ -8549,7 +8647,7 @@
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="B60" s="0" t="n">
         <v>7</v>
@@ -8564,7 +8662,7 @@
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="B61" s="0" t="n">
         <v>0</v>
@@ -8579,7 +8677,7 @@
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="B62" s="0" t="n">
         <v>1</v>
@@ -8594,7 +8692,7 @@
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="B63" s="0" t="n">
         <v>2</v>
@@ -8609,7 +8707,7 @@
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="B64" s="0" t="n">
         <v>3</v>
@@ -8624,7 +8722,7 @@
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="B65" s="0" t="n">
         <v>4</v>
@@ -8639,7 +8737,7 @@
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="B66" s="0" t="n">
         <v>5</v>
@@ -8654,7 +8752,7 @@
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="B67" s="0" t="n">
         <v>6</v>
@@ -8669,7 +8767,7 @@
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="B68" s="0" t="n">
         <v>7</v>
@@ -8684,7 +8782,7 @@
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="B69" s="0" t="n">
         <v>0</v>
@@ -8699,7 +8797,7 @@
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="B70" s="0" t="n">
         <v>1</v>
@@ -8714,7 +8812,7 @@
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="B71" s="0" t="n">
         <v>2</v>
@@ -8729,7 +8827,7 @@
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="B72" s="0" t="n">
         <v>3</v>
@@ -8744,7 +8842,7 @@
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="B73" s="0" t="n">
         <v>4</v>
@@ -8759,7 +8857,7 @@
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="B74" s="0" t="n">
         <v>5</v>
@@ -8774,7 +8872,7 @@
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="B75" s="0" t="n">
         <v>6</v>
@@ -8789,7 +8887,7 @@
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="B76" s="0" t="n">
         <v>7</v>
@@ -8804,7 +8902,7 @@
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="B77" s="0" t="n">
         <v>0</v>
@@ -8819,7 +8917,7 @@
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="B78" s="0" t="n">
         <v>1</v>
@@ -8834,7 +8932,7 @@
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="B79" s="0" t="n">
         <v>2</v>
@@ -8849,7 +8947,7 @@
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="B80" s="0" t="n">
         <v>3</v>
@@ -8864,7 +8962,7 @@
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="B81" s="0" t="n">
         <v>4</v>
@@ -8879,7 +8977,7 @@
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="B82" s="0" t="n">
         <v>5</v>
@@ -8894,7 +8992,7 @@
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="B83" s="0" t="n">
         <v>6</v>
@@ -8909,7 +9007,7 @@
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="B84" s="0" t="n">
         <v>7</v>
@@ -8924,7 +9022,7 @@
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="6" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="B85" s="0" t="n">
         <v>0</v>
@@ -8939,7 +9037,7 @@
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="6" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="B86" s="0" t="n">
         <v>1</v>
@@ -8954,7 +9052,7 @@
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="6" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="B87" s="0" t="n">
         <v>2</v>
@@ -8969,7 +9067,7 @@
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="6" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="B88" s="0" t="n">
         <v>3</v>
@@ -8984,7 +9082,7 @@
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="B89" s="0" t="n">
         <v>4</v>
@@ -8999,7 +9097,7 @@
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="B90" s="0" t="n">
         <v>5</v>
@@ -9014,7 +9112,7 @@
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="B91" s="0" t="n">
         <v>6</v>
@@ -9029,7 +9127,7 @@
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="B92" s="0" t="n">
         <v>7</v>
@@ -9044,7 +9142,7 @@
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="B93" s="0" t="n">
         <v>0</v>
@@ -9059,7 +9157,7 @@
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="B94" s="0" t="n">
         <v>1</v>
@@ -9074,7 +9172,7 @@
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="B95" s="0" t="n">
         <v>2</v>
@@ -9089,7 +9187,7 @@
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="B96" s="0" t="n">
         <v>3</v>
@@ -9104,7 +9202,7 @@
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="B97" s="0" t="n">
         <v>4</v>
@@ -9119,7 +9217,7 @@
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="B98" s="0" t="n">
         <v>5</v>
@@ -9134,7 +9232,7 @@
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="B99" s="0" t="n">
         <v>6</v>
@@ -9149,7 +9247,7 @@
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="B100" s="0" t="n">
         <v>7</v>
@@ -9164,7 +9262,7 @@
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="B101" s="0" t="n">
         <v>0</v>
@@ -9179,7 +9277,7 @@
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="B102" s="0" t="n">
         <v>1</v>
@@ -9194,7 +9292,7 @@
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="B103" s="0" t="n">
         <v>2</v>
@@ -9209,7 +9307,7 @@
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="B104" s="0" t="n">
         <v>3</v>
@@ -9224,7 +9322,7 @@
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="B105" s="0" t="n">
         <v>4</v>
@@ -9239,7 +9337,7 @@
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="B106" s="0" t="n">
         <v>5</v>
@@ -9254,7 +9352,7 @@
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="B107" s="0" t="n">
         <v>6</v>
@@ -9269,7 +9367,7 @@
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="B108" s="0" t="n">
         <v>7</v>
@@ -9284,7 +9382,7 @@
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="B109" s="0" t="n">
         <v>0</v>
@@ -9299,7 +9397,7 @@
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="B110" s="0" t="n">
         <v>1</v>
@@ -9314,7 +9412,7 @@
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="B111" s="0" t="n">
         <v>2</v>
@@ -9329,7 +9427,7 @@
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="B112" s="0" t="n">
         <v>3</v>
@@ -9344,7 +9442,7 @@
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="B113" s="0" t="n">
         <v>4</v>
@@ -9359,7 +9457,7 @@
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="B114" s="0" t="n">
         <v>5</v>
@@ -9374,7 +9472,7 @@
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="B115" s="0" t="n">
         <v>6</v>
@@ -9389,7 +9487,7 @@
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="B116" s="0" t="n">
         <v>7</v>
@@ -9404,7 +9502,7 @@
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B117" s="0" t="n">
         <v>0</v>
@@ -9419,7 +9517,7 @@
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B118" s="0" t="n">
         <v>1</v>
@@ -9434,7 +9532,7 @@
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B119" s="0" t="n">
         <v>2</v>
@@ -9449,7 +9547,7 @@
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B120" s="0" t="n">
         <v>3</v>
@@ -9464,7 +9562,7 @@
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B121" s="0" t="n">
         <v>4</v>
@@ -9479,7 +9577,7 @@
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B122" s="0" t="n">
         <v>5</v>
@@ -9494,7 +9592,7 @@
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B123" s="0" t="n">
         <v>6</v>
@@ -9509,7 +9607,7 @@
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="B124" s="0" t="n">
         <v>0</v>
@@ -9524,7 +9622,7 @@
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="B125" s="0" t="n">
         <v>1</v>
@@ -9539,7 +9637,7 @@
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="B126" s="0" t="n">
         <v>2</v>
@@ -9554,7 +9652,7 @@
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="B127" s="0" t="n">
         <v>3</v>
@@ -9569,7 +9667,7 @@
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="B128" s="0" t="n">
         <v>4</v>
@@ -9584,7 +9682,7 @@
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="B129" s="0" t="n">
         <v>5</v>
@@ -9599,7 +9697,7 @@
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="B130" s="0" t="n">
         <v>6</v>
@@ -9614,7 +9712,7 @@
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="B131" s="0" t="n">
         <v>7</v>
@@ -9629,7 +9727,7 @@
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="B132" s="0" t="n">
         <v>0</v>
@@ -9644,7 +9742,7 @@
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="B133" s="0" t="n">
         <v>1</v>
@@ -9659,7 +9757,7 @@
     </row>
     <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="B134" s="0" t="n">
         <v>2</v>
@@ -9674,7 +9772,7 @@
     </row>
     <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="B135" s="0" t="n">
         <v>3</v>
@@ -9689,7 +9787,7 @@
     </row>
     <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="B136" s="0" t="n">
         <v>4</v>
@@ -9704,7 +9802,7 @@
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="B137" s="0" t="n">
         <v>5</v>
@@ -9719,7 +9817,7 @@
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="6" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="B138" s="0" t="n">
         <v>3</v>
@@ -9734,7 +9832,7 @@
     </row>
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="B139" s="0" t="n">
         <v>4</v>
@@ -9749,7 +9847,7 @@
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="B140" s="0" t="n">
         <v>5</v>
@@ -9764,7 +9862,7 @@
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="B141" s="0" t="n">
         <v>6</v>
@@ -9779,7 +9877,7 @@
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="B142" s="0" t="n">
         <v>7</v>
@@ -9794,7 +9892,7 @@
     </row>
     <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B143" s="0" t="n">
         <v>7</v>
@@ -9809,7 +9907,7 @@
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="B144" s="0" t="n">
         <v>3</v>
@@ -9824,7 +9922,7 @@
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="B145" s="0" t="n">
         <v>4</v>
@@ -9839,7 +9937,7 @@
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="B146" s="0" t="n">
         <v>5</v>
@@ -9854,7 +9952,7 @@
     </row>
     <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="B147" s="0" t="n">
         <v>5</v>
@@ -9869,7 +9967,7 @@
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="B148" s="0" t="n">
         <v>6</v>
@@ -9884,7 +9982,7 @@
     </row>
     <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="B149" s="0" t="n">
         <v>7</v>
@@ -9899,7 +9997,7 @@
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="B150" s="0" t="n">
         <v>0</v>
@@ -9914,7 +10012,7 @@
     </row>
     <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="B151" s="0" t="n">
         <v>1</v>
@@ -9929,7 +10027,7 @@
     </row>
     <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="B152" s="0" t="n">
         <v>2</v>
@@ -9944,7 +10042,7 @@
     </row>
     <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="B153" s="0" t="n">
         <v>3</v>
@@ -9959,7 +10057,7 @@
     </row>
     <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="B154" s="0" t="n">
         <v>4</v>
@@ -9974,7 +10072,7 @@
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="B155" s="0" t="n">
         <v>5</v>
@@ -9989,7 +10087,7 @@
     </row>
     <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="B156" s="0" t="n">
         <v>6</v>
@@ -10004,7 +10102,7 @@
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="B157" s="0" t="n">
         <v>7</v>
@@ -10019,7 +10117,7 @@
     </row>
     <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="B158" s="0" t="n">
         <v>0</v>
@@ -10034,7 +10132,7 @@
     </row>
     <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="B159" s="0" t="n">
         <v>1</v>
@@ -10049,7 +10147,7 @@
     </row>
     <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="B160" s="0" t="n">
         <v>6</v>
@@ -10064,7 +10162,7 @@
     </row>
     <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="B161" s="0" t="n">
         <v>7</v>
@@ -10079,7 +10177,7 @@
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="B162" s="0" t="n">
         <v>0</v>
@@ -10094,7 +10192,7 @@
     </row>
     <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="B163" s="0" t="n">
         <v>1</v>
@@ -10109,7 +10207,7 @@
     </row>
     <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="B164" s="0" t="n">
         <v>2</v>
@@ -10124,7 +10222,7 @@
     </row>
     <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="B165" s="0" t="n">
         <v>6</v>
@@ -10139,7 +10237,7 @@
     </row>
     <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="B166" s="0" t="n">
         <v>7</v>
@@ -10154,7 +10252,7 @@
     </row>
     <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="B167" s="0" t="n">
         <v>0</v>
@@ -10169,7 +10267,7 @@
     </row>
     <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="B168" s="0" t="n">
         <v>1</v>
@@ -10184,7 +10282,7 @@
     </row>
     <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="B169" s="0" t="n">
         <v>2</v>
@@ -10199,7 +10297,7 @@
     </row>
     <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="B170" s="0" t="n">
         <v>3</v>
@@ -10214,7 +10312,7 @@
     </row>
     <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="B171" s="0" t="n">
         <v>4</v>
@@ -10229,7 +10327,7 @@
     </row>
     <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="B172" s="0" t="n">
         <v>2</v>
@@ -10244,7 +10342,7 @@
     </row>
     <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="B173" s="0" t="n">
         <v>3</v>
@@ -10259,7 +10357,7 @@
     </row>
     <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="B174" s="0" t="n">
         <v>4</v>
@@ -10274,7 +10372,7 @@
     </row>
     <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="B175" s="0" t="n">
         <v>5</v>
@@ -10289,7 +10387,7 @@
     </row>
     <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="B176" s="0" t="n">
         <v>6</v>
@@ -10304,7 +10402,7 @@
     </row>
     <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="B177" s="0" t="n">
         <v>7</v>
@@ -10319,7 +10417,7 @@
     </row>
     <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="B178" s="0" t="n">
         <v>0</v>
@@ -10334,7 +10432,7 @@
     </row>
     <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="B179" s="0" t="n">
         <v>1</v>
@@ -10349,7 +10447,7 @@
     </row>
     <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="B180" s="0" t="n">
         <v>2</v>
@@ -10364,7 +10462,7 @@
     </row>
     <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="B181" s="0" t="n">
         <v>3</v>
@@ -10379,7 +10477,7 @@
     </row>
     <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="B182" s="0" t="n">
         <v>4</v>
@@ -10394,7 +10492,7 @@
     </row>
     <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="0" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="B183" s="0" t="n">
         <v>5</v>
@@ -10409,7 +10507,7 @@
     </row>
     <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="0" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="B184" s="0" t="n">
         <v>6</v>
@@ -10424,7 +10522,7 @@
     </row>
     <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="B185" s="0" t="n">
         <v>7</v>
@@ -10439,7 +10537,7 @@
     </row>
     <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="B186" s="0" t="n">
         <v>0</v>
@@ -10454,7 +10552,7 @@
     </row>
     <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="0" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="B187" s="0" t="n">
         <v>1</v>
@@ -10469,7 +10567,7 @@
     </row>
     <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="0" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="B188" s="0" t="n">
         <v>2</v>
@@ -10484,7 +10582,7 @@
     </row>
     <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="0" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="B189" s="0" t="n">
         <v>3</v>
@@ -10499,7 +10597,7 @@
     </row>
     <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="0" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="B190" s="0" t="n">
         <v>4</v>
@@ -10514,7 +10612,7 @@
     </row>
     <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="0" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="B191" s="0" t="n">
         <v>5</v>
@@ -10529,7 +10627,7 @@
     </row>
     <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="0" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="B192" s="0" t="n">
         <v>6</v>
@@ -10544,7 +10642,7 @@
     </row>
     <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="0" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="B193" s="0" t="n">
         <v>7</v>
@@ -10558,210 +10656,348 @@
       </c>
     </row>
     <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A194" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="B194" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="C194" s="4" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D194" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C194, Levels!B:B, 0), 1, 1)),", ",IF(A194 &lt;&gt; "", """mem"": bit" &amp; B194 &amp; "(" &amp; A194 &amp; "),", ""),"""good"": ",IF(A194 &lt;&gt; "", 1, 0),"},")</f>
-        <v>193: { "levelId": 3, "good": 0},</v>
+        <v>193: { "levelId": 10, "mem": bit0(0x2249a1),"good": 1},</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A195" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="B195" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="C195" s="4" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D195" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C195, Levels!B:B, 0), 1, 1)),", ",IF(A195 &lt;&gt; "", """mem"": bit" &amp; B195 &amp; "(" &amp; A195 &amp; "),", ""),"""good"": ",IF(A195 &lt;&gt; "", 1, 0),"},")</f>
-        <v>194: { "levelId": 3, "good": 0},</v>
+        <v>194: { "levelId": 10, "mem": bit1(0x2249a1),"good": 1},</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A196" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="B196" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="C196" s="4" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D196" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C196, Levels!B:B, 0), 1, 1)),", ",IF(A196 &lt;&gt; "", """mem"": bit" &amp; B196 &amp; "(" &amp; A196 &amp; "),", ""),"""good"": ",IF(A196 &lt;&gt; "", 1, 0),"},")</f>
-        <v>195: { "levelId": 3, "good": 0},</v>
+        <v>195: { "levelId": 10, "mem": bit2(0x2249a1),"good": 1},</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A197" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="B197" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="C197" s="4" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D197" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C197, Levels!B:B, 0), 1, 1)),", ",IF(A197 &lt;&gt; "", """mem"": bit" &amp; B197 &amp; "(" &amp; A197 &amp; "),", ""),"""good"": ",IF(A197 &lt;&gt; "", 1, 0),"},")</f>
-        <v>196: { "levelId": 3, "good": 0},</v>
+        <v>196: { "levelId": 10, "mem": bit3(0x2249a1),"good": 1},</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A198" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="B198" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="C198" s="4" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D198" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C198, Levels!B:B, 0), 1, 1)),", ",IF(A198 &lt;&gt; "", """mem"": bit" &amp; B198 &amp; "(" &amp; A198 &amp; "),", ""),"""good"": ",IF(A198 &lt;&gt; "", 1, 0),"},")</f>
-        <v>197: { "levelId": 3, "good": 0},</v>
+        <v>197: { "levelId": 10, "mem": bit4(0x2249a1),"good": 1},</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A199" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="B199" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="C199" s="4" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D199" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C199, Levels!B:B, 0), 1, 1)),", ",IF(A199 &lt;&gt; "", """mem"": bit" &amp; B199 &amp; "(" &amp; A199 &amp; "),", ""),"""good"": ",IF(A199 &lt;&gt; "", 1, 0),"},")</f>
-        <v>198: { "levelId": 3, "good": 0},</v>
+        <v>198: { "levelId": 10, "mem": bit2(0x2249a2),"good": 1},</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A200" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="B200" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="C200" s="4" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D200" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C200, Levels!B:B, 0), 1, 1)),", ",IF(A200 &lt;&gt; "", """mem"": bit" &amp; B200 &amp; "(" &amp; A200 &amp; "),", ""),"""good"": ",IF(A200 &lt;&gt; "", 1, 0),"},")</f>
-        <v>199: { "levelId": 3, "good": 0},</v>
+        <v>199: { "levelId": 10, "mem": bit3(0x2249a2),"good": 1},</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A201" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="B201" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="C201" s="4" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D201" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C201, Levels!B:B, 0), 1, 1)),", ",IF(A201 &lt;&gt; "", """mem"": bit" &amp; B201 &amp; "(" &amp; A201 &amp; "),", ""),"""good"": ",IF(A201 &lt;&gt; "", 1, 0),"},")</f>
-        <v>200: { "levelId": 3, "good": 0},</v>
+        <v>200: { "levelId": 10, "mem": bit4(0x2249a2),"good": 1},</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A202" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="B202" s="0" t="n">
+        <v>5</v>
+      </c>
       <c r="C202" s="4" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D202" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C202, Levels!B:B, 0), 1, 1)),", ",IF(A202 &lt;&gt; "", """mem"": bit" &amp; B202 &amp; "(" &amp; A202 &amp; "),", ""),"""good"": ",IF(A202 &lt;&gt; "", 1, 0),"},")</f>
-        <v>201: { "levelId": 3, "good": 0},</v>
+        <v>201: { "levelId": 10, "mem": bit5(0x2249a2),"good": 1},</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A203" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="B203" s="0" t="n">
+        <v>6</v>
+      </c>
       <c r="C203" s="4" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D203" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C203, Levels!B:B, 0), 1, 1)),", ",IF(A203 &lt;&gt; "", """mem"": bit" &amp; B203 &amp; "(" &amp; A203 &amp; "),", ""),"""good"": ",IF(A203 &lt;&gt; "", 1, 0),"},")</f>
-        <v>202: { "levelId": 3, "good": 0},</v>
+        <v>202: { "levelId": 10, "mem": bit6(0x2249a2),"good": 1},</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A204" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="B204" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="C204" s="4" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D204" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C204, Levels!B:B, 0), 1, 1)),", ",IF(A204 &lt;&gt; "", """mem"": bit" &amp; B204 &amp; "(" &amp; A204 &amp; "),", ""),"""good"": ",IF(A204 &lt;&gt; "", 1, 0),"},")</f>
-        <v>203: { "levelId": 3, "good": 0},</v>
+        <v>203: { "levelId": 10, "mem": bit1(0x2249a4),"good": 1},</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A205" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="B205" s="0" t="n">
+        <v>5</v>
+      </c>
       <c r="C205" s="4" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D205" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C205, Levels!B:B, 0), 1, 1)),", ",IF(A205 &lt;&gt; "", """mem"": bit" &amp; B205 &amp; "(" &amp; A205 &amp; "),", ""),"""good"": ",IF(A205 &lt;&gt; "", 1, 0),"},")</f>
-        <v>204: { "levelId": 3, "good": 0},</v>
+        <v>204: { "levelId": 10, "mem": bit5(0x2249a3),"good": 1},</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A206" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="B206" s="0" t="n">
+        <v>6</v>
+      </c>
       <c r="C206" s="4" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D206" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C206, Levels!B:B, 0), 1, 1)),", ",IF(A206 &lt;&gt; "", """mem"": bit" &amp; B206 &amp; "(" &amp; A206 &amp; "),", ""),"""good"": ",IF(A206 &lt;&gt; "", 1, 0),"},")</f>
-        <v>205: { "levelId": 3, "good": 0},</v>
+        <v>205: { "levelId": 10, "mem": bit6(0x2249a3),"good": 1},</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A207" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="B207" s="0" t="n">
+        <v>7</v>
+      </c>
       <c r="C207" s="4" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D207" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C207, Levels!B:B, 0), 1, 1)),", ",IF(A207 &lt;&gt; "", """mem"": bit" &amp; B207 &amp; "(" &amp; A207 &amp; "),", ""),"""good"": ",IF(A207 &lt;&gt; "", 1, 0),"},")</f>
-        <v>206: { "levelId": 3, "good": 0},</v>
+        <v>206: { "levelId": 10, "mem": bit7(0x2249a3),"good": 1},</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A208" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="B208" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="C208" s="4" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D208" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C208, Levels!B:B, 0), 1, 1)),", ",IF(A208 &lt;&gt; "", """mem"": bit" &amp; B208 &amp; "(" &amp; A208 &amp; "),", ""),"""good"": ",IF(A208 &lt;&gt; "", 1, 0),"},")</f>
-        <v>207: { "levelId": 3, "good": 0},</v>
+        <v>207: { "levelId": 10, "mem": bit0(0x2249a4),"good": 1},</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A209" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="B209" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="C209" s="4" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D209" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C209, Levels!B:B, 0), 1, 1)),", ",IF(A209 &lt;&gt; "", """mem"": bit" &amp; B209 &amp; "(" &amp; A209 &amp; "),", ""),"""good"": ",IF(A209 &lt;&gt; "", 1, 0),"},")</f>
-        <v>208: { "levelId": 3, "good": 0},</v>
+        <v>208: { "levelId": 10, "mem": bit3(0x2249a4),"good": 1},</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A210" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="B210" s="0" t="n">
+        <v>5</v>
+      </c>
       <c r="C210" s="4" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D210" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C210, Levels!B:B, 0), 1, 1)),", ",IF(A210 &lt;&gt; "", """mem"": bit" &amp; B210 &amp; "(" &amp; A210 &amp; "),", ""),"""good"": ",IF(A210 &lt;&gt; "", 1, 0),"},")</f>
-        <v>209: { "levelId": 3, "good": 0},</v>
+        <v>209: { "levelId": 10, "mem": bit5(0x2249a4),"good": 1},</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A211" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="B211" s="0" t="n">
+        <v>6</v>
+      </c>
       <c r="C211" s="4" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D211" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C211, Levels!B:B, 0), 1, 1)),", ",IF(A211 &lt;&gt; "", """mem"": bit" &amp; B211 &amp; "(" &amp; A211 &amp; "),", ""),"""good"": ",IF(A211 &lt;&gt; "", 1, 0),"},")</f>
-        <v>210: { "levelId": 3, "good": 0},</v>
+        <v>210: { "levelId": 10, "mem": bit6(0x2249a4),"good": 1},</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A212" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="B212" s="0" t="n">
+        <v>7</v>
+      </c>
       <c r="C212" s="4" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D212" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C212, Levels!B:B, 0), 1, 1)),", ",IF(A212 &lt;&gt; "", """mem"": bit" &amp; B212 &amp; "(" &amp; A212 &amp; "),", ""),"""good"": ",IF(A212 &lt;&gt; "", 1, 0),"},")</f>
-        <v>211: { "levelId": 3, "good": 0},</v>
+        <v>211: { "levelId": 10, "mem": bit7(0x2249a4),"good": 1},</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A213" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="B213" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="C213" s="4" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D213" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C213, Levels!B:B, 0), 1, 1)),", ",IF(A213 &lt;&gt; "", """mem"": bit" &amp; B213 &amp; "(" &amp; A213 &amp; "),", ""),"""good"": ",IF(A213 &lt;&gt; "", 1, 0),"},")</f>
-        <v>212: { "levelId": 3, "good": 0},</v>
+        <v>212: { "levelId": 10, "mem": bit0(0x2249a5),"good": 1},</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A214" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="B214" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="C214" s="4" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D214" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C214, Levels!B:B, 0), 1, 1)),", ",IF(A214 &lt;&gt; "", """mem"": bit" &amp; B214 &amp; "(" &amp; A214 &amp; "),", ""),"""good"": ",IF(A214 &lt;&gt; "", 1, 0),"},")</f>
-        <v>213: { "levelId": 3, "good": 0},</v>
+        <v>213: { "levelId": 10, "mem": bit1(0x2249a5),"good": 1},</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A215" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="B215" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="C215" s="4" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D215" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C215, Levels!B:B, 0), 1, 1)),", ",IF(A215 &lt;&gt; "", """mem"": bit" &amp; B215 &amp; "(" &amp; A215 &amp; "),", ""),"""good"": ",IF(A215 &lt;&gt; "", 1, 0),"},")</f>
-        <v>214: { "levelId": 3, "good": 0},</v>
+        <v>214: { "levelId": 10, "mem": bit2(0x2249a5),"good": 1},</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A216" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="B216" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="C216" s="4" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D216" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C216, Levels!B:B, 0), 1, 1)),", ",IF(A216 &lt;&gt; "", """mem"": bit" &amp; B216 &amp; "(" &amp; A216 &amp; "),", ""),"""good"": ",IF(A216 &lt;&gt; "", 1, 0),"},")</f>
-        <v>215: { "levelId": 3, "good": 0},</v>
+        <v>215: { "levelId": 10, "mem": bit4(0x2249a4),"good": 1},</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17859,7 +18095,7 @@
       <selection pane="bottomLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.93"/>
@@ -17869,13 +18105,13 @@
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>4</v>
@@ -17886,7 +18122,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>7</v>
@@ -17900,12 +18136,12 @@
       </c>
       <c r="G2" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D2:D81)</f>
-        <v>1: { "levelId": 1, "mem": bit7(0x2249f0),"good": 1},2: { "levelId": 2, "mem": bit0(0x2249f1),"good": 1},3: { "levelId": 2, "mem": bit1(0x2249f1),"good": 1},4: { "levelId": 2, "mem": bit5(0x2249f1),"good": 1},5: { "levelId": 2, "mem": bit6(0x2249f1),"good": 1},6: { "levelId": 1, "mem": bit7(0x2249f1),"good": 1},7: { "levelId": 5, "mem": bit0(0x2249f2),"good": 1},8: { "levelId": 5, "mem": bit1(0x2249f2),"good": 1},9: { "levelId": 5, "mem": bit2(0x2249f2),"good": 1},10: { "levelId": 5, "mem": bit3(0x2249f2),"good": 1},11: { "levelId": 5, "mem": bit4(0x2249f2),"good": 1},12: { "levelId": 6, "mem": bit5(0x2249f2),"good": 1},13: { "levelId": 6, "mem": bit7(0x2249f2),"good": 1},14: { "levelId": 6, "mem": bit1(0x2249f3),"good": 1},15: { "levelId": 6, "mem": bit6(0x2249f2),"good": 1},16: { "levelId": 6, "mem": bit0(0x2249f3),"good": 1},17: { "levelId": 6, "mem": bit3(0x2249f3),"good": 1},18: { "levelId": 6, "mem": bit2(0x2249f3),"good": 1},19: { "levelId": 8, "mem": bit5(0x2249f3),"good": 1},20: { "levelId": 8, "mem": bit4(0x2249f3),"good": 1},21: { "levelId": 3, "good": 0},22: { "levelId": 3, "good": 0},23: { "levelId": 3, "good": 0},24: { "levelId": 3, "good": 0},25: { "levelId": 3, "good": 0},26: { "levelId": 3, "good": 0},27: { "levelId": 3, "good": 0},28: { "levelId": 3, "good": 0},29: { "levelId": 3, "good": 0},30: { "levelId": 3, "good": 0},31: { "levelId": 3, "good": 0},32: { "levelId": 3, "good": 0},33: { "levelId": 3, "good": 0},34: { "levelId": 3, "good": 0},35: { "levelId": 3, "good": 0},36: { "levelId": 3, "good": 0},37: { "levelId": 3, "good": 0},38: { "levelId": 3, "good": 0},39: { "levelId": 3, "good": 0},40: { "levelId": 3, "good": 0},41: { "levelId": 3, "good": 0},42: { "levelId": 3, "good": 0},43: { "levelId": 3, "good": 0},44: { "levelId": 3, "good": 0},45: { "levelId": 3, "good": 0},46: { "levelId": 3, "good": 0},47: { "levelId": 3, "good": 0},48: { "levelId": 3, "good": 0},49: { "levelId": 3, "good": 0},50: { "levelId": 3, "good": 0},51: { "levelId": 3, "good": 0},52: { "levelId": 3, "good": 0},53: { "levelId": 3, "good": 0},54: { "levelId": 3, "good": 0},55: { "levelId": 3, "good": 0},56: { "levelId": 3, "good": 0},57: { "levelId": 3, "good": 0},58: { "levelId": 3, "good": 0},59: { "levelId": 3, "good": 0},60: { "levelId": 3, "good": 0},61: { "levelId": 3, "good": 0},62: { "levelId": 3, "good": 0},63: { "levelId": 3, "good": 0},64: { "levelId": 3, "good": 0},65: { "levelId": 3, "good": 0},66: { "levelId": 3, "good": 0},67: { "levelId": 3, "good": 0},68: { "levelId": 3, "good": 0},69: { "levelId": 3, "good": 0},70: { "levelId": 3, "good": 0},71: { "levelId": 3, "good": 0},72: { "levelId": 3, "good": 0},73: { "levelId": 3, "good": 0},74: { "levelId": 3, "good": 0},75: { "levelId": 3, "good": 0},76: { "levelId": 3, "good": 0},77: { "levelId": 3, "good": 0},78: { "levelId": 3, "good": 0},79: { "levelId": 3, "good": 0},80: { "levelId": 3, "good": 0},</v>
+        <v>1: { "levelId": 1, "mem": bit7(0x2249f0),"good": 1},2: { "levelId": 2, "mem": bit0(0x2249f1),"good": 1},3: { "levelId": 2, "mem": bit1(0x2249f1),"good": 1},4: { "levelId": 2, "mem": bit5(0x2249f1),"good": 1},5: { "levelId": 2, "mem": bit6(0x2249f1),"good": 1},6: { "levelId": 1, "mem": bit7(0x2249f1),"good": 1},7: { "levelId": 5, "mem": bit0(0x2249f2),"good": 1},8: { "levelId": 5, "mem": bit1(0x2249f2),"good": 1},9: { "levelId": 5, "mem": bit2(0x2249f2),"good": 1},10: { "levelId": 5, "mem": bit3(0x2249f2),"good": 1},11: { "levelId": 5, "mem": bit4(0x2249f2),"good": 1},12: { "levelId": 6, "mem": bit5(0x2249f2),"good": 1},13: { "levelId": 6, "mem": bit7(0x2249f2),"good": 1},14: { "levelId": 6, "mem": bit1(0x2249f3),"good": 1},15: { "levelId": 6, "mem": bit6(0x2249f2),"good": 1},16: { "levelId": 6, "mem": bit0(0x2249f3),"good": 1},17: { "levelId": 6, "mem": bit3(0x2249f3),"good": 1},18: { "levelId": 6, "mem": bit2(0x2249f3),"good": 1},19: { "levelId": 8, "mem": bit5(0x2249f3),"good": 1},20: { "levelId": 8, "mem": bit4(0x2249f3),"good": 1},21: { "levelId": 10, "mem": bit0(0x2249f4),"good": 1},22: { "levelId": 10, "mem": bit6(0x2249f3),"good": 1},23: { "levelId": 3, "good": 0},24: { "levelId": 3, "good": 0},25: { "levelId": 3, "good": 0},26: { "levelId": 3, "good": 0},27: { "levelId": 3, "good": 0},28: { "levelId": 3, "good": 0},29: { "levelId": 3, "good": 0},30: { "levelId": 3, "good": 0},31: { "levelId": 3, "good": 0},32: { "levelId": 3, "good": 0},33: { "levelId": 3, "good": 0},34: { "levelId": 3, "good": 0},35: { "levelId": 3, "good": 0},36: { "levelId": 3, "good": 0},37: { "levelId": 3, "good": 0},38: { "levelId": 3, "good": 0},39: { "levelId": 3, "good": 0},40: { "levelId": 3, "good": 0},41: { "levelId": 3, "good": 0},42: { "levelId": 3, "good": 0},43: { "levelId": 3, "good": 0},44: { "levelId": 3, "good": 0},45: { "levelId": 3, "good": 0},46: { "levelId": 3, "good": 0},47: { "levelId": 3, "good": 0},48: { "levelId": 3, "good": 0},49: { "levelId": 3, "good": 0},50: { "levelId": 3, "good": 0},51: { "levelId": 3, "good": 0},52: { "levelId": 3, "good": 0},53: { "levelId": 3, "good": 0},54: { "levelId": 3, "good": 0},55: { "levelId": 3, "good": 0},56: { "levelId": 3, "good": 0},57: { "levelId": 3, "good": 0},58: { "levelId": 3, "good": 0},59: { "levelId": 3, "good": 0},60: { "levelId": 3, "good": 0},61: { "levelId": 3, "good": 0},62: { "levelId": 3, "good": 0},63: { "levelId": 3, "good": 0},64: { "levelId": 3, "good": 0},65: { "levelId": 3, "good": 0},66: { "levelId": 3, "good": 0},67: { "levelId": 3, "good": 0},68: { "levelId": 3, "good": 0},69: { "levelId": 3, "good": 0},70: { "levelId": 3, "good": 0},71: { "levelId": 3, "good": 0},72: { "levelId": 3, "good": 0},73: { "levelId": 3, "good": 0},74: { "levelId": 3, "good": 0},75: { "levelId": 3, "good": 0},76: { "levelId": 3, "good": 0},77: { "levelId": 3, "good": 0},78: { "levelId": 3, "good": 0},79: { "levelId": 3, "good": 0},80: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>97</v>
+        <v>111</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0</v>
@@ -17920,7 +18156,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>97</v>
+        <v>111</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>1</v>
@@ -17935,7 +18171,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>97</v>
+        <v>111</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>5</v>
@@ -17950,7 +18186,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>97</v>
+        <v>111</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>6</v>
@@ -17965,7 +18201,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>97</v>
+        <v>111</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>7</v>
@@ -17980,7 +18216,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>0</v>
@@ -17995,7 +18231,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>1</v>
@@ -18010,7 +18246,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>2</v>
@@ -18025,7 +18261,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>3</v>
@@ -18040,7 +18276,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>4</v>
@@ -18055,7 +18291,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>5</v>
@@ -18070,7 +18306,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>7</v>
@@ -18085,7 +18321,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>1</v>
@@ -18100,7 +18336,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>6</v>
@@ -18115,7 +18351,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>0</v>
@@ -18130,7 +18366,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>3</v>
@@ -18145,7 +18381,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>2</v>
@@ -18160,7 +18396,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>5</v>
@@ -18175,7 +18411,7 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>4</v>
@@ -18189,21 +18425,33 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="C22" s="4" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D22" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C22, Levels!B:B, 0), 1, 1)),", ",IF(A22 &lt;&gt; "", """mem"": bit" &amp; B22 &amp; "(" &amp; A22 &amp; "),", ""),"""good"": ",IF(A22 &lt;&gt; "", 1, 0),"},")</f>
-        <v>21: { "levelId": 3, "good": 0},</v>
+        <v>21: { "levelId": 10, "mem": bit0(0x2249f4),"good": 1},</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>6</v>
+      </c>
       <c r="C23" s="4" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D23" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C23, Levels!B:B, 0), 1, 1)),", ",IF(A23 &lt;&gt; "", """mem"": bit" &amp; B23 &amp; "(" &amp; A23 &amp; "),", ""),"""good"": ",IF(A23 &lt;&gt; "", 1, 0),"},")</f>
-        <v>22: { "levelId": 3, "good": 0},</v>
+        <v>22: { "levelId": 10, "mem": bit6(0x2249f3),"good": 1},</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Finished optimizing lum achievements, added a new achievement for the CoBD, and fixed the bad ending achievement
</commit_message>
<xml_diff>
--- a/Rayman 2.xlsx
+++ b/Rayman 2.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1438" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1501" uniqueCount="130">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -235,6 +235,30 @@
     <t xml:space="preserve">MenhirArea2</t>
   </si>
   <si>
+    <t xml:space="preserve">788950</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MenhirArea3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">78402C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BadDreamsArea1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">in the Cave of Bad Dreams</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cave of Bad Dreams</t>
+  </si>
+  <si>
+    <t xml:space="preserve">788148</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BadDreamsArea2</t>
+  </si>
+  <si>
     <t xml:space="preserve">Index</t>
   </si>
   <si>
@@ -350,6 +374,27 @@
   </si>
   <si>
     <t xml:space="preserve">0x2249a5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x2249e5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x2249e6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x2249e7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x2249e8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x2249e9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x2249ea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x2249eb</t>
   </si>
   <si>
     <t xml:space="preserve">Level ID</t>
@@ -581,7 +626,7 @@
       <selection pane="bottomLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.66"/>
@@ -611,7 +656,7 @@
       </c>
       <c r="H1" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(E2:E1000)</f>
-        <v>0x784BFC: { "id": 0x784BFC, "areaName": "Menu", "displayName": "Main Menu", "levelName": "Menu" },0x789668: { "id": 0x789668, "areaName": "Intro", "displayName": "somewhere in the Glade of Dreams…", "levelName": "None" },0x778C74: { "id": 0x778C74, "areaName": "BuccaneerBrig", "displayName": "in the Buccaneer’s brig", "levelName": "None" },0x78D424: { "id": 0x78D424, "areaName": "WoodsOfLight", "displayName": "in the Woods of Light", "levelName": "Woods of Light" },0x790570: { "id": 0x790570, "areaName": "HallOfDoors", "displayName": "in the Hall of Doors", "levelName": "Hall of Doors" },0x7875A8: { "id": 0x7875A8, "areaName": "FairyGladeArea1", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x78A320: { "id": 0x78A320, "areaName": "FairyGladeArea2", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x7A1BD8: { "id": 0x7A1BD8, "areaName": "FairyGladeArea3", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x77BFFC: { "id": 0x77BFFC, "areaName": "FairyGladeArea4", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x771B74: { "id": 0x771B74, "areaName": "FairyGladeArea5", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x74AAA8: { "id": 0x74AAA8, "areaName": "Results", "displayName": "viewing level results…", "levelName": "None" },0x788708: { "id": 0x788708, "areaName": "MarshesArea1", "displayName": "in the Marshes of Awakening", "levelName": "Marshes of Awakening" },0x7786E8: { "id": 0x7786E8, "areaName": "MarshesArea2", "displayName": "in the Marshes of Awakening", "levelName": "Marshes of Awakening" },0x790598: { "id": 0x790598, "areaName": "BayouArea1", "displayName": "in the Bayou", "levelName": "Bayou" },0x788764: { "id": 0x788764, "areaName": "BayouArea2", "displayName": "in the Bayou", "levelName": "Bayou" },0x7928A4: { "id": 0x7928A4, "areaName": "SoWaIArea1", "displayName": "in the Sanctuary of Water and Ice", "levelName": "Sanctuary of Water and Ice" },0x774694: { "id": 0x774694, "areaName": "SoWaIArea2", "displayName": "in the Sanctuary of Water and Ice", "levelName": "Sanctuary of Water and Ice" },0x76F100: { "id": 0x76F100, "areaName": "Polokus", "displayName": "in Polokus’s dream", "levelName": "Polokus" },0x0: { "id": 0x0, "areaName": "None", "displayName": "somewhere in the Glade of Dreams…", "levelName": "None" },0x751974: { "id": 0x751974, "areaName": "Bonus", "displayName": "in the bonus stage", "levelName": "None" },0x776C08: { "id": 0x776C08, "areaName": "MenhirArea1", "displayName": "in the Menhir Hills", "levelName": "Menhir Hills" },0x78FBD8: { "id": 0x78FBD8, "areaName": "MenhirArea2", "displayName": "in the Menhir Hills", "levelName": "Menhir Hills" },</v>
+        <v>0x784BFC: { "id": 0x784BFC, "areaName": "Menu", "displayName": "Main Menu", "levelName": "Menu" },0x789668: { "id": 0x789668, "areaName": "Intro", "displayName": "somewhere in the Glade of Dreams…", "levelName": "None" },0x778C74: { "id": 0x778C74, "areaName": "BuccaneerBrig", "displayName": "in the Buccaneer’s brig", "levelName": "None" },0x78D424: { "id": 0x78D424, "areaName": "WoodsOfLight", "displayName": "in the Woods of Light", "levelName": "Woods of Light" },0x790570: { "id": 0x790570, "areaName": "HallOfDoors", "displayName": "in the Hall of Doors", "levelName": "Hall of Doors" },0x7875A8: { "id": 0x7875A8, "areaName": "FairyGladeArea1", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x78A320: { "id": 0x78A320, "areaName": "FairyGladeArea2", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x7A1BD8: { "id": 0x7A1BD8, "areaName": "FairyGladeArea3", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x77BFFC: { "id": 0x77BFFC, "areaName": "FairyGladeArea4", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x771B74: { "id": 0x771B74, "areaName": "FairyGladeArea5", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x74AAA8: { "id": 0x74AAA8, "areaName": "Results", "displayName": "viewing level results…", "levelName": "None" },0x788708: { "id": 0x788708, "areaName": "MarshesArea1", "displayName": "in the Marshes of Awakening", "levelName": "Marshes of Awakening" },0x7786E8: { "id": 0x7786E8, "areaName": "MarshesArea2", "displayName": "in the Marshes of Awakening", "levelName": "Marshes of Awakening" },0x790598: { "id": 0x790598, "areaName": "BayouArea1", "displayName": "in the Bayou", "levelName": "Bayou" },0x788764: { "id": 0x788764, "areaName": "BayouArea2", "displayName": "in the Bayou", "levelName": "Bayou" },0x7928A4: { "id": 0x7928A4, "areaName": "SoWaIArea1", "displayName": "in the Sanctuary of Water and Ice", "levelName": "Sanctuary of Water and Ice" },0x774694: { "id": 0x774694, "areaName": "SoWaIArea2", "displayName": "in the Sanctuary of Water and Ice", "levelName": "Sanctuary of Water and Ice" },0x76F100: { "id": 0x76F100, "areaName": "Polokus", "displayName": "in Polokus’s dream", "levelName": "Polokus" },0x0: { "id": 0x0, "areaName": "None", "displayName": "somewhere in the Glade of Dreams…", "levelName": "None" },0x751974: { "id": 0x751974, "areaName": "Bonus", "displayName": "in the bonus stage", "levelName": "None" },0x776C08: { "id": 0x776C08, "areaName": "MenhirArea1", "displayName": "in the Menhir Hills", "levelName": "Menhir Hills" },0x78FBD8: { "id": 0x78FBD8, "areaName": "MenhirArea2", "displayName": "in the Menhir Hills", "levelName": "Menhir Hills" },0x788950: { "id": 0x788950, "areaName": "MenhirArea3", "displayName": "in the Menhir Hills", "levelName": "Menhir Hills" },0x78402C: { "id": 0x78402C, "areaName": "BadDreamsArea1", "displayName": "in the Cave of Bad Dreams", "levelName": "Cave of Bad Dreams" },0x788148: { "id": 0x788148, "areaName": "BadDreamsArea2", "displayName": "in the Cave of Bad Dreams", "levelName": "Cave of Bad Dreams" },</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1011,13 +1056,58 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D24" s="4"/>
+      <c r="A24" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E24" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("0x", A24,": { ""id"": ","0x", A24,", ""areaName"": """,B24,""", ""displayName"": """,C24,""", ""levelName"": """,D24,""" },")</f>
+        <v>0x788950: { "id": 0x788950, "areaName": "MenhirArea3", "displayName": "in the Menhir Hills", "levelName": "Menhir Hills" },</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D25" s="4"/>
+      <c r="A25" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E25" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("0x", A25,": { ""id"": ","0x", A25,", ""areaName"": """,B25,""", ""displayName"": """,C25,""", ""levelName"": """,D25,""" },")</f>
+        <v>0x78402C: { "id": 0x78402C, "areaName": "BadDreamsArea1", "displayName": "in the Cave of Bad Dreams", "levelName": "Cave of Bad Dreams" },</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D26" s="4"/>
+      <c r="A26" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E26" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("0x", A26,": { ""id"": ","0x", A26,", ""areaName"": """,B26,""", ""displayName"": """,C26,""", ""levelName"": """,D26,""" },")</f>
+        <v>0x788148: { "id": 0x788148, "areaName": "BadDreamsArea2", "displayName": "in the Cave of Bad Dreams", "levelName": "Cave of Bad Dreams" },</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D27" s="4"/>
@@ -4013,10 +4103,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
+      <selection pane="bottomLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.21"/>
@@ -4028,22 +4118,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>4</v>
@@ -4119,7 +4209,7 @@
       </c>
       <c r="E4" s="0" t="n">
         <f aca="false">COUNTIFS(Lums!C3:C1002, "=" &amp; B4)</f>
-        <v>785</v>
+        <v>735</v>
       </c>
       <c r="F4" s="0" t="n">
         <f aca="false">COUNTIFS(Cages!C3:C83, "=" &amp; B4)</f>
@@ -4324,18 +4414,26 @@
         <f aca="false">ROW()-1</f>
         <v>11</v>
       </c>
-      <c r="B12" s="4"/>
+      <c r="B12" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="E12" s="0" t="n">
         <f aca="false">COUNTIFS(Lums!C11:C1010, "=" &amp; B12)</f>
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="F12" s="0" t="n">
         <f aca="false">COUNTIFS(Cages!C11:C91, "=" &amp; B12)</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G12" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A12,": { ""id"": ",A12,", ""name"": """,B12,""", ""lums"": ",C12,", ""cages"": ",D12," },")</f>
-        <v>11: { "id": 11, "name": "", "lums": , "cages":  },</v>
+        <v>11: { "id": 11, "name": "Cave of Bad Dreams", "lums": 50, "cages": 0 },</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7735,12 +7833,12 @@
   <dimension ref="A1:H1001"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A243" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="bottomLeft" activeCell="C267" activeCellId="0" sqref="C267"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.93"/>
@@ -7749,10 +7847,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>3</v>
@@ -7765,12 +7863,12 @@
       </c>
       <c r="H1" s="5" t="str">
         <f aca="false">_xlfn.CONCAT(D2:D1001)</f>
-        <v>1: { "levelId": 2, "mem": bit0(0x224988),"good": 1, "addr": 0x224988, "bit": 0},2: { "levelId": 2, "mem": bit1(0x224988),"good": 1, "addr": 0x224988, "bit": 1},3: { "levelId": 2, "mem": bit2(0x224988),"good": 1, "addr": 0x224988, "bit": 2},4: { "levelId": 2, "mem": bit3(0x224988),"good": 1, "addr": 0x224988, "bit": 3},5: { "levelId": 2, "mem": bit4(0x224988),"good": 1, "addr": 0x224988, "bit": 4},6: { "levelId": 2, "mem": bit5(0x224988),"good": 1, "addr": 0x224988, "bit": 5},7: { "levelId": 2, "mem": bit6(0x224988),"good": 1, "addr": 0x224988, "bit": 6},8: { "levelId": 2, "mem": bit7(0x224988),"good": 1, "addr": 0x224988, "bit": 7},9: { "levelId": 2, "mem": bit2(0x224989),"good": 1, "addr": 0x224989, "bit": 2},10: { "levelId": 2, "mem": bit1(0x22498a),"good": 1, "addr": 0x22498a, "bit": 1},11: { "levelId": 2, "mem": bit2(0x22498a),"good": 1, "addr": 0x22498a, "bit": 2},12: { "levelId": 2, "mem": bit3(0x22498a),"good": 1, "addr": 0x22498a, "bit": 3},13: { "levelId": 2, "mem": bit4(0x22498a),"good": 1, "addr": 0x22498a, "bit": 4},14: { "levelId": 2, "mem": bit5(0x22498a),"good": 1, "addr": 0x22498a, "bit": 5},15: { "levelId": 2, "mem": bit6(0x22498a),"good": 1, "addr": 0x22498a, "bit": 6},16: { "levelId": 2, "mem": bit7(0x22498a),"good": 1, "addr": 0x22498a, "bit": 7},17: { "levelId": 2, "mem": bit5(0x22498b),"good": 1, "addr": 0x22498b, "bit": 5},18: { "levelId": 2, "mem": bit6(0x22498b),"good": 1, "addr": 0x22498b, "bit": 6},19: { "levelId": 2, "mem": bit7(0x22498b),"good": 1, "addr": 0x22498b, "bit": 7},20: { "levelId": 2, "mem": bit0(0x22498c),"good": 1, "addr": 0x22498c, "bit": 0},21: { "levelId": 2, "mem": bit1(0x22498c),"good": 1, "addr": 0x22498c, "bit": 1},22: { "levelId": 2, "mem": bit2(0x22498c),"good": 1, "addr": 0x22498c, "bit": 2},23: { "levelId": 2, "mem": bit3(0x22498c),"good": 1, "addr": 0x22498c, "bit": 3},24: { "levelId": 2, "mem": bit4(0x22498c),"good": 1, "addr": 0x22498c, "bit": 4},25: { "levelId": 2, "mem": bit5(0x22498c),"good": 1, "addr": 0x22498c, "bit": 5},26: { "levelId": 2, "mem": bit6(0x22498c),"good": 1, "addr": 0x22498c, "bit": 6},27: { "levelId": 2, "mem": bit7(0x22498c),"good": 1, "addr": 0x22498c, "bit": 7},28: { "levelId": 2, "mem": bit0(0x22498d),"good": 1, "addr": 0x22498d, "bit": 0},29: { "levelId": 2, "mem": bit1(0x22498d),"good": 1, "addr": 0x22498d, "bit": 1},30: { "levelId": 2, "mem": bit2(0x22498d),"good": 1, "addr": 0x22498d, "bit": 2},31: { "levelId": 2, "mem": bit3(0x22498d),"good": 1, "addr": 0x22498d, "bit": 3},32: { "levelId": 2, "mem": bit4(0x22498d),"good": 1, "addr": 0x22498d, "bit": 4},33: { "levelId": 2, "mem": bit5(0x22498d),"good": 1, "addr": 0x22498d, "bit": 5},34: { "levelId": 2, "mem": bit6(0x22498d),"good": 1, "addr": 0x22498d, "bit": 6},35: { "levelId": 2, "mem": bit7(0x22498d),"good": 1, "addr": 0x22498d, "bit": 7},36: { "levelId": 2, "mem": bit0(0x22498e),"good": 1, "addr": 0x22498e, "bit": 0},37: { "levelId": 2, "mem": bit1(0x22498e),"good": 1, "addr": 0x22498e, "bit": 1},38: { "levelId": 5, "mem": bit2(0x22498e),"good": 1, "addr": 0x22498e, "bit": 2},39: { "levelId": 5, "mem": bit3(0x22498e),"good": 1, "addr": 0x22498e, "bit": 3},40: { "levelId": 5, "mem": bit4(0x22498e),"good": 1, "addr": 0x22498e, "bit": 4},41: { "levelId": 5, "mem": bit5(0x22498e),"good": 1, "addr": 0x22498e, "bit": 5},42: { "levelId": 5, "mem": bit6(0x22498e),"good": 1, "addr": 0x22498e, "bit": 6},43: { "levelId": 5, "mem": bit7(0x22498e),"good": 1, "addr": 0x22498e, "bit": 7},44: { "levelId": 5, "mem": bit0(0x22498f),"good": 1, "addr": 0x22498f, "bit": 0},45: { "levelId": 5, "mem": bit1(0x22498f),"good": 1, "addr": 0x22498f, "bit": 1},46: { "levelId": 5, "mem": bit2(0x22498f),"good": 1, "addr": 0x22498f, "bit": 2},47: { "levelId": 5, "mem": bit3(0x22498f),"good": 1, "addr": 0x22498f, "bit": 3},48: { "levelId": 5, "mem": bit4(0x22498f),"good": 1, "addr": 0x22498f, "bit": 4},49: { "levelId": 5, "mem": bit5(0x22498f),"good": 1, "addr": 0x22498f, "bit": 5},50: { "levelId": 5, "mem": bit6(0x22498f),"good": 1, "addr": 0x22498f, "bit": 6},51: { "levelId": 5, "mem": bit7(0x22498f),"good": 1, "addr": 0x22498f, "bit": 7},52: { "levelId": 5, "mem": bit0(0x224990),"good": 1, "addr": 0x224990, "bit": 0},53: { "levelId": 5, "mem": bit1(0x224990),"good": 1, "addr": 0x224990, "bit": 1},54: { "levelId": 5, "mem": bit2(0x224990),"good": 1, "addr": 0x224990, "bit": 2},55: { "levelId": 5, "mem": bit3(0x224990),"good": 1, "addr": 0x224990, "bit": 3},56: { "levelId": 5, "mem": bit4(0x224990),"good": 1, "addr": 0x224990, "bit": 4},57: { "levelId": 5, "mem": bit5(0x224990),"good": 1, "addr": 0x224990, "bit": 5},58: { "levelId": 5, "mem": bit6(0x224990),"good": 1, "addr": 0x224990, "bit": 6},59: { "levelId": 5, "mem": bit7(0x224990),"good": 1, "addr": 0x224990, "bit": 7},60: { "levelId": 5, "mem": bit0(0x224991),"good": 1, "addr": 0x224991, "bit": 0},61: { "levelId": 5, "mem": bit1(0x224991),"good": 1, "addr": 0x224991, "bit": 1},62: { "levelId": 5, "mem": bit2(0x224991),"good": 1, "addr": 0x224991, "bit": 2},63: { "levelId": 5, "mem": bit3(0x224991),"good": 1, "addr": 0x224991, "bit": 3},64: { "levelId": 5, "mem": bit4(0x224991),"good": 1, "addr": 0x224991, "bit": 4},65: { "levelId": 5, "mem": bit5(0x224991),"good": 1, "addr": 0x224991, "bit": 5},66: { "levelId": 5, "mem": bit6(0x224991),"good": 1, "addr": 0x224991, "bit": 6},67: { "levelId": 5, "mem": bit7(0x224991),"good": 1, "addr": 0x224991, "bit": 7},68: { "levelId": 5, "mem": bit0(0x224992),"good": 1, "addr": 0x224992, "bit": 0},69: { "levelId": 5, "mem": bit1(0x224992),"good": 1, "addr": 0x224992, "bit": 1},70: { "levelId": 5, "mem": bit2(0x224992),"good": 1, "addr": 0x224992, "bit": 2},71: { "levelId": 5, "mem": bit3(0x224992),"good": 1, "addr": 0x224992, "bit": 3},72: { "levelId": 5, "mem": bit4(0x224992),"good": 1, "addr": 0x224992, "bit": 4},73: { "levelId": 5, "mem": bit5(0x224992),"good": 1, "addr": 0x224992, "bit": 5},74: { "levelId": 5, "mem": bit6(0x224992),"good": 1, "addr": 0x224992, "bit": 6},75: { "levelId": 5, "mem": bit7(0x224992),"good": 1, "addr": 0x224992, "bit": 7},76: { "levelId": 5, "mem": bit0(0x224993),"good": 1, "addr": 0x224993, "bit": 0},77: { "levelId": 5, "mem": bit1(0x224993),"good": 1, "addr": 0x224993, "bit": 1},78: { "levelId": 5, "mem": bit2(0x224993),"good": 1, "addr": 0x224993, "bit": 2},79: { "levelId": 5, "mem": bit3(0x224993),"good": 1, "addr": 0x224993, "bit": 3},80: { "levelId": 5, "mem": bit4(0x224993),"good": 1, "addr": 0x224993, "bit": 4},81: { "levelId": 5, "mem": bit5(0x224993),"good": 1, "addr": 0x224993, "bit": 5},82: { "levelId": 5, "mem": bit6(0x224993),"good": 1, "addr": 0x224993, "bit": 6},83: { "levelId": 5, "mem": bit7(0x224993),"good": 1, "addr": 0x224993, "bit": 7},84: { "levelId": 5, "mem": bit0(0x224994),"good": 1, "addr": 0x224994, "bit": 0},85: { "levelId": 5, "mem": bit1(0x224994),"good": 1, "addr": 0x224994, "bit": 1},86: { "levelId": 5, "mem": bit2(0x224994),"good": 1, "addr": 0x224994, "bit": 2},87: { "levelId": 5, "mem": bit3(0x224994),"good": 1, "addr": 0x224994, "bit": 3},88: { "levelId": 6, "mem": bit4(0x224994),"good": 1, "addr": 0x224994, "bit": 4},89: { "levelId": 6, "mem": bit5(0x224994),"good": 1, "addr": 0x224994, "bit": 5},90: { "levelId": 6, "mem": bit6(0x224994),"good": 1, "addr": 0x224994, "bit": 6},91: { "levelId": 6, "mem": bit7(0x224994),"good": 1, "addr": 0x224994, "bit": 7},92: { "levelId": 6, "mem": bit0(0x224995),"good": 1, "addr": 0x224995, "bit": 0},93: { "levelId": 6, "mem": bit1(0x224995),"good": 1, "addr": 0x224995, "bit": 1},94: { "levelId": 6, "mem": bit2(0x224995),"good": 1, "addr": 0x224995, "bit": 2},95: { "levelId": 6, "mem": bit3(0x224995),"good": 1, "addr": 0x224995, "bit": 3},96: { "levelId": 6, "mem": bit4(0x224995),"good": 1, "addr": 0x224995, "bit": 4},97: { "levelId": 6, "mem": bit5(0x224995),"good": 1, "addr": 0x224995, "bit": 5},98: { "levelId": 6, "mem": bit6(0x224995),"good": 1, "addr": 0x224995, "bit": 6},99: { "levelId": 6, "mem": bit7(0x224995),"good": 1, "addr": 0x224995, "bit": 7},100: { "levelId": 6, "mem": bit0(0x224996),"good": 1, "addr": 0x224996, "bit": 0},101: { "levelId": 6, "mem": bit1(0x224996),"good": 1, "addr": 0x224996, "bit": 1},102: { "levelId": 6, "mem": bit2(0x224996),"good": 1, "addr": 0x224996, "bit": 2},103: { "levelId": 6, "mem": bit3(0x224996),"good": 1, "addr": 0x224996, "bit": 3},104: { "levelId": 6, "mem": bit4(0x224996),"good": 1, "addr": 0x224996, "bit": 4},105: { "levelId": 6, "mem": bit5(0x224996),"good": 1, "addr": 0x224996, "bit": 5},106: { "levelId": 6, "mem": bit6(0x224996),"good": 1, "addr": 0x224996, "bit": 6},107: { "levelId": 6, "mem": bit7(0x224996),"good": 1, "addr": 0x224996, "bit": 7},108: { "levelId": 6, "mem": bit0(0x224997),"good": 1, "addr": 0x224997, "bit": 0},109: { "levelId": 6, "mem": bit1(0x224997),"good": 1, "addr": 0x224997, "bit": 1},110: { "levelId": 6, "mem": bit2(0x224997),"good": 1, "addr": 0x224997, "bit": 2},111: { "levelId": 6, "mem": bit3(0x224997),"good": 1, "addr": 0x224997, "bit": 3},112: { "levelId": 6, "mem": bit4(0x224997),"good": 1, "addr": 0x224997, "bit": 4},113: { "levelId": 6, "mem": bit5(0x224997),"good": 1, "addr": 0x224997, "bit": 5},114: { "levelId": 6, "mem": bit6(0x224997),"good": 1, "addr": 0x224997, "bit": 6},115: { "levelId": 6, "mem": bit7(0x224997),"good": 1, "addr": 0x224997, "bit": 7},116: { "levelId": 6, "mem": bit0(0x224998),"good": 1, "addr": 0x224998, "bit": 0},117: { "levelId": 6, "mem": bit1(0x224998),"good": 1, "addr": 0x224998, "bit": 1},118: { "levelId": 6, "mem": bit2(0x224998),"good": 1, "addr": 0x224998, "bit": 2},119: { "levelId": 6, "mem": bit3(0x224998),"good": 1, "addr": 0x224998, "bit": 3},120: { "levelId": 6, "mem": bit4(0x224998),"good": 1, "addr": 0x224998, "bit": 4},121: { "levelId": 6, "mem": bit5(0x224998),"good": 1, "addr": 0x224998, "bit": 5},122: { "levelId": 6, "mem": bit6(0x224998),"good": 1, "addr": 0x224998, "bit": 6},123: { "levelId": 6, "mem": bit0(0x224999),"good": 1, "addr": 0x224999, "bit": 0},124: { "levelId": 6, "mem": bit1(0x224999),"good": 1, "addr": 0x224999, "bit": 1},125: { "levelId": 6, "mem": bit2(0x224999),"good": 1, "addr": 0x224999, "bit": 2},126: { "levelId": 6, "mem": bit3(0x224999),"good": 1, "addr": 0x224999, "bit": 3},127: { "levelId": 6, "mem": bit4(0x224999),"good": 1, "addr": 0x224999, "bit": 4},128: { "levelId": 6, "mem": bit5(0x224999),"good": 1, "addr": 0x224999, "bit": 5},129: { "levelId": 6, "mem": bit6(0x224999),"good": 1, "addr": 0x224999, "bit": 6},130: { "levelId": 6, "mem": bit7(0x224999),"good": 1, "addr": 0x224999, "bit": 7},131: { "levelId": 6, "mem": bit0(0x22499a),"good": 1, "addr": 0x22499a, "bit": 0},132: { "levelId": 6, "mem": bit1(0x22499a),"good": 1, "addr": 0x22499a, "bit": 1},133: { "levelId": 6, "mem": bit2(0x22499a),"good": 1, "addr": 0x22499a, "bit": 2},134: { "levelId": 6, "mem": bit3(0x22499a),"good": 1, "addr": 0x22499a, "bit": 3},135: { "levelId": 6, "mem": bit4(0x22499a),"good": 1, "addr": 0x22499a, "bit": 4},136: { "levelId": 6, "mem": bit5(0x22499a),"good": 1, "addr": 0x22499a, "bit": 5},137: { "levelId": 1, "mem": bit3(0x224a36),"good": 1, "addr": 0x224a36, "bit": 3},138: { "levelId": 1, "mem": bit4(0x224a36),"good": 1, "addr": 0x224a36, "bit": 4},139: { "levelId": 1, "mem": bit5(0x224a36),"good": 1, "addr": 0x224a36, "bit": 5},140: { "levelId": 1, "mem": bit6(0x224a36),"good": 1, "addr": 0x224a36, "bit": 6},141: { "levelId": 1, "mem": bit7(0x224a36),"good": 1, "addr": 0x224a36, "bit": 7},142: { "levelId": 6, "mem": bit7(0x224998),"good": 1, "addr": 0x224998, "bit": 7},143: { "levelId": 8, "mem": bit3(0x22499b),"good": 1, "addr": 0x22499b, "bit": 3},144: { "levelId": 8, "mem": bit4(0x22499b),"good": 1, "addr": 0x22499b, "bit": 4},145: { "levelId": 8, "mem": bit5(0x22499b),"good": 1, "addr": 0x22499b, "bit": 5},146: { "levelId": 8, "mem": bit5(0x22499c),"good": 1, "addr": 0x22499c, "bit": 5},147: { "levelId": 8, "mem": bit6(0x22499c),"good": 1, "addr": 0x22499c, "bit": 6},148: { "levelId": 8, "mem": bit7(0x22499c),"good": 1, "addr": 0x22499c, "bit": 7},149: { "levelId": 8, "mem": bit0(0x22499d),"good": 1, "addr": 0x22499d, "bit": 0},150: { "levelId": 8, "mem": bit1(0x22499d),"good": 1, "addr": 0x22499d, "bit": 1},151: { "levelId": 8, "mem": bit2(0x22499d),"good": 1, "addr": 0x22499d, "bit": 2},152: { "levelId": 8, "mem": bit3(0x22499d),"good": 1, "addr": 0x22499d, "bit": 3},153: { "levelId": 8, "mem": bit4(0x22499d),"good": 1, "addr": 0x22499d, "bit": 4},154: { "levelId": 8, "mem": bit5(0x22499d),"good": 1, "addr": 0x22499d, "bit": 5},155: { "levelId": 8, "mem": bit6(0x22499d),"good": 1, "addr": 0x22499d, "bit": 6},156: { "levelId": 8, "mem": bit7(0x22499d),"good": 1, "addr": 0x22499d, "bit": 7},157: { "levelId": 8, "mem": bit0(0x22499e),"good": 1, "addr": 0x22499e, "bit": 0},158: { "levelId": 8, "mem": bit1(0x22499e),"good": 1, "addr": 0x22499e, "bit": 1},159: { "levelId": 8, "mem": bit6(0x22499a),"good": 1, "addr": 0x22499a, "bit": 6},160: { "levelId": 8, "mem": bit7(0x22499a),"good": 1, "addr": 0x22499a, "bit": 7},161: { "levelId": 8, "mem": bit0(0x22499b),"good": 1, "addr": 0x22499b, "bit": 0},162: { "levelId": 8, "mem": bit1(0x22499b),"good": 1, "addr": 0x22499b, "bit": 1},163: { "levelId": 8, "mem": bit2(0x22499b),"good": 1, "addr": 0x22499b, "bit": 2},164: { "levelId": 8, "mem": bit6(0x22499b),"good": 1, "addr": 0x22499b, "bit": 6},165: { "levelId": 8, "mem": bit7(0x22499b),"good": 1, "addr": 0x22499b, "bit": 7},166: { "levelId": 8, "mem": bit0(0x22499c),"good": 1, "addr": 0x22499c, "bit": 0},167: { "levelId": 8, "mem": bit1(0x22499c),"good": 1, "addr": 0x22499c, "bit": 1},168: { "levelId": 8, "mem": bit2(0x22499c),"good": 1, "addr": 0x22499c, "bit": 2},169: { "levelId": 8, "mem": bit3(0x22499c),"good": 1, "addr": 0x22499c, "bit": 3},170: { "levelId": 8, "mem": bit4(0x22499c),"good": 1, "addr": 0x22499c, "bit": 4},171: { "levelId": 8, "mem": bit2(0x22499e),"good": 1, "addr": 0x22499e, "bit": 2},172: { "levelId": 8, "mem": bit3(0x22499e),"good": 1, "addr": 0x22499e, "bit": 3},173: { "levelId": 8, "mem": bit4(0x22499e),"good": 1, "addr": 0x22499e, "bit": 4},174: { "levelId": 8, "mem": bit5(0x22499e),"good": 1, "addr": 0x22499e, "bit": 5},175: { "levelId": 8, "mem": bit6(0x22499e),"good": 1, "addr": 0x22499e, "bit": 6},176: { "levelId": 8, "mem": bit7(0x22499e),"good": 1, "addr": 0x22499e, "bit": 7},177: { "levelId": 8, "mem": bit0(0x22499f),"good": 1, "addr": 0x22499f, "bit": 0},178: { "levelId": 8, "mem": bit1(0x22499f),"good": 1, "addr": 0x22499f, "bit": 1},179: { "levelId": 8, "mem": bit2(0x22499f),"good": 1, "addr": 0x22499f, "bit": 2},180: { "levelId": 8, "mem": bit3(0x22499f),"good": 1, "addr": 0x22499f, "bit": 3},181: { "levelId": 8, "mem": bit4(0x22499f),"good": 1, "addr": 0x22499f, "bit": 4},182: { "levelId": 8, "mem": bit5(0x22499f),"good": 1, "addr": 0x22499f, "bit": 5},183: { "levelId": 8, "mem": bit6(0x22499f),"good": 1, "addr": 0x22499f, "bit": 6},184: { "levelId": 8, "mem": bit7(0x22499f),"good": 1, "addr": 0x22499f, "bit": 7},185: { "levelId": 8, "mem": bit0(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 0},186: { "levelId": 8, "mem": bit1(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 1},187: { "levelId": 8, "mem": bit2(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 2},188: { "levelId": 8, "mem": bit3(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 3},189: { "levelId": 8, "mem": bit4(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 4},190: { "levelId": 8, "mem": bit5(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 5},191: { "levelId": 8, "mem": bit6(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 6},192: { "levelId": 8, "mem": bit7(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 7},193: { "levelId": 10, "mem": bit0(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 0},194: { "levelId": 10, "mem": bit1(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 1},195: { "levelId": 10, "mem": bit2(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 2},196: { "levelId": 10, "mem": bit3(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 3},197: { "levelId": 10, "mem": bit4(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 4},198: { "levelId": 10, "mem": bit2(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 2},199: { "levelId": 10, "mem": bit3(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 3},200: { "levelId": 10, "mem": bit4(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 4},201: { "levelId": 10, "mem": bit5(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 5},202: { "levelId": 10, "mem": bit6(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 6},203: { "levelId": 10, "mem": bit1(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 1},204: { "levelId": 10, "mem": bit5(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 5},205: { "levelId": 10, "mem": bit6(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 6},206: { "levelId": 10, "mem": bit7(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 7},207: { "levelId": 10, "mem": bit0(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 0},208: { "levelId": 10, "mem": bit3(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 3},209: { "levelId": 10, "mem": bit5(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 5},210: { "levelId": 10, "mem": bit6(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 6},211: { "levelId": 10, "mem": bit7(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 7},212: { "levelId": 10, "mem": bit0(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 0},213: { "levelId": 10, "mem": bit1(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 1},214: { "levelId": 10, "mem": bit2(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 2},215: { "levelId": 10, "mem": bit4(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 4},216: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},217: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},218: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},219: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},220: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},221: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},222: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},223: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},224: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},225: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},226: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},227: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},228: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},229: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},230: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},231: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},232: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},233: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},234: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},235: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},236: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},237: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},238: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},239: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},240: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},241: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},242: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},243: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},244: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},245: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},246: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},247: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},248: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},249: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},250: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},251: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},252: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},253: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},254: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},255: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},256: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},257: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},258: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},259: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},260: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},261: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},262: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},263: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},264: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},265: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},266: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},267: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},268: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},269: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},270: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},271: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},272: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},273: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},274: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},275: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},276: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},277: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},278: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},279: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},280: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},281: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},282: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},283: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},284: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},285: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},286: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},287: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},288: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},289: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},290: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},291: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},292: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},293: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},294: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},295: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},296: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},297: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},298: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},299: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},300: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},301: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},302: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},303: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},304: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},305: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},306: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},307: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},308: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},309: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},310: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},311: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},312: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},313: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},314: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},315: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},316: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},317: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},318: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},319: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},320: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},321: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},322: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},323: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},324: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},325: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},326: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},327: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},328: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},329: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},330: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},331: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},332: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},333: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},334: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},335: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},336: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},337: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},338: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},339: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},340: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},341: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},342: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},343: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},344: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},345: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},346: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},347: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},348: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},349: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},350: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},351: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},352: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},353: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},354: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},355: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},356: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},357: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},358: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},359: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},360: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},361: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},362: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},363: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},364: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},365: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},366: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},367: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},368: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},369: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},370: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},371: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},372: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},373: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},374: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},375: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},376: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},377: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},378: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},379: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},380: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},381: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},382: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},383: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},384: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},385: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},386: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},387: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},388: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},389: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},390: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},391: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},392: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},393: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},394: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},395: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},396: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},397: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},398: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},399: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},400: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},401: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},402: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},403: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},404: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},405: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},406: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},407: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},408: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},409: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},410: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},411: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},412: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},413: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},414: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},415: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},416: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},417: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},418: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},419: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},420: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},421: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},422: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},423: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},424: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},425: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},426: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},427: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},428: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},429: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},430: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},431: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},432: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},433: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},434: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},435: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},436: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},437: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},438: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},439: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},440: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},441: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},442: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},443: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},444: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},445: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},446: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},447: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},448: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},449: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},450: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},451: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},452: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},453: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},454: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},455: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},456: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},457: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},458: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},459: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},460: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},461: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},462: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},463: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},464: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},465: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},466: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},467: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},468: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},469: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},470: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},471: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},472: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},473: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},474: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},475: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},476: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},477: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},478: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},479: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},480: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},481: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},482: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},483: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},484: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},485: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},486: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},487: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},488: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},489: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},490: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},491: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},492: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},493: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},494: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},495: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},496: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},497: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},498: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},499: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},500: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},501: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},502: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},503: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},504: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},505: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},506: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},507: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},508: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},509: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},510: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},511: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},512: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},513: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},514: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},515: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},516: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},517: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},518: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},519: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},520: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},521: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},522: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},523: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},524: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},525: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},526: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},527: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},528: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},529: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},530: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},531: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},532: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},533: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},534: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},535: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},536: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},537: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},538: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},539: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},540: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},541: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},542: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},543: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},544: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},545: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},546: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},547: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},548: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},549: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},550: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},551: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},552: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},553: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},554: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},555: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},556: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},557: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},558: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},559: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},560: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},561: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},562: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},563: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},564: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},565: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},566: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},567: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},568: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},569: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},570: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},571: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},572: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},573: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},574: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},575: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},576: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},577: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},578: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},579: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},580: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},581: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},582: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},583: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},584: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},585: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},586: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},587: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},588: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},589: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},590: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},591: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},592: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},593: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},594: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},595: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},596: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},597: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},598: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},599: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},600: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},601: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},602: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},603: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},604: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},605: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},606: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},607: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},608: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},609: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},610: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},611: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},612: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},613: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},614: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},615: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},616: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},617: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},618: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},619: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},620: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},621: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},622: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},623: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},624: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},625: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},626: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},627: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},628: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},629: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},630: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},631: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},632: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},633: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},634: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},635: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},636: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},637: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},638: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},639: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},640: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},641: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},642: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},643: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},644: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},645: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},646: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},647: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},648: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},649: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},650: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},651: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},652: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},653: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},654: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},655: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},656: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},657: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},658: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},659: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},660: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},661: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},662: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},663: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},664: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},665: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},666: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},667: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},668: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},669: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},670: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},671: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},672: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},673: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},674: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},675: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},676: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},677: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},678: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},679: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},680: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},681: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},682: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},683: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},684: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},685: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},686: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},687: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},688: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},689: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},690: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},691: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},692: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},693: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},694: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},695: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},696: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},697: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},698: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},699: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},700: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},701: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},702: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},703: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},704: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},705: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},706: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},707: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},708: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},709: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},710: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},711: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},712: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},713: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},714: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},715: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},716: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},717: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},718: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},719: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},720: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},721: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},722: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},723: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},724: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},725: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},726: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},727: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},728: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},729: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},730: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},731: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},732: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},733: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},734: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},735: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},736: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},737: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},738: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},739: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},740: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},741: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},742: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},743: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},744: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},745: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},746: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},747: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},748: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},749: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},750: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},751: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},752: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},753: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},754: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},755: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},756: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},757: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},758: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},759: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},760: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},761: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},762: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},763: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},764: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},765: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},766: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},767: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},768: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},769: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},770: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},771: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},772: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},773: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},774: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},775: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},776: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},777: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},778: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},779: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},780: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},781: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},782: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},783: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},784: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},785: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},786: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},787: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},788: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},789: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},790: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},791: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},792: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},793: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},794: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},795: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},796: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},797: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},798: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},799: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},800: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},801: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},802: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},803: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},804: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},805: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},806: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},807: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},808: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},809: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},810: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},811: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},812: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},813: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},814: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},815: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},816: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},817: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},818: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},819: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},820: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},821: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},822: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},823: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},824: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},825: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},826: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},827: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},828: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},829: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},830: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},831: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},832: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},833: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},834: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},835: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},836: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},837: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},838: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},839: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},840: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},841: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},842: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},843: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},844: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},845: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},846: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},847: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},848: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},849: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},850: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},851: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},852: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},853: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},854: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},855: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},856: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},857: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},858: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},859: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},860: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},861: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},862: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},863: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},864: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},865: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},866: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},867: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},868: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},869: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},870: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},871: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},872: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},873: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},874: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},875: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},876: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},877: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},878: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},879: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},880: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},881: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},882: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},883: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},884: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},885: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},886: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},887: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},888: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},889: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},890: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},891: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},892: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},893: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},894: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},895: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},896: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},897: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},898: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},899: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},900: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},901: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},902: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},903: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},904: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},905: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},906: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},907: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},908: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},909: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},910: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},911: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},912: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},913: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},914: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},915: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},916: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},917: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},918: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},919: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},920: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},921: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},922: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},923: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},924: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},925: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},926: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},927: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},928: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},929: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},930: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},931: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},932: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},933: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},934: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},935: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},936: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},937: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},938: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},939: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},940: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},941: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},942: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},943: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},944: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},945: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},946: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},947: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},948: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},949: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},950: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},951: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},952: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},953: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},954: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},955: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},956: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},957: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},958: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},959: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},960: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},961: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},962: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},963: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},964: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},965: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},966: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},967: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},968: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},969: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},970: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},971: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},972: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},973: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},974: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},975: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},976: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},977: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},978: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},979: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},980: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},981: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},982: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},983: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},984: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},985: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},986: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},987: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},988: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},989: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},990: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},991: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},992: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},993: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},994: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},995: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},996: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},997: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},998: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},999: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},1000: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>1: { "levelId": 2, "mem": bit0(0x224988),"good": 1, "addr": 0x224988, "bit": 0},2: { "levelId": 2, "mem": bit1(0x224988),"good": 1, "addr": 0x224988, "bit": 1},3: { "levelId": 2, "mem": bit2(0x224988),"good": 1, "addr": 0x224988, "bit": 2},4: { "levelId": 2, "mem": bit3(0x224988),"good": 1, "addr": 0x224988, "bit": 3},5: { "levelId": 2, "mem": bit4(0x224988),"good": 1, "addr": 0x224988, "bit": 4},6: { "levelId": 2, "mem": bit5(0x224988),"good": 1, "addr": 0x224988, "bit": 5},7: { "levelId": 2, "mem": bit6(0x224988),"good": 1, "addr": 0x224988, "bit": 6},8: { "levelId": 2, "mem": bit7(0x224988),"good": 1, "addr": 0x224988, "bit": 7},9: { "levelId": 2, "mem": bit2(0x224989),"good": 1, "addr": 0x224989, "bit": 2},10: { "levelId": 2, "mem": bit1(0x22498a),"good": 1, "addr": 0x22498a, "bit": 1},11: { "levelId": 2, "mem": bit2(0x22498a),"good": 1, "addr": 0x22498a, "bit": 2},12: { "levelId": 2, "mem": bit3(0x22498a),"good": 1, "addr": 0x22498a, "bit": 3},13: { "levelId": 2, "mem": bit4(0x22498a),"good": 1, "addr": 0x22498a, "bit": 4},14: { "levelId": 2, "mem": bit5(0x22498a),"good": 1, "addr": 0x22498a, "bit": 5},15: { "levelId": 2, "mem": bit6(0x22498a),"good": 1, "addr": 0x22498a, "bit": 6},16: { "levelId": 2, "mem": bit7(0x22498a),"good": 1, "addr": 0x22498a, "bit": 7},17: { "levelId": 2, "mem": bit5(0x22498b),"good": 1, "addr": 0x22498b, "bit": 5},18: { "levelId": 2, "mem": bit6(0x22498b),"good": 1, "addr": 0x22498b, "bit": 6},19: { "levelId": 2, "mem": bit7(0x22498b),"good": 1, "addr": 0x22498b, "bit": 7},20: { "levelId": 2, "mem": bit0(0x22498c),"good": 1, "addr": 0x22498c, "bit": 0},21: { "levelId": 2, "mem": bit1(0x22498c),"good": 1, "addr": 0x22498c, "bit": 1},22: { "levelId": 2, "mem": bit2(0x22498c),"good": 1, "addr": 0x22498c, "bit": 2},23: { "levelId": 2, "mem": bit3(0x22498c),"good": 1, "addr": 0x22498c, "bit": 3},24: { "levelId": 2, "mem": bit4(0x22498c),"good": 1, "addr": 0x22498c, "bit": 4},25: { "levelId": 2, "mem": bit5(0x22498c),"good": 1, "addr": 0x22498c, "bit": 5},26: { "levelId": 2, "mem": bit6(0x22498c),"good": 1, "addr": 0x22498c, "bit": 6},27: { "levelId": 2, "mem": bit7(0x22498c),"good": 1, "addr": 0x22498c, "bit": 7},28: { "levelId": 2, "mem": bit0(0x22498d),"good": 1, "addr": 0x22498d, "bit": 0},29: { "levelId": 2, "mem": bit1(0x22498d),"good": 1, "addr": 0x22498d, "bit": 1},30: { "levelId": 2, "mem": bit2(0x22498d),"good": 1, "addr": 0x22498d, "bit": 2},31: { "levelId": 2, "mem": bit3(0x22498d),"good": 1, "addr": 0x22498d, "bit": 3},32: { "levelId": 2, "mem": bit4(0x22498d),"good": 1, "addr": 0x22498d, "bit": 4},33: { "levelId": 2, "mem": bit5(0x22498d),"good": 1, "addr": 0x22498d, "bit": 5},34: { "levelId": 2, "mem": bit6(0x22498d),"good": 1, "addr": 0x22498d, "bit": 6},35: { "levelId": 2, "mem": bit7(0x22498d),"good": 1, "addr": 0x22498d, "bit": 7},36: { "levelId": 2, "mem": bit0(0x22498e),"good": 1, "addr": 0x22498e, "bit": 0},37: { "levelId": 2, "mem": bit1(0x22498e),"good": 1, "addr": 0x22498e, "bit": 1},38: { "levelId": 5, "mem": bit2(0x22498e),"good": 1, "addr": 0x22498e, "bit": 2},39: { "levelId": 5, "mem": bit3(0x22498e),"good": 1, "addr": 0x22498e, "bit": 3},40: { "levelId": 5, "mem": bit4(0x22498e),"good": 1, "addr": 0x22498e, "bit": 4},41: { "levelId": 5, "mem": bit5(0x22498e),"good": 1, "addr": 0x22498e, "bit": 5},42: { "levelId": 5, "mem": bit6(0x22498e),"good": 1, "addr": 0x22498e, "bit": 6},43: { "levelId": 5, "mem": bit7(0x22498e),"good": 1, "addr": 0x22498e, "bit": 7},44: { "levelId": 5, "mem": bit0(0x22498f),"good": 1, "addr": 0x22498f, "bit": 0},45: { "levelId": 5, "mem": bit1(0x22498f),"good": 1, "addr": 0x22498f, "bit": 1},46: { "levelId": 5, "mem": bit2(0x22498f),"good": 1, "addr": 0x22498f, "bit": 2},47: { "levelId": 5, "mem": bit3(0x22498f),"good": 1, "addr": 0x22498f, "bit": 3},48: { "levelId": 5, "mem": bit4(0x22498f),"good": 1, "addr": 0x22498f, "bit": 4},49: { "levelId": 5, "mem": bit5(0x22498f),"good": 1, "addr": 0x22498f, "bit": 5},50: { "levelId": 5, "mem": bit6(0x22498f),"good": 1, "addr": 0x22498f, "bit": 6},51: { "levelId": 5, "mem": bit7(0x22498f),"good": 1, "addr": 0x22498f, "bit": 7},52: { "levelId": 5, "mem": bit0(0x224990),"good": 1, "addr": 0x224990, "bit": 0},53: { "levelId": 5, "mem": bit1(0x224990),"good": 1, "addr": 0x224990, "bit": 1},54: { "levelId": 5, "mem": bit2(0x224990),"good": 1, "addr": 0x224990, "bit": 2},55: { "levelId": 5, "mem": bit3(0x224990),"good": 1, "addr": 0x224990, "bit": 3},56: { "levelId": 5, "mem": bit4(0x224990),"good": 1, "addr": 0x224990, "bit": 4},57: { "levelId": 5, "mem": bit5(0x224990),"good": 1, "addr": 0x224990, "bit": 5},58: { "levelId": 5, "mem": bit6(0x224990),"good": 1, "addr": 0x224990, "bit": 6},59: { "levelId": 5, "mem": bit7(0x224990),"good": 1, "addr": 0x224990, "bit": 7},60: { "levelId": 5, "mem": bit0(0x224991),"good": 1, "addr": 0x224991, "bit": 0},61: { "levelId": 5, "mem": bit1(0x224991),"good": 1, "addr": 0x224991, "bit": 1},62: { "levelId": 5, "mem": bit2(0x224991),"good": 1, "addr": 0x224991, "bit": 2},63: { "levelId": 5, "mem": bit3(0x224991),"good": 1, "addr": 0x224991, "bit": 3},64: { "levelId": 5, "mem": bit4(0x224991),"good": 1, "addr": 0x224991, "bit": 4},65: { "levelId": 5, "mem": bit5(0x224991),"good": 1, "addr": 0x224991, "bit": 5},66: { "levelId": 5, "mem": bit6(0x224991),"good": 1, "addr": 0x224991, "bit": 6},67: { "levelId": 5, "mem": bit7(0x224991),"good": 1, "addr": 0x224991, "bit": 7},68: { "levelId": 5, "mem": bit0(0x224992),"good": 1, "addr": 0x224992, "bit": 0},69: { "levelId": 5, "mem": bit1(0x224992),"good": 1, "addr": 0x224992, "bit": 1},70: { "levelId": 5, "mem": bit2(0x224992),"good": 1, "addr": 0x224992, "bit": 2},71: { "levelId": 5, "mem": bit3(0x224992),"good": 1, "addr": 0x224992, "bit": 3},72: { "levelId": 5, "mem": bit4(0x224992),"good": 1, "addr": 0x224992, "bit": 4},73: { "levelId": 5, "mem": bit5(0x224992),"good": 1, "addr": 0x224992, "bit": 5},74: { "levelId": 5, "mem": bit6(0x224992),"good": 1, "addr": 0x224992, "bit": 6},75: { "levelId": 5, "mem": bit7(0x224992),"good": 1, "addr": 0x224992, "bit": 7},76: { "levelId": 5, "mem": bit0(0x224993),"good": 1, "addr": 0x224993, "bit": 0},77: { "levelId": 5, "mem": bit1(0x224993),"good": 1, "addr": 0x224993, "bit": 1},78: { "levelId": 5, "mem": bit2(0x224993),"good": 1, "addr": 0x224993, "bit": 2},79: { "levelId": 5, "mem": bit3(0x224993),"good": 1, "addr": 0x224993, "bit": 3},80: { "levelId": 5, "mem": bit4(0x224993),"good": 1, "addr": 0x224993, "bit": 4},81: { "levelId": 5, "mem": bit5(0x224993),"good": 1, "addr": 0x224993, "bit": 5},82: { "levelId": 5, "mem": bit6(0x224993),"good": 1, "addr": 0x224993, "bit": 6},83: { "levelId": 5, "mem": bit7(0x224993),"good": 1, "addr": 0x224993, "bit": 7},84: { "levelId": 5, "mem": bit0(0x224994),"good": 1, "addr": 0x224994, "bit": 0},85: { "levelId": 5, "mem": bit1(0x224994),"good": 1, "addr": 0x224994, "bit": 1},86: { "levelId": 5, "mem": bit2(0x224994),"good": 1, "addr": 0x224994, "bit": 2},87: { "levelId": 5, "mem": bit3(0x224994),"good": 1, "addr": 0x224994, "bit": 3},88: { "levelId": 6, "mem": bit4(0x224994),"good": 1, "addr": 0x224994, "bit": 4},89: { "levelId": 6, "mem": bit5(0x224994),"good": 1, "addr": 0x224994, "bit": 5},90: { "levelId": 6, "mem": bit6(0x224994),"good": 1, "addr": 0x224994, "bit": 6},91: { "levelId": 6, "mem": bit7(0x224994),"good": 1, "addr": 0x224994, "bit": 7},92: { "levelId": 6, "mem": bit0(0x224995),"good": 1, "addr": 0x224995, "bit": 0},93: { "levelId": 6, "mem": bit1(0x224995),"good": 1, "addr": 0x224995, "bit": 1},94: { "levelId": 6, "mem": bit2(0x224995),"good": 1, "addr": 0x224995, "bit": 2},95: { "levelId": 6, "mem": bit3(0x224995),"good": 1, "addr": 0x224995, "bit": 3},96: { "levelId": 6, "mem": bit4(0x224995),"good": 1, "addr": 0x224995, "bit": 4},97: { "levelId": 6, "mem": bit5(0x224995),"good": 1, "addr": 0x224995, "bit": 5},98: { "levelId": 6, "mem": bit6(0x224995),"good": 1, "addr": 0x224995, "bit": 6},99: { "levelId": 6, "mem": bit7(0x224995),"good": 1, "addr": 0x224995, "bit": 7},100: { "levelId": 6, "mem": bit0(0x224996),"good": 1, "addr": 0x224996, "bit": 0},101: { "levelId": 6, "mem": bit1(0x224996),"good": 1, "addr": 0x224996, "bit": 1},102: { "levelId": 6, "mem": bit2(0x224996),"good": 1, "addr": 0x224996, "bit": 2},103: { "levelId": 6, "mem": bit3(0x224996),"good": 1, "addr": 0x224996, "bit": 3},104: { "levelId": 6, "mem": bit4(0x224996),"good": 1, "addr": 0x224996, "bit": 4},105: { "levelId": 6, "mem": bit5(0x224996),"good": 1, "addr": 0x224996, "bit": 5},106: { "levelId": 6, "mem": bit6(0x224996),"good": 1, "addr": 0x224996, "bit": 6},107: { "levelId": 6, "mem": bit7(0x224996),"good": 1, "addr": 0x224996, "bit": 7},108: { "levelId": 6, "mem": bit0(0x224997),"good": 1, "addr": 0x224997, "bit": 0},109: { "levelId": 6, "mem": bit1(0x224997),"good": 1, "addr": 0x224997, "bit": 1},110: { "levelId": 6, "mem": bit2(0x224997),"good": 1, "addr": 0x224997, "bit": 2},111: { "levelId": 6, "mem": bit3(0x224997),"good": 1, "addr": 0x224997, "bit": 3},112: { "levelId": 6, "mem": bit4(0x224997),"good": 1, "addr": 0x224997, "bit": 4},113: { "levelId": 6, "mem": bit5(0x224997),"good": 1, "addr": 0x224997, "bit": 5},114: { "levelId": 6, "mem": bit6(0x224997),"good": 1, "addr": 0x224997, "bit": 6},115: { "levelId": 6, "mem": bit7(0x224997),"good": 1, "addr": 0x224997, "bit": 7},116: { "levelId": 6, "mem": bit0(0x224998),"good": 1, "addr": 0x224998, "bit": 0},117: { "levelId": 6, "mem": bit1(0x224998),"good": 1, "addr": 0x224998, "bit": 1},118: { "levelId": 6, "mem": bit2(0x224998),"good": 1, "addr": 0x224998, "bit": 2},119: { "levelId": 6, "mem": bit3(0x224998),"good": 1, "addr": 0x224998, "bit": 3},120: { "levelId": 6, "mem": bit4(0x224998),"good": 1, "addr": 0x224998, "bit": 4},121: { "levelId": 6, "mem": bit5(0x224998),"good": 1, "addr": 0x224998, "bit": 5},122: { "levelId": 6, "mem": bit6(0x224998),"good": 1, "addr": 0x224998, "bit": 6},123: { "levelId": 6, "mem": bit0(0x224999),"good": 1, "addr": 0x224999, "bit": 0},124: { "levelId": 6, "mem": bit1(0x224999),"good": 1, "addr": 0x224999, "bit": 1},125: { "levelId": 6, "mem": bit2(0x224999),"good": 1, "addr": 0x224999, "bit": 2},126: { "levelId": 6, "mem": bit3(0x224999),"good": 1, "addr": 0x224999, "bit": 3},127: { "levelId": 6, "mem": bit4(0x224999),"good": 1, "addr": 0x224999, "bit": 4},128: { "levelId": 6, "mem": bit5(0x224999),"good": 1, "addr": 0x224999, "bit": 5},129: { "levelId": 6, "mem": bit6(0x224999),"good": 1, "addr": 0x224999, "bit": 6},130: { "levelId": 6, "mem": bit7(0x224999),"good": 1, "addr": 0x224999, "bit": 7},131: { "levelId": 6, "mem": bit0(0x22499a),"good": 1, "addr": 0x22499a, "bit": 0},132: { "levelId": 6, "mem": bit1(0x22499a),"good": 1, "addr": 0x22499a, "bit": 1},133: { "levelId": 6, "mem": bit2(0x22499a),"good": 1, "addr": 0x22499a, "bit": 2},134: { "levelId": 6, "mem": bit3(0x22499a),"good": 1, "addr": 0x22499a, "bit": 3},135: { "levelId": 6, "mem": bit4(0x22499a),"good": 1, "addr": 0x22499a, "bit": 4},136: { "levelId": 6, "mem": bit5(0x22499a),"good": 1, "addr": 0x22499a, "bit": 5},137: { "levelId": 1, "mem": bit3(0x224a36),"good": 1, "addr": 0x224a36, "bit": 3},138: { "levelId": 1, "mem": bit4(0x224a36),"good": 1, "addr": 0x224a36, "bit": 4},139: { "levelId": 1, "mem": bit5(0x224a36),"good": 1, "addr": 0x224a36, "bit": 5},140: { "levelId": 1, "mem": bit6(0x224a36),"good": 1, "addr": 0x224a36, "bit": 6},141: { "levelId": 1, "mem": bit7(0x224a36),"good": 1, "addr": 0x224a36, "bit": 7},142: { "levelId": 6, "mem": bit7(0x224998),"good": 1, "addr": 0x224998, "bit": 7},143: { "levelId": 8, "mem": bit3(0x22499b),"good": 1, "addr": 0x22499b, "bit": 3},144: { "levelId": 8, "mem": bit4(0x22499b),"good": 1, "addr": 0x22499b, "bit": 4},145: { "levelId": 8, "mem": bit5(0x22499b),"good": 1, "addr": 0x22499b, "bit": 5},146: { "levelId": 8, "mem": bit5(0x22499c),"good": 1, "addr": 0x22499c, "bit": 5},147: { "levelId": 8, "mem": bit6(0x22499c),"good": 1, "addr": 0x22499c, "bit": 6},148: { "levelId": 8, "mem": bit7(0x22499c),"good": 1, "addr": 0x22499c, "bit": 7},149: { "levelId": 8, "mem": bit0(0x22499d),"good": 1, "addr": 0x22499d, "bit": 0},150: { "levelId": 8, "mem": bit1(0x22499d),"good": 1, "addr": 0x22499d, "bit": 1},151: { "levelId": 8, "mem": bit2(0x22499d),"good": 1, "addr": 0x22499d, "bit": 2},152: { "levelId": 8, "mem": bit3(0x22499d),"good": 1, "addr": 0x22499d, "bit": 3},153: { "levelId": 8, "mem": bit4(0x22499d),"good": 1, "addr": 0x22499d, "bit": 4},154: { "levelId": 8, "mem": bit5(0x22499d),"good": 1, "addr": 0x22499d, "bit": 5},155: { "levelId": 8, "mem": bit6(0x22499d),"good": 1, "addr": 0x22499d, "bit": 6},156: { "levelId": 8, "mem": bit7(0x22499d),"good": 1, "addr": 0x22499d, "bit": 7},157: { "levelId": 8, "mem": bit0(0x22499e),"good": 1, "addr": 0x22499e, "bit": 0},158: { "levelId": 8, "mem": bit1(0x22499e),"good": 1, "addr": 0x22499e, "bit": 1},159: { "levelId": 8, "mem": bit6(0x22499a),"good": 1, "addr": 0x22499a, "bit": 6},160: { "levelId": 8, "mem": bit7(0x22499a),"good": 1, "addr": 0x22499a, "bit": 7},161: { "levelId": 8, "mem": bit0(0x22499b),"good": 1, "addr": 0x22499b, "bit": 0},162: { "levelId": 8, "mem": bit1(0x22499b),"good": 1, "addr": 0x22499b, "bit": 1},163: { "levelId": 8, "mem": bit2(0x22499b),"good": 1, "addr": 0x22499b, "bit": 2},164: { "levelId": 8, "mem": bit6(0x22499b),"good": 1, "addr": 0x22499b, "bit": 6},165: { "levelId": 8, "mem": bit7(0x22499b),"good": 1, "addr": 0x22499b, "bit": 7},166: { "levelId": 8, "mem": bit0(0x22499c),"good": 1, "addr": 0x22499c, "bit": 0},167: { "levelId": 8, "mem": bit1(0x22499c),"good": 1, "addr": 0x22499c, "bit": 1},168: { "levelId": 8, "mem": bit2(0x22499c),"good": 1, "addr": 0x22499c, "bit": 2},169: { "levelId": 8, "mem": bit3(0x22499c),"good": 1, "addr": 0x22499c, "bit": 3},170: { "levelId": 8, "mem": bit4(0x22499c),"good": 1, "addr": 0x22499c, "bit": 4},171: { "levelId": 8, "mem": bit2(0x22499e),"good": 1, "addr": 0x22499e, "bit": 2},172: { "levelId": 8, "mem": bit3(0x22499e),"good": 1, "addr": 0x22499e, "bit": 3},173: { "levelId": 8, "mem": bit4(0x22499e),"good": 1, "addr": 0x22499e, "bit": 4},174: { "levelId": 8, "mem": bit5(0x22499e),"good": 1, "addr": 0x22499e, "bit": 5},175: { "levelId": 8, "mem": bit6(0x22499e),"good": 1, "addr": 0x22499e, "bit": 6},176: { "levelId": 8, "mem": bit7(0x22499e),"good": 1, "addr": 0x22499e, "bit": 7},177: { "levelId": 8, "mem": bit0(0x22499f),"good": 1, "addr": 0x22499f, "bit": 0},178: { "levelId": 8, "mem": bit1(0x22499f),"good": 1, "addr": 0x22499f, "bit": 1},179: { "levelId": 8, "mem": bit2(0x22499f),"good": 1, "addr": 0x22499f, "bit": 2},180: { "levelId": 8, "mem": bit3(0x22499f),"good": 1, "addr": 0x22499f, "bit": 3},181: { "levelId": 8, "mem": bit4(0x22499f),"good": 1, "addr": 0x22499f, "bit": 4},182: { "levelId": 8, "mem": bit5(0x22499f),"good": 1, "addr": 0x22499f, "bit": 5},183: { "levelId": 8, "mem": bit6(0x22499f),"good": 1, "addr": 0x22499f, "bit": 6},184: { "levelId": 8, "mem": bit7(0x22499f),"good": 1, "addr": 0x22499f, "bit": 7},185: { "levelId": 8, "mem": bit0(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 0},186: { "levelId": 8, "mem": bit1(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 1},187: { "levelId": 8, "mem": bit2(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 2},188: { "levelId": 8, "mem": bit3(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 3},189: { "levelId": 8, "mem": bit4(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 4},190: { "levelId": 8, "mem": bit5(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 5},191: { "levelId": 8, "mem": bit6(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 6},192: { "levelId": 8, "mem": bit7(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 7},193: { "levelId": 10, "mem": bit0(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 0},194: { "levelId": 10, "mem": bit1(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 1},195: { "levelId": 10, "mem": bit2(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 2},196: { "levelId": 10, "mem": bit3(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 3},197: { "levelId": 10, "mem": bit4(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 4},198: { "levelId": 10, "mem": bit2(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 2},199: { "levelId": 10, "mem": bit3(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 3},200: { "levelId": 10, "mem": bit4(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 4},201: { "levelId": 10, "mem": bit5(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 5},202: { "levelId": 10, "mem": bit6(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 6},203: { "levelId": 10, "mem": bit1(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 1},204: { "levelId": 10, "mem": bit5(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 5},205: { "levelId": 10, "mem": bit6(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 6},206: { "levelId": 10, "mem": bit7(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 7},207: { "levelId": 10, "mem": bit0(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 0},208: { "levelId": 10, "mem": bit3(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 3},209: { "levelId": 10, "mem": bit5(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 5},210: { "levelId": 10, "mem": bit6(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 6},211: { "levelId": 10, "mem": bit7(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 7},212: { "levelId": 10, "mem": bit0(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 0},213: { "levelId": 10, "mem": bit1(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 1},214: { "levelId": 10, "mem": bit2(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 2},215: { "levelId": 10, "mem": bit4(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 4},216: { "levelId": 11, "mem": bit6(0x2249e5),"good": 1, "addr": 0x2249e5, "bit": 6},217: { "levelId": 11, "mem": bit7(0x2249e5),"good": 1, "addr": 0x2249e5, "bit": 7},218: { "levelId": 11, "mem": bit0(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 0},219: { "levelId": 11, "mem": bit1(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 1},220: { "levelId": 11, "mem": bit2(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 2},221: { "levelId": 11, "mem": bit3(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 3},222: { "levelId": 11, "mem": bit4(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 4},223: { "levelId": 11, "mem": bit5(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 5},224: { "levelId": 11, "mem": bit6(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 6},225: { "levelId": 11, "mem": bit7(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 7},226: { "levelId": 11, "mem": bit0(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 0},227: { "levelId": 11, "mem": bit1(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 1},228: { "levelId": 11, "mem": bit2(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 2},229: { "levelId": 11, "mem": bit3(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 3},230: { "levelId": 11, "mem": bit4(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 4},231: { "levelId": 11, "mem": bit5(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 5},232: { "levelId": 11, "mem": bit6(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 6},233: { "levelId": 11, "mem": bit7(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 7},234: { "levelId": 11, "mem": bit0(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 0},235: { "levelId": 11, "mem": bit1(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 1},236: { "levelId": 11, "mem": bit2(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 2},237: { "levelId": 11, "mem": bit3(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 3},238: { "levelId": 11, "mem": bit4(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 4},239: { "levelId": 11, "mem": bit5(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 5},240: { "levelId": 11, "mem": bit6(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 6},241: { "levelId": 11, "mem": bit7(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 7},242: { "levelId": 11, "mem": bit0(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 0},243: { "levelId": 11, "mem": bit1(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 1},244: { "levelId": 11, "mem": bit2(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 2},245: { "levelId": 11, "mem": bit3(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 3},246: { "levelId": 11, "mem": bit4(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 4},247: { "levelId": 11, "mem": bit5(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 5},248: { "levelId": 11, "mem": bit6(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 6},249: { "levelId": 11, "mem": bit7(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 7},250: { "levelId": 11, "mem": bit0(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 0},251: { "levelId": 11, "mem": bit1(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 1},252: { "levelId": 11, "mem": bit2(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 2},253: { "levelId": 11, "mem": bit3(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 3},254: { "levelId": 11, "mem": bit4(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 4},255: { "levelId": 11, "mem": bit5(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 5},256: { "levelId": 11, "mem": bit6(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 6},257: { "levelId": 11, "mem": bit7(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 7},258: { "levelId": 11, "mem": bit0(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 0},259: { "levelId": 11, "mem": bit1(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 1},260: { "levelId": 11, "mem": bit2(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 2},261: { "levelId": 11, "mem": bit3(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 3},262: { "levelId": 11, "mem": bit4(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 4},263: { "levelId": 11, "mem": bit5(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 5},264: { "levelId": 11, "mem": bit6(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 6},265: { "levelId": 11, "mem": bit7(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 7},266: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},267: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},268: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},269: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},270: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},271: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},272: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},273: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},274: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},275: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},276: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},277: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},278: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},279: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},280: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},281: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},282: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},283: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},284: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},285: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},286: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},287: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},288: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},289: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},290: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},291: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},292: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},293: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},294: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},295: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},296: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},297: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},298: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},299: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},300: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},301: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},302: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},303: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},304: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},305: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},306: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},307: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},308: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},309: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},310: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},311: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},312: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},313: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},314: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},315: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},316: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},317: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},318: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},319: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},320: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},321: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},322: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},323: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},324: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},325: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},326: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},327: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},328: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},329: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},330: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},331: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},332: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},333: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},334: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},335: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},336: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},337: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},338: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},339: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},340: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},341: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},342: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},343: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},344: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},345: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},346: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},347: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},348: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},349: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},350: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},351: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},352: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},353: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},354: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},355: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},356: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},357: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},358: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},359: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},360: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},361: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},362: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},363: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},364: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},365: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},366: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},367: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},368: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},369: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},370: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},371: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},372: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},373: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},374: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},375: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},376: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},377: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},378: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},379: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},380: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},381: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},382: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},383: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},384: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},385: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},386: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},387: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},388: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},389: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},390: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},391: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},392: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},393: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},394: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},395: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},396: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},397: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},398: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},399: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},400: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},401: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},402: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},403: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},404: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},405: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},406: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},407: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},408: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},409: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},410: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},411: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},412: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},413: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},414: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},415: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},416: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},417: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},418: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},419: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},420: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},421: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},422: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},423: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},424: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},425: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},426: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},427: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},428: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},429: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},430: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},431: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},432: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},433: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},434: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},435: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},436: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},437: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},438: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},439: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},440: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},441: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},442: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},443: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},444: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},445: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},446: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},447: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},448: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},449: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},450: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},451: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},452: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},453: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},454: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},455: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},456: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},457: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},458: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},459: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},460: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},461: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},462: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},463: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},464: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},465: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},466: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},467: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},468: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},469: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},470: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},471: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},472: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},473: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},474: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},475: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},476: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},477: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},478: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},479: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},480: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},481: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},482: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},483: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},484: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},485: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},486: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},487: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},488: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},489: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},490: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},491: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},492: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},493: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},494: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},495: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},496: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},497: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},498: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},499: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},500: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},501: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},502: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},503: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},504: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},505: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},506: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},507: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},508: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},509: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},510: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},511: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},512: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},513: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},514: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},515: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},516: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},517: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},518: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},519: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},520: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},521: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},522: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},523: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},524: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},525: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},526: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},527: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},528: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},529: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},530: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},531: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},532: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},533: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},534: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},535: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},536: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},537: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},538: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},539: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},540: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},541: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},542: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},543: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},544: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},545: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},546: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},547: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},548: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},549: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},550: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},551: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},552: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},553: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},554: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},555: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},556: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},557: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},558: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},559: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},560: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},561: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},562: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},563: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},564: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},565: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},566: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},567: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},568: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},569: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},570: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},571: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},572: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},573: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},574: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},575: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},576: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},577: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},578: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},579: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},580: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},581: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},582: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},583: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},584: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},585: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},586: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},587: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},588: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},589: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},590: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},591: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},592: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},593: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},594: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},595: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},596: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},597: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},598: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},599: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},600: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},601: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},602: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},603: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},604: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},605: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},606: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},607: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},608: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},609: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},610: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},611: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},612: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},613: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},614: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},615: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},616: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},617: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},618: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},619: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},620: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},621: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},622: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},623: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},624: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},625: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},626: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},627: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},628: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},629: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},630: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},631: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},632: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},633: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},634: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},635: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},636: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},637: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},638: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},639: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},640: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},641: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},642: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},643: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},644: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},645: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},646: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},647: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},648: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},649: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},650: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},651: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},652: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},653: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},654: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},655: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},656: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},657: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},658: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},659: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},660: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},661: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},662: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},663: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},664: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},665: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},666: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},667: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},668: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},669: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},670: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},671: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},672: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},673: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},674: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},675: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},676: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},677: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},678: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},679: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},680: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},681: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},682: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},683: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},684: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},685: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},686: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},687: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},688: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},689: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},690: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},691: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},692: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},693: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},694: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},695: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},696: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},697: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},698: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},699: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},700: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},701: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},702: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},703: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},704: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},705: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},706: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},707: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},708: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},709: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},710: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},711: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},712: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},713: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},714: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},715: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},716: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},717: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},718: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},719: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},720: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},721: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},722: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},723: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},724: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},725: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},726: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},727: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},728: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},729: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},730: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},731: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},732: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},733: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},734: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},735: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},736: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},737: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},738: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},739: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},740: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},741: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},742: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},743: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},744: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},745: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},746: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},747: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},748: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},749: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},750: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},751: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},752: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},753: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},754: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},755: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},756: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},757: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},758: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},759: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},760: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},761: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},762: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},763: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},764: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},765: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},766: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},767: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},768: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},769: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},770: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},771: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},772: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},773: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},774: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},775: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},776: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},777: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},778: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},779: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},780: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},781: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},782: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},783: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},784: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},785: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},786: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},787: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},788: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},789: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},790: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},791: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},792: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},793: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},794: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},795: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},796: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},797: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},798: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},799: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},800: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},801: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},802: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},803: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},804: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},805: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},806: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},807: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},808: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},809: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},810: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},811: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},812: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},813: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},814: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},815: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},816: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},817: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},818: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},819: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},820: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},821: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},822: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},823: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},824: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},825: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},826: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},827: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},828: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},829: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},830: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},831: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},832: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},833: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},834: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},835: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},836: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},837: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},838: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},839: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},840: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},841: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},842: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},843: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},844: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},845: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},846: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},847: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},848: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},849: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},850: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},851: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},852: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},853: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},854: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},855: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},856: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},857: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},858: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},859: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},860: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},861: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},862: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},863: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},864: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},865: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},866: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},867: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},868: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},869: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},870: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},871: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},872: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},873: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},874: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},875: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},876: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},877: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},878: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},879: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},880: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},881: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},882: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},883: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},884: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},885: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},886: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},887: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},888: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},889: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},890: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},891: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},892: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},893: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},894: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},895: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},896: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},897: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},898: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},899: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},900: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},901: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},902: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},903: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},904: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},905: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},906: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},907: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},908: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},909: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},910: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},911: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},912: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},913: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},914: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},915: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},916: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},917: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},918: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},919: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},920: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},921: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},922: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},923: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},924: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},925: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},926: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},927: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},928: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},929: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},930: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},931: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},932: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},933: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},934: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},935: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},936: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},937: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},938: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},939: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},940: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},941: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},942: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},943: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},944: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},945: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},946: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},947: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},948: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},949: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},950: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},951: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},952: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},953: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},954: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},955: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},956: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},957: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},958: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},959: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},960: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},961: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},962: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},963: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},964: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},965: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},966: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},967: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},968: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},969: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},970: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},971: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},972: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},973: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},974: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},975: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},976: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},977: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},978: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},979: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},980: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},981: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},982: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},983: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},984: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},985: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},986: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},987: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},988: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},989: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},990: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},991: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},992: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},993: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},994: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},995: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},996: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},997: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},998: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},999: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},1000: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0</v>
@@ -7785,7 +7883,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1</v>
@@ -7801,7 +7899,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>2</v>
@@ -7817,7 +7915,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>3</v>
@@ -7833,7 +7931,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>4</v>
@@ -7849,7 +7947,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>5</v>
@@ -7865,7 +7963,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>6</v>
@@ -7881,7 +7979,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>7</v>
@@ -7897,7 +7995,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>2</v>
@@ -7912,7 +8010,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>1</v>
@@ -7927,7 +8025,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>2</v>
@@ -7942,7 +8040,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>3</v>
@@ -7957,7 +8055,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>4</v>
@@ -7972,7 +8070,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>5</v>
@@ -7987,7 +8085,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>6</v>
@@ -8002,7 +8100,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>7</v>
@@ -8017,7 +8115,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>5</v>
@@ -8032,7 +8130,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>6</v>
@@ -8047,7 +8145,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>7</v>
@@ -8062,7 +8160,7 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>0</v>
@@ -8077,7 +8175,7 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="6" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>1</v>
@@ -8092,7 +8190,7 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>2</v>
@@ -8107,7 +8205,7 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>3</v>
@@ -8122,7 +8220,7 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="6" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>4</v>
@@ -8137,7 +8235,7 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="6" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>5</v>
@@ -8152,7 +8250,7 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="6" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>6</v>
@@ -8167,7 +8265,7 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="6" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>7</v>
@@ -8182,7 +8280,7 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="6" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>0</v>
@@ -8197,7 +8295,7 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="6" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>1</v>
@@ -8212,7 +8310,7 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="6" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>2</v>
@@ -8227,7 +8325,7 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="6" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>3</v>
@@ -8242,7 +8340,7 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="6" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>4</v>
@@ -8257,7 +8355,7 @@
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="6" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>5</v>
@@ -8272,7 +8370,7 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="6" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>6</v>
@@ -8287,7 +8385,7 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="6" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>7</v>
@@ -8302,7 +8400,7 @@
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="6" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>0</v>
@@ -8317,7 +8415,7 @@
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="6" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>1</v>
@@ -8332,7 +8430,7 @@
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>2</v>
@@ -8347,7 +8445,7 @@
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>3</v>
@@ -8362,7 +8460,7 @@
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>4</v>
@@ -8377,7 +8475,7 @@
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>5</v>
@@ -8392,7 +8490,7 @@
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>6</v>
@@ -8407,7 +8505,7 @@
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="B44" s="0" t="n">
         <v>7</v>
@@ -8422,7 +8520,7 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="B45" s="0" t="n">
         <v>0</v>
@@ -8437,7 +8535,7 @@
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="B46" s="0" t="n">
         <v>1</v>
@@ -8452,7 +8550,7 @@
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="B47" s="0" t="n">
         <v>2</v>
@@ -8467,7 +8565,7 @@
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="B48" s="0" t="n">
         <v>3</v>
@@ -8482,7 +8580,7 @@
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="B49" s="0" t="n">
         <v>4</v>
@@ -8497,7 +8595,7 @@
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="B50" s="0" t="n">
         <v>5</v>
@@ -8512,7 +8610,7 @@
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="B51" s="0" t="n">
         <v>6</v>
@@ -8527,7 +8625,7 @@
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="B52" s="0" t="n">
         <v>7</v>
@@ -8542,7 +8640,7 @@
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="B53" s="0" t="n">
         <v>0</v>
@@ -8557,7 +8655,7 @@
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="B54" s="0" t="n">
         <v>1</v>
@@ -8572,7 +8670,7 @@
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="B55" s="0" t="n">
         <v>2</v>
@@ -8587,7 +8685,7 @@
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="B56" s="0" t="n">
         <v>3</v>
@@ -8602,7 +8700,7 @@
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="B57" s="0" t="n">
         <v>4</v>
@@ -8617,7 +8715,7 @@
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="B58" s="0" t="n">
         <v>5</v>
@@ -8632,7 +8730,7 @@
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="B59" s="0" t="n">
         <v>6</v>
@@ -8647,7 +8745,7 @@
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="B60" s="0" t="n">
         <v>7</v>
@@ -8662,7 +8760,7 @@
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="B61" s="0" t="n">
         <v>0</v>
@@ -8677,7 +8775,7 @@
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="B62" s="0" t="n">
         <v>1</v>
@@ -8692,7 +8790,7 @@
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="B63" s="0" t="n">
         <v>2</v>
@@ -8707,7 +8805,7 @@
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="B64" s="0" t="n">
         <v>3</v>
@@ -8722,7 +8820,7 @@
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="B65" s="0" t="n">
         <v>4</v>
@@ -8737,7 +8835,7 @@
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="B66" s="0" t="n">
         <v>5</v>
@@ -8752,7 +8850,7 @@
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="B67" s="0" t="n">
         <v>6</v>
@@ -8767,7 +8865,7 @@
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="B68" s="0" t="n">
         <v>7</v>
@@ -8782,7 +8880,7 @@
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="B69" s="0" t="n">
         <v>0</v>
@@ -8797,7 +8895,7 @@
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="B70" s="0" t="n">
         <v>1</v>
@@ -8812,7 +8910,7 @@
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="B71" s="0" t="n">
         <v>2</v>
@@ -8827,7 +8925,7 @@
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="B72" s="0" t="n">
         <v>3</v>
@@ -8842,7 +8940,7 @@
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="B73" s="0" t="n">
         <v>4</v>
@@ -8857,7 +8955,7 @@
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="B74" s="0" t="n">
         <v>5</v>
@@ -8872,7 +8970,7 @@
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="B75" s="0" t="n">
         <v>6</v>
@@ -8887,7 +8985,7 @@
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="B76" s="0" t="n">
         <v>7</v>
@@ -8902,7 +9000,7 @@
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="B77" s="0" t="n">
         <v>0</v>
@@ -8917,7 +9015,7 @@
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="B78" s="0" t="n">
         <v>1</v>
@@ -8932,7 +9030,7 @@
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="B79" s="0" t="n">
         <v>2</v>
@@ -8947,7 +9045,7 @@
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="B80" s="0" t="n">
         <v>3</v>
@@ -8962,7 +9060,7 @@
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="B81" s="0" t="n">
         <v>4</v>
@@ -8977,7 +9075,7 @@
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="B82" s="0" t="n">
         <v>5</v>
@@ -8992,7 +9090,7 @@
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="B83" s="0" t="n">
         <v>6</v>
@@ -9007,7 +9105,7 @@
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="B84" s="0" t="n">
         <v>7</v>
@@ -9022,7 +9120,7 @@
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="6" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="B85" s="0" t="n">
         <v>0</v>
@@ -9037,7 +9135,7 @@
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="6" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="B86" s="0" t="n">
         <v>1</v>
@@ -9052,7 +9150,7 @@
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="6" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="B87" s="0" t="n">
         <v>2</v>
@@ -9067,7 +9165,7 @@
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="6" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="B88" s="0" t="n">
         <v>3</v>
@@ -9082,7 +9180,7 @@
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="B89" s="0" t="n">
         <v>4</v>
@@ -9097,7 +9195,7 @@
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="B90" s="0" t="n">
         <v>5</v>
@@ -9112,7 +9210,7 @@
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="B91" s="0" t="n">
         <v>6</v>
@@ -9127,7 +9225,7 @@
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="B92" s="0" t="n">
         <v>7</v>
@@ -9142,7 +9240,7 @@
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="B93" s="0" t="n">
         <v>0</v>
@@ -9157,7 +9255,7 @@
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="B94" s="0" t="n">
         <v>1</v>
@@ -9172,7 +9270,7 @@
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="B95" s="0" t="n">
         <v>2</v>
@@ -9187,7 +9285,7 @@
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="B96" s="0" t="n">
         <v>3</v>
@@ -9202,7 +9300,7 @@
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="B97" s="0" t="n">
         <v>4</v>
@@ -9217,7 +9315,7 @@
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="B98" s="0" t="n">
         <v>5</v>
@@ -9232,7 +9330,7 @@
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="B99" s="0" t="n">
         <v>6</v>
@@ -9247,7 +9345,7 @@
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="B100" s="0" t="n">
         <v>7</v>
@@ -9262,7 +9360,7 @@
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="B101" s="0" t="n">
         <v>0</v>
@@ -9277,7 +9375,7 @@
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="B102" s="0" t="n">
         <v>1</v>
@@ -9292,7 +9390,7 @@
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="B103" s="0" t="n">
         <v>2</v>
@@ -9307,7 +9405,7 @@
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="B104" s="0" t="n">
         <v>3</v>
@@ -9322,7 +9420,7 @@
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="B105" s="0" t="n">
         <v>4</v>
@@ -9337,7 +9435,7 @@
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="B106" s="0" t="n">
         <v>5</v>
@@ -9352,7 +9450,7 @@
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="B107" s="0" t="n">
         <v>6</v>
@@ -9367,7 +9465,7 @@
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="B108" s="0" t="n">
         <v>7</v>
@@ -9382,7 +9480,7 @@
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="B109" s="0" t="n">
         <v>0</v>
@@ -9397,7 +9495,7 @@
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="B110" s="0" t="n">
         <v>1</v>
@@ -9412,7 +9510,7 @@
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="B111" s="0" t="n">
         <v>2</v>
@@ -9427,7 +9525,7 @@
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="B112" s="0" t="n">
         <v>3</v>
@@ -9442,7 +9540,7 @@
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="B113" s="0" t="n">
         <v>4</v>
@@ -9457,7 +9555,7 @@
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="B114" s="0" t="n">
         <v>5</v>
@@ -9472,7 +9570,7 @@
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="B115" s="0" t="n">
         <v>6</v>
@@ -9487,7 +9585,7 @@
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="B116" s="0" t="n">
         <v>7</v>
@@ -9502,7 +9600,7 @@
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="B117" s="0" t="n">
         <v>0</v>
@@ -9517,7 +9615,7 @@
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="B118" s="0" t="n">
         <v>1</v>
@@ -9532,7 +9630,7 @@
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="B119" s="0" t="n">
         <v>2</v>
@@ -9547,7 +9645,7 @@
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="B120" s="0" t="n">
         <v>3</v>
@@ -9562,7 +9660,7 @@
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="B121" s="0" t="n">
         <v>4</v>
@@ -9577,7 +9675,7 @@
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="B122" s="0" t="n">
         <v>5</v>
@@ -9592,7 +9690,7 @@
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="B123" s="0" t="n">
         <v>6</v>
@@ -9607,7 +9705,7 @@
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="B124" s="0" t="n">
         <v>0</v>
@@ -9622,7 +9720,7 @@
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="B125" s="0" t="n">
         <v>1</v>
@@ -9637,7 +9735,7 @@
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="B126" s="0" t="n">
         <v>2</v>
@@ -9652,7 +9750,7 @@
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="B127" s="0" t="n">
         <v>3</v>
@@ -9667,7 +9765,7 @@
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="B128" s="0" t="n">
         <v>4</v>
@@ -9682,7 +9780,7 @@
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="B129" s="0" t="n">
         <v>5</v>
@@ -9697,7 +9795,7 @@
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="B130" s="0" t="n">
         <v>6</v>
@@ -9712,7 +9810,7 @@
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="B131" s="0" t="n">
         <v>7</v>
@@ -9727,7 +9825,7 @@
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="B132" s="0" t="n">
         <v>0</v>
@@ -9742,7 +9840,7 @@
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="B133" s="0" t="n">
         <v>1</v>
@@ -9757,7 +9855,7 @@
     </row>
     <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="B134" s="0" t="n">
         <v>2</v>
@@ -9772,7 +9870,7 @@
     </row>
     <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="B135" s="0" t="n">
         <v>3</v>
@@ -9787,7 +9885,7 @@
     </row>
     <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="B136" s="0" t="n">
         <v>4</v>
@@ -9802,7 +9900,7 @@
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="B137" s="0" t="n">
         <v>5</v>
@@ -9817,7 +9915,7 @@
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="6" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="B138" s="0" t="n">
         <v>3</v>
@@ -9832,7 +9930,7 @@
     </row>
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="B139" s="0" t="n">
         <v>4</v>
@@ -9847,7 +9945,7 @@
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="B140" s="0" t="n">
         <v>5</v>
@@ -9862,7 +9960,7 @@
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="B141" s="0" t="n">
         <v>6</v>
@@ -9877,7 +9975,7 @@
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="B142" s="0" t="n">
         <v>7</v>
@@ -9892,7 +9990,7 @@
     </row>
     <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="B143" s="0" t="n">
         <v>7</v>
@@ -9907,7 +10005,7 @@
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="B144" s="0" t="n">
         <v>3</v>
@@ -9922,7 +10020,7 @@
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="B145" s="0" t="n">
         <v>4</v>
@@ -9937,7 +10035,7 @@
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="B146" s="0" t="n">
         <v>5</v>
@@ -9952,7 +10050,7 @@
     </row>
     <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="B147" s="0" t="n">
         <v>5</v>
@@ -9967,7 +10065,7 @@
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="B148" s="0" t="n">
         <v>6</v>
@@ -9982,7 +10080,7 @@
     </row>
     <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="B149" s="0" t="n">
         <v>7</v>
@@ -9997,7 +10095,7 @@
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="B150" s="0" t="n">
         <v>0</v>
@@ -10012,7 +10110,7 @@
     </row>
     <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="B151" s="0" t="n">
         <v>1</v>
@@ -10027,7 +10125,7 @@
     </row>
     <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="B152" s="0" t="n">
         <v>2</v>
@@ -10042,7 +10140,7 @@
     </row>
     <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="B153" s="0" t="n">
         <v>3</v>
@@ -10057,7 +10155,7 @@
     </row>
     <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="B154" s="0" t="n">
         <v>4</v>
@@ -10072,7 +10170,7 @@
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="B155" s="0" t="n">
         <v>5</v>
@@ -10087,7 +10185,7 @@
     </row>
     <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="B156" s="0" t="n">
         <v>6</v>
@@ -10102,7 +10200,7 @@
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="B157" s="0" t="n">
         <v>7</v>
@@ -10117,7 +10215,7 @@
     </row>
     <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="B158" s="0" t="n">
         <v>0</v>
@@ -10132,7 +10230,7 @@
     </row>
     <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="B159" s="0" t="n">
         <v>1</v>
@@ -10147,7 +10245,7 @@
     </row>
     <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="B160" s="0" t="n">
         <v>6</v>
@@ -10162,7 +10260,7 @@
     </row>
     <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="B161" s="0" t="n">
         <v>7</v>
@@ -10177,7 +10275,7 @@
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="B162" s="0" t="n">
         <v>0</v>
@@ -10192,7 +10290,7 @@
     </row>
     <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="B163" s="0" t="n">
         <v>1</v>
@@ -10207,7 +10305,7 @@
     </row>
     <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="B164" s="0" t="n">
         <v>2</v>
@@ -10222,7 +10320,7 @@
     </row>
     <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="B165" s="0" t="n">
         <v>6</v>
@@ -10237,7 +10335,7 @@
     </row>
     <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="B166" s="0" t="n">
         <v>7</v>
@@ -10252,7 +10350,7 @@
     </row>
     <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="B167" s="0" t="n">
         <v>0</v>
@@ -10267,7 +10365,7 @@
     </row>
     <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="B168" s="0" t="n">
         <v>1</v>
@@ -10282,7 +10380,7 @@
     </row>
     <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="B169" s="0" t="n">
         <v>2</v>
@@ -10297,7 +10395,7 @@
     </row>
     <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="B170" s="0" t="n">
         <v>3</v>
@@ -10312,7 +10410,7 @@
     </row>
     <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="B171" s="0" t="n">
         <v>4</v>
@@ -10327,7 +10425,7 @@
     </row>
     <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="B172" s="0" t="n">
         <v>2</v>
@@ -10342,7 +10440,7 @@
     </row>
     <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="B173" s="0" t="n">
         <v>3</v>
@@ -10357,7 +10455,7 @@
     </row>
     <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="B174" s="0" t="n">
         <v>4</v>
@@ -10372,7 +10470,7 @@
     </row>
     <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="B175" s="0" t="n">
         <v>5</v>
@@ -10387,7 +10485,7 @@
     </row>
     <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="B176" s="0" t="n">
         <v>6</v>
@@ -10402,7 +10500,7 @@
     </row>
     <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="B177" s="0" t="n">
         <v>7</v>
@@ -10417,7 +10515,7 @@
     </row>
     <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="B178" s="0" t="n">
         <v>0</v>
@@ -10432,7 +10530,7 @@
     </row>
     <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="B179" s="0" t="n">
         <v>1</v>
@@ -10447,7 +10545,7 @@
     </row>
     <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="B180" s="0" t="n">
         <v>2</v>
@@ -10462,7 +10560,7 @@
     </row>
     <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="B181" s="0" t="n">
         <v>3</v>
@@ -10477,7 +10575,7 @@
     </row>
     <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="B182" s="0" t="n">
         <v>4</v>
@@ -10492,7 +10590,7 @@
     </row>
     <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="0" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="B183" s="0" t="n">
         <v>5</v>
@@ -10507,7 +10605,7 @@
     </row>
     <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="0" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="B184" s="0" t="n">
         <v>6</v>
@@ -10522,7 +10620,7 @@
     </row>
     <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="B185" s="0" t="n">
         <v>7</v>
@@ -10537,7 +10635,7 @@
     </row>
     <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="B186" s="0" t="n">
         <v>0</v>
@@ -10552,7 +10650,7 @@
     </row>
     <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="0" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="B187" s="0" t="n">
         <v>1</v>
@@ -10567,7 +10665,7 @@
     </row>
     <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="0" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="B188" s="0" t="n">
         <v>2</v>
@@ -10582,7 +10680,7 @@
     </row>
     <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="0" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="B189" s="0" t="n">
         <v>3</v>
@@ -10597,7 +10695,7 @@
     </row>
     <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="0" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="B190" s="0" t="n">
         <v>4</v>
@@ -10612,7 +10710,7 @@
     </row>
     <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="0" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="B191" s="0" t="n">
         <v>5</v>
@@ -10627,7 +10725,7 @@
     </row>
     <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="0" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="B192" s="0" t="n">
         <v>6</v>
@@ -10642,7 +10740,7 @@
     </row>
     <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="0" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="B193" s="0" t="n">
         <v>7</v>
@@ -10657,7 +10755,7 @@
     </row>
     <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="0" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="B194" s="0" t="n">
         <v>0</v>
@@ -10672,7 +10770,7 @@
     </row>
     <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="0" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="B195" s="0" t="n">
         <v>1</v>
@@ -10687,7 +10785,7 @@
     </row>
     <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="0" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="B196" s="0" t="n">
         <v>2</v>
@@ -10702,7 +10800,7 @@
     </row>
     <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="0" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="B197" s="0" t="n">
         <v>3</v>
@@ -10717,7 +10815,7 @@
     </row>
     <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="0" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="B198" s="0" t="n">
         <v>4</v>
@@ -10732,7 +10830,7 @@
     </row>
     <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="0" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="B199" s="0" t="n">
         <v>2</v>
@@ -10747,7 +10845,7 @@
     </row>
     <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="B200" s="0" t="n">
         <v>3</v>
@@ -10762,7 +10860,7 @@
     </row>
     <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="0" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="B201" s="0" t="n">
         <v>4</v>
@@ -10777,7 +10875,7 @@
     </row>
     <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="0" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="B202" s="0" t="n">
         <v>5</v>
@@ -10792,7 +10890,7 @@
     </row>
     <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="0" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="B203" s="0" t="n">
         <v>6</v>
@@ -10807,7 +10905,7 @@
     </row>
     <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="0" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="B204" s="0" t="n">
         <v>1</v>
@@ -10822,7 +10920,7 @@
     </row>
     <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="0" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="B205" s="0" t="n">
         <v>5</v>
@@ -10837,7 +10935,7 @@
     </row>
     <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="0" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="B206" s="0" t="n">
         <v>6</v>
@@ -10852,7 +10950,7 @@
     </row>
     <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="0" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="B207" s="0" t="n">
         <v>7</v>
@@ -10867,7 +10965,7 @@
     </row>
     <row r="208" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="0" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="B208" s="0" t="n">
         <v>0</v>
@@ -10882,7 +10980,7 @@
     </row>
     <row r="209" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="0" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="B209" s="0" t="n">
         <v>3</v>
@@ -10897,7 +10995,7 @@
     </row>
     <row r="210" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="0" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="B210" s="0" t="n">
         <v>5</v>
@@ -10912,7 +11010,7 @@
     </row>
     <row r="211" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="0" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="B211" s="0" t="n">
         <v>6</v>
@@ -10927,7 +11025,7 @@
     </row>
     <row r="212" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="0" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="B212" s="0" t="n">
         <v>7</v>
@@ -10942,7 +11040,7 @@
     </row>
     <row r="213" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="0" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="B213" s="0" t="n">
         <v>0</v>
@@ -10957,7 +11055,7 @@
     </row>
     <row r="214" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="0" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="B214" s="0" t="n">
         <v>1</v>
@@ -10972,7 +11070,7 @@
     </row>
     <row r="215" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="0" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="B215" s="0" t="n">
         <v>2</v>
@@ -10987,7 +11085,7 @@
     </row>
     <row r="216" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="0" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="B216" s="0" t="n">
         <v>4</v>
@@ -11001,453 +11099,753 @@
       </c>
     </row>
     <row r="217" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A217" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="B217" s="0" t="n">
+        <v>6</v>
+      </c>
       <c r="C217" s="4" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="D217" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C217, Levels!B:B, 0), 1, 1)),", ",IF(A217 &lt;&gt; "", """mem"": bit" &amp; B217 &amp; "(" &amp; A217 &amp; "),", ""),"""good"": ",IF(A217 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A217 &lt;&gt; "", A217, -1),", ""bit"": ",IF(B217 &lt;&gt; "", B217, -1),"},")</f>
-        <v>216: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>216: { "levelId": 11, "mem": bit6(0x2249e5),"good": 1, "addr": 0x2249e5, "bit": 6},</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A218" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="B218" s="0" t="n">
+        <v>7</v>
+      </c>
       <c r="C218" s="4" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="D218" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C218, Levels!B:B, 0), 1, 1)),", ",IF(A218 &lt;&gt; "", """mem"": bit" &amp; B218 &amp; "(" &amp; A218 &amp; "),", ""),"""good"": ",IF(A218 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A218 &lt;&gt; "", A218, -1),", ""bit"": ",IF(B218 &lt;&gt; "", B218, -1),"},")</f>
-        <v>217: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>217: { "levelId": 11, "mem": bit7(0x2249e5),"good": 1, "addr": 0x2249e5, "bit": 7},</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A219" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="B219" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="C219" s="4" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="D219" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C219, Levels!B:B, 0), 1, 1)),", ",IF(A219 &lt;&gt; "", """mem"": bit" &amp; B219 &amp; "(" &amp; A219 &amp; "),", ""),"""good"": ",IF(A219 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A219 &lt;&gt; "", A219, -1),", ""bit"": ",IF(B219 &lt;&gt; "", B219, -1),"},")</f>
-        <v>218: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>218: { "levelId": 11, "mem": bit0(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 0},</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A220" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="B220" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="C220" s="4" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="D220" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C220, Levels!B:B, 0), 1, 1)),", ",IF(A220 &lt;&gt; "", """mem"": bit" &amp; B220 &amp; "(" &amp; A220 &amp; "),", ""),"""good"": ",IF(A220 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A220 &lt;&gt; "", A220, -1),", ""bit"": ",IF(B220 &lt;&gt; "", B220, -1),"},")</f>
-        <v>219: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>219: { "levelId": 11, "mem": bit1(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 1},</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A221" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="B221" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="C221" s="4" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="D221" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C221, Levels!B:B, 0), 1, 1)),", ",IF(A221 &lt;&gt; "", """mem"": bit" &amp; B221 &amp; "(" &amp; A221 &amp; "),", ""),"""good"": ",IF(A221 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A221 &lt;&gt; "", A221, -1),", ""bit"": ",IF(B221 &lt;&gt; "", B221, -1),"},")</f>
-        <v>220: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>220: { "levelId": 11, "mem": bit2(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 2},</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A222" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="B222" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="C222" s="4" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="D222" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C222, Levels!B:B, 0), 1, 1)),", ",IF(A222 &lt;&gt; "", """mem"": bit" &amp; B222 &amp; "(" &amp; A222 &amp; "),", ""),"""good"": ",IF(A222 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A222 &lt;&gt; "", A222, -1),", ""bit"": ",IF(B222 &lt;&gt; "", B222, -1),"},")</f>
-        <v>221: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>221: { "levelId": 11, "mem": bit3(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 3},</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A223" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="B223" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="C223" s="4" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="D223" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C223, Levels!B:B, 0), 1, 1)),", ",IF(A223 &lt;&gt; "", """mem"": bit" &amp; B223 &amp; "(" &amp; A223 &amp; "),", ""),"""good"": ",IF(A223 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A223 &lt;&gt; "", A223, -1),", ""bit"": ",IF(B223 &lt;&gt; "", B223, -1),"},")</f>
-        <v>222: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>222: { "levelId": 11, "mem": bit4(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 4},</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A224" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="B224" s="0" t="n">
+        <v>5</v>
+      </c>
       <c r="C224" s="4" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="D224" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C224, Levels!B:B, 0), 1, 1)),", ",IF(A224 &lt;&gt; "", """mem"": bit" &amp; B224 &amp; "(" &amp; A224 &amp; "),", ""),"""good"": ",IF(A224 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A224 &lt;&gt; "", A224, -1),", ""bit"": ",IF(B224 &lt;&gt; "", B224, -1),"},")</f>
-        <v>223: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>223: { "levelId": 11, "mem": bit5(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 5},</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A225" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="B225" s="0" t="n">
+        <v>6</v>
+      </c>
       <c r="C225" s="4" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="D225" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C225, Levels!B:B, 0), 1, 1)),", ",IF(A225 &lt;&gt; "", """mem"": bit" &amp; B225 &amp; "(" &amp; A225 &amp; "),", ""),"""good"": ",IF(A225 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A225 &lt;&gt; "", A225, -1),", ""bit"": ",IF(B225 &lt;&gt; "", B225, -1),"},")</f>
-        <v>224: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>224: { "levelId": 11, "mem": bit6(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 6},</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A226" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="B226" s="0" t="n">
+        <v>7</v>
+      </c>
       <c r="C226" s="4" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="D226" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C226, Levels!B:B, 0), 1, 1)),", ",IF(A226 &lt;&gt; "", """mem"": bit" &amp; B226 &amp; "(" &amp; A226 &amp; "),", ""),"""good"": ",IF(A226 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A226 &lt;&gt; "", A226, -1),", ""bit"": ",IF(B226 &lt;&gt; "", B226, -1),"},")</f>
-        <v>225: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>225: { "levelId": 11, "mem": bit7(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 7},</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A227" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="B227" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="C227" s="4" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="D227" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C227, Levels!B:B, 0), 1, 1)),", ",IF(A227 &lt;&gt; "", """mem"": bit" &amp; B227 &amp; "(" &amp; A227 &amp; "),", ""),"""good"": ",IF(A227 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A227 &lt;&gt; "", A227, -1),", ""bit"": ",IF(B227 &lt;&gt; "", B227, -1),"},")</f>
-        <v>226: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>226: { "levelId": 11, "mem": bit0(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 0},</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A228" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="B228" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="C228" s="4" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="D228" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C228, Levels!B:B, 0), 1, 1)),", ",IF(A228 &lt;&gt; "", """mem"": bit" &amp; B228 &amp; "(" &amp; A228 &amp; "),", ""),"""good"": ",IF(A228 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A228 &lt;&gt; "", A228, -1),", ""bit"": ",IF(B228 &lt;&gt; "", B228, -1),"},")</f>
-        <v>227: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>227: { "levelId": 11, "mem": bit1(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 1},</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A229" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="B229" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="C229" s="4" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="D229" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C229, Levels!B:B, 0), 1, 1)),", ",IF(A229 &lt;&gt; "", """mem"": bit" &amp; B229 &amp; "(" &amp; A229 &amp; "),", ""),"""good"": ",IF(A229 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A229 &lt;&gt; "", A229, -1),", ""bit"": ",IF(B229 &lt;&gt; "", B229, -1),"},")</f>
-        <v>228: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>228: { "levelId": 11, "mem": bit2(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 2},</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A230" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="B230" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="C230" s="4" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="D230" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C230, Levels!B:B, 0), 1, 1)),", ",IF(A230 &lt;&gt; "", """mem"": bit" &amp; B230 &amp; "(" &amp; A230 &amp; "),", ""),"""good"": ",IF(A230 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A230 &lt;&gt; "", A230, -1),", ""bit"": ",IF(B230 &lt;&gt; "", B230, -1),"},")</f>
-        <v>229: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>229: { "levelId": 11, "mem": bit3(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 3},</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A231" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="B231" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="C231" s="4" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="D231" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C231, Levels!B:B, 0), 1, 1)),", ",IF(A231 &lt;&gt; "", """mem"": bit" &amp; B231 &amp; "(" &amp; A231 &amp; "),", ""),"""good"": ",IF(A231 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A231 &lt;&gt; "", A231, -1),", ""bit"": ",IF(B231 &lt;&gt; "", B231, -1),"},")</f>
-        <v>230: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>230: { "levelId": 11, "mem": bit4(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 4},</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A232" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="B232" s="0" t="n">
+        <v>5</v>
+      </c>
       <c r="C232" s="4" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="D232" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C232, Levels!B:B, 0), 1, 1)),", ",IF(A232 &lt;&gt; "", """mem"": bit" &amp; B232 &amp; "(" &amp; A232 &amp; "),", ""),"""good"": ",IF(A232 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A232 &lt;&gt; "", A232, -1),", ""bit"": ",IF(B232 &lt;&gt; "", B232, -1),"},")</f>
-        <v>231: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>231: { "levelId": 11, "mem": bit5(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 5},</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A233" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="B233" s="0" t="n">
+        <v>6</v>
+      </c>
       <c r="C233" s="4" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="D233" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C233, Levels!B:B, 0), 1, 1)),", ",IF(A233 &lt;&gt; "", """mem"": bit" &amp; B233 &amp; "(" &amp; A233 &amp; "),", ""),"""good"": ",IF(A233 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A233 &lt;&gt; "", A233, -1),", ""bit"": ",IF(B233 &lt;&gt; "", B233, -1),"},")</f>
-        <v>232: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>232: { "levelId": 11, "mem": bit6(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 6},</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A234" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="B234" s="0" t="n">
+        <v>7</v>
+      </c>
       <c r="C234" s="4" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="D234" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C234, Levels!B:B, 0), 1, 1)),", ",IF(A234 &lt;&gt; "", """mem"": bit" &amp; B234 &amp; "(" &amp; A234 &amp; "),", ""),"""good"": ",IF(A234 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A234 &lt;&gt; "", A234, -1),", ""bit"": ",IF(B234 &lt;&gt; "", B234, -1),"},")</f>
-        <v>233: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>233: { "levelId": 11, "mem": bit7(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 7},</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A235" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="B235" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="C235" s="4" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="D235" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C235, Levels!B:B, 0), 1, 1)),", ",IF(A235 &lt;&gt; "", """mem"": bit" &amp; B235 &amp; "(" &amp; A235 &amp; "),", ""),"""good"": ",IF(A235 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A235 &lt;&gt; "", A235, -1),", ""bit"": ",IF(B235 &lt;&gt; "", B235, -1),"},")</f>
-        <v>234: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>234: { "levelId": 11, "mem": bit0(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 0},</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A236" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="B236" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="C236" s="4" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="D236" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C236, Levels!B:B, 0), 1, 1)),", ",IF(A236 &lt;&gt; "", """mem"": bit" &amp; B236 &amp; "(" &amp; A236 &amp; "),", ""),"""good"": ",IF(A236 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A236 &lt;&gt; "", A236, -1),", ""bit"": ",IF(B236 &lt;&gt; "", B236, -1),"},")</f>
-        <v>235: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>235: { "levelId": 11, "mem": bit1(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 1},</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A237" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="B237" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="C237" s="4" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="D237" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C237, Levels!B:B, 0), 1, 1)),", ",IF(A237 &lt;&gt; "", """mem"": bit" &amp; B237 &amp; "(" &amp; A237 &amp; "),", ""),"""good"": ",IF(A237 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A237 &lt;&gt; "", A237, -1),", ""bit"": ",IF(B237 &lt;&gt; "", B237, -1),"},")</f>
-        <v>236: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>236: { "levelId": 11, "mem": bit2(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 2},</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A238" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="B238" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="C238" s="4" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="D238" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C238, Levels!B:B, 0), 1, 1)),", ",IF(A238 &lt;&gt; "", """mem"": bit" &amp; B238 &amp; "(" &amp; A238 &amp; "),", ""),"""good"": ",IF(A238 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A238 &lt;&gt; "", A238, -1),", ""bit"": ",IF(B238 &lt;&gt; "", B238, -1),"},")</f>
-        <v>237: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>237: { "levelId": 11, "mem": bit3(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 3},</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A239" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="B239" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="C239" s="4" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="D239" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C239, Levels!B:B, 0), 1, 1)),", ",IF(A239 &lt;&gt; "", """mem"": bit" &amp; B239 &amp; "(" &amp; A239 &amp; "),", ""),"""good"": ",IF(A239 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A239 &lt;&gt; "", A239, -1),", ""bit"": ",IF(B239 &lt;&gt; "", B239, -1),"},")</f>
-        <v>238: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>238: { "levelId": 11, "mem": bit4(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 4},</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A240" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="B240" s="0" t="n">
+        <v>5</v>
+      </c>
       <c r="C240" s="4" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="D240" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C240, Levels!B:B, 0), 1, 1)),", ",IF(A240 &lt;&gt; "", """mem"": bit" &amp; B240 &amp; "(" &amp; A240 &amp; "),", ""),"""good"": ",IF(A240 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A240 &lt;&gt; "", A240, -1),", ""bit"": ",IF(B240 &lt;&gt; "", B240, -1),"},")</f>
-        <v>239: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>239: { "levelId": 11, "mem": bit5(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 5},</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A241" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="B241" s="0" t="n">
+        <v>6</v>
+      </c>
       <c r="C241" s="4" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="D241" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C241, Levels!B:B, 0), 1, 1)),", ",IF(A241 &lt;&gt; "", """mem"": bit" &amp; B241 &amp; "(" &amp; A241 &amp; "),", ""),"""good"": ",IF(A241 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A241 &lt;&gt; "", A241, -1),", ""bit"": ",IF(B241 &lt;&gt; "", B241, -1),"},")</f>
-        <v>240: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>240: { "levelId": 11, "mem": bit6(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 6},</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A242" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="B242" s="0" t="n">
+        <v>7</v>
+      </c>
       <c r="C242" s="4" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="D242" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C242, Levels!B:B, 0), 1, 1)),", ",IF(A242 &lt;&gt; "", """mem"": bit" &amp; B242 &amp; "(" &amp; A242 &amp; "),", ""),"""good"": ",IF(A242 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A242 &lt;&gt; "", A242, -1),", ""bit"": ",IF(B242 &lt;&gt; "", B242, -1),"},")</f>
-        <v>241: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>241: { "levelId": 11, "mem": bit7(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 7},</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A243" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="B243" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="C243" s="4" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="D243" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C243, Levels!B:B, 0), 1, 1)),", ",IF(A243 &lt;&gt; "", """mem"": bit" &amp; B243 &amp; "(" &amp; A243 &amp; "),", ""),"""good"": ",IF(A243 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A243 &lt;&gt; "", A243, -1),", ""bit"": ",IF(B243 &lt;&gt; "", B243, -1),"},")</f>
-        <v>242: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>242: { "levelId": 11, "mem": bit0(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 0},</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A244" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="B244" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="C244" s="4" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="D244" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C244, Levels!B:B, 0), 1, 1)),", ",IF(A244 &lt;&gt; "", """mem"": bit" &amp; B244 &amp; "(" &amp; A244 &amp; "),", ""),"""good"": ",IF(A244 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A244 &lt;&gt; "", A244, -1),", ""bit"": ",IF(B244 &lt;&gt; "", B244, -1),"},")</f>
-        <v>243: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>243: { "levelId": 11, "mem": bit1(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 1},</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A245" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="B245" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="C245" s="4" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="D245" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C245, Levels!B:B, 0), 1, 1)),", ",IF(A245 &lt;&gt; "", """mem"": bit" &amp; B245 &amp; "(" &amp; A245 &amp; "),", ""),"""good"": ",IF(A245 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A245 &lt;&gt; "", A245, -1),", ""bit"": ",IF(B245 &lt;&gt; "", B245, -1),"},")</f>
-        <v>244: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>244: { "levelId": 11, "mem": bit2(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 2},</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A246" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="B246" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="C246" s="4" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="D246" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C246, Levels!B:B, 0), 1, 1)),", ",IF(A246 &lt;&gt; "", """mem"": bit" &amp; B246 &amp; "(" &amp; A246 &amp; "),", ""),"""good"": ",IF(A246 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A246 &lt;&gt; "", A246, -1),", ""bit"": ",IF(B246 &lt;&gt; "", B246, -1),"},")</f>
-        <v>245: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>245: { "levelId": 11, "mem": bit3(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 3},</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A247" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="B247" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="C247" s="4" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="D247" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C247, Levels!B:B, 0), 1, 1)),", ",IF(A247 &lt;&gt; "", """mem"": bit" &amp; B247 &amp; "(" &amp; A247 &amp; "),", ""),"""good"": ",IF(A247 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A247 &lt;&gt; "", A247, -1),", ""bit"": ",IF(B247 &lt;&gt; "", B247, -1),"},")</f>
-        <v>246: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>246: { "levelId": 11, "mem": bit4(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 4},</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A248" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="B248" s="0" t="n">
+        <v>5</v>
+      </c>
       <c r="C248" s="4" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="D248" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C248, Levels!B:B, 0), 1, 1)),", ",IF(A248 &lt;&gt; "", """mem"": bit" &amp; B248 &amp; "(" &amp; A248 &amp; "),", ""),"""good"": ",IF(A248 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A248 &lt;&gt; "", A248, -1),", ""bit"": ",IF(B248 &lt;&gt; "", B248, -1),"},")</f>
-        <v>247: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>247: { "levelId": 11, "mem": bit5(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 5},</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A249" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="B249" s="0" t="n">
+        <v>6</v>
+      </c>
       <c r="C249" s="4" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="D249" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C249, Levels!B:B, 0), 1, 1)),", ",IF(A249 &lt;&gt; "", """mem"": bit" &amp; B249 &amp; "(" &amp; A249 &amp; "),", ""),"""good"": ",IF(A249 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A249 &lt;&gt; "", A249, -1),", ""bit"": ",IF(B249 &lt;&gt; "", B249, -1),"},")</f>
-        <v>248: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>248: { "levelId": 11, "mem": bit6(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 6},</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A250" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="B250" s="0" t="n">
+        <v>7</v>
+      </c>
       <c r="C250" s="4" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="D250" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C250, Levels!B:B, 0), 1, 1)),", ",IF(A250 &lt;&gt; "", """mem"": bit" &amp; B250 &amp; "(" &amp; A250 &amp; "),", ""),"""good"": ",IF(A250 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A250 &lt;&gt; "", A250, -1),", ""bit"": ",IF(B250 &lt;&gt; "", B250, -1),"},")</f>
-        <v>249: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>249: { "levelId": 11, "mem": bit7(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 7},</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A251" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="B251" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="C251" s="4" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="D251" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C251, Levels!B:B, 0), 1, 1)),", ",IF(A251 &lt;&gt; "", """mem"": bit" &amp; B251 &amp; "(" &amp; A251 &amp; "),", ""),"""good"": ",IF(A251 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A251 &lt;&gt; "", A251, -1),", ""bit"": ",IF(B251 &lt;&gt; "", B251, -1),"},")</f>
-        <v>250: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>250: { "levelId": 11, "mem": bit0(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 0},</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A252" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="B252" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="C252" s="4" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="D252" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C252, Levels!B:B, 0), 1, 1)),", ",IF(A252 &lt;&gt; "", """mem"": bit" &amp; B252 &amp; "(" &amp; A252 &amp; "),", ""),"""good"": ",IF(A252 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A252 &lt;&gt; "", A252, -1),", ""bit"": ",IF(B252 &lt;&gt; "", B252, -1),"},")</f>
-        <v>251: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>251: { "levelId": 11, "mem": bit1(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 1},</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A253" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="B253" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="C253" s="4" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="D253" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C253, Levels!B:B, 0), 1, 1)),", ",IF(A253 &lt;&gt; "", """mem"": bit" &amp; B253 &amp; "(" &amp; A253 &amp; "),", ""),"""good"": ",IF(A253 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A253 &lt;&gt; "", A253, -1),", ""bit"": ",IF(B253 &lt;&gt; "", B253, -1),"},")</f>
-        <v>252: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>252: { "levelId": 11, "mem": bit2(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 2},</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A254" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="B254" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="C254" s="4" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="D254" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C254, Levels!B:B, 0), 1, 1)),", ",IF(A254 &lt;&gt; "", """mem"": bit" &amp; B254 &amp; "(" &amp; A254 &amp; "),", ""),"""good"": ",IF(A254 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A254 &lt;&gt; "", A254, -1),", ""bit"": ",IF(B254 &lt;&gt; "", B254, -1),"},")</f>
-        <v>253: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>253: { "levelId": 11, "mem": bit3(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 3},</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A255" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="B255" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="C255" s="4" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="D255" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C255, Levels!B:B, 0), 1, 1)),", ",IF(A255 &lt;&gt; "", """mem"": bit" &amp; B255 &amp; "(" &amp; A255 &amp; "),", ""),"""good"": ",IF(A255 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A255 &lt;&gt; "", A255, -1),", ""bit"": ",IF(B255 &lt;&gt; "", B255, -1),"},")</f>
-        <v>254: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>254: { "levelId": 11, "mem": bit4(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 4},</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A256" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="B256" s="0" t="n">
+        <v>5</v>
+      </c>
       <c r="C256" s="4" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="D256" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C256, Levels!B:B, 0), 1, 1)),", ",IF(A256 &lt;&gt; "", """mem"": bit" &amp; B256 &amp; "(" &amp; A256 &amp; "),", ""),"""good"": ",IF(A256 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A256 &lt;&gt; "", A256, -1),", ""bit"": ",IF(B256 &lt;&gt; "", B256, -1),"},")</f>
-        <v>255: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>255: { "levelId": 11, "mem": bit5(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 5},</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A257" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="B257" s="0" t="n">
+        <v>6</v>
+      </c>
       <c r="C257" s="4" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="D257" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C257, Levels!B:B, 0), 1, 1)),", ",IF(A257 &lt;&gt; "", """mem"": bit" &amp; B257 &amp; "(" &amp; A257 &amp; "),", ""),"""good"": ",IF(A257 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A257 &lt;&gt; "", A257, -1),", ""bit"": ",IF(B257 &lt;&gt; "", B257, -1),"},")</f>
-        <v>256: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>256: { "levelId": 11, "mem": bit6(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 6},</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A258" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="B258" s="0" t="n">
+        <v>7</v>
+      </c>
       <c r="C258" s="4" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="D258" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C258, Levels!B:B, 0), 1, 1)),", ",IF(A258 &lt;&gt; "", """mem"": bit" &amp; B258 &amp; "(" &amp; A258 &amp; "),", ""),"""good"": ",IF(A258 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A258 &lt;&gt; "", A258, -1),", ""bit"": ",IF(B258 &lt;&gt; "", B258, -1),"},")</f>
-        <v>257: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>257: { "levelId": 11, "mem": bit7(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 7},</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A259" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="B259" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="C259" s="4" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="D259" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C259, Levels!B:B, 0), 1, 1)),", ",IF(A259 &lt;&gt; "", """mem"": bit" &amp; B259 &amp; "(" &amp; A259 &amp; "),", ""),"""good"": ",IF(A259 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A259 &lt;&gt; "", A259, -1),", ""bit"": ",IF(B259 &lt;&gt; "", B259, -1),"},")</f>
-        <v>258: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>258: { "levelId": 11, "mem": bit0(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 0},</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A260" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="B260" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="C260" s="4" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="D260" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C260, Levels!B:B, 0), 1, 1)),", ",IF(A260 &lt;&gt; "", """mem"": bit" &amp; B260 &amp; "(" &amp; A260 &amp; "),", ""),"""good"": ",IF(A260 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A260 &lt;&gt; "", A260, -1),", ""bit"": ",IF(B260 &lt;&gt; "", B260, -1),"},")</f>
-        <v>259: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>259: { "levelId": 11, "mem": bit1(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 1},</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A261" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="B261" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="C261" s="4" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="D261" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C261, Levels!B:B, 0), 1, 1)),", ",IF(A261 &lt;&gt; "", """mem"": bit" &amp; B261 &amp; "(" &amp; A261 &amp; "),", ""),"""good"": ",IF(A261 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A261 &lt;&gt; "", A261, -1),", ""bit"": ",IF(B261 &lt;&gt; "", B261, -1),"},")</f>
-        <v>260: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>260: { "levelId": 11, "mem": bit2(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 2},</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A262" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="B262" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="C262" s="4" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="D262" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C262, Levels!B:B, 0), 1, 1)),", ",IF(A262 &lt;&gt; "", """mem"": bit" &amp; B262 &amp; "(" &amp; A262 &amp; "),", ""),"""good"": ",IF(A262 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A262 &lt;&gt; "", A262, -1),", ""bit"": ",IF(B262 &lt;&gt; "", B262, -1),"},")</f>
-        <v>261: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>261: { "levelId": 11, "mem": bit3(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 3},</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A263" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="B263" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="C263" s="4" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="D263" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C263, Levels!B:B, 0), 1, 1)),", ",IF(A263 &lt;&gt; "", """mem"": bit" &amp; B263 &amp; "(" &amp; A263 &amp; "),", ""),"""good"": ",IF(A263 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A263 &lt;&gt; "", A263, -1),", ""bit"": ",IF(B263 &lt;&gt; "", B263, -1),"},")</f>
-        <v>262: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>262: { "levelId": 11, "mem": bit4(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 4},</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A264" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="B264" s="0" t="n">
+        <v>5</v>
+      </c>
       <c r="C264" s="4" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="D264" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C264, Levels!B:B, 0), 1, 1)),", ",IF(A264 &lt;&gt; "", """mem"": bit" &amp; B264 &amp; "(" &amp; A264 &amp; "),", ""),"""good"": ",IF(A264 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A264 &lt;&gt; "", A264, -1),", ""bit"": ",IF(B264 &lt;&gt; "", B264, -1),"},")</f>
-        <v>263: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>263: { "levelId": 11, "mem": bit5(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 5},</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A265" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="B265" s="0" t="n">
+        <v>6</v>
+      </c>
       <c r="C265" s="4" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="D265" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C265, Levels!B:B, 0), 1, 1)),", ",IF(A265 &lt;&gt; "", """mem"": bit" &amp; B265 &amp; "(" &amp; A265 &amp; "),", ""),"""good"": ",IF(A265 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A265 &lt;&gt; "", A265, -1),", ""bit"": ",IF(B265 &lt;&gt; "", B265, -1),"},")</f>
-        <v>264: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>264: { "levelId": 11, "mem": bit6(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 6},</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A266" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="B266" s="0" t="n">
+        <v>7</v>
+      </c>
       <c r="C266" s="4" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="D266" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C266, Levels!B:B, 0), 1, 1)),", ",IF(A266 &lt;&gt; "", """mem"": bit" &amp; B266 &amp; "(" &amp; A266 &amp; "),", ""),"""good"": ",IF(A266 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A266 &lt;&gt; "", A266, -1),", ""bit"": ",IF(B266 &lt;&gt; "", B266, -1),"},")</f>
-        <v>265: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>265: { "levelId": 11, "mem": bit7(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 7},</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18095,7 +18493,7 @@
       <selection pane="bottomLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.93"/>
@@ -18105,13 +18503,13 @@
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>4</v>
@@ -18122,7 +18520,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>110</v>
+        <v>125</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>7</v>
@@ -18141,7 +18539,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>111</v>
+        <v>126</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0</v>
@@ -18156,7 +18554,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>111</v>
+        <v>126</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>1</v>
@@ -18171,7 +18569,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>111</v>
+        <v>126</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>5</v>
@@ -18186,7 +18584,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>111</v>
+        <v>126</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>6</v>
@@ -18201,7 +18599,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>111</v>
+        <v>126</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>7</v>
@@ -18216,7 +18614,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>112</v>
+        <v>127</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>0</v>
@@ -18231,7 +18629,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>112</v>
+        <v>127</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>1</v>
@@ -18246,7 +18644,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>112</v>
+        <v>127</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>2</v>
@@ -18261,7 +18659,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>112</v>
+        <v>127</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>3</v>
@@ -18276,7 +18674,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>112</v>
+        <v>127</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>4</v>
@@ -18291,7 +18689,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>112</v>
+        <v>127</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>5</v>
@@ -18306,7 +18704,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>112</v>
+        <v>127</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>7</v>
@@ -18321,7 +18719,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>113</v>
+        <v>128</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>1</v>
@@ -18336,7 +18734,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>112</v>
+        <v>127</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>6</v>
@@ -18351,7 +18749,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>113</v>
+        <v>128</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>0</v>
@@ -18366,7 +18764,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>113</v>
+        <v>128</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>3</v>
@@ -18381,7 +18779,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>113</v>
+        <v>128</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>2</v>
@@ -18396,7 +18794,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>113</v>
+        <v>128</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>5</v>
@@ -18411,7 +18809,7 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>113</v>
+        <v>128</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>4</v>
@@ -18426,7 +18824,7 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>114</v>
+        <v>129</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>0</v>
@@ -18441,7 +18839,7 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>113</v>
+        <v>128</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>6</v>

</xml_diff>

<commit_message>
Refactored the Menhir Hills completionist achievement and updated its title because yikes
</commit_message>
<xml_diff>
--- a/Rayman 2.xlsx
+++ b/Rayman 2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Areas" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1501" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1538" uniqueCount="134">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -259,6 +259,12 @@
     <t xml:space="preserve">BadDreamsArea2</t>
   </si>
   <si>
+    <t xml:space="preserve">75AADC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MenhirArea4</t>
+  </si>
+  <si>
     <t xml:space="preserve">Index</t>
   </si>
   <si>
@@ -395,6 +401,12 @@
   </si>
   <si>
     <t xml:space="preserve">0x2249eb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x2249a6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x2249a7</t>
   </si>
   <si>
     <t xml:space="preserve">Level ID</t>
@@ -626,7 +638,7 @@
       <selection pane="bottomLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.66"/>
@@ -656,7 +668,7 @@
       </c>
       <c r="H1" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(E2:E1000)</f>
-        <v>0x784BFC: { "id": 0x784BFC, "areaName": "Menu", "displayName": "Main Menu", "levelName": "Menu" },0x789668: { "id": 0x789668, "areaName": "Intro", "displayName": "somewhere in the Glade of Dreams…", "levelName": "None" },0x778C74: { "id": 0x778C74, "areaName": "BuccaneerBrig", "displayName": "in the Buccaneer’s brig", "levelName": "None" },0x78D424: { "id": 0x78D424, "areaName": "WoodsOfLight", "displayName": "in the Woods of Light", "levelName": "Woods of Light" },0x790570: { "id": 0x790570, "areaName": "HallOfDoors", "displayName": "in the Hall of Doors", "levelName": "Hall of Doors" },0x7875A8: { "id": 0x7875A8, "areaName": "FairyGladeArea1", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x78A320: { "id": 0x78A320, "areaName": "FairyGladeArea2", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x7A1BD8: { "id": 0x7A1BD8, "areaName": "FairyGladeArea3", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x77BFFC: { "id": 0x77BFFC, "areaName": "FairyGladeArea4", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x771B74: { "id": 0x771B74, "areaName": "FairyGladeArea5", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x74AAA8: { "id": 0x74AAA8, "areaName": "Results", "displayName": "viewing level results…", "levelName": "None" },0x788708: { "id": 0x788708, "areaName": "MarshesArea1", "displayName": "in the Marshes of Awakening", "levelName": "Marshes of Awakening" },0x7786E8: { "id": 0x7786E8, "areaName": "MarshesArea2", "displayName": "in the Marshes of Awakening", "levelName": "Marshes of Awakening" },0x790598: { "id": 0x790598, "areaName": "BayouArea1", "displayName": "in the Bayou", "levelName": "Bayou" },0x788764: { "id": 0x788764, "areaName": "BayouArea2", "displayName": "in the Bayou", "levelName": "Bayou" },0x7928A4: { "id": 0x7928A4, "areaName": "SoWaIArea1", "displayName": "in the Sanctuary of Water and Ice", "levelName": "Sanctuary of Water and Ice" },0x774694: { "id": 0x774694, "areaName": "SoWaIArea2", "displayName": "in the Sanctuary of Water and Ice", "levelName": "Sanctuary of Water and Ice" },0x76F100: { "id": 0x76F100, "areaName": "Polokus", "displayName": "in Polokus’s dream", "levelName": "Polokus" },0x0: { "id": 0x0, "areaName": "None", "displayName": "somewhere in the Glade of Dreams…", "levelName": "None" },0x751974: { "id": 0x751974, "areaName": "Bonus", "displayName": "in the bonus stage", "levelName": "None" },0x776C08: { "id": 0x776C08, "areaName": "MenhirArea1", "displayName": "in the Menhir Hills", "levelName": "Menhir Hills" },0x78FBD8: { "id": 0x78FBD8, "areaName": "MenhirArea2", "displayName": "in the Menhir Hills", "levelName": "Menhir Hills" },0x788950: { "id": 0x788950, "areaName": "MenhirArea3", "displayName": "in the Menhir Hills", "levelName": "Menhir Hills" },0x78402C: { "id": 0x78402C, "areaName": "BadDreamsArea1", "displayName": "in the Cave of Bad Dreams", "levelName": "Cave of Bad Dreams" },0x788148: { "id": 0x788148, "areaName": "BadDreamsArea2", "displayName": "in the Cave of Bad Dreams", "levelName": "Cave of Bad Dreams" },</v>
+        <v>0x784BFC: { "id": 0x784BFC, "areaName": "Menu", "displayName": "Main Menu", "levelName": "Menu" },0x789668: { "id": 0x789668, "areaName": "Intro", "displayName": "somewhere in the Glade of Dreams…", "levelName": "None" },0x778C74: { "id": 0x778C74, "areaName": "BuccaneerBrig", "displayName": "in the Buccaneer’s brig", "levelName": "None" },0x78D424: { "id": 0x78D424, "areaName": "WoodsOfLight", "displayName": "in the Woods of Light", "levelName": "Woods of Light" },0x790570: { "id": 0x790570, "areaName": "HallOfDoors", "displayName": "in the Hall of Doors", "levelName": "Hall of Doors" },0x7875A8: { "id": 0x7875A8, "areaName": "FairyGladeArea1", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x78A320: { "id": 0x78A320, "areaName": "FairyGladeArea2", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x7A1BD8: { "id": 0x7A1BD8, "areaName": "FairyGladeArea3", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x77BFFC: { "id": 0x77BFFC, "areaName": "FairyGladeArea4", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x771B74: { "id": 0x771B74, "areaName": "FairyGladeArea5", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x74AAA8: { "id": 0x74AAA8, "areaName": "Results", "displayName": "viewing level results…", "levelName": "None" },0x788708: { "id": 0x788708, "areaName": "MarshesArea1", "displayName": "in the Marshes of Awakening", "levelName": "Marshes of Awakening" },0x7786E8: { "id": 0x7786E8, "areaName": "MarshesArea2", "displayName": "in the Marshes of Awakening", "levelName": "Marshes of Awakening" },0x790598: { "id": 0x790598, "areaName": "BayouArea1", "displayName": "in the Bayou", "levelName": "Bayou" },0x788764: { "id": 0x788764, "areaName": "BayouArea2", "displayName": "in the Bayou", "levelName": "Bayou" },0x7928A4: { "id": 0x7928A4, "areaName": "SoWaIArea1", "displayName": "in the Sanctuary of Water and Ice", "levelName": "Sanctuary of Water and Ice" },0x774694: { "id": 0x774694, "areaName": "SoWaIArea2", "displayName": "in the Sanctuary of Water and Ice", "levelName": "Sanctuary of Water and Ice" },0x76F100: { "id": 0x76F100, "areaName": "Polokus", "displayName": "in Polokus’s dream", "levelName": "Polokus" },0x0: { "id": 0x0, "areaName": "None", "displayName": "somewhere in the Glade of Dreams…", "levelName": "None" },0x751974: { "id": 0x751974, "areaName": "Bonus", "displayName": "in the bonus stage", "levelName": "None" },0x776C08: { "id": 0x776C08, "areaName": "MenhirArea1", "displayName": "in the Menhir Hills", "levelName": "Menhir Hills" },0x78FBD8: { "id": 0x78FBD8, "areaName": "MenhirArea2", "displayName": "in the Menhir Hills", "levelName": "Menhir Hills" },0x788950: { "id": 0x788950, "areaName": "MenhirArea3", "displayName": "in the Menhir Hills", "levelName": "Menhir Hills" },0x78402C: { "id": 0x78402C, "areaName": "BadDreamsArea1", "displayName": "in the Cave of Bad Dreams", "levelName": "Cave of Bad Dreams" },0x788148: { "id": 0x788148, "areaName": "BadDreamsArea2", "displayName": "in the Cave of Bad Dreams", "levelName": "Cave of Bad Dreams" },0x75AADC: { "id": 0x75AADC, "areaName": "MenhirArea4", "displayName": "in the Menhir Hills", "levelName": "Menhir Hills" },</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1110,7 +1122,22 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D27" s="4"/>
+      <c r="A27" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E27" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("0x", A27,": { ""id"": ","0x", A27,", ""areaName"": """,B27,""", ""displayName"": """,C27,""", ""levelName"": """,D27,""" },")</f>
+        <v>0x75AADC: { "id": 0x75AADC, "areaName": "MenhirArea4", "displayName": "in the Menhir Hills", "levelName": "Menhir Hills" },</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D28" s="4"/>
@@ -4106,7 +4133,7 @@
       <selection pane="bottomLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.21"/>
@@ -4118,22 +4145,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>4</v>
@@ -4209,11 +4236,11 @@
       </c>
       <c r="E4" s="0" t="n">
         <f aca="false">COUNTIFS(Lums!C3:C1002, "=" &amp; B4)</f>
-        <v>735</v>
+        <v>708</v>
       </c>
       <c r="F4" s="0" t="n">
         <f aca="false">COUNTIFS(Cages!C3:C83, "=" &amp; B4)</f>
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="G4" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A4,": { ""id"": ",A4,", ""name"": """,B4,""", ""lums"": ",C4,", ""cages"": ",D4," },")</f>
@@ -4398,11 +4425,11 @@
       </c>
       <c r="E11" s="0" t="n">
         <f aca="false">COUNTIFS(Lums!C10:C1009, "=" &amp; B11)</f>
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="F11" s="0" t="n">
         <f aca="false">COUNTIFS(Cages!C10:C90, "=" &amp; B11)</f>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G11" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A11,": { ""id"": ",A11,", ""name"": """,B11,""", ""lums"": ",C11,", ""cages"": ",D11," },")</f>
@@ -7832,13 +7859,13 @@
   </sheetPr>
   <dimension ref="A1:H1001"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A243" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A266" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C267" activeCellId="0" sqref="C267"/>
+      <selection pane="bottomLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.93"/>
@@ -7847,10 +7874,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>3</v>
@@ -7863,12 +7890,12 @@
       </c>
       <c r="H1" s="5" t="str">
         <f aca="false">_xlfn.CONCAT(D2:D1001)</f>
-        <v>1: { "levelId": 2, "mem": bit0(0x224988),"good": 1, "addr": 0x224988, "bit": 0},2: { "levelId": 2, "mem": bit1(0x224988),"good": 1, "addr": 0x224988, "bit": 1},3: { "levelId": 2, "mem": bit2(0x224988),"good": 1, "addr": 0x224988, "bit": 2},4: { "levelId": 2, "mem": bit3(0x224988),"good": 1, "addr": 0x224988, "bit": 3},5: { "levelId": 2, "mem": bit4(0x224988),"good": 1, "addr": 0x224988, "bit": 4},6: { "levelId": 2, "mem": bit5(0x224988),"good": 1, "addr": 0x224988, "bit": 5},7: { "levelId": 2, "mem": bit6(0x224988),"good": 1, "addr": 0x224988, "bit": 6},8: { "levelId": 2, "mem": bit7(0x224988),"good": 1, "addr": 0x224988, "bit": 7},9: { "levelId": 2, "mem": bit2(0x224989),"good": 1, "addr": 0x224989, "bit": 2},10: { "levelId": 2, "mem": bit1(0x22498a),"good": 1, "addr": 0x22498a, "bit": 1},11: { "levelId": 2, "mem": bit2(0x22498a),"good": 1, "addr": 0x22498a, "bit": 2},12: { "levelId": 2, "mem": bit3(0x22498a),"good": 1, "addr": 0x22498a, "bit": 3},13: { "levelId": 2, "mem": bit4(0x22498a),"good": 1, "addr": 0x22498a, "bit": 4},14: { "levelId": 2, "mem": bit5(0x22498a),"good": 1, "addr": 0x22498a, "bit": 5},15: { "levelId": 2, "mem": bit6(0x22498a),"good": 1, "addr": 0x22498a, "bit": 6},16: { "levelId": 2, "mem": bit7(0x22498a),"good": 1, "addr": 0x22498a, "bit": 7},17: { "levelId": 2, "mem": bit5(0x22498b),"good": 1, "addr": 0x22498b, "bit": 5},18: { "levelId": 2, "mem": bit6(0x22498b),"good": 1, "addr": 0x22498b, "bit": 6},19: { "levelId": 2, "mem": bit7(0x22498b),"good": 1, "addr": 0x22498b, "bit": 7},20: { "levelId": 2, "mem": bit0(0x22498c),"good": 1, "addr": 0x22498c, "bit": 0},21: { "levelId": 2, "mem": bit1(0x22498c),"good": 1, "addr": 0x22498c, "bit": 1},22: { "levelId": 2, "mem": bit2(0x22498c),"good": 1, "addr": 0x22498c, "bit": 2},23: { "levelId": 2, "mem": bit3(0x22498c),"good": 1, "addr": 0x22498c, "bit": 3},24: { "levelId": 2, "mem": bit4(0x22498c),"good": 1, "addr": 0x22498c, "bit": 4},25: { "levelId": 2, "mem": bit5(0x22498c),"good": 1, "addr": 0x22498c, "bit": 5},26: { "levelId": 2, "mem": bit6(0x22498c),"good": 1, "addr": 0x22498c, "bit": 6},27: { "levelId": 2, "mem": bit7(0x22498c),"good": 1, "addr": 0x22498c, "bit": 7},28: { "levelId": 2, "mem": bit0(0x22498d),"good": 1, "addr": 0x22498d, "bit": 0},29: { "levelId": 2, "mem": bit1(0x22498d),"good": 1, "addr": 0x22498d, "bit": 1},30: { "levelId": 2, "mem": bit2(0x22498d),"good": 1, "addr": 0x22498d, "bit": 2},31: { "levelId": 2, "mem": bit3(0x22498d),"good": 1, "addr": 0x22498d, "bit": 3},32: { "levelId": 2, "mem": bit4(0x22498d),"good": 1, "addr": 0x22498d, "bit": 4},33: { "levelId": 2, "mem": bit5(0x22498d),"good": 1, "addr": 0x22498d, "bit": 5},34: { "levelId": 2, "mem": bit6(0x22498d),"good": 1, "addr": 0x22498d, "bit": 6},35: { "levelId": 2, "mem": bit7(0x22498d),"good": 1, "addr": 0x22498d, "bit": 7},36: { "levelId": 2, "mem": bit0(0x22498e),"good": 1, "addr": 0x22498e, "bit": 0},37: { "levelId": 2, "mem": bit1(0x22498e),"good": 1, "addr": 0x22498e, "bit": 1},38: { "levelId": 5, "mem": bit2(0x22498e),"good": 1, "addr": 0x22498e, "bit": 2},39: { "levelId": 5, "mem": bit3(0x22498e),"good": 1, "addr": 0x22498e, "bit": 3},40: { "levelId": 5, "mem": bit4(0x22498e),"good": 1, "addr": 0x22498e, "bit": 4},41: { "levelId": 5, "mem": bit5(0x22498e),"good": 1, "addr": 0x22498e, "bit": 5},42: { "levelId": 5, "mem": bit6(0x22498e),"good": 1, "addr": 0x22498e, "bit": 6},43: { "levelId": 5, "mem": bit7(0x22498e),"good": 1, "addr": 0x22498e, "bit": 7},44: { "levelId": 5, "mem": bit0(0x22498f),"good": 1, "addr": 0x22498f, "bit": 0},45: { "levelId": 5, "mem": bit1(0x22498f),"good": 1, "addr": 0x22498f, "bit": 1},46: { "levelId": 5, "mem": bit2(0x22498f),"good": 1, "addr": 0x22498f, "bit": 2},47: { "levelId": 5, "mem": bit3(0x22498f),"good": 1, "addr": 0x22498f, "bit": 3},48: { "levelId": 5, "mem": bit4(0x22498f),"good": 1, "addr": 0x22498f, "bit": 4},49: { "levelId": 5, "mem": bit5(0x22498f),"good": 1, "addr": 0x22498f, "bit": 5},50: { "levelId": 5, "mem": bit6(0x22498f),"good": 1, "addr": 0x22498f, "bit": 6},51: { "levelId": 5, "mem": bit7(0x22498f),"good": 1, "addr": 0x22498f, "bit": 7},52: { "levelId": 5, "mem": bit0(0x224990),"good": 1, "addr": 0x224990, "bit": 0},53: { "levelId": 5, "mem": bit1(0x224990),"good": 1, "addr": 0x224990, "bit": 1},54: { "levelId": 5, "mem": bit2(0x224990),"good": 1, "addr": 0x224990, "bit": 2},55: { "levelId": 5, "mem": bit3(0x224990),"good": 1, "addr": 0x224990, "bit": 3},56: { "levelId": 5, "mem": bit4(0x224990),"good": 1, "addr": 0x224990, "bit": 4},57: { "levelId": 5, "mem": bit5(0x224990),"good": 1, "addr": 0x224990, "bit": 5},58: { "levelId": 5, "mem": bit6(0x224990),"good": 1, "addr": 0x224990, "bit": 6},59: { "levelId": 5, "mem": bit7(0x224990),"good": 1, "addr": 0x224990, "bit": 7},60: { "levelId": 5, "mem": bit0(0x224991),"good": 1, "addr": 0x224991, "bit": 0},61: { "levelId": 5, "mem": bit1(0x224991),"good": 1, "addr": 0x224991, "bit": 1},62: { "levelId": 5, "mem": bit2(0x224991),"good": 1, "addr": 0x224991, "bit": 2},63: { "levelId": 5, "mem": bit3(0x224991),"good": 1, "addr": 0x224991, "bit": 3},64: { "levelId": 5, "mem": bit4(0x224991),"good": 1, "addr": 0x224991, "bit": 4},65: { "levelId": 5, "mem": bit5(0x224991),"good": 1, "addr": 0x224991, "bit": 5},66: { "levelId": 5, "mem": bit6(0x224991),"good": 1, "addr": 0x224991, "bit": 6},67: { "levelId": 5, "mem": bit7(0x224991),"good": 1, "addr": 0x224991, "bit": 7},68: { "levelId": 5, "mem": bit0(0x224992),"good": 1, "addr": 0x224992, "bit": 0},69: { "levelId": 5, "mem": bit1(0x224992),"good": 1, "addr": 0x224992, "bit": 1},70: { "levelId": 5, "mem": bit2(0x224992),"good": 1, "addr": 0x224992, "bit": 2},71: { "levelId": 5, "mem": bit3(0x224992),"good": 1, "addr": 0x224992, "bit": 3},72: { "levelId": 5, "mem": bit4(0x224992),"good": 1, "addr": 0x224992, "bit": 4},73: { "levelId": 5, "mem": bit5(0x224992),"good": 1, "addr": 0x224992, "bit": 5},74: { "levelId": 5, "mem": bit6(0x224992),"good": 1, "addr": 0x224992, "bit": 6},75: { "levelId": 5, "mem": bit7(0x224992),"good": 1, "addr": 0x224992, "bit": 7},76: { "levelId": 5, "mem": bit0(0x224993),"good": 1, "addr": 0x224993, "bit": 0},77: { "levelId": 5, "mem": bit1(0x224993),"good": 1, "addr": 0x224993, "bit": 1},78: { "levelId": 5, "mem": bit2(0x224993),"good": 1, "addr": 0x224993, "bit": 2},79: { "levelId": 5, "mem": bit3(0x224993),"good": 1, "addr": 0x224993, "bit": 3},80: { "levelId": 5, "mem": bit4(0x224993),"good": 1, "addr": 0x224993, "bit": 4},81: { "levelId": 5, "mem": bit5(0x224993),"good": 1, "addr": 0x224993, "bit": 5},82: { "levelId": 5, "mem": bit6(0x224993),"good": 1, "addr": 0x224993, "bit": 6},83: { "levelId": 5, "mem": bit7(0x224993),"good": 1, "addr": 0x224993, "bit": 7},84: { "levelId": 5, "mem": bit0(0x224994),"good": 1, "addr": 0x224994, "bit": 0},85: { "levelId": 5, "mem": bit1(0x224994),"good": 1, "addr": 0x224994, "bit": 1},86: { "levelId": 5, "mem": bit2(0x224994),"good": 1, "addr": 0x224994, "bit": 2},87: { "levelId": 5, "mem": bit3(0x224994),"good": 1, "addr": 0x224994, "bit": 3},88: { "levelId": 6, "mem": bit4(0x224994),"good": 1, "addr": 0x224994, "bit": 4},89: { "levelId": 6, "mem": bit5(0x224994),"good": 1, "addr": 0x224994, "bit": 5},90: { "levelId": 6, "mem": bit6(0x224994),"good": 1, "addr": 0x224994, "bit": 6},91: { "levelId": 6, "mem": bit7(0x224994),"good": 1, "addr": 0x224994, "bit": 7},92: { "levelId": 6, "mem": bit0(0x224995),"good": 1, "addr": 0x224995, "bit": 0},93: { "levelId": 6, "mem": bit1(0x224995),"good": 1, "addr": 0x224995, "bit": 1},94: { "levelId": 6, "mem": bit2(0x224995),"good": 1, "addr": 0x224995, "bit": 2},95: { "levelId": 6, "mem": bit3(0x224995),"good": 1, "addr": 0x224995, "bit": 3},96: { "levelId": 6, "mem": bit4(0x224995),"good": 1, "addr": 0x224995, "bit": 4},97: { "levelId": 6, "mem": bit5(0x224995),"good": 1, "addr": 0x224995, "bit": 5},98: { "levelId": 6, "mem": bit6(0x224995),"good": 1, "addr": 0x224995, "bit": 6},99: { "levelId": 6, "mem": bit7(0x224995),"good": 1, "addr": 0x224995, "bit": 7},100: { "levelId": 6, "mem": bit0(0x224996),"good": 1, "addr": 0x224996, "bit": 0},101: { "levelId": 6, "mem": bit1(0x224996),"good": 1, "addr": 0x224996, "bit": 1},102: { "levelId": 6, "mem": bit2(0x224996),"good": 1, "addr": 0x224996, "bit": 2},103: { "levelId": 6, "mem": bit3(0x224996),"good": 1, "addr": 0x224996, "bit": 3},104: { "levelId": 6, "mem": bit4(0x224996),"good": 1, "addr": 0x224996, "bit": 4},105: { "levelId": 6, "mem": bit5(0x224996),"good": 1, "addr": 0x224996, "bit": 5},106: { "levelId": 6, "mem": bit6(0x224996),"good": 1, "addr": 0x224996, "bit": 6},107: { "levelId": 6, "mem": bit7(0x224996),"good": 1, "addr": 0x224996, "bit": 7},108: { "levelId": 6, "mem": bit0(0x224997),"good": 1, "addr": 0x224997, "bit": 0},109: { "levelId": 6, "mem": bit1(0x224997),"good": 1, "addr": 0x224997, "bit": 1},110: { "levelId": 6, "mem": bit2(0x224997),"good": 1, "addr": 0x224997, "bit": 2},111: { "levelId": 6, "mem": bit3(0x224997),"good": 1, "addr": 0x224997, "bit": 3},112: { "levelId": 6, "mem": bit4(0x224997),"good": 1, "addr": 0x224997, "bit": 4},113: { "levelId": 6, "mem": bit5(0x224997),"good": 1, "addr": 0x224997, "bit": 5},114: { "levelId": 6, "mem": bit6(0x224997),"good": 1, "addr": 0x224997, "bit": 6},115: { "levelId": 6, "mem": bit7(0x224997),"good": 1, "addr": 0x224997, "bit": 7},116: { "levelId": 6, "mem": bit0(0x224998),"good": 1, "addr": 0x224998, "bit": 0},117: { "levelId": 6, "mem": bit1(0x224998),"good": 1, "addr": 0x224998, "bit": 1},118: { "levelId": 6, "mem": bit2(0x224998),"good": 1, "addr": 0x224998, "bit": 2},119: { "levelId": 6, "mem": bit3(0x224998),"good": 1, "addr": 0x224998, "bit": 3},120: { "levelId": 6, "mem": bit4(0x224998),"good": 1, "addr": 0x224998, "bit": 4},121: { "levelId": 6, "mem": bit5(0x224998),"good": 1, "addr": 0x224998, "bit": 5},122: { "levelId": 6, "mem": bit6(0x224998),"good": 1, "addr": 0x224998, "bit": 6},123: { "levelId": 6, "mem": bit0(0x224999),"good": 1, "addr": 0x224999, "bit": 0},124: { "levelId": 6, "mem": bit1(0x224999),"good": 1, "addr": 0x224999, "bit": 1},125: { "levelId": 6, "mem": bit2(0x224999),"good": 1, "addr": 0x224999, "bit": 2},126: { "levelId": 6, "mem": bit3(0x224999),"good": 1, "addr": 0x224999, "bit": 3},127: { "levelId": 6, "mem": bit4(0x224999),"good": 1, "addr": 0x224999, "bit": 4},128: { "levelId": 6, "mem": bit5(0x224999),"good": 1, "addr": 0x224999, "bit": 5},129: { "levelId": 6, "mem": bit6(0x224999),"good": 1, "addr": 0x224999, "bit": 6},130: { "levelId": 6, "mem": bit7(0x224999),"good": 1, "addr": 0x224999, "bit": 7},131: { "levelId": 6, "mem": bit0(0x22499a),"good": 1, "addr": 0x22499a, "bit": 0},132: { "levelId": 6, "mem": bit1(0x22499a),"good": 1, "addr": 0x22499a, "bit": 1},133: { "levelId": 6, "mem": bit2(0x22499a),"good": 1, "addr": 0x22499a, "bit": 2},134: { "levelId": 6, "mem": bit3(0x22499a),"good": 1, "addr": 0x22499a, "bit": 3},135: { "levelId": 6, "mem": bit4(0x22499a),"good": 1, "addr": 0x22499a, "bit": 4},136: { "levelId": 6, "mem": bit5(0x22499a),"good": 1, "addr": 0x22499a, "bit": 5},137: { "levelId": 1, "mem": bit3(0x224a36),"good": 1, "addr": 0x224a36, "bit": 3},138: { "levelId": 1, "mem": bit4(0x224a36),"good": 1, "addr": 0x224a36, "bit": 4},139: { "levelId": 1, "mem": bit5(0x224a36),"good": 1, "addr": 0x224a36, "bit": 5},140: { "levelId": 1, "mem": bit6(0x224a36),"good": 1, "addr": 0x224a36, "bit": 6},141: { "levelId": 1, "mem": bit7(0x224a36),"good": 1, "addr": 0x224a36, "bit": 7},142: { "levelId": 6, "mem": bit7(0x224998),"good": 1, "addr": 0x224998, "bit": 7},143: { "levelId": 8, "mem": bit3(0x22499b),"good": 1, "addr": 0x22499b, "bit": 3},144: { "levelId": 8, "mem": bit4(0x22499b),"good": 1, "addr": 0x22499b, "bit": 4},145: { "levelId": 8, "mem": bit5(0x22499b),"good": 1, "addr": 0x22499b, "bit": 5},146: { "levelId": 8, "mem": bit5(0x22499c),"good": 1, "addr": 0x22499c, "bit": 5},147: { "levelId": 8, "mem": bit6(0x22499c),"good": 1, "addr": 0x22499c, "bit": 6},148: { "levelId": 8, "mem": bit7(0x22499c),"good": 1, "addr": 0x22499c, "bit": 7},149: { "levelId": 8, "mem": bit0(0x22499d),"good": 1, "addr": 0x22499d, "bit": 0},150: { "levelId": 8, "mem": bit1(0x22499d),"good": 1, "addr": 0x22499d, "bit": 1},151: { "levelId": 8, "mem": bit2(0x22499d),"good": 1, "addr": 0x22499d, "bit": 2},152: { "levelId": 8, "mem": bit3(0x22499d),"good": 1, "addr": 0x22499d, "bit": 3},153: { "levelId": 8, "mem": bit4(0x22499d),"good": 1, "addr": 0x22499d, "bit": 4},154: { "levelId": 8, "mem": bit5(0x22499d),"good": 1, "addr": 0x22499d, "bit": 5},155: { "levelId": 8, "mem": bit6(0x22499d),"good": 1, "addr": 0x22499d, "bit": 6},156: { "levelId": 8, "mem": bit7(0x22499d),"good": 1, "addr": 0x22499d, "bit": 7},157: { "levelId": 8, "mem": bit0(0x22499e),"good": 1, "addr": 0x22499e, "bit": 0},158: { "levelId": 8, "mem": bit1(0x22499e),"good": 1, "addr": 0x22499e, "bit": 1},159: { "levelId": 8, "mem": bit6(0x22499a),"good": 1, "addr": 0x22499a, "bit": 6},160: { "levelId": 8, "mem": bit7(0x22499a),"good": 1, "addr": 0x22499a, "bit": 7},161: { "levelId": 8, "mem": bit0(0x22499b),"good": 1, "addr": 0x22499b, "bit": 0},162: { "levelId": 8, "mem": bit1(0x22499b),"good": 1, "addr": 0x22499b, "bit": 1},163: { "levelId": 8, "mem": bit2(0x22499b),"good": 1, "addr": 0x22499b, "bit": 2},164: { "levelId": 8, "mem": bit6(0x22499b),"good": 1, "addr": 0x22499b, "bit": 6},165: { "levelId": 8, "mem": bit7(0x22499b),"good": 1, "addr": 0x22499b, "bit": 7},166: { "levelId": 8, "mem": bit0(0x22499c),"good": 1, "addr": 0x22499c, "bit": 0},167: { "levelId": 8, "mem": bit1(0x22499c),"good": 1, "addr": 0x22499c, "bit": 1},168: { "levelId": 8, "mem": bit2(0x22499c),"good": 1, "addr": 0x22499c, "bit": 2},169: { "levelId": 8, "mem": bit3(0x22499c),"good": 1, "addr": 0x22499c, "bit": 3},170: { "levelId": 8, "mem": bit4(0x22499c),"good": 1, "addr": 0x22499c, "bit": 4},171: { "levelId": 8, "mem": bit2(0x22499e),"good": 1, "addr": 0x22499e, "bit": 2},172: { "levelId": 8, "mem": bit3(0x22499e),"good": 1, "addr": 0x22499e, "bit": 3},173: { "levelId": 8, "mem": bit4(0x22499e),"good": 1, "addr": 0x22499e, "bit": 4},174: { "levelId": 8, "mem": bit5(0x22499e),"good": 1, "addr": 0x22499e, "bit": 5},175: { "levelId": 8, "mem": bit6(0x22499e),"good": 1, "addr": 0x22499e, "bit": 6},176: { "levelId": 8, "mem": bit7(0x22499e),"good": 1, "addr": 0x22499e, "bit": 7},177: { "levelId": 8, "mem": bit0(0x22499f),"good": 1, "addr": 0x22499f, "bit": 0},178: { "levelId": 8, "mem": bit1(0x22499f),"good": 1, "addr": 0x22499f, "bit": 1},179: { "levelId": 8, "mem": bit2(0x22499f),"good": 1, "addr": 0x22499f, "bit": 2},180: { "levelId": 8, "mem": bit3(0x22499f),"good": 1, "addr": 0x22499f, "bit": 3},181: { "levelId": 8, "mem": bit4(0x22499f),"good": 1, "addr": 0x22499f, "bit": 4},182: { "levelId": 8, "mem": bit5(0x22499f),"good": 1, "addr": 0x22499f, "bit": 5},183: { "levelId": 8, "mem": bit6(0x22499f),"good": 1, "addr": 0x22499f, "bit": 6},184: { "levelId": 8, "mem": bit7(0x22499f),"good": 1, "addr": 0x22499f, "bit": 7},185: { "levelId": 8, "mem": bit0(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 0},186: { "levelId": 8, "mem": bit1(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 1},187: { "levelId": 8, "mem": bit2(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 2},188: { "levelId": 8, "mem": bit3(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 3},189: { "levelId": 8, "mem": bit4(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 4},190: { "levelId": 8, "mem": bit5(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 5},191: { "levelId": 8, "mem": bit6(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 6},192: { "levelId": 8, "mem": bit7(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 7},193: { "levelId": 10, "mem": bit0(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 0},194: { "levelId": 10, "mem": bit1(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 1},195: { "levelId": 10, "mem": bit2(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 2},196: { "levelId": 10, "mem": bit3(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 3},197: { "levelId": 10, "mem": bit4(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 4},198: { "levelId": 10, "mem": bit2(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 2},199: { "levelId": 10, "mem": bit3(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 3},200: { "levelId": 10, "mem": bit4(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 4},201: { "levelId": 10, "mem": bit5(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 5},202: { "levelId": 10, "mem": bit6(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 6},203: { "levelId": 10, "mem": bit1(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 1},204: { "levelId": 10, "mem": bit5(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 5},205: { "levelId": 10, "mem": bit6(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 6},206: { "levelId": 10, "mem": bit7(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 7},207: { "levelId": 10, "mem": bit0(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 0},208: { "levelId": 10, "mem": bit3(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 3},209: { "levelId": 10, "mem": bit5(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 5},210: { "levelId": 10, "mem": bit6(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 6},211: { "levelId": 10, "mem": bit7(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 7},212: { "levelId": 10, "mem": bit0(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 0},213: { "levelId": 10, "mem": bit1(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 1},214: { "levelId": 10, "mem": bit2(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 2},215: { "levelId": 10, "mem": bit4(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 4},216: { "levelId": 11, "mem": bit6(0x2249e5),"good": 1, "addr": 0x2249e5, "bit": 6},217: { "levelId": 11, "mem": bit7(0x2249e5),"good": 1, "addr": 0x2249e5, "bit": 7},218: { "levelId": 11, "mem": bit0(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 0},219: { "levelId": 11, "mem": bit1(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 1},220: { "levelId": 11, "mem": bit2(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 2},221: { "levelId": 11, "mem": bit3(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 3},222: { "levelId": 11, "mem": bit4(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 4},223: { "levelId": 11, "mem": bit5(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 5},224: { "levelId": 11, "mem": bit6(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 6},225: { "levelId": 11, "mem": bit7(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 7},226: { "levelId": 11, "mem": bit0(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 0},227: { "levelId": 11, "mem": bit1(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 1},228: { "levelId": 11, "mem": bit2(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 2},229: { "levelId": 11, "mem": bit3(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 3},230: { "levelId": 11, "mem": bit4(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 4},231: { "levelId": 11, "mem": bit5(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 5},232: { "levelId": 11, "mem": bit6(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 6},233: { "levelId": 11, "mem": bit7(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 7},234: { "levelId": 11, "mem": bit0(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 0},235: { "levelId": 11, "mem": bit1(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 1},236: { "levelId": 11, "mem": bit2(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 2},237: { "levelId": 11, "mem": bit3(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 3},238: { "levelId": 11, "mem": bit4(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 4},239: { "levelId": 11, "mem": bit5(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 5},240: { "levelId": 11, "mem": bit6(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 6},241: { "levelId": 11, "mem": bit7(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 7},242: { "levelId": 11, "mem": bit0(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 0},243: { "levelId": 11, "mem": bit1(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 1},244: { "levelId": 11, "mem": bit2(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 2},245: { "levelId": 11, "mem": bit3(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 3},246: { "levelId": 11, "mem": bit4(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 4},247: { "levelId": 11, "mem": bit5(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 5},248: { "levelId": 11, "mem": bit6(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 6},249: { "levelId": 11, "mem": bit7(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 7},250: { "levelId": 11, "mem": bit0(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 0},251: { "levelId": 11, "mem": bit1(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 1},252: { "levelId": 11, "mem": bit2(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 2},253: { "levelId": 11, "mem": bit3(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 3},254: { "levelId": 11, "mem": bit4(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 4},255: { "levelId": 11, "mem": bit5(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 5},256: { "levelId": 11, "mem": bit6(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 6},257: { "levelId": 11, "mem": bit7(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 7},258: { "levelId": 11, "mem": bit0(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 0},259: { "levelId": 11, "mem": bit1(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 1},260: { "levelId": 11, "mem": bit2(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 2},261: { "levelId": 11, "mem": bit3(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 3},262: { "levelId": 11, "mem": bit4(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 4},263: { "levelId": 11, "mem": bit5(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 5},264: { "levelId": 11, "mem": bit6(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 6},265: { "levelId": 11, "mem": bit7(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 7},266: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},267: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},268: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},269: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},270: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},271: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},272: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},273: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},274: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},275: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},276: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},277: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},278: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},279: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},280: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},281: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},282: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},283: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},284: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},285: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},286: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},287: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},288: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},289: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},290: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},291: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},292: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},293: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},294: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},295: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},296: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},297: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},298: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},299: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},300: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},301: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},302: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},303: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},304: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},305: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},306: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},307: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},308: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},309: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},310: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},311: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},312: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},313: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},314: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},315: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},316: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},317: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},318: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},319: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},320: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},321: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},322: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},323: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},324: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},325: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},326: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},327: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},328: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},329: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},330: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},331: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},332: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},333: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},334: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},335: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},336: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},337: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},338: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},339: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},340: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},341: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},342: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},343: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},344: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},345: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},346: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},347: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},348: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},349: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},350: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},351: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},352: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},353: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},354: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},355: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},356: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},357: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},358: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},359: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},360: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},361: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},362: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},363: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},364: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},365: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},366: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},367: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},368: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},369: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},370: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},371: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},372: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},373: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},374: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},375: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},376: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},377: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},378: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},379: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},380: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},381: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},382: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},383: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},384: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},385: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},386: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},387: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},388: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},389: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},390: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},391: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},392: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},393: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},394: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},395: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},396: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},397: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},398: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},399: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},400: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},401: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},402: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},403: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},404: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},405: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},406: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},407: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},408: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},409: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},410: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},411: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},412: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},413: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},414: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},415: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},416: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},417: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},418: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},419: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},420: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},421: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},422: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},423: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},424: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},425: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},426: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},427: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},428: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},429: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},430: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},431: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},432: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},433: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},434: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},435: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},436: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},437: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},438: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},439: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},440: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},441: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},442: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},443: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},444: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},445: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},446: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},447: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},448: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},449: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},450: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},451: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},452: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},453: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},454: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},455: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},456: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},457: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},458: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},459: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},460: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},461: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},462: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},463: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},464: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},465: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},466: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},467: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},468: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},469: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},470: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},471: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},472: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},473: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},474: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},475: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},476: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},477: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},478: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},479: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},480: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},481: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},482: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},483: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},484: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},485: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},486: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},487: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},488: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},489: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},490: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},491: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},492: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},493: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},494: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},495: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},496: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},497: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},498: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},499: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},500: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},501: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},502: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},503: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},504: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},505: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},506: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},507: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},508: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},509: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},510: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},511: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},512: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},513: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},514: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},515: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},516: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},517: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},518: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},519: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},520: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},521: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},522: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},523: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},524: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},525: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},526: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},527: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},528: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},529: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},530: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},531: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},532: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},533: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},534: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},535: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},536: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},537: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},538: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},539: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},540: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},541: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},542: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},543: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},544: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},545: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},546: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},547: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},548: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},549: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},550: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},551: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},552: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},553: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},554: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},555: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},556: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},557: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},558: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},559: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},560: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},561: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},562: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},563: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},564: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},565: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},566: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},567: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},568: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},569: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},570: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},571: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},572: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},573: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},574: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},575: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},576: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},577: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},578: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},579: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},580: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},581: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},582: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},583: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},584: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},585: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},586: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},587: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},588: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},589: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},590: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},591: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},592: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},593: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},594: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},595: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},596: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},597: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},598: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},599: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},600: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},601: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},602: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},603: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},604: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},605: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},606: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},607: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},608: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},609: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},610: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},611: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},612: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},613: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},614: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},615: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},616: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},617: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},618: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},619: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},620: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},621: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},622: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},623: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},624: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},625: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},626: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},627: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},628: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},629: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},630: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},631: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},632: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},633: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},634: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},635: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},636: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},637: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},638: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},639: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},640: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},641: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},642: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},643: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},644: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},645: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},646: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},647: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},648: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},649: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},650: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},651: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},652: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},653: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},654: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},655: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},656: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},657: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},658: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},659: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},660: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},661: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},662: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},663: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},664: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},665: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},666: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},667: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},668: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},669: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},670: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},671: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},672: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},673: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},674: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},675: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},676: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},677: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},678: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},679: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},680: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},681: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},682: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},683: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},684: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},685: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},686: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},687: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},688: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},689: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},690: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},691: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},692: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},693: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},694: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},695: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},696: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},697: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},698: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},699: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},700: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},701: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},702: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},703: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},704: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},705: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},706: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},707: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},708: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},709: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},710: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},711: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},712: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},713: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},714: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},715: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},716: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},717: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},718: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},719: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},720: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},721: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},722: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},723: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},724: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},725: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},726: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},727: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},728: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},729: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},730: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},731: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},732: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},733: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},734: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},735: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},736: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},737: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},738: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},739: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},740: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},741: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},742: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},743: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},744: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},745: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},746: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},747: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},748: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},749: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},750: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},751: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},752: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},753: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},754: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},755: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},756: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},757: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},758: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},759: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},760: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},761: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},762: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},763: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},764: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},765: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},766: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},767: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},768: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},769: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},770: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},771: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},772: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},773: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},774: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},775: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},776: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},777: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},778: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},779: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},780: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},781: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},782: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},783: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},784: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},785: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},786: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},787: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},788: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},789: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},790: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},791: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},792: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},793: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},794: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},795: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},796: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},797: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},798: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},799: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},800: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},801: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},802: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},803: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},804: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},805: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},806: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},807: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},808: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},809: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},810: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},811: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},812: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},813: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},814: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},815: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},816: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},817: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},818: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},819: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},820: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},821: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},822: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},823: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},824: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},825: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},826: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},827: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},828: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},829: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},830: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},831: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},832: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},833: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},834: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},835: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},836: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},837: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},838: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},839: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},840: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},841: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},842: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},843: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},844: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},845: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},846: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},847: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},848: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},849: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},850: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},851: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},852: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},853: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},854: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},855: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},856: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},857: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},858: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},859: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},860: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},861: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},862: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},863: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},864: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},865: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},866: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},867: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},868: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},869: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},870: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},871: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},872: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},873: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},874: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},875: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},876: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},877: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},878: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},879: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},880: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},881: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},882: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},883: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},884: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},885: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},886: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},887: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},888: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},889: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},890: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},891: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},892: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},893: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},894: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},895: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},896: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},897: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},898: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},899: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},900: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},901: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},902: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},903: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},904: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},905: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},906: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},907: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},908: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},909: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},910: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},911: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},912: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},913: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},914: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},915: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},916: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},917: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},918: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},919: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},920: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},921: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},922: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},923: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},924: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},925: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},926: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},927: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},928: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},929: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},930: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},931: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},932: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},933: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},934: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},935: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},936: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},937: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},938: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},939: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},940: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},941: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},942: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},943: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},944: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},945: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},946: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},947: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},948: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},949: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},950: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},951: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},952: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},953: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},954: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},955: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},956: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},957: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},958: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},959: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},960: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},961: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},962: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},963: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},964: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},965: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},966: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},967: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},968: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},969: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},970: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},971: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},972: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},973: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},974: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},975: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},976: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},977: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},978: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},979: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},980: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},981: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},982: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},983: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},984: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},985: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},986: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},987: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},988: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},989: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},990: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},991: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},992: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},993: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},994: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},995: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},996: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},997: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},998: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},999: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},1000: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>1: { "levelId": 2, "mem": bit0(0x224988),"good": 1, "addr": 0x224988, "bit": 0},2: { "levelId": 2, "mem": bit1(0x224988),"good": 1, "addr": 0x224988, "bit": 1},3: { "levelId": 2, "mem": bit2(0x224988),"good": 1, "addr": 0x224988, "bit": 2},4: { "levelId": 2, "mem": bit3(0x224988),"good": 1, "addr": 0x224988, "bit": 3},5: { "levelId": 2, "mem": bit4(0x224988),"good": 1, "addr": 0x224988, "bit": 4},6: { "levelId": 2, "mem": bit5(0x224988),"good": 1, "addr": 0x224988, "bit": 5},7: { "levelId": 2, "mem": bit6(0x224988),"good": 1, "addr": 0x224988, "bit": 6},8: { "levelId": 2, "mem": bit7(0x224988),"good": 1, "addr": 0x224988, "bit": 7},9: { "levelId": 2, "mem": bit2(0x224989),"good": 1, "addr": 0x224989, "bit": 2},10: { "levelId": 2, "mem": bit1(0x22498a),"good": 1, "addr": 0x22498a, "bit": 1},11: { "levelId": 2, "mem": bit2(0x22498a),"good": 1, "addr": 0x22498a, "bit": 2},12: { "levelId": 2, "mem": bit3(0x22498a),"good": 1, "addr": 0x22498a, "bit": 3},13: { "levelId": 2, "mem": bit4(0x22498a),"good": 1, "addr": 0x22498a, "bit": 4},14: { "levelId": 2, "mem": bit5(0x22498a),"good": 1, "addr": 0x22498a, "bit": 5},15: { "levelId": 2, "mem": bit6(0x22498a),"good": 1, "addr": 0x22498a, "bit": 6},16: { "levelId": 2, "mem": bit7(0x22498a),"good": 1, "addr": 0x22498a, "bit": 7},17: { "levelId": 2, "mem": bit5(0x22498b),"good": 1, "addr": 0x22498b, "bit": 5},18: { "levelId": 2, "mem": bit6(0x22498b),"good": 1, "addr": 0x22498b, "bit": 6},19: { "levelId": 2, "mem": bit7(0x22498b),"good": 1, "addr": 0x22498b, "bit": 7},20: { "levelId": 2, "mem": bit0(0x22498c),"good": 1, "addr": 0x22498c, "bit": 0},21: { "levelId": 2, "mem": bit1(0x22498c),"good": 1, "addr": 0x22498c, "bit": 1},22: { "levelId": 2, "mem": bit2(0x22498c),"good": 1, "addr": 0x22498c, "bit": 2},23: { "levelId": 2, "mem": bit3(0x22498c),"good": 1, "addr": 0x22498c, "bit": 3},24: { "levelId": 2, "mem": bit4(0x22498c),"good": 1, "addr": 0x22498c, "bit": 4},25: { "levelId": 2, "mem": bit5(0x22498c),"good": 1, "addr": 0x22498c, "bit": 5},26: { "levelId": 2, "mem": bit6(0x22498c),"good": 1, "addr": 0x22498c, "bit": 6},27: { "levelId": 2, "mem": bit7(0x22498c),"good": 1, "addr": 0x22498c, "bit": 7},28: { "levelId": 2, "mem": bit0(0x22498d),"good": 1, "addr": 0x22498d, "bit": 0},29: { "levelId": 2, "mem": bit1(0x22498d),"good": 1, "addr": 0x22498d, "bit": 1},30: { "levelId": 2, "mem": bit2(0x22498d),"good": 1, "addr": 0x22498d, "bit": 2},31: { "levelId": 2, "mem": bit3(0x22498d),"good": 1, "addr": 0x22498d, "bit": 3},32: { "levelId": 2, "mem": bit4(0x22498d),"good": 1, "addr": 0x22498d, "bit": 4},33: { "levelId": 2, "mem": bit5(0x22498d),"good": 1, "addr": 0x22498d, "bit": 5},34: { "levelId": 2, "mem": bit6(0x22498d),"good": 1, "addr": 0x22498d, "bit": 6},35: { "levelId": 2, "mem": bit7(0x22498d),"good": 1, "addr": 0x22498d, "bit": 7},36: { "levelId": 2, "mem": bit0(0x22498e),"good": 1, "addr": 0x22498e, "bit": 0},37: { "levelId": 2, "mem": bit1(0x22498e),"good": 1, "addr": 0x22498e, "bit": 1},38: { "levelId": 5, "mem": bit2(0x22498e),"good": 1, "addr": 0x22498e, "bit": 2},39: { "levelId": 5, "mem": bit3(0x22498e),"good": 1, "addr": 0x22498e, "bit": 3},40: { "levelId": 5, "mem": bit4(0x22498e),"good": 1, "addr": 0x22498e, "bit": 4},41: { "levelId": 5, "mem": bit5(0x22498e),"good": 1, "addr": 0x22498e, "bit": 5},42: { "levelId": 5, "mem": bit6(0x22498e),"good": 1, "addr": 0x22498e, "bit": 6},43: { "levelId": 5, "mem": bit7(0x22498e),"good": 1, "addr": 0x22498e, "bit": 7},44: { "levelId": 5, "mem": bit0(0x22498f),"good": 1, "addr": 0x22498f, "bit": 0},45: { "levelId": 5, "mem": bit1(0x22498f),"good": 1, "addr": 0x22498f, "bit": 1},46: { "levelId": 5, "mem": bit2(0x22498f),"good": 1, "addr": 0x22498f, "bit": 2},47: { "levelId": 5, "mem": bit3(0x22498f),"good": 1, "addr": 0x22498f, "bit": 3},48: { "levelId": 5, "mem": bit4(0x22498f),"good": 1, "addr": 0x22498f, "bit": 4},49: { "levelId": 5, "mem": bit5(0x22498f),"good": 1, "addr": 0x22498f, "bit": 5},50: { "levelId": 5, "mem": bit6(0x22498f),"good": 1, "addr": 0x22498f, "bit": 6},51: { "levelId": 5, "mem": bit7(0x22498f),"good": 1, "addr": 0x22498f, "bit": 7},52: { "levelId": 5, "mem": bit0(0x224990),"good": 1, "addr": 0x224990, "bit": 0},53: { "levelId": 5, "mem": bit1(0x224990),"good": 1, "addr": 0x224990, "bit": 1},54: { "levelId": 5, "mem": bit2(0x224990),"good": 1, "addr": 0x224990, "bit": 2},55: { "levelId": 5, "mem": bit3(0x224990),"good": 1, "addr": 0x224990, "bit": 3},56: { "levelId": 5, "mem": bit4(0x224990),"good": 1, "addr": 0x224990, "bit": 4},57: { "levelId": 5, "mem": bit5(0x224990),"good": 1, "addr": 0x224990, "bit": 5},58: { "levelId": 5, "mem": bit6(0x224990),"good": 1, "addr": 0x224990, "bit": 6},59: { "levelId": 5, "mem": bit7(0x224990),"good": 1, "addr": 0x224990, "bit": 7},60: { "levelId": 5, "mem": bit0(0x224991),"good": 1, "addr": 0x224991, "bit": 0},61: { "levelId": 5, "mem": bit1(0x224991),"good": 1, "addr": 0x224991, "bit": 1},62: { "levelId": 5, "mem": bit2(0x224991),"good": 1, "addr": 0x224991, "bit": 2},63: { "levelId": 5, "mem": bit3(0x224991),"good": 1, "addr": 0x224991, "bit": 3},64: { "levelId": 5, "mem": bit4(0x224991),"good": 1, "addr": 0x224991, "bit": 4},65: { "levelId": 5, "mem": bit5(0x224991),"good": 1, "addr": 0x224991, "bit": 5},66: { "levelId": 5, "mem": bit6(0x224991),"good": 1, "addr": 0x224991, "bit": 6},67: { "levelId": 5, "mem": bit7(0x224991),"good": 1, "addr": 0x224991, "bit": 7},68: { "levelId": 5, "mem": bit0(0x224992),"good": 1, "addr": 0x224992, "bit": 0},69: { "levelId": 5, "mem": bit1(0x224992),"good": 1, "addr": 0x224992, "bit": 1},70: { "levelId": 5, "mem": bit2(0x224992),"good": 1, "addr": 0x224992, "bit": 2},71: { "levelId": 5, "mem": bit3(0x224992),"good": 1, "addr": 0x224992, "bit": 3},72: { "levelId": 5, "mem": bit4(0x224992),"good": 1, "addr": 0x224992, "bit": 4},73: { "levelId": 5, "mem": bit5(0x224992),"good": 1, "addr": 0x224992, "bit": 5},74: { "levelId": 5, "mem": bit6(0x224992),"good": 1, "addr": 0x224992, "bit": 6},75: { "levelId": 5, "mem": bit7(0x224992),"good": 1, "addr": 0x224992, "bit": 7},76: { "levelId": 5, "mem": bit0(0x224993),"good": 1, "addr": 0x224993, "bit": 0},77: { "levelId": 5, "mem": bit1(0x224993),"good": 1, "addr": 0x224993, "bit": 1},78: { "levelId": 5, "mem": bit2(0x224993),"good": 1, "addr": 0x224993, "bit": 2},79: { "levelId": 5, "mem": bit3(0x224993),"good": 1, "addr": 0x224993, "bit": 3},80: { "levelId": 5, "mem": bit4(0x224993),"good": 1, "addr": 0x224993, "bit": 4},81: { "levelId": 5, "mem": bit5(0x224993),"good": 1, "addr": 0x224993, "bit": 5},82: { "levelId": 5, "mem": bit6(0x224993),"good": 1, "addr": 0x224993, "bit": 6},83: { "levelId": 5, "mem": bit7(0x224993),"good": 1, "addr": 0x224993, "bit": 7},84: { "levelId": 5, "mem": bit0(0x224994),"good": 1, "addr": 0x224994, "bit": 0},85: { "levelId": 5, "mem": bit1(0x224994),"good": 1, "addr": 0x224994, "bit": 1},86: { "levelId": 5, "mem": bit2(0x224994),"good": 1, "addr": 0x224994, "bit": 2},87: { "levelId": 5, "mem": bit3(0x224994),"good": 1, "addr": 0x224994, "bit": 3},88: { "levelId": 6, "mem": bit4(0x224994),"good": 1, "addr": 0x224994, "bit": 4},89: { "levelId": 6, "mem": bit5(0x224994),"good": 1, "addr": 0x224994, "bit": 5},90: { "levelId": 6, "mem": bit6(0x224994),"good": 1, "addr": 0x224994, "bit": 6},91: { "levelId": 6, "mem": bit7(0x224994),"good": 1, "addr": 0x224994, "bit": 7},92: { "levelId": 6, "mem": bit0(0x224995),"good": 1, "addr": 0x224995, "bit": 0},93: { "levelId": 6, "mem": bit1(0x224995),"good": 1, "addr": 0x224995, "bit": 1},94: { "levelId": 6, "mem": bit2(0x224995),"good": 1, "addr": 0x224995, "bit": 2},95: { "levelId": 6, "mem": bit3(0x224995),"good": 1, "addr": 0x224995, "bit": 3},96: { "levelId": 6, "mem": bit4(0x224995),"good": 1, "addr": 0x224995, "bit": 4},97: { "levelId": 6, "mem": bit5(0x224995),"good": 1, "addr": 0x224995, "bit": 5},98: { "levelId": 6, "mem": bit6(0x224995),"good": 1, "addr": 0x224995, "bit": 6},99: { "levelId": 6, "mem": bit7(0x224995),"good": 1, "addr": 0x224995, "bit": 7},100: { "levelId": 6, "mem": bit0(0x224996),"good": 1, "addr": 0x224996, "bit": 0},101: { "levelId": 6, "mem": bit1(0x224996),"good": 1, "addr": 0x224996, "bit": 1},102: { "levelId": 6, "mem": bit2(0x224996),"good": 1, "addr": 0x224996, "bit": 2},103: { "levelId": 6, "mem": bit3(0x224996),"good": 1, "addr": 0x224996, "bit": 3},104: { "levelId": 6, "mem": bit4(0x224996),"good": 1, "addr": 0x224996, "bit": 4},105: { "levelId": 6, "mem": bit5(0x224996),"good": 1, "addr": 0x224996, "bit": 5},106: { "levelId": 6, "mem": bit6(0x224996),"good": 1, "addr": 0x224996, "bit": 6},107: { "levelId": 6, "mem": bit7(0x224996),"good": 1, "addr": 0x224996, "bit": 7},108: { "levelId": 6, "mem": bit0(0x224997),"good": 1, "addr": 0x224997, "bit": 0},109: { "levelId": 6, "mem": bit1(0x224997),"good": 1, "addr": 0x224997, "bit": 1},110: { "levelId": 6, "mem": bit2(0x224997),"good": 1, "addr": 0x224997, "bit": 2},111: { "levelId": 6, "mem": bit3(0x224997),"good": 1, "addr": 0x224997, "bit": 3},112: { "levelId": 6, "mem": bit4(0x224997),"good": 1, "addr": 0x224997, "bit": 4},113: { "levelId": 6, "mem": bit5(0x224997),"good": 1, "addr": 0x224997, "bit": 5},114: { "levelId": 6, "mem": bit6(0x224997),"good": 1, "addr": 0x224997, "bit": 6},115: { "levelId": 6, "mem": bit7(0x224997),"good": 1, "addr": 0x224997, "bit": 7},116: { "levelId": 6, "mem": bit0(0x224998),"good": 1, "addr": 0x224998, "bit": 0},117: { "levelId": 6, "mem": bit1(0x224998),"good": 1, "addr": 0x224998, "bit": 1},118: { "levelId": 6, "mem": bit2(0x224998),"good": 1, "addr": 0x224998, "bit": 2},119: { "levelId": 6, "mem": bit3(0x224998),"good": 1, "addr": 0x224998, "bit": 3},120: { "levelId": 6, "mem": bit4(0x224998),"good": 1, "addr": 0x224998, "bit": 4},121: { "levelId": 6, "mem": bit5(0x224998),"good": 1, "addr": 0x224998, "bit": 5},122: { "levelId": 6, "mem": bit6(0x224998),"good": 1, "addr": 0x224998, "bit": 6},123: { "levelId": 6, "mem": bit0(0x224999),"good": 1, "addr": 0x224999, "bit": 0},124: { "levelId": 6, "mem": bit1(0x224999),"good": 1, "addr": 0x224999, "bit": 1},125: { "levelId": 6, "mem": bit2(0x224999),"good": 1, "addr": 0x224999, "bit": 2},126: { "levelId": 6, "mem": bit3(0x224999),"good": 1, "addr": 0x224999, "bit": 3},127: { "levelId": 6, "mem": bit4(0x224999),"good": 1, "addr": 0x224999, "bit": 4},128: { "levelId": 6, "mem": bit5(0x224999),"good": 1, "addr": 0x224999, "bit": 5},129: { "levelId": 6, "mem": bit6(0x224999),"good": 1, "addr": 0x224999, "bit": 6},130: { "levelId": 6, "mem": bit7(0x224999),"good": 1, "addr": 0x224999, "bit": 7},131: { "levelId": 6, "mem": bit0(0x22499a),"good": 1, "addr": 0x22499a, "bit": 0},132: { "levelId": 6, "mem": bit1(0x22499a),"good": 1, "addr": 0x22499a, "bit": 1},133: { "levelId": 6, "mem": bit2(0x22499a),"good": 1, "addr": 0x22499a, "bit": 2},134: { "levelId": 6, "mem": bit3(0x22499a),"good": 1, "addr": 0x22499a, "bit": 3},135: { "levelId": 6, "mem": bit4(0x22499a),"good": 1, "addr": 0x22499a, "bit": 4},136: { "levelId": 6, "mem": bit5(0x22499a),"good": 1, "addr": 0x22499a, "bit": 5},137: { "levelId": 1, "mem": bit3(0x224a36),"good": 1, "addr": 0x224a36, "bit": 3},138: { "levelId": 1, "mem": bit4(0x224a36),"good": 1, "addr": 0x224a36, "bit": 4},139: { "levelId": 1, "mem": bit5(0x224a36),"good": 1, "addr": 0x224a36, "bit": 5},140: { "levelId": 1, "mem": bit6(0x224a36),"good": 1, "addr": 0x224a36, "bit": 6},141: { "levelId": 1, "mem": bit7(0x224a36),"good": 1, "addr": 0x224a36, "bit": 7},142: { "levelId": 6, "mem": bit7(0x224998),"good": 1, "addr": 0x224998, "bit": 7},143: { "levelId": 8, "mem": bit3(0x22499b),"good": 1, "addr": 0x22499b, "bit": 3},144: { "levelId": 8, "mem": bit4(0x22499b),"good": 1, "addr": 0x22499b, "bit": 4},145: { "levelId": 8, "mem": bit5(0x22499b),"good": 1, "addr": 0x22499b, "bit": 5},146: { "levelId": 8, "mem": bit5(0x22499c),"good": 1, "addr": 0x22499c, "bit": 5},147: { "levelId": 8, "mem": bit6(0x22499c),"good": 1, "addr": 0x22499c, "bit": 6},148: { "levelId": 8, "mem": bit7(0x22499c),"good": 1, "addr": 0x22499c, "bit": 7},149: { "levelId": 8, "mem": bit0(0x22499d),"good": 1, "addr": 0x22499d, "bit": 0},150: { "levelId": 8, "mem": bit1(0x22499d),"good": 1, "addr": 0x22499d, "bit": 1},151: { "levelId": 8, "mem": bit2(0x22499d),"good": 1, "addr": 0x22499d, "bit": 2},152: { "levelId": 8, "mem": bit3(0x22499d),"good": 1, "addr": 0x22499d, "bit": 3},153: { "levelId": 8, "mem": bit4(0x22499d),"good": 1, "addr": 0x22499d, "bit": 4},154: { "levelId": 8, "mem": bit5(0x22499d),"good": 1, "addr": 0x22499d, "bit": 5},155: { "levelId": 8, "mem": bit6(0x22499d),"good": 1, "addr": 0x22499d, "bit": 6},156: { "levelId": 8, "mem": bit7(0x22499d),"good": 1, "addr": 0x22499d, "bit": 7},157: { "levelId": 8, "mem": bit0(0x22499e),"good": 1, "addr": 0x22499e, "bit": 0},158: { "levelId": 8, "mem": bit1(0x22499e),"good": 1, "addr": 0x22499e, "bit": 1},159: { "levelId": 8, "mem": bit6(0x22499a),"good": 1, "addr": 0x22499a, "bit": 6},160: { "levelId": 8, "mem": bit7(0x22499a),"good": 1, "addr": 0x22499a, "bit": 7},161: { "levelId": 8, "mem": bit0(0x22499b),"good": 1, "addr": 0x22499b, "bit": 0},162: { "levelId": 8, "mem": bit1(0x22499b),"good": 1, "addr": 0x22499b, "bit": 1},163: { "levelId": 8, "mem": bit2(0x22499b),"good": 1, "addr": 0x22499b, "bit": 2},164: { "levelId": 8, "mem": bit6(0x22499b),"good": 1, "addr": 0x22499b, "bit": 6},165: { "levelId": 8, "mem": bit7(0x22499b),"good": 1, "addr": 0x22499b, "bit": 7},166: { "levelId": 8, "mem": bit0(0x22499c),"good": 1, "addr": 0x22499c, "bit": 0},167: { "levelId": 8, "mem": bit1(0x22499c),"good": 1, "addr": 0x22499c, "bit": 1},168: { "levelId": 8, "mem": bit2(0x22499c),"good": 1, "addr": 0x22499c, "bit": 2},169: { "levelId": 8, "mem": bit3(0x22499c),"good": 1, "addr": 0x22499c, "bit": 3},170: { "levelId": 8, "mem": bit4(0x22499c),"good": 1, "addr": 0x22499c, "bit": 4},171: { "levelId": 8, "mem": bit2(0x22499e),"good": 1, "addr": 0x22499e, "bit": 2},172: { "levelId": 8, "mem": bit3(0x22499e),"good": 1, "addr": 0x22499e, "bit": 3},173: { "levelId": 8, "mem": bit4(0x22499e),"good": 1, "addr": 0x22499e, "bit": 4},174: { "levelId": 8, "mem": bit5(0x22499e),"good": 1, "addr": 0x22499e, "bit": 5},175: { "levelId": 8, "mem": bit6(0x22499e),"good": 1, "addr": 0x22499e, "bit": 6},176: { "levelId": 8, "mem": bit7(0x22499e),"good": 1, "addr": 0x22499e, "bit": 7},177: { "levelId": 8, "mem": bit0(0x22499f),"good": 1, "addr": 0x22499f, "bit": 0},178: { "levelId": 8, "mem": bit1(0x22499f),"good": 1, "addr": 0x22499f, "bit": 1},179: { "levelId": 8, "mem": bit2(0x22499f),"good": 1, "addr": 0x22499f, "bit": 2},180: { "levelId": 8, "mem": bit3(0x22499f),"good": 1, "addr": 0x22499f, "bit": 3},181: { "levelId": 8, "mem": bit4(0x22499f),"good": 1, "addr": 0x22499f, "bit": 4},182: { "levelId": 8, "mem": bit5(0x22499f),"good": 1, "addr": 0x22499f, "bit": 5},183: { "levelId": 8, "mem": bit6(0x22499f),"good": 1, "addr": 0x22499f, "bit": 6},184: { "levelId": 8, "mem": bit7(0x22499f),"good": 1, "addr": 0x22499f, "bit": 7},185: { "levelId": 8, "mem": bit0(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 0},186: { "levelId": 8, "mem": bit1(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 1},187: { "levelId": 8, "mem": bit2(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 2},188: { "levelId": 8, "mem": bit3(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 3},189: { "levelId": 8, "mem": bit4(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 4},190: { "levelId": 8, "mem": bit5(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 5},191: { "levelId": 8, "mem": bit6(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 6},192: { "levelId": 8, "mem": bit7(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 7},193: { "levelId": 10, "mem": bit0(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 0},194: { "levelId": 10, "mem": bit1(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 1},195: { "levelId": 10, "mem": bit2(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 2},196: { "levelId": 10, "mem": bit3(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 3},197: { "levelId": 10, "mem": bit4(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 4},198: { "levelId": 10, "mem": bit2(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 2},199: { "levelId": 10, "mem": bit3(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 3},200: { "levelId": 10, "mem": bit4(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 4},201: { "levelId": 10, "mem": bit5(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 5},202: { "levelId": 10, "mem": bit6(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 6},203: { "levelId": 10, "mem": bit1(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 1},204: { "levelId": 10, "mem": bit5(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 5},205: { "levelId": 10, "mem": bit6(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 6},206: { "levelId": 10, "mem": bit7(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 7},207: { "levelId": 10, "mem": bit0(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 0},208: { "levelId": 10, "mem": bit3(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 3},209: { "levelId": 10, "mem": bit5(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 5},210: { "levelId": 10, "mem": bit6(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 6},211: { "levelId": 10, "mem": bit7(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 7},212: { "levelId": 10, "mem": bit0(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 0},213: { "levelId": 10, "mem": bit1(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 1},214: { "levelId": 10, "mem": bit2(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 2},215: { "levelId": 10, "mem": bit4(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 4},216: { "levelId": 11, "mem": bit6(0x2249e5),"good": 1, "addr": 0x2249e5, "bit": 6},217: { "levelId": 11, "mem": bit7(0x2249e5),"good": 1, "addr": 0x2249e5, "bit": 7},218: { "levelId": 11, "mem": bit0(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 0},219: { "levelId": 11, "mem": bit1(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 1},220: { "levelId": 11, "mem": bit2(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 2},221: { "levelId": 11, "mem": bit3(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 3},222: { "levelId": 11, "mem": bit4(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 4},223: { "levelId": 11, "mem": bit5(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 5},224: { "levelId": 11, "mem": bit6(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 6},225: { "levelId": 11, "mem": bit7(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 7},226: { "levelId": 11, "mem": bit0(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 0},227: { "levelId": 11, "mem": bit1(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 1},228: { "levelId": 11, "mem": bit2(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 2},229: { "levelId": 11, "mem": bit3(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 3},230: { "levelId": 11, "mem": bit4(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 4},231: { "levelId": 11, "mem": bit5(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 5},232: { "levelId": 11, "mem": bit6(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 6},233: { "levelId": 11, "mem": bit7(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 7},234: { "levelId": 11, "mem": bit0(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 0},235: { "levelId": 11, "mem": bit1(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 1},236: { "levelId": 11, "mem": bit2(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 2},237: { "levelId": 11, "mem": bit3(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 3},238: { "levelId": 11, "mem": bit4(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 4},239: { "levelId": 11, "mem": bit5(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 5},240: { "levelId": 11, "mem": bit6(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 6},241: { "levelId": 11, "mem": bit7(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 7},242: { "levelId": 11, "mem": bit0(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 0},243: { "levelId": 11, "mem": bit1(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 1},244: { "levelId": 11, "mem": bit2(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 2},245: { "levelId": 11, "mem": bit3(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 3},246: { "levelId": 11, "mem": bit4(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 4},247: { "levelId": 11, "mem": bit5(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 5},248: { "levelId": 11, "mem": bit6(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 6},249: { "levelId": 11, "mem": bit7(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 7},250: { "levelId": 11, "mem": bit0(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 0},251: { "levelId": 11, "mem": bit1(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 1},252: { "levelId": 11, "mem": bit2(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 2},253: { "levelId": 11, "mem": bit3(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 3},254: { "levelId": 11, "mem": bit4(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 4},255: { "levelId": 11, "mem": bit5(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 5},256: { "levelId": 11, "mem": bit6(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 6},257: { "levelId": 11, "mem": bit7(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 7},258: { "levelId": 11, "mem": bit0(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 0},259: { "levelId": 11, "mem": bit1(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 1},260: { "levelId": 11, "mem": bit2(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 2},261: { "levelId": 11, "mem": bit3(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 3},262: { "levelId": 11, "mem": bit4(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 4},263: { "levelId": 11, "mem": bit5(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 5},264: { "levelId": 11, "mem": bit6(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 6},265: { "levelId": 11, "mem": bit7(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 7},266: { "levelId": 10, "mem": bit2(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 2},267: { "levelId": 10, "mem": bit2(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 2},268: { "levelId": 10, "mem": bit3(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 3},269: { "levelId": 10, "mem": bit4(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 4},270: { "levelId": 10, "mem": bit0(0x2249a6),"good": 1, "addr": 0x2249a6, "bit": 0},271: { "levelId": 10, "mem": bit1(0x2249a6),"good": 1, "addr": 0x2249a6, "bit": 1},272: { "levelId": 10, "mem": bit2(0x2249a6),"good": 1, "addr": 0x2249a6, "bit": 2},273: { "levelId": 10, "mem": bit3(0x2249a6),"good": 1, "addr": 0x2249a6, "bit": 3},274: { "levelId": 10, "mem": bit6(0x2249a6),"good": 1, "addr": 0x2249a6, "bit": 6},275: { "levelId": 10, "mem": bit7(0x2249a6),"good": 1, "addr": 0x2249a6, "bit": 7},276: { "levelId": 10, "mem": bit0(0x2249a7),"good": 1, "addr": 0x2249a7, "bit": 0},277: { "levelId": 10, "mem": bit1(0x2249a7),"good": 1, "addr": 0x2249a7, "bit": 1},278: { "levelId": 10, "mem": bit5(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 5},279: { "levelId": 10, "mem": bit6(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 6},280: { "levelId": 10, "mem": bit7(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 7},281: { "levelId": 10, "mem": bit0(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 0},282: { "levelId": 10, "mem": bit1(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 1},283: { "levelId": 10, "mem": bit7(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 7},284: { "levelId": 10, "mem": bit0(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 0},285: { "levelId": 10, "mem": bit1(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 1},286: { "levelId": 10, "mem": bit3(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 3},287: { "levelId": 10, "mem": bit4(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 4},288: { "levelId": 10, "mem": bit5(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 5},289: { "levelId": 10, "mem": bit6(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 6},290: { "levelId": 10, "mem": bit7(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 7},291: { "levelId": 10, "mem": bit4(0x2249a6),"good": 1, "addr": 0x2249a6, "bit": 4},292: { "levelId": 10, "mem": bit5(0x2249a6),"good": 1, "addr": 0x2249a6, "bit": 5},293: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},294: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},295: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},296: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},297: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},298: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},299: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},300: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},301: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},302: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},303: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},304: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},305: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},306: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},307: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},308: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},309: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},310: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},311: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},312: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},313: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},314: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},315: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},316: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},317: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},318: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},319: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},320: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},321: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},322: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},323: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},324: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},325: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},326: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},327: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},328: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},329: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},330: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},331: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},332: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},333: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},334: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},335: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},336: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},337: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},338: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},339: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},340: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},341: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},342: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},343: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},344: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},345: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},346: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},347: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},348: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},349: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},350: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},351: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},352: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},353: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},354: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},355: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},356: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},357: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},358: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},359: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},360: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},361: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},362: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},363: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},364: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},365: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},366: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},367: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},368: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},369: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},370: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},371: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},372: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},373: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},374: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},375: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},376: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},377: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},378: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},379: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},380: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},381: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},382: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},383: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},384: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},385: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},386: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},387: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},388: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},389: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},390: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},391: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},392: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},393: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},394: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},395: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},396: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},397: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},398: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},399: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},400: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},401: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},402: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},403: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},404: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},405: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},406: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},407: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},408: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},409: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},410: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},411: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},412: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},413: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},414: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},415: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},416: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},417: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},418: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},419: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},420: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},421: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},422: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},423: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},424: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},425: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},426: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},427: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},428: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},429: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},430: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},431: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},432: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},433: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},434: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},435: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},436: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},437: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},438: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},439: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},440: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},441: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},442: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},443: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},444: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},445: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},446: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},447: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},448: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},449: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},450: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},451: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},452: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},453: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},454: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},455: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},456: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},457: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},458: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},459: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},460: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},461: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},462: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},463: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},464: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},465: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},466: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},467: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},468: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},469: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},470: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},471: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},472: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},473: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},474: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},475: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},476: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},477: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},478: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},479: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},480: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},481: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},482: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},483: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},484: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},485: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},486: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},487: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},488: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},489: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},490: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},491: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},492: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},493: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},494: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},495: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},496: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},497: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},498: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},499: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},500: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},501: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},502: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},503: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},504: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},505: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},506: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},507: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},508: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},509: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},510: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},511: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},512: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},513: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},514: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},515: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},516: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},517: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},518: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},519: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},520: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},521: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},522: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},523: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},524: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},525: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},526: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},527: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},528: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},529: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},530: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},531: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},532: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},533: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},534: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},535: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},536: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},537: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},538: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},539: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},540: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},541: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},542: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},543: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},544: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},545: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},546: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},547: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},548: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},549: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},550: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},551: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},552: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},553: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},554: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},555: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},556: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},557: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},558: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},559: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},560: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},561: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},562: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},563: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},564: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},565: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},566: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},567: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},568: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},569: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},570: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},571: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},572: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},573: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},574: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},575: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},576: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},577: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},578: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},579: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},580: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},581: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},582: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},583: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},584: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},585: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},586: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},587: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},588: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},589: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},590: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},591: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},592: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},593: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},594: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},595: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},596: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},597: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},598: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},599: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},600: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},601: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},602: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},603: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},604: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},605: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},606: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},607: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},608: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},609: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},610: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},611: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},612: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},613: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},614: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},615: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},616: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},617: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},618: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},619: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},620: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},621: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},622: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},623: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},624: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},625: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},626: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},627: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},628: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},629: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},630: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},631: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},632: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},633: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},634: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},635: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},636: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},637: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},638: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},639: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},640: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},641: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},642: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},643: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},644: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},645: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},646: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},647: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},648: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},649: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},650: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},651: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},652: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},653: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},654: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},655: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},656: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},657: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},658: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},659: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},660: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},661: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},662: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},663: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},664: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},665: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},666: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},667: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},668: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},669: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},670: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},671: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},672: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},673: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},674: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},675: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},676: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},677: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},678: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},679: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},680: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},681: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},682: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},683: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},684: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},685: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},686: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},687: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},688: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},689: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},690: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},691: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},692: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},693: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},694: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},695: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},696: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},697: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},698: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},699: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},700: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},701: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},702: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},703: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},704: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},705: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},706: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},707: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},708: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},709: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},710: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},711: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},712: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},713: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},714: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},715: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},716: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},717: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},718: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},719: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},720: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},721: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},722: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},723: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},724: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},725: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},726: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},727: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},728: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},729: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},730: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},731: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},732: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},733: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},734: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},735: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},736: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},737: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},738: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},739: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},740: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},741: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},742: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},743: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},744: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},745: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},746: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},747: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},748: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},749: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},750: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},751: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},752: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},753: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},754: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},755: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},756: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},757: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},758: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},759: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},760: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},761: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},762: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},763: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},764: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},765: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},766: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},767: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},768: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},769: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},770: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},771: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},772: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},773: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},774: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},775: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},776: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},777: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},778: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},779: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},780: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},781: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},782: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},783: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},784: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},785: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},786: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},787: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},788: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},789: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},790: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},791: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},792: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},793: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},794: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},795: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},796: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},797: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},798: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},799: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},800: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},801: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},802: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},803: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},804: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},805: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},806: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},807: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},808: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},809: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},810: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},811: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},812: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},813: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},814: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},815: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},816: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},817: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},818: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},819: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},820: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},821: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},822: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},823: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},824: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},825: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},826: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},827: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},828: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},829: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},830: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},831: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},832: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},833: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},834: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},835: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},836: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},837: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},838: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},839: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},840: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},841: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},842: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},843: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},844: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},845: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},846: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},847: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},848: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},849: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},850: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},851: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},852: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},853: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},854: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},855: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},856: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},857: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},858: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},859: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},860: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},861: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},862: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},863: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},864: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},865: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},866: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},867: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},868: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},869: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},870: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},871: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},872: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},873: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},874: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},875: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},876: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},877: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},878: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},879: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},880: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},881: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},882: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},883: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},884: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},885: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},886: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},887: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},888: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},889: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},890: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},891: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},892: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},893: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},894: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},895: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},896: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},897: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},898: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},899: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},900: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},901: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},902: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},903: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},904: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},905: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},906: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},907: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},908: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},909: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},910: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},911: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},912: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},913: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},914: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},915: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},916: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},917: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},918: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},919: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},920: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},921: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},922: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},923: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},924: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},925: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},926: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},927: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},928: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},929: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},930: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},931: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},932: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},933: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},934: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},935: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},936: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},937: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},938: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},939: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},940: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},941: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},942: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},943: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},944: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},945: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},946: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},947: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},948: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},949: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},950: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},951: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},952: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},953: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},954: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},955: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},956: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},957: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},958: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},959: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},960: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},961: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},962: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},963: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},964: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},965: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},966: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},967: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},968: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},969: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},970: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},971: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},972: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},973: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},974: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},975: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},976: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},977: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},978: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},979: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},980: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},981: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},982: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},983: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},984: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},985: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},986: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},987: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},988: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},989: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},990: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},991: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},992: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},993: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},994: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},995: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},996: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},997: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},998: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},999: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},1000: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0</v>
@@ -7883,7 +7910,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1</v>
@@ -7899,7 +7926,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>2</v>
@@ -7915,7 +7942,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>3</v>
@@ -7931,7 +7958,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>4</v>
@@ -7947,7 +7974,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>5</v>
@@ -7963,7 +7990,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>6</v>
@@ -7979,7 +8006,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>7</v>
@@ -7995,7 +8022,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>2</v>
@@ -8010,7 +8037,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>1</v>
@@ -8025,7 +8052,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>2</v>
@@ -8040,7 +8067,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>3</v>
@@ -8055,7 +8082,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>4</v>
@@ -8070,7 +8097,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>5</v>
@@ -8085,7 +8112,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>6</v>
@@ -8100,7 +8127,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>7</v>
@@ -8115,7 +8142,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>5</v>
@@ -8130,7 +8157,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>6</v>
@@ -8145,7 +8172,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>7</v>
@@ -8160,7 +8187,7 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>0</v>
@@ -8175,7 +8202,7 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="6" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>1</v>
@@ -8190,7 +8217,7 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>2</v>
@@ -8205,7 +8232,7 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>3</v>
@@ -8220,7 +8247,7 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="6" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>4</v>
@@ -8235,7 +8262,7 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="6" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>5</v>
@@ -8250,7 +8277,7 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="6" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>6</v>
@@ -8265,7 +8292,7 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="6" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>7</v>
@@ -8280,7 +8307,7 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="6" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>0</v>
@@ -8295,7 +8322,7 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="6" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>1</v>
@@ -8310,7 +8337,7 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="6" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>2</v>
@@ -8325,7 +8352,7 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="6" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>3</v>
@@ -8340,7 +8367,7 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="6" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>4</v>
@@ -8355,7 +8382,7 @@
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="6" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>5</v>
@@ -8370,7 +8397,7 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="6" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>6</v>
@@ -8385,7 +8412,7 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="6" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>7</v>
@@ -8400,7 +8427,7 @@
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="6" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>0</v>
@@ -8415,7 +8442,7 @@
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="6" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>1</v>
@@ -8430,7 +8457,7 @@
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>2</v>
@@ -8445,7 +8472,7 @@
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>3</v>
@@ -8460,7 +8487,7 @@
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>4</v>
@@ -8475,7 +8502,7 @@
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>5</v>
@@ -8490,7 +8517,7 @@
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>6</v>
@@ -8505,7 +8532,7 @@
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B44" s="0" t="n">
         <v>7</v>
@@ -8520,7 +8547,7 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B45" s="0" t="n">
         <v>0</v>
@@ -8535,7 +8562,7 @@
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B46" s="0" t="n">
         <v>1</v>
@@ -8550,7 +8577,7 @@
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B47" s="0" t="n">
         <v>2</v>
@@ -8565,7 +8592,7 @@
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B48" s="0" t="n">
         <v>3</v>
@@ -8580,7 +8607,7 @@
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B49" s="0" t="n">
         <v>4</v>
@@ -8595,7 +8622,7 @@
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B50" s="0" t="n">
         <v>5</v>
@@ -8610,7 +8637,7 @@
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B51" s="0" t="n">
         <v>6</v>
@@ -8625,7 +8652,7 @@
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B52" s="0" t="n">
         <v>7</v>
@@ -8640,7 +8667,7 @@
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B53" s="0" t="n">
         <v>0</v>
@@ -8655,7 +8682,7 @@
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B54" s="0" t="n">
         <v>1</v>
@@ -8670,7 +8697,7 @@
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B55" s="0" t="n">
         <v>2</v>
@@ -8685,7 +8712,7 @@
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B56" s="0" t="n">
         <v>3</v>
@@ -8700,7 +8727,7 @@
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B57" s="0" t="n">
         <v>4</v>
@@ -8715,7 +8742,7 @@
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B58" s="0" t="n">
         <v>5</v>
@@ -8730,7 +8757,7 @@
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B59" s="0" t="n">
         <v>6</v>
@@ -8745,7 +8772,7 @@
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B60" s="0" t="n">
         <v>7</v>
@@ -8760,7 +8787,7 @@
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B61" s="0" t="n">
         <v>0</v>
@@ -8775,7 +8802,7 @@
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B62" s="0" t="n">
         <v>1</v>
@@ -8790,7 +8817,7 @@
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B63" s="0" t="n">
         <v>2</v>
@@ -8805,7 +8832,7 @@
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B64" s="0" t="n">
         <v>3</v>
@@ -8820,7 +8847,7 @@
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B65" s="0" t="n">
         <v>4</v>
@@ -8835,7 +8862,7 @@
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B66" s="0" t="n">
         <v>5</v>
@@ -8850,7 +8877,7 @@
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B67" s="0" t="n">
         <v>6</v>
@@ -8865,7 +8892,7 @@
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B68" s="0" t="n">
         <v>7</v>
@@ -8880,7 +8907,7 @@
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B69" s="0" t="n">
         <v>0</v>
@@ -8895,7 +8922,7 @@
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B70" s="0" t="n">
         <v>1</v>
@@ -8910,7 +8937,7 @@
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B71" s="0" t="n">
         <v>2</v>
@@ -8925,7 +8952,7 @@
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B72" s="0" t="n">
         <v>3</v>
@@ -8940,7 +8967,7 @@
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B73" s="0" t="n">
         <v>4</v>
@@ -8955,7 +8982,7 @@
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B74" s="0" t="n">
         <v>5</v>
@@ -8970,7 +8997,7 @@
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B75" s="0" t="n">
         <v>6</v>
@@ -8985,7 +9012,7 @@
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B76" s="0" t="n">
         <v>7</v>
@@ -9000,7 +9027,7 @@
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B77" s="0" t="n">
         <v>0</v>
@@ -9015,7 +9042,7 @@
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B78" s="0" t="n">
         <v>1</v>
@@ -9030,7 +9057,7 @@
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B79" s="0" t="n">
         <v>2</v>
@@ -9045,7 +9072,7 @@
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B80" s="0" t="n">
         <v>3</v>
@@ -9060,7 +9087,7 @@
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B81" s="0" t="n">
         <v>4</v>
@@ -9075,7 +9102,7 @@
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B82" s="0" t="n">
         <v>5</v>
@@ -9090,7 +9117,7 @@
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B83" s="0" t="n">
         <v>6</v>
@@ -9105,7 +9132,7 @@
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B84" s="0" t="n">
         <v>7</v>
@@ -9120,7 +9147,7 @@
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="6" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B85" s="0" t="n">
         <v>0</v>
@@ -9135,7 +9162,7 @@
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="6" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B86" s="0" t="n">
         <v>1</v>
@@ -9150,7 +9177,7 @@
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="6" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B87" s="0" t="n">
         <v>2</v>
@@ -9165,7 +9192,7 @@
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="6" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B88" s="0" t="n">
         <v>3</v>
@@ -9180,7 +9207,7 @@
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B89" s="0" t="n">
         <v>4</v>
@@ -9195,7 +9222,7 @@
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B90" s="0" t="n">
         <v>5</v>
@@ -9210,7 +9237,7 @@
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B91" s="0" t="n">
         <v>6</v>
@@ -9225,7 +9252,7 @@
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B92" s="0" t="n">
         <v>7</v>
@@ -9240,7 +9267,7 @@
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B93" s="0" t="n">
         <v>0</v>
@@ -9255,7 +9282,7 @@
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B94" s="0" t="n">
         <v>1</v>
@@ -9270,7 +9297,7 @@
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B95" s="0" t="n">
         <v>2</v>
@@ -9285,7 +9312,7 @@
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B96" s="0" t="n">
         <v>3</v>
@@ -9300,7 +9327,7 @@
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B97" s="0" t="n">
         <v>4</v>
@@ -9315,7 +9342,7 @@
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B98" s="0" t="n">
         <v>5</v>
@@ -9330,7 +9357,7 @@
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B99" s="0" t="n">
         <v>6</v>
@@ -9345,7 +9372,7 @@
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B100" s="0" t="n">
         <v>7</v>
@@ -9360,7 +9387,7 @@
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B101" s="0" t="n">
         <v>0</v>
@@ -9375,7 +9402,7 @@
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B102" s="0" t="n">
         <v>1</v>
@@ -9390,7 +9417,7 @@
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B103" s="0" t="n">
         <v>2</v>
@@ -9405,7 +9432,7 @@
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B104" s="0" t="n">
         <v>3</v>
@@ -9420,7 +9447,7 @@
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B105" s="0" t="n">
         <v>4</v>
@@ -9435,7 +9462,7 @@
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B106" s="0" t="n">
         <v>5</v>
@@ -9450,7 +9477,7 @@
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B107" s="0" t="n">
         <v>6</v>
@@ -9465,7 +9492,7 @@
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B108" s="0" t="n">
         <v>7</v>
@@ -9480,7 +9507,7 @@
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B109" s="0" t="n">
         <v>0</v>
@@ -9495,7 +9522,7 @@
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B110" s="0" t="n">
         <v>1</v>
@@ -9510,7 +9537,7 @@
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B111" s="0" t="n">
         <v>2</v>
@@ -9525,7 +9552,7 @@
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B112" s="0" t="n">
         <v>3</v>
@@ -9540,7 +9567,7 @@
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B113" s="0" t="n">
         <v>4</v>
@@ -9555,7 +9582,7 @@
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B114" s="0" t="n">
         <v>5</v>
@@ -9570,7 +9597,7 @@
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B115" s="0" t="n">
         <v>6</v>
@@ -9585,7 +9612,7 @@
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B116" s="0" t="n">
         <v>7</v>
@@ -9600,7 +9627,7 @@
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B117" s="0" t="n">
         <v>0</v>
@@ -9615,7 +9642,7 @@
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B118" s="0" t="n">
         <v>1</v>
@@ -9630,7 +9657,7 @@
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B119" s="0" t="n">
         <v>2</v>
@@ -9645,7 +9672,7 @@
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B120" s="0" t="n">
         <v>3</v>
@@ -9660,7 +9687,7 @@
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B121" s="0" t="n">
         <v>4</v>
@@ -9675,7 +9702,7 @@
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B122" s="0" t="n">
         <v>5</v>
@@ -9690,7 +9717,7 @@
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B123" s="0" t="n">
         <v>6</v>
@@ -9705,7 +9732,7 @@
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B124" s="0" t="n">
         <v>0</v>
@@ -9720,7 +9747,7 @@
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B125" s="0" t="n">
         <v>1</v>
@@ -9735,7 +9762,7 @@
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B126" s="0" t="n">
         <v>2</v>
@@ -9750,7 +9777,7 @@
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B127" s="0" t="n">
         <v>3</v>
@@ -9765,7 +9792,7 @@
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B128" s="0" t="n">
         <v>4</v>
@@ -9780,7 +9807,7 @@
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B129" s="0" t="n">
         <v>5</v>
@@ -9795,7 +9822,7 @@
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B130" s="0" t="n">
         <v>6</v>
@@ -9810,7 +9837,7 @@
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B131" s="0" t="n">
         <v>7</v>
@@ -9825,7 +9852,7 @@
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B132" s="0" t="n">
         <v>0</v>
@@ -9840,7 +9867,7 @@
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B133" s="0" t="n">
         <v>1</v>
@@ -9855,7 +9882,7 @@
     </row>
     <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B134" s="0" t="n">
         <v>2</v>
@@ -9870,7 +9897,7 @@
     </row>
     <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B135" s="0" t="n">
         <v>3</v>
@@ -9885,7 +9912,7 @@
     </row>
     <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B136" s="0" t="n">
         <v>4</v>
@@ -9900,7 +9927,7 @@
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B137" s="0" t="n">
         <v>5</v>
@@ -9915,7 +9942,7 @@
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="6" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B138" s="0" t="n">
         <v>3</v>
@@ -9930,7 +9957,7 @@
     </row>
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B139" s="0" t="n">
         <v>4</v>
@@ -9945,7 +9972,7 @@
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B140" s="0" t="n">
         <v>5</v>
@@ -9960,7 +9987,7 @@
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B141" s="0" t="n">
         <v>6</v>
@@ -9975,7 +10002,7 @@
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B142" s="0" t="n">
         <v>7</v>
@@ -9990,7 +10017,7 @@
     </row>
     <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B143" s="0" t="n">
         <v>7</v>
@@ -10005,7 +10032,7 @@
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B144" s="0" t="n">
         <v>3</v>
@@ -10020,7 +10047,7 @@
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B145" s="0" t="n">
         <v>4</v>
@@ -10035,7 +10062,7 @@
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B146" s="0" t="n">
         <v>5</v>
@@ -10050,7 +10077,7 @@
     </row>
     <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B147" s="0" t="n">
         <v>5</v>
@@ -10065,7 +10092,7 @@
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B148" s="0" t="n">
         <v>6</v>
@@ -10080,7 +10107,7 @@
     </row>
     <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B149" s="0" t="n">
         <v>7</v>
@@ -10095,7 +10122,7 @@
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B150" s="0" t="n">
         <v>0</v>
@@ -10110,7 +10137,7 @@
     </row>
     <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B151" s="0" t="n">
         <v>1</v>
@@ -10125,7 +10152,7 @@
     </row>
     <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B152" s="0" t="n">
         <v>2</v>
@@ -10140,7 +10167,7 @@
     </row>
     <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B153" s="0" t="n">
         <v>3</v>
@@ -10155,7 +10182,7 @@
     </row>
     <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B154" s="0" t="n">
         <v>4</v>
@@ -10170,7 +10197,7 @@
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B155" s="0" t="n">
         <v>5</v>
@@ -10185,7 +10212,7 @@
     </row>
     <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B156" s="0" t="n">
         <v>6</v>
@@ -10200,7 +10227,7 @@
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B157" s="0" t="n">
         <v>7</v>
@@ -10215,7 +10242,7 @@
     </row>
     <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B158" s="0" t="n">
         <v>0</v>
@@ -10230,7 +10257,7 @@
     </row>
     <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B159" s="0" t="n">
         <v>1</v>
@@ -10245,7 +10272,7 @@
     </row>
     <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B160" s="0" t="n">
         <v>6</v>
@@ -10260,7 +10287,7 @@
     </row>
     <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B161" s="0" t="n">
         <v>7</v>
@@ -10275,7 +10302,7 @@
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B162" s="0" t="n">
         <v>0</v>
@@ -10290,7 +10317,7 @@
     </row>
     <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B163" s="0" t="n">
         <v>1</v>
@@ -10305,7 +10332,7 @@
     </row>
     <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B164" s="0" t="n">
         <v>2</v>
@@ -10320,7 +10347,7 @@
     </row>
     <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B165" s="0" t="n">
         <v>6</v>
@@ -10335,7 +10362,7 @@
     </row>
     <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B166" s="0" t="n">
         <v>7</v>
@@ -10350,7 +10377,7 @@
     </row>
     <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B167" s="0" t="n">
         <v>0</v>
@@ -10365,7 +10392,7 @@
     </row>
     <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B168" s="0" t="n">
         <v>1</v>
@@ -10380,7 +10407,7 @@
     </row>
     <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B169" s="0" t="n">
         <v>2</v>
@@ -10395,7 +10422,7 @@
     </row>
     <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B170" s="0" t="n">
         <v>3</v>
@@ -10410,7 +10437,7 @@
     </row>
     <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B171" s="0" t="n">
         <v>4</v>
@@ -10425,7 +10452,7 @@
     </row>
     <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B172" s="0" t="n">
         <v>2</v>
@@ -10440,7 +10467,7 @@
     </row>
     <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B173" s="0" t="n">
         <v>3</v>
@@ -10455,7 +10482,7 @@
     </row>
     <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B174" s="0" t="n">
         <v>4</v>
@@ -10470,7 +10497,7 @@
     </row>
     <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B175" s="0" t="n">
         <v>5</v>
@@ -10485,7 +10512,7 @@
     </row>
     <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B176" s="0" t="n">
         <v>6</v>
@@ -10500,7 +10527,7 @@
     </row>
     <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B177" s="0" t="n">
         <v>7</v>
@@ -10515,7 +10542,7 @@
     </row>
     <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B178" s="0" t="n">
         <v>0</v>
@@ -10530,7 +10557,7 @@
     </row>
     <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B179" s="0" t="n">
         <v>1</v>
@@ -10545,7 +10572,7 @@
     </row>
     <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B180" s="0" t="n">
         <v>2</v>
@@ -10560,7 +10587,7 @@
     </row>
     <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B181" s="0" t="n">
         <v>3</v>
@@ -10575,7 +10602,7 @@
     </row>
     <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B182" s="0" t="n">
         <v>4</v>
@@ -10590,7 +10617,7 @@
     </row>
     <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B183" s="0" t="n">
         <v>5</v>
@@ -10605,7 +10632,7 @@
     </row>
     <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B184" s="0" t="n">
         <v>6</v>
@@ -10620,7 +10647,7 @@
     </row>
     <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B185" s="0" t="n">
         <v>7</v>
@@ -10635,7 +10662,7 @@
     </row>
     <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B186" s="0" t="n">
         <v>0</v>
@@ -10650,7 +10677,7 @@
     </row>
     <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B187" s="0" t="n">
         <v>1</v>
@@ -10665,7 +10692,7 @@
     </row>
     <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B188" s="0" t="n">
         <v>2</v>
@@ -10680,7 +10707,7 @@
     </row>
     <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B189" s="0" t="n">
         <v>3</v>
@@ -10695,7 +10722,7 @@
     </row>
     <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B190" s="0" t="n">
         <v>4</v>
@@ -10710,7 +10737,7 @@
     </row>
     <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B191" s="0" t="n">
         <v>5</v>
@@ -10725,7 +10752,7 @@
     </row>
     <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B192" s="0" t="n">
         <v>6</v>
@@ -10740,7 +10767,7 @@
     </row>
     <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B193" s="0" t="n">
         <v>7</v>
@@ -10755,7 +10782,7 @@
     </row>
     <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B194" s="0" t="n">
         <v>0</v>
@@ -10770,7 +10797,7 @@
     </row>
     <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B195" s="0" t="n">
         <v>1</v>
@@ -10785,7 +10812,7 @@
     </row>
     <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B196" s="0" t="n">
         <v>2</v>
@@ -10800,7 +10827,7 @@
     </row>
     <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B197" s="0" t="n">
         <v>3</v>
@@ -10815,7 +10842,7 @@
     </row>
     <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B198" s="0" t="n">
         <v>4</v>
@@ -10830,7 +10857,7 @@
     </row>
     <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B199" s="0" t="n">
         <v>2</v>
@@ -10845,7 +10872,7 @@
     </row>
     <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B200" s="0" t="n">
         <v>3</v>
@@ -10860,7 +10887,7 @@
     </row>
     <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B201" s="0" t="n">
         <v>4</v>
@@ -10875,7 +10902,7 @@
     </row>
     <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B202" s="0" t="n">
         <v>5</v>
@@ -10890,7 +10917,7 @@
     </row>
     <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B203" s="0" t="n">
         <v>6</v>
@@ -10905,7 +10932,7 @@
     </row>
     <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B204" s="0" t="n">
         <v>1</v>
@@ -10920,7 +10947,7 @@
     </row>
     <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B205" s="0" t="n">
         <v>5</v>
@@ -10935,7 +10962,7 @@
     </row>
     <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B206" s="0" t="n">
         <v>6</v>
@@ -10950,7 +10977,7 @@
     </row>
     <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B207" s="0" t="n">
         <v>7</v>
@@ -10965,7 +10992,7 @@
     </row>
     <row r="208" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B208" s="0" t="n">
         <v>0</v>
@@ -10980,7 +11007,7 @@
     </row>
     <row r="209" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B209" s="0" t="n">
         <v>3</v>
@@ -10995,7 +11022,7 @@
     </row>
     <row r="210" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B210" s="0" t="n">
         <v>5</v>
@@ -11010,7 +11037,7 @@
     </row>
     <row r="211" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B211" s="0" t="n">
         <v>6</v>
@@ -11025,7 +11052,7 @@
     </row>
     <row r="212" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B212" s="0" t="n">
         <v>7</v>
@@ -11040,7 +11067,7 @@
     </row>
     <row r="213" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B213" s="0" t="n">
         <v>0</v>
@@ -11055,7 +11082,7 @@
     </row>
     <row r="214" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B214" s="0" t="n">
         <v>1</v>
@@ -11070,7 +11097,7 @@
     </row>
     <row r="215" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B215" s="0" t="n">
         <v>2</v>
@@ -11085,7 +11112,7 @@
     </row>
     <row r="216" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B216" s="0" t="n">
         <v>4</v>
@@ -11100,7 +11127,7 @@
     </row>
     <row r="217" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B217" s="0" t="n">
         <v>6</v>
@@ -11115,7 +11142,7 @@
     </row>
     <row r="218" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B218" s="0" t="n">
         <v>7</v>
@@ -11130,7 +11157,7 @@
     </row>
     <row r="219" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B219" s="0" t="n">
         <v>0</v>
@@ -11145,7 +11172,7 @@
     </row>
     <row r="220" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B220" s="0" t="n">
         <v>1</v>
@@ -11160,7 +11187,7 @@
     </row>
     <row r="221" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B221" s="0" t="n">
         <v>2</v>
@@ -11175,7 +11202,7 @@
     </row>
     <row r="222" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B222" s="0" t="n">
         <v>3</v>
@@ -11190,7 +11217,7 @@
     </row>
     <row r="223" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B223" s="0" t="n">
         <v>4</v>
@@ -11205,7 +11232,7 @@
     </row>
     <row r="224" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B224" s="0" t="n">
         <v>5</v>
@@ -11220,7 +11247,7 @@
     </row>
     <row r="225" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B225" s="0" t="n">
         <v>6</v>
@@ -11235,7 +11262,7 @@
     </row>
     <row r="226" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B226" s="0" t="n">
         <v>7</v>
@@ -11250,7 +11277,7 @@
     </row>
     <row r="227" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B227" s="0" t="n">
         <v>0</v>
@@ -11265,7 +11292,7 @@
     </row>
     <row r="228" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B228" s="0" t="n">
         <v>1</v>
@@ -11280,7 +11307,7 @@
     </row>
     <row r="229" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B229" s="0" t="n">
         <v>2</v>
@@ -11295,7 +11322,7 @@
     </row>
     <row r="230" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B230" s="0" t="n">
         <v>3</v>
@@ -11310,7 +11337,7 @@
     </row>
     <row r="231" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B231" s="0" t="n">
         <v>4</v>
@@ -11325,7 +11352,7 @@
     </row>
     <row r="232" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B232" s="0" t="n">
         <v>5</v>
@@ -11340,7 +11367,7 @@
     </row>
     <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B233" s="0" t="n">
         <v>6</v>
@@ -11355,7 +11382,7 @@
     </row>
     <row r="234" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B234" s="0" t="n">
         <v>7</v>
@@ -11370,7 +11397,7 @@
     </row>
     <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B235" s="0" t="n">
         <v>0</v>
@@ -11385,7 +11412,7 @@
     </row>
     <row r="236" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B236" s="0" t="n">
         <v>1</v>
@@ -11400,7 +11427,7 @@
     </row>
     <row r="237" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B237" s="0" t="n">
         <v>2</v>
@@ -11415,7 +11442,7 @@
     </row>
     <row r="238" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B238" s="0" t="n">
         <v>3</v>
@@ -11430,7 +11457,7 @@
     </row>
     <row r="239" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B239" s="0" t="n">
         <v>4</v>
@@ -11445,7 +11472,7 @@
     </row>
     <row r="240" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B240" s="0" t="n">
         <v>5</v>
@@ -11460,7 +11487,7 @@
     </row>
     <row r="241" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B241" s="0" t="n">
         <v>6</v>
@@ -11475,7 +11502,7 @@
     </row>
     <row r="242" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B242" s="0" t="n">
         <v>7</v>
@@ -11490,7 +11517,7 @@
     </row>
     <row r="243" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B243" s="0" t="n">
         <v>0</v>
@@ -11505,7 +11532,7 @@
     </row>
     <row r="244" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B244" s="0" t="n">
         <v>1</v>
@@ -11520,7 +11547,7 @@
     </row>
     <row r="245" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B245" s="0" t="n">
         <v>2</v>
@@ -11535,7 +11562,7 @@
     </row>
     <row r="246" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B246" s="0" t="n">
         <v>3</v>
@@ -11550,7 +11577,7 @@
     </row>
     <row r="247" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B247" s="0" t="n">
         <v>4</v>
@@ -11565,7 +11592,7 @@
     </row>
     <row r="248" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B248" s="0" t="n">
         <v>5</v>
@@ -11580,7 +11607,7 @@
     </row>
     <row r="249" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B249" s="0" t="n">
         <v>6</v>
@@ -11595,7 +11622,7 @@
     </row>
     <row r="250" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B250" s="0" t="n">
         <v>7</v>
@@ -11610,7 +11637,7 @@
     </row>
     <row r="251" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B251" s="0" t="n">
         <v>0</v>
@@ -11625,7 +11652,7 @@
     </row>
     <row r="252" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B252" s="0" t="n">
         <v>1</v>
@@ -11640,7 +11667,7 @@
     </row>
     <row r="253" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B253" s="0" t="n">
         <v>2</v>
@@ -11655,7 +11682,7 @@
     </row>
     <row r="254" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B254" s="0" t="n">
         <v>3</v>
@@ -11670,7 +11697,7 @@
     </row>
     <row r="255" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B255" s="0" t="n">
         <v>4</v>
@@ -11685,7 +11712,7 @@
     </row>
     <row r="256" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B256" s="0" t="n">
         <v>5</v>
@@ -11700,7 +11727,7 @@
     </row>
     <row r="257" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B257" s="0" t="n">
         <v>6</v>
@@ -11715,7 +11742,7 @@
     </row>
     <row r="258" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B258" s="0" t="n">
         <v>7</v>
@@ -11730,7 +11757,7 @@
     </row>
     <row r="259" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B259" s="0" t="n">
         <v>0</v>
@@ -11745,7 +11772,7 @@
     </row>
     <row r="260" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B260" s="0" t="n">
         <v>1</v>
@@ -11760,7 +11787,7 @@
     </row>
     <row r="261" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B261" s="0" t="n">
         <v>2</v>
@@ -11775,7 +11802,7 @@
     </row>
     <row r="262" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B262" s="0" t="n">
         <v>3</v>
@@ -11790,7 +11817,7 @@
     </row>
     <row r="263" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B263" s="0" t="n">
         <v>4</v>
@@ -11805,7 +11832,7 @@
     </row>
     <row r="264" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B264" s="0" t="n">
         <v>5</v>
@@ -11820,7 +11847,7 @@
     </row>
     <row r="265" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B265" s="0" t="n">
         <v>6</v>
@@ -11835,7 +11862,7 @@
     </row>
     <row r="266" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B266" s="0" t="n">
         <v>7</v>
@@ -11849,246 +11876,408 @@
       </c>
     </row>
     <row r="267" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A267" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="B267" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="C267" s="4" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D267" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C267, Levels!B:B, 0), 1, 1)),", ",IF(A267 &lt;&gt; "", """mem"": bit" &amp; B267 &amp; "(" &amp; A267 &amp; "),", ""),"""good"": ",IF(A267 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A267 &lt;&gt; "", A267, -1),", ""bit"": ",IF(B267 &lt;&gt; "", B267, -1),"},")</f>
-        <v>266: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>266: { "levelId": 10, "mem": bit2(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 2},</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A268" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="B268" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="C268" s="4" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D268" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C268, Levels!B:B, 0), 1, 1)),", ",IF(A268 &lt;&gt; "", """mem"": bit" &amp; B268 &amp; "(" &amp; A268 &amp; "),", ""),"""good"": ",IF(A268 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A268 &lt;&gt; "", A268, -1),", ""bit"": ",IF(B268 &lt;&gt; "", B268, -1),"},")</f>
-        <v>267: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>267: { "levelId": 10, "mem": bit2(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 2},</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A269" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="B269" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="C269" s="4" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D269" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C269, Levels!B:B, 0), 1, 1)),", ",IF(A269 &lt;&gt; "", """mem"": bit" &amp; B269 &amp; "(" &amp; A269 &amp; "),", ""),"""good"": ",IF(A269 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A269 &lt;&gt; "", A269, -1),", ""bit"": ",IF(B269 &lt;&gt; "", B269, -1),"},")</f>
-        <v>268: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>268: { "levelId": 10, "mem": bit3(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 3},</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A270" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="B270" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="C270" s="4" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D270" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C270, Levels!B:B, 0), 1, 1)),", ",IF(A270 &lt;&gt; "", """mem"": bit" &amp; B270 &amp; "(" &amp; A270 &amp; "),", ""),"""good"": ",IF(A270 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A270 &lt;&gt; "", A270, -1),", ""bit"": ",IF(B270 &lt;&gt; "", B270, -1),"},")</f>
-        <v>269: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>269: { "levelId": 10, "mem": bit4(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 4},</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A271" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="B271" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="C271" s="4" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D271" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C271, Levels!B:B, 0), 1, 1)),", ",IF(A271 &lt;&gt; "", """mem"": bit" &amp; B271 &amp; "(" &amp; A271 &amp; "),", ""),"""good"": ",IF(A271 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A271 &lt;&gt; "", A271, -1),", ""bit"": ",IF(B271 &lt;&gt; "", B271, -1),"},")</f>
-        <v>270: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>270: { "levelId": 10, "mem": bit0(0x2249a6),"good": 1, "addr": 0x2249a6, "bit": 0},</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A272" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="B272" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="C272" s="4" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D272" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C272, Levels!B:B, 0), 1, 1)),", ",IF(A272 &lt;&gt; "", """mem"": bit" &amp; B272 &amp; "(" &amp; A272 &amp; "),", ""),"""good"": ",IF(A272 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A272 &lt;&gt; "", A272, -1),", ""bit"": ",IF(B272 &lt;&gt; "", B272, -1),"},")</f>
-        <v>271: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>271: { "levelId": 10, "mem": bit1(0x2249a6),"good": 1, "addr": 0x2249a6, "bit": 1},</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A273" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="B273" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="C273" s="4" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D273" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C273, Levels!B:B, 0), 1, 1)),", ",IF(A273 &lt;&gt; "", """mem"": bit" &amp; B273 &amp; "(" &amp; A273 &amp; "),", ""),"""good"": ",IF(A273 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A273 &lt;&gt; "", A273, -1),", ""bit"": ",IF(B273 &lt;&gt; "", B273, -1),"},")</f>
-        <v>272: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>272: { "levelId": 10, "mem": bit2(0x2249a6),"good": 1, "addr": 0x2249a6, "bit": 2},</v>
       </c>
     </row>
     <row r="274" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A274" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="B274" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="C274" s="4" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D274" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C274, Levels!B:B, 0), 1, 1)),", ",IF(A274 &lt;&gt; "", """mem"": bit" &amp; B274 &amp; "(" &amp; A274 &amp; "),", ""),"""good"": ",IF(A274 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A274 &lt;&gt; "", A274, -1),", ""bit"": ",IF(B274 &lt;&gt; "", B274, -1),"},")</f>
-        <v>273: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>273: { "levelId": 10, "mem": bit3(0x2249a6),"good": 1, "addr": 0x2249a6, "bit": 3},</v>
       </c>
     </row>
     <row r="275" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A275" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="B275" s="0" t="n">
+        <v>6</v>
+      </c>
       <c r="C275" s="4" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D275" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C275, Levels!B:B, 0), 1, 1)),", ",IF(A275 &lt;&gt; "", """mem"": bit" &amp; B275 &amp; "(" &amp; A275 &amp; "),", ""),"""good"": ",IF(A275 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A275 &lt;&gt; "", A275, -1),", ""bit"": ",IF(B275 &lt;&gt; "", B275, -1),"},")</f>
-        <v>274: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>274: { "levelId": 10, "mem": bit6(0x2249a6),"good": 1, "addr": 0x2249a6, "bit": 6},</v>
       </c>
     </row>
     <row r="276" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A276" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="B276" s="0" t="n">
+        <v>7</v>
+      </c>
       <c r="C276" s="4" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D276" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C276, Levels!B:B, 0), 1, 1)),", ",IF(A276 &lt;&gt; "", """mem"": bit" &amp; B276 &amp; "(" &amp; A276 &amp; "),", ""),"""good"": ",IF(A276 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A276 &lt;&gt; "", A276, -1),", ""bit"": ",IF(B276 &lt;&gt; "", B276, -1),"},")</f>
-        <v>275: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>275: { "levelId": 10, "mem": bit7(0x2249a6),"good": 1, "addr": 0x2249a6, "bit": 7},</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A277" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="B277" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="C277" s="4" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D277" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C277, Levels!B:B, 0), 1, 1)),", ",IF(A277 &lt;&gt; "", """mem"": bit" &amp; B277 &amp; "(" &amp; A277 &amp; "),", ""),"""good"": ",IF(A277 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A277 &lt;&gt; "", A277, -1),", ""bit"": ",IF(B277 &lt;&gt; "", B277, -1),"},")</f>
-        <v>276: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>276: { "levelId": 10, "mem": bit0(0x2249a7),"good": 1, "addr": 0x2249a7, "bit": 0},</v>
       </c>
     </row>
     <row r="278" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A278" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="B278" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="C278" s="4" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D278" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C278, Levels!B:B, 0), 1, 1)),", ",IF(A278 &lt;&gt; "", """mem"": bit" &amp; B278 &amp; "(" &amp; A278 &amp; "),", ""),"""good"": ",IF(A278 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A278 &lt;&gt; "", A278, -1),", ""bit"": ",IF(B278 &lt;&gt; "", B278, -1),"},")</f>
-        <v>277: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>277: { "levelId": 10, "mem": bit1(0x2249a7),"good": 1, "addr": 0x2249a7, "bit": 1},</v>
       </c>
     </row>
     <row r="279" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A279" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="B279" s="0" t="n">
+        <v>5</v>
+      </c>
       <c r="C279" s="4" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D279" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C279, Levels!B:B, 0), 1, 1)),", ",IF(A279 &lt;&gt; "", """mem"": bit" &amp; B279 &amp; "(" &amp; A279 &amp; "),", ""),"""good"": ",IF(A279 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A279 &lt;&gt; "", A279, -1),", ""bit"": ",IF(B279 &lt;&gt; "", B279, -1),"},")</f>
-        <v>278: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>278: { "levelId": 10, "mem": bit5(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 5},</v>
       </c>
     </row>
     <row r="280" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A280" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="B280" s="0" t="n">
+        <v>6</v>
+      </c>
       <c r="C280" s="4" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D280" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C280, Levels!B:B, 0), 1, 1)),", ",IF(A280 &lt;&gt; "", """mem"": bit" &amp; B280 &amp; "(" &amp; A280 &amp; "),", ""),"""good"": ",IF(A280 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A280 &lt;&gt; "", A280, -1),", ""bit"": ",IF(B280 &lt;&gt; "", B280, -1),"},")</f>
-        <v>279: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>279: { "levelId": 10, "mem": bit6(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 6},</v>
       </c>
     </row>
     <row r="281" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A281" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="B281" s="0" t="n">
+        <v>7</v>
+      </c>
       <c r="C281" s="4" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D281" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C281, Levels!B:B, 0), 1, 1)),", ",IF(A281 &lt;&gt; "", """mem"": bit" &amp; B281 &amp; "(" &amp; A281 &amp; "),", ""),"""good"": ",IF(A281 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A281 &lt;&gt; "", A281, -1),", ""bit"": ",IF(B281 &lt;&gt; "", B281, -1),"},")</f>
-        <v>280: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>280: { "levelId": 10, "mem": bit7(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 7},</v>
       </c>
     </row>
     <row r="282" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A282" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="B282" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="C282" s="4" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D282" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C282, Levels!B:B, 0), 1, 1)),", ",IF(A282 &lt;&gt; "", """mem"": bit" &amp; B282 &amp; "(" &amp; A282 &amp; "),", ""),"""good"": ",IF(A282 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A282 &lt;&gt; "", A282, -1),", ""bit"": ",IF(B282 &lt;&gt; "", B282, -1),"},")</f>
-        <v>281: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>281: { "levelId": 10, "mem": bit0(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 0},</v>
       </c>
     </row>
     <row r="283" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A283" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="B283" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="C283" s="4" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D283" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C283, Levels!B:B, 0), 1, 1)),", ",IF(A283 &lt;&gt; "", """mem"": bit" &amp; B283 &amp; "(" &amp; A283 &amp; "),", ""),"""good"": ",IF(A283 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A283 &lt;&gt; "", A283, -1),", ""bit"": ",IF(B283 &lt;&gt; "", B283, -1),"},")</f>
-        <v>282: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>282: { "levelId": 10, "mem": bit1(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 1},</v>
       </c>
     </row>
     <row r="284" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A284" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="B284" s="0" t="n">
+        <v>7</v>
+      </c>
       <c r="C284" s="4" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D284" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C284, Levels!B:B, 0), 1, 1)),", ",IF(A284 &lt;&gt; "", """mem"": bit" &amp; B284 &amp; "(" &amp; A284 &amp; "),", ""),"""good"": ",IF(A284 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A284 &lt;&gt; "", A284, -1),", ""bit"": ",IF(B284 &lt;&gt; "", B284, -1),"},")</f>
-        <v>283: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>283: { "levelId": 10, "mem": bit7(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 7},</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A285" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="B285" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="C285" s="4" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D285" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C285, Levels!B:B, 0), 1, 1)),", ",IF(A285 &lt;&gt; "", """mem"": bit" &amp; B285 &amp; "(" &amp; A285 &amp; "),", ""),"""good"": ",IF(A285 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A285 &lt;&gt; "", A285, -1),", ""bit"": ",IF(B285 &lt;&gt; "", B285, -1),"},")</f>
-        <v>284: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>284: { "levelId": 10, "mem": bit0(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 0},</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A286" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="B286" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="C286" s="4" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D286" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C286, Levels!B:B, 0), 1, 1)),", ",IF(A286 &lt;&gt; "", """mem"": bit" &amp; B286 &amp; "(" &amp; A286 &amp; "),", ""),"""good"": ",IF(A286 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A286 &lt;&gt; "", A286, -1),", ""bit"": ",IF(B286 &lt;&gt; "", B286, -1),"},")</f>
-        <v>285: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>285: { "levelId": 10, "mem": bit1(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 1},</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A287" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="B287" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="C287" s="4" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D287" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C287, Levels!B:B, 0), 1, 1)),", ",IF(A287 &lt;&gt; "", """mem"": bit" &amp; B287 &amp; "(" &amp; A287 &amp; "),", ""),"""good"": ",IF(A287 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A287 &lt;&gt; "", A287, -1),", ""bit"": ",IF(B287 &lt;&gt; "", B287, -1),"},")</f>
-        <v>286: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>286: { "levelId": 10, "mem": bit3(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 3},</v>
       </c>
     </row>
     <row r="288" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A288" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="B288" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="C288" s="4" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D288" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C288, Levels!B:B, 0), 1, 1)),", ",IF(A288 &lt;&gt; "", """mem"": bit" &amp; B288 &amp; "(" &amp; A288 &amp; "),", ""),"""good"": ",IF(A288 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A288 &lt;&gt; "", A288, -1),", ""bit"": ",IF(B288 &lt;&gt; "", B288, -1),"},")</f>
-        <v>287: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>287: { "levelId": 10, "mem": bit4(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 4},</v>
       </c>
     </row>
     <row r="289" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A289" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="B289" s="0" t="n">
+        <v>5</v>
+      </c>
       <c r="C289" s="4" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D289" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C289, Levels!B:B, 0), 1, 1)),", ",IF(A289 &lt;&gt; "", """mem"": bit" &amp; B289 &amp; "(" &amp; A289 &amp; "),", ""),"""good"": ",IF(A289 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A289 &lt;&gt; "", A289, -1),", ""bit"": ",IF(B289 &lt;&gt; "", B289, -1),"},")</f>
-        <v>288: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>288: { "levelId": 10, "mem": bit5(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 5},</v>
       </c>
     </row>
     <row r="290" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A290" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="B290" s="0" t="n">
+        <v>6</v>
+      </c>
       <c r="C290" s="4" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D290" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C290, Levels!B:B, 0), 1, 1)),", ",IF(A290 &lt;&gt; "", """mem"": bit" &amp; B290 &amp; "(" &amp; A290 &amp; "),", ""),"""good"": ",IF(A290 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A290 &lt;&gt; "", A290, -1),", ""bit"": ",IF(B290 &lt;&gt; "", B290, -1),"},")</f>
-        <v>289: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>289: { "levelId": 10, "mem": bit6(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 6},</v>
       </c>
     </row>
     <row r="291" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A291" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="B291" s="0" t="n">
+        <v>7</v>
+      </c>
       <c r="C291" s="4" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D291" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C291, Levels!B:B, 0), 1, 1)),", ",IF(A291 &lt;&gt; "", """mem"": bit" &amp; B291 &amp; "(" &amp; A291 &amp; "),", ""),"""good"": ",IF(A291 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A291 &lt;&gt; "", A291, -1),", ""bit"": ",IF(B291 &lt;&gt; "", B291, -1),"},")</f>
-        <v>290: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>290: { "levelId": 10, "mem": bit7(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 7},</v>
       </c>
     </row>
     <row r="292" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A292" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="B292" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="C292" s="4" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D292" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C292, Levels!B:B, 0), 1, 1)),", ",IF(A292 &lt;&gt; "", """mem"": bit" &amp; B292 &amp; "(" &amp; A292 &amp; "),", ""),"""good"": ",IF(A292 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A292 &lt;&gt; "", A292, -1),", ""bit"": ",IF(B292 &lt;&gt; "", B292, -1),"},")</f>
-        <v>291: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>291: { "levelId": 10, "mem": bit4(0x2249a6),"good": 1, "addr": 0x2249a6, "bit": 4},</v>
       </c>
     </row>
     <row r="293" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A293" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="B293" s="0" t="n">
+        <v>5</v>
+      </c>
       <c r="C293" s="4" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D293" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C293, Levels!B:B, 0), 1, 1)),", ",IF(A293 &lt;&gt; "", """mem"": bit" &amp; B293 &amp; "(" &amp; A293 &amp; "),", ""),"""good"": ",IF(A293 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A293 &lt;&gt; "", A293, -1),", ""bit"": ",IF(B293 &lt;&gt; "", B293, -1),"},")</f>
-        <v>292: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>292: { "levelId": 10, "mem": bit5(0x2249a6),"good": 1, "addr": 0x2249a6, "bit": 5},</v>
       </c>
     </row>
     <row r="294" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18485,15 +18674,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G1081"/>
+  <dimension ref="A1:H1081"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="B2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+      <selection pane="bottomLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.93"/>
@@ -18503,13 +18692,13 @@
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>4</v>
@@ -18517,10 +18706,14 @@
       <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="H1" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT(D2:D81)</f>
+        <v>1: { "levelId": 1, "mem": bit7(0x2249f0),"good": 1},2: { "levelId": 2, "mem": bit0(0x2249f1),"good": 1},3: { "levelId": 2, "mem": bit1(0x2249f1),"good": 1},4: { "levelId": 2, "mem": bit5(0x2249f1),"good": 1},5: { "levelId": 2, "mem": bit6(0x2249f1),"good": 1},6: { "levelId": 1, "mem": bit7(0x2249f1),"good": 1},7: { "levelId": 5, "mem": bit0(0x2249f2),"good": 1},8: { "levelId": 5, "mem": bit1(0x2249f2),"good": 1},9: { "levelId": 5, "mem": bit2(0x2249f2),"good": 1},10: { "levelId": 5, "mem": bit3(0x2249f2),"good": 1},11: { "levelId": 5, "mem": bit4(0x2249f2),"good": 1},12: { "levelId": 6, "mem": bit5(0x2249f2),"good": 1},13: { "levelId": 6, "mem": bit7(0x2249f2),"good": 1},14: { "levelId": 6, "mem": bit1(0x2249f3),"good": 1},15: { "levelId": 6, "mem": bit6(0x2249f2),"good": 1},16: { "levelId": 6, "mem": bit0(0x2249f3),"good": 1},17: { "levelId": 6, "mem": bit3(0x2249f3),"good": 1},18: { "levelId": 6, "mem": bit2(0x2249f3),"good": 1},19: { "levelId": 8, "mem": bit5(0x2249f3),"good": 1},20: { "levelId": 8, "mem": bit4(0x2249f3),"good": 1},21: { "levelId": 10, "mem": bit0(0x2249f4),"good": 1},22: { "levelId": 10, "mem": bit6(0x2249f3),"good": 1},23: { "levelId": 10, "mem": bit3(0x2249f4),"good": 1},24: { "levelId": 10, "mem": bit5(0x2249f4),"good": 1},25: { "levelId": 10, "mem": bit7(0x2249f3),"good": 1},26: { "levelId": 10, "mem": bit1(0x2249f4),"good": 1},27: { "levelId": 10, "mem": bit2(0x2249f4),"good": 1},28: { "levelId": 10, "mem": bit4(0x2249f4),"good": 1},29: { "levelId": 3, "good": 0},30: { "levelId": 3, "good": 0},31: { "levelId": 3, "good": 0},32: { "levelId": 3, "good": 0},33: { "levelId": 3, "good": 0},34: { "levelId": 3, "good": 0},35: { "levelId": 3, "good": 0},36: { "levelId": 3, "good": 0},37: { "levelId": 3, "good": 0},38: { "levelId": 3, "good": 0},39: { "levelId": 3, "good": 0},40: { "levelId": 3, "good": 0},41: { "levelId": 3, "good": 0},42: { "levelId": 3, "good": 0},43: { "levelId": 3, "good": 0},44: { "levelId": 3, "good": 0},45: { "levelId": 3, "good": 0},46: { "levelId": 3, "good": 0},47: { "levelId": 3, "good": 0},48: { "levelId": 3, "good": 0},49: { "levelId": 3, "good": 0},50: { "levelId": 3, "good": 0},51: { "levelId": 3, "good": 0},52: { "levelId": 3, "good": 0},53: { "levelId": 3, "good": 0},54: { "levelId": 3, "good": 0},55: { "levelId": 3, "good": 0},56: { "levelId": 3, "good": 0},57: { "levelId": 3, "good": 0},58: { "levelId": 3, "good": 0},59: { "levelId": 3, "good": 0},60: { "levelId": 3, "good": 0},61: { "levelId": 3, "good": 0},62: { "levelId": 3, "good": 0},63: { "levelId": 3, "good": 0},64: { "levelId": 3, "good": 0},65: { "levelId": 3, "good": 0},66: { "levelId": 3, "good": 0},67: { "levelId": 3, "good": 0},68: { "levelId": 3, "good": 0},69: { "levelId": 3, "good": 0},70: { "levelId": 3, "good": 0},71: { "levelId": 3, "good": 0},72: { "levelId": 3, "good": 0},73: { "levelId": 3, "good": 0},74: { "levelId": 3, "good": 0},75: { "levelId": 3, "good": 0},76: { "levelId": 3, "good": 0},77: { "levelId": 3, "good": 0},78: { "levelId": 3, "good": 0},79: { "levelId": 3, "good": 0},80: { "levelId": 3, "good": 0},</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>7</v>
@@ -18532,14 +18725,10 @@
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C2, Levels!B:B, 0), 1, 1)),", ",IF(A2 &lt;&gt; "", """mem"": bit" &amp; B2 &amp; "(" &amp; A2 &amp; "),", ""),"""good"": ",IF(A2 &lt;&gt; "", 1, 0),"},")</f>
         <v>1: { "levelId": 1, "mem": bit7(0x2249f0),"good": 1},</v>
       </c>
-      <c r="G2" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT(D2:D81)</f>
-        <v>1: { "levelId": 1, "mem": bit7(0x2249f0),"good": 1},2: { "levelId": 2, "mem": bit0(0x2249f1),"good": 1},3: { "levelId": 2, "mem": bit1(0x2249f1),"good": 1},4: { "levelId": 2, "mem": bit5(0x2249f1),"good": 1},5: { "levelId": 2, "mem": bit6(0x2249f1),"good": 1},6: { "levelId": 1, "mem": bit7(0x2249f1),"good": 1},7: { "levelId": 5, "mem": bit0(0x2249f2),"good": 1},8: { "levelId": 5, "mem": bit1(0x2249f2),"good": 1},9: { "levelId": 5, "mem": bit2(0x2249f2),"good": 1},10: { "levelId": 5, "mem": bit3(0x2249f2),"good": 1},11: { "levelId": 5, "mem": bit4(0x2249f2),"good": 1},12: { "levelId": 6, "mem": bit5(0x2249f2),"good": 1},13: { "levelId": 6, "mem": bit7(0x2249f2),"good": 1},14: { "levelId": 6, "mem": bit1(0x2249f3),"good": 1},15: { "levelId": 6, "mem": bit6(0x2249f2),"good": 1},16: { "levelId": 6, "mem": bit0(0x2249f3),"good": 1},17: { "levelId": 6, "mem": bit3(0x2249f3),"good": 1},18: { "levelId": 6, "mem": bit2(0x2249f3),"good": 1},19: { "levelId": 8, "mem": bit5(0x2249f3),"good": 1},20: { "levelId": 8, "mem": bit4(0x2249f3),"good": 1},21: { "levelId": 10, "mem": bit0(0x2249f4),"good": 1},22: { "levelId": 10, "mem": bit6(0x2249f3),"good": 1},23: { "levelId": 3, "good": 0},24: { "levelId": 3, "good": 0},25: { "levelId": 3, "good": 0},26: { "levelId": 3, "good": 0},27: { "levelId": 3, "good": 0},28: { "levelId": 3, "good": 0},29: { "levelId": 3, "good": 0},30: { "levelId": 3, "good": 0},31: { "levelId": 3, "good": 0},32: { "levelId": 3, "good": 0},33: { "levelId": 3, "good": 0},34: { "levelId": 3, "good": 0},35: { "levelId": 3, "good": 0},36: { "levelId": 3, "good": 0},37: { "levelId": 3, "good": 0},38: { "levelId": 3, "good": 0},39: { "levelId": 3, "good": 0},40: { "levelId": 3, "good": 0},41: { "levelId": 3, "good": 0},42: { "levelId": 3, "good": 0},43: { "levelId": 3, "good": 0},44: { "levelId": 3, "good": 0},45: { "levelId": 3, "good": 0},46: { "levelId": 3, "good": 0},47: { "levelId": 3, "good": 0},48: { "levelId": 3, "good": 0},49: { "levelId": 3, "good": 0},50: { "levelId": 3, "good": 0},51: { "levelId": 3, "good": 0},52: { "levelId": 3, "good": 0},53: { "levelId": 3, "good": 0},54: { "levelId": 3, "good": 0},55: { "levelId": 3, "good": 0},56: { "levelId": 3, "good": 0},57: { "levelId": 3, "good": 0},58: { "levelId": 3, "good": 0},59: { "levelId": 3, "good": 0},60: { "levelId": 3, "good": 0},61: { "levelId": 3, "good": 0},62: { "levelId": 3, "good": 0},63: { "levelId": 3, "good": 0},64: { "levelId": 3, "good": 0},65: { "levelId": 3, "good": 0},66: { "levelId": 3, "good": 0},67: { "levelId": 3, "good": 0},68: { "levelId": 3, "good": 0},69: { "levelId": 3, "good": 0},70: { "levelId": 3, "good": 0},71: { "levelId": 3, "good": 0},72: { "levelId": 3, "good": 0},73: { "levelId": 3, "good": 0},74: { "levelId": 3, "good": 0},75: { "levelId": 3, "good": 0},76: { "levelId": 3, "good": 0},77: { "levelId": 3, "good": 0},78: { "levelId": 3, "good": 0},79: { "levelId": 3, "good": 0},80: { "levelId": 3, "good": 0},</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0</v>
@@ -18554,7 +18743,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>1</v>
@@ -18569,7 +18758,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>5</v>
@@ -18584,7 +18773,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>6</v>
@@ -18599,7 +18788,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>7</v>
@@ -18614,7 +18803,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>0</v>
@@ -18629,7 +18818,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>1</v>
@@ -18644,7 +18833,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>2</v>
@@ -18659,7 +18848,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>3</v>
@@ -18674,7 +18863,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>4</v>
@@ -18689,7 +18878,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>5</v>
@@ -18704,7 +18893,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>7</v>
@@ -18719,7 +18908,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>1</v>
@@ -18734,7 +18923,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>6</v>
@@ -18749,7 +18938,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>0</v>
@@ -18764,7 +18953,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>3</v>
@@ -18779,7 +18968,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>2</v>
@@ -18794,7 +18983,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>5</v>
@@ -18809,7 +18998,7 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>4</v>
@@ -18824,7 +19013,7 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>0</v>
@@ -18839,7 +19028,7 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>6</v>
@@ -18853,57 +19042,93 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="C24" s="4" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D24" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C24, Levels!B:B, 0), 1, 1)),", ",IF(A24 &lt;&gt; "", """mem"": bit" &amp; B24 &amp; "(" &amp; A24 &amp; "),", ""),"""good"": ",IF(A24 &lt;&gt; "", 1, 0),"},")</f>
-        <v>23: { "levelId": 3, "good": 0},</v>
+        <v>23: { "levelId": 10, "mem": bit3(0x2249f4),"good": 1},</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>5</v>
+      </c>
       <c r="C25" s="4" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D25" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C25, Levels!B:B, 0), 1, 1)),", ",IF(A25 &lt;&gt; "", """mem"": bit" &amp; B25 &amp; "(" &amp; A25 &amp; "),", ""),"""good"": ",IF(A25 &lt;&gt; "", 1, 0),"},")</f>
-        <v>24: { "levelId": 3, "good": 0},</v>
+        <v>24: { "levelId": 10, "mem": bit5(0x2249f4),"good": 1},</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>7</v>
+      </c>
       <c r="C26" s="4" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D26" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C26, Levels!B:B, 0), 1, 1)),", ",IF(A26 &lt;&gt; "", """mem"": bit" &amp; B26 &amp; "(" &amp; A26 &amp; "),", ""),"""good"": ",IF(A26 &lt;&gt; "", 1, 0),"},")</f>
-        <v>25: { "levelId": 3, "good": 0},</v>
+        <v>25: { "levelId": 10, "mem": bit7(0x2249f3),"good": 1},</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="C27" s="4" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D27" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C27, Levels!B:B, 0), 1, 1)),", ",IF(A27 &lt;&gt; "", """mem"": bit" &amp; B27 &amp; "(" &amp; A27 &amp; "),", ""),"""good"": ",IF(A27 &lt;&gt; "", 1, 0),"},")</f>
-        <v>26: { "levelId": 3, "good": 0},</v>
+        <v>26: { "levelId": 10, "mem": bit1(0x2249f4),"good": 1},</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="C28" s="4" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D28" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C28, Levels!B:B, 0), 1, 1)),", ",IF(A28 &lt;&gt; "", """mem"": bit" &amp; B28 &amp; "(" &amp; A28 &amp; "),", ""),"""good"": ",IF(A28 &lt;&gt; "", 1, 0),"},")</f>
-        <v>27: { "levelId": 3, "good": 0},</v>
+        <v>27: { "levelId": 10, "mem": bit2(0x2249f4),"good": 1},</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="C29" s="4" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D29" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C29, Levels!B:B, 0), 1, 1)),", ",IF(A29 &lt;&gt; "", """mem"": bit" &amp; B29 &amp; "(" &amp; A29 &amp; "),", ""),"""good"": ",IF(A29 &lt;&gt; "", 1, 0),"},")</f>
-        <v>28: { "levelId": 3, "good": 0},</v>
+        <v>28: { "levelId": 10, "mem": bit4(0x2249f4),"good": 1},</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Some work on The Canopy
</commit_message>
<xml_diff>
--- a/Rayman 2.xlsx
+++ b/Rayman 2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Areas" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1538" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1573" uniqueCount="144">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -265,6 +265,24 @@
     <t xml:space="preserve">MenhirArea4</t>
   </si>
   <si>
+    <t xml:space="preserve">75BE94</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CanopyArea1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">in the Canopy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Canopy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">78C480</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CanopyArea2</t>
+  </si>
+  <si>
     <t xml:space="preserve">Index</t>
   </si>
   <si>
@@ -407,6 +425,18 @@
   </si>
   <si>
     <t xml:space="preserve">0x2249a7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x2249a8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x2249a9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x2249aa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x2249ab</t>
   </si>
   <si>
     <t xml:space="preserve">Level ID</t>
@@ -638,7 +668,7 @@
       <selection pane="bottomLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.66"/>
@@ -668,7 +698,7 @@
       </c>
       <c r="H1" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(E2:E1000)</f>
-        <v>0x784BFC: { "id": 0x784BFC, "areaName": "Menu", "displayName": "Main Menu", "levelName": "Menu" },0x789668: { "id": 0x789668, "areaName": "Intro", "displayName": "somewhere in the Glade of Dreams…", "levelName": "None" },0x778C74: { "id": 0x778C74, "areaName": "BuccaneerBrig", "displayName": "in the Buccaneer’s brig", "levelName": "None" },0x78D424: { "id": 0x78D424, "areaName": "WoodsOfLight", "displayName": "in the Woods of Light", "levelName": "Woods of Light" },0x790570: { "id": 0x790570, "areaName": "HallOfDoors", "displayName": "in the Hall of Doors", "levelName": "Hall of Doors" },0x7875A8: { "id": 0x7875A8, "areaName": "FairyGladeArea1", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x78A320: { "id": 0x78A320, "areaName": "FairyGladeArea2", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x7A1BD8: { "id": 0x7A1BD8, "areaName": "FairyGladeArea3", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x77BFFC: { "id": 0x77BFFC, "areaName": "FairyGladeArea4", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x771B74: { "id": 0x771B74, "areaName": "FairyGladeArea5", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x74AAA8: { "id": 0x74AAA8, "areaName": "Results", "displayName": "viewing level results…", "levelName": "None" },0x788708: { "id": 0x788708, "areaName": "MarshesArea1", "displayName": "in the Marshes of Awakening", "levelName": "Marshes of Awakening" },0x7786E8: { "id": 0x7786E8, "areaName": "MarshesArea2", "displayName": "in the Marshes of Awakening", "levelName": "Marshes of Awakening" },0x790598: { "id": 0x790598, "areaName": "BayouArea1", "displayName": "in the Bayou", "levelName": "Bayou" },0x788764: { "id": 0x788764, "areaName": "BayouArea2", "displayName": "in the Bayou", "levelName": "Bayou" },0x7928A4: { "id": 0x7928A4, "areaName": "SoWaIArea1", "displayName": "in the Sanctuary of Water and Ice", "levelName": "Sanctuary of Water and Ice" },0x774694: { "id": 0x774694, "areaName": "SoWaIArea2", "displayName": "in the Sanctuary of Water and Ice", "levelName": "Sanctuary of Water and Ice" },0x76F100: { "id": 0x76F100, "areaName": "Polokus", "displayName": "in Polokus’s dream", "levelName": "Polokus" },0x0: { "id": 0x0, "areaName": "None", "displayName": "somewhere in the Glade of Dreams…", "levelName": "None" },0x751974: { "id": 0x751974, "areaName": "Bonus", "displayName": "in the bonus stage", "levelName": "None" },0x776C08: { "id": 0x776C08, "areaName": "MenhirArea1", "displayName": "in the Menhir Hills", "levelName": "Menhir Hills" },0x78FBD8: { "id": 0x78FBD8, "areaName": "MenhirArea2", "displayName": "in the Menhir Hills", "levelName": "Menhir Hills" },0x788950: { "id": 0x788950, "areaName": "MenhirArea3", "displayName": "in the Menhir Hills", "levelName": "Menhir Hills" },0x78402C: { "id": 0x78402C, "areaName": "BadDreamsArea1", "displayName": "in the Cave of Bad Dreams", "levelName": "Cave of Bad Dreams" },0x788148: { "id": 0x788148, "areaName": "BadDreamsArea2", "displayName": "in the Cave of Bad Dreams", "levelName": "Cave of Bad Dreams" },0x75AADC: { "id": 0x75AADC, "areaName": "MenhirArea4", "displayName": "in the Menhir Hills", "levelName": "Menhir Hills" },</v>
+        <v>0x784BFC: { "id": 0x784BFC, "areaName": "Menu", "displayName": "Main Menu", "levelName": "Menu" },0x789668: { "id": 0x789668, "areaName": "Intro", "displayName": "somewhere in the Glade of Dreams…", "levelName": "None" },0x778C74: { "id": 0x778C74, "areaName": "BuccaneerBrig", "displayName": "in the Buccaneer’s brig", "levelName": "None" },0x78D424: { "id": 0x78D424, "areaName": "WoodsOfLight", "displayName": "in the Woods of Light", "levelName": "Woods of Light" },0x790570: { "id": 0x790570, "areaName": "HallOfDoors", "displayName": "in the Hall of Doors", "levelName": "Hall of Doors" },0x7875A8: { "id": 0x7875A8, "areaName": "FairyGladeArea1", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x78A320: { "id": 0x78A320, "areaName": "FairyGladeArea2", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x7A1BD8: { "id": 0x7A1BD8, "areaName": "FairyGladeArea3", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x77BFFC: { "id": 0x77BFFC, "areaName": "FairyGladeArea4", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x771B74: { "id": 0x771B74, "areaName": "FairyGladeArea5", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x74AAA8: { "id": 0x74AAA8, "areaName": "Results", "displayName": "viewing level results…", "levelName": "None" },0x788708: { "id": 0x788708, "areaName": "MarshesArea1", "displayName": "in the Marshes of Awakening", "levelName": "Marshes of Awakening" },0x7786E8: { "id": 0x7786E8, "areaName": "MarshesArea2", "displayName": "in the Marshes of Awakening", "levelName": "Marshes of Awakening" },0x790598: { "id": 0x790598, "areaName": "BayouArea1", "displayName": "in the Bayou", "levelName": "Bayou" },0x788764: { "id": 0x788764, "areaName": "BayouArea2", "displayName": "in the Bayou", "levelName": "Bayou" },0x7928A4: { "id": 0x7928A4, "areaName": "SoWaIArea1", "displayName": "in the Sanctuary of Water and Ice", "levelName": "Sanctuary of Water and Ice" },0x774694: { "id": 0x774694, "areaName": "SoWaIArea2", "displayName": "in the Sanctuary of Water and Ice", "levelName": "Sanctuary of Water and Ice" },0x76F100: { "id": 0x76F100, "areaName": "Polokus", "displayName": "in Polokus’s dream", "levelName": "Polokus" },0x0: { "id": 0x0, "areaName": "None", "displayName": "somewhere in the Glade of Dreams…", "levelName": "None" },0x751974: { "id": 0x751974, "areaName": "Bonus", "displayName": "in the bonus stage", "levelName": "None" },0x776C08: { "id": 0x776C08, "areaName": "MenhirArea1", "displayName": "in the Menhir Hills", "levelName": "Menhir Hills" },0x78FBD8: { "id": 0x78FBD8, "areaName": "MenhirArea2", "displayName": "in the Menhir Hills", "levelName": "Menhir Hills" },0x788950: { "id": 0x788950, "areaName": "MenhirArea3", "displayName": "in the Menhir Hills", "levelName": "Menhir Hills" },0x78402C: { "id": 0x78402C, "areaName": "BadDreamsArea1", "displayName": "in the Cave of Bad Dreams", "levelName": "Cave of Bad Dreams" },0x788148: { "id": 0x788148, "areaName": "BadDreamsArea2", "displayName": "in the Cave of Bad Dreams", "levelName": "Cave of Bad Dreams" },0x75AADC: { "id": 0x75AADC, "areaName": "MenhirArea4", "displayName": "in the Menhir Hills", "levelName": "Menhir Hills" },0x75BE94: { "id": 0x75BE94, "areaName": "CanopyArea1", "displayName": "in the Canopy", "levelName": "Canopy" },0x78C480: { "id": 0x78C480, "areaName": "CanopyArea2", "displayName": "in the Canopy", "levelName": "Canopy" },</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1140,10 +1170,40 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D28" s="4"/>
+      <c r="A28" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E28" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("0x", A28,": { ""id"": ","0x", A28,", ""areaName"": """,B28,""", ""displayName"": """,C28,""", ""levelName"": """,D28,""" },")</f>
+        <v>0x75BE94: { "id": 0x75BE94, "areaName": "CanopyArea1", "displayName": "in the Canopy", "levelName": "Canopy" },</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D29" s="4"/>
+      <c r="A29" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E29" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("0x", A29,": { ""id"": ","0x", A29,", ""areaName"": """,B29,""", ""displayName"": """,C29,""", ""levelName"": """,D29,""" },")</f>
+        <v>0x78C480: { "id": 0x78C480, "areaName": "CanopyArea2", "displayName": "in the Canopy", "levelName": "Canopy" },</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D30" s="4"/>
@@ -4130,10 +4190,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="bottomLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.21"/>
@@ -4145,22 +4205,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>4</v>
@@ -4236,7 +4296,7 @@
       </c>
       <c r="E4" s="0" t="n">
         <f aca="false">COUNTIFS(Lums!C3:C1002, "=" &amp; B4)</f>
-        <v>708</v>
+        <v>684</v>
       </c>
       <c r="F4" s="0" t="n">
         <f aca="false">COUNTIFS(Cages!C3:C83, "=" &amp; B4)</f>
@@ -4468,18 +4528,26 @@
         <f aca="false">ROW()-1</f>
         <v>12</v>
       </c>
-      <c r="B13" s="4"/>
+      <c r="B13" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="E13" s="0" t="n">
         <f aca="false">COUNTIFS(Lums!C12:C1011, "=" &amp; B13)</f>
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="F13" s="0" t="n">
         <f aca="false">COUNTIFS(Cages!C12:C92, "=" &amp; B13)</f>
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="G13" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A13,": { ""id"": ",A13,", ""name"": """,B13,""", ""lums"": ",C13,", ""cages"": ",D13," },")</f>
-        <v>12: { "id": 12, "name": "", "lums": , "cages":  },</v>
+        <v>12: { "id": 12, "name": "Canopy", "lums": 50, "cages": 4 },</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7859,13 +7927,13 @@
   </sheetPr>
   <dimension ref="A1:H1001"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A266" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A290" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+      <selection pane="bottomLeft" activeCell="C318" activeCellId="0" sqref="C318"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.93"/>
@@ -7874,10 +7942,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>3</v>
@@ -7890,12 +7958,12 @@
       </c>
       <c r="H1" s="5" t="str">
         <f aca="false">_xlfn.CONCAT(D2:D1001)</f>
-        <v>1: { "levelId": 2, "mem": bit0(0x224988),"good": 1, "addr": 0x224988, "bit": 0},2: { "levelId": 2, "mem": bit1(0x224988),"good": 1, "addr": 0x224988, "bit": 1},3: { "levelId": 2, "mem": bit2(0x224988),"good": 1, "addr": 0x224988, "bit": 2},4: { "levelId": 2, "mem": bit3(0x224988),"good": 1, "addr": 0x224988, "bit": 3},5: { "levelId": 2, "mem": bit4(0x224988),"good": 1, "addr": 0x224988, "bit": 4},6: { "levelId": 2, "mem": bit5(0x224988),"good": 1, "addr": 0x224988, "bit": 5},7: { "levelId": 2, "mem": bit6(0x224988),"good": 1, "addr": 0x224988, "bit": 6},8: { "levelId": 2, "mem": bit7(0x224988),"good": 1, "addr": 0x224988, "bit": 7},9: { "levelId": 2, "mem": bit2(0x224989),"good": 1, "addr": 0x224989, "bit": 2},10: { "levelId": 2, "mem": bit1(0x22498a),"good": 1, "addr": 0x22498a, "bit": 1},11: { "levelId": 2, "mem": bit2(0x22498a),"good": 1, "addr": 0x22498a, "bit": 2},12: { "levelId": 2, "mem": bit3(0x22498a),"good": 1, "addr": 0x22498a, "bit": 3},13: { "levelId": 2, "mem": bit4(0x22498a),"good": 1, "addr": 0x22498a, "bit": 4},14: { "levelId": 2, "mem": bit5(0x22498a),"good": 1, "addr": 0x22498a, "bit": 5},15: { "levelId": 2, "mem": bit6(0x22498a),"good": 1, "addr": 0x22498a, "bit": 6},16: { "levelId": 2, "mem": bit7(0x22498a),"good": 1, "addr": 0x22498a, "bit": 7},17: { "levelId": 2, "mem": bit5(0x22498b),"good": 1, "addr": 0x22498b, "bit": 5},18: { "levelId": 2, "mem": bit6(0x22498b),"good": 1, "addr": 0x22498b, "bit": 6},19: { "levelId": 2, "mem": bit7(0x22498b),"good": 1, "addr": 0x22498b, "bit": 7},20: { "levelId": 2, "mem": bit0(0x22498c),"good": 1, "addr": 0x22498c, "bit": 0},21: { "levelId": 2, "mem": bit1(0x22498c),"good": 1, "addr": 0x22498c, "bit": 1},22: { "levelId": 2, "mem": bit2(0x22498c),"good": 1, "addr": 0x22498c, "bit": 2},23: { "levelId": 2, "mem": bit3(0x22498c),"good": 1, "addr": 0x22498c, "bit": 3},24: { "levelId": 2, "mem": bit4(0x22498c),"good": 1, "addr": 0x22498c, "bit": 4},25: { "levelId": 2, "mem": bit5(0x22498c),"good": 1, "addr": 0x22498c, "bit": 5},26: { "levelId": 2, "mem": bit6(0x22498c),"good": 1, "addr": 0x22498c, "bit": 6},27: { "levelId": 2, "mem": bit7(0x22498c),"good": 1, "addr": 0x22498c, "bit": 7},28: { "levelId": 2, "mem": bit0(0x22498d),"good": 1, "addr": 0x22498d, "bit": 0},29: { "levelId": 2, "mem": bit1(0x22498d),"good": 1, "addr": 0x22498d, "bit": 1},30: { "levelId": 2, "mem": bit2(0x22498d),"good": 1, "addr": 0x22498d, "bit": 2},31: { "levelId": 2, "mem": bit3(0x22498d),"good": 1, "addr": 0x22498d, "bit": 3},32: { "levelId": 2, "mem": bit4(0x22498d),"good": 1, "addr": 0x22498d, "bit": 4},33: { "levelId": 2, "mem": bit5(0x22498d),"good": 1, "addr": 0x22498d, "bit": 5},34: { "levelId": 2, "mem": bit6(0x22498d),"good": 1, "addr": 0x22498d, "bit": 6},35: { "levelId": 2, "mem": bit7(0x22498d),"good": 1, "addr": 0x22498d, "bit": 7},36: { "levelId": 2, "mem": bit0(0x22498e),"good": 1, "addr": 0x22498e, "bit": 0},37: { "levelId": 2, "mem": bit1(0x22498e),"good": 1, "addr": 0x22498e, "bit": 1},38: { "levelId": 5, "mem": bit2(0x22498e),"good": 1, "addr": 0x22498e, "bit": 2},39: { "levelId": 5, "mem": bit3(0x22498e),"good": 1, "addr": 0x22498e, "bit": 3},40: { "levelId": 5, "mem": bit4(0x22498e),"good": 1, "addr": 0x22498e, "bit": 4},41: { "levelId": 5, "mem": bit5(0x22498e),"good": 1, "addr": 0x22498e, "bit": 5},42: { "levelId": 5, "mem": bit6(0x22498e),"good": 1, "addr": 0x22498e, "bit": 6},43: { "levelId": 5, "mem": bit7(0x22498e),"good": 1, "addr": 0x22498e, "bit": 7},44: { "levelId": 5, "mem": bit0(0x22498f),"good": 1, "addr": 0x22498f, "bit": 0},45: { "levelId": 5, "mem": bit1(0x22498f),"good": 1, "addr": 0x22498f, "bit": 1},46: { "levelId": 5, "mem": bit2(0x22498f),"good": 1, "addr": 0x22498f, "bit": 2},47: { "levelId": 5, "mem": bit3(0x22498f),"good": 1, "addr": 0x22498f, "bit": 3},48: { "levelId": 5, "mem": bit4(0x22498f),"good": 1, "addr": 0x22498f, "bit": 4},49: { "levelId": 5, "mem": bit5(0x22498f),"good": 1, "addr": 0x22498f, "bit": 5},50: { "levelId": 5, "mem": bit6(0x22498f),"good": 1, "addr": 0x22498f, "bit": 6},51: { "levelId": 5, "mem": bit7(0x22498f),"good": 1, "addr": 0x22498f, "bit": 7},52: { "levelId": 5, "mem": bit0(0x224990),"good": 1, "addr": 0x224990, "bit": 0},53: { "levelId": 5, "mem": bit1(0x224990),"good": 1, "addr": 0x224990, "bit": 1},54: { "levelId": 5, "mem": bit2(0x224990),"good": 1, "addr": 0x224990, "bit": 2},55: { "levelId": 5, "mem": bit3(0x224990),"good": 1, "addr": 0x224990, "bit": 3},56: { "levelId": 5, "mem": bit4(0x224990),"good": 1, "addr": 0x224990, "bit": 4},57: { "levelId": 5, "mem": bit5(0x224990),"good": 1, "addr": 0x224990, "bit": 5},58: { "levelId": 5, "mem": bit6(0x224990),"good": 1, "addr": 0x224990, "bit": 6},59: { "levelId": 5, "mem": bit7(0x224990),"good": 1, "addr": 0x224990, "bit": 7},60: { "levelId": 5, "mem": bit0(0x224991),"good": 1, "addr": 0x224991, "bit": 0},61: { "levelId": 5, "mem": bit1(0x224991),"good": 1, "addr": 0x224991, "bit": 1},62: { "levelId": 5, "mem": bit2(0x224991),"good": 1, "addr": 0x224991, "bit": 2},63: { "levelId": 5, "mem": bit3(0x224991),"good": 1, "addr": 0x224991, "bit": 3},64: { "levelId": 5, "mem": bit4(0x224991),"good": 1, "addr": 0x224991, "bit": 4},65: { "levelId": 5, "mem": bit5(0x224991),"good": 1, "addr": 0x224991, "bit": 5},66: { "levelId": 5, "mem": bit6(0x224991),"good": 1, "addr": 0x224991, "bit": 6},67: { "levelId": 5, "mem": bit7(0x224991),"good": 1, "addr": 0x224991, "bit": 7},68: { "levelId": 5, "mem": bit0(0x224992),"good": 1, "addr": 0x224992, "bit": 0},69: { "levelId": 5, "mem": bit1(0x224992),"good": 1, "addr": 0x224992, "bit": 1},70: { "levelId": 5, "mem": bit2(0x224992),"good": 1, "addr": 0x224992, "bit": 2},71: { "levelId": 5, "mem": bit3(0x224992),"good": 1, "addr": 0x224992, "bit": 3},72: { "levelId": 5, "mem": bit4(0x224992),"good": 1, "addr": 0x224992, "bit": 4},73: { "levelId": 5, "mem": bit5(0x224992),"good": 1, "addr": 0x224992, "bit": 5},74: { "levelId": 5, "mem": bit6(0x224992),"good": 1, "addr": 0x224992, "bit": 6},75: { "levelId": 5, "mem": bit7(0x224992),"good": 1, "addr": 0x224992, "bit": 7},76: { "levelId": 5, "mem": bit0(0x224993),"good": 1, "addr": 0x224993, "bit": 0},77: { "levelId": 5, "mem": bit1(0x224993),"good": 1, "addr": 0x224993, "bit": 1},78: { "levelId": 5, "mem": bit2(0x224993),"good": 1, "addr": 0x224993, "bit": 2},79: { "levelId": 5, "mem": bit3(0x224993),"good": 1, "addr": 0x224993, "bit": 3},80: { "levelId": 5, "mem": bit4(0x224993),"good": 1, "addr": 0x224993, "bit": 4},81: { "levelId": 5, "mem": bit5(0x224993),"good": 1, "addr": 0x224993, "bit": 5},82: { "levelId": 5, "mem": bit6(0x224993),"good": 1, "addr": 0x224993, "bit": 6},83: { "levelId": 5, "mem": bit7(0x224993),"good": 1, "addr": 0x224993, "bit": 7},84: { "levelId": 5, "mem": bit0(0x224994),"good": 1, "addr": 0x224994, "bit": 0},85: { "levelId": 5, "mem": bit1(0x224994),"good": 1, "addr": 0x224994, "bit": 1},86: { "levelId": 5, "mem": bit2(0x224994),"good": 1, "addr": 0x224994, "bit": 2},87: { "levelId": 5, "mem": bit3(0x224994),"good": 1, "addr": 0x224994, "bit": 3},88: { "levelId": 6, "mem": bit4(0x224994),"good": 1, "addr": 0x224994, "bit": 4},89: { "levelId": 6, "mem": bit5(0x224994),"good": 1, "addr": 0x224994, "bit": 5},90: { "levelId": 6, "mem": bit6(0x224994),"good": 1, "addr": 0x224994, "bit": 6},91: { "levelId": 6, "mem": bit7(0x224994),"good": 1, "addr": 0x224994, "bit": 7},92: { "levelId": 6, "mem": bit0(0x224995),"good": 1, "addr": 0x224995, "bit": 0},93: { "levelId": 6, "mem": bit1(0x224995),"good": 1, "addr": 0x224995, "bit": 1},94: { "levelId": 6, "mem": bit2(0x224995),"good": 1, "addr": 0x224995, "bit": 2},95: { "levelId": 6, "mem": bit3(0x224995),"good": 1, "addr": 0x224995, "bit": 3},96: { "levelId": 6, "mem": bit4(0x224995),"good": 1, "addr": 0x224995, "bit": 4},97: { "levelId": 6, "mem": bit5(0x224995),"good": 1, "addr": 0x224995, "bit": 5},98: { "levelId": 6, "mem": bit6(0x224995),"good": 1, "addr": 0x224995, "bit": 6},99: { "levelId": 6, "mem": bit7(0x224995),"good": 1, "addr": 0x224995, "bit": 7},100: { "levelId": 6, "mem": bit0(0x224996),"good": 1, "addr": 0x224996, "bit": 0},101: { "levelId": 6, "mem": bit1(0x224996),"good": 1, "addr": 0x224996, "bit": 1},102: { "levelId": 6, "mem": bit2(0x224996),"good": 1, "addr": 0x224996, "bit": 2},103: { "levelId": 6, "mem": bit3(0x224996),"good": 1, "addr": 0x224996, "bit": 3},104: { "levelId": 6, "mem": bit4(0x224996),"good": 1, "addr": 0x224996, "bit": 4},105: { "levelId": 6, "mem": bit5(0x224996),"good": 1, "addr": 0x224996, "bit": 5},106: { "levelId": 6, "mem": bit6(0x224996),"good": 1, "addr": 0x224996, "bit": 6},107: { "levelId": 6, "mem": bit7(0x224996),"good": 1, "addr": 0x224996, "bit": 7},108: { "levelId": 6, "mem": bit0(0x224997),"good": 1, "addr": 0x224997, "bit": 0},109: { "levelId": 6, "mem": bit1(0x224997),"good": 1, "addr": 0x224997, "bit": 1},110: { "levelId": 6, "mem": bit2(0x224997),"good": 1, "addr": 0x224997, "bit": 2},111: { "levelId": 6, "mem": bit3(0x224997),"good": 1, "addr": 0x224997, "bit": 3},112: { "levelId": 6, "mem": bit4(0x224997),"good": 1, "addr": 0x224997, "bit": 4},113: { "levelId": 6, "mem": bit5(0x224997),"good": 1, "addr": 0x224997, "bit": 5},114: { "levelId": 6, "mem": bit6(0x224997),"good": 1, "addr": 0x224997, "bit": 6},115: { "levelId": 6, "mem": bit7(0x224997),"good": 1, "addr": 0x224997, "bit": 7},116: { "levelId": 6, "mem": bit0(0x224998),"good": 1, "addr": 0x224998, "bit": 0},117: { "levelId": 6, "mem": bit1(0x224998),"good": 1, "addr": 0x224998, "bit": 1},118: { "levelId": 6, "mem": bit2(0x224998),"good": 1, "addr": 0x224998, "bit": 2},119: { "levelId": 6, "mem": bit3(0x224998),"good": 1, "addr": 0x224998, "bit": 3},120: { "levelId": 6, "mem": bit4(0x224998),"good": 1, "addr": 0x224998, "bit": 4},121: { "levelId": 6, "mem": bit5(0x224998),"good": 1, "addr": 0x224998, "bit": 5},122: { "levelId": 6, "mem": bit6(0x224998),"good": 1, "addr": 0x224998, "bit": 6},123: { "levelId": 6, "mem": bit0(0x224999),"good": 1, "addr": 0x224999, "bit": 0},124: { "levelId": 6, "mem": bit1(0x224999),"good": 1, "addr": 0x224999, "bit": 1},125: { "levelId": 6, "mem": bit2(0x224999),"good": 1, "addr": 0x224999, "bit": 2},126: { "levelId": 6, "mem": bit3(0x224999),"good": 1, "addr": 0x224999, "bit": 3},127: { "levelId": 6, "mem": bit4(0x224999),"good": 1, "addr": 0x224999, "bit": 4},128: { "levelId": 6, "mem": bit5(0x224999),"good": 1, "addr": 0x224999, "bit": 5},129: { "levelId": 6, "mem": bit6(0x224999),"good": 1, "addr": 0x224999, "bit": 6},130: { "levelId": 6, "mem": bit7(0x224999),"good": 1, "addr": 0x224999, "bit": 7},131: { "levelId": 6, "mem": bit0(0x22499a),"good": 1, "addr": 0x22499a, "bit": 0},132: { "levelId": 6, "mem": bit1(0x22499a),"good": 1, "addr": 0x22499a, "bit": 1},133: { "levelId": 6, "mem": bit2(0x22499a),"good": 1, "addr": 0x22499a, "bit": 2},134: { "levelId": 6, "mem": bit3(0x22499a),"good": 1, "addr": 0x22499a, "bit": 3},135: { "levelId": 6, "mem": bit4(0x22499a),"good": 1, "addr": 0x22499a, "bit": 4},136: { "levelId": 6, "mem": bit5(0x22499a),"good": 1, "addr": 0x22499a, "bit": 5},137: { "levelId": 1, "mem": bit3(0x224a36),"good": 1, "addr": 0x224a36, "bit": 3},138: { "levelId": 1, "mem": bit4(0x224a36),"good": 1, "addr": 0x224a36, "bit": 4},139: { "levelId": 1, "mem": bit5(0x224a36),"good": 1, "addr": 0x224a36, "bit": 5},140: { "levelId": 1, "mem": bit6(0x224a36),"good": 1, "addr": 0x224a36, "bit": 6},141: { "levelId": 1, "mem": bit7(0x224a36),"good": 1, "addr": 0x224a36, "bit": 7},142: { "levelId": 6, "mem": bit7(0x224998),"good": 1, "addr": 0x224998, "bit": 7},143: { "levelId": 8, "mem": bit3(0x22499b),"good": 1, "addr": 0x22499b, "bit": 3},144: { "levelId": 8, "mem": bit4(0x22499b),"good": 1, "addr": 0x22499b, "bit": 4},145: { "levelId": 8, "mem": bit5(0x22499b),"good": 1, "addr": 0x22499b, "bit": 5},146: { "levelId": 8, "mem": bit5(0x22499c),"good": 1, "addr": 0x22499c, "bit": 5},147: { "levelId": 8, "mem": bit6(0x22499c),"good": 1, "addr": 0x22499c, "bit": 6},148: { "levelId": 8, "mem": bit7(0x22499c),"good": 1, "addr": 0x22499c, "bit": 7},149: { "levelId": 8, "mem": bit0(0x22499d),"good": 1, "addr": 0x22499d, "bit": 0},150: { "levelId": 8, "mem": bit1(0x22499d),"good": 1, "addr": 0x22499d, "bit": 1},151: { "levelId": 8, "mem": bit2(0x22499d),"good": 1, "addr": 0x22499d, "bit": 2},152: { "levelId": 8, "mem": bit3(0x22499d),"good": 1, "addr": 0x22499d, "bit": 3},153: { "levelId": 8, "mem": bit4(0x22499d),"good": 1, "addr": 0x22499d, "bit": 4},154: { "levelId": 8, "mem": bit5(0x22499d),"good": 1, "addr": 0x22499d, "bit": 5},155: { "levelId": 8, "mem": bit6(0x22499d),"good": 1, "addr": 0x22499d, "bit": 6},156: { "levelId": 8, "mem": bit7(0x22499d),"good": 1, "addr": 0x22499d, "bit": 7},157: { "levelId": 8, "mem": bit0(0x22499e),"good": 1, "addr": 0x22499e, "bit": 0},158: { "levelId": 8, "mem": bit1(0x22499e),"good": 1, "addr": 0x22499e, "bit": 1},159: { "levelId": 8, "mem": bit6(0x22499a),"good": 1, "addr": 0x22499a, "bit": 6},160: { "levelId": 8, "mem": bit7(0x22499a),"good": 1, "addr": 0x22499a, "bit": 7},161: { "levelId": 8, "mem": bit0(0x22499b),"good": 1, "addr": 0x22499b, "bit": 0},162: { "levelId": 8, "mem": bit1(0x22499b),"good": 1, "addr": 0x22499b, "bit": 1},163: { "levelId": 8, "mem": bit2(0x22499b),"good": 1, "addr": 0x22499b, "bit": 2},164: { "levelId": 8, "mem": bit6(0x22499b),"good": 1, "addr": 0x22499b, "bit": 6},165: { "levelId": 8, "mem": bit7(0x22499b),"good": 1, "addr": 0x22499b, "bit": 7},166: { "levelId": 8, "mem": bit0(0x22499c),"good": 1, "addr": 0x22499c, "bit": 0},167: { "levelId": 8, "mem": bit1(0x22499c),"good": 1, "addr": 0x22499c, "bit": 1},168: { "levelId": 8, "mem": bit2(0x22499c),"good": 1, "addr": 0x22499c, "bit": 2},169: { "levelId": 8, "mem": bit3(0x22499c),"good": 1, "addr": 0x22499c, "bit": 3},170: { "levelId": 8, "mem": bit4(0x22499c),"good": 1, "addr": 0x22499c, "bit": 4},171: { "levelId": 8, "mem": bit2(0x22499e),"good": 1, "addr": 0x22499e, "bit": 2},172: { "levelId": 8, "mem": bit3(0x22499e),"good": 1, "addr": 0x22499e, "bit": 3},173: { "levelId": 8, "mem": bit4(0x22499e),"good": 1, "addr": 0x22499e, "bit": 4},174: { "levelId": 8, "mem": bit5(0x22499e),"good": 1, "addr": 0x22499e, "bit": 5},175: { "levelId": 8, "mem": bit6(0x22499e),"good": 1, "addr": 0x22499e, "bit": 6},176: { "levelId": 8, "mem": bit7(0x22499e),"good": 1, "addr": 0x22499e, "bit": 7},177: { "levelId": 8, "mem": bit0(0x22499f),"good": 1, "addr": 0x22499f, "bit": 0},178: { "levelId": 8, "mem": bit1(0x22499f),"good": 1, "addr": 0x22499f, "bit": 1},179: { "levelId": 8, "mem": bit2(0x22499f),"good": 1, "addr": 0x22499f, "bit": 2},180: { "levelId": 8, "mem": bit3(0x22499f),"good": 1, "addr": 0x22499f, "bit": 3},181: { "levelId": 8, "mem": bit4(0x22499f),"good": 1, "addr": 0x22499f, "bit": 4},182: { "levelId": 8, "mem": bit5(0x22499f),"good": 1, "addr": 0x22499f, "bit": 5},183: { "levelId": 8, "mem": bit6(0x22499f),"good": 1, "addr": 0x22499f, "bit": 6},184: { "levelId": 8, "mem": bit7(0x22499f),"good": 1, "addr": 0x22499f, "bit": 7},185: { "levelId": 8, "mem": bit0(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 0},186: { "levelId": 8, "mem": bit1(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 1},187: { "levelId": 8, "mem": bit2(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 2},188: { "levelId": 8, "mem": bit3(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 3},189: { "levelId": 8, "mem": bit4(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 4},190: { "levelId": 8, "mem": bit5(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 5},191: { "levelId": 8, "mem": bit6(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 6},192: { "levelId": 8, "mem": bit7(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 7},193: { "levelId": 10, "mem": bit0(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 0},194: { "levelId": 10, "mem": bit1(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 1},195: { "levelId": 10, "mem": bit2(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 2},196: { "levelId": 10, "mem": bit3(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 3},197: { "levelId": 10, "mem": bit4(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 4},198: { "levelId": 10, "mem": bit2(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 2},199: { "levelId": 10, "mem": bit3(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 3},200: { "levelId": 10, "mem": bit4(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 4},201: { "levelId": 10, "mem": bit5(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 5},202: { "levelId": 10, "mem": bit6(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 6},203: { "levelId": 10, "mem": bit1(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 1},204: { "levelId": 10, "mem": bit5(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 5},205: { "levelId": 10, "mem": bit6(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 6},206: { "levelId": 10, "mem": bit7(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 7},207: { "levelId": 10, "mem": bit0(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 0},208: { "levelId": 10, "mem": bit3(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 3},209: { "levelId": 10, "mem": bit5(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 5},210: { "levelId": 10, "mem": bit6(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 6},211: { "levelId": 10, "mem": bit7(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 7},212: { "levelId": 10, "mem": bit0(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 0},213: { "levelId": 10, "mem": bit1(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 1},214: { "levelId": 10, "mem": bit2(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 2},215: { "levelId": 10, "mem": bit4(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 4},216: { "levelId": 11, "mem": bit6(0x2249e5),"good": 1, "addr": 0x2249e5, "bit": 6},217: { "levelId": 11, "mem": bit7(0x2249e5),"good": 1, "addr": 0x2249e5, "bit": 7},218: { "levelId": 11, "mem": bit0(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 0},219: { "levelId": 11, "mem": bit1(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 1},220: { "levelId": 11, "mem": bit2(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 2},221: { "levelId": 11, "mem": bit3(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 3},222: { "levelId": 11, "mem": bit4(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 4},223: { "levelId": 11, "mem": bit5(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 5},224: { "levelId": 11, "mem": bit6(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 6},225: { "levelId": 11, "mem": bit7(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 7},226: { "levelId": 11, "mem": bit0(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 0},227: { "levelId": 11, "mem": bit1(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 1},228: { "levelId": 11, "mem": bit2(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 2},229: { "levelId": 11, "mem": bit3(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 3},230: { "levelId": 11, "mem": bit4(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 4},231: { "levelId": 11, "mem": bit5(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 5},232: { "levelId": 11, "mem": bit6(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 6},233: { "levelId": 11, "mem": bit7(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 7},234: { "levelId": 11, "mem": bit0(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 0},235: { "levelId": 11, "mem": bit1(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 1},236: { "levelId": 11, "mem": bit2(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 2},237: { "levelId": 11, "mem": bit3(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 3},238: { "levelId": 11, "mem": bit4(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 4},239: { "levelId": 11, "mem": bit5(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 5},240: { "levelId": 11, "mem": bit6(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 6},241: { "levelId": 11, "mem": bit7(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 7},242: { "levelId": 11, "mem": bit0(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 0},243: { "levelId": 11, "mem": bit1(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 1},244: { "levelId": 11, "mem": bit2(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 2},245: { "levelId": 11, "mem": bit3(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 3},246: { "levelId": 11, "mem": bit4(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 4},247: { "levelId": 11, "mem": bit5(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 5},248: { "levelId": 11, "mem": bit6(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 6},249: { "levelId": 11, "mem": bit7(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 7},250: { "levelId": 11, "mem": bit0(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 0},251: { "levelId": 11, "mem": bit1(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 1},252: { "levelId": 11, "mem": bit2(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 2},253: { "levelId": 11, "mem": bit3(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 3},254: { "levelId": 11, "mem": bit4(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 4},255: { "levelId": 11, "mem": bit5(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 5},256: { "levelId": 11, "mem": bit6(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 6},257: { "levelId": 11, "mem": bit7(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 7},258: { "levelId": 11, "mem": bit0(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 0},259: { "levelId": 11, "mem": bit1(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 1},260: { "levelId": 11, "mem": bit2(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 2},261: { "levelId": 11, "mem": bit3(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 3},262: { "levelId": 11, "mem": bit4(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 4},263: { "levelId": 11, "mem": bit5(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 5},264: { "levelId": 11, "mem": bit6(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 6},265: { "levelId": 11, "mem": bit7(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 7},266: { "levelId": 10, "mem": bit2(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 2},267: { "levelId": 10, "mem": bit2(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 2},268: { "levelId": 10, "mem": bit3(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 3},269: { "levelId": 10, "mem": bit4(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 4},270: { "levelId": 10, "mem": bit0(0x2249a6),"good": 1, "addr": 0x2249a6, "bit": 0},271: { "levelId": 10, "mem": bit1(0x2249a6),"good": 1, "addr": 0x2249a6, "bit": 1},272: { "levelId": 10, "mem": bit2(0x2249a6),"good": 1, "addr": 0x2249a6, "bit": 2},273: { "levelId": 10, "mem": bit3(0x2249a6),"good": 1, "addr": 0x2249a6, "bit": 3},274: { "levelId": 10, "mem": bit6(0x2249a6),"good": 1, "addr": 0x2249a6, "bit": 6},275: { "levelId": 10, "mem": bit7(0x2249a6),"good": 1, "addr": 0x2249a6, "bit": 7},276: { "levelId": 10, "mem": bit0(0x2249a7),"good": 1, "addr": 0x2249a7, "bit": 0},277: { "levelId": 10, "mem": bit1(0x2249a7),"good": 1, "addr": 0x2249a7, "bit": 1},278: { "levelId": 10, "mem": bit5(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 5},279: { "levelId": 10, "mem": bit6(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 6},280: { "levelId": 10, "mem": bit7(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 7},281: { "levelId": 10, "mem": bit0(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 0},282: { "levelId": 10, "mem": bit1(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 1},283: { "levelId": 10, "mem": bit7(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 7},284: { "levelId": 10, "mem": bit0(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 0},285: { "levelId": 10, "mem": bit1(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 1},286: { "levelId": 10, "mem": bit3(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 3},287: { "levelId": 10, "mem": bit4(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 4},288: { "levelId": 10, "mem": bit5(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 5},289: { "levelId": 10, "mem": bit6(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 6},290: { "levelId": 10, "mem": bit7(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 7},291: { "levelId": 10, "mem": bit4(0x2249a6),"good": 1, "addr": 0x2249a6, "bit": 4},292: { "levelId": 10, "mem": bit5(0x2249a6),"good": 1, "addr": 0x2249a6, "bit": 5},293: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},294: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},295: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},296: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},297: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},298: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},299: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},300: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},301: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},302: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},303: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},304: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},305: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},306: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},307: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},308: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},309: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},310: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},311: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},312: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},313: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},314: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},315: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},316: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},317: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},318: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},319: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},320: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},321: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},322: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},323: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},324: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},325: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},326: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},327: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},328: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},329: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},330: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},331: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},332: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},333: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},334: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},335: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},336: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},337: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},338: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},339: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},340: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},341: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},342: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},343: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},344: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},345: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},346: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},347: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},348: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},349: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},350: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},351: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},352: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},353: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},354: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},355: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},356: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},357: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},358: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},359: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},360: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},361: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},362: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},363: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},364: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},365: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},366: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},367: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},368: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},369: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},370: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},371: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},372: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},373: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},374: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},375: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},376: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},377: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},378: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},379: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},380: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},381: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},382: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},383: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},384: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},385: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},386: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},387: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},388: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},389: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},390: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},391: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},392: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},393: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},394: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},395: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},396: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},397: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},398: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},399: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},400: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},401: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},402: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},403: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},404: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},405: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},406: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},407: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},408: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},409: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},410: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},411: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},412: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},413: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},414: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},415: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},416: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},417: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},418: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},419: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},420: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},421: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},422: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},423: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},424: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},425: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},426: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},427: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},428: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},429: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},430: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},431: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},432: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},433: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},434: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},435: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},436: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},437: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},438: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},439: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},440: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},441: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},442: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},443: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},444: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},445: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},446: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},447: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},448: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},449: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},450: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},451: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},452: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},453: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},454: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},455: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},456: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},457: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},458: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},459: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},460: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},461: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},462: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},463: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},464: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},465: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},466: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},467: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},468: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},469: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},470: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},471: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},472: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},473: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},474: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},475: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},476: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},477: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},478: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},479: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},480: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},481: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},482: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},483: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},484: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},485: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},486: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},487: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},488: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},489: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},490: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},491: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},492: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},493: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},494: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},495: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},496: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},497: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},498: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},499: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},500: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},501: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},502: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},503: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},504: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},505: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},506: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},507: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},508: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},509: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},510: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},511: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},512: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},513: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},514: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},515: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},516: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},517: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},518: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},519: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},520: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},521: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},522: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},523: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},524: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},525: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},526: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},527: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},528: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},529: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},530: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},531: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},532: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},533: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},534: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},535: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},536: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},537: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},538: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},539: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},540: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},541: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},542: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},543: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},544: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},545: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},546: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},547: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},548: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},549: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},550: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},551: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},552: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},553: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},554: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},555: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},556: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},557: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},558: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},559: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},560: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},561: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},562: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},563: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},564: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},565: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},566: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},567: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},568: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},569: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},570: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},571: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},572: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},573: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},574: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},575: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},576: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},577: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},578: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},579: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},580: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},581: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},582: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},583: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},584: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},585: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},586: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},587: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},588: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},589: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},590: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},591: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},592: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},593: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},594: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},595: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},596: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},597: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},598: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},599: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},600: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},601: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},602: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},603: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},604: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},605: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},606: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},607: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},608: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},609: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},610: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},611: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},612: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},613: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},614: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},615: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},616: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},617: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},618: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},619: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},620: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},621: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},622: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},623: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},624: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},625: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},626: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},627: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},628: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},629: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},630: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},631: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},632: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},633: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},634: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},635: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},636: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},637: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},638: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},639: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},640: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},641: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},642: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},643: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},644: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},645: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},646: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},647: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},648: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},649: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},650: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},651: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},652: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},653: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},654: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},655: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},656: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},657: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},658: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},659: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},660: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},661: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},662: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},663: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},664: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},665: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},666: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},667: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},668: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},669: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},670: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},671: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},672: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},673: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},674: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},675: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},676: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},677: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},678: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},679: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},680: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},681: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},682: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},683: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},684: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},685: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},686: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},687: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},688: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},689: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},690: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},691: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},692: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},693: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},694: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},695: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},696: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},697: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},698: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},699: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},700: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},701: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},702: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},703: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},704: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},705: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},706: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},707: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},708: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},709: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},710: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},711: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},712: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},713: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},714: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},715: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},716: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},717: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},718: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},719: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},720: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},721: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},722: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},723: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},724: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},725: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},726: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},727: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},728: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},729: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},730: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},731: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},732: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},733: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},734: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},735: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},736: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},737: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},738: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},739: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},740: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},741: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},742: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},743: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},744: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},745: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},746: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},747: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},748: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},749: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},750: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},751: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},752: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},753: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},754: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},755: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},756: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},757: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},758: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},759: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},760: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},761: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},762: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},763: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},764: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},765: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},766: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},767: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},768: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},769: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},770: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},771: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},772: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},773: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},774: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},775: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},776: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},777: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},778: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},779: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},780: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},781: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},782: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},783: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},784: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},785: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},786: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},787: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},788: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},789: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},790: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},791: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},792: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},793: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},794: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},795: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},796: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},797: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},798: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},799: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},800: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},801: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},802: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},803: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},804: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},805: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},806: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},807: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},808: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},809: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},810: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},811: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},812: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},813: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},814: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},815: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},816: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},817: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},818: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},819: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},820: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},821: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},822: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},823: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},824: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},825: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},826: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},827: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},828: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},829: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},830: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},831: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},832: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},833: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},834: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},835: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},836: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},837: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},838: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},839: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},840: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},841: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},842: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},843: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},844: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},845: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},846: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},847: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},848: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},849: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},850: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},851: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},852: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},853: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},854: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},855: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},856: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},857: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},858: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},859: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},860: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},861: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},862: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},863: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},864: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},865: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},866: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},867: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},868: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},869: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},870: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},871: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},872: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},873: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},874: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},875: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},876: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},877: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},878: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},879: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},880: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},881: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},882: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},883: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},884: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},885: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},886: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},887: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},888: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},889: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},890: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},891: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},892: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},893: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},894: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},895: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},896: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},897: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},898: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},899: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},900: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},901: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},902: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},903: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},904: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},905: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},906: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},907: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},908: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},909: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},910: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},911: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},912: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},913: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},914: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},915: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},916: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},917: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},918: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},919: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},920: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},921: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},922: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},923: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},924: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},925: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},926: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},927: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},928: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},929: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},930: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},931: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},932: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},933: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},934: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},935: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},936: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},937: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},938: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},939: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},940: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},941: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},942: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},943: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},944: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},945: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},946: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},947: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},948: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},949: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},950: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},951: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},952: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},953: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},954: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},955: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},956: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},957: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},958: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},959: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},960: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},961: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},962: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},963: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},964: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},965: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},966: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},967: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},968: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},969: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},970: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},971: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},972: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},973: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},974: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},975: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},976: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},977: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},978: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},979: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},980: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},981: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},982: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},983: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},984: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},985: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},986: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},987: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},988: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},989: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},990: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},991: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},992: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},993: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},994: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},995: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},996: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},997: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},998: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},999: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},1000: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>1: { "levelId": 2, "mem": bit0(0x224988),"good": 1, "addr": 0x224988, "bit": 0},2: { "levelId": 2, "mem": bit1(0x224988),"good": 1, "addr": 0x224988, "bit": 1},3: { "levelId": 2, "mem": bit2(0x224988),"good": 1, "addr": 0x224988, "bit": 2},4: { "levelId": 2, "mem": bit3(0x224988),"good": 1, "addr": 0x224988, "bit": 3},5: { "levelId": 2, "mem": bit4(0x224988),"good": 1, "addr": 0x224988, "bit": 4},6: { "levelId": 2, "mem": bit5(0x224988),"good": 1, "addr": 0x224988, "bit": 5},7: { "levelId": 2, "mem": bit6(0x224988),"good": 1, "addr": 0x224988, "bit": 6},8: { "levelId": 2, "mem": bit7(0x224988),"good": 1, "addr": 0x224988, "bit": 7},9: { "levelId": 2, "mem": bit2(0x224989),"good": 1, "addr": 0x224989, "bit": 2},10: { "levelId": 2, "mem": bit1(0x22498a),"good": 1, "addr": 0x22498a, "bit": 1},11: { "levelId": 2, "mem": bit2(0x22498a),"good": 1, "addr": 0x22498a, "bit": 2},12: { "levelId": 2, "mem": bit3(0x22498a),"good": 1, "addr": 0x22498a, "bit": 3},13: { "levelId": 2, "mem": bit4(0x22498a),"good": 1, "addr": 0x22498a, "bit": 4},14: { "levelId": 2, "mem": bit5(0x22498a),"good": 1, "addr": 0x22498a, "bit": 5},15: { "levelId": 2, "mem": bit6(0x22498a),"good": 1, "addr": 0x22498a, "bit": 6},16: { "levelId": 2, "mem": bit7(0x22498a),"good": 1, "addr": 0x22498a, "bit": 7},17: { "levelId": 2, "mem": bit5(0x22498b),"good": 1, "addr": 0x22498b, "bit": 5},18: { "levelId": 2, "mem": bit6(0x22498b),"good": 1, "addr": 0x22498b, "bit": 6},19: { "levelId": 2, "mem": bit7(0x22498b),"good": 1, "addr": 0x22498b, "bit": 7},20: { "levelId": 2, "mem": bit0(0x22498c),"good": 1, "addr": 0x22498c, "bit": 0},21: { "levelId": 2, "mem": bit1(0x22498c),"good": 1, "addr": 0x22498c, "bit": 1},22: { "levelId": 2, "mem": bit2(0x22498c),"good": 1, "addr": 0x22498c, "bit": 2},23: { "levelId": 2, "mem": bit3(0x22498c),"good": 1, "addr": 0x22498c, "bit": 3},24: { "levelId": 2, "mem": bit4(0x22498c),"good": 1, "addr": 0x22498c, "bit": 4},25: { "levelId": 2, "mem": bit5(0x22498c),"good": 1, "addr": 0x22498c, "bit": 5},26: { "levelId": 2, "mem": bit6(0x22498c),"good": 1, "addr": 0x22498c, "bit": 6},27: { "levelId": 2, "mem": bit7(0x22498c),"good": 1, "addr": 0x22498c, "bit": 7},28: { "levelId": 2, "mem": bit0(0x22498d),"good": 1, "addr": 0x22498d, "bit": 0},29: { "levelId": 2, "mem": bit1(0x22498d),"good": 1, "addr": 0x22498d, "bit": 1},30: { "levelId": 2, "mem": bit2(0x22498d),"good": 1, "addr": 0x22498d, "bit": 2},31: { "levelId": 2, "mem": bit3(0x22498d),"good": 1, "addr": 0x22498d, "bit": 3},32: { "levelId": 2, "mem": bit4(0x22498d),"good": 1, "addr": 0x22498d, "bit": 4},33: { "levelId": 2, "mem": bit5(0x22498d),"good": 1, "addr": 0x22498d, "bit": 5},34: { "levelId": 2, "mem": bit6(0x22498d),"good": 1, "addr": 0x22498d, "bit": 6},35: { "levelId": 2, "mem": bit7(0x22498d),"good": 1, "addr": 0x22498d, "bit": 7},36: { "levelId": 2, "mem": bit0(0x22498e),"good": 1, "addr": 0x22498e, "bit": 0},37: { "levelId": 2, "mem": bit1(0x22498e),"good": 1, "addr": 0x22498e, "bit": 1},38: { "levelId": 5, "mem": bit2(0x22498e),"good": 1, "addr": 0x22498e, "bit": 2},39: { "levelId": 5, "mem": bit3(0x22498e),"good": 1, "addr": 0x22498e, "bit": 3},40: { "levelId": 5, "mem": bit4(0x22498e),"good": 1, "addr": 0x22498e, "bit": 4},41: { "levelId": 5, "mem": bit5(0x22498e),"good": 1, "addr": 0x22498e, "bit": 5},42: { "levelId": 5, "mem": bit6(0x22498e),"good": 1, "addr": 0x22498e, "bit": 6},43: { "levelId": 5, "mem": bit7(0x22498e),"good": 1, "addr": 0x22498e, "bit": 7},44: { "levelId": 5, "mem": bit0(0x22498f),"good": 1, "addr": 0x22498f, "bit": 0},45: { "levelId": 5, "mem": bit1(0x22498f),"good": 1, "addr": 0x22498f, "bit": 1},46: { "levelId": 5, "mem": bit2(0x22498f),"good": 1, "addr": 0x22498f, "bit": 2},47: { "levelId": 5, "mem": bit3(0x22498f),"good": 1, "addr": 0x22498f, "bit": 3},48: { "levelId": 5, "mem": bit4(0x22498f),"good": 1, "addr": 0x22498f, "bit": 4},49: { "levelId": 5, "mem": bit5(0x22498f),"good": 1, "addr": 0x22498f, "bit": 5},50: { "levelId": 5, "mem": bit6(0x22498f),"good": 1, "addr": 0x22498f, "bit": 6},51: { "levelId": 5, "mem": bit7(0x22498f),"good": 1, "addr": 0x22498f, "bit": 7},52: { "levelId": 5, "mem": bit0(0x224990),"good": 1, "addr": 0x224990, "bit": 0},53: { "levelId": 5, "mem": bit1(0x224990),"good": 1, "addr": 0x224990, "bit": 1},54: { "levelId": 5, "mem": bit2(0x224990),"good": 1, "addr": 0x224990, "bit": 2},55: { "levelId": 5, "mem": bit3(0x224990),"good": 1, "addr": 0x224990, "bit": 3},56: { "levelId": 5, "mem": bit4(0x224990),"good": 1, "addr": 0x224990, "bit": 4},57: { "levelId": 5, "mem": bit5(0x224990),"good": 1, "addr": 0x224990, "bit": 5},58: { "levelId": 5, "mem": bit6(0x224990),"good": 1, "addr": 0x224990, "bit": 6},59: { "levelId": 5, "mem": bit7(0x224990),"good": 1, "addr": 0x224990, "bit": 7},60: { "levelId": 5, "mem": bit0(0x224991),"good": 1, "addr": 0x224991, "bit": 0},61: { "levelId": 5, "mem": bit1(0x224991),"good": 1, "addr": 0x224991, "bit": 1},62: { "levelId": 5, "mem": bit2(0x224991),"good": 1, "addr": 0x224991, "bit": 2},63: { "levelId": 5, "mem": bit3(0x224991),"good": 1, "addr": 0x224991, "bit": 3},64: { "levelId": 5, "mem": bit4(0x224991),"good": 1, "addr": 0x224991, "bit": 4},65: { "levelId": 5, "mem": bit5(0x224991),"good": 1, "addr": 0x224991, "bit": 5},66: { "levelId": 5, "mem": bit6(0x224991),"good": 1, "addr": 0x224991, "bit": 6},67: { "levelId": 5, "mem": bit7(0x224991),"good": 1, "addr": 0x224991, "bit": 7},68: { "levelId": 5, "mem": bit0(0x224992),"good": 1, "addr": 0x224992, "bit": 0},69: { "levelId": 5, "mem": bit1(0x224992),"good": 1, "addr": 0x224992, "bit": 1},70: { "levelId": 5, "mem": bit2(0x224992),"good": 1, "addr": 0x224992, "bit": 2},71: { "levelId": 5, "mem": bit3(0x224992),"good": 1, "addr": 0x224992, "bit": 3},72: { "levelId": 5, "mem": bit4(0x224992),"good": 1, "addr": 0x224992, "bit": 4},73: { "levelId": 5, "mem": bit5(0x224992),"good": 1, "addr": 0x224992, "bit": 5},74: { "levelId": 5, "mem": bit6(0x224992),"good": 1, "addr": 0x224992, "bit": 6},75: { "levelId": 5, "mem": bit7(0x224992),"good": 1, "addr": 0x224992, "bit": 7},76: { "levelId": 5, "mem": bit0(0x224993),"good": 1, "addr": 0x224993, "bit": 0},77: { "levelId": 5, "mem": bit1(0x224993),"good": 1, "addr": 0x224993, "bit": 1},78: { "levelId": 5, "mem": bit2(0x224993),"good": 1, "addr": 0x224993, "bit": 2},79: { "levelId": 5, "mem": bit3(0x224993),"good": 1, "addr": 0x224993, "bit": 3},80: { "levelId": 5, "mem": bit4(0x224993),"good": 1, "addr": 0x224993, "bit": 4},81: { "levelId": 5, "mem": bit5(0x224993),"good": 1, "addr": 0x224993, "bit": 5},82: { "levelId": 5, "mem": bit6(0x224993),"good": 1, "addr": 0x224993, "bit": 6},83: { "levelId": 5, "mem": bit7(0x224993),"good": 1, "addr": 0x224993, "bit": 7},84: { "levelId": 5, "mem": bit0(0x224994),"good": 1, "addr": 0x224994, "bit": 0},85: { "levelId": 5, "mem": bit1(0x224994),"good": 1, "addr": 0x224994, "bit": 1},86: { "levelId": 5, "mem": bit2(0x224994),"good": 1, "addr": 0x224994, "bit": 2},87: { "levelId": 5, "mem": bit3(0x224994),"good": 1, "addr": 0x224994, "bit": 3},88: { "levelId": 6, "mem": bit4(0x224994),"good": 1, "addr": 0x224994, "bit": 4},89: { "levelId": 6, "mem": bit5(0x224994),"good": 1, "addr": 0x224994, "bit": 5},90: { "levelId": 6, "mem": bit6(0x224994),"good": 1, "addr": 0x224994, "bit": 6},91: { "levelId": 6, "mem": bit7(0x224994),"good": 1, "addr": 0x224994, "bit": 7},92: { "levelId": 6, "mem": bit0(0x224995),"good": 1, "addr": 0x224995, "bit": 0},93: { "levelId": 6, "mem": bit1(0x224995),"good": 1, "addr": 0x224995, "bit": 1},94: { "levelId": 6, "mem": bit2(0x224995),"good": 1, "addr": 0x224995, "bit": 2},95: { "levelId": 6, "mem": bit3(0x224995),"good": 1, "addr": 0x224995, "bit": 3},96: { "levelId": 6, "mem": bit4(0x224995),"good": 1, "addr": 0x224995, "bit": 4},97: { "levelId": 6, "mem": bit5(0x224995),"good": 1, "addr": 0x224995, "bit": 5},98: { "levelId": 6, "mem": bit6(0x224995),"good": 1, "addr": 0x224995, "bit": 6},99: { "levelId": 6, "mem": bit7(0x224995),"good": 1, "addr": 0x224995, "bit": 7},100: { "levelId": 6, "mem": bit0(0x224996),"good": 1, "addr": 0x224996, "bit": 0},101: { "levelId": 6, "mem": bit1(0x224996),"good": 1, "addr": 0x224996, "bit": 1},102: { "levelId": 6, "mem": bit2(0x224996),"good": 1, "addr": 0x224996, "bit": 2},103: { "levelId": 6, "mem": bit3(0x224996),"good": 1, "addr": 0x224996, "bit": 3},104: { "levelId": 6, "mem": bit4(0x224996),"good": 1, "addr": 0x224996, "bit": 4},105: { "levelId": 6, "mem": bit5(0x224996),"good": 1, "addr": 0x224996, "bit": 5},106: { "levelId": 6, "mem": bit6(0x224996),"good": 1, "addr": 0x224996, "bit": 6},107: { "levelId": 6, "mem": bit7(0x224996),"good": 1, "addr": 0x224996, "bit": 7},108: { "levelId": 6, "mem": bit0(0x224997),"good": 1, "addr": 0x224997, "bit": 0},109: { "levelId": 6, "mem": bit1(0x224997),"good": 1, "addr": 0x224997, "bit": 1},110: { "levelId": 6, "mem": bit2(0x224997),"good": 1, "addr": 0x224997, "bit": 2},111: { "levelId": 6, "mem": bit3(0x224997),"good": 1, "addr": 0x224997, "bit": 3},112: { "levelId": 6, "mem": bit4(0x224997),"good": 1, "addr": 0x224997, "bit": 4},113: { "levelId": 6, "mem": bit5(0x224997),"good": 1, "addr": 0x224997, "bit": 5},114: { "levelId": 6, "mem": bit6(0x224997),"good": 1, "addr": 0x224997, "bit": 6},115: { "levelId": 6, "mem": bit7(0x224997),"good": 1, "addr": 0x224997, "bit": 7},116: { "levelId": 6, "mem": bit0(0x224998),"good": 1, "addr": 0x224998, "bit": 0},117: { "levelId": 6, "mem": bit1(0x224998),"good": 1, "addr": 0x224998, "bit": 1},118: { "levelId": 6, "mem": bit2(0x224998),"good": 1, "addr": 0x224998, "bit": 2},119: { "levelId": 6, "mem": bit3(0x224998),"good": 1, "addr": 0x224998, "bit": 3},120: { "levelId": 6, "mem": bit4(0x224998),"good": 1, "addr": 0x224998, "bit": 4},121: { "levelId": 6, "mem": bit5(0x224998),"good": 1, "addr": 0x224998, "bit": 5},122: { "levelId": 6, "mem": bit6(0x224998),"good": 1, "addr": 0x224998, "bit": 6},123: { "levelId": 6, "mem": bit0(0x224999),"good": 1, "addr": 0x224999, "bit": 0},124: { "levelId": 6, "mem": bit1(0x224999),"good": 1, "addr": 0x224999, "bit": 1},125: { "levelId": 6, "mem": bit2(0x224999),"good": 1, "addr": 0x224999, "bit": 2},126: { "levelId": 6, "mem": bit3(0x224999),"good": 1, "addr": 0x224999, "bit": 3},127: { "levelId": 6, "mem": bit4(0x224999),"good": 1, "addr": 0x224999, "bit": 4},128: { "levelId": 6, "mem": bit5(0x224999),"good": 1, "addr": 0x224999, "bit": 5},129: { "levelId": 6, "mem": bit6(0x224999),"good": 1, "addr": 0x224999, "bit": 6},130: { "levelId": 6, "mem": bit7(0x224999),"good": 1, "addr": 0x224999, "bit": 7},131: { "levelId": 6, "mem": bit0(0x22499a),"good": 1, "addr": 0x22499a, "bit": 0},132: { "levelId": 6, "mem": bit1(0x22499a),"good": 1, "addr": 0x22499a, "bit": 1},133: { "levelId": 6, "mem": bit2(0x22499a),"good": 1, "addr": 0x22499a, "bit": 2},134: { "levelId": 6, "mem": bit3(0x22499a),"good": 1, "addr": 0x22499a, "bit": 3},135: { "levelId": 6, "mem": bit4(0x22499a),"good": 1, "addr": 0x22499a, "bit": 4},136: { "levelId": 6, "mem": bit5(0x22499a),"good": 1, "addr": 0x22499a, "bit": 5},137: { "levelId": 1, "mem": bit3(0x224a36),"good": 1, "addr": 0x224a36, "bit": 3},138: { "levelId": 1, "mem": bit4(0x224a36),"good": 1, "addr": 0x224a36, "bit": 4},139: { "levelId": 1, "mem": bit5(0x224a36),"good": 1, "addr": 0x224a36, "bit": 5},140: { "levelId": 1, "mem": bit6(0x224a36),"good": 1, "addr": 0x224a36, "bit": 6},141: { "levelId": 1, "mem": bit7(0x224a36),"good": 1, "addr": 0x224a36, "bit": 7},142: { "levelId": 6, "mem": bit7(0x224998),"good": 1, "addr": 0x224998, "bit": 7},143: { "levelId": 8, "mem": bit3(0x22499b),"good": 1, "addr": 0x22499b, "bit": 3},144: { "levelId": 8, "mem": bit4(0x22499b),"good": 1, "addr": 0x22499b, "bit": 4},145: { "levelId": 8, "mem": bit5(0x22499b),"good": 1, "addr": 0x22499b, "bit": 5},146: { "levelId": 8, "mem": bit5(0x22499c),"good": 1, "addr": 0x22499c, "bit": 5},147: { "levelId": 8, "mem": bit6(0x22499c),"good": 1, "addr": 0x22499c, "bit": 6},148: { "levelId": 8, "mem": bit7(0x22499c),"good": 1, "addr": 0x22499c, "bit": 7},149: { "levelId": 8, "mem": bit0(0x22499d),"good": 1, "addr": 0x22499d, "bit": 0},150: { "levelId": 8, "mem": bit1(0x22499d),"good": 1, "addr": 0x22499d, "bit": 1},151: { "levelId": 8, "mem": bit2(0x22499d),"good": 1, "addr": 0x22499d, "bit": 2},152: { "levelId": 8, "mem": bit3(0x22499d),"good": 1, "addr": 0x22499d, "bit": 3},153: { "levelId": 8, "mem": bit4(0x22499d),"good": 1, "addr": 0x22499d, "bit": 4},154: { "levelId": 8, "mem": bit5(0x22499d),"good": 1, "addr": 0x22499d, "bit": 5},155: { "levelId": 8, "mem": bit6(0x22499d),"good": 1, "addr": 0x22499d, "bit": 6},156: { "levelId": 8, "mem": bit7(0x22499d),"good": 1, "addr": 0x22499d, "bit": 7},157: { "levelId": 8, "mem": bit0(0x22499e),"good": 1, "addr": 0x22499e, "bit": 0},158: { "levelId": 8, "mem": bit1(0x22499e),"good": 1, "addr": 0x22499e, "bit": 1},159: { "levelId": 8, "mem": bit6(0x22499a),"good": 1, "addr": 0x22499a, "bit": 6},160: { "levelId": 8, "mem": bit7(0x22499a),"good": 1, "addr": 0x22499a, "bit": 7},161: { "levelId": 8, "mem": bit0(0x22499b),"good": 1, "addr": 0x22499b, "bit": 0},162: { "levelId": 8, "mem": bit1(0x22499b),"good": 1, "addr": 0x22499b, "bit": 1},163: { "levelId": 8, "mem": bit2(0x22499b),"good": 1, "addr": 0x22499b, "bit": 2},164: { "levelId": 8, "mem": bit6(0x22499b),"good": 1, "addr": 0x22499b, "bit": 6},165: { "levelId": 8, "mem": bit7(0x22499b),"good": 1, "addr": 0x22499b, "bit": 7},166: { "levelId": 8, "mem": bit0(0x22499c),"good": 1, "addr": 0x22499c, "bit": 0},167: { "levelId": 8, "mem": bit1(0x22499c),"good": 1, "addr": 0x22499c, "bit": 1},168: { "levelId": 8, "mem": bit2(0x22499c),"good": 1, "addr": 0x22499c, "bit": 2},169: { "levelId": 8, "mem": bit3(0x22499c),"good": 1, "addr": 0x22499c, "bit": 3},170: { "levelId": 8, "mem": bit4(0x22499c),"good": 1, "addr": 0x22499c, "bit": 4},171: { "levelId": 8, "mem": bit2(0x22499e),"good": 1, "addr": 0x22499e, "bit": 2},172: { "levelId": 8, "mem": bit3(0x22499e),"good": 1, "addr": 0x22499e, "bit": 3},173: { "levelId": 8, "mem": bit4(0x22499e),"good": 1, "addr": 0x22499e, "bit": 4},174: { "levelId": 8, "mem": bit5(0x22499e),"good": 1, "addr": 0x22499e, "bit": 5},175: { "levelId": 8, "mem": bit6(0x22499e),"good": 1, "addr": 0x22499e, "bit": 6},176: { "levelId": 8, "mem": bit7(0x22499e),"good": 1, "addr": 0x22499e, "bit": 7},177: { "levelId": 8, "mem": bit0(0x22499f),"good": 1, "addr": 0x22499f, "bit": 0},178: { "levelId": 8, "mem": bit1(0x22499f),"good": 1, "addr": 0x22499f, "bit": 1},179: { "levelId": 8, "mem": bit2(0x22499f),"good": 1, "addr": 0x22499f, "bit": 2},180: { "levelId": 8, "mem": bit3(0x22499f),"good": 1, "addr": 0x22499f, "bit": 3},181: { "levelId": 8, "mem": bit4(0x22499f),"good": 1, "addr": 0x22499f, "bit": 4},182: { "levelId": 8, "mem": bit5(0x22499f),"good": 1, "addr": 0x22499f, "bit": 5},183: { "levelId": 8, "mem": bit6(0x22499f),"good": 1, "addr": 0x22499f, "bit": 6},184: { "levelId": 8, "mem": bit7(0x22499f),"good": 1, "addr": 0x22499f, "bit": 7},185: { "levelId": 8, "mem": bit0(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 0},186: { "levelId": 8, "mem": bit1(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 1},187: { "levelId": 8, "mem": bit2(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 2},188: { "levelId": 8, "mem": bit3(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 3},189: { "levelId": 8, "mem": bit4(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 4},190: { "levelId": 8, "mem": bit5(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 5},191: { "levelId": 8, "mem": bit6(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 6},192: { "levelId": 8, "mem": bit7(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 7},193: { "levelId": 10, "mem": bit0(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 0},194: { "levelId": 10, "mem": bit1(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 1},195: { "levelId": 10, "mem": bit2(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 2},196: { "levelId": 10, "mem": bit3(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 3},197: { "levelId": 10, "mem": bit4(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 4},198: { "levelId": 10, "mem": bit2(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 2},199: { "levelId": 10, "mem": bit3(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 3},200: { "levelId": 10, "mem": bit4(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 4},201: { "levelId": 10, "mem": bit5(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 5},202: { "levelId": 10, "mem": bit6(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 6},203: { "levelId": 10, "mem": bit1(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 1},204: { "levelId": 10, "mem": bit5(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 5},205: { "levelId": 10, "mem": bit6(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 6},206: { "levelId": 10, "mem": bit7(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 7},207: { "levelId": 10, "mem": bit0(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 0},208: { "levelId": 10, "mem": bit3(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 3},209: { "levelId": 10, "mem": bit5(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 5},210: { "levelId": 10, "mem": bit6(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 6},211: { "levelId": 10, "mem": bit7(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 7},212: { "levelId": 10, "mem": bit0(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 0},213: { "levelId": 10, "mem": bit1(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 1},214: { "levelId": 10, "mem": bit2(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 2},215: { "levelId": 10, "mem": bit4(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 4},216: { "levelId": 11, "mem": bit6(0x2249e5),"good": 1, "addr": 0x2249e5, "bit": 6},217: { "levelId": 11, "mem": bit7(0x2249e5),"good": 1, "addr": 0x2249e5, "bit": 7},218: { "levelId": 11, "mem": bit0(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 0},219: { "levelId": 11, "mem": bit1(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 1},220: { "levelId": 11, "mem": bit2(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 2},221: { "levelId": 11, "mem": bit3(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 3},222: { "levelId": 11, "mem": bit4(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 4},223: { "levelId": 11, "mem": bit5(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 5},224: { "levelId": 11, "mem": bit6(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 6},225: { "levelId": 11, "mem": bit7(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 7},226: { "levelId": 11, "mem": bit0(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 0},227: { "levelId": 11, "mem": bit1(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 1},228: { "levelId": 11, "mem": bit2(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 2},229: { "levelId": 11, "mem": bit3(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 3},230: { "levelId": 11, "mem": bit4(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 4},231: { "levelId": 11, "mem": bit5(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 5},232: { "levelId": 11, "mem": bit6(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 6},233: { "levelId": 11, "mem": bit7(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 7},234: { "levelId": 11, "mem": bit0(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 0},235: { "levelId": 11, "mem": bit1(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 1},236: { "levelId": 11, "mem": bit2(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 2},237: { "levelId": 11, "mem": bit3(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 3},238: { "levelId": 11, "mem": bit4(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 4},239: { "levelId": 11, "mem": bit5(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 5},240: { "levelId": 11, "mem": bit6(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 6},241: { "levelId": 11, "mem": bit7(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 7},242: { "levelId": 11, "mem": bit0(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 0},243: { "levelId": 11, "mem": bit1(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 1},244: { "levelId": 11, "mem": bit2(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 2},245: { "levelId": 11, "mem": bit3(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 3},246: { "levelId": 11, "mem": bit4(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 4},247: { "levelId": 11, "mem": bit5(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 5},248: { "levelId": 11, "mem": bit6(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 6},249: { "levelId": 11, "mem": bit7(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 7},250: { "levelId": 11, "mem": bit0(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 0},251: { "levelId": 11, "mem": bit1(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 1},252: { "levelId": 11, "mem": bit2(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 2},253: { "levelId": 11, "mem": bit3(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 3},254: { "levelId": 11, "mem": bit4(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 4},255: { "levelId": 11, "mem": bit5(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 5},256: { "levelId": 11, "mem": bit6(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 6},257: { "levelId": 11, "mem": bit7(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 7},258: { "levelId": 11, "mem": bit0(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 0},259: { "levelId": 11, "mem": bit1(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 1},260: { "levelId": 11, "mem": bit2(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 2},261: { "levelId": 11, "mem": bit3(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 3},262: { "levelId": 11, "mem": bit4(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 4},263: { "levelId": 11, "mem": bit5(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 5},264: { "levelId": 11, "mem": bit6(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 6},265: { "levelId": 11, "mem": bit7(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 7},266: { "levelId": 10, "mem": bit2(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 2},267: { "levelId": 10, "mem": bit2(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 2},268: { "levelId": 10, "mem": bit3(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 3},269: { "levelId": 10, "mem": bit4(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 4},270: { "levelId": 10, "mem": bit0(0x2249a6),"good": 1, "addr": 0x2249a6, "bit": 0},271: { "levelId": 10, "mem": bit1(0x2249a6),"good": 1, "addr": 0x2249a6, "bit": 1},272: { "levelId": 10, "mem": bit2(0x2249a6),"good": 1, "addr": 0x2249a6, "bit": 2},273: { "levelId": 10, "mem": bit3(0x2249a6),"good": 1, "addr": 0x2249a6, "bit": 3},274: { "levelId": 10, "mem": bit6(0x2249a6),"good": 1, "addr": 0x2249a6, "bit": 6},275: { "levelId": 10, "mem": bit7(0x2249a6),"good": 1, "addr": 0x2249a6, "bit": 7},276: { "levelId": 10, "mem": bit0(0x2249a7),"good": 1, "addr": 0x2249a7, "bit": 0},277: { "levelId": 10, "mem": bit1(0x2249a7),"good": 1, "addr": 0x2249a7, "bit": 1},278: { "levelId": 10, "mem": bit5(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 5},279: { "levelId": 10, "mem": bit6(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 6},280: { "levelId": 10, "mem": bit7(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 7},281: { "levelId": 10, "mem": bit0(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 0},282: { "levelId": 10, "mem": bit1(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 1},283: { "levelId": 10, "mem": bit7(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 7},284: { "levelId": 10, "mem": bit0(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 0},285: { "levelId": 10, "mem": bit1(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 1},286: { "levelId": 10, "mem": bit3(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 3},287: { "levelId": 10, "mem": bit4(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 4},288: { "levelId": 10, "mem": bit5(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 5},289: { "levelId": 10, "mem": bit6(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 6},290: { "levelId": 10, "mem": bit7(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 7},291: { "levelId": 10, "mem": bit4(0x2249a6),"good": 1, "addr": 0x2249a6, "bit": 4},292: { "levelId": 10, "mem": bit5(0x2249a6),"good": 1, "addr": 0x2249a6, "bit": 5},293: { "levelId": 12, "mem": bit2(0x2249a7),"good": 1, "addr": 0x2249a7, "bit": 2},294: { "levelId": 12, "mem": bit3(0x2249a7),"good": 1, "addr": 0x2249a7, "bit": 3},295: { "levelId": 12, "mem": bit4(0x2249a7),"good": 1, "addr": 0x2249a7, "bit": 4},296: { "levelId": 12, "mem": bit5(0x2249a7),"good": 1, "addr": 0x2249a7, "bit": 5},297: { "levelId": 12, "mem": bit6(0x2249a7),"good": 1, "addr": 0x2249a7, "bit": 6},298: { "levelId": 12, "mem": bit7(0x2249a7),"good": 1, "addr": 0x2249a7, "bit": 7},299: { "levelId": 12, "mem": bit0(0x2249a8),"good": 1, "addr": 0x2249a8, "bit": 0},300: { "levelId": 12, "mem": bit1(0x2249a8),"good": 1, "addr": 0x2249a8, "bit": 1},301: { "levelId": 12, "mem": bit2(0x2249a8),"good": 1, "addr": 0x2249a8, "bit": 2},302: { "levelId": 12, "mem": bit3(0x2249a8),"good": 1, "addr": 0x2249a8, "bit": 3},303: { "levelId": 12, "mem": bit4(0x2249a8),"good": 1, "addr": 0x2249a8, "bit": 4},304: { "levelId": 12, "mem": bit5(0x2249a8),"good": 1, "addr": 0x2249a8, "bit": 5},305: { "levelId": 12, "mem": bit6(0x2249a8),"good": 1, "addr": 0x2249a8, "bit": 6},306: { "levelId": 12, "mem": bit7(0x2249a8),"good": 1, "addr": 0x2249a8, "bit": 7},307: { "levelId": 12, "mem": bit0(0x2249a9),"good": 1, "addr": 0x2249a9, "bit": 0},308: { "levelId": 12, "mem": bit1(0x2249a9),"good": 1, "addr": 0x2249a9, "bit": 1},309: { "levelId": 12, "mem": bit2(0x2249a9),"good": 1, "addr": 0x2249a9, "bit": 2},310: { "levelId": 12, "mem": bit3(0x2249a9),"good": 1, "addr": 0x2249a9, "bit": 3},311: { "levelId": 12, "mem": bit4(0x2249a9),"good": 1, "addr": 0x2249a9, "bit": 4},312: { "levelId": 12, "mem": bit5(0x2249a9),"good": 1, "addr": 0x2249a9, "bit": 5},313: { "levelId": 12, "mem": bit6(0x2249a9),"good": 1, "addr": 0x2249a9, "bit": 6},314: { "levelId": 12, "mem": bit1(0x2249aa),"good": 1, "addr": 0x2249aa, "bit": 1},315: { "levelId": 12, "mem": bit2(0x2249aa),"good": 1, "addr": 0x2249aa, "bit": 2},316: { "levelId": 12, "mem": bit2(0x2249ab),"good": 1, "addr": 0x2249ab, "bit": 2},317: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},318: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},319: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},320: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},321: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},322: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},323: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},324: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},325: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},326: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},327: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},328: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},329: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},330: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},331: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},332: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},333: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},334: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},335: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},336: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},337: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},338: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},339: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},340: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},341: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},342: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},343: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},344: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},345: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},346: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},347: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},348: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},349: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},350: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},351: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},352: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},353: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},354: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},355: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},356: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},357: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},358: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},359: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},360: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},361: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},362: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},363: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},364: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},365: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},366: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},367: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},368: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},369: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},370: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},371: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},372: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},373: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},374: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},375: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},376: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},377: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},378: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},379: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},380: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},381: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},382: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},383: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},384: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},385: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},386: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},387: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},388: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},389: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},390: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},391: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},392: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},393: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},394: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},395: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},396: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},397: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},398: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},399: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},400: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},401: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},402: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},403: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},404: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},405: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},406: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},407: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},408: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},409: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},410: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},411: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},412: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},413: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},414: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},415: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},416: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},417: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},418: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},419: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},420: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},421: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},422: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},423: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},424: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},425: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},426: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},427: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},428: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},429: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},430: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},431: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},432: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},433: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},434: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},435: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},436: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},437: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},438: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},439: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},440: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},441: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},442: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},443: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},444: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},445: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},446: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},447: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},448: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},449: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},450: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},451: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},452: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},453: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},454: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},455: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},456: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},457: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},458: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},459: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},460: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},461: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},462: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},463: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},464: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},465: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},466: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},467: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},468: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},469: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},470: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},471: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},472: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},473: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},474: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},475: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},476: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},477: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},478: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},479: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},480: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},481: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},482: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},483: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},484: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},485: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},486: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},487: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},488: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},489: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},490: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},491: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},492: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},493: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},494: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},495: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},496: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},497: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},498: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},499: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},500: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},501: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},502: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},503: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},504: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},505: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},506: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},507: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},508: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},509: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},510: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},511: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},512: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},513: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},514: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},515: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},516: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},517: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},518: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},519: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},520: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},521: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},522: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},523: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},524: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},525: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},526: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},527: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},528: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},529: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},530: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},531: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},532: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},533: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},534: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},535: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},536: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},537: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},538: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},539: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},540: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},541: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},542: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},543: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},544: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},545: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},546: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},547: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},548: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},549: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},550: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},551: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},552: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},553: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},554: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},555: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},556: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},557: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},558: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},559: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},560: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},561: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},562: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},563: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},564: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},565: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},566: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},567: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},568: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},569: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},570: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},571: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},572: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},573: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},574: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},575: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},576: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},577: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},578: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},579: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},580: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},581: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},582: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},583: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},584: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},585: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},586: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},587: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},588: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},589: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},590: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},591: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},592: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},593: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},594: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},595: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},596: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},597: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},598: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},599: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},600: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},601: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},602: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},603: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},604: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},605: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},606: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},607: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},608: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},609: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},610: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},611: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},612: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},613: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},614: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},615: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},616: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},617: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},618: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},619: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},620: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},621: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},622: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},623: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},624: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},625: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},626: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},627: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},628: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},629: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},630: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},631: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},632: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},633: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},634: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},635: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},636: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},637: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},638: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},639: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},640: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},641: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},642: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},643: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},644: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},645: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},646: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},647: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},648: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},649: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},650: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},651: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},652: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},653: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},654: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},655: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},656: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},657: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},658: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},659: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},660: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},661: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},662: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},663: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},664: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},665: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},666: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},667: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},668: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},669: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},670: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},671: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},672: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},673: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},674: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},675: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},676: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},677: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},678: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},679: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},680: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},681: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},682: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},683: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},684: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},685: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},686: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},687: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},688: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},689: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},690: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},691: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},692: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},693: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},694: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},695: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},696: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},697: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},698: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},699: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},700: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},701: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},702: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},703: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},704: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},705: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},706: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},707: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},708: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},709: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},710: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},711: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},712: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},713: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},714: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},715: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},716: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},717: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},718: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},719: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},720: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},721: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},722: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},723: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},724: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},725: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},726: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},727: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},728: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},729: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},730: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},731: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},732: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},733: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},734: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},735: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},736: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},737: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},738: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},739: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},740: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},741: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},742: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},743: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},744: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},745: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},746: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},747: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},748: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},749: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},750: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},751: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},752: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},753: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},754: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},755: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},756: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},757: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},758: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},759: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},760: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},761: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},762: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},763: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},764: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},765: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},766: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},767: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},768: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},769: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},770: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},771: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},772: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},773: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},774: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},775: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},776: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},777: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},778: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},779: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},780: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},781: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},782: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},783: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},784: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},785: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},786: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},787: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},788: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},789: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},790: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},791: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},792: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},793: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},794: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},795: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},796: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},797: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},798: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},799: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},800: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},801: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},802: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},803: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},804: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},805: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},806: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},807: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},808: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},809: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},810: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},811: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},812: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},813: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},814: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},815: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},816: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},817: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},818: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},819: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},820: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},821: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},822: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},823: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},824: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},825: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},826: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},827: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},828: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},829: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},830: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},831: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},832: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},833: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},834: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},835: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},836: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},837: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},838: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},839: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},840: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},841: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},842: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},843: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},844: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},845: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},846: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},847: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},848: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},849: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},850: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},851: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},852: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},853: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},854: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},855: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},856: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},857: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},858: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},859: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},860: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},861: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},862: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},863: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},864: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},865: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},866: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},867: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},868: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},869: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},870: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},871: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},872: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},873: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},874: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},875: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},876: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},877: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},878: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},879: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},880: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},881: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},882: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},883: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},884: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},885: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},886: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},887: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},888: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},889: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},890: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},891: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},892: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},893: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},894: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},895: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},896: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},897: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},898: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},899: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},900: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},901: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},902: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},903: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},904: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},905: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},906: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},907: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},908: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},909: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},910: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},911: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},912: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},913: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},914: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},915: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},916: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},917: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},918: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},919: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},920: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},921: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},922: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},923: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},924: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},925: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},926: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},927: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},928: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},929: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},930: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},931: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},932: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},933: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},934: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},935: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},936: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},937: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},938: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},939: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},940: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},941: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},942: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},943: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},944: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},945: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},946: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},947: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},948: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},949: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},950: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},951: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},952: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},953: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},954: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},955: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},956: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},957: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},958: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},959: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},960: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},961: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},962: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},963: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},964: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},965: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},966: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},967: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},968: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},969: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},970: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},971: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},972: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},973: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},974: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},975: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},976: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},977: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},978: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},979: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},980: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},981: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},982: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},983: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},984: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},985: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},986: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},987: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},988: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},989: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},990: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},991: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},992: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},993: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},994: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},995: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},996: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},997: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},998: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},999: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},1000: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0</v>
@@ -7910,7 +7978,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1</v>
@@ -7926,7 +7994,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>2</v>
@@ -7942,7 +8010,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>3</v>
@@ -7958,7 +8026,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>4</v>
@@ -7974,7 +8042,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>5</v>
@@ -7990,7 +8058,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>6</v>
@@ -8006,7 +8074,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>7</v>
@@ -8022,7 +8090,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>2</v>
@@ -8037,7 +8105,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>1</v>
@@ -8052,7 +8120,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>2</v>
@@ -8067,7 +8135,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>3</v>
@@ -8082,7 +8150,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>4</v>
@@ -8097,7 +8165,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>5</v>
@@ -8112,7 +8180,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>6</v>
@@ -8127,7 +8195,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>7</v>
@@ -8142,7 +8210,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>5</v>
@@ -8157,7 +8225,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>6</v>
@@ -8172,7 +8240,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>7</v>
@@ -8187,7 +8255,7 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>0</v>
@@ -8202,7 +8270,7 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="6" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>1</v>
@@ -8217,7 +8285,7 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>2</v>
@@ -8232,7 +8300,7 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>3</v>
@@ -8247,7 +8315,7 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="6" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>4</v>
@@ -8262,7 +8330,7 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="6" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>5</v>
@@ -8277,7 +8345,7 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="6" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>6</v>
@@ -8292,7 +8360,7 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="6" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>7</v>
@@ -8307,7 +8375,7 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="6" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>0</v>
@@ -8322,7 +8390,7 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="6" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>1</v>
@@ -8337,7 +8405,7 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="6" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>2</v>
@@ -8352,7 +8420,7 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="6" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>3</v>
@@ -8367,7 +8435,7 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="6" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>4</v>
@@ -8382,7 +8450,7 @@
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="6" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>5</v>
@@ -8397,7 +8465,7 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="6" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>6</v>
@@ -8412,7 +8480,7 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="6" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>7</v>
@@ -8427,7 +8495,7 @@
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="6" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>0</v>
@@ -8442,7 +8510,7 @@
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="6" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>1</v>
@@ -8457,7 +8525,7 @@
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>2</v>
@@ -8472,7 +8540,7 @@
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>3</v>
@@ -8487,7 +8555,7 @@
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>4</v>
@@ -8502,7 +8570,7 @@
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>5</v>
@@ -8517,7 +8585,7 @@
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>6</v>
@@ -8532,7 +8600,7 @@
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="B44" s="0" t="n">
         <v>7</v>
@@ -8547,7 +8615,7 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="B45" s="0" t="n">
         <v>0</v>
@@ -8562,7 +8630,7 @@
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="B46" s="0" t="n">
         <v>1</v>
@@ -8577,7 +8645,7 @@
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="B47" s="0" t="n">
         <v>2</v>
@@ -8592,7 +8660,7 @@
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="B48" s="0" t="n">
         <v>3</v>
@@ -8607,7 +8675,7 @@
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="B49" s="0" t="n">
         <v>4</v>
@@ -8622,7 +8690,7 @@
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="B50" s="0" t="n">
         <v>5</v>
@@ -8637,7 +8705,7 @@
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="B51" s="0" t="n">
         <v>6</v>
@@ -8652,7 +8720,7 @@
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="B52" s="0" t="n">
         <v>7</v>
@@ -8667,7 +8735,7 @@
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="B53" s="0" t="n">
         <v>0</v>
@@ -8682,7 +8750,7 @@
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="B54" s="0" t="n">
         <v>1</v>
@@ -8697,7 +8765,7 @@
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="B55" s="0" t="n">
         <v>2</v>
@@ -8712,7 +8780,7 @@
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="B56" s="0" t="n">
         <v>3</v>
@@ -8727,7 +8795,7 @@
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="B57" s="0" t="n">
         <v>4</v>
@@ -8742,7 +8810,7 @@
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="B58" s="0" t="n">
         <v>5</v>
@@ -8757,7 +8825,7 @@
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="B59" s="0" t="n">
         <v>6</v>
@@ -8772,7 +8840,7 @@
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="B60" s="0" t="n">
         <v>7</v>
@@ -8787,7 +8855,7 @@
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="B61" s="0" t="n">
         <v>0</v>
@@ -8802,7 +8870,7 @@
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="B62" s="0" t="n">
         <v>1</v>
@@ -8817,7 +8885,7 @@
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="B63" s="0" t="n">
         <v>2</v>
@@ -8832,7 +8900,7 @@
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="B64" s="0" t="n">
         <v>3</v>
@@ -8847,7 +8915,7 @@
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="B65" s="0" t="n">
         <v>4</v>
@@ -8862,7 +8930,7 @@
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="B66" s="0" t="n">
         <v>5</v>
@@ -8877,7 +8945,7 @@
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="B67" s="0" t="n">
         <v>6</v>
@@ -8892,7 +8960,7 @@
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="B68" s="0" t="n">
         <v>7</v>
@@ -8907,7 +8975,7 @@
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="B69" s="0" t="n">
         <v>0</v>
@@ -8922,7 +8990,7 @@
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="B70" s="0" t="n">
         <v>1</v>
@@ -8937,7 +9005,7 @@
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="B71" s="0" t="n">
         <v>2</v>
@@ -8952,7 +9020,7 @@
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="B72" s="0" t="n">
         <v>3</v>
@@ -8967,7 +9035,7 @@
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="B73" s="0" t="n">
         <v>4</v>
@@ -8982,7 +9050,7 @@
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="B74" s="0" t="n">
         <v>5</v>
@@ -8997,7 +9065,7 @@
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="B75" s="0" t="n">
         <v>6</v>
@@ -9012,7 +9080,7 @@
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="B76" s="0" t="n">
         <v>7</v>
@@ -9027,7 +9095,7 @@
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B77" s="0" t="n">
         <v>0</v>
@@ -9042,7 +9110,7 @@
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B78" s="0" t="n">
         <v>1</v>
@@ -9057,7 +9125,7 @@
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B79" s="0" t="n">
         <v>2</v>
@@ -9072,7 +9140,7 @@
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B80" s="0" t="n">
         <v>3</v>
@@ -9087,7 +9155,7 @@
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B81" s="0" t="n">
         <v>4</v>
@@ -9102,7 +9170,7 @@
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B82" s="0" t="n">
         <v>5</v>
@@ -9117,7 +9185,7 @@
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B83" s="0" t="n">
         <v>6</v>
@@ -9132,7 +9200,7 @@
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B84" s="0" t="n">
         <v>7</v>
@@ -9147,7 +9215,7 @@
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="6" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="B85" s="0" t="n">
         <v>0</v>
@@ -9162,7 +9230,7 @@
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="6" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="B86" s="0" t="n">
         <v>1</v>
@@ -9177,7 +9245,7 @@
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="6" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="B87" s="0" t="n">
         <v>2</v>
@@ -9192,7 +9260,7 @@
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="6" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="B88" s="0" t="n">
         <v>3</v>
@@ -9207,7 +9275,7 @@
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="B89" s="0" t="n">
         <v>4</v>
@@ -9222,7 +9290,7 @@
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="B90" s="0" t="n">
         <v>5</v>
@@ -9237,7 +9305,7 @@
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="B91" s="0" t="n">
         <v>6</v>
@@ -9252,7 +9320,7 @@
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="B92" s="0" t="n">
         <v>7</v>
@@ -9267,7 +9335,7 @@
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="B93" s="0" t="n">
         <v>0</v>
@@ -9282,7 +9350,7 @@
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="B94" s="0" t="n">
         <v>1</v>
@@ -9297,7 +9365,7 @@
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="B95" s="0" t="n">
         <v>2</v>
@@ -9312,7 +9380,7 @@
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="B96" s="0" t="n">
         <v>3</v>
@@ -9327,7 +9395,7 @@
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="B97" s="0" t="n">
         <v>4</v>
@@ -9342,7 +9410,7 @@
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="B98" s="0" t="n">
         <v>5</v>
@@ -9357,7 +9425,7 @@
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="B99" s="0" t="n">
         <v>6</v>
@@ -9372,7 +9440,7 @@
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="B100" s="0" t="n">
         <v>7</v>
@@ -9387,7 +9455,7 @@
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="B101" s="0" t="n">
         <v>0</v>
@@ -9402,7 +9470,7 @@
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="B102" s="0" t="n">
         <v>1</v>
@@ -9417,7 +9485,7 @@
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="B103" s="0" t="n">
         <v>2</v>
@@ -9432,7 +9500,7 @@
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="B104" s="0" t="n">
         <v>3</v>
@@ -9447,7 +9515,7 @@
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="B105" s="0" t="n">
         <v>4</v>
@@ -9462,7 +9530,7 @@
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="B106" s="0" t="n">
         <v>5</v>
@@ -9477,7 +9545,7 @@
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="B107" s="0" t="n">
         <v>6</v>
@@ -9492,7 +9560,7 @@
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="B108" s="0" t="n">
         <v>7</v>
@@ -9507,7 +9575,7 @@
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="B109" s="0" t="n">
         <v>0</v>
@@ -9522,7 +9590,7 @@
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="B110" s="0" t="n">
         <v>1</v>
@@ -9537,7 +9605,7 @@
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="B111" s="0" t="n">
         <v>2</v>
@@ -9552,7 +9620,7 @@
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="B112" s="0" t="n">
         <v>3</v>
@@ -9567,7 +9635,7 @@
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="B113" s="0" t="n">
         <v>4</v>
@@ -9582,7 +9650,7 @@
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="B114" s="0" t="n">
         <v>5</v>
@@ -9597,7 +9665,7 @@
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="B115" s="0" t="n">
         <v>6</v>
@@ -9612,7 +9680,7 @@
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="B116" s="0" t="n">
         <v>7</v>
@@ -9627,7 +9695,7 @@
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="B117" s="0" t="n">
         <v>0</v>
@@ -9642,7 +9710,7 @@
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="B118" s="0" t="n">
         <v>1</v>
@@ -9657,7 +9725,7 @@
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="B119" s="0" t="n">
         <v>2</v>
@@ -9672,7 +9740,7 @@
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="B120" s="0" t="n">
         <v>3</v>
@@ -9687,7 +9755,7 @@
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="B121" s="0" t="n">
         <v>4</v>
@@ -9702,7 +9770,7 @@
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="B122" s="0" t="n">
         <v>5</v>
@@ -9717,7 +9785,7 @@
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="B123" s="0" t="n">
         <v>6</v>
@@ -9732,7 +9800,7 @@
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B124" s="0" t="n">
         <v>0</v>
@@ -9747,7 +9815,7 @@
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B125" s="0" t="n">
         <v>1</v>
@@ -9762,7 +9830,7 @@
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B126" s="0" t="n">
         <v>2</v>
@@ -9777,7 +9845,7 @@
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B127" s="0" t="n">
         <v>3</v>
@@ -9792,7 +9860,7 @@
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B128" s="0" t="n">
         <v>4</v>
@@ -9807,7 +9875,7 @@
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B129" s="0" t="n">
         <v>5</v>
@@ -9822,7 +9890,7 @@
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B130" s="0" t="n">
         <v>6</v>
@@ -9837,7 +9905,7 @@
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B131" s="0" t="n">
         <v>7</v>
@@ -9852,7 +9920,7 @@
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="B132" s="0" t="n">
         <v>0</v>
@@ -9867,7 +9935,7 @@
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="B133" s="0" t="n">
         <v>1</v>
@@ -9882,7 +9950,7 @@
     </row>
     <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="B134" s="0" t="n">
         <v>2</v>
@@ -9897,7 +9965,7 @@
     </row>
     <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="B135" s="0" t="n">
         <v>3</v>
@@ -9912,7 +9980,7 @@
     </row>
     <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="B136" s="0" t="n">
         <v>4</v>
@@ -9927,7 +9995,7 @@
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="B137" s="0" t="n">
         <v>5</v>
@@ -9942,7 +10010,7 @@
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="6" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="B138" s="0" t="n">
         <v>3</v>
@@ -9957,7 +10025,7 @@
     </row>
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="B139" s="0" t="n">
         <v>4</v>
@@ -9972,7 +10040,7 @@
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="B140" s="0" t="n">
         <v>5</v>
@@ -9987,7 +10055,7 @@
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="B141" s="0" t="n">
         <v>6</v>
@@ -10002,7 +10070,7 @@
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="B142" s="0" t="n">
         <v>7</v>
@@ -10017,7 +10085,7 @@
     </row>
     <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="B143" s="0" t="n">
         <v>7</v>
@@ -10032,7 +10100,7 @@
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="B144" s="0" t="n">
         <v>3</v>
@@ -10047,7 +10115,7 @@
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="B145" s="0" t="n">
         <v>4</v>
@@ -10062,7 +10130,7 @@
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="B146" s="0" t="n">
         <v>5</v>
@@ -10077,7 +10145,7 @@
     </row>
     <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="B147" s="0" t="n">
         <v>5</v>
@@ -10092,7 +10160,7 @@
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="B148" s="0" t="n">
         <v>6</v>
@@ -10107,7 +10175,7 @@
     </row>
     <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="B149" s="0" t="n">
         <v>7</v>
@@ -10122,7 +10190,7 @@
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="B150" s="0" t="n">
         <v>0</v>
@@ -10137,7 +10205,7 @@
     </row>
     <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="B151" s="0" t="n">
         <v>1</v>
@@ -10152,7 +10220,7 @@
     </row>
     <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="B152" s="0" t="n">
         <v>2</v>
@@ -10167,7 +10235,7 @@
     </row>
     <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="B153" s="0" t="n">
         <v>3</v>
@@ -10182,7 +10250,7 @@
     </row>
     <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="B154" s="0" t="n">
         <v>4</v>
@@ -10197,7 +10265,7 @@
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="B155" s="0" t="n">
         <v>5</v>
@@ -10212,7 +10280,7 @@
     </row>
     <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="B156" s="0" t="n">
         <v>6</v>
@@ -10227,7 +10295,7 @@
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="B157" s="0" t="n">
         <v>7</v>
@@ -10242,7 +10310,7 @@
     </row>
     <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="B158" s="0" t="n">
         <v>0</v>
@@ -10257,7 +10325,7 @@
     </row>
     <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="B159" s="0" t="n">
         <v>1</v>
@@ -10272,7 +10340,7 @@
     </row>
     <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="B160" s="0" t="n">
         <v>6</v>
@@ -10287,7 +10355,7 @@
     </row>
     <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="B161" s="0" t="n">
         <v>7</v>
@@ -10302,7 +10370,7 @@
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="B162" s="0" t="n">
         <v>0</v>
@@ -10317,7 +10385,7 @@
     </row>
     <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="B163" s="0" t="n">
         <v>1</v>
@@ -10332,7 +10400,7 @@
     </row>
     <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="B164" s="0" t="n">
         <v>2</v>
@@ -10347,7 +10415,7 @@
     </row>
     <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="B165" s="0" t="n">
         <v>6</v>
@@ -10362,7 +10430,7 @@
     </row>
     <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="B166" s="0" t="n">
         <v>7</v>
@@ -10377,7 +10445,7 @@
     </row>
     <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="B167" s="0" t="n">
         <v>0</v>
@@ -10392,7 +10460,7 @@
     </row>
     <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="B168" s="0" t="n">
         <v>1</v>
@@ -10407,7 +10475,7 @@
     </row>
     <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="B169" s="0" t="n">
         <v>2</v>
@@ -10422,7 +10490,7 @@
     </row>
     <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="B170" s="0" t="n">
         <v>3</v>
@@ -10437,7 +10505,7 @@
     </row>
     <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="B171" s="0" t="n">
         <v>4</v>
@@ -10452,7 +10520,7 @@
     </row>
     <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="B172" s="0" t="n">
         <v>2</v>
@@ -10467,7 +10535,7 @@
     </row>
     <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="B173" s="0" t="n">
         <v>3</v>
@@ -10482,7 +10550,7 @@
     </row>
     <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="B174" s="0" t="n">
         <v>4</v>
@@ -10497,7 +10565,7 @@
     </row>
     <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="B175" s="0" t="n">
         <v>5</v>
@@ -10512,7 +10580,7 @@
     </row>
     <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="B176" s="0" t="n">
         <v>6</v>
@@ -10527,7 +10595,7 @@
     </row>
     <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="B177" s="0" t="n">
         <v>7</v>
@@ -10542,7 +10610,7 @@
     </row>
     <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="B178" s="0" t="n">
         <v>0</v>
@@ -10557,7 +10625,7 @@
     </row>
     <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="B179" s="0" t="n">
         <v>1</v>
@@ -10572,7 +10640,7 @@
     </row>
     <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="B180" s="0" t="n">
         <v>2</v>
@@ -10587,7 +10655,7 @@
     </row>
     <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="B181" s="0" t="n">
         <v>3</v>
@@ -10602,7 +10670,7 @@
     </row>
     <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="B182" s="0" t="n">
         <v>4</v>
@@ -10617,7 +10685,7 @@
     </row>
     <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="0" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="B183" s="0" t="n">
         <v>5</v>
@@ -10632,7 +10700,7 @@
     </row>
     <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="0" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="B184" s="0" t="n">
         <v>6</v>
@@ -10647,7 +10715,7 @@
     </row>
     <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="B185" s="0" t="n">
         <v>7</v>
@@ -10662,7 +10730,7 @@
     </row>
     <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="B186" s="0" t="n">
         <v>0</v>
@@ -10677,7 +10745,7 @@
     </row>
     <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="0" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="B187" s="0" t="n">
         <v>1</v>
@@ -10692,7 +10760,7 @@
     </row>
     <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="0" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="B188" s="0" t="n">
         <v>2</v>
@@ -10707,7 +10775,7 @@
     </row>
     <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="0" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="B189" s="0" t="n">
         <v>3</v>
@@ -10722,7 +10790,7 @@
     </row>
     <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="0" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="B190" s="0" t="n">
         <v>4</v>
@@ -10737,7 +10805,7 @@
     </row>
     <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="0" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="B191" s="0" t="n">
         <v>5</v>
@@ -10752,7 +10820,7 @@
     </row>
     <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="0" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="B192" s="0" t="n">
         <v>6</v>
@@ -10767,7 +10835,7 @@
     </row>
     <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="0" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="B193" s="0" t="n">
         <v>7</v>
@@ -10782,7 +10850,7 @@
     </row>
     <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="0" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="B194" s="0" t="n">
         <v>0</v>
@@ -10797,7 +10865,7 @@
     </row>
     <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="0" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="B195" s="0" t="n">
         <v>1</v>
@@ -10812,7 +10880,7 @@
     </row>
     <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="0" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="B196" s="0" t="n">
         <v>2</v>
@@ -10827,7 +10895,7 @@
     </row>
     <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="0" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="B197" s="0" t="n">
         <v>3</v>
@@ -10842,7 +10910,7 @@
     </row>
     <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="0" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="B198" s="0" t="n">
         <v>4</v>
@@ -10857,7 +10925,7 @@
     </row>
     <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="0" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="B199" s="0" t="n">
         <v>2</v>
@@ -10872,7 +10940,7 @@
     </row>
     <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="B200" s="0" t="n">
         <v>3</v>
@@ -10887,7 +10955,7 @@
     </row>
     <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="0" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="B201" s="0" t="n">
         <v>4</v>
@@ -10902,7 +10970,7 @@
     </row>
     <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="0" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="B202" s="0" t="n">
         <v>5</v>
@@ -10917,7 +10985,7 @@
     </row>
     <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="0" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="B203" s="0" t="n">
         <v>6</v>
@@ -10932,7 +11000,7 @@
     </row>
     <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="0" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B204" s="0" t="n">
         <v>1</v>
@@ -10947,7 +11015,7 @@
     </row>
     <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="0" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="B205" s="0" t="n">
         <v>5</v>
@@ -10962,7 +11030,7 @@
     </row>
     <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="0" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="B206" s="0" t="n">
         <v>6</v>
@@ -10977,7 +11045,7 @@
     </row>
     <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="0" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="B207" s="0" t="n">
         <v>7</v>
@@ -10992,7 +11060,7 @@
     </row>
     <row r="208" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="0" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B208" s="0" t="n">
         <v>0</v>
@@ -11007,7 +11075,7 @@
     </row>
     <row r="209" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="0" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B209" s="0" t="n">
         <v>3</v>
@@ -11022,7 +11090,7 @@
     </row>
     <row r="210" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="0" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B210" s="0" t="n">
         <v>5</v>
@@ -11037,7 +11105,7 @@
     </row>
     <row r="211" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="0" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B211" s="0" t="n">
         <v>6</v>
@@ -11052,7 +11120,7 @@
     </row>
     <row r="212" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="0" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B212" s="0" t="n">
         <v>7</v>
@@ -11067,7 +11135,7 @@
     </row>
     <row r="213" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="0" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="B213" s="0" t="n">
         <v>0</v>
@@ -11082,7 +11150,7 @@
     </row>
     <row r="214" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="0" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="B214" s="0" t="n">
         <v>1</v>
@@ -11097,7 +11165,7 @@
     </row>
     <row r="215" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="0" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="B215" s="0" t="n">
         <v>2</v>
@@ -11112,7 +11180,7 @@
     </row>
     <row r="216" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="0" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B216" s="0" t="n">
         <v>4</v>
@@ -11127,7 +11195,7 @@
     </row>
     <row r="217" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="0" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B217" s="0" t="n">
         <v>6</v>
@@ -11142,7 +11210,7 @@
     </row>
     <row r="218" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="0" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B218" s="0" t="n">
         <v>7</v>
@@ -11157,7 +11225,7 @@
     </row>
     <row r="219" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="0" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="B219" s="0" t="n">
         <v>0</v>
@@ -11172,7 +11240,7 @@
     </row>
     <row r="220" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="0" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="B220" s="0" t="n">
         <v>1</v>
@@ -11187,7 +11255,7 @@
     </row>
     <row r="221" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="0" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="B221" s="0" t="n">
         <v>2</v>
@@ -11202,7 +11270,7 @@
     </row>
     <row r="222" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="0" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="B222" s="0" t="n">
         <v>3</v>
@@ -11217,7 +11285,7 @@
     </row>
     <row r="223" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="0" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="B223" s="0" t="n">
         <v>4</v>
@@ -11232,7 +11300,7 @@
     </row>
     <row r="224" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="0" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="B224" s="0" t="n">
         <v>5</v>
@@ -11247,7 +11315,7 @@
     </row>
     <row r="225" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="0" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="B225" s="0" t="n">
         <v>6</v>
@@ -11262,7 +11330,7 @@
     </row>
     <row r="226" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="0" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="B226" s="0" t="n">
         <v>7</v>
@@ -11277,7 +11345,7 @@
     </row>
     <row r="227" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="0" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="B227" s="0" t="n">
         <v>0</v>
@@ -11292,7 +11360,7 @@
     </row>
     <row r="228" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="0" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="B228" s="0" t="n">
         <v>1</v>
@@ -11307,7 +11375,7 @@
     </row>
     <row r="229" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="0" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="B229" s="0" t="n">
         <v>2</v>
@@ -11322,7 +11390,7 @@
     </row>
     <row r="230" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="0" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="B230" s="0" t="n">
         <v>3</v>
@@ -11337,7 +11405,7 @@
     </row>
     <row r="231" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="0" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="B231" s="0" t="n">
         <v>4</v>
@@ -11352,7 +11420,7 @@
     </row>
     <row r="232" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="0" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="B232" s="0" t="n">
         <v>5</v>
@@ -11367,7 +11435,7 @@
     </row>
     <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="0" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="B233" s="0" t="n">
         <v>6</v>
@@ -11382,7 +11450,7 @@
     </row>
     <row r="234" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="0" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="B234" s="0" t="n">
         <v>7</v>
@@ -11397,7 +11465,7 @@
     </row>
     <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="0" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="B235" s="0" t="n">
         <v>0</v>
@@ -11412,7 +11480,7 @@
     </row>
     <row r="236" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="0" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="B236" s="0" t="n">
         <v>1</v>
@@ -11427,7 +11495,7 @@
     </row>
     <row r="237" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="0" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="B237" s="0" t="n">
         <v>2</v>
@@ -11442,7 +11510,7 @@
     </row>
     <row r="238" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="0" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="B238" s="0" t="n">
         <v>3</v>
@@ -11457,7 +11525,7 @@
     </row>
     <row r="239" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="0" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="B239" s="0" t="n">
         <v>4</v>
@@ -11472,7 +11540,7 @@
     </row>
     <row r="240" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="0" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="B240" s="0" t="n">
         <v>5</v>
@@ -11487,7 +11555,7 @@
     </row>
     <row r="241" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="0" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="B241" s="0" t="n">
         <v>6</v>
@@ -11502,7 +11570,7 @@
     </row>
     <row r="242" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="0" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="B242" s="0" t="n">
         <v>7</v>
@@ -11517,7 +11585,7 @@
     </row>
     <row r="243" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="0" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="B243" s="0" t="n">
         <v>0</v>
@@ -11532,7 +11600,7 @@
     </row>
     <row r="244" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="0" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="B244" s="0" t="n">
         <v>1</v>
@@ -11547,7 +11615,7 @@
     </row>
     <row r="245" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="0" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="B245" s="0" t="n">
         <v>2</v>
@@ -11562,7 +11630,7 @@
     </row>
     <row r="246" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="0" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="B246" s="0" t="n">
         <v>3</v>
@@ -11577,7 +11645,7 @@
     </row>
     <row r="247" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="0" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="B247" s="0" t="n">
         <v>4</v>
@@ -11592,7 +11660,7 @@
     </row>
     <row r="248" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="0" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="B248" s="0" t="n">
         <v>5</v>
@@ -11607,7 +11675,7 @@
     </row>
     <row r="249" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="0" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="B249" s="0" t="n">
         <v>6</v>
@@ -11622,7 +11690,7 @@
     </row>
     <row r="250" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="0" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="B250" s="0" t="n">
         <v>7</v>
@@ -11637,7 +11705,7 @@
     </row>
     <row r="251" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="0" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="B251" s="0" t="n">
         <v>0</v>
@@ -11652,7 +11720,7 @@
     </row>
     <row r="252" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="0" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="B252" s="0" t="n">
         <v>1</v>
@@ -11667,7 +11735,7 @@
     </row>
     <row r="253" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="0" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="B253" s="0" t="n">
         <v>2</v>
@@ -11682,7 +11750,7 @@
     </row>
     <row r="254" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="0" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="B254" s="0" t="n">
         <v>3</v>
@@ -11697,7 +11765,7 @@
     </row>
     <row r="255" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="0" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="B255" s="0" t="n">
         <v>4</v>
@@ -11712,7 +11780,7 @@
     </row>
     <row r="256" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="0" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="B256" s="0" t="n">
         <v>5</v>
@@ -11727,7 +11795,7 @@
     </row>
     <row r="257" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="0" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="B257" s="0" t="n">
         <v>6</v>
@@ -11742,7 +11810,7 @@
     </row>
     <row r="258" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="0" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="B258" s="0" t="n">
         <v>7</v>
@@ -11757,7 +11825,7 @@
     </row>
     <row r="259" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="0" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="B259" s="0" t="n">
         <v>0</v>
@@ -11772,7 +11840,7 @@
     </row>
     <row r="260" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="0" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="B260" s="0" t="n">
         <v>1</v>
@@ -11787,7 +11855,7 @@
     </row>
     <row r="261" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="0" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="B261" s="0" t="n">
         <v>2</v>
@@ -11802,7 +11870,7 @@
     </row>
     <row r="262" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="0" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="B262" s="0" t="n">
         <v>3</v>
@@ -11817,7 +11885,7 @@
     </row>
     <row r="263" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="0" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="B263" s="0" t="n">
         <v>4</v>
@@ -11832,7 +11900,7 @@
     </row>
     <row r="264" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="0" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="B264" s="0" t="n">
         <v>5</v>
@@ -11847,7 +11915,7 @@
     </row>
     <row r="265" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="0" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="B265" s="0" t="n">
         <v>6</v>
@@ -11862,7 +11930,7 @@
     </row>
     <row r="266" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="0" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="B266" s="0" t="n">
         <v>7</v>
@@ -11877,7 +11945,7 @@
     </row>
     <row r="267" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="0" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B267" s="0" t="n">
         <v>2</v>
@@ -11892,7 +11960,7 @@
     </row>
     <row r="268" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="0" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="B268" s="0" t="n">
         <v>2</v>
@@ -11907,7 +11975,7 @@
     </row>
     <row r="269" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="0" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="B269" s="0" t="n">
         <v>3</v>
@@ -11922,7 +11990,7 @@
     </row>
     <row r="270" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="0" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="B270" s="0" t="n">
         <v>4</v>
@@ -11937,7 +12005,7 @@
     </row>
     <row r="271" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="0" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="B271" s="0" t="n">
         <v>0</v>
@@ -11952,7 +12020,7 @@
     </row>
     <row r="272" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="0" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="B272" s="0" t="n">
         <v>1</v>
@@ -11967,7 +12035,7 @@
     </row>
     <row r="273" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="0" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="B273" s="0" t="n">
         <v>2</v>
@@ -11982,7 +12050,7 @@
     </row>
     <row r="274" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A274" s="0" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="B274" s="0" t="n">
         <v>3</v>
@@ -11997,7 +12065,7 @@
     </row>
     <row r="275" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="0" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="B275" s="0" t="n">
         <v>6</v>
@@ -12012,7 +12080,7 @@
     </row>
     <row r="276" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="0" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="B276" s="0" t="n">
         <v>7</v>
@@ -12027,7 +12095,7 @@
     </row>
     <row r="277" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="0" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="B277" s="0" t="n">
         <v>0</v>
@@ -12042,7 +12110,7 @@
     </row>
     <row r="278" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="0" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="B278" s="0" t="n">
         <v>1</v>
@@ -12057,7 +12125,7 @@
     </row>
     <row r="279" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A279" s="0" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="B279" s="0" t="n">
         <v>5</v>
@@ -12072,7 +12140,7 @@
     </row>
     <row r="280" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="0" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="B280" s="0" t="n">
         <v>6</v>
@@ -12087,7 +12155,7 @@
     </row>
     <row r="281" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A281" s="0" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="B281" s="0" t="n">
         <v>7</v>
@@ -12102,7 +12170,7 @@
     </row>
     <row r="282" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="0" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="B282" s="0" t="n">
         <v>0</v>
@@ -12117,7 +12185,7 @@
     </row>
     <row r="283" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A283" s="0" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="B283" s="0" t="n">
         <v>1</v>
@@ -12132,7 +12200,7 @@
     </row>
     <row r="284" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="0" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="B284" s="0" t="n">
         <v>7</v>
@@ -12147,7 +12215,7 @@
     </row>
     <row r="285" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="0" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="B285" s="0" t="n">
         <v>0</v>
@@ -12162,7 +12230,7 @@
     </row>
     <row r="286" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="0" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="B286" s="0" t="n">
         <v>1</v>
@@ -12177,7 +12245,7 @@
     </row>
     <row r="287" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="0" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="B287" s="0" t="n">
         <v>3</v>
@@ -12192,7 +12260,7 @@
     </row>
     <row r="288" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A288" s="0" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="B288" s="0" t="n">
         <v>4</v>
@@ -12207,7 +12275,7 @@
     </row>
     <row r="289" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="0" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="B289" s="0" t="n">
         <v>5</v>
@@ -12222,7 +12290,7 @@
     </row>
     <row r="290" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="0" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="B290" s="0" t="n">
         <v>6</v>
@@ -12237,7 +12305,7 @@
     </row>
     <row r="291" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A291" s="0" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="B291" s="0" t="n">
         <v>7</v>
@@ -12252,7 +12320,7 @@
     </row>
     <row r="292" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="0" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="B292" s="0" t="n">
         <v>4</v>
@@ -12267,7 +12335,7 @@
     </row>
     <row r="293" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A293" s="0" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="B293" s="0" t="n">
         <v>5</v>
@@ -12281,219 +12349,363 @@
       </c>
     </row>
     <row r="294" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A294" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="B294" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="C294" s="4" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="D294" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C294, Levels!B:B, 0), 1, 1)),", ",IF(A294 &lt;&gt; "", """mem"": bit" &amp; B294 &amp; "(" &amp; A294 &amp; "),", ""),"""good"": ",IF(A294 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A294 &lt;&gt; "", A294, -1),", ""bit"": ",IF(B294 &lt;&gt; "", B294, -1),"},")</f>
-        <v>293: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>293: { "levelId": 12, "mem": bit2(0x2249a7),"good": 1, "addr": 0x2249a7, "bit": 2},</v>
       </c>
     </row>
     <row r="295" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A295" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="B295" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="C295" s="4" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="D295" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C295, Levels!B:B, 0), 1, 1)),", ",IF(A295 &lt;&gt; "", """mem"": bit" &amp; B295 &amp; "(" &amp; A295 &amp; "),", ""),"""good"": ",IF(A295 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A295 &lt;&gt; "", A295, -1),", ""bit"": ",IF(B295 &lt;&gt; "", B295, -1),"},")</f>
-        <v>294: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>294: { "levelId": 12, "mem": bit3(0x2249a7),"good": 1, "addr": 0x2249a7, "bit": 3},</v>
       </c>
     </row>
     <row r="296" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A296" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="B296" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="C296" s="4" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="D296" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C296, Levels!B:B, 0), 1, 1)),", ",IF(A296 &lt;&gt; "", """mem"": bit" &amp; B296 &amp; "(" &amp; A296 &amp; "),", ""),"""good"": ",IF(A296 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A296 &lt;&gt; "", A296, -1),", ""bit"": ",IF(B296 &lt;&gt; "", B296, -1),"},")</f>
-        <v>295: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>295: { "levelId": 12, "mem": bit4(0x2249a7),"good": 1, "addr": 0x2249a7, "bit": 4},</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A297" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="B297" s="0" t="n">
+        <v>5</v>
+      </c>
       <c r="C297" s="4" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="D297" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C297, Levels!B:B, 0), 1, 1)),", ",IF(A297 &lt;&gt; "", """mem"": bit" &amp; B297 &amp; "(" &amp; A297 &amp; "),", ""),"""good"": ",IF(A297 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A297 &lt;&gt; "", A297, -1),", ""bit"": ",IF(B297 &lt;&gt; "", B297, -1),"},")</f>
-        <v>296: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>296: { "levelId": 12, "mem": bit5(0x2249a7),"good": 1, "addr": 0x2249a7, "bit": 5},</v>
       </c>
     </row>
     <row r="298" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A298" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="B298" s="0" t="n">
+        <v>6</v>
+      </c>
       <c r="C298" s="4" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="D298" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C298, Levels!B:B, 0), 1, 1)),", ",IF(A298 &lt;&gt; "", """mem"": bit" &amp; B298 &amp; "(" &amp; A298 &amp; "),", ""),"""good"": ",IF(A298 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A298 &lt;&gt; "", A298, -1),", ""bit"": ",IF(B298 &lt;&gt; "", B298, -1),"},")</f>
-        <v>297: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>297: { "levelId": 12, "mem": bit6(0x2249a7),"good": 1, "addr": 0x2249a7, "bit": 6},</v>
       </c>
     </row>
     <row r="299" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A299" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="B299" s="0" t="n">
+        <v>7</v>
+      </c>
       <c r="C299" s="4" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="D299" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C299, Levels!B:B, 0), 1, 1)),", ",IF(A299 &lt;&gt; "", """mem"": bit" &amp; B299 &amp; "(" &amp; A299 &amp; "),", ""),"""good"": ",IF(A299 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A299 &lt;&gt; "", A299, -1),", ""bit"": ",IF(B299 &lt;&gt; "", B299, -1),"},")</f>
-        <v>298: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>298: { "levelId": 12, "mem": bit7(0x2249a7),"good": 1, "addr": 0x2249a7, "bit": 7},</v>
       </c>
     </row>
     <row r="300" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A300" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="B300" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="C300" s="4" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="D300" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C300, Levels!B:B, 0), 1, 1)),", ",IF(A300 &lt;&gt; "", """mem"": bit" &amp; B300 &amp; "(" &amp; A300 &amp; "),", ""),"""good"": ",IF(A300 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A300 &lt;&gt; "", A300, -1),", ""bit"": ",IF(B300 &lt;&gt; "", B300, -1),"},")</f>
-        <v>299: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>299: { "levelId": 12, "mem": bit0(0x2249a8),"good": 1, "addr": 0x2249a8, "bit": 0},</v>
       </c>
     </row>
     <row r="301" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A301" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="B301" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="C301" s="4" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="D301" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C301, Levels!B:B, 0), 1, 1)),", ",IF(A301 &lt;&gt; "", """mem"": bit" &amp; B301 &amp; "(" &amp; A301 &amp; "),", ""),"""good"": ",IF(A301 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A301 &lt;&gt; "", A301, -1),", ""bit"": ",IF(B301 &lt;&gt; "", B301, -1),"},")</f>
-        <v>300: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>300: { "levelId": 12, "mem": bit1(0x2249a8),"good": 1, "addr": 0x2249a8, "bit": 1},</v>
       </c>
     </row>
     <row r="302" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A302" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="B302" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="C302" s="4" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="D302" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C302, Levels!B:B, 0), 1, 1)),", ",IF(A302 &lt;&gt; "", """mem"": bit" &amp; B302 &amp; "(" &amp; A302 &amp; "),", ""),"""good"": ",IF(A302 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A302 &lt;&gt; "", A302, -1),", ""bit"": ",IF(B302 &lt;&gt; "", B302, -1),"},")</f>
-        <v>301: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>301: { "levelId": 12, "mem": bit2(0x2249a8),"good": 1, "addr": 0x2249a8, "bit": 2},</v>
       </c>
     </row>
     <row r="303" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A303" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="B303" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="C303" s="4" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="D303" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C303, Levels!B:B, 0), 1, 1)),", ",IF(A303 &lt;&gt; "", """mem"": bit" &amp; B303 &amp; "(" &amp; A303 &amp; "),", ""),"""good"": ",IF(A303 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A303 &lt;&gt; "", A303, -1),", ""bit"": ",IF(B303 &lt;&gt; "", B303, -1),"},")</f>
-        <v>302: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>302: { "levelId": 12, "mem": bit3(0x2249a8),"good": 1, "addr": 0x2249a8, "bit": 3},</v>
       </c>
     </row>
     <row r="304" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A304" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="B304" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="C304" s="4" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="D304" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C304, Levels!B:B, 0), 1, 1)),", ",IF(A304 &lt;&gt; "", """mem"": bit" &amp; B304 &amp; "(" &amp; A304 &amp; "),", ""),"""good"": ",IF(A304 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A304 &lt;&gt; "", A304, -1),", ""bit"": ",IF(B304 &lt;&gt; "", B304, -1),"},")</f>
-        <v>303: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>303: { "levelId": 12, "mem": bit4(0x2249a8),"good": 1, "addr": 0x2249a8, "bit": 4},</v>
       </c>
     </row>
     <row r="305" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A305" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="B305" s="0" t="n">
+        <v>5</v>
+      </c>
       <c r="C305" s="4" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="D305" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C305, Levels!B:B, 0), 1, 1)),", ",IF(A305 &lt;&gt; "", """mem"": bit" &amp; B305 &amp; "(" &amp; A305 &amp; "),", ""),"""good"": ",IF(A305 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A305 &lt;&gt; "", A305, -1),", ""bit"": ",IF(B305 &lt;&gt; "", B305, -1),"},")</f>
-        <v>304: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>304: { "levelId": 12, "mem": bit5(0x2249a8),"good": 1, "addr": 0x2249a8, "bit": 5},</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A306" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="B306" s="0" t="n">
+        <v>6</v>
+      </c>
       <c r="C306" s="4" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="D306" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C306, Levels!B:B, 0), 1, 1)),", ",IF(A306 &lt;&gt; "", """mem"": bit" &amp; B306 &amp; "(" &amp; A306 &amp; "),", ""),"""good"": ",IF(A306 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A306 &lt;&gt; "", A306, -1),", ""bit"": ",IF(B306 &lt;&gt; "", B306, -1),"},")</f>
-        <v>305: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>305: { "levelId": 12, "mem": bit6(0x2249a8),"good": 1, "addr": 0x2249a8, "bit": 6},</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A307" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="B307" s="0" t="n">
+        <v>7</v>
+      </c>
       <c r="C307" s="4" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="D307" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C307, Levels!B:B, 0), 1, 1)),", ",IF(A307 &lt;&gt; "", """mem"": bit" &amp; B307 &amp; "(" &amp; A307 &amp; "),", ""),"""good"": ",IF(A307 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A307 &lt;&gt; "", A307, -1),", ""bit"": ",IF(B307 &lt;&gt; "", B307, -1),"},")</f>
-        <v>306: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>306: { "levelId": 12, "mem": bit7(0x2249a8),"good": 1, "addr": 0x2249a8, "bit": 7},</v>
       </c>
     </row>
     <row r="308" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A308" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="B308" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="C308" s="4" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="D308" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C308, Levels!B:B, 0), 1, 1)),", ",IF(A308 &lt;&gt; "", """mem"": bit" &amp; B308 &amp; "(" &amp; A308 &amp; "),", ""),"""good"": ",IF(A308 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A308 &lt;&gt; "", A308, -1),", ""bit"": ",IF(B308 &lt;&gt; "", B308, -1),"},")</f>
-        <v>307: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>307: { "levelId": 12, "mem": bit0(0x2249a9),"good": 1, "addr": 0x2249a9, "bit": 0},</v>
       </c>
     </row>
     <row r="309" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A309" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="B309" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="C309" s="4" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="D309" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C309, Levels!B:B, 0), 1, 1)),", ",IF(A309 &lt;&gt; "", """mem"": bit" &amp; B309 &amp; "(" &amp; A309 &amp; "),", ""),"""good"": ",IF(A309 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A309 &lt;&gt; "", A309, -1),", ""bit"": ",IF(B309 &lt;&gt; "", B309, -1),"},")</f>
-        <v>308: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>308: { "levelId": 12, "mem": bit1(0x2249a9),"good": 1, "addr": 0x2249a9, "bit": 1},</v>
       </c>
     </row>
     <row r="310" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A310" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="B310" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="C310" s="4" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="D310" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C310, Levels!B:B, 0), 1, 1)),", ",IF(A310 &lt;&gt; "", """mem"": bit" &amp; B310 &amp; "(" &amp; A310 &amp; "),", ""),"""good"": ",IF(A310 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A310 &lt;&gt; "", A310, -1),", ""bit"": ",IF(B310 &lt;&gt; "", B310, -1),"},")</f>
-        <v>309: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>309: { "levelId": 12, "mem": bit2(0x2249a9),"good": 1, "addr": 0x2249a9, "bit": 2},</v>
       </c>
     </row>
     <row r="311" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A311" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="B311" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="C311" s="4" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="D311" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C311, Levels!B:B, 0), 1, 1)),", ",IF(A311 &lt;&gt; "", """mem"": bit" &amp; B311 &amp; "(" &amp; A311 &amp; "),", ""),"""good"": ",IF(A311 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A311 &lt;&gt; "", A311, -1),", ""bit"": ",IF(B311 &lt;&gt; "", B311, -1),"},")</f>
-        <v>310: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>310: { "levelId": 12, "mem": bit3(0x2249a9),"good": 1, "addr": 0x2249a9, "bit": 3},</v>
       </c>
     </row>
     <row r="312" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A312" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="B312" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="C312" s="4" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="D312" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C312, Levels!B:B, 0), 1, 1)),", ",IF(A312 &lt;&gt; "", """mem"": bit" &amp; B312 &amp; "(" &amp; A312 &amp; "),", ""),"""good"": ",IF(A312 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A312 &lt;&gt; "", A312, -1),", ""bit"": ",IF(B312 &lt;&gt; "", B312, -1),"},")</f>
-        <v>311: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>311: { "levelId": 12, "mem": bit4(0x2249a9),"good": 1, "addr": 0x2249a9, "bit": 4},</v>
       </c>
     </row>
     <row r="313" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A313" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="B313" s="0" t="n">
+        <v>5</v>
+      </c>
       <c r="C313" s="4" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="D313" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C313, Levels!B:B, 0), 1, 1)),", ",IF(A313 &lt;&gt; "", """mem"": bit" &amp; B313 &amp; "(" &amp; A313 &amp; "),", ""),"""good"": ",IF(A313 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A313 &lt;&gt; "", A313, -1),", ""bit"": ",IF(B313 &lt;&gt; "", B313, -1),"},")</f>
-        <v>312: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>312: { "levelId": 12, "mem": bit5(0x2249a9),"good": 1, "addr": 0x2249a9, "bit": 5},</v>
       </c>
     </row>
     <row r="314" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A314" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="B314" s="0" t="n">
+        <v>6</v>
+      </c>
       <c r="C314" s="4" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="D314" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C314, Levels!B:B, 0), 1, 1)),", ",IF(A314 &lt;&gt; "", """mem"": bit" &amp; B314 &amp; "(" &amp; A314 &amp; "),", ""),"""good"": ",IF(A314 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A314 &lt;&gt; "", A314, -1),", ""bit"": ",IF(B314 &lt;&gt; "", B314, -1),"},")</f>
-        <v>313: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>313: { "levelId": 12, "mem": bit6(0x2249a9),"good": 1, "addr": 0x2249a9, "bit": 6},</v>
       </c>
     </row>
     <row r="315" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A315" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="B315" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="C315" s="4" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="D315" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C315, Levels!B:B, 0), 1, 1)),", ",IF(A315 &lt;&gt; "", """mem"": bit" &amp; B315 &amp; "(" &amp; A315 &amp; "),", ""),"""good"": ",IF(A315 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A315 &lt;&gt; "", A315, -1),", ""bit"": ",IF(B315 &lt;&gt; "", B315, -1),"},")</f>
-        <v>314: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>314: { "levelId": 12, "mem": bit1(0x2249aa),"good": 1, "addr": 0x2249aa, "bit": 1},</v>
       </c>
     </row>
     <row r="316" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A316" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="B316" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="C316" s="4" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="D316" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C316, Levels!B:B, 0), 1, 1)),", ",IF(A316 &lt;&gt; "", """mem"": bit" &amp; B316 &amp; "(" &amp; A316 &amp; "),", ""),"""good"": ",IF(A316 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A316 &lt;&gt; "", A316, -1),", ""bit"": ",IF(B316 &lt;&gt; "", B316, -1),"},")</f>
-        <v>315: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>315: { "levelId": 12, "mem": bit2(0x2249aa),"good": 1, "addr": 0x2249aa, "bit": 2},</v>
       </c>
     </row>
     <row r="317" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A317" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="B317" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="C317" s="4" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="D317" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C317, Levels!B:B, 0), 1, 1)),", ",IF(A317 &lt;&gt; "", """mem"": bit" &amp; B317 &amp; "(" &amp; A317 &amp; "),", ""),"""good"": ",IF(A317 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A317 &lt;&gt; "", A317, -1),", ""bit"": ",IF(B317 &lt;&gt; "", B317, -1),"},")</f>
-        <v>316: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>316: { "levelId": 12, "mem": bit2(0x2249ab),"good": 1, "addr": 0x2249ab, "bit": 2},</v>
       </c>
     </row>
     <row r="318" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18676,13 +18888,13 @@
   </sheetPr>
   <dimension ref="A1:H1081"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="B2" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="B11" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
+      <selection pane="bottomLeft" activeCell="C31" activeCellId="0" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.93"/>
@@ -18692,13 +18904,13 @@
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>4</v>
@@ -18708,12 +18920,12 @@
       </c>
       <c r="H1" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D2:D81)</f>
-        <v>1: { "levelId": 1, "mem": bit7(0x2249f0),"good": 1},2: { "levelId": 2, "mem": bit0(0x2249f1),"good": 1},3: { "levelId": 2, "mem": bit1(0x2249f1),"good": 1},4: { "levelId": 2, "mem": bit5(0x2249f1),"good": 1},5: { "levelId": 2, "mem": bit6(0x2249f1),"good": 1},6: { "levelId": 1, "mem": bit7(0x2249f1),"good": 1},7: { "levelId": 5, "mem": bit0(0x2249f2),"good": 1},8: { "levelId": 5, "mem": bit1(0x2249f2),"good": 1},9: { "levelId": 5, "mem": bit2(0x2249f2),"good": 1},10: { "levelId": 5, "mem": bit3(0x2249f2),"good": 1},11: { "levelId": 5, "mem": bit4(0x2249f2),"good": 1},12: { "levelId": 6, "mem": bit5(0x2249f2),"good": 1},13: { "levelId": 6, "mem": bit7(0x2249f2),"good": 1},14: { "levelId": 6, "mem": bit1(0x2249f3),"good": 1},15: { "levelId": 6, "mem": bit6(0x2249f2),"good": 1},16: { "levelId": 6, "mem": bit0(0x2249f3),"good": 1},17: { "levelId": 6, "mem": bit3(0x2249f3),"good": 1},18: { "levelId": 6, "mem": bit2(0x2249f3),"good": 1},19: { "levelId": 8, "mem": bit5(0x2249f3),"good": 1},20: { "levelId": 8, "mem": bit4(0x2249f3),"good": 1},21: { "levelId": 10, "mem": bit0(0x2249f4),"good": 1},22: { "levelId": 10, "mem": bit6(0x2249f3),"good": 1},23: { "levelId": 10, "mem": bit3(0x2249f4),"good": 1},24: { "levelId": 10, "mem": bit5(0x2249f4),"good": 1},25: { "levelId": 10, "mem": bit7(0x2249f3),"good": 1},26: { "levelId": 10, "mem": bit1(0x2249f4),"good": 1},27: { "levelId": 10, "mem": bit2(0x2249f4),"good": 1},28: { "levelId": 10, "mem": bit4(0x2249f4),"good": 1},29: { "levelId": 3, "good": 0},30: { "levelId": 3, "good": 0},31: { "levelId": 3, "good": 0},32: { "levelId": 3, "good": 0},33: { "levelId": 3, "good": 0},34: { "levelId": 3, "good": 0},35: { "levelId": 3, "good": 0},36: { "levelId": 3, "good": 0},37: { "levelId": 3, "good": 0},38: { "levelId": 3, "good": 0},39: { "levelId": 3, "good": 0},40: { "levelId": 3, "good": 0},41: { "levelId": 3, "good": 0},42: { "levelId": 3, "good": 0},43: { "levelId": 3, "good": 0},44: { "levelId": 3, "good": 0},45: { "levelId": 3, "good": 0},46: { "levelId": 3, "good": 0},47: { "levelId": 3, "good": 0},48: { "levelId": 3, "good": 0},49: { "levelId": 3, "good": 0},50: { "levelId": 3, "good": 0},51: { "levelId": 3, "good": 0},52: { "levelId": 3, "good": 0},53: { "levelId": 3, "good": 0},54: { "levelId": 3, "good": 0},55: { "levelId": 3, "good": 0},56: { "levelId": 3, "good": 0},57: { "levelId": 3, "good": 0},58: { "levelId": 3, "good": 0},59: { "levelId": 3, "good": 0},60: { "levelId": 3, "good": 0},61: { "levelId": 3, "good": 0},62: { "levelId": 3, "good": 0},63: { "levelId": 3, "good": 0},64: { "levelId": 3, "good": 0},65: { "levelId": 3, "good": 0},66: { "levelId": 3, "good": 0},67: { "levelId": 3, "good": 0},68: { "levelId": 3, "good": 0},69: { "levelId": 3, "good": 0},70: { "levelId": 3, "good": 0},71: { "levelId": 3, "good": 0},72: { "levelId": 3, "good": 0},73: { "levelId": 3, "good": 0},74: { "levelId": 3, "good": 0},75: { "levelId": 3, "good": 0},76: { "levelId": 3, "good": 0},77: { "levelId": 3, "good": 0},78: { "levelId": 3, "good": 0},79: { "levelId": 3, "good": 0},80: { "levelId": 3, "good": 0},</v>
+        <v>1: { "levelId": 1, "mem": bit7(0x2249f0),"good": 1},2: { "levelId": 2, "mem": bit0(0x2249f1),"good": 1},3: { "levelId": 2, "mem": bit1(0x2249f1),"good": 1},4: { "levelId": 2, "mem": bit5(0x2249f1),"good": 1},5: { "levelId": 2, "mem": bit6(0x2249f1),"good": 1},6: { "levelId": 1, "mem": bit7(0x2249f1),"good": 1},7: { "levelId": 5, "mem": bit0(0x2249f2),"good": 1},8: { "levelId": 5, "mem": bit1(0x2249f2),"good": 1},9: { "levelId": 5, "mem": bit2(0x2249f2),"good": 1},10: { "levelId": 5, "mem": bit3(0x2249f2),"good": 1},11: { "levelId": 5, "mem": bit4(0x2249f2),"good": 1},12: { "levelId": 6, "mem": bit5(0x2249f2),"good": 1},13: { "levelId": 6, "mem": bit7(0x2249f2),"good": 1},14: { "levelId": 6, "mem": bit1(0x2249f3),"good": 1},15: { "levelId": 6, "mem": bit6(0x2249f2),"good": 1},16: { "levelId": 6, "mem": bit0(0x2249f3),"good": 1},17: { "levelId": 6, "mem": bit3(0x2249f3),"good": 1},18: { "levelId": 6, "mem": bit2(0x2249f3),"good": 1},19: { "levelId": 8, "mem": bit5(0x2249f3),"good": 1},20: { "levelId": 8, "mem": bit4(0x2249f3),"good": 1},21: { "levelId": 10, "mem": bit0(0x2249f4),"good": 1},22: { "levelId": 10, "mem": bit6(0x2249f3),"good": 1},23: { "levelId": 10, "mem": bit3(0x2249f4),"good": 1},24: { "levelId": 10, "mem": bit5(0x2249f4),"good": 1},25: { "levelId": 10, "mem": bit7(0x2249f3),"good": 1},26: { "levelId": 10, "mem": bit1(0x2249f4),"good": 1},27: { "levelId": 10, "mem": bit2(0x2249f4),"good": 1},28: { "levelId": 10, "mem": bit4(0x2249f4),"good": 1},29: { "levelId": 3, "mem": bit6(0x2249f4),"good": 1},30: { "levelId": 3, "mem": bit7(0x2249f4),"good": 1},31: { "levelId": 3, "good": 0},32: { "levelId": 3, "good": 0},33: { "levelId": 3, "good": 0},34: { "levelId": 3, "good": 0},35: { "levelId": 3, "good": 0},36: { "levelId": 3, "good": 0},37: { "levelId": 3, "good": 0},38: { "levelId": 3, "good": 0},39: { "levelId": 3, "good": 0},40: { "levelId": 3, "good": 0},41: { "levelId": 3, "good": 0},42: { "levelId": 3, "good": 0},43: { "levelId": 3, "good": 0},44: { "levelId": 3, "good": 0},45: { "levelId": 3, "good": 0},46: { "levelId": 3, "good": 0},47: { "levelId": 3, "good": 0},48: { "levelId": 3, "good": 0},49: { "levelId": 3, "good": 0},50: { "levelId": 3, "good": 0},51: { "levelId": 3, "good": 0},52: { "levelId": 3, "good": 0},53: { "levelId": 3, "good": 0},54: { "levelId": 3, "good": 0},55: { "levelId": 3, "good": 0},56: { "levelId": 3, "good": 0},57: { "levelId": 3, "good": 0},58: { "levelId": 3, "good": 0},59: { "levelId": 3, "good": 0},60: { "levelId": 3, "good": 0},61: { "levelId": 3, "good": 0},62: { "levelId": 3, "good": 0},63: { "levelId": 3, "good": 0},64: { "levelId": 3, "good": 0},65: { "levelId": 3, "good": 0},66: { "levelId": 3, "good": 0},67: { "levelId": 3, "good": 0},68: { "levelId": 3, "good": 0},69: { "levelId": 3, "good": 0},70: { "levelId": 3, "good": 0},71: { "levelId": 3, "good": 0},72: { "levelId": 3, "good": 0},73: { "levelId": 3, "good": 0},74: { "levelId": 3, "good": 0},75: { "levelId": 3, "good": 0},76: { "levelId": 3, "good": 0},77: { "levelId": 3, "good": 0},78: { "levelId": 3, "good": 0},79: { "levelId": 3, "good": 0},80: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>7</v>
@@ -18728,7 +18940,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0</v>
@@ -18743,7 +18955,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>1</v>
@@ -18758,7 +18970,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>5</v>
@@ -18773,7 +18985,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>6</v>
@@ -18788,7 +19000,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>7</v>
@@ -18803,7 +19015,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>0</v>
@@ -18818,7 +19030,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>1</v>
@@ -18833,7 +19045,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>2</v>
@@ -18848,7 +19060,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>3</v>
@@ -18863,7 +19075,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>4</v>
@@ -18878,7 +19090,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>5</v>
@@ -18893,7 +19105,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>7</v>
@@ -18908,7 +19120,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>1</v>
@@ -18923,7 +19135,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>6</v>
@@ -18938,7 +19150,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>0</v>
@@ -18953,7 +19165,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>3</v>
@@ -18968,7 +19180,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>2</v>
@@ -18983,7 +19195,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>5</v>
@@ -18998,7 +19210,7 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>4</v>
@@ -19013,7 +19225,7 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>0</v>
@@ -19028,7 +19240,7 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>6</v>
@@ -19043,7 +19255,7 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>3</v>
@@ -19058,7 +19270,7 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>5</v>
@@ -19073,7 +19285,7 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>7</v>
@@ -19088,7 +19300,7 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>1</v>
@@ -19103,7 +19315,7 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>2</v>
@@ -19118,7 +19330,7 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>4</v>
@@ -19132,21 +19344,33 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>6</v>
+      </c>
       <c r="C30" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D30" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C30, Levels!B:B, 0), 1, 1)),", ",IF(A30 &lt;&gt; "", """mem"": bit" &amp; B30 &amp; "(" &amp; A30 &amp; "),", ""),"""good"": ",IF(A30 &lt;&gt; "", 1, 0),"},")</f>
-        <v>29: { "levelId": 3, "good": 0},</v>
+        <v>29: { "levelId": 3, "mem": bit6(0x2249f4),"good": 1},</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>7</v>
+      </c>
       <c r="C31" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D31" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C31, Levels!B:B, 0), 1, 1)),", ",IF(A31 &lt;&gt; "", """mem"": bit" &amp; B31 &amp; "(" &amp; A31 &amp; "),", ""),"""good"": ",IF(A31 &lt;&gt; "", 1, 0),"},")</f>
-        <v>30: { "levelId": 3, "good": 0},</v>
+        <v>30: { "levelId": 3, "mem": bit7(0x2249f4),"good": 1},</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Updated the achievements for the Canopy
</commit_message>
<xml_diff>
--- a/Rayman 2.xlsx
+++ b/Rayman 2.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1573" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1605" uniqueCount="149">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -283,6 +283,12 @@
     <t xml:space="preserve">CanopyArea2</t>
   </si>
   <si>
+    <t xml:space="preserve">790A4C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CanopyArea3</t>
+  </si>
+  <si>
     <t xml:space="preserve">Index</t>
   </si>
   <si>
@@ -439,6 +445,12 @@
     <t xml:space="preserve">0x2249ab</t>
   </si>
   <si>
+    <t xml:space="preserve">0x2249ac</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x2249ad</t>
+  </si>
+  <si>
     <t xml:space="preserve">Level ID</t>
   </si>
   <si>
@@ -455,6 +467,9 @@
   </si>
   <si>
     <t xml:space="preserve">0x2249f4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x2249f5</t>
   </si>
 </sst>
 </file>
@@ -668,7 +683,7 @@
       <selection pane="bottomLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.90234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.66"/>
@@ -698,7 +713,7 @@
       </c>
       <c r="H1" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(E2:E1000)</f>
-        <v>0x784BFC: { "id": 0x784BFC, "areaName": "Menu", "displayName": "Main Menu", "levelName": "Menu" },0x789668: { "id": 0x789668, "areaName": "Intro", "displayName": "somewhere in the Glade of Dreams…", "levelName": "None" },0x778C74: { "id": 0x778C74, "areaName": "BuccaneerBrig", "displayName": "in the Buccaneer’s brig", "levelName": "None" },0x78D424: { "id": 0x78D424, "areaName": "WoodsOfLight", "displayName": "in the Woods of Light", "levelName": "Woods of Light" },0x790570: { "id": 0x790570, "areaName": "HallOfDoors", "displayName": "in the Hall of Doors", "levelName": "Hall of Doors" },0x7875A8: { "id": 0x7875A8, "areaName": "FairyGladeArea1", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x78A320: { "id": 0x78A320, "areaName": "FairyGladeArea2", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x7A1BD8: { "id": 0x7A1BD8, "areaName": "FairyGladeArea3", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x77BFFC: { "id": 0x77BFFC, "areaName": "FairyGladeArea4", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x771B74: { "id": 0x771B74, "areaName": "FairyGladeArea5", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x74AAA8: { "id": 0x74AAA8, "areaName": "Results", "displayName": "viewing level results…", "levelName": "None" },0x788708: { "id": 0x788708, "areaName": "MarshesArea1", "displayName": "in the Marshes of Awakening", "levelName": "Marshes of Awakening" },0x7786E8: { "id": 0x7786E8, "areaName": "MarshesArea2", "displayName": "in the Marshes of Awakening", "levelName": "Marshes of Awakening" },0x790598: { "id": 0x790598, "areaName": "BayouArea1", "displayName": "in the Bayou", "levelName": "Bayou" },0x788764: { "id": 0x788764, "areaName": "BayouArea2", "displayName": "in the Bayou", "levelName": "Bayou" },0x7928A4: { "id": 0x7928A4, "areaName": "SoWaIArea1", "displayName": "in the Sanctuary of Water and Ice", "levelName": "Sanctuary of Water and Ice" },0x774694: { "id": 0x774694, "areaName": "SoWaIArea2", "displayName": "in the Sanctuary of Water and Ice", "levelName": "Sanctuary of Water and Ice" },0x76F100: { "id": 0x76F100, "areaName": "Polokus", "displayName": "in Polokus’s dream", "levelName": "Polokus" },0x0: { "id": 0x0, "areaName": "None", "displayName": "somewhere in the Glade of Dreams…", "levelName": "None" },0x751974: { "id": 0x751974, "areaName": "Bonus", "displayName": "in the bonus stage", "levelName": "None" },0x776C08: { "id": 0x776C08, "areaName": "MenhirArea1", "displayName": "in the Menhir Hills", "levelName": "Menhir Hills" },0x78FBD8: { "id": 0x78FBD8, "areaName": "MenhirArea2", "displayName": "in the Menhir Hills", "levelName": "Menhir Hills" },0x788950: { "id": 0x788950, "areaName": "MenhirArea3", "displayName": "in the Menhir Hills", "levelName": "Menhir Hills" },0x78402C: { "id": 0x78402C, "areaName": "BadDreamsArea1", "displayName": "in the Cave of Bad Dreams", "levelName": "Cave of Bad Dreams" },0x788148: { "id": 0x788148, "areaName": "BadDreamsArea2", "displayName": "in the Cave of Bad Dreams", "levelName": "Cave of Bad Dreams" },0x75AADC: { "id": 0x75AADC, "areaName": "MenhirArea4", "displayName": "in the Menhir Hills", "levelName": "Menhir Hills" },0x75BE94: { "id": 0x75BE94, "areaName": "CanopyArea1", "displayName": "in the Canopy", "levelName": "Canopy" },0x78C480: { "id": 0x78C480, "areaName": "CanopyArea2", "displayName": "in the Canopy", "levelName": "Canopy" },</v>
+        <v>0x784BFC: { "id": 0x784BFC, "areaName": "Menu", "displayName": "Main Menu", "levelName": "Menu" },0x789668: { "id": 0x789668, "areaName": "Intro", "displayName": "somewhere in the Glade of Dreams…", "levelName": "None" },0x778C74: { "id": 0x778C74, "areaName": "BuccaneerBrig", "displayName": "in the Buccaneer’s brig", "levelName": "None" },0x78D424: { "id": 0x78D424, "areaName": "WoodsOfLight", "displayName": "in the Woods of Light", "levelName": "Woods of Light" },0x790570: { "id": 0x790570, "areaName": "HallOfDoors", "displayName": "in the Hall of Doors", "levelName": "Hall of Doors" },0x7875A8: { "id": 0x7875A8, "areaName": "FairyGladeArea1", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x78A320: { "id": 0x78A320, "areaName": "FairyGladeArea2", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x7A1BD8: { "id": 0x7A1BD8, "areaName": "FairyGladeArea3", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x77BFFC: { "id": 0x77BFFC, "areaName": "FairyGladeArea4", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x771B74: { "id": 0x771B74, "areaName": "FairyGladeArea5", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x74AAA8: { "id": 0x74AAA8, "areaName": "Results", "displayName": "viewing level results…", "levelName": "None" },0x788708: { "id": 0x788708, "areaName": "MarshesArea1", "displayName": "in the Marshes of Awakening", "levelName": "Marshes of Awakening" },0x7786E8: { "id": 0x7786E8, "areaName": "MarshesArea2", "displayName": "in the Marshes of Awakening", "levelName": "Marshes of Awakening" },0x790598: { "id": 0x790598, "areaName": "BayouArea1", "displayName": "in the Bayou", "levelName": "Bayou" },0x788764: { "id": 0x788764, "areaName": "BayouArea2", "displayName": "in the Bayou", "levelName": "Bayou" },0x7928A4: { "id": 0x7928A4, "areaName": "SoWaIArea1", "displayName": "in the Sanctuary of Water and Ice", "levelName": "Sanctuary of Water and Ice" },0x774694: { "id": 0x774694, "areaName": "SoWaIArea2", "displayName": "in the Sanctuary of Water and Ice", "levelName": "Sanctuary of Water and Ice" },0x76F100: { "id": 0x76F100, "areaName": "Polokus", "displayName": "in Polokus’s dream", "levelName": "Polokus" },0x0: { "id": 0x0, "areaName": "None", "displayName": "somewhere in the Glade of Dreams…", "levelName": "None" },0x751974: { "id": 0x751974, "areaName": "Bonus", "displayName": "in the bonus stage", "levelName": "None" },0x776C08: { "id": 0x776C08, "areaName": "MenhirArea1", "displayName": "in the Menhir Hills", "levelName": "Menhir Hills" },0x78FBD8: { "id": 0x78FBD8, "areaName": "MenhirArea2", "displayName": "in the Menhir Hills", "levelName": "Menhir Hills" },0x788950: { "id": 0x788950, "areaName": "MenhirArea3", "displayName": "in the Menhir Hills", "levelName": "Menhir Hills" },0x78402C: { "id": 0x78402C, "areaName": "BadDreamsArea1", "displayName": "in the Cave of Bad Dreams", "levelName": "Cave of Bad Dreams" },0x788148: { "id": 0x788148, "areaName": "BadDreamsArea2", "displayName": "in the Cave of Bad Dreams", "levelName": "Cave of Bad Dreams" },0x75AADC: { "id": 0x75AADC, "areaName": "MenhirArea4", "displayName": "in the Menhir Hills", "levelName": "Menhir Hills" },0x75BE94: { "id": 0x75BE94, "areaName": "CanopyArea1", "displayName": "in the Canopy", "levelName": "Canopy" },0x78C480: { "id": 0x78C480, "areaName": "CanopyArea2", "displayName": "in the Canopy", "levelName": "Canopy" },0x790A4C: { "id": 0x790A4C, "areaName": "CanopyArea3", "displayName": "in the Canopy", "levelName": "Canopy" },</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1206,7 +1221,22 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D30" s="4"/>
+      <c r="A30" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E30" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("0x", A30,": { ""id"": ","0x", A30,", ""areaName"": """,B30,""", ""displayName"": """,C30,""", ""levelName"": """,D30,""" },")</f>
+        <v>0x790A4C: { "id": 0x790A4C, "areaName": "CanopyArea3", "displayName": "in the Canopy", "levelName": "Canopy" },</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D31" s="4"/>
@@ -4190,10 +4220,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+      <selection pane="bottomLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.21"/>
@@ -4205,22 +4235,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>4</v>
@@ -4296,11 +4326,11 @@
       </c>
       <c r="E4" s="0" t="n">
         <f aca="false">COUNTIFS(Lums!C3:C1002, "=" &amp; B4)</f>
-        <v>684</v>
+        <v>658</v>
       </c>
       <c r="F4" s="0" t="n">
         <f aca="false">COUNTIFS(Cages!C3:C83, "=" &amp; B4)</f>
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="G4" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A4,": { ""id"": ",A4,", ""name"": """,B4,""", ""lums"": ",C4,", ""cages"": ",D4," },")</f>
@@ -4539,11 +4569,11 @@
       </c>
       <c r="E13" s="0" t="n">
         <f aca="false">COUNTIFS(Lums!C12:C1011, "=" &amp; B13)</f>
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="F13" s="0" t="n">
         <f aca="false">COUNTIFS(Cages!C12:C92, "=" &amp; B13)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G13" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A13,": { ""id"": ",A13,", ""name"": """,B13,""", ""lums"": ",C13,", ""cages"": ",D13," },")</f>
@@ -7928,12 +7958,12 @@
   <dimension ref="A1:H1001"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A290" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A306" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C318" activeCellId="0" sqref="C318"/>
+      <selection pane="bottomLeft" activeCell="C344" activeCellId="0" sqref="C344"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.93"/>
@@ -7942,10 +7972,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>3</v>
@@ -7958,12 +7988,12 @@
       </c>
       <c r="H1" s="5" t="str">
         <f aca="false">_xlfn.CONCAT(D2:D1001)</f>
-        <v>1: { "levelId": 2, "mem": bit0(0x224988),"good": 1, "addr": 0x224988, "bit": 0},2: { "levelId": 2, "mem": bit1(0x224988),"good": 1, "addr": 0x224988, "bit": 1},3: { "levelId": 2, "mem": bit2(0x224988),"good": 1, "addr": 0x224988, "bit": 2},4: { "levelId": 2, "mem": bit3(0x224988),"good": 1, "addr": 0x224988, "bit": 3},5: { "levelId": 2, "mem": bit4(0x224988),"good": 1, "addr": 0x224988, "bit": 4},6: { "levelId": 2, "mem": bit5(0x224988),"good": 1, "addr": 0x224988, "bit": 5},7: { "levelId": 2, "mem": bit6(0x224988),"good": 1, "addr": 0x224988, "bit": 6},8: { "levelId": 2, "mem": bit7(0x224988),"good": 1, "addr": 0x224988, "bit": 7},9: { "levelId": 2, "mem": bit2(0x224989),"good": 1, "addr": 0x224989, "bit": 2},10: { "levelId": 2, "mem": bit1(0x22498a),"good": 1, "addr": 0x22498a, "bit": 1},11: { "levelId": 2, "mem": bit2(0x22498a),"good": 1, "addr": 0x22498a, "bit": 2},12: { "levelId": 2, "mem": bit3(0x22498a),"good": 1, "addr": 0x22498a, "bit": 3},13: { "levelId": 2, "mem": bit4(0x22498a),"good": 1, "addr": 0x22498a, "bit": 4},14: { "levelId": 2, "mem": bit5(0x22498a),"good": 1, "addr": 0x22498a, "bit": 5},15: { "levelId": 2, "mem": bit6(0x22498a),"good": 1, "addr": 0x22498a, "bit": 6},16: { "levelId": 2, "mem": bit7(0x22498a),"good": 1, "addr": 0x22498a, "bit": 7},17: { "levelId": 2, "mem": bit5(0x22498b),"good": 1, "addr": 0x22498b, "bit": 5},18: { "levelId": 2, "mem": bit6(0x22498b),"good": 1, "addr": 0x22498b, "bit": 6},19: { "levelId": 2, "mem": bit7(0x22498b),"good": 1, "addr": 0x22498b, "bit": 7},20: { "levelId": 2, "mem": bit0(0x22498c),"good": 1, "addr": 0x22498c, "bit": 0},21: { "levelId": 2, "mem": bit1(0x22498c),"good": 1, "addr": 0x22498c, "bit": 1},22: { "levelId": 2, "mem": bit2(0x22498c),"good": 1, "addr": 0x22498c, "bit": 2},23: { "levelId": 2, "mem": bit3(0x22498c),"good": 1, "addr": 0x22498c, "bit": 3},24: { "levelId": 2, "mem": bit4(0x22498c),"good": 1, "addr": 0x22498c, "bit": 4},25: { "levelId": 2, "mem": bit5(0x22498c),"good": 1, "addr": 0x22498c, "bit": 5},26: { "levelId": 2, "mem": bit6(0x22498c),"good": 1, "addr": 0x22498c, "bit": 6},27: { "levelId": 2, "mem": bit7(0x22498c),"good": 1, "addr": 0x22498c, "bit": 7},28: { "levelId": 2, "mem": bit0(0x22498d),"good": 1, "addr": 0x22498d, "bit": 0},29: { "levelId": 2, "mem": bit1(0x22498d),"good": 1, "addr": 0x22498d, "bit": 1},30: { "levelId": 2, "mem": bit2(0x22498d),"good": 1, "addr": 0x22498d, "bit": 2},31: { "levelId": 2, "mem": bit3(0x22498d),"good": 1, "addr": 0x22498d, "bit": 3},32: { "levelId": 2, "mem": bit4(0x22498d),"good": 1, "addr": 0x22498d, "bit": 4},33: { "levelId": 2, "mem": bit5(0x22498d),"good": 1, "addr": 0x22498d, "bit": 5},34: { "levelId": 2, "mem": bit6(0x22498d),"good": 1, "addr": 0x22498d, "bit": 6},35: { "levelId": 2, "mem": bit7(0x22498d),"good": 1, "addr": 0x22498d, "bit": 7},36: { "levelId": 2, "mem": bit0(0x22498e),"good": 1, "addr": 0x22498e, "bit": 0},37: { "levelId": 2, "mem": bit1(0x22498e),"good": 1, "addr": 0x22498e, "bit": 1},38: { "levelId": 5, "mem": bit2(0x22498e),"good": 1, "addr": 0x22498e, "bit": 2},39: { "levelId": 5, "mem": bit3(0x22498e),"good": 1, "addr": 0x22498e, "bit": 3},40: { "levelId": 5, "mem": bit4(0x22498e),"good": 1, "addr": 0x22498e, "bit": 4},41: { "levelId": 5, "mem": bit5(0x22498e),"good": 1, "addr": 0x22498e, "bit": 5},42: { "levelId": 5, "mem": bit6(0x22498e),"good": 1, "addr": 0x22498e, "bit": 6},43: { "levelId": 5, "mem": bit7(0x22498e),"good": 1, "addr": 0x22498e, "bit": 7},44: { "levelId": 5, "mem": bit0(0x22498f),"good": 1, "addr": 0x22498f, "bit": 0},45: { "levelId": 5, "mem": bit1(0x22498f),"good": 1, "addr": 0x22498f, "bit": 1},46: { "levelId": 5, "mem": bit2(0x22498f),"good": 1, "addr": 0x22498f, "bit": 2},47: { "levelId": 5, "mem": bit3(0x22498f),"good": 1, "addr": 0x22498f, "bit": 3},48: { "levelId": 5, "mem": bit4(0x22498f),"good": 1, "addr": 0x22498f, "bit": 4},49: { "levelId": 5, "mem": bit5(0x22498f),"good": 1, "addr": 0x22498f, "bit": 5},50: { "levelId": 5, "mem": bit6(0x22498f),"good": 1, "addr": 0x22498f, "bit": 6},51: { "levelId": 5, "mem": bit7(0x22498f),"good": 1, "addr": 0x22498f, "bit": 7},52: { "levelId": 5, "mem": bit0(0x224990),"good": 1, "addr": 0x224990, "bit": 0},53: { "levelId": 5, "mem": bit1(0x224990),"good": 1, "addr": 0x224990, "bit": 1},54: { "levelId": 5, "mem": bit2(0x224990),"good": 1, "addr": 0x224990, "bit": 2},55: { "levelId": 5, "mem": bit3(0x224990),"good": 1, "addr": 0x224990, "bit": 3},56: { "levelId": 5, "mem": bit4(0x224990),"good": 1, "addr": 0x224990, "bit": 4},57: { "levelId": 5, "mem": bit5(0x224990),"good": 1, "addr": 0x224990, "bit": 5},58: { "levelId": 5, "mem": bit6(0x224990),"good": 1, "addr": 0x224990, "bit": 6},59: { "levelId": 5, "mem": bit7(0x224990),"good": 1, "addr": 0x224990, "bit": 7},60: { "levelId": 5, "mem": bit0(0x224991),"good": 1, "addr": 0x224991, "bit": 0},61: { "levelId": 5, "mem": bit1(0x224991),"good": 1, "addr": 0x224991, "bit": 1},62: { "levelId": 5, "mem": bit2(0x224991),"good": 1, "addr": 0x224991, "bit": 2},63: { "levelId": 5, "mem": bit3(0x224991),"good": 1, "addr": 0x224991, "bit": 3},64: { "levelId": 5, "mem": bit4(0x224991),"good": 1, "addr": 0x224991, "bit": 4},65: { "levelId": 5, "mem": bit5(0x224991),"good": 1, "addr": 0x224991, "bit": 5},66: { "levelId": 5, "mem": bit6(0x224991),"good": 1, "addr": 0x224991, "bit": 6},67: { "levelId": 5, "mem": bit7(0x224991),"good": 1, "addr": 0x224991, "bit": 7},68: { "levelId": 5, "mem": bit0(0x224992),"good": 1, "addr": 0x224992, "bit": 0},69: { "levelId": 5, "mem": bit1(0x224992),"good": 1, "addr": 0x224992, "bit": 1},70: { "levelId": 5, "mem": bit2(0x224992),"good": 1, "addr": 0x224992, "bit": 2},71: { "levelId": 5, "mem": bit3(0x224992),"good": 1, "addr": 0x224992, "bit": 3},72: { "levelId": 5, "mem": bit4(0x224992),"good": 1, "addr": 0x224992, "bit": 4},73: { "levelId": 5, "mem": bit5(0x224992),"good": 1, "addr": 0x224992, "bit": 5},74: { "levelId": 5, "mem": bit6(0x224992),"good": 1, "addr": 0x224992, "bit": 6},75: { "levelId": 5, "mem": bit7(0x224992),"good": 1, "addr": 0x224992, "bit": 7},76: { "levelId": 5, "mem": bit0(0x224993),"good": 1, "addr": 0x224993, "bit": 0},77: { "levelId": 5, "mem": bit1(0x224993),"good": 1, "addr": 0x224993, "bit": 1},78: { "levelId": 5, "mem": bit2(0x224993),"good": 1, "addr": 0x224993, "bit": 2},79: { "levelId": 5, "mem": bit3(0x224993),"good": 1, "addr": 0x224993, "bit": 3},80: { "levelId": 5, "mem": bit4(0x224993),"good": 1, "addr": 0x224993, "bit": 4},81: { "levelId": 5, "mem": bit5(0x224993),"good": 1, "addr": 0x224993, "bit": 5},82: { "levelId": 5, "mem": bit6(0x224993),"good": 1, "addr": 0x224993, "bit": 6},83: { "levelId": 5, "mem": bit7(0x224993),"good": 1, "addr": 0x224993, "bit": 7},84: { "levelId": 5, "mem": bit0(0x224994),"good": 1, "addr": 0x224994, "bit": 0},85: { "levelId": 5, "mem": bit1(0x224994),"good": 1, "addr": 0x224994, "bit": 1},86: { "levelId": 5, "mem": bit2(0x224994),"good": 1, "addr": 0x224994, "bit": 2},87: { "levelId": 5, "mem": bit3(0x224994),"good": 1, "addr": 0x224994, "bit": 3},88: { "levelId": 6, "mem": bit4(0x224994),"good": 1, "addr": 0x224994, "bit": 4},89: { "levelId": 6, "mem": bit5(0x224994),"good": 1, "addr": 0x224994, "bit": 5},90: { "levelId": 6, "mem": bit6(0x224994),"good": 1, "addr": 0x224994, "bit": 6},91: { "levelId": 6, "mem": bit7(0x224994),"good": 1, "addr": 0x224994, "bit": 7},92: { "levelId": 6, "mem": bit0(0x224995),"good": 1, "addr": 0x224995, "bit": 0},93: { "levelId": 6, "mem": bit1(0x224995),"good": 1, "addr": 0x224995, "bit": 1},94: { "levelId": 6, "mem": bit2(0x224995),"good": 1, "addr": 0x224995, "bit": 2},95: { "levelId": 6, "mem": bit3(0x224995),"good": 1, "addr": 0x224995, "bit": 3},96: { "levelId": 6, "mem": bit4(0x224995),"good": 1, "addr": 0x224995, "bit": 4},97: { "levelId": 6, "mem": bit5(0x224995),"good": 1, "addr": 0x224995, "bit": 5},98: { "levelId": 6, "mem": bit6(0x224995),"good": 1, "addr": 0x224995, "bit": 6},99: { "levelId": 6, "mem": bit7(0x224995),"good": 1, "addr": 0x224995, "bit": 7},100: { "levelId": 6, "mem": bit0(0x224996),"good": 1, "addr": 0x224996, "bit": 0},101: { "levelId": 6, "mem": bit1(0x224996),"good": 1, "addr": 0x224996, "bit": 1},102: { "levelId": 6, "mem": bit2(0x224996),"good": 1, "addr": 0x224996, "bit": 2},103: { "levelId": 6, "mem": bit3(0x224996),"good": 1, "addr": 0x224996, "bit": 3},104: { "levelId": 6, "mem": bit4(0x224996),"good": 1, "addr": 0x224996, "bit": 4},105: { "levelId": 6, "mem": bit5(0x224996),"good": 1, "addr": 0x224996, "bit": 5},106: { "levelId": 6, "mem": bit6(0x224996),"good": 1, "addr": 0x224996, "bit": 6},107: { "levelId": 6, "mem": bit7(0x224996),"good": 1, "addr": 0x224996, "bit": 7},108: { "levelId": 6, "mem": bit0(0x224997),"good": 1, "addr": 0x224997, "bit": 0},109: { "levelId": 6, "mem": bit1(0x224997),"good": 1, "addr": 0x224997, "bit": 1},110: { "levelId": 6, "mem": bit2(0x224997),"good": 1, "addr": 0x224997, "bit": 2},111: { "levelId": 6, "mem": bit3(0x224997),"good": 1, "addr": 0x224997, "bit": 3},112: { "levelId": 6, "mem": bit4(0x224997),"good": 1, "addr": 0x224997, "bit": 4},113: { "levelId": 6, "mem": bit5(0x224997),"good": 1, "addr": 0x224997, "bit": 5},114: { "levelId": 6, "mem": bit6(0x224997),"good": 1, "addr": 0x224997, "bit": 6},115: { "levelId": 6, "mem": bit7(0x224997),"good": 1, "addr": 0x224997, "bit": 7},116: { "levelId": 6, "mem": bit0(0x224998),"good": 1, "addr": 0x224998, "bit": 0},117: { "levelId": 6, "mem": bit1(0x224998),"good": 1, "addr": 0x224998, "bit": 1},118: { "levelId": 6, "mem": bit2(0x224998),"good": 1, "addr": 0x224998, "bit": 2},119: { "levelId": 6, "mem": bit3(0x224998),"good": 1, "addr": 0x224998, "bit": 3},120: { "levelId": 6, "mem": bit4(0x224998),"good": 1, "addr": 0x224998, "bit": 4},121: { "levelId": 6, "mem": bit5(0x224998),"good": 1, "addr": 0x224998, "bit": 5},122: { "levelId": 6, "mem": bit6(0x224998),"good": 1, "addr": 0x224998, "bit": 6},123: { "levelId": 6, "mem": bit0(0x224999),"good": 1, "addr": 0x224999, "bit": 0},124: { "levelId": 6, "mem": bit1(0x224999),"good": 1, "addr": 0x224999, "bit": 1},125: { "levelId": 6, "mem": bit2(0x224999),"good": 1, "addr": 0x224999, "bit": 2},126: { "levelId": 6, "mem": bit3(0x224999),"good": 1, "addr": 0x224999, "bit": 3},127: { "levelId": 6, "mem": bit4(0x224999),"good": 1, "addr": 0x224999, "bit": 4},128: { "levelId": 6, "mem": bit5(0x224999),"good": 1, "addr": 0x224999, "bit": 5},129: { "levelId": 6, "mem": bit6(0x224999),"good": 1, "addr": 0x224999, "bit": 6},130: { "levelId": 6, "mem": bit7(0x224999),"good": 1, "addr": 0x224999, "bit": 7},131: { "levelId": 6, "mem": bit0(0x22499a),"good": 1, "addr": 0x22499a, "bit": 0},132: { "levelId": 6, "mem": bit1(0x22499a),"good": 1, "addr": 0x22499a, "bit": 1},133: { "levelId": 6, "mem": bit2(0x22499a),"good": 1, "addr": 0x22499a, "bit": 2},134: { "levelId": 6, "mem": bit3(0x22499a),"good": 1, "addr": 0x22499a, "bit": 3},135: { "levelId": 6, "mem": bit4(0x22499a),"good": 1, "addr": 0x22499a, "bit": 4},136: { "levelId": 6, "mem": bit5(0x22499a),"good": 1, "addr": 0x22499a, "bit": 5},137: { "levelId": 1, "mem": bit3(0x224a36),"good": 1, "addr": 0x224a36, "bit": 3},138: { "levelId": 1, "mem": bit4(0x224a36),"good": 1, "addr": 0x224a36, "bit": 4},139: { "levelId": 1, "mem": bit5(0x224a36),"good": 1, "addr": 0x224a36, "bit": 5},140: { "levelId": 1, "mem": bit6(0x224a36),"good": 1, "addr": 0x224a36, "bit": 6},141: { "levelId": 1, "mem": bit7(0x224a36),"good": 1, "addr": 0x224a36, "bit": 7},142: { "levelId": 6, "mem": bit7(0x224998),"good": 1, "addr": 0x224998, "bit": 7},143: { "levelId": 8, "mem": bit3(0x22499b),"good": 1, "addr": 0x22499b, "bit": 3},144: { "levelId": 8, "mem": bit4(0x22499b),"good": 1, "addr": 0x22499b, "bit": 4},145: { "levelId": 8, "mem": bit5(0x22499b),"good": 1, "addr": 0x22499b, "bit": 5},146: { "levelId": 8, "mem": bit5(0x22499c),"good": 1, "addr": 0x22499c, "bit": 5},147: { "levelId": 8, "mem": bit6(0x22499c),"good": 1, "addr": 0x22499c, "bit": 6},148: { "levelId": 8, "mem": bit7(0x22499c),"good": 1, "addr": 0x22499c, "bit": 7},149: { "levelId": 8, "mem": bit0(0x22499d),"good": 1, "addr": 0x22499d, "bit": 0},150: { "levelId": 8, "mem": bit1(0x22499d),"good": 1, "addr": 0x22499d, "bit": 1},151: { "levelId": 8, "mem": bit2(0x22499d),"good": 1, "addr": 0x22499d, "bit": 2},152: { "levelId": 8, "mem": bit3(0x22499d),"good": 1, "addr": 0x22499d, "bit": 3},153: { "levelId": 8, "mem": bit4(0x22499d),"good": 1, "addr": 0x22499d, "bit": 4},154: { "levelId": 8, "mem": bit5(0x22499d),"good": 1, "addr": 0x22499d, "bit": 5},155: { "levelId": 8, "mem": bit6(0x22499d),"good": 1, "addr": 0x22499d, "bit": 6},156: { "levelId": 8, "mem": bit7(0x22499d),"good": 1, "addr": 0x22499d, "bit": 7},157: { "levelId": 8, "mem": bit0(0x22499e),"good": 1, "addr": 0x22499e, "bit": 0},158: { "levelId": 8, "mem": bit1(0x22499e),"good": 1, "addr": 0x22499e, "bit": 1},159: { "levelId": 8, "mem": bit6(0x22499a),"good": 1, "addr": 0x22499a, "bit": 6},160: { "levelId": 8, "mem": bit7(0x22499a),"good": 1, "addr": 0x22499a, "bit": 7},161: { "levelId": 8, "mem": bit0(0x22499b),"good": 1, "addr": 0x22499b, "bit": 0},162: { "levelId": 8, "mem": bit1(0x22499b),"good": 1, "addr": 0x22499b, "bit": 1},163: { "levelId": 8, "mem": bit2(0x22499b),"good": 1, "addr": 0x22499b, "bit": 2},164: { "levelId": 8, "mem": bit6(0x22499b),"good": 1, "addr": 0x22499b, "bit": 6},165: { "levelId": 8, "mem": bit7(0x22499b),"good": 1, "addr": 0x22499b, "bit": 7},166: { "levelId": 8, "mem": bit0(0x22499c),"good": 1, "addr": 0x22499c, "bit": 0},167: { "levelId": 8, "mem": bit1(0x22499c),"good": 1, "addr": 0x22499c, "bit": 1},168: { "levelId": 8, "mem": bit2(0x22499c),"good": 1, "addr": 0x22499c, "bit": 2},169: { "levelId": 8, "mem": bit3(0x22499c),"good": 1, "addr": 0x22499c, "bit": 3},170: { "levelId": 8, "mem": bit4(0x22499c),"good": 1, "addr": 0x22499c, "bit": 4},171: { "levelId": 8, "mem": bit2(0x22499e),"good": 1, "addr": 0x22499e, "bit": 2},172: { "levelId": 8, "mem": bit3(0x22499e),"good": 1, "addr": 0x22499e, "bit": 3},173: { "levelId": 8, "mem": bit4(0x22499e),"good": 1, "addr": 0x22499e, "bit": 4},174: { "levelId": 8, "mem": bit5(0x22499e),"good": 1, "addr": 0x22499e, "bit": 5},175: { "levelId": 8, "mem": bit6(0x22499e),"good": 1, "addr": 0x22499e, "bit": 6},176: { "levelId": 8, "mem": bit7(0x22499e),"good": 1, "addr": 0x22499e, "bit": 7},177: { "levelId": 8, "mem": bit0(0x22499f),"good": 1, "addr": 0x22499f, "bit": 0},178: { "levelId": 8, "mem": bit1(0x22499f),"good": 1, "addr": 0x22499f, "bit": 1},179: { "levelId": 8, "mem": bit2(0x22499f),"good": 1, "addr": 0x22499f, "bit": 2},180: { "levelId": 8, "mem": bit3(0x22499f),"good": 1, "addr": 0x22499f, "bit": 3},181: { "levelId": 8, "mem": bit4(0x22499f),"good": 1, "addr": 0x22499f, "bit": 4},182: { "levelId": 8, "mem": bit5(0x22499f),"good": 1, "addr": 0x22499f, "bit": 5},183: { "levelId": 8, "mem": bit6(0x22499f),"good": 1, "addr": 0x22499f, "bit": 6},184: { "levelId": 8, "mem": bit7(0x22499f),"good": 1, "addr": 0x22499f, "bit": 7},185: { "levelId": 8, "mem": bit0(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 0},186: { "levelId": 8, "mem": bit1(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 1},187: { "levelId": 8, "mem": bit2(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 2},188: { "levelId": 8, "mem": bit3(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 3},189: { "levelId": 8, "mem": bit4(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 4},190: { "levelId": 8, "mem": bit5(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 5},191: { "levelId": 8, "mem": bit6(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 6},192: { "levelId": 8, "mem": bit7(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 7},193: { "levelId": 10, "mem": bit0(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 0},194: { "levelId": 10, "mem": bit1(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 1},195: { "levelId": 10, "mem": bit2(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 2},196: { "levelId": 10, "mem": bit3(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 3},197: { "levelId": 10, "mem": bit4(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 4},198: { "levelId": 10, "mem": bit2(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 2},199: { "levelId": 10, "mem": bit3(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 3},200: { "levelId": 10, "mem": bit4(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 4},201: { "levelId": 10, "mem": bit5(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 5},202: { "levelId": 10, "mem": bit6(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 6},203: { "levelId": 10, "mem": bit1(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 1},204: { "levelId": 10, "mem": bit5(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 5},205: { "levelId": 10, "mem": bit6(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 6},206: { "levelId": 10, "mem": bit7(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 7},207: { "levelId": 10, "mem": bit0(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 0},208: { "levelId": 10, "mem": bit3(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 3},209: { "levelId": 10, "mem": bit5(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 5},210: { "levelId": 10, "mem": bit6(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 6},211: { "levelId": 10, "mem": bit7(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 7},212: { "levelId": 10, "mem": bit0(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 0},213: { "levelId": 10, "mem": bit1(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 1},214: { "levelId": 10, "mem": bit2(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 2},215: { "levelId": 10, "mem": bit4(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 4},216: { "levelId": 11, "mem": bit6(0x2249e5),"good": 1, "addr": 0x2249e5, "bit": 6},217: { "levelId": 11, "mem": bit7(0x2249e5),"good": 1, "addr": 0x2249e5, "bit": 7},218: { "levelId": 11, "mem": bit0(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 0},219: { "levelId": 11, "mem": bit1(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 1},220: { "levelId": 11, "mem": bit2(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 2},221: { "levelId": 11, "mem": bit3(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 3},222: { "levelId": 11, "mem": bit4(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 4},223: { "levelId": 11, "mem": bit5(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 5},224: { "levelId": 11, "mem": bit6(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 6},225: { "levelId": 11, "mem": bit7(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 7},226: { "levelId": 11, "mem": bit0(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 0},227: { "levelId": 11, "mem": bit1(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 1},228: { "levelId": 11, "mem": bit2(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 2},229: { "levelId": 11, "mem": bit3(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 3},230: { "levelId": 11, "mem": bit4(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 4},231: { "levelId": 11, "mem": bit5(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 5},232: { "levelId": 11, "mem": bit6(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 6},233: { "levelId": 11, "mem": bit7(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 7},234: { "levelId": 11, "mem": bit0(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 0},235: { "levelId": 11, "mem": bit1(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 1},236: { "levelId": 11, "mem": bit2(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 2},237: { "levelId": 11, "mem": bit3(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 3},238: { "levelId": 11, "mem": bit4(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 4},239: { "levelId": 11, "mem": bit5(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 5},240: { "levelId": 11, "mem": bit6(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 6},241: { "levelId": 11, "mem": bit7(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 7},242: { "levelId": 11, "mem": bit0(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 0},243: { "levelId": 11, "mem": bit1(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 1},244: { "levelId": 11, "mem": bit2(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 2},245: { "levelId": 11, "mem": bit3(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 3},246: { "levelId": 11, "mem": bit4(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 4},247: { "levelId": 11, "mem": bit5(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 5},248: { "levelId": 11, "mem": bit6(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 6},249: { "levelId": 11, "mem": bit7(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 7},250: { "levelId": 11, "mem": bit0(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 0},251: { "levelId": 11, "mem": bit1(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 1},252: { "levelId": 11, "mem": bit2(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 2},253: { "levelId": 11, "mem": bit3(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 3},254: { "levelId": 11, "mem": bit4(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 4},255: { "levelId": 11, "mem": bit5(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 5},256: { "levelId": 11, "mem": bit6(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 6},257: { "levelId": 11, "mem": bit7(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 7},258: { "levelId": 11, "mem": bit0(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 0},259: { "levelId": 11, "mem": bit1(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 1},260: { "levelId": 11, "mem": bit2(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 2},261: { "levelId": 11, "mem": bit3(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 3},262: { "levelId": 11, "mem": bit4(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 4},263: { "levelId": 11, "mem": bit5(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 5},264: { "levelId": 11, "mem": bit6(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 6},265: { "levelId": 11, "mem": bit7(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 7},266: { "levelId": 10, "mem": bit2(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 2},267: { "levelId": 10, "mem": bit2(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 2},268: { "levelId": 10, "mem": bit3(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 3},269: { "levelId": 10, "mem": bit4(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 4},270: { "levelId": 10, "mem": bit0(0x2249a6),"good": 1, "addr": 0x2249a6, "bit": 0},271: { "levelId": 10, "mem": bit1(0x2249a6),"good": 1, "addr": 0x2249a6, "bit": 1},272: { "levelId": 10, "mem": bit2(0x2249a6),"good": 1, "addr": 0x2249a6, "bit": 2},273: { "levelId": 10, "mem": bit3(0x2249a6),"good": 1, "addr": 0x2249a6, "bit": 3},274: { "levelId": 10, "mem": bit6(0x2249a6),"good": 1, "addr": 0x2249a6, "bit": 6},275: { "levelId": 10, "mem": bit7(0x2249a6),"good": 1, "addr": 0x2249a6, "bit": 7},276: { "levelId": 10, "mem": bit0(0x2249a7),"good": 1, "addr": 0x2249a7, "bit": 0},277: { "levelId": 10, "mem": bit1(0x2249a7),"good": 1, "addr": 0x2249a7, "bit": 1},278: { "levelId": 10, "mem": bit5(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 5},279: { "levelId": 10, "mem": bit6(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 6},280: { "levelId": 10, "mem": bit7(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 7},281: { "levelId": 10, "mem": bit0(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 0},282: { "levelId": 10, "mem": bit1(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 1},283: { "levelId": 10, "mem": bit7(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 7},284: { "levelId": 10, "mem": bit0(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 0},285: { "levelId": 10, "mem": bit1(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 1},286: { "levelId": 10, "mem": bit3(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 3},287: { "levelId": 10, "mem": bit4(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 4},288: { "levelId": 10, "mem": bit5(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 5},289: { "levelId": 10, "mem": bit6(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 6},290: { "levelId": 10, "mem": bit7(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 7},291: { "levelId": 10, "mem": bit4(0x2249a6),"good": 1, "addr": 0x2249a6, "bit": 4},292: { "levelId": 10, "mem": bit5(0x2249a6),"good": 1, "addr": 0x2249a6, "bit": 5},293: { "levelId": 12, "mem": bit2(0x2249a7),"good": 1, "addr": 0x2249a7, "bit": 2},294: { "levelId": 12, "mem": bit3(0x2249a7),"good": 1, "addr": 0x2249a7, "bit": 3},295: { "levelId": 12, "mem": bit4(0x2249a7),"good": 1, "addr": 0x2249a7, "bit": 4},296: { "levelId": 12, "mem": bit5(0x2249a7),"good": 1, "addr": 0x2249a7, "bit": 5},297: { "levelId": 12, "mem": bit6(0x2249a7),"good": 1, "addr": 0x2249a7, "bit": 6},298: { "levelId": 12, "mem": bit7(0x2249a7),"good": 1, "addr": 0x2249a7, "bit": 7},299: { "levelId": 12, "mem": bit0(0x2249a8),"good": 1, "addr": 0x2249a8, "bit": 0},300: { "levelId": 12, "mem": bit1(0x2249a8),"good": 1, "addr": 0x2249a8, "bit": 1},301: { "levelId": 12, "mem": bit2(0x2249a8),"good": 1, "addr": 0x2249a8, "bit": 2},302: { "levelId": 12, "mem": bit3(0x2249a8),"good": 1, "addr": 0x2249a8, "bit": 3},303: { "levelId": 12, "mem": bit4(0x2249a8),"good": 1, "addr": 0x2249a8, "bit": 4},304: { "levelId": 12, "mem": bit5(0x2249a8),"good": 1, "addr": 0x2249a8, "bit": 5},305: { "levelId": 12, "mem": bit6(0x2249a8),"good": 1, "addr": 0x2249a8, "bit": 6},306: { "levelId": 12, "mem": bit7(0x2249a8),"good": 1, "addr": 0x2249a8, "bit": 7},307: { "levelId": 12, "mem": bit0(0x2249a9),"good": 1, "addr": 0x2249a9, "bit": 0},308: { "levelId": 12, "mem": bit1(0x2249a9),"good": 1, "addr": 0x2249a9, "bit": 1},309: { "levelId": 12, "mem": bit2(0x2249a9),"good": 1, "addr": 0x2249a9, "bit": 2},310: { "levelId": 12, "mem": bit3(0x2249a9),"good": 1, "addr": 0x2249a9, "bit": 3},311: { "levelId": 12, "mem": bit4(0x2249a9),"good": 1, "addr": 0x2249a9, "bit": 4},312: { "levelId": 12, "mem": bit5(0x2249a9),"good": 1, "addr": 0x2249a9, "bit": 5},313: { "levelId": 12, "mem": bit6(0x2249a9),"good": 1, "addr": 0x2249a9, "bit": 6},314: { "levelId": 12, "mem": bit1(0x2249aa),"good": 1, "addr": 0x2249aa, "bit": 1},315: { "levelId": 12, "mem": bit2(0x2249aa),"good": 1, "addr": 0x2249aa, "bit": 2},316: { "levelId": 12, "mem": bit2(0x2249ab),"good": 1, "addr": 0x2249ab, "bit": 2},317: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},318: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},319: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},320: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},321: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},322: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},323: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},324: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},325: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},326: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},327: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},328: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},329: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},330: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},331: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},332: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},333: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},334: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},335: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},336: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},337: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},338: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},339: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},340: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},341: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},342: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},343: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},344: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},345: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},346: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},347: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},348: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},349: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},350: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},351: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},352: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},353: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},354: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},355: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},356: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},357: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},358: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},359: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},360: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},361: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},362: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},363: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},364: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},365: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},366: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},367: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},368: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},369: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},370: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},371: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},372: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},373: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},374: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},375: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},376: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},377: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},378: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},379: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},380: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},381: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},382: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},383: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},384: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},385: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},386: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},387: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},388: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},389: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},390: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},391: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},392: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},393: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},394: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},395: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},396: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},397: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},398: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},399: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},400: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},401: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},402: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},403: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},404: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},405: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},406: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},407: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},408: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},409: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},410: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},411: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},412: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},413: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},414: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},415: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},416: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},417: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},418: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},419: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},420: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},421: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},422: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},423: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},424: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},425: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},426: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},427: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},428: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},429: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},430: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},431: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},432: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},433: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},434: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},435: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},436: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},437: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},438: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},439: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},440: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},441: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},442: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},443: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},444: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},445: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},446: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},447: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},448: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},449: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},450: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},451: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},452: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},453: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},454: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},455: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},456: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},457: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},458: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},459: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},460: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},461: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},462: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},463: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},464: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},465: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},466: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},467: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},468: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},469: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},470: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},471: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},472: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},473: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},474: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},475: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},476: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},477: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},478: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},479: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},480: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},481: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},482: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},483: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},484: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},485: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},486: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},487: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},488: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},489: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},490: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},491: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},492: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},493: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},494: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},495: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},496: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},497: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},498: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},499: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},500: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},501: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},502: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},503: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},504: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},505: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},506: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},507: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},508: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},509: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},510: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},511: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},512: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},513: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},514: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},515: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},516: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},517: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},518: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},519: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},520: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},521: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},522: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},523: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},524: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},525: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},526: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},527: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},528: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},529: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},530: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},531: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},532: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},533: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},534: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},535: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},536: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},537: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},538: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},539: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},540: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},541: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},542: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},543: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},544: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},545: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},546: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},547: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},548: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},549: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},550: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},551: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},552: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},553: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},554: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},555: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},556: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},557: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},558: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},559: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},560: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},561: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},562: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},563: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},564: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},565: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},566: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},567: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},568: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},569: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},570: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},571: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},572: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},573: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},574: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},575: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},576: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},577: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},578: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},579: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},580: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},581: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},582: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},583: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},584: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},585: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},586: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},587: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},588: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},589: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},590: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},591: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},592: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},593: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},594: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},595: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},596: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},597: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},598: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},599: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},600: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},601: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},602: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},603: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},604: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},605: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},606: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},607: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},608: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},609: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},610: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},611: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},612: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},613: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},614: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},615: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},616: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},617: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},618: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},619: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},620: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},621: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},622: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},623: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},624: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},625: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},626: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},627: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},628: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},629: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},630: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},631: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},632: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},633: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},634: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},635: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},636: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},637: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},638: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},639: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},640: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},641: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},642: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},643: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},644: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},645: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},646: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},647: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},648: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},649: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},650: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},651: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},652: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},653: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},654: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},655: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},656: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},657: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},658: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},659: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},660: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},661: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},662: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},663: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},664: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},665: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},666: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},667: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},668: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},669: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},670: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},671: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},672: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},673: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},674: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},675: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},676: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},677: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},678: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},679: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},680: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},681: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},682: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},683: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},684: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},685: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},686: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},687: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},688: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},689: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},690: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},691: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},692: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},693: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},694: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},695: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},696: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},697: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},698: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},699: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},700: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},701: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},702: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},703: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},704: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},705: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},706: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},707: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},708: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},709: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},710: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},711: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},712: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},713: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},714: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},715: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},716: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},717: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},718: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},719: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},720: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},721: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},722: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},723: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},724: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},725: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},726: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},727: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},728: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},729: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},730: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},731: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},732: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},733: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},734: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},735: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},736: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},737: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},738: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},739: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},740: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},741: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},742: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},743: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},744: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},745: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},746: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},747: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},748: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},749: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},750: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},751: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},752: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},753: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},754: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},755: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},756: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},757: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},758: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},759: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},760: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},761: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},762: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},763: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},764: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},765: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},766: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},767: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},768: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},769: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},770: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},771: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},772: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},773: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},774: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},775: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},776: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},777: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},778: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},779: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},780: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},781: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},782: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},783: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},784: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},785: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},786: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},787: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},788: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},789: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},790: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},791: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},792: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},793: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},794: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},795: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},796: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},797: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},798: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},799: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},800: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},801: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},802: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},803: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},804: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},805: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},806: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},807: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},808: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},809: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},810: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},811: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},812: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},813: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},814: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},815: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},816: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},817: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},818: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},819: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},820: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},821: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},822: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},823: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},824: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},825: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},826: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},827: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},828: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},829: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},830: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},831: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},832: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},833: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},834: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},835: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},836: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},837: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},838: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},839: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},840: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},841: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},842: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},843: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},844: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},845: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},846: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},847: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},848: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},849: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},850: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},851: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},852: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},853: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},854: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},855: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},856: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},857: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},858: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},859: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},860: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},861: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},862: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},863: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},864: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},865: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},866: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},867: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},868: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},869: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},870: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},871: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},872: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},873: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},874: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},875: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},876: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},877: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},878: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},879: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},880: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},881: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},882: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},883: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},884: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},885: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},886: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},887: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},888: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},889: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},890: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},891: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},892: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},893: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},894: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},895: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},896: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},897: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},898: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},899: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},900: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},901: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},902: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},903: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},904: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},905: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},906: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},907: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},908: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},909: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},910: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},911: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},912: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},913: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},914: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},915: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},916: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},917: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},918: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},919: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},920: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},921: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},922: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},923: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},924: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},925: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},926: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},927: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},928: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},929: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},930: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},931: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},932: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},933: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},934: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},935: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},936: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},937: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},938: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},939: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},940: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},941: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},942: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},943: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},944: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},945: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},946: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},947: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},948: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},949: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},950: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},951: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},952: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},953: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},954: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},955: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},956: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},957: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},958: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},959: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},960: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},961: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},962: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},963: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},964: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},965: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},966: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},967: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},968: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},969: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},970: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},971: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},972: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},973: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},974: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},975: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},976: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},977: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},978: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},979: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},980: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},981: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},982: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},983: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},984: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},985: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},986: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},987: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},988: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},989: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},990: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},991: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},992: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},993: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},994: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},995: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},996: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},997: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},998: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},999: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},1000: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>1: { "levelId": 2, "mem": bit0(0x224988),"good": 1, "addr": 0x224988, "bit": 0},2: { "levelId": 2, "mem": bit1(0x224988),"good": 1, "addr": 0x224988, "bit": 1},3: { "levelId": 2, "mem": bit2(0x224988),"good": 1, "addr": 0x224988, "bit": 2},4: { "levelId": 2, "mem": bit3(0x224988),"good": 1, "addr": 0x224988, "bit": 3},5: { "levelId": 2, "mem": bit4(0x224988),"good": 1, "addr": 0x224988, "bit": 4},6: { "levelId": 2, "mem": bit5(0x224988),"good": 1, "addr": 0x224988, "bit": 5},7: { "levelId": 2, "mem": bit6(0x224988),"good": 1, "addr": 0x224988, "bit": 6},8: { "levelId": 2, "mem": bit7(0x224988),"good": 1, "addr": 0x224988, "bit": 7},9: { "levelId": 2, "mem": bit2(0x224989),"good": 1, "addr": 0x224989, "bit": 2},10: { "levelId": 2, "mem": bit1(0x22498a),"good": 1, "addr": 0x22498a, "bit": 1},11: { "levelId": 2, "mem": bit2(0x22498a),"good": 1, "addr": 0x22498a, "bit": 2},12: { "levelId": 2, "mem": bit3(0x22498a),"good": 1, "addr": 0x22498a, "bit": 3},13: { "levelId": 2, "mem": bit4(0x22498a),"good": 1, "addr": 0x22498a, "bit": 4},14: { "levelId": 2, "mem": bit5(0x22498a),"good": 1, "addr": 0x22498a, "bit": 5},15: { "levelId": 2, "mem": bit6(0x22498a),"good": 1, "addr": 0x22498a, "bit": 6},16: { "levelId": 2, "mem": bit7(0x22498a),"good": 1, "addr": 0x22498a, "bit": 7},17: { "levelId": 2, "mem": bit5(0x22498b),"good": 1, "addr": 0x22498b, "bit": 5},18: { "levelId": 2, "mem": bit6(0x22498b),"good": 1, "addr": 0x22498b, "bit": 6},19: { "levelId": 2, "mem": bit7(0x22498b),"good": 1, "addr": 0x22498b, "bit": 7},20: { "levelId": 2, "mem": bit0(0x22498c),"good": 1, "addr": 0x22498c, "bit": 0},21: { "levelId": 2, "mem": bit1(0x22498c),"good": 1, "addr": 0x22498c, "bit": 1},22: { "levelId": 2, "mem": bit2(0x22498c),"good": 1, "addr": 0x22498c, "bit": 2},23: { "levelId": 2, "mem": bit3(0x22498c),"good": 1, "addr": 0x22498c, "bit": 3},24: { "levelId": 2, "mem": bit4(0x22498c),"good": 1, "addr": 0x22498c, "bit": 4},25: { "levelId": 2, "mem": bit5(0x22498c),"good": 1, "addr": 0x22498c, "bit": 5},26: { "levelId": 2, "mem": bit6(0x22498c),"good": 1, "addr": 0x22498c, "bit": 6},27: { "levelId": 2, "mem": bit7(0x22498c),"good": 1, "addr": 0x22498c, "bit": 7},28: { "levelId": 2, "mem": bit0(0x22498d),"good": 1, "addr": 0x22498d, "bit": 0},29: { "levelId": 2, "mem": bit1(0x22498d),"good": 1, "addr": 0x22498d, "bit": 1},30: { "levelId": 2, "mem": bit2(0x22498d),"good": 1, "addr": 0x22498d, "bit": 2},31: { "levelId": 2, "mem": bit3(0x22498d),"good": 1, "addr": 0x22498d, "bit": 3},32: { "levelId": 2, "mem": bit4(0x22498d),"good": 1, "addr": 0x22498d, "bit": 4},33: { "levelId": 2, "mem": bit5(0x22498d),"good": 1, "addr": 0x22498d, "bit": 5},34: { "levelId": 2, "mem": bit6(0x22498d),"good": 1, "addr": 0x22498d, "bit": 6},35: { "levelId": 2, "mem": bit7(0x22498d),"good": 1, "addr": 0x22498d, "bit": 7},36: { "levelId": 2, "mem": bit0(0x22498e),"good": 1, "addr": 0x22498e, "bit": 0},37: { "levelId": 2, "mem": bit1(0x22498e),"good": 1, "addr": 0x22498e, "bit": 1},38: { "levelId": 5, "mem": bit2(0x22498e),"good": 1, "addr": 0x22498e, "bit": 2},39: { "levelId": 5, "mem": bit3(0x22498e),"good": 1, "addr": 0x22498e, "bit": 3},40: { "levelId": 5, "mem": bit4(0x22498e),"good": 1, "addr": 0x22498e, "bit": 4},41: { "levelId": 5, "mem": bit5(0x22498e),"good": 1, "addr": 0x22498e, "bit": 5},42: { "levelId": 5, "mem": bit6(0x22498e),"good": 1, "addr": 0x22498e, "bit": 6},43: { "levelId": 5, "mem": bit7(0x22498e),"good": 1, "addr": 0x22498e, "bit": 7},44: { "levelId": 5, "mem": bit0(0x22498f),"good": 1, "addr": 0x22498f, "bit": 0},45: { "levelId": 5, "mem": bit1(0x22498f),"good": 1, "addr": 0x22498f, "bit": 1},46: { "levelId": 5, "mem": bit2(0x22498f),"good": 1, "addr": 0x22498f, "bit": 2},47: { "levelId": 5, "mem": bit3(0x22498f),"good": 1, "addr": 0x22498f, "bit": 3},48: { "levelId": 5, "mem": bit4(0x22498f),"good": 1, "addr": 0x22498f, "bit": 4},49: { "levelId": 5, "mem": bit5(0x22498f),"good": 1, "addr": 0x22498f, "bit": 5},50: { "levelId": 5, "mem": bit6(0x22498f),"good": 1, "addr": 0x22498f, "bit": 6},51: { "levelId": 5, "mem": bit7(0x22498f),"good": 1, "addr": 0x22498f, "bit": 7},52: { "levelId": 5, "mem": bit0(0x224990),"good": 1, "addr": 0x224990, "bit": 0},53: { "levelId": 5, "mem": bit1(0x224990),"good": 1, "addr": 0x224990, "bit": 1},54: { "levelId": 5, "mem": bit2(0x224990),"good": 1, "addr": 0x224990, "bit": 2},55: { "levelId": 5, "mem": bit3(0x224990),"good": 1, "addr": 0x224990, "bit": 3},56: { "levelId": 5, "mem": bit4(0x224990),"good": 1, "addr": 0x224990, "bit": 4},57: { "levelId": 5, "mem": bit5(0x224990),"good": 1, "addr": 0x224990, "bit": 5},58: { "levelId": 5, "mem": bit6(0x224990),"good": 1, "addr": 0x224990, "bit": 6},59: { "levelId": 5, "mem": bit7(0x224990),"good": 1, "addr": 0x224990, "bit": 7},60: { "levelId": 5, "mem": bit0(0x224991),"good": 1, "addr": 0x224991, "bit": 0},61: { "levelId": 5, "mem": bit1(0x224991),"good": 1, "addr": 0x224991, "bit": 1},62: { "levelId": 5, "mem": bit2(0x224991),"good": 1, "addr": 0x224991, "bit": 2},63: { "levelId": 5, "mem": bit3(0x224991),"good": 1, "addr": 0x224991, "bit": 3},64: { "levelId": 5, "mem": bit4(0x224991),"good": 1, "addr": 0x224991, "bit": 4},65: { "levelId": 5, "mem": bit5(0x224991),"good": 1, "addr": 0x224991, "bit": 5},66: { "levelId": 5, "mem": bit6(0x224991),"good": 1, "addr": 0x224991, "bit": 6},67: { "levelId": 5, "mem": bit7(0x224991),"good": 1, "addr": 0x224991, "bit": 7},68: { "levelId": 5, "mem": bit0(0x224992),"good": 1, "addr": 0x224992, "bit": 0},69: { "levelId": 5, "mem": bit1(0x224992),"good": 1, "addr": 0x224992, "bit": 1},70: { "levelId": 5, "mem": bit2(0x224992),"good": 1, "addr": 0x224992, "bit": 2},71: { "levelId": 5, "mem": bit3(0x224992),"good": 1, "addr": 0x224992, "bit": 3},72: { "levelId": 5, "mem": bit4(0x224992),"good": 1, "addr": 0x224992, "bit": 4},73: { "levelId": 5, "mem": bit5(0x224992),"good": 1, "addr": 0x224992, "bit": 5},74: { "levelId": 5, "mem": bit6(0x224992),"good": 1, "addr": 0x224992, "bit": 6},75: { "levelId": 5, "mem": bit7(0x224992),"good": 1, "addr": 0x224992, "bit": 7},76: { "levelId": 5, "mem": bit0(0x224993),"good": 1, "addr": 0x224993, "bit": 0},77: { "levelId": 5, "mem": bit1(0x224993),"good": 1, "addr": 0x224993, "bit": 1},78: { "levelId": 5, "mem": bit2(0x224993),"good": 1, "addr": 0x224993, "bit": 2},79: { "levelId": 5, "mem": bit3(0x224993),"good": 1, "addr": 0x224993, "bit": 3},80: { "levelId": 5, "mem": bit4(0x224993),"good": 1, "addr": 0x224993, "bit": 4},81: { "levelId": 5, "mem": bit5(0x224993),"good": 1, "addr": 0x224993, "bit": 5},82: { "levelId": 5, "mem": bit6(0x224993),"good": 1, "addr": 0x224993, "bit": 6},83: { "levelId": 5, "mem": bit7(0x224993),"good": 1, "addr": 0x224993, "bit": 7},84: { "levelId": 5, "mem": bit0(0x224994),"good": 1, "addr": 0x224994, "bit": 0},85: { "levelId": 5, "mem": bit1(0x224994),"good": 1, "addr": 0x224994, "bit": 1},86: { "levelId": 5, "mem": bit2(0x224994),"good": 1, "addr": 0x224994, "bit": 2},87: { "levelId": 5, "mem": bit3(0x224994),"good": 1, "addr": 0x224994, "bit": 3},88: { "levelId": 6, "mem": bit4(0x224994),"good": 1, "addr": 0x224994, "bit": 4},89: { "levelId": 6, "mem": bit5(0x224994),"good": 1, "addr": 0x224994, "bit": 5},90: { "levelId": 6, "mem": bit6(0x224994),"good": 1, "addr": 0x224994, "bit": 6},91: { "levelId": 6, "mem": bit7(0x224994),"good": 1, "addr": 0x224994, "bit": 7},92: { "levelId": 6, "mem": bit0(0x224995),"good": 1, "addr": 0x224995, "bit": 0},93: { "levelId": 6, "mem": bit1(0x224995),"good": 1, "addr": 0x224995, "bit": 1},94: { "levelId": 6, "mem": bit2(0x224995),"good": 1, "addr": 0x224995, "bit": 2},95: { "levelId": 6, "mem": bit3(0x224995),"good": 1, "addr": 0x224995, "bit": 3},96: { "levelId": 6, "mem": bit4(0x224995),"good": 1, "addr": 0x224995, "bit": 4},97: { "levelId": 6, "mem": bit5(0x224995),"good": 1, "addr": 0x224995, "bit": 5},98: { "levelId": 6, "mem": bit6(0x224995),"good": 1, "addr": 0x224995, "bit": 6},99: { "levelId": 6, "mem": bit7(0x224995),"good": 1, "addr": 0x224995, "bit": 7},100: { "levelId": 6, "mem": bit0(0x224996),"good": 1, "addr": 0x224996, "bit": 0},101: { "levelId": 6, "mem": bit1(0x224996),"good": 1, "addr": 0x224996, "bit": 1},102: { "levelId": 6, "mem": bit2(0x224996),"good": 1, "addr": 0x224996, "bit": 2},103: { "levelId": 6, "mem": bit3(0x224996),"good": 1, "addr": 0x224996, "bit": 3},104: { "levelId": 6, "mem": bit4(0x224996),"good": 1, "addr": 0x224996, "bit": 4},105: { "levelId": 6, "mem": bit5(0x224996),"good": 1, "addr": 0x224996, "bit": 5},106: { "levelId": 6, "mem": bit6(0x224996),"good": 1, "addr": 0x224996, "bit": 6},107: { "levelId": 6, "mem": bit7(0x224996),"good": 1, "addr": 0x224996, "bit": 7},108: { "levelId": 6, "mem": bit0(0x224997),"good": 1, "addr": 0x224997, "bit": 0},109: { "levelId": 6, "mem": bit1(0x224997),"good": 1, "addr": 0x224997, "bit": 1},110: { "levelId": 6, "mem": bit2(0x224997),"good": 1, "addr": 0x224997, "bit": 2},111: { "levelId": 6, "mem": bit3(0x224997),"good": 1, "addr": 0x224997, "bit": 3},112: { "levelId": 6, "mem": bit4(0x224997),"good": 1, "addr": 0x224997, "bit": 4},113: { "levelId": 6, "mem": bit5(0x224997),"good": 1, "addr": 0x224997, "bit": 5},114: { "levelId": 6, "mem": bit6(0x224997),"good": 1, "addr": 0x224997, "bit": 6},115: { "levelId": 6, "mem": bit7(0x224997),"good": 1, "addr": 0x224997, "bit": 7},116: { "levelId": 6, "mem": bit0(0x224998),"good": 1, "addr": 0x224998, "bit": 0},117: { "levelId": 6, "mem": bit1(0x224998),"good": 1, "addr": 0x224998, "bit": 1},118: { "levelId": 6, "mem": bit2(0x224998),"good": 1, "addr": 0x224998, "bit": 2},119: { "levelId": 6, "mem": bit3(0x224998),"good": 1, "addr": 0x224998, "bit": 3},120: { "levelId": 6, "mem": bit4(0x224998),"good": 1, "addr": 0x224998, "bit": 4},121: { "levelId": 6, "mem": bit5(0x224998),"good": 1, "addr": 0x224998, "bit": 5},122: { "levelId": 6, "mem": bit6(0x224998),"good": 1, "addr": 0x224998, "bit": 6},123: { "levelId": 6, "mem": bit0(0x224999),"good": 1, "addr": 0x224999, "bit": 0},124: { "levelId": 6, "mem": bit1(0x224999),"good": 1, "addr": 0x224999, "bit": 1},125: { "levelId": 6, "mem": bit2(0x224999),"good": 1, "addr": 0x224999, "bit": 2},126: { "levelId": 6, "mem": bit3(0x224999),"good": 1, "addr": 0x224999, "bit": 3},127: { "levelId": 6, "mem": bit4(0x224999),"good": 1, "addr": 0x224999, "bit": 4},128: { "levelId": 6, "mem": bit5(0x224999),"good": 1, "addr": 0x224999, "bit": 5},129: { "levelId": 6, "mem": bit6(0x224999),"good": 1, "addr": 0x224999, "bit": 6},130: { "levelId": 6, "mem": bit7(0x224999),"good": 1, "addr": 0x224999, "bit": 7},131: { "levelId": 6, "mem": bit0(0x22499a),"good": 1, "addr": 0x22499a, "bit": 0},132: { "levelId": 6, "mem": bit1(0x22499a),"good": 1, "addr": 0x22499a, "bit": 1},133: { "levelId": 6, "mem": bit2(0x22499a),"good": 1, "addr": 0x22499a, "bit": 2},134: { "levelId": 6, "mem": bit3(0x22499a),"good": 1, "addr": 0x22499a, "bit": 3},135: { "levelId": 6, "mem": bit4(0x22499a),"good": 1, "addr": 0x22499a, "bit": 4},136: { "levelId": 6, "mem": bit5(0x22499a),"good": 1, "addr": 0x22499a, "bit": 5},137: { "levelId": 1, "mem": bit3(0x224a36),"good": 1, "addr": 0x224a36, "bit": 3},138: { "levelId": 1, "mem": bit4(0x224a36),"good": 1, "addr": 0x224a36, "bit": 4},139: { "levelId": 1, "mem": bit5(0x224a36),"good": 1, "addr": 0x224a36, "bit": 5},140: { "levelId": 1, "mem": bit6(0x224a36),"good": 1, "addr": 0x224a36, "bit": 6},141: { "levelId": 1, "mem": bit7(0x224a36),"good": 1, "addr": 0x224a36, "bit": 7},142: { "levelId": 6, "mem": bit7(0x224998),"good": 1, "addr": 0x224998, "bit": 7},143: { "levelId": 8, "mem": bit3(0x22499b),"good": 1, "addr": 0x22499b, "bit": 3},144: { "levelId": 8, "mem": bit4(0x22499b),"good": 1, "addr": 0x22499b, "bit": 4},145: { "levelId": 8, "mem": bit5(0x22499b),"good": 1, "addr": 0x22499b, "bit": 5},146: { "levelId": 8, "mem": bit5(0x22499c),"good": 1, "addr": 0x22499c, "bit": 5},147: { "levelId": 8, "mem": bit6(0x22499c),"good": 1, "addr": 0x22499c, "bit": 6},148: { "levelId": 8, "mem": bit7(0x22499c),"good": 1, "addr": 0x22499c, "bit": 7},149: { "levelId": 8, "mem": bit0(0x22499d),"good": 1, "addr": 0x22499d, "bit": 0},150: { "levelId": 8, "mem": bit1(0x22499d),"good": 1, "addr": 0x22499d, "bit": 1},151: { "levelId": 8, "mem": bit2(0x22499d),"good": 1, "addr": 0x22499d, "bit": 2},152: { "levelId": 8, "mem": bit3(0x22499d),"good": 1, "addr": 0x22499d, "bit": 3},153: { "levelId": 8, "mem": bit4(0x22499d),"good": 1, "addr": 0x22499d, "bit": 4},154: { "levelId": 8, "mem": bit5(0x22499d),"good": 1, "addr": 0x22499d, "bit": 5},155: { "levelId": 8, "mem": bit6(0x22499d),"good": 1, "addr": 0x22499d, "bit": 6},156: { "levelId": 8, "mem": bit7(0x22499d),"good": 1, "addr": 0x22499d, "bit": 7},157: { "levelId": 8, "mem": bit0(0x22499e),"good": 1, "addr": 0x22499e, "bit": 0},158: { "levelId": 8, "mem": bit1(0x22499e),"good": 1, "addr": 0x22499e, "bit": 1},159: { "levelId": 8, "mem": bit6(0x22499a),"good": 1, "addr": 0x22499a, "bit": 6},160: { "levelId": 8, "mem": bit7(0x22499a),"good": 1, "addr": 0x22499a, "bit": 7},161: { "levelId": 8, "mem": bit0(0x22499b),"good": 1, "addr": 0x22499b, "bit": 0},162: { "levelId": 8, "mem": bit1(0x22499b),"good": 1, "addr": 0x22499b, "bit": 1},163: { "levelId": 8, "mem": bit2(0x22499b),"good": 1, "addr": 0x22499b, "bit": 2},164: { "levelId": 8, "mem": bit6(0x22499b),"good": 1, "addr": 0x22499b, "bit": 6},165: { "levelId": 8, "mem": bit7(0x22499b),"good": 1, "addr": 0x22499b, "bit": 7},166: { "levelId": 8, "mem": bit0(0x22499c),"good": 1, "addr": 0x22499c, "bit": 0},167: { "levelId": 8, "mem": bit1(0x22499c),"good": 1, "addr": 0x22499c, "bit": 1},168: { "levelId": 8, "mem": bit2(0x22499c),"good": 1, "addr": 0x22499c, "bit": 2},169: { "levelId": 8, "mem": bit3(0x22499c),"good": 1, "addr": 0x22499c, "bit": 3},170: { "levelId": 8, "mem": bit4(0x22499c),"good": 1, "addr": 0x22499c, "bit": 4},171: { "levelId": 8, "mem": bit2(0x22499e),"good": 1, "addr": 0x22499e, "bit": 2},172: { "levelId": 8, "mem": bit3(0x22499e),"good": 1, "addr": 0x22499e, "bit": 3},173: { "levelId": 8, "mem": bit4(0x22499e),"good": 1, "addr": 0x22499e, "bit": 4},174: { "levelId": 8, "mem": bit5(0x22499e),"good": 1, "addr": 0x22499e, "bit": 5},175: { "levelId": 8, "mem": bit6(0x22499e),"good": 1, "addr": 0x22499e, "bit": 6},176: { "levelId": 8, "mem": bit7(0x22499e),"good": 1, "addr": 0x22499e, "bit": 7},177: { "levelId": 8, "mem": bit0(0x22499f),"good": 1, "addr": 0x22499f, "bit": 0},178: { "levelId": 8, "mem": bit1(0x22499f),"good": 1, "addr": 0x22499f, "bit": 1},179: { "levelId": 8, "mem": bit2(0x22499f),"good": 1, "addr": 0x22499f, "bit": 2},180: { "levelId": 8, "mem": bit3(0x22499f),"good": 1, "addr": 0x22499f, "bit": 3},181: { "levelId": 8, "mem": bit4(0x22499f),"good": 1, "addr": 0x22499f, "bit": 4},182: { "levelId": 8, "mem": bit5(0x22499f),"good": 1, "addr": 0x22499f, "bit": 5},183: { "levelId": 8, "mem": bit6(0x22499f),"good": 1, "addr": 0x22499f, "bit": 6},184: { "levelId": 8, "mem": bit7(0x22499f),"good": 1, "addr": 0x22499f, "bit": 7},185: { "levelId": 8, "mem": bit0(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 0},186: { "levelId": 8, "mem": bit1(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 1},187: { "levelId": 8, "mem": bit2(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 2},188: { "levelId": 8, "mem": bit3(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 3},189: { "levelId": 8, "mem": bit4(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 4},190: { "levelId": 8, "mem": bit5(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 5},191: { "levelId": 8, "mem": bit6(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 6},192: { "levelId": 8, "mem": bit7(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 7},193: { "levelId": 10, "mem": bit0(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 0},194: { "levelId": 10, "mem": bit1(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 1},195: { "levelId": 10, "mem": bit2(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 2},196: { "levelId": 10, "mem": bit3(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 3},197: { "levelId": 10, "mem": bit4(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 4},198: { "levelId": 10, "mem": bit2(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 2},199: { "levelId": 10, "mem": bit3(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 3},200: { "levelId": 10, "mem": bit4(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 4},201: { "levelId": 10, "mem": bit5(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 5},202: { "levelId": 10, "mem": bit6(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 6},203: { "levelId": 10, "mem": bit1(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 1},204: { "levelId": 10, "mem": bit5(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 5},205: { "levelId": 10, "mem": bit6(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 6},206: { "levelId": 10, "mem": bit7(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 7},207: { "levelId": 10, "mem": bit0(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 0},208: { "levelId": 10, "mem": bit3(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 3},209: { "levelId": 10, "mem": bit5(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 5},210: { "levelId": 10, "mem": bit6(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 6},211: { "levelId": 10, "mem": bit7(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 7},212: { "levelId": 10, "mem": bit0(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 0},213: { "levelId": 10, "mem": bit1(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 1},214: { "levelId": 10, "mem": bit2(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 2},215: { "levelId": 10, "mem": bit4(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 4},216: { "levelId": 11, "mem": bit6(0x2249e5),"good": 1, "addr": 0x2249e5, "bit": 6},217: { "levelId": 11, "mem": bit7(0x2249e5),"good": 1, "addr": 0x2249e5, "bit": 7},218: { "levelId": 11, "mem": bit0(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 0},219: { "levelId": 11, "mem": bit1(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 1},220: { "levelId": 11, "mem": bit2(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 2},221: { "levelId": 11, "mem": bit3(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 3},222: { "levelId": 11, "mem": bit4(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 4},223: { "levelId": 11, "mem": bit5(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 5},224: { "levelId": 11, "mem": bit6(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 6},225: { "levelId": 11, "mem": bit7(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 7},226: { "levelId": 11, "mem": bit0(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 0},227: { "levelId": 11, "mem": bit1(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 1},228: { "levelId": 11, "mem": bit2(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 2},229: { "levelId": 11, "mem": bit3(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 3},230: { "levelId": 11, "mem": bit4(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 4},231: { "levelId": 11, "mem": bit5(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 5},232: { "levelId": 11, "mem": bit6(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 6},233: { "levelId": 11, "mem": bit7(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 7},234: { "levelId": 11, "mem": bit0(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 0},235: { "levelId": 11, "mem": bit1(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 1},236: { "levelId": 11, "mem": bit2(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 2},237: { "levelId": 11, "mem": bit3(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 3},238: { "levelId": 11, "mem": bit4(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 4},239: { "levelId": 11, "mem": bit5(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 5},240: { "levelId": 11, "mem": bit6(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 6},241: { "levelId": 11, "mem": bit7(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 7},242: { "levelId": 11, "mem": bit0(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 0},243: { "levelId": 11, "mem": bit1(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 1},244: { "levelId": 11, "mem": bit2(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 2},245: { "levelId": 11, "mem": bit3(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 3},246: { "levelId": 11, "mem": bit4(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 4},247: { "levelId": 11, "mem": bit5(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 5},248: { "levelId": 11, "mem": bit6(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 6},249: { "levelId": 11, "mem": bit7(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 7},250: { "levelId": 11, "mem": bit0(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 0},251: { "levelId": 11, "mem": bit1(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 1},252: { "levelId": 11, "mem": bit2(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 2},253: { "levelId": 11, "mem": bit3(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 3},254: { "levelId": 11, "mem": bit4(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 4},255: { "levelId": 11, "mem": bit5(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 5},256: { "levelId": 11, "mem": bit6(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 6},257: { "levelId": 11, "mem": bit7(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 7},258: { "levelId": 11, "mem": bit0(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 0},259: { "levelId": 11, "mem": bit1(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 1},260: { "levelId": 11, "mem": bit2(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 2},261: { "levelId": 11, "mem": bit3(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 3},262: { "levelId": 11, "mem": bit4(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 4},263: { "levelId": 11, "mem": bit5(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 5},264: { "levelId": 11, "mem": bit6(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 6},265: { "levelId": 11, "mem": bit7(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 7},266: { "levelId": 10, "mem": bit2(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 2},267: { "levelId": 10, "mem": bit2(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 2},268: { "levelId": 10, "mem": bit3(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 3},269: { "levelId": 10, "mem": bit4(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 4},270: { "levelId": 10, "mem": bit0(0x2249a6),"good": 1, "addr": 0x2249a6, "bit": 0},271: { "levelId": 10, "mem": bit1(0x2249a6),"good": 1, "addr": 0x2249a6, "bit": 1},272: { "levelId": 10, "mem": bit2(0x2249a6),"good": 1, "addr": 0x2249a6, "bit": 2},273: { "levelId": 10, "mem": bit3(0x2249a6),"good": 1, "addr": 0x2249a6, "bit": 3},274: { "levelId": 10, "mem": bit6(0x2249a6),"good": 1, "addr": 0x2249a6, "bit": 6},275: { "levelId": 10, "mem": bit7(0x2249a6),"good": 1, "addr": 0x2249a6, "bit": 7},276: { "levelId": 10, "mem": bit0(0x2249a7),"good": 1, "addr": 0x2249a7, "bit": 0},277: { "levelId": 10, "mem": bit1(0x2249a7),"good": 1, "addr": 0x2249a7, "bit": 1},278: { "levelId": 10, "mem": bit5(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 5},279: { "levelId": 10, "mem": bit6(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 6},280: { "levelId": 10, "mem": bit7(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 7},281: { "levelId": 10, "mem": bit0(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 0},282: { "levelId": 10, "mem": bit1(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 1},283: { "levelId": 10, "mem": bit7(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 7},284: { "levelId": 10, "mem": bit0(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 0},285: { "levelId": 10, "mem": bit1(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 1},286: { "levelId": 10, "mem": bit3(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 3},287: { "levelId": 10, "mem": bit4(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 4},288: { "levelId": 10, "mem": bit5(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 5},289: { "levelId": 10, "mem": bit6(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 6},290: { "levelId": 10, "mem": bit7(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 7},291: { "levelId": 10, "mem": bit4(0x2249a6),"good": 1, "addr": 0x2249a6, "bit": 4},292: { "levelId": 10, "mem": bit5(0x2249a6),"good": 1, "addr": 0x2249a6, "bit": 5},293: { "levelId": 12, "mem": bit2(0x2249a7),"good": 1, "addr": 0x2249a7, "bit": 2},294: { "levelId": 12, "mem": bit3(0x2249a7),"good": 1, "addr": 0x2249a7, "bit": 3},295: { "levelId": 12, "mem": bit4(0x2249a7),"good": 1, "addr": 0x2249a7, "bit": 4},296: { "levelId": 12, "mem": bit5(0x2249a7),"good": 1, "addr": 0x2249a7, "bit": 5},297: { "levelId": 12, "mem": bit6(0x2249a7),"good": 1, "addr": 0x2249a7, "bit": 6},298: { "levelId": 12, "mem": bit7(0x2249a7),"good": 1, "addr": 0x2249a7, "bit": 7},299: { "levelId": 12, "mem": bit0(0x2249a8),"good": 1, "addr": 0x2249a8, "bit": 0},300: { "levelId": 12, "mem": bit1(0x2249a8),"good": 1, "addr": 0x2249a8, "bit": 1},301: { "levelId": 12, "mem": bit2(0x2249a8),"good": 1, "addr": 0x2249a8, "bit": 2},302: { "levelId": 12, "mem": bit3(0x2249a8),"good": 1, "addr": 0x2249a8, "bit": 3},303: { "levelId": 12, "mem": bit4(0x2249a8),"good": 1, "addr": 0x2249a8, "bit": 4},304: { "levelId": 12, "mem": bit5(0x2249a8),"good": 1, "addr": 0x2249a8, "bit": 5},305: { "levelId": 12, "mem": bit6(0x2249a8),"good": 1, "addr": 0x2249a8, "bit": 6},306: { "levelId": 12, "mem": bit7(0x2249a8),"good": 1, "addr": 0x2249a8, "bit": 7},307: { "levelId": 12, "mem": bit0(0x2249a9),"good": 1, "addr": 0x2249a9, "bit": 0},308: { "levelId": 12, "mem": bit1(0x2249a9),"good": 1, "addr": 0x2249a9, "bit": 1},309: { "levelId": 12, "mem": bit2(0x2249a9),"good": 1, "addr": 0x2249a9, "bit": 2},310: { "levelId": 12, "mem": bit3(0x2249a9),"good": 1, "addr": 0x2249a9, "bit": 3},311: { "levelId": 12, "mem": bit4(0x2249a9),"good": 1, "addr": 0x2249a9, "bit": 4},312: { "levelId": 12, "mem": bit5(0x2249a9),"good": 1, "addr": 0x2249a9, "bit": 5},313: { "levelId": 12, "mem": bit6(0x2249a9),"good": 1, "addr": 0x2249a9, "bit": 6},314: { "levelId": 12, "mem": bit1(0x2249aa),"good": 1, "addr": 0x2249aa, "bit": 1},315: { "levelId": 12, "mem": bit2(0x2249aa),"good": 1, "addr": 0x2249aa, "bit": 2},316: { "levelId": 12, "mem": bit2(0x2249ab),"good": 1, "addr": 0x2249ab, "bit": 2},317: { "levelId": 12, "mem": bit3(0x2249aa),"good": 1, "addr": 0x2249aa, "bit": 3},318: { "levelId": 12, "mem": bit4(0x2249ab),"good": 1, "addr": 0x2249ab, "bit": 4},319: { "levelId": 12, "mem": bit7(0x2249a9),"good": 1, "addr": 0x2249a9, "bit": 7},320: { "levelId": 12, "mem": bit0(0x2249aa),"good": 1, "addr": 0x2249aa, "bit": 0},321: { "levelId": 12, "mem": bit4(0x2249aa),"good": 1, "addr": 0x2249aa, "bit": 4},322: { "levelId": 12, "mem": bit5(0x2249aa),"good": 1, "addr": 0x2249aa, "bit": 5},323: { "levelId": 12, "mem": bit6(0x2249aa),"good": 1, "addr": 0x2249aa, "bit": 6},324: { "levelId": 12, "mem": bit7(0x2249aa),"good": 1, "addr": 0x2249aa, "bit": 7},325: { "levelId": 12, "mem": bit1(0x2249ab),"good": 1, "addr": 0x2249ab, "bit": 1},326: { "levelId": 12, "mem": bit3(0x2249ab),"good": 1, "addr": 0x2249ab, "bit": 3},327: { "levelId": 12, "mem": bit5(0x2249ab),"good": 1, "addr": 0x2249ab, "bit": 5},328: { "levelId": 12, "mem": bit0(0x2249ab),"good": 1, "addr": 0x2249ab, "bit": 0},329: { "levelId": 12, "mem": bit6(0x2249ab),"good": 1, "addr": 0x2249ab, "bit": 6},330: { "levelId": 12, "mem": bit7(0x2249ab),"good": 1, "addr": 0x2249ab, "bit": 7},331: { "levelId": 12, "mem": bit0(0x2249ac),"good": 1, "addr": 0x2249ac, "bit": 0},332: { "levelId": 12, "mem": bit1(0x2249ac),"good": 1, "addr": 0x2249ac, "bit": 1},333: { "levelId": 12, "mem": bit2(0x2249ac),"good": 1, "addr": 0x2249ac, "bit": 2},334: { "levelId": 12, "mem": bit3(0x2249ac),"good": 1, "addr": 0x2249ac, "bit": 3},335: { "levelId": 12, "mem": bit4(0x2249ac),"good": 1, "addr": 0x2249ac, "bit": 4},336: { "levelId": 12, "mem": bit5(0x2249ac),"good": 1, "addr": 0x2249ac, "bit": 5},337: { "levelId": 12, "mem": bit6(0x2249ac),"good": 1, "addr": 0x2249ac, "bit": 6},338: { "levelId": 12, "mem": bit7(0x2249ac),"good": 1, "addr": 0x2249ac, "bit": 7},339: { "levelId": 12, "mem": bit0(0x2249ad),"good": 1, "addr": 0x2249ad, "bit": 0},340: { "levelId": 12, "mem": bit1(0x2249ad),"good": 1, "addr": 0x2249ad, "bit": 1},341: { "levelId": 12, "mem": bit2(0x2249ad),"good": 1, "addr": 0x2249ad, "bit": 2},342: { "levelId": 12, "mem": bit3(0x2249ad),"good": 1, "addr": 0x2249ad, "bit": 3},343: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},344: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},345: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},346: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},347: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},348: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},349: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},350: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},351: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},352: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},353: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},354: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},355: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},356: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},357: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},358: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},359: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},360: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},361: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},362: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},363: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},364: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},365: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},366: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},367: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},368: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},369: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},370: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},371: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},372: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},373: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},374: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},375: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},376: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},377: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},378: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},379: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},380: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},381: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},382: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},383: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},384: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},385: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},386: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},387: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},388: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},389: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},390: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},391: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},392: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},393: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},394: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},395: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},396: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},397: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},398: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},399: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},400: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},401: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},402: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},403: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},404: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},405: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},406: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},407: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},408: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},409: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},410: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},411: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},412: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},413: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},414: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},415: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},416: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},417: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},418: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},419: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},420: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},421: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},422: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},423: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},424: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},425: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},426: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},427: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},428: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},429: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},430: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},431: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},432: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},433: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},434: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},435: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},436: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},437: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},438: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},439: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},440: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},441: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},442: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},443: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},444: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},445: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},446: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},447: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},448: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},449: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},450: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},451: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},452: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},453: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},454: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},455: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},456: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},457: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},458: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},459: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},460: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},461: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},462: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},463: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},464: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},465: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},466: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},467: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},468: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},469: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},470: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},471: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},472: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},473: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},474: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},475: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},476: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},477: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},478: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},479: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},480: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},481: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},482: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},483: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},484: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},485: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},486: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},487: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},488: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},489: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},490: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},491: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},492: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},493: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},494: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},495: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},496: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},497: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},498: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},499: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},500: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},501: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},502: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},503: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},504: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},505: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},506: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},507: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},508: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},509: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},510: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},511: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},512: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},513: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},514: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},515: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},516: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},517: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},518: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},519: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},520: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},521: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},522: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},523: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},524: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},525: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},526: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},527: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},528: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},529: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},530: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},531: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},532: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},533: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},534: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},535: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},536: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},537: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},538: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},539: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},540: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},541: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},542: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},543: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},544: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},545: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},546: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},547: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},548: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},549: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},550: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},551: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},552: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},553: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},554: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},555: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},556: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},557: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},558: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},559: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},560: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},561: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},562: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},563: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},564: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},565: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},566: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},567: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},568: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},569: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},570: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},571: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},572: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},573: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},574: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},575: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},576: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},577: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},578: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},579: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},580: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},581: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},582: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},583: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},584: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},585: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},586: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},587: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},588: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},589: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},590: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},591: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},592: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},593: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},594: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},595: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},596: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},597: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},598: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},599: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},600: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},601: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},602: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},603: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},604: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},605: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},606: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},607: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},608: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},609: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},610: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},611: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},612: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},613: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},614: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},615: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},616: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},617: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},618: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},619: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},620: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},621: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},622: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},623: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},624: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},625: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},626: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},627: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},628: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},629: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},630: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},631: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},632: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},633: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},634: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},635: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},636: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},637: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},638: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},639: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},640: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},641: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},642: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},643: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},644: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},645: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},646: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},647: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},648: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},649: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},650: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},651: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},652: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},653: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},654: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},655: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},656: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},657: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},658: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},659: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},660: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},661: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},662: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},663: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},664: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},665: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},666: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},667: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},668: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},669: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},670: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},671: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},672: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},673: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},674: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},675: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},676: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},677: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},678: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},679: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},680: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},681: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},682: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},683: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},684: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},685: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},686: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},687: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},688: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},689: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},690: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},691: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},692: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},693: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},694: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},695: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},696: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},697: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},698: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},699: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},700: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},701: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},702: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},703: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},704: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},705: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},706: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},707: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},708: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},709: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},710: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},711: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},712: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},713: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},714: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},715: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},716: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},717: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},718: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},719: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},720: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},721: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},722: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},723: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},724: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},725: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},726: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},727: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},728: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},729: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},730: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},731: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},732: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},733: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},734: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},735: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},736: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},737: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},738: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},739: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},740: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},741: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},742: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},743: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},744: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},745: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},746: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},747: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},748: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},749: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},750: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},751: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},752: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},753: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},754: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},755: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},756: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},757: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},758: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},759: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},760: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},761: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},762: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},763: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},764: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},765: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},766: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},767: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},768: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},769: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},770: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},771: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},772: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},773: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},774: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},775: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},776: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},777: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},778: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},779: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},780: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},781: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},782: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},783: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},784: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},785: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},786: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},787: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},788: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},789: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},790: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},791: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},792: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},793: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},794: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},795: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},796: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},797: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},798: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},799: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},800: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},801: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},802: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},803: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},804: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},805: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},806: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},807: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},808: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},809: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},810: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},811: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},812: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},813: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},814: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},815: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},816: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},817: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},818: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},819: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},820: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},821: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},822: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},823: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},824: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},825: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},826: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},827: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},828: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},829: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},830: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},831: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},832: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},833: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},834: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},835: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},836: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},837: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},838: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},839: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},840: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},841: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},842: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},843: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},844: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},845: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},846: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},847: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},848: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},849: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},850: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},851: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},852: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},853: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},854: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},855: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},856: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},857: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},858: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},859: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},860: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},861: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},862: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},863: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},864: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},865: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},866: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},867: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},868: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},869: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},870: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},871: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},872: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},873: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},874: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},875: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},876: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},877: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},878: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},879: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},880: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},881: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},882: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},883: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},884: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},885: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},886: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},887: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},888: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},889: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},890: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},891: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},892: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},893: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},894: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},895: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},896: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},897: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},898: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},899: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},900: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},901: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},902: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},903: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},904: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},905: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},906: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},907: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},908: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},909: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},910: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},911: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},912: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},913: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},914: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},915: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},916: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},917: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},918: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},919: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},920: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},921: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},922: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},923: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},924: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},925: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},926: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},927: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},928: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},929: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},930: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},931: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},932: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},933: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},934: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},935: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},936: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},937: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},938: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},939: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},940: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},941: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},942: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},943: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},944: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},945: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},946: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},947: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},948: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},949: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},950: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},951: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},952: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},953: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},954: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},955: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},956: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},957: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},958: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},959: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},960: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},961: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},962: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},963: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},964: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},965: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},966: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},967: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},968: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},969: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},970: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},971: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},972: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},973: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},974: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},975: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},976: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},977: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},978: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},979: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},980: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},981: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},982: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},983: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},984: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},985: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},986: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},987: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},988: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},989: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},990: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},991: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},992: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},993: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},994: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},995: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},996: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},997: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},998: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},999: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},1000: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0</v>
@@ -7978,7 +8008,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1</v>
@@ -7994,7 +8024,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>2</v>
@@ -8010,7 +8040,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>3</v>
@@ -8026,7 +8056,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>4</v>
@@ -8042,7 +8072,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>5</v>
@@ -8058,7 +8088,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>6</v>
@@ -8074,7 +8104,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>7</v>
@@ -8090,7 +8120,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>2</v>
@@ -8105,7 +8135,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>1</v>
@@ -8120,7 +8150,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>2</v>
@@ -8135,7 +8165,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>3</v>
@@ -8150,7 +8180,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>4</v>
@@ -8165,7 +8195,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>5</v>
@@ -8180,7 +8210,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>6</v>
@@ -8195,7 +8225,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>7</v>
@@ -8210,7 +8240,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>5</v>
@@ -8225,7 +8255,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>6</v>
@@ -8240,7 +8270,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>7</v>
@@ -8255,7 +8285,7 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>0</v>
@@ -8270,7 +8300,7 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="6" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>1</v>
@@ -8285,7 +8315,7 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>2</v>
@@ -8300,7 +8330,7 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>3</v>
@@ -8315,7 +8345,7 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="6" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>4</v>
@@ -8330,7 +8360,7 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="6" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>5</v>
@@ -8345,7 +8375,7 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="6" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>6</v>
@@ -8360,7 +8390,7 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="6" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>7</v>
@@ -8375,7 +8405,7 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="6" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>0</v>
@@ -8390,7 +8420,7 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="6" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>1</v>
@@ -8405,7 +8435,7 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="6" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>2</v>
@@ -8420,7 +8450,7 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="6" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>3</v>
@@ -8435,7 +8465,7 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="6" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>4</v>
@@ -8450,7 +8480,7 @@
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="6" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>5</v>
@@ -8465,7 +8495,7 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="6" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>6</v>
@@ -8480,7 +8510,7 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="6" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>7</v>
@@ -8495,7 +8525,7 @@
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="6" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>0</v>
@@ -8510,7 +8540,7 @@
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="6" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>1</v>
@@ -8525,7 +8555,7 @@
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>2</v>
@@ -8540,7 +8570,7 @@
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>3</v>
@@ -8555,7 +8585,7 @@
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>4</v>
@@ -8570,7 +8600,7 @@
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>5</v>
@@ -8585,7 +8615,7 @@
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>6</v>
@@ -8600,7 +8630,7 @@
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B44" s="0" t="n">
         <v>7</v>
@@ -8615,7 +8645,7 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B45" s="0" t="n">
         <v>0</v>
@@ -8630,7 +8660,7 @@
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B46" s="0" t="n">
         <v>1</v>
@@ -8645,7 +8675,7 @@
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B47" s="0" t="n">
         <v>2</v>
@@ -8660,7 +8690,7 @@
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B48" s="0" t="n">
         <v>3</v>
@@ -8675,7 +8705,7 @@
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B49" s="0" t="n">
         <v>4</v>
@@ -8690,7 +8720,7 @@
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B50" s="0" t="n">
         <v>5</v>
@@ -8705,7 +8735,7 @@
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B51" s="0" t="n">
         <v>6</v>
@@ -8720,7 +8750,7 @@
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B52" s="0" t="n">
         <v>7</v>
@@ -8735,7 +8765,7 @@
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B53" s="0" t="n">
         <v>0</v>
@@ -8750,7 +8780,7 @@
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B54" s="0" t="n">
         <v>1</v>
@@ -8765,7 +8795,7 @@
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B55" s="0" t="n">
         <v>2</v>
@@ -8780,7 +8810,7 @@
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B56" s="0" t="n">
         <v>3</v>
@@ -8795,7 +8825,7 @@
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B57" s="0" t="n">
         <v>4</v>
@@ -8810,7 +8840,7 @@
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B58" s="0" t="n">
         <v>5</v>
@@ -8825,7 +8855,7 @@
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B59" s="0" t="n">
         <v>6</v>
@@ -8840,7 +8870,7 @@
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B60" s="0" t="n">
         <v>7</v>
@@ -8855,7 +8885,7 @@
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B61" s="0" t="n">
         <v>0</v>
@@ -8870,7 +8900,7 @@
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B62" s="0" t="n">
         <v>1</v>
@@ -8885,7 +8915,7 @@
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B63" s="0" t="n">
         <v>2</v>
@@ -8900,7 +8930,7 @@
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B64" s="0" t="n">
         <v>3</v>
@@ -8915,7 +8945,7 @@
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B65" s="0" t="n">
         <v>4</v>
@@ -8930,7 +8960,7 @@
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B66" s="0" t="n">
         <v>5</v>
@@ -8945,7 +8975,7 @@
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B67" s="0" t="n">
         <v>6</v>
@@ -8960,7 +8990,7 @@
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B68" s="0" t="n">
         <v>7</v>
@@ -8975,7 +9005,7 @@
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B69" s="0" t="n">
         <v>0</v>
@@ -8990,7 +9020,7 @@
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B70" s="0" t="n">
         <v>1</v>
@@ -9005,7 +9035,7 @@
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B71" s="0" t="n">
         <v>2</v>
@@ -9020,7 +9050,7 @@
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B72" s="0" t="n">
         <v>3</v>
@@ -9035,7 +9065,7 @@
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B73" s="0" t="n">
         <v>4</v>
@@ -9050,7 +9080,7 @@
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B74" s="0" t="n">
         <v>5</v>
@@ -9065,7 +9095,7 @@
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B75" s="0" t="n">
         <v>6</v>
@@ -9080,7 +9110,7 @@
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B76" s="0" t="n">
         <v>7</v>
@@ -9095,7 +9125,7 @@
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B77" s="0" t="n">
         <v>0</v>
@@ -9110,7 +9140,7 @@
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B78" s="0" t="n">
         <v>1</v>
@@ -9125,7 +9155,7 @@
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B79" s="0" t="n">
         <v>2</v>
@@ -9140,7 +9170,7 @@
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B80" s="0" t="n">
         <v>3</v>
@@ -9155,7 +9185,7 @@
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B81" s="0" t="n">
         <v>4</v>
@@ -9170,7 +9200,7 @@
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B82" s="0" t="n">
         <v>5</v>
@@ -9185,7 +9215,7 @@
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B83" s="0" t="n">
         <v>6</v>
@@ -9200,7 +9230,7 @@
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B84" s="0" t="n">
         <v>7</v>
@@ -9215,7 +9245,7 @@
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="6" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B85" s="0" t="n">
         <v>0</v>
@@ -9230,7 +9260,7 @@
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="6" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B86" s="0" t="n">
         <v>1</v>
@@ -9245,7 +9275,7 @@
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="6" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B87" s="0" t="n">
         <v>2</v>
@@ -9260,7 +9290,7 @@
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="6" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B88" s="0" t="n">
         <v>3</v>
@@ -9275,7 +9305,7 @@
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B89" s="0" t="n">
         <v>4</v>
@@ -9290,7 +9320,7 @@
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B90" s="0" t="n">
         <v>5</v>
@@ -9305,7 +9335,7 @@
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B91" s="0" t="n">
         <v>6</v>
@@ -9320,7 +9350,7 @@
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B92" s="0" t="n">
         <v>7</v>
@@ -9335,7 +9365,7 @@
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B93" s="0" t="n">
         <v>0</v>
@@ -9350,7 +9380,7 @@
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B94" s="0" t="n">
         <v>1</v>
@@ -9365,7 +9395,7 @@
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B95" s="0" t="n">
         <v>2</v>
@@ -9380,7 +9410,7 @@
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B96" s="0" t="n">
         <v>3</v>
@@ -9395,7 +9425,7 @@
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B97" s="0" t="n">
         <v>4</v>
@@ -9410,7 +9440,7 @@
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B98" s="0" t="n">
         <v>5</v>
@@ -9425,7 +9455,7 @@
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B99" s="0" t="n">
         <v>6</v>
@@ -9440,7 +9470,7 @@
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B100" s="0" t="n">
         <v>7</v>
@@ -9455,7 +9485,7 @@
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B101" s="0" t="n">
         <v>0</v>
@@ -9470,7 +9500,7 @@
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B102" s="0" t="n">
         <v>1</v>
@@ -9485,7 +9515,7 @@
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B103" s="0" t="n">
         <v>2</v>
@@ -9500,7 +9530,7 @@
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B104" s="0" t="n">
         <v>3</v>
@@ -9515,7 +9545,7 @@
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B105" s="0" t="n">
         <v>4</v>
@@ -9530,7 +9560,7 @@
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B106" s="0" t="n">
         <v>5</v>
@@ -9545,7 +9575,7 @@
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B107" s="0" t="n">
         <v>6</v>
@@ -9560,7 +9590,7 @@
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B108" s="0" t="n">
         <v>7</v>
@@ -9575,7 +9605,7 @@
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B109" s="0" t="n">
         <v>0</v>
@@ -9590,7 +9620,7 @@
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B110" s="0" t="n">
         <v>1</v>
@@ -9605,7 +9635,7 @@
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B111" s="0" t="n">
         <v>2</v>
@@ -9620,7 +9650,7 @@
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B112" s="0" t="n">
         <v>3</v>
@@ -9635,7 +9665,7 @@
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B113" s="0" t="n">
         <v>4</v>
@@ -9650,7 +9680,7 @@
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B114" s="0" t="n">
         <v>5</v>
@@ -9665,7 +9695,7 @@
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B115" s="0" t="n">
         <v>6</v>
@@ -9680,7 +9710,7 @@
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B116" s="0" t="n">
         <v>7</v>
@@ -9695,7 +9725,7 @@
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B117" s="0" t="n">
         <v>0</v>
@@ -9710,7 +9740,7 @@
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B118" s="0" t="n">
         <v>1</v>
@@ -9725,7 +9755,7 @@
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B119" s="0" t="n">
         <v>2</v>
@@ -9740,7 +9770,7 @@
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B120" s="0" t="n">
         <v>3</v>
@@ -9755,7 +9785,7 @@
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B121" s="0" t="n">
         <v>4</v>
@@ -9770,7 +9800,7 @@
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B122" s="0" t="n">
         <v>5</v>
@@ -9785,7 +9815,7 @@
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B123" s="0" t="n">
         <v>6</v>
@@ -9800,7 +9830,7 @@
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B124" s="0" t="n">
         <v>0</v>
@@ -9815,7 +9845,7 @@
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B125" s="0" t="n">
         <v>1</v>
@@ -9830,7 +9860,7 @@
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B126" s="0" t="n">
         <v>2</v>
@@ -9845,7 +9875,7 @@
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B127" s="0" t="n">
         <v>3</v>
@@ -9860,7 +9890,7 @@
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B128" s="0" t="n">
         <v>4</v>
@@ -9875,7 +9905,7 @@
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B129" s="0" t="n">
         <v>5</v>
@@ -9890,7 +9920,7 @@
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B130" s="0" t="n">
         <v>6</v>
@@ -9905,7 +9935,7 @@
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B131" s="0" t="n">
         <v>7</v>
@@ -9920,7 +9950,7 @@
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B132" s="0" t="n">
         <v>0</v>
@@ -9935,7 +9965,7 @@
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B133" s="0" t="n">
         <v>1</v>
@@ -9950,7 +9980,7 @@
     </row>
     <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B134" s="0" t="n">
         <v>2</v>
@@ -9965,7 +9995,7 @@
     </row>
     <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B135" s="0" t="n">
         <v>3</v>
@@ -9980,7 +10010,7 @@
     </row>
     <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B136" s="0" t="n">
         <v>4</v>
@@ -9995,7 +10025,7 @@
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B137" s="0" t="n">
         <v>5</v>
@@ -10010,7 +10040,7 @@
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="6" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B138" s="0" t="n">
         <v>3</v>
@@ -10025,7 +10055,7 @@
     </row>
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B139" s="0" t="n">
         <v>4</v>
@@ -10040,7 +10070,7 @@
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B140" s="0" t="n">
         <v>5</v>
@@ -10055,7 +10085,7 @@
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B141" s="0" t="n">
         <v>6</v>
@@ -10070,7 +10100,7 @@
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B142" s="0" t="n">
         <v>7</v>
@@ -10085,7 +10115,7 @@
     </row>
     <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B143" s="0" t="n">
         <v>7</v>
@@ -10100,7 +10130,7 @@
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B144" s="0" t="n">
         <v>3</v>
@@ -10115,7 +10145,7 @@
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B145" s="0" t="n">
         <v>4</v>
@@ -10130,7 +10160,7 @@
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B146" s="0" t="n">
         <v>5</v>
@@ -10145,7 +10175,7 @@
     </row>
     <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B147" s="0" t="n">
         <v>5</v>
@@ -10160,7 +10190,7 @@
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B148" s="0" t="n">
         <v>6</v>
@@ -10175,7 +10205,7 @@
     </row>
     <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B149" s="0" t="n">
         <v>7</v>
@@ -10190,7 +10220,7 @@
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B150" s="0" t="n">
         <v>0</v>
@@ -10205,7 +10235,7 @@
     </row>
     <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B151" s="0" t="n">
         <v>1</v>
@@ -10220,7 +10250,7 @@
     </row>
     <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B152" s="0" t="n">
         <v>2</v>
@@ -10235,7 +10265,7 @@
     </row>
     <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B153" s="0" t="n">
         <v>3</v>
@@ -10250,7 +10280,7 @@
     </row>
     <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B154" s="0" t="n">
         <v>4</v>
@@ -10265,7 +10295,7 @@
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B155" s="0" t="n">
         <v>5</v>
@@ -10280,7 +10310,7 @@
     </row>
     <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B156" s="0" t="n">
         <v>6</v>
@@ -10295,7 +10325,7 @@
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B157" s="0" t="n">
         <v>7</v>
@@ -10310,7 +10340,7 @@
     </row>
     <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B158" s="0" t="n">
         <v>0</v>
@@ -10325,7 +10355,7 @@
     </row>
     <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B159" s="0" t="n">
         <v>1</v>
@@ -10340,7 +10370,7 @@
     </row>
     <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B160" s="0" t="n">
         <v>6</v>
@@ -10355,7 +10385,7 @@
     </row>
     <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B161" s="0" t="n">
         <v>7</v>
@@ -10370,7 +10400,7 @@
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B162" s="0" t="n">
         <v>0</v>
@@ -10385,7 +10415,7 @@
     </row>
     <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B163" s="0" t="n">
         <v>1</v>
@@ -10400,7 +10430,7 @@
     </row>
     <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B164" s="0" t="n">
         <v>2</v>
@@ -10415,7 +10445,7 @@
     </row>
     <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B165" s="0" t="n">
         <v>6</v>
@@ -10430,7 +10460,7 @@
     </row>
     <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B166" s="0" t="n">
         <v>7</v>
@@ -10445,7 +10475,7 @@
     </row>
     <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B167" s="0" t="n">
         <v>0</v>
@@ -10460,7 +10490,7 @@
     </row>
     <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B168" s="0" t="n">
         <v>1</v>
@@ -10475,7 +10505,7 @@
     </row>
     <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B169" s="0" t="n">
         <v>2</v>
@@ -10490,7 +10520,7 @@
     </row>
     <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B170" s="0" t="n">
         <v>3</v>
@@ -10505,7 +10535,7 @@
     </row>
     <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B171" s="0" t="n">
         <v>4</v>
@@ -10520,7 +10550,7 @@
     </row>
     <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B172" s="0" t="n">
         <v>2</v>
@@ -10535,7 +10565,7 @@
     </row>
     <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B173" s="0" t="n">
         <v>3</v>
@@ -10550,7 +10580,7 @@
     </row>
     <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B174" s="0" t="n">
         <v>4</v>
@@ -10565,7 +10595,7 @@
     </row>
     <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B175" s="0" t="n">
         <v>5</v>
@@ -10580,7 +10610,7 @@
     </row>
     <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B176" s="0" t="n">
         <v>6</v>
@@ -10595,7 +10625,7 @@
     </row>
     <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B177" s="0" t="n">
         <v>7</v>
@@ -10610,7 +10640,7 @@
     </row>
     <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B178" s="0" t="n">
         <v>0</v>
@@ -10625,7 +10655,7 @@
     </row>
     <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B179" s="0" t="n">
         <v>1</v>
@@ -10640,7 +10670,7 @@
     </row>
     <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B180" s="0" t="n">
         <v>2</v>
@@ -10655,7 +10685,7 @@
     </row>
     <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B181" s="0" t="n">
         <v>3</v>
@@ -10670,7 +10700,7 @@
     </row>
     <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B182" s="0" t="n">
         <v>4</v>
@@ -10685,7 +10715,7 @@
     </row>
     <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B183" s="0" t="n">
         <v>5</v>
@@ -10700,7 +10730,7 @@
     </row>
     <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B184" s="0" t="n">
         <v>6</v>
@@ -10715,7 +10745,7 @@
     </row>
     <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B185" s="0" t="n">
         <v>7</v>
@@ -10730,7 +10760,7 @@
     </row>
     <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B186" s="0" t="n">
         <v>0</v>
@@ -10745,7 +10775,7 @@
     </row>
     <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B187" s="0" t="n">
         <v>1</v>
@@ -10760,7 +10790,7 @@
     </row>
     <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B188" s="0" t="n">
         <v>2</v>
@@ -10775,7 +10805,7 @@
     </row>
     <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B189" s="0" t="n">
         <v>3</v>
@@ -10790,7 +10820,7 @@
     </row>
     <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B190" s="0" t="n">
         <v>4</v>
@@ -10805,7 +10835,7 @@
     </row>
     <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B191" s="0" t="n">
         <v>5</v>
@@ -10820,7 +10850,7 @@
     </row>
     <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B192" s="0" t="n">
         <v>6</v>
@@ -10835,7 +10865,7 @@
     </row>
     <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B193" s="0" t="n">
         <v>7</v>
@@ -10850,7 +10880,7 @@
     </row>
     <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B194" s="0" t="n">
         <v>0</v>
@@ -10865,7 +10895,7 @@
     </row>
     <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B195" s="0" t="n">
         <v>1</v>
@@ -10880,7 +10910,7 @@
     </row>
     <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B196" s="0" t="n">
         <v>2</v>
@@ -10895,7 +10925,7 @@
     </row>
     <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B197" s="0" t="n">
         <v>3</v>
@@ -10910,7 +10940,7 @@
     </row>
     <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B198" s="0" t="n">
         <v>4</v>
@@ -10925,7 +10955,7 @@
     </row>
     <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B199" s="0" t="n">
         <v>2</v>
@@ -10940,7 +10970,7 @@
     </row>
     <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B200" s="0" t="n">
         <v>3</v>
@@ -10955,7 +10985,7 @@
     </row>
     <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B201" s="0" t="n">
         <v>4</v>
@@ -10970,7 +11000,7 @@
     </row>
     <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B202" s="0" t="n">
         <v>5</v>
@@ -10985,7 +11015,7 @@
     </row>
     <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B203" s="0" t="n">
         <v>6</v>
@@ -11000,7 +11030,7 @@
     </row>
     <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B204" s="0" t="n">
         <v>1</v>
@@ -11015,7 +11045,7 @@
     </row>
     <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B205" s="0" t="n">
         <v>5</v>
@@ -11030,7 +11060,7 @@
     </row>
     <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B206" s="0" t="n">
         <v>6</v>
@@ -11045,7 +11075,7 @@
     </row>
     <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B207" s="0" t="n">
         <v>7</v>
@@ -11060,7 +11090,7 @@
     </row>
     <row r="208" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B208" s="0" t="n">
         <v>0</v>
@@ -11075,7 +11105,7 @@
     </row>
     <row r="209" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B209" s="0" t="n">
         <v>3</v>
@@ -11090,7 +11120,7 @@
     </row>
     <row r="210" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B210" s="0" t="n">
         <v>5</v>
@@ -11105,7 +11135,7 @@
     </row>
     <row r="211" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B211" s="0" t="n">
         <v>6</v>
@@ -11120,7 +11150,7 @@
     </row>
     <row r="212" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B212" s="0" t="n">
         <v>7</v>
@@ -11135,7 +11165,7 @@
     </row>
     <row r="213" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B213" s="0" t="n">
         <v>0</v>
@@ -11150,7 +11180,7 @@
     </row>
     <row r="214" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B214" s="0" t="n">
         <v>1</v>
@@ -11165,7 +11195,7 @@
     </row>
     <row r="215" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B215" s="0" t="n">
         <v>2</v>
@@ -11180,7 +11210,7 @@
     </row>
     <row r="216" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B216" s="0" t="n">
         <v>4</v>
@@ -11195,7 +11225,7 @@
     </row>
     <row r="217" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="0" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B217" s="0" t="n">
         <v>6</v>
@@ -11210,7 +11240,7 @@
     </row>
     <row r="218" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="0" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B218" s="0" t="n">
         <v>7</v>
@@ -11225,7 +11255,7 @@
     </row>
     <row r="219" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="0" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B219" s="0" t="n">
         <v>0</v>
@@ -11240,7 +11270,7 @@
     </row>
     <row r="220" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="0" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B220" s="0" t="n">
         <v>1</v>
@@ -11255,7 +11285,7 @@
     </row>
     <row r="221" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="0" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B221" s="0" t="n">
         <v>2</v>
@@ -11270,7 +11300,7 @@
     </row>
     <row r="222" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="0" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B222" s="0" t="n">
         <v>3</v>
@@ -11285,7 +11315,7 @@
     </row>
     <row r="223" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="0" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B223" s="0" t="n">
         <v>4</v>
@@ -11300,7 +11330,7 @@
     </row>
     <row r="224" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="0" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B224" s="0" t="n">
         <v>5</v>
@@ -11315,7 +11345,7 @@
     </row>
     <row r="225" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="0" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B225" s="0" t="n">
         <v>6</v>
@@ -11330,7 +11360,7 @@
     </row>
     <row r="226" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="0" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B226" s="0" t="n">
         <v>7</v>
@@ -11345,7 +11375,7 @@
     </row>
     <row r="227" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="0" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B227" s="0" t="n">
         <v>0</v>
@@ -11360,7 +11390,7 @@
     </row>
     <row r="228" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="0" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B228" s="0" t="n">
         <v>1</v>
@@ -11375,7 +11405,7 @@
     </row>
     <row r="229" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="0" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B229" s="0" t="n">
         <v>2</v>
@@ -11390,7 +11420,7 @@
     </row>
     <row r="230" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="0" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B230" s="0" t="n">
         <v>3</v>
@@ -11405,7 +11435,7 @@
     </row>
     <row r="231" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="0" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B231" s="0" t="n">
         <v>4</v>
@@ -11420,7 +11450,7 @@
     </row>
     <row r="232" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="0" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B232" s="0" t="n">
         <v>5</v>
@@ -11435,7 +11465,7 @@
     </row>
     <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="0" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B233" s="0" t="n">
         <v>6</v>
@@ -11450,7 +11480,7 @@
     </row>
     <row r="234" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="0" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B234" s="0" t="n">
         <v>7</v>
@@ -11465,7 +11495,7 @@
     </row>
     <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="0" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B235" s="0" t="n">
         <v>0</v>
@@ -11480,7 +11510,7 @@
     </row>
     <row r="236" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="0" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B236" s="0" t="n">
         <v>1</v>
@@ -11495,7 +11525,7 @@
     </row>
     <row r="237" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="0" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B237" s="0" t="n">
         <v>2</v>
@@ -11510,7 +11540,7 @@
     </row>
     <row r="238" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="0" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B238" s="0" t="n">
         <v>3</v>
@@ -11525,7 +11555,7 @@
     </row>
     <row r="239" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="0" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B239" s="0" t="n">
         <v>4</v>
@@ -11540,7 +11570,7 @@
     </row>
     <row r="240" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="0" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B240" s="0" t="n">
         <v>5</v>
@@ -11555,7 +11585,7 @@
     </row>
     <row r="241" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="0" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B241" s="0" t="n">
         <v>6</v>
@@ -11570,7 +11600,7 @@
     </row>
     <row r="242" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="0" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B242" s="0" t="n">
         <v>7</v>
@@ -11585,7 +11615,7 @@
     </row>
     <row r="243" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B243" s="0" t="n">
         <v>0</v>
@@ -11600,7 +11630,7 @@
     </row>
     <row r="244" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B244" s="0" t="n">
         <v>1</v>
@@ -11615,7 +11645,7 @@
     </row>
     <row r="245" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B245" s="0" t="n">
         <v>2</v>
@@ -11630,7 +11660,7 @@
     </row>
     <row r="246" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B246" s="0" t="n">
         <v>3</v>
@@ -11645,7 +11675,7 @@
     </row>
     <row r="247" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B247" s="0" t="n">
         <v>4</v>
@@ -11660,7 +11690,7 @@
     </row>
     <row r="248" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B248" s="0" t="n">
         <v>5</v>
@@ -11675,7 +11705,7 @@
     </row>
     <row r="249" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B249" s="0" t="n">
         <v>6</v>
@@ -11690,7 +11720,7 @@
     </row>
     <row r="250" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B250" s="0" t="n">
         <v>7</v>
@@ -11705,7 +11735,7 @@
     </row>
     <row r="251" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B251" s="0" t="n">
         <v>0</v>
@@ -11720,7 +11750,7 @@
     </row>
     <row r="252" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B252" s="0" t="n">
         <v>1</v>
@@ -11735,7 +11765,7 @@
     </row>
     <row r="253" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B253" s="0" t="n">
         <v>2</v>
@@ -11750,7 +11780,7 @@
     </row>
     <row r="254" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B254" s="0" t="n">
         <v>3</v>
@@ -11765,7 +11795,7 @@
     </row>
     <row r="255" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B255" s="0" t="n">
         <v>4</v>
@@ -11780,7 +11810,7 @@
     </row>
     <row r="256" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B256" s="0" t="n">
         <v>5</v>
@@ -11795,7 +11825,7 @@
     </row>
     <row r="257" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B257" s="0" t="n">
         <v>6</v>
@@ -11810,7 +11840,7 @@
     </row>
     <row r="258" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B258" s="0" t="n">
         <v>7</v>
@@ -11825,7 +11855,7 @@
     </row>
     <row r="259" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B259" s="0" t="n">
         <v>0</v>
@@ -11840,7 +11870,7 @@
     </row>
     <row r="260" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B260" s="0" t="n">
         <v>1</v>
@@ -11855,7 +11885,7 @@
     </row>
     <row r="261" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B261" s="0" t="n">
         <v>2</v>
@@ -11870,7 +11900,7 @@
     </row>
     <row r="262" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B262" s="0" t="n">
         <v>3</v>
@@ -11885,7 +11915,7 @@
     </row>
     <row r="263" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B263" s="0" t="n">
         <v>4</v>
@@ -11900,7 +11930,7 @@
     </row>
     <row r="264" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B264" s="0" t="n">
         <v>5</v>
@@ -11915,7 +11945,7 @@
     </row>
     <row r="265" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B265" s="0" t="n">
         <v>6</v>
@@ -11930,7 +11960,7 @@
     </row>
     <row r="266" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B266" s="0" t="n">
         <v>7</v>
@@ -11945,7 +11975,7 @@
     </row>
     <row r="267" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B267" s="0" t="n">
         <v>2</v>
@@ -11960,7 +11990,7 @@
     </row>
     <row r="268" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B268" s="0" t="n">
         <v>2</v>
@@ -11975,7 +12005,7 @@
     </row>
     <row r="269" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B269" s="0" t="n">
         <v>3</v>
@@ -11990,7 +12020,7 @@
     </row>
     <row r="270" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B270" s="0" t="n">
         <v>4</v>
@@ -12005,7 +12035,7 @@
     </row>
     <row r="271" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B271" s="0" t="n">
         <v>0</v>
@@ -12020,7 +12050,7 @@
     </row>
     <row r="272" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B272" s="0" t="n">
         <v>1</v>
@@ -12035,7 +12065,7 @@
     </row>
     <row r="273" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B273" s="0" t="n">
         <v>2</v>
@@ -12050,7 +12080,7 @@
     </row>
     <row r="274" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A274" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B274" s="0" t="n">
         <v>3</v>
@@ -12065,7 +12095,7 @@
     </row>
     <row r="275" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B275" s="0" t="n">
         <v>6</v>
@@ -12080,7 +12110,7 @@
     </row>
     <row r="276" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B276" s="0" t="n">
         <v>7</v>
@@ -12095,7 +12125,7 @@
     </row>
     <row r="277" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="0" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B277" s="0" t="n">
         <v>0</v>
@@ -12110,7 +12140,7 @@
     </row>
     <row r="278" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="0" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B278" s="0" t="n">
         <v>1</v>
@@ -12125,7 +12155,7 @@
     </row>
     <row r="279" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A279" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B279" s="0" t="n">
         <v>5</v>
@@ -12140,7 +12170,7 @@
     </row>
     <row r="280" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B280" s="0" t="n">
         <v>6</v>
@@ -12155,7 +12185,7 @@
     </row>
     <row r="281" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A281" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B281" s="0" t="n">
         <v>7</v>
@@ -12170,7 +12200,7 @@
     </row>
     <row r="282" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B282" s="0" t="n">
         <v>0</v>
@@ -12185,7 +12215,7 @@
     </row>
     <row r="283" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A283" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B283" s="0" t="n">
         <v>1</v>
@@ -12200,7 +12230,7 @@
     </row>
     <row r="284" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B284" s="0" t="n">
         <v>7</v>
@@ -12215,7 +12245,7 @@
     </row>
     <row r="285" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B285" s="0" t="n">
         <v>0</v>
@@ -12230,7 +12260,7 @@
     </row>
     <row r="286" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B286" s="0" t="n">
         <v>1</v>
@@ -12245,7 +12275,7 @@
     </row>
     <row r="287" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B287" s="0" t="n">
         <v>3</v>
@@ -12260,7 +12290,7 @@
     </row>
     <row r="288" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A288" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B288" s="0" t="n">
         <v>4</v>
@@ -12275,7 +12305,7 @@
     </row>
     <row r="289" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B289" s="0" t="n">
         <v>5</v>
@@ -12290,7 +12320,7 @@
     </row>
     <row r="290" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B290" s="0" t="n">
         <v>6</v>
@@ -12305,7 +12335,7 @@
     </row>
     <row r="291" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A291" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B291" s="0" t="n">
         <v>7</v>
@@ -12320,7 +12350,7 @@
     </row>
     <row r="292" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B292" s="0" t="n">
         <v>4</v>
@@ -12335,7 +12365,7 @@
     </row>
     <row r="293" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A293" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B293" s="0" t="n">
         <v>5</v>
@@ -12350,7 +12380,7 @@
     </row>
     <row r="294" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A294" s="0" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B294" s="0" t="n">
         <v>2</v>
@@ -12365,7 +12395,7 @@
     </row>
     <row r="295" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A295" s="0" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B295" s="0" t="n">
         <v>3</v>
@@ -12380,7 +12410,7 @@
     </row>
     <row r="296" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A296" s="0" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B296" s="0" t="n">
         <v>4</v>
@@ -12395,7 +12425,7 @@
     </row>
     <row r="297" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A297" s="0" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B297" s="0" t="n">
         <v>5</v>
@@ -12410,7 +12440,7 @@
     </row>
     <row r="298" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A298" s="0" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B298" s="0" t="n">
         <v>6</v>
@@ -12425,7 +12455,7 @@
     </row>
     <row r="299" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A299" s="0" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B299" s="0" t="n">
         <v>7</v>
@@ -12440,7 +12470,7 @@
     </row>
     <row r="300" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="0" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B300" s="0" t="n">
         <v>0</v>
@@ -12455,7 +12485,7 @@
     </row>
     <row r="301" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A301" s="0" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B301" s="0" t="n">
         <v>1</v>
@@ -12470,7 +12500,7 @@
     </row>
     <row r="302" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A302" s="0" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B302" s="0" t="n">
         <v>2</v>
@@ -12485,7 +12515,7 @@
     </row>
     <row r="303" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A303" s="0" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B303" s="0" t="n">
         <v>3</v>
@@ -12500,7 +12530,7 @@
     </row>
     <row r="304" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A304" s="0" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B304" s="0" t="n">
         <v>4</v>
@@ -12515,7 +12545,7 @@
     </row>
     <row r="305" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A305" s="0" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B305" s="0" t="n">
         <v>5</v>
@@ -12530,7 +12560,7 @@
     </row>
     <row r="306" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A306" s="0" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B306" s="0" t="n">
         <v>6</v>
@@ -12545,7 +12575,7 @@
     </row>
     <row r="307" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A307" s="0" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B307" s="0" t="n">
         <v>7</v>
@@ -12560,7 +12590,7 @@
     </row>
     <row r="308" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A308" s="0" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B308" s="0" t="n">
         <v>0</v>
@@ -12575,7 +12605,7 @@
     </row>
     <row r="309" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A309" s="0" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B309" s="0" t="n">
         <v>1</v>
@@ -12590,7 +12620,7 @@
     </row>
     <row r="310" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A310" s="0" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B310" s="0" t="n">
         <v>2</v>
@@ -12605,7 +12635,7 @@
     </row>
     <row r="311" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A311" s="0" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B311" s="0" t="n">
         <v>3</v>
@@ -12620,7 +12650,7 @@
     </row>
     <row r="312" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="0" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B312" s="0" t="n">
         <v>4</v>
@@ -12635,7 +12665,7 @@
     </row>
     <row r="313" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A313" s="0" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B313" s="0" t="n">
         <v>5</v>
@@ -12650,7 +12680,7 @@
     </row>
     <row r="314" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A314" s="0" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B314" s="0" t="n">
         <v>6</v>
@@ -12665,7 +12695,7 @@
     </row>
     <row r="315" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A315" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B315" s="0" t="n">
         <v>1</v>
@@ -12680,7 +12710,7 @@
     </row>
     <row r="316" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A316" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B316" s="0" t="n">
         <v>2</v>
@@ -12695,7 +12725,7 @@
     </row>
     <row r="317" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A317" s="0" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B317" s="0" t="n">
         <v>2</v>
@@ -12709,237 +12739,393 @@
       </c>
     </row>
     <row r="318" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A318" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="B318" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="C318" s="4" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="D318" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C318, Levels!B:B, 0), 1, 1)),", ",IF(A318 &lt;&gt; "", """mem"": bit" &amp; B318 &amp; "(" &amp; A318 &amp; "),", ""),"""good"": ",IF(A318 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A318 &lt;&gt; "", A318, -1),", ""bit"": ",IF(B318 &lt;&gt; "", B318, -1),"},")</f>
-        <v>317: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>317: { "levelId": 12, "mem": bit3(0x2249aa),"good": 1, "addr": 0x2249aa, "bit": 3},</v>
       </c>
     </row>
     <row r="319" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A319" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="B319" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="C319" s="4" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="D319" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C319, Levels!B:B, 0), 1, 1)),", ",IF(A319 &lt;&gt; "", """mem"": bit" &amp; B319 &amp; "(" &amp; A319 &amp; "),", ""),"""good"": ",IF(A319 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A319 &lt;&gt; "", A319, -1),", ""bit"": ",IF(B319 &lt;&gt; "", B319, -1),"},")</f>
-        <v>318: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>318: { "levelId": 12, "mem": bit4(0x2249ab),"good": 1, "addr": 0x2249ab, "bit": 4},</v>
       </c>
     </row>
     <row r="320" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A320" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="B320" s="0" t="n">
+        <v>7</v>
+      </c>
       <c r="C320" s="4" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="D320" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C320, Levels!B:B, 0), 1, 1)),", ",IF(A320 &lt;&gt; "", """mem"": bit" &amp; B320 &amp; "(" &amp; A320 &amp; "),", ""),"""good"": ",IF(A320 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A320 &lt;&gt; "", A320, -1),", ""bit"": ",IF(B320 &lt;&gt; "", B320, -1),"},")</f>
-        <v>319: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>319: { "levelId": 12, "mem": bit7(0x2249a9),"good": 1, "addr": 0x2249a9, "bit": 7},</v>
       </c>
     </row>
     <row r="321" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A321" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="B321" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="C321" s="4" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="D321" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C321, Levels!B:B, 0), 1, 1)),", ",IF(A321 &lt;&gt; "", """mem"": bit" &amp; B321 &amp; "(" &amp; A321 &amp; "),", ""),"""good"": ",IF(A321 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A321 &lt;&gt; "", A321, -1),", ""bit"": ",IF(B321 &lt;&gt; "", B321, -1),"},")</f>
-        <v>320: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>320: { "levelId": 12, "mem": bit0(0x2249aa),"good": 1, "addr": 0x2249aa, "bit": 0},</v>
       </c>
     </row>
     <row r="322" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A322" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="B322" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="C322" s="4" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="D322" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C322, Levels!B:B, 0), 1, 1)),", ",IF(A322 &lt;&gt; "", """mem"": bit" &amp; B322 &amp; "(" &amp; A322 &amp; "),", ""),"""good"": ",IF(A322 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A322 &lt;&gt; "", A322, -1),", ""bit"": ",IF(B322 &lt;&gt; "", B322, -1),"},")</f>
-        <v>321: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>321: { "levelId": 12, "mem": bit4(0x2249aa),"good": 1, "addr": 0x2249aa, "bit": 4},</v>
       </c>
     </row>
     <row r="323" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A323" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="B323" s="0" t="n">
+        <v>5</v>
+      </c>
       <c r="C323" s="4" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="D323" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C323, Levels!B:B, 0), 1, 1)),", ",IF(A323 &lt;&gt; "", """mem"": bit" &amp; B323 &amp; "(" &amp; A323 &amp; "),", ""),"""good"": ",IF(A323 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A323 &lt;&gt; "", A323, -1),", ""bit"": ",IF(B323 &lt;&gt; "", B323, -1),"},")</f>
-        <v>322: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>322: { "levelId": 12, "mem": bit5(0x2249aa),"good": 1, "addr": 0x2249aa, "bit": 5},</v>
       </c>
     </row>
     <row r="324" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A324" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="B324" s="0" t="n">
+        <v>6</v>
+      </c>
       <c r="C324" s="4" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="D324" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C324, Levels!B:B, 0), 1, 1)),", ",IF(A324 &lt;&gt; "", """mem"": bit" &amp; B324 &amp; "(" &amp; A324 &amp; "),", ""),"""good"": ",IF(A324 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A324 &lt;&gt; "", A324, -1),", ""bit"": ",IF(B324 &lt;&gt; "", B324, -1),"},")</f>
-        <v>323: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>323: { "levelId": 12, "mem": bit6(0x2249aa),"good": 1, "addr": 0x2249aa, "bit": 6},</v>
       </c>
     </row>
     <row r="325" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A325" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="B325" s="0" t="n">
+        <v>7</v>
+      </c>
       <c r="C325" s="4" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="D325" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C325, Levels!B:B, 0), 1, 1)),", ",IF(A325 &lt;&gt; "", """mem"": bit" &amp; B325 &amp; "(" &amp; A325 &amp; "),", ""),"""good"": ",IF(A325 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A325 &lt;&gt; "", A325, -1),", ""bit"": ",IF(B325 &lt;&gt; "", B325, -1),"},")</f>
-        <v>324: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>324: { "levelId": 12, "mem": bit7(0x2249aa),"good": 1, "addr": 0x2249aa, "bit": 7},</v>
       </c>
     </row>
     <row r="326" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A326" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="B326" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="C326" s="4" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="D326" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C326, Levels!B:B, 0), 1, 1)),", ",IF(A326 &lt;&gt; "", """mem"": bit" &amp; B326 &amp; "(" &amp; A326 &amp; "),", ""),"""good"": ",IF(A326 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A326 &lt;&gt; "", A326, -1),", ""bit"": ",IF(B326 &lt;&gt; "", B326, -1),"},")</f>
-        <v>325: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>325: { "levelId": 12, "mem": bit1(0x2249ab),"good": 1, "addr": 0x2249ab, "bit": 1},</v>
       </c>
     </row>
     <row r="327" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A327" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="B327" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="C327" s="4" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="D327" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C327, Levels!B:B, 0), 1, 1)),", ",IF(A327 &lt;&gt; "", """mem"": bit" &amp; B327 &amp; "(" &amp; A327 &amp; "),", ""),"""good"": ",IF(A327 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A327 &lt;&gt; "", A327, -1),", ""bit"": ",IF(B327 &lt;&gt; "", B327, -1),"},")</f>
-        <v>326: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>326: { "levelId": 12, "mem": bit3(0x2249ab),"good": 1, "addr": 0x2249ab, "bit": 3},</v>
       </c>
     </row>
     <row r="328" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A328" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="B328" s="0" t="n">
+        <v>5</v>
+      </c>
       <c r="C328" s="4" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="D328" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C328, Levels!B:B, 0), 1, 1)),", ",IF(A328 &lt;&gt; "", """mem"": bit" &amp; B328 &amp; "(" &amp; A328 &amp; "),", ""),"""good"": ",IF(A328 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A328 &lt;&gt; "", A328, -1),", ""bit"": ",IF(B328 &lt;&gt; "", B328, -1),"},")</f>
-        <v>327: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>327: { "levelId": 12, "mem": bit5(0x2249ab),"good": 1, "addr": 0x2249ab, "bit": 5},</v>
       </c>
     </row>
     <row r="329" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A329" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="B329" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="C329" s="4" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="D329" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C329, Levels!B:B, 0), 1, 1)),", ",IF(A329 &lt;&gt; "", """mem"": bit" &amp; B329 &amp; "(" &amp; A329 &amp; "),", ""),"""good"": ",IF(A329 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A329 &lt;&gt; "", A329, -1),", ""bit"": ",IF(B329 &lt;&gt; "", B329, -1),"},")</f>
-        <v>328: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>328: { "levelId": 12, "mem": bit0(0x2249ab),"good": 1, "addr": 0x2249ab, "bit": 0},</v>
       </c>
     </row>
     <row r="330" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A330" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="B330" s="0" t="n">
+        <v>6</v>
+      </c>
       <c r="C330" s="4" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="D330" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C330, Levels!B:B, 0), 1, 1)),", ",IF(A330 &lt;&gt; "", """mem"": bit" &amp; B330 &amp; "(" &amp; A330 &amp; "),", ""),"""good"": ",IF(A330 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A330 &lt;&gt; "", A330, -1),", ""bit"": ",IF(B330 &lt;&gt; "", B330, -1),"},")</f>
-        <v>329: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>329: { "levelId": 12, "mem": bit6(0x2249ab),"good": 1, "addr": 0x2249ab, "bit": 6},</v>
       </c>
     </row>
     <row r="331" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A331" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="B331" s="0" t="n">
+        <v>7</v>
+      </c>
       <c r="C331" s="4" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="D331" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C331, Levels!B:B, 0), 1, 1)),", ",IF(A331 &lt;&gt; "", """mem"": bit" &amp; B331 &amp; "(" &amp; A331 &amp; "),", ""),"""good"": ",IF(A331 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A331 &lt;&gt; "", A331, -1),", ""bit"": ",IF(B331 &lt;&gt; "", B331, -1),"},")</f>
-        <v>330: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>330: { "levelId": 12, "mem": bit7(0x2249ab),"good": 1, "addr": 0x2249ab, "bit": 7},</v>
       </c>
     </row>
     <row r="332" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A332" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="B332" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="C332" s="4" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="D332" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C332, Levels!B:B, 0), 1, 1)),", ",IF(A332 &lt;&gt; "", """mem"": bit" &amp; B332 &amp; "(" &amp; A332 &amp; "),", ""),"""good"": ",IF(A332 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A332 &lt;&gt; "", A332, -1),", ""bit"": ",IF(B332 &lt;&gt; "", B332, -1),"},")</f>
-        <v>331: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>331: { "levelId": 12, "mem": bit0(0x2249ac),"good": 1, "addr": 0x2249ac, "bit": 0},</v>
       </c>
     </row>
     <row r="333" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A333" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="B333" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="C333" s="4" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="D333" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C333, Levels!B:B, 0), 1, 1)),", ",IF(A333 &lt;&gt; "", """mem"": bit" &amp; B333 &amp; "(" &amp; A333 &amp; "),", ""),"""good"": ",IF(A333 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A333 &lt;&gt; "", A333, -1),", ""bit"": ",IF(B333 &lt;&gt; "", B333, -1),"},")</f>
-        <v>332: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>332: { "levelId": 12, "mem": bit1(0x2249ac),"good": 1, "addr": 0x2249ac, "bit": 1},</v>
       </c>
     </row>
     <row r="334" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A334" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="B334" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="C334" s="4" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="D334" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C334, Levels!B:B, 0), 1, 1)),", ",IF(A334 &lt;&gt; "", """mem"": bit" &amp; B334 &amp; "(" &amp; A334 &amp; "),", ""),"""good"": ",IF(A334 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A334 &lt;&gt; "", A334, -1),", ""bit"": ",IF(B334 &lt;&gt; "", B334, -1),"},")</f>
-        <v>333: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>333: { "levelId": 12, "mem": bit2(0x2249ac),"good": 1, "addr": 0x2249ac, "bit": 2},</v>
       </c>
     </row>
     <row r="335" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A335" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="B335" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="C335" s="4" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="D335" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C335, Levels!B:B, 0), 1, 1)),", ",IF(A335 &lt;&gt; "", """mem"": bit" &amp; B335 &amp; "(" &amp; A335 &amp; "),", ""),"""good"": ",IF(A335 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A335 &lt;&gt; "", A335, -1),", ""bit"": ",IF(B335 &lt;&gt; "", B335, -1),"},")</f>
-        <v>334: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>334: { "levelId": 12, "mem": bit3(0x2249ac),"good": 1, "addr": 0x2249ac, "bit": 3},</v>
       </c>
     </row>
     <row r="336" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A336" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="B336" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="C336" s="4" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="D336" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C336, Levels!B:B, 0), 1, 1)),", ",IF(A336 &lt;&gt; "", """mem"": bit" &amp; B336 &amp; "(" &amp; A336 &amp; "),", ""),"""good"": ",IF(A336 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A336 &lt;&gt; "", A336, -1),", ""bit"": ",IF(B336 &lt;&gt; "", B336, -1),"},")</f>
-        <v>335: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>335: { "levelId": 12, "mem": bit4(0x2249ac),"good": 1, "addr": 0x2249ac, "bit": 4},</v>
       </c>
     </row>
     <row r="337" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A337" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="B337" s="0" t="n">
+        <v>5</v>
+      </c>
       <c r="C337" s="4" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="D337" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C337, Levels!B:B, 0), 1, 1)),", ",IF(A337 &lt;&gt; "", """mem"": bit" &amp; B337 &amp; "(" &amp; A337 &amp; "),", ""),"""good"": ",IF(A337 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A337 &lt;&gt; "", A337, -1),", ""bit"": ",IF(B337 &lt;&gt; "", B337, -1),"},")</f>
-        <v>336: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>336: { "levelId": 12, "mem": bit5(0x2249ac),"good": 1, "addr": 0x2249ac, "bit": 5},</v>
       </c>
     </row>
     <row r="338" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A338" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="B338" s="0" t="n">
+        <v>6</v>
+      </c>
       <c r="C338" s="4" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="D338" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C338, Levels!B:B, 0), 1, 1)),", ",IF(A338 &lt;&gt; "", """mem"": bit" &amp; B338 &amp; "(" &amp; A338 &amp; "),", ""),"""good"": ",IF(A338 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A338 &lt;&gt; "", A338, -1),", ""bit"": ",IF(B338 &lt;&gt; "", B338, -1),"},")</f>
-        <v>337: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>337: { "levelId": 12, "mem": bit6(0x2249ac),"good": 1, "addr": 0x2249ac, "bit": 6},</v>
       </c>
     </row>
     <row r="339" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A339" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="B339" s="0" t="n">
+        <v>7</v>
+      </c>
       <c r="C339" s="4" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="D339" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C339, Levels!B:B, 0), 1, 1)),", ",IF(A339 &lt;&gt; "", """mem"": bit" &amp; B339 &amp; "(" &amp; A339 &amp; "),", ""),"""good"": ",IF(A339 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A339 &lt;&gt; "", A339, -1),", ""bit"": ",IF(B339 &lt;&gt; "", B339, -1),"},")</f>
-        <v>338: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>338: { "levelId": 12, "mem": bit7(0x2249ac),"good": 1, "addr": 0x2249ac, "bit": 7},</v>
       </c>
     </row>
     <row r="340" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A340" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="B340" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="C340" s="4" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="D340" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C340, Levels!B:B, 0), 1, 1)),", ",IF(A340 &lt;&gt; "", """mem"": bit" &amp; B340 &amp; "(" &amp; A340 &amp; "),", ""),"""good"": ",IF(A340 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A340 &lt;&gt; "", A340, -1),", ""bit"": ",IF(B340 &lt;&gt; "", B340, -1),"},")</f>
-        <v>339: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>339: { "levelId": 12, "mem": bit0(0x2249ad),"good": 1, "addr": 0x2249ad, "bit": 0},</v>
       </c>
     </row>
     <row r="341" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A341" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="B341" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="C341" s="4" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="D341" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C341, Levels!B:B, 0), 1, 1)),", ",IF(A341 &lt;&gt; "", """mem"": bit" &amp; B341 &amp; "(" &amp; A341 &amp; "),", ""),"""good"": ",IF(A341 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A341 &lt;&gt; "", A341, -1),", ""bit"": ",IF(B341 &lt;&gt; "", B341, -1),"},")</f>
-        <v>340: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>340: { "levelId": 12, "mem": bit1(0x2249ad),"good": 1, "addr": 0x2249ad, "bit": 1},</v>
       </c>
     </row>
     <row r="342" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A342" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="B342" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="C342" s="4" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="D342" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C342, Levels!B:B, 0), 1, 1)),", ",IF(A342 &lt;&gt; "", """mem"": bit" &amp; B342 &amp; "(" &amp; A342 &amp; "),", ""),"""good"": ",IF(A342 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A342 &lt;&gt; "", A342, -1),", ""bit"": ",IF(B342 &lt;&gt; "", B342, -1),"},")</f>
-        <v>341: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>341: { "levelId": 12, "mem": bit2(0x2249ad),"good": 1, "addr": 0x2249ad, "bit": 2},</v>
       </c>
     </row>
     <row r="343" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A343" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="B343" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="C343" s="4" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="D343" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C343, Levels!B:B, 0), 1, 1)),", ",IF(A343 &lt;&gt; "", """mem"": bit" &amp; B343 &amp; "(" &amp; A343 &amp; "),", ""),"""good"": ",IF(A343 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A343 &lt;&gt; "", A343, -1),", ""bit"": ",IF(B343 &lt;&gt; "", B343, -1),"},")</f>
-        <v>342: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>342: { "levelId": 12, "mem": bit3(0x2249ad),"good": 1, "addr": 0x2249ad, "bit": 3},</v>
       </c>
     </row>
     <row r="344" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18891,10 +19077,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="B11" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C31" activeCellId="0" sqref="C31"/>
+      <selection pane="bottomLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.93"/>
@@ -18904,13 +19090,13 @@
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>4</v>
@@ -18920,12 +19106,12 @@
       </c>
       <c r="H1" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D2:D81)</f>
-        <v>1: { "levelId": 1, "mem": bit7(0x2249f0),"good": 1},2: { "levelId": 2, "mem": bit0(0x2249f1),"good": 1},3: { "levelId": 2, "mem": bit1(0x2249f1),"good": 1},4: { "levelId": 2, "mem": bit5(0x2249f1),"good": 1},5: { "levelId": 2, "mem": bit6(0x2249f1),"good": 1},6: { "levelId": 1, "mem": bit7(0x2249f1),"good": 1},7: { "levelId": 5, "mem": bit0(0x2249f2),"good": 1},8: { "levelId": 5, "mem": bit1(0x2249f2),"good": 1},9: { "levelId": 5, "mem": bit2(0x2249f2),"good": 1},10: { "levelId": 5, "mem": bit3(0x2249f2),"good": 1},11: { "levelId": 5, "mem": bit4(0x2249f2),"good": 1},12: { "levelId": 6, "mem": bit5(0x2249f2),"good": 1},13: { "levelId": 6, "mem": bit7(0x2249f2),"good": 1},14: { "levelId": 6, "mem": bit1(0x2249f3),"good": 1},15: { "levelId": 6, "mem": bit6(0x2249f2),"good": 1},16: { "levelId": 6, "mem": bit0(0x2249f3),"good": 1},17: { "levelId": 6, "mem": bit3(0x2249f3),"good": 1},18: { "levelId": 6, "mem": bit2(0x2249f3),"good": 1},19: { "levelId": 8, "mem": bit5(0x2249f3),"good": 1},20: { "levelId": 8, "mem": bit4(0x2249f3),"good": 1},21: { "levelId": 10, "mem": bit0(0x2249f4),"good": 1},22: { "levelId": 10, "mem": bit6(0x2249f3),"good": 1},23: { "levelId": 10, "mem": bit3(0x2249f4),"good": 1},24: { "levelId": 10, "mem": bit5(0x2249f4),"good": 1},25: { "levelId": 10, "mem": bit7(0x2249f3),"good": 1},26: { "levelId": 10, "mem": bit1(0x2249f4),"good": 1},27: { "levelId": 10, "mem": bit2(0x2249f4),"good": 1},28: { "levelId": 10, "mem": bit4(0x2249f4),"good": 1},29: { "levelId": 3, "mem": bit6(0x2249f4),"good": 1},30: { "levelId": 3, "mem": bit7(0x2249f4),"good": 1},31: { "levelId": 3, "good": 0},32: { "levelId": 3, "good": 0},33: { "levelId": 3, "good": 0},34: { "levelId": 3, "good": 0},35: { "levelId": 3, "good": 0},36: { "levelId": 3, "good": 0},37: { "levelId": 3, "good": 0},38: { "levelId": 3, "good": 0},39: { "levelId": 3, "good": 0},40: { "levelId": 3, "good": 0},41: { "levelId": 3, "good": 0},42: { "levelId": 3, "good": 0},43: { "levelId": 3, "good": 0},44: { "levelId": 3, "good": 0},45: { "levelId": 3, "good": 0},46: { "levelId": 3, "good": 0},47: { "levelId": 3, "good": 0},48: { "levelId": 3, "good": 0},49: { "levelId": 3, "good": 0},50: { "levelId": 3, "good": 0},51: { "levelId": 3, "good": 0},52: { "levelId": 3, "good": 0},53: { "levelId": 3, "good": 0},54: { "levelId": 3, "good": 0},55: { "levelId": 3, "good": 0},56: { "levelId": 3, "good": 0},57: { "levelId": 3, "good": 0},58: { "levelId": 3, "good": 0},59: { "levelId": 3, "good": 0},60: { "levelId": 3, "good": 0},61: { "levelId": 3, "good": 0},62: { "levelId": 3, "good": 0},63: { "levelId": 3, "good": 0},64: { "levelId": 3, "good": 0},65: { "levelId": 3, "good": 0},66: { "levelId": 3, "good": 0},67: { "levelId": 3, "good": 0},68: { "levelId": 3, "good": 0},69: { "levelId": 3, "good": 0},70: { "levelId": 3, "good": 0},71: { "levelId": 3, "good": 0},72: { "levelId": 3, "good": 0},73: { "levelId": 3, "good": 0},74: { "levelId": 3, "good": 0},75: { "levelId": 3, "good": 0},76: { "levelId": 3, "good": 0},77: { "levelId": 3, "good": 0},78: { "levelId": 3, "good": 0},79: { "levelId": 3, "good": 0},80: { "levelId": 3, "good": 0},</v>
+        <v>1: { "levelId": 1, "mem": bit7(0x2249f0),"good": 1},2: { "levelId": 2, "mem": bit0(0x2249f1),"good": 1},3: { "levelId": 2, "mem": bit1(0x2249f1),"good": 1},4: { "levelId": 2, "mem": bit5(0x2249f1),"good": 1},5: { "levelId": 2, "mem": bit6(0x2249f1),"good": 1},6: { "levelId": 1, "mem": bit7(0x2249f1),"good": 1},7: { "levelId": 5, "mem": bit0(0x2249f2),"good": 1},8: { "levelId": 5, "mem": bit1(0x2249f2),"good": 1},9: { "levelId": 5, "mem": bit2(0x2249f2),"good": 1},10: { "levelId": 5, "mem": bit3(0x2249f2),"good": 1},11: { "levelId": 5, "mem": bit4(0x2249f2),"good": 1},12: { "levelId": 6, "mem": bit5(0x2249f2),"good": 1},13: { "levelId": 6, "mem": bit7(0x2249f2),"good": 1},14: { "levelId": 6, "mem": bit1(0x2249f3),"good": 1},15: { "levelId": 6, "mem": bit6(0x2249f2),"good": 1},16: { "levelId": 6, "mem": bit0(0x2249f3),"good": 1},17: { "levelId": 6, "mem": bit3(0x2249f3),"good": 1},18: { "levelId": 6, "mem": bit2(0x2249f3),"good": 1},19: { "levelId": 8, "mem": bit5(0x2249f3),"good": 1},20: { "levelId": 8, "mem": bit4(0x2249f3),"good": 1},21: { "levelId": 10, "mem": bit0(0x2249f4),"good": 1},22: { "levelId": 10, "mem": bit6(0x2249f3),"good": 1},23: { "levelId": 10, "mem": bit3(0x2249f4),"good": 1},24: { "levelId": 10, "mem": bit5(0x2249f4),"good": 1},25: { "levelId": 10, "mem": bit7(0x2249f3),"good": 1},26: { "levelId": 10, "mem": bit1(0x2249f4),"good": 1},27: { "levelId": 10, "mem": bit2(0x2249f4),"good": 1},28: { "levelId": 10, "mem": bit4(0x2249f4),"good": 1},29: { "levelId": 12, "mem": bit6(0x2249f4),"good": 1},30: { "levelId": 12, "mem": bit7(0x2249f4),"good": 1},31: { "levelId": 12, "mem": bit1(0x2249f5),"good": 1},32: { "levelId": 12, "mem": bit0(0x2249f5),"good": 1},33: { "levelId": 3, "good": 0},34: { "levelId": 3, "good": 0},35: { "levelId": 3, "good": 0},36: { "levelId": 3, "good": 0},37: { "levelId": 3, "good": 0},38: { "levelId": 3, "good": 0},39: { "levelId": 3, "good": 0},40: { "levelId": 3, "good": 0},41: { "levelId": 3, "good": 0},42: { "levelId": 3, "good": 0},43: { "levelId": 3, "good": 0},44: { "levelId": 3, "good": 0},45: { "levelId": 3, "good": 0},46: { "levelId": 3, "good": 0},47: { "levelId": 3, "good": 0},48: { "levelId": 3, "good": 0},49: { "levelId": 3, "good": 0},50: { "levelId": 3, "good": 0},51: { "levelId": 3, "good": 0},52: { "levelId": 3, "good": 0},53: { "levelId": 3, "good": 0},54: { "levelId": 3, "good": 0},55: { "levelId": 3, "good": 0},56: { "levelId": 3, "good": 0},57: { "levelId": 3, "good": 0},58: { "levelId": 3, "good": 0},59: { "levelId": 3, "good": 0},60: { "levelId": 3, "good": 0},61: { "levelId": 3, "good": 0},62: { "levelId": 3, "good": 0},63: { "levelId": 3, "good": 0},64: { "levelId": 3, "good": 0},65: { "levelId": 3, "good": 0},66: { "levelId": 3, "good": 0},67: { "levelId": 3, "good": 0},68: { "levelId": 3, "good": 0},69: { "levelId": 3, "good": 0},70: { "levelId": 3, "good": 0},71: { "levelId": 3, "good": 0},72: { "levelId": 3, "good": 0},73: { "levelId": 3, "good": 0},74: { "levelId": 3, "good": 0},75: { "levelId": 3, "good": 0},76: { "levelId": 3, "good": 0},77: { "levelId": 3, "good": 0},78: { "levelId": 3, "good": 0},79: { "levelId": 3, "good": 0},80: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>7</v>
@@ -18940,7 +19126,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0</v>
@@ -18955,7 +19141,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>1</v>
@@ -18970,7 +19156,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>5</v>
@@ -18985,7 +19171,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>6</v>
@@ -19000,7 +19186,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>7</v>
@@ -19015,7 +19201,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>0</v>
@@ -19030,7 +19216,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>1</v>
@@ -19045,7 +19231,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>2</v>
@@ -19060,7 +19246,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>3</v>
@@ -19075,7 +19261,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>4</v>
@@ -19090,7 +19276,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>5</v>
@@ -19105,7 +19291,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>7</v>
@@ -19120,7 +19306,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>1</v>
@@ -19135,7 +19321,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>6</v>
@@ -19150,7 +19336,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>0</v>
@@ -19165,7 +19351,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>3</v>
@@ -19180,7 +19366,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>2</v>
@@ -19195,7 +19381,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>5</v>
@@ -19210,7 +19396,7 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>4</v>
@@ -19225,7 +19411,7 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>0</v>
@@ -19240,7 +19426,7 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>6</v>
@@ -19255,7 +19441,7 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>3</v>
@@ -19270,7 +19456,7 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>5</v>
@@ -19285,7 +19471,7 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>7</v>
@@ -19300,7 +19486,7 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>1</v>
@@ -19315,7 +19501,7 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>2</v>
@@ -19330,7 +19516,7 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>4</v>
@@ -19345,50 +19531,62 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>6</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="D30" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C30, Levels!B:B, 0), 1, 1)),", ",IF(A30 &lt;&gt; "", """mem"": bit" &amp; B30 &amp; "(" &amp; A30 &amp; "),", ""),"""good"": ",IF(A30 &lt;&gt; "", 1, 0),"},")</f>
-        <v>29: { "levelId": 3, "mem": bit6(0x2249f4),"good": 1},</v>
+        <v>29: { "levelId": 12, "mem": bit6(0x2249f4),"good": 1},</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>7</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="D31" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C31, Levels!B:B, 0), 1, 1)),", ",IF(A31 &lt;&gt; "", """mem"": bit" &amp; B31 &amp; "(" &amp; A31 &amp; "),", ""),"""good"": ",IF(A31 &lt;&gt; "", 1, 0),"},")</f>
-        <v>30: { "levelId": 3, "mem": bit7(0x2249f4),"good": 1},</v>
+        <v>30: { "levelId": 12, "mem": bit7(0x2249f4),"good": 1},</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="C32" s="4" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="D32" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C32, Levels!B:B, 0), 1, 1)),", ",IF(A32 &lt;&gt; "", """mem"": bit" &amp; B32 &amp; "(" &amp; A32 &amp; "),", ""),"""good"": ",IF(A32 &lt;&gt; "", 1, 0),"},")</f>
-        <v>31: { "levelId": 3, "good": 0},</v>
+        <v>31: { "levelId": 12, "mem": bit1(0x2249f5),"good": 1},</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="C33" s="4" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="D33" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C33, Levels!B:B, 0), 1, 1)),", ",IF(A33 &lt;&gt; "", """mem"": bit" &amp; B33 &amp; "(" &amp; A33 &amp; "),", ""),"""good"": ",IF(A33 &lt;&gt; "", 1, 0),"},")</f>
-        <v>32: { "levelId": 3, "good": 0},</v>
+        <v>32: { "levelId": 12, "mem": bit0(0x2249f5),"good": 1},</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Fixed the completionist achievement for Whale Bay and began refactoring the bonus stage achievements and leaderboard
</commit_message>
<xml_diff>
--- a/Rayman 2.xlsx
+++ b/Rayman 2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Areas" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1605" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1672" uniqueCount="163">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -289,6 +289,30 @@
     <t xml:space="preserve">CanopyArea3</t>
   </si>
   <si>
+    <t xml:space="preserve">78AB50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WhaleBay1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">in Whale Bay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Whale Bay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">77295C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WhaleBay2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">783C54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WhaleBay3</t>
+  </si>
+  <si>
     <t xml:space="preserve">Index</t>
   </si>
   <si>
@@ -449,6 +473,24 @@
   </si>
   <si>
     <t xml:space="preserve">0x2249ad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x2249ae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x2249af</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x2249b0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x2249b1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x2249b2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x2249b3</t>
   </si>
   <si>
     <t xml:space="preserve">Level ID</t>
@@ -683,7 +725,7 @@
       <selection pane="bottomLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.66"/>
@@ -713,7 +755,7 @@
       </c>
       <c r="H1" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(E2:E1000)</f>
-        <v>0x784BFC: { "id": 0x784BFC, "areaName": "Menu", "displayName": "Main Menu", "levelName": "Menu" },0x789668: { "id": 0x789668, "areaName": "Intro", "displayName": "somewhere in the Glade of Dreams…", "levelName": "None" },0x778C74: { "id": 0x778C74, "areaName": "BuccaneerBrig", "displayName": "in the Buccaneer’s brig", "levelName": "None" },0x78D424: { "id": 0x78D424, "areaName": "WoodsOfLight", "displayName": "in the Woods of Light", "levelName": "Woods of Light" },0x790570: { "id": 0x790570, "areaName": "HallOfDoors", "displayName": "in the Hall of Doors", "levelName": "Hall of Doors" },0x7875A8: { "id": 0x7875A8, "areaName": "FairyGladeArea1", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x78A320: { "id": 0x78A320, "areaName": "FairyGladeArea2", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x7A1BD8: { "id": 0x7A1BD8, "areaName": "FairyGladeArea3", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x77BFFC: { "id": 0x77BFFC, "areaName": "FairyGladeArea4", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x771B74: { "id": 0x771B74, "areaName": "FairyGladeArea5", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x74AAA8: { "id": 0x74AAA8, "areaName": "Results", "displayName": "viewing level results…", "levelName": "None" },0x788708: { "id": 0x788708, "areaName": "MarshesArea1", "displayName": "in the Marshes of Awakening", "levelName": "Marshes of Awakening" },0x7786E8: { "id": 0x7786E8, "areaName": "MarshesArea2", "displayName": "in the Marshes of Awakening", "levelName": "Marshes of Awakening" },0x790598: { "id": 0x790598, "areaName": "BayouArea1", "displayName": "in the Bayou", "levelName": "Bayou" },0x788764: { "id": 0x788764, "areaName": "BayouArea2", "displayName": "in the Bayou", "levelName": "Bayou" },0x7928A4: { "id": 0x7928A4, "areaName": "SoWaIArea1", "displayName": "in the Sanctuary of Water and Ice", "levelName": "Sanctuary of Water and Ice" },0x774694: { "id": 0x774694, "areaName": "SoWaIArea2", "displayName": "in the Sanctuary of Water and Ice", "levelName": "Sanctuary of Water and Ice" },0x76F100: { "id": 0x76F100, "areaName": "Polokus", "displayName": "in Polokus’s dream", "levelName": "Polokus" },0x0: { "id": 0x0, "areaName": "None", "displayName": "somewhere in the Glade of Dreams…", "levelName": "None" },0x751974: { "id": 0x751974, "areaName": "Bonus", "displayName": "in the bonus stage", "levelName": "None" },0x776C08: { "id": 0x776C08, "areaName": "MenhirArea1", "displayName": "in the Menhir Hills", "levelName": "Menhir Hills" },0x78FBD8: { "id": 0x78FBD8, "areaName": "MenhirArea2", "displayName": "in the Menhir Hills", "levelName": "Menhir Hills" },0x788950: { "id": 0x788950, "areaName": "MenhirArea3", "displayName": "in the Menhir Hills", "levelName": "Menhir Hills" },0x78402C: { "id": 0x78402C, "areaName": "BadDreamsArea1", "displayName": "in the Cave of Bad Dreams", "levelName": "Cave of Bad Dreams" },0x788148: { "id": 0x788148, "areaName": "BadDreamsArea2", "displayName": "in the Cave of Bad Dreams", "levelName": "Cave of Bad Dreams" },0x75AADC: { "id": 0x75AADC, "areaName": "MenhirArea4", "displayName": "in the Menhir Hills", "levelName": "Menhir Hills" },0x75BE94: { "id": 0x75BE94, "areaName": "CanopyArea1", "displayName": "in the Canopy", "levelName": "Canopy" },0x78C480: { "id": 0x78C480, "areaName": "CanopyArea2", "displayName": "in the Canopy", "levelName": "Canopy" },0x790A4C: { "id": 0x790A4C, "areaName": "CanopyArea3", "displayName": "in the Canopy", "levelName": "Canopy" },</v>
+        <v>0x784BFC: { "id": 0x784BFC, "areaName": "Menu", "displayName": "Main Menu", "levelName": "Menu" },0x789668: { "id": 0x789668, "areaName": "Intro", "displayName": "somewhere in the Glade of Dreams…", "levelName": "None" },0x778C74: { "id": 0x778C74, "areaName": "BuccaneerBrig", "displayName": "in the Buccaneer’s brig", "levelName": "None" },0x78D424: { "id": 0x78D424, "areaName": "WoodsOfLight", "displayName": "in the Woods of Light", "levelName": "Woods of Light" },0x790570: { "id": 0x790570, "areaName": "HallOfDoors", "displayName": "in the Hall of Doors", "levelName": "Hall of Doors" },0x7875A8: { "id": 0x7875A8, "areaName": "FairyGladeArea1", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x78A320: { "id": 0x78A320, "areaName": "FairyGladeArea2", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x7A1BD8: { "id": 0x7A1BD8, "areaName": "FairyGladeArea3", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x77BFFC: { "id": 0x77BFFC, "areaName": "FairyGladeArea4", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x771B74: { "id": 0x771B74, "areaName": "FairyGladeArea5", "displayName": "in the Fairy Glade", "levelName": "Fairy Glade" },0x74AAA8: { "id": 0x74AAA8, "areaName": "Results", "displayName": "viewing level results…", "levelName": "None" },0x788708: { "id": 0x788708, "areaName": "MarshesArea1", "displayName": "in the Marshes of Awakening", "levelName": "Marshes of Awakening" },0x7786E8: { "id": 0x7786E8, "areaName": "MarshesArea2", "displayName": "in the Marshes of Awakening", "levelName": "Marshes of Awakening" },0x790598: { "id": 0x790598, "areaName": "BayouArea1", "displayName": "in the Bayou", "levelName": "Bayou" },0x788764: { "id": 0x788764, "areaName": "BayouArea2", "displayName": "in the Bayou", "levelName": "Bayou" },0x7928A4: { "id": 0x7928A4, "areaName": "SoWaIArea1", "displayName": "in the Sanctuary of Water and Ice", "levelName": "Sanctuary of Water and Ice" },0x774694: { "id": 0x774694, "areaName": "SoWaIArea2", "displayName": "in the Sanctuary of Water and Ice", "levelName": "Sanctuary of Water and Ice" },0x76F100: { "id": 0x76F100, "areaName": "Polokus", "displayName": "in Polokus’s dream", "levelName": "Polokus" },0x0: { "id": 0x0, "areaName": "None", "displayName": "somewhere in the Glade of Dreams…", "levelName": "None" },0x751974: { "id": 0x751974, "areaName": "Bonus", "displayName": "in the bonus stage", "levelName": "None" },0x776C08: { "id": 0x776C08, "areaName": "MenhirArea1", "displayName": "in the Menhir Hills", "levelName": "Menhir Hills" },0x78FBD8: { "id": 0x78FBD8, "areaName": "MenhirArea2", "displayName": "in the Menhir Hills", "levelName": "Menhir Hills" },0x788950: { "id": 0x788950, "areaName": "MenhirArea3", "displayName": "in the Menhir Hills", "levelName": "Menhir Hills" },0x78402C: { "id": 0x78402C, "areaName": "BadDreamsArea1", "displayName": "in the Cave of Bad Dreams", "levelName": "Cave of Bad Dreams" },0x788148: { "id": 0x788148, "areaName": "BadDreamsArea2", "displayName": "in the Cave of Bad Dreams", "levelName": "Cave of Bad Dreams" },0x75AADC: { "id": 0x75AADC, "areaName": "MenhirArea4", "displayName": "in the Menhir Hills", "levelName": "Menhir Hills" },0x75BE94: { "id": 0x75BE94, "areaName": "CanopyArea1", "displayName": "in the Canopy", "levelName": "Canopy" },0x78C480: { "id": 0x78C480, "areaName": "CanopyArea2", "displayName": "in the Canopy", "levelName": "Canopy" },0x790A4C: { "id": 0x790A4C, "areaName": "CanopyArea3", "displayName": "in the Canopy", "levelName": "Canopy" },0x78AB50: { "id": 0x78AB50, "areaName": "WhaleBay1", "displayName": "in Whale Bay", "levelName": "Whale Bay" },0x77295C: { "id": 0x77295C, "areaName": "WhaleBay2", "displayName": "in Whale Bay", "levelName": "Whale Bay" },0x783C54: { "id": 0x783C54, "areaName": "WhaleBay3", "displayName": "in Whale Bay", "levelName": "Whale Bay" },</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1239,13 +1281,58 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D31" s="4"/>
+      <c r="A31" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E31" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("0x", A31,": { ""id"": ","0x", A31,", ""areaName"": """,B31,""", ""displayName"": """,C31,""", ""levelName"": """,D31,""" },")</f>
+        <v>0x78AB50: { "id": 0x78AB50, "areaName": "WhaleBay1", "displayName": "in Whale Bay", "levelName": "Whale Bay" },</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D32" s="4"/>
+      <c r="A32" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E32" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("0x", A32,": { ""id"": ","0x", A32,", ""areaName"": """,B32,""", ""displayName"": """,C32,""", ""levelName"": """,D32,""" },")</f>
+        <v>0x77295C: { "id": 0x77295C, "areaName": "WhaleBay2", "displayName": "in Whale Bay", "levelName": "Whale Bay" },</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D33" s="4"/>
+      <c r="A33" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E33" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("0x", A33,": { ""id"": ","0x", A33,", ""areaName"": """,B33,""", ""displayName"": """,C33,""", ""levelName"": """,D33,""" },")</f>
+        <v>0x783C54: { "id": 0x783C54, "areaName": "WhaleBay3", "displayName": "in Whale Bay", "levelName": "Whale Bay" },</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D34" s="4"/>
@@ -4220,10 +4307,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+      <selection pane="bottomLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.21"/>
@@ -4235,22 +4322,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>4</v>
@@ -4326,11 +4413,11 @@
       </c>
       <c r="E4" s="0" t="n">
         <f aca="false">COUNTIFS(Lums!C3:C1002, "=" &amp; B4)</f>
-        <v>658</v>
+        <v>608</v>
       </c>
       <c r="F4" s="0" t="n">
         <f aca="false">COUNTIFS(Cages!C3:C83, "=" &amp; B4)</f>
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G4" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A4,": { ""id"": ",A4,", ""name"": """,B4,""", ""lums"": ",C4,", ""cages"": ",D4," },")</f>
@@ -4585,18 +4672,26 @@
         <f aca="false">ROW()-1</f>
         <v>13</v>
       </c>
-      <c r="B14" s="4"/>
+      <c r="B14" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="E14" s="0" t="n">
         <f aca="false">COUNTIFS(Lums!C13:C1012, "=" &amp; B14)</f>
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="F14" s="0" t="n">
         <f aca="false">COUNTIFS(Cages!C13:C93, "=" &amp; B14)</f>
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="G14" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(A14,": { ""id"": ",A14,", ""name"": """,B14,""", ""lums"": ",C14,", ""cages"": ",D14," },")</f>
-        <v>13: { "id": 13, "name": "", "lums": , "cages":  },</v>
+        <v>13: { "id": 13, "name": "Whale Bay", "lums": 50, "cages": 4 },</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7957,13 +8052,13 @@
   </sheetPr>
   <dimension ref="A1:H1001"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A306" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A362" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C344" activeCellId="0" sqref="C344"/>
+      <selection pane="bottomLeft" activeCell="C394" activeCellId="0" sqref="C394"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.93"/>
@@ -7972,10 +8067,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>3</v>
@@ -7988,12 +8083,12 @@
       </c>
       <c r="H1" s="5" t="str">
         <f aca="false">_xlfn.CONCAT(D2:D1001)</f>
-        <v>1: { "levelId": 2, "mem": bit0(0x224988),"good": 1, "addr": 0x224988, "bit": 0},2: { "levelId": 2, "mem": bit1(0x224988),"good": 1, "addr": 0x224988, "bit": 1},3: { "levelId": 2, "mem": bit2(0x224988),"good": 1, "addr": 0x224988, "bit": 2},4: { "levelId": 2, "mem": bit3(0x224988),"good": 1, "addr": 0x224988, "bit": 3},5: { "levelId": 2, "mem": bit4(0x224988),"good": 1, "addr": 0x224988, "bit": 4},6: { "levelId": 2, "mem": bit5(0x224988),"good": 1, "addr": 0x224988, "bit": 5},7: { "levelId": 2, "mem": bit6(0x224988),"good": 1, "addr": 0x224988, "bit": 6},8: { "levelId": 2, "mem": bit7(0x224988),"good": 1, "addr": 0x224988, "bit": 7},9: { "levelId": 2, "mem": bit2(0x224989),"good": 1, "addr": 0x224989, "bit": 2},10: { "levelId": 2, "mem": bit1(0x22498a),"good": 1, "addr": 0x22498a, "bit": 1},11: { "levelId": 2, "mem": bit2(0x22498a),"good": 1, "addr": 0x22498a, "bit": 2},12: { "levelId": 2, "mem": bit3(0x22498a),"good": 1, "addr": 0x22498a, "bit": 3},13: { "levelId": 2, "mem": bit4(0x22498a),"good": 1, "addr": 0x22498a, "bit": 4},14: { "levelId": 2, "mem": bit5(0x22498a),"good": 1, "addr": 0x22498a, "bit": 5},15: { "levelId": 2, "mem": bit6(0x22498a),"good": 1, "addr": 0x22498a, "bit": 6},16: { "levelId": 2, "mem": bit7(0x22498a),"good": 1, "addr": 0x22498a, "bit": 7},17: { "levelId": 2, "mem": bit5(0x22498b),"good": 1, "addr": 0x22498b, "bit": 5},18: { "levelId": 2, "mem": bit6(0x22498b),"good": 1, "addr": 0x22498b, "bit": 6},19: { "levelId": 2, "mem": bit7(0x22498b),"good": 1, "addr": 0x22498b, "bit": 7},20: { "levelId": 2, "mem": bit0(0x22498c),"good": 1, "addr": 0x22498c, "bit": 0},21: { "levelId": 2, "mem": bit1(0x22498c),"good": 1, "addr": 0x22498c, "bit": 1},22: { "levelId": 2, "mem": bit2(0x22498c),"good": 1, "addr": 0x22498c, "bit": 2},23: { "levelId": 2, "mem": bit3(0x22498c),"good": 1, "addr": 0x22498c, "bit": 3},24: { "levelId": 2, "mem": bit4(0x22498c),"good": 1, "addr": 0x22498c, "bit": 4},25: { "levelId": 2, "mem": bit5(0x22498c),"good": 1, "addr": 0x22498c, "bit": 5},26: { "levelId": 2, "mem": bit6(0x22498c),"good": 1, "addr": 0x22498c, "bit": 6},27: { "levelId": 2, "mem": bit7(0x22498c),"good": 1, "addr": 0x22498c, "bit": 7},28: { "levelId": 2, "mem": bit0(0x22498d),"good": 1, "addr": 0x22498d, "bit": 0},29: { "levelId": 2, "mem": bit1(0x22498d),"good": 1, "addr": 0x22498d, "bit": 1},30: { "levelId": 2, "mem": bit2(0x22498d),"good": 1, "addr": 0x22498d, "bit": 2},31: { "levelId": 2, "mem": bit3(0x22498d),"good": 1, "addr": 0x22498d, "bit": 3},32: { "levelId": 2, "mem": bit4(0x22498d),"good": 1, "addr": 0x22498d, "bit": 4},33: { "levelId": 2, "mem": bit5(0x22498d),"good": 1, "addr": 0x22498d, "bit": 5},34: { "levelId": 2, "mem": bit6(0x22498d),"good": 1, "addr": 0x22498d, "bit": 6},35: { "levelId": 2, "mem": bit7(0x22498d),"good": 1, "addr": 0x22498d, "bit": 7},36: { "levelId": 2, "mem": bit0(0x22498e),"good": 1, "addr": 0x22498e, "bit": 0},37: { "levelId": 2, "mem": bit1(0x22498e),"good": 1, "addr": 0x22498e, "bit": 1},38: { "levelId": 5, "mem": bit2(0x22498e),"good": 1, "addr": 0x22498e, "bit": 2},39: { "levelId": 5, "mem": bit3(0x22498e),"good": 1, "addr": 0x22498e, "bit": 3},40: { "levelId": 5, "mem": bit4(0x22498e),"good": 1, "addr": 0x22498e, "bit": 4},41: { "levelId": 5, "mem": bit5(0x22498e),"good": 1, "addr": 0x22498e, "bit": 5},42: { "levelId": 5, "mem": bit6(0x22498e),"good": 1, "addr": 0x22498e, "bit": 6},43: { "levelId": 5, "mem": bit7(0x22498e),"good": 1, "addr": 0x22498e, "bit": 7},44: { "levelId": 5, "mem": bit0(0x22498f),"good": 1, "addr": 0x22498f, "bit": 0},45: { "levelId": 5, "mem": bit1(0x22498f),"good": 1, "addr": 0x22498f, "bit": 1},46: { "levelId": 5, "mem": bit2(0x22498f),"good": 1, "addr": 0x22498f, "bit": 2},47: { "levelId": 5, "mem": bit3(0x22498f),"good": 1, "addr": 0x22498f, "bit": 3},48: { "levelId": 5, "mem": bit4(0x22498f),"good": 1, "addr": 0x22498f, "bit": 4},49: { "levelId": 5, "mem": bit5(0x22498f),"good": 1, "addr": 0x22498f, "bit": 5},50: { "levelId": 5, "mem": bit6(0x22498f),"good": 1, "addr": 0x22498f, "bit": 6},51: { "levelId": 5, "mem": bit7(0x22498f),"good": 1, "addr": 0x22498f, "bit": 7},52: { "levelId": 5, "mem": bit0(0x224990),"good": 1, "addr": 0x224990, "bit": 0},53: { "levelId": 5, "mem": bit1(0x224990),"good": 1, "addr": 0x224990, "bit": 1},54: { "levelId": 5, "mem": bit2(0x224990),"good": 1, "addr": 0x224990, "bit": 2},55: { "levelId": 5, "mem": bit3(0x224990),"good": 1, "addr": 0x224990, "bit": 3},56: { "levelId": 5, "mem": bit4(0x224990),"good": 1, "addr": 0x224990, "bit": 4},57: { "levelId": 5, "mem": bit5(0x224990),"good": 1, "addr": 0x224990, "bit": 5},58: { "levelId": 5, "mem": bit6(0x224990),"good": 1, "addr": 0x224990, "bit": 6},59: { "levelId": 5, "mem": bit7(0x224990),"good": 1, "addr": 0x224990, "bit": 7},60: { "levelId": 5, "mem": bit0(0x224991),"good": 1, "addr": 0x224991, "bit": 0},61: { "levelId": 5, "mem": bit1(0x224991),"good": 1, "addr": 0x224991, "bit": 1},62: { "levelId": 5, "mem": bit2(0x224991),"good": 1, "addr": 0x224991, "bit": 2},63: { "levelId": 5, "mem": bit3(0x224991),"good": 1, "addr": 0x224991, "bit": 3},64: { "levelId": 5, "mem": bit4(0x224991),"good": 1, "addr": 0x224991, "bit": 4},65: { "levelId": 5, "mem": bit5(0x224991),"good": 1, "addr": 0x224991, "bit": 5},66: { "levelId": 5, "mem": bit6(0x224991),"good": 1, "addr": 0x224991, "bit": 6},67: { "levelId": 5, "mem": bit7(0x224991),"good": 1, "addr": 0x224991, "bit": 7},68: { "levelId": 5, "mem": bit0(0x224992),"good": 1, "addr": 0x224992, "bit": 0},69: { "levelId": 5, "mem": bit1(0x224992),"good": 1, "addr": 0x224992, "bit": 1},70: { "levelId": 5, "mem": bit2(0x224992),"good": 1, "addr": 0x224992, "bit": 2},71: { "levelId": 5, "mem": bit3(0x224992),"good": 1, "addr": 0x224992, "bit": 3},72: { "levelId": 5, "mem": bit4(0x224992),"good": 1, "addr": 0x224992, "bit": 4},73: { "levelId": 5, "mem": bit5(0x224992),"good": 1, "addr": 0x224992, "bit": 5},74: { "levelId": 5, "mem": bit6(0x224992),"good": 1, "addr": 0x224992, "bit": 6},75: { "levelId": 5, "mem": bit7(0x224992),"good": 1, "addr": 0x224992, "bit": 7},76: { "levelId": 5, "mem": bit0(0x224993),"good": 1, "addr": 0x224993, "bit": 0},77: { "levelId": 5, "mem": bit1(0x224993),"good": 1, "addr": 0x224993, "bit": 1},78: { "levelId": 5, "mem": bit2(0x224993),"good": 1, "addr": 0x224993, "bit": 2},79: { "levelId": 5, "mem": bit3(0x224993),"good": 1, "addr": 0x224993, "bit": 3},80: { "levelId": 5, "mem": bit4(0x224993),"good": 1, "addr": 0x224993, "bit": 4},81: { "levelId": 5, "mem": bit5(0x224993),"good": 1, "addr": 0x224993, "bit": 5},82: { "levelId": 5, "mem": bit6(0x224993),"good": 1, "addr": 0x224993, "bit": 6},83: { "levelId": 5, "mem": bit7(0x224993),"good": 1, "addr": 0x224993, "bit": 7},84: { "levelId": 5, "mem": bit0(0x224994),"good": 1, "addr": 0x224994, "bit": 0},85: { "levelId": 5, "mem": bit1(0x224994),"good": 1, "addr": 0x224994, "bit": 1},86: { "levelId": 5, "mem": bit2(0x224994),"good": 1, "addr": 0x224994, "bit": 2},87: { "levelId": 5, "mem": bit3(0x224994),"good": 1, "addr": 0x224994, "bit": 3},88: { "levelId": 6, "mem": bit4(0x224994),"good": 1, "addr": 0x224994, "bit": 4},89: { "levelId": 6, "mem": bit5(0x224994),"good": 1, "addr": 0x224994, "bit": 5},90: { "levelId": 6, "mem": bit6(0x224994),"good": 1, "addr": 0x224994, "bit": 6},91: { "levelId": 6, "mem": bit7(0x224994),"good": 1, "addr": 0x224994, "bit": 7},92: { "levelId": 6, "mem": bit0(0x224995),"good": 1, "addr": 0x224995, "bit": 0},93: { "levelId": 6, "mem": bit1(0x224995),"good": 1, "addr": 0x224995, "bit": 1},94: { "levelId": 6, "mem": bit2(0x224995),"good": 1, "addr": 0x224995, "bit": 2},95: { "levelId": 6, "mem": bit3(0x224995),"good": 1, "addr": 0x224995, "bit": 3},96: { "levelId": 6, "mem": bit4(0x224995),"good": 1, "addr": 0x224995, "bit": 4},97: { "levelId": 6, "mem": bit5(0x224995),"good": 1, "addr": 0x224995, "bit": 5},98: { "levelId": 6, "mem": bit6(0x224995),"good": 1, "addr": 0x224995, "bit": 6},99: { "levelId": 6, "mem": bit7(0x224995),"good": 1, "addr": 0x224995, "bit": 7},100: { "levelId": 6, "mem": bit0(0x224996),"good": 1, "addr": 0x224996, "bit": 0},101: { "levelId": 6, "mem": bit1(0x224996),"good": 1, "addr": 0x224996, "bit": 1},102: { "levelId": 6, "mem": bit2(0x224996),"good": 1, "addr": 0x224996, "bit": 2},103: { "levelId": 6, "mem": bit3(0x224996),"good": 1, "addr": 0x224996, "bit": 3},104: { "levelId": 6, "mem": bit4(0x224996),"good": 1, "addr": 0x224996, "bit": 4},105: { "levelId": 6, "mem": bit5(0x224996),"good": 1, "addr": 0x224996, "bit": 5},106: { "levelId": 6, "mem": bit6(0x224996),"good": 1, "addr": 0x224996, "bit": 6},107: { "levelId": 6, "mem": bit7(0x224996),"good": 1, "addr": 0x224996, "bit": 7},108: { "levelId": 6, "mem": bit0(0x224997),"good": 1, "addr": 0x224997, "bit": 0},109: { "levelId": 6, "mem": bit1(0x224997),"good": 1, "addr": 0x224997, "bit": 1},110: { "levelId": 6, "mem": bit2(0x224997),"good": 1, "addr": 0x224997, "bit": 2},111: { "levelId": 6, "mem": bit3(0x224997),"good": 1, "addr": 0x224997, "bit": 3},112: { "levelId": 6, "mem": bit4(0x224997),"good": 1, "addr": 0x224997, "bit": 4},113: { "levelId": 6, "mem": bit5(0x224997),"good": 1, "addr": 0x224997, "bit": 5},114: { "levelId": 6, "mem": bit6(0x224997),"good": 1, "addr": 0x224997, "bit": 6},115: { "levelId": 6, "mem": bit7(0x224997),"good": 1, "addr": 0x224997, "bit": 7},116: { "levelId": 6, "mem": bit0(0x224998),"good": 1, "addr": 0x224998, "bit": 0},117: { "levelId": 6, "mem": bit1(0x224998),"good": 1, "addr": 0x224998, "bit": 1},118: { "levelId": 6, "mem": bit2(0x224998),"good": 1, "addr": 0x224998, "bit": 2},119: { "levelId": 6, "mem": bit3(0x224998),"good": 1, "addr": 0x224998, "bit": 3},120: { "levelId": 6, "mem": bit4(0x224998),"good": 1, "addr": 0x224998, "bit": 4},121: { "levelId": 6, "mem": bit5(0x224998),"good": 1, "addr": 0x224998, "bit": 5},122: { "levelId": 6, "mem": bit6(0x224998),"good": 1, "addr": 0x224998, "bit": 6},123: { "levelId": 6, "mem": bit0(0x224999),"good": 1, "addr": 0x224999, "bit": 0},124: { "levelId": 6, "mem": bit1(0x224999),"good": 1, "addr": 0x224999, "bit": 1},125: { "levelId": 6, "mem": bit2(0x224999),"good": 1, "addr": 0x224999, "bit": 2},126: { "levelId": 6, "mem": bit3(0x224999),"good": 1, "addr": 0x224999, "bit": 3},127: { "levelId": 6, "mem": bit4(0x224999),"good": 1, "addr": 0x224999, "bit": 4},128: { "levelId": 6, "mem": bit5(0x224999),"good": 1, "addr": 0x224999, "bit": 5},129: { "levelId": 6, "mem": bit6(0x224999),"good": 1, "addr": 0x224999, "bit": 6},130: { "levelId": 6, "mem": bit7(0x224999),"good": 1, "addr": 0x224999, "bit": 7},131: { "levelId": 6, "mem": bit0(0x22499a),"good": 1, "addr": 0x22499a, "bit": 0},132: { "levelId": 6, "mem": bit1(0x22499a),"good": 1, "addr": 0x22499a, "bit": 1},133: { "levelId": 6, "mem": bit2(0x22499a),"good": 1, "addr": 0x22499a, "bit": 2},134: { "levelId": 6, "mem": bit3(0x22499a),"good": 1, "addr": 0x22499a, "bit": 3},135: { "levelId": 6, "mem": bit4(0x22499a),"good": 1, "addr": 0x22499a, "bit": 4},136: { "levelId": 6, "mem": bit5(0x22499a),"good": 1, "addr": 0x22499a, "bit": 5},137: { "levelId": 1, "mem": bit3(0x224a36),"good": 1, "addr": 0x224a36, "bit": 3},138: { "levelId": 1, "mem": bit4(0x224a36),"good": 1, "addr": 0x224a36, "bit": 4},139: { "levelId": 1, "mem": bit5(0x224a36),"good": 1, "addr": 0x224a36, "bit": 5},140: { "levelId": 1, "mem": bit6(0x224a36),"good": 1, "addr": 0x224a36, "bit": 6},141: { "levelId": 1, "mem": bit7(0x224a36),"good": 1, "addr": 0x224a36, "bit": 7},142: { "levelId": 6, "mem": bit7(0x224998),"good": 1, "addr": 0x224998, "bit": 7},143: { "levelId": 8, "mem": bit3(0x22499b),"good": 1, "addr": 0x22499b, "bit": 3},144: { "levelId": 8, "mem": bit4(0x22499b),"good": 1, "addr": 0x22499b, "bit": 4},145: { "levelId": 8, "mem": bit5(0x22499b),"good": 1, "addr": 0x22499b, "bit": 5},146: { "levelId": 8, "mem": bit5(0x22499c),"good": 1, "addr": 0x22499c, "bit": 5},147: { "levelId": 8, "mem": bit6(0x22499c),"good": 1, "addr": 0x22499c, "bit": 6},148: { "levelId": 8, "mem": bit7(0x22499c),"good": 1, "addr": 0x22499c, "bit": 7},149: { "levelId": 8, "mem": bit0(0x22499d),"good": 1, "addr": 0x22499d, "bit": 0},150: { "levelId": 8, "mem": bit1(0x22499d),"good": 1, "addr": 0x22499d, "bit": 1},151: { "levelId": 8, "mem": bit2(0x22499d),"good": 1, "addr": 0x22499d, "bit": 2},152: { "levelId": 8, "mem": bit3(0x22499d),"good": 1, "addr": 0x22499d, "bit": 3},153: { "levelId": 8, "mem": bit4(0x22499d),"good": 1, "addr": 0x22499d, "bit": 4},154: { "levelId": 8, "mem": bit5(0x22499d),"good": 1, "addr": 0x22499d, "bit": 5},155: { "levelId": 8, "mem": bit6(0x22499d),"good": 1, "addr": 0x22499d, "bit": 6},156: { "levelId": 8, "mem": bit7(0x22499d),"good": 1, "addr": 0x22499d, "bit": 7},157: { "levelId": 8, "mem": bit0(0x22499e),"good": 1, "addr": 0x22499e, "bit": 0},158: { "levelId": 8, "mem": bit1(0x22499e),"good": 1, "addr": 0x22499e, "bit": 1},159: { "levelId": 8, "mem": bit6(0x22499a),"good": 1, "addr": 0x22499a, "bit": 6},160: { "levelId": 8, "mem": bit7(0x22499a),"good": 1, "addr": 0x22499a, "bit": 7},161: { "levelId": 8, "mem": bit0(0x22499b),"good": 1, "addr": 0x22499b, "bit": 0},162: { "levelId": 8, "mem": bit1(0x22499b),"good": 1, "addr": 0x22499b, "bit": 1},163: { "levelId": 8, "mem": bit2(0x22499b),"good": 1, "addr": 0x22499b, "bit": 2},164: { "levelId": 8, "mem": bit6(0x22499b),"good": 1, "addr": 0x22499b, "bit": 6},165: { "levelId": 8, "mem": bit7(0x22499b),"good": 1, "addr": 0x22499b, "bit": 7},166: { "levelId": 8, "mem": bit0(0x22499c),"good": 1, "addr": 0x22499c, "bit": 0},167: { "levelId": 8, "mem": bit1(0x22499c),"good": 1, "addr": 0x22499c, "bit": 1},168: { "levelId": 8, "mem": bit2(0x22499c),"good": 1, "addr": 0x22499c, "bit": 2},169: { "levelId": 8, "mem": bit3(0x22499c),"good": 1, "addr": 0x22499c, "bit": 3},170: { "levelId": 8, "mem": bit4(0x22499c),"good": 1, "addr": 0x22499c, "bit": 4},171: { "levelId": 8, "mem": bit2(0x22499e),"good": 1, "addr": 0x22499e, "bit": 2},172: { "levelId": 8, "mem": bit3(0x22499e),"good": 1, "addr": 0x22499e, "bit": 3},173: { "levelId": 8, "mem": bit4(0x22499e),"good": 1, "addr": 0x22499e, "bit": 4},174: { "levelId": 8, "mem": bit5(0x22499e),"good": 1, "addr": 0x22499e, "bit": 5},175: { "levelId": 8, "mem": bit6(0x22499e),"good": 1, "addr": 0x22499e, "bit": 6},176: { "levelId": 8, "mem": bit7(0x22499e),"good": 1, "addr": 0x22499e, "bit": 7},177: { "levelId": 8, "mem": bit0(0x22499f),"good": 1, "addr": 0x22499f, "bit": 0},178: { "levelId": 8, "mem": bit1(0x22499f),"good": 1, "addr": 0x22499f, "bit": 1},179: { "levelId": 8, "mem": bit2(0x22499f),"good": 1, "addr": 0x22499f, "bit": 2},180: { "levelId": 8, "mem": bit3(0x22499f),"good": 1, "addr": 0x22499f, "bit": 3},181: { "levelId": 8, "mem": bit4(0x22499f),"good": 1, "addr": 0x22499f, "bit": 4},182: { "levelId": 8, "mem": bit5(0x22499f),"good": 1, "addr": 0x22499f, "bit": 5},183: { "levelId": 8, "mem": bit6(0x22499f),"good": 1, "addr": 0x22499f, "bit": 6},184: { "levelId": 8, "mem": bit7(0x22499f),"good": 1, "addr": 0x22499f, "bit": 7},185: { "levelId": 8, "mem": bit0(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 0},186: { "levelId": 8, "mem": bit1(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 1},187: { "levelId": 8, "mem": bit2(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 2},188: { "levelId": 8, "mem": bit3(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 3},189: { "levelId": 8, "mem": bit4(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 4},190: { "levelId": 8, "mem": bit5(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 5},191: { "levelId": 8, "mem": bit6(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 6},192: { "levelId": 8, "mem": bit7(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 7},193: { "levelId": 10, "mem": bit0(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 0},194: { "levelId": 10, "mem": bit1(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 1},195: { "levelId": 10, "mem": bit2(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 2},196: { "levelId": 10, "mem": bit3(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 3},197: { "levelId": 10, "mem": bit4(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 4},198: { "levelId": 10, "mem": bit2(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 2},199: { "levelId": 10, "mem": bit3(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 3},200: { "levelId": 10, "mem": bit4(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 4},201: { "levelId": 10, "mem": bit5(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 5},202: { "levelId": 10, "mem": bit6(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 6},203: { "levelId": 10, "mem": bit1(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 1},204: { "levelId": 10, "mem": bit5(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 5},205: { "levelId": 10, "mem": bit6(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 6},206: { "levelId": 10, "mem": bit7(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 7},207: { "levelId": 10, "mem": bit0(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 0},208: { "levelId": 10, "mem": bit3(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 3},209: { "levelId": 10, "mem": bit5(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 5},210: { "levelId": 10, "mem": bit6(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 6},211: { "levelId": 10, "mem": bit7(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 7},212: { "levelId": 10, "mem": bit0(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 0},213: { "levelId": 10, "mem": bit1(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 1},214: { "levelId": 10, "mem": bit2(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 2},215: { "levelId": 10, "mem": bit4(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 4},216: { "levelId": 11, "mem": bit6(0x2249e5),"good": 1, "addr": 0x2249e5, "bit": 6},217: { "levelId": 11, "mem": bit7(0x2249e5),"good": 1, "addr": 0x2249e5, "bit": 7},218: { "levelId": 11, "mem": bit0(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 0},219: { "levelId": 11, "mem": bit1(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 1},220: { "levelId": 11, "mem": bit2(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 2},221: { "levelId": 11, "mem": bit3(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 3},222: { "levelId": 11, "mem": bit4(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 4},223: { "levelId": 11, "mem": bit5(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 5},224: { "levelId": 11, "mem": bit6(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 6},225: { "levelId": 11, "mem": bit7(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 7},226: { "levelId": 11, "mem": bit0(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 0},227: { "levelId": 11, "mem": bit1(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 1},228: { "levelId": 11, "mem": bit2(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 2},229: { "levelId": 11, "mem": bit3(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 3},230: { "levelId": 11, "mem": bit4(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 4},231: { "levelId": 11, "mem": bit5(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 5},232: { "levelId": 11, "mem": bit6(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 6},233: { "levelId": 11, "mem": bit7(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 7},234: { "levelId": 11, "mem": bit0(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 0},235: { "levelId": 11, "mem": bit1(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 1},236: { "levelId": 11, "mem": bit2(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 2},237: { "levelId": 11, "mem": bit3(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 3},238: { "levelId": 11, "mem": bit4(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 4},239: { "levelId": 11, "mem": bit5(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 5},240: { "levelId": 11, "mem": bit6(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 6},241: { "levelId": 11, "mem": bit7(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 7},242: { "levelId": 11, "mem": bit0(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 0},243: { "levelId": 11, "mem": bit1(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 1},244: { "levelId": 11, "mem": bit2(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 2},245: { "levelId": 11, "mem": bit3(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 3},246: { "levelId": 11, "mem": bit4(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 4},247: { "levelId": 11, "mem": bit5(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 5},248: { "levelId": 11, "mem": bit6(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 6},249: { "levelId": 11, "mem": bit7(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 7},250: { "levelId": 11, "mem": bit0(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 0},251: { "levelId": 11, "mem": bit1(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 1},252: { "levelId": 11, "mem": bit2(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 2},253: { "levelId": 11, "mem": bit3(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 3},254: { "levelId": 11, "mem": bit4(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 4},255: { "levelId": 11, "mem": bit5(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 5},256: { "levelId": 11, "mem": bit6(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 6},257: { "levelId": 11, "mem": bit7(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 7},258: { "levelId": 11, "mem": bit0(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 0},259: { "levelId": 11, "mem": bit1(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 1},260: { "levelId": 11, "mem": bit2(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 2},261: { "levelId": 11, "mem": bit3(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 3},262: { "levelId": 11, "mem": bit4(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 4},263: { "levelId": 11, "mem": bit5(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 5},264: { "levelId": 11, "mem": bit6(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 6},265: { "levelId": 11, "mem": bit7(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 7},266: { "levelId": 10, "mem": bit2(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 2},267: { "levelId": 10, "mem": bit2(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 2},268: { "levelId": 10, "mem": bit3(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 3},269: { "levelId": 10, "mem": bit4(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 4},270: { "levelId": 10, "mem": bit0(0x2249a6),"good": 1, "addr": 0x2249a6, "bit": 0},271: { "levelId": 10, "mem": bit1(0x2249a6),"good": 1, "addr": 0x2249a6, "bit": 1},272: { "levelId": 10, "mem": bit2(0x2249a6),"good": 1, "addr": 0x2249a6, "bit": 2},273: { "levelId": 10, "mem": bit3(0x2249a6),"good": 1, "addr": 0x2249a6, "bit": 3},274: { "levelId": 10, "mem": bit6(0x2249a6),"good": 1, "addr": 0x2249a6, "bit": 6},275: { "levelId": 10, "mem": bit7(0x2249a6),"good": 1, "addr": 0x2249a6, "bit": 7},276: { "levelId": 10, "mem": bit0(0x2249a7),"good": 1, "addr": 0x2249a7, "bit": 0},277: { "levelId": 10, "mem": bit1(0x2249a7),"good": 1, "addr": 0x2249a7, "bit": 1},278: { "levelId": 10, "mem": bit5(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 5},279: { "levelId": 10, "mem": bit6(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 6},280: { "levelId": 10, "mem": bit7(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 7},281: { "levelId": 10, "mem": bit0(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 0},282: { "levelId": 10, "mem": bit1(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 1},283: { "levelId": 10, "mem": bit7(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 7},284: { "levelId": 10, "mem": bit0(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 0},285: { "levelId": 10, "mem": bit1(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 1},286: { "levelId": 10, "mem": bit3(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 3},287: { "levelId": 10, "mem": bit4(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 4},288: { "levelId": 10, "mem": bit5(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 5},289: { "levelId": 10, "mem": bit6(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 6},290: { "levelId": 10, "mem": bit7(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 7},291: { "levelId": 10, "mem": bit4(0x2249a6),"good": 1, "addr": 0x2249a6, "bit": 4},292: { "levelId": 10, "mem": bit5(0x2249a6),"good": 1, "addr": 0x2249a6, "bit": 5},293: { "levelId": 12, "mem": bit2(0x2249a7),"good": 1, "addr": 0x2249a7, "bit": 2},294: { "levelId": 12, "mem": bit3(0x2249a7),"good": 1, "addr": 0x2249a7, "bit": 3},295: { "levelId": 12, "mem": bit4(0x2249a7),"good": 1, "addr": 0x2249a7, "bit": 4},296: { "levelId": 12, "mem": bit5(0x2249a7),"good": 1, "addr": 0x2249a7, "bit": 5},297: { "levelId": 12, "mem": bit6(0x2249a7),"good": 1, "addr": 0x2249a7, "bit": 6},298: { "levelId": 12, "mem": bit7(0x2249a7),"good": 1, "addr": 0x2249a7, "bit": 7},299: { "levelId": 12, "mem": bit0(0x2249a8),"good": 1, "addr": 0x2249a8, "bit": 0},300: { "levelId": 12, "mem": bit1(0x2249a8),"good": 1, "addr": 0x2249a8, "bit": 1},301: { "levelId": 12, "mem": bit2(0x2249a8),"good": 1, "addr": 0x2249a8, "bit": 2},302: { "levelId": 12, "mem": bit3(0x2249a8),"good": 1, "addr": 0x2249a8, "bit": 3},303: { "levelId": 12, "mem": bit4(0x2249a8),"good": 1, "addr": 0x2249a8, "bit": 4},304: { "levelId": 12, "mem": bit5(0x2249a8),"good": 1, "addr": 0x2249a8, "bit": 5},305: { "levelId": 12, "mem": bit6(0x2249a8),"good": 1, "addr": 0x2249a8, "bit": 6},306: { "levelId": 12, "mem": bit7(0x2249a8),"good": 1, "addr": 0x2249a8, "bit": 7},307: { "levelId": 12, "mem": bit0(0x2249a9),"good": 1, "addr": 0x2249a9, "bit": 0},308: { "levelId": 12, "mem": bit1(0x2249a9),"good": 1, "addr": 0x2249a9, "bit": 1},309: { "levelId": 12, "mem": bit2(0x2249a9),"good": 1, "addr": 0x2249a9, "bit": 2},310: { "levelId": 12, "mem": bit3(0x2249a9),"good": 1, "addr": 0x2249a9, "bit": 3},311: { "levelId": 12, "mem": bit4(0x2249a9),"good": 1, "addr": 0x2249a9, "bit": 4},312: { "levelId": 12, "mem": bit5(0x2249a9),"good": 1, "addr": 0x2249a9, "bit": 5},313: { "levelId": 12, "mem": bit6(0x2249a9),"good": 1, "addr": 0x2249a9, "bit": 6},314: { "levelId": 12, "mem": bit1(0x2249aa),"good": 1, "addr": 0x2249aa, "bit": 1},315: { "levelId": 12, "mem": bit2(0x2249aa),"good": 1, "addr": 0x2249aa, "bit": 2},316: { "levelId": 12, "mem": bit2(0x2249ab),"good": 1, "addr": 0x2249ab, "bit": 2},317: { "levelId": 12, "mem": bit3(0x2249aa),"good": 1, "addr": 0x2249aa, "bit": 3},318: { "levelId": 12, "mem": bit4(0x2249ab),"good": 1, "addr": 0x2249ab, "bit": 4},319: { "levelId": 12, "mem": bit7(0x2249a9),"good": 1, "addr": 0x2249a9, "bit": 7},320: { "levelId": 12, "mem": bit0(0x2249aa),"good": 1, "addr": 0x2249aa, "bit": 0},321: { "levelId": 12, "mem": bit4(0x2249aa),"good": 1, "addr": 0x2249aa, "bit": 4},322: { "levelId": 12, "mem": bit5(0x2249aa),"good": 1, "addr": 0x2249aa, "bit": 5},323: { "levelId": 12, "mem": bit6(0x2249aa),"good": 1, "addr": 0x2249aa, "bit": 6},324: { "levelId": 12, "mem": bit7(0x2249aa),"good": 1, "addr": 0x2249aa, "bit": 7},325: { "levelId": 12, "mem": bit1(0x2249ab),"good": 1, "addr": 0x2249ab, "bit": 1},326: { "levelId": 12, "mem": bit3(0x2249ab),"good": 1, "addr": 0x2249ab, "bit": 3},327: { "levelId": 12, "mem": bit5(0x2249ab),"good": 1, "addr": 0x2249ab, "bit": 5},328: { "levelId": 12, "mem": bit0(0x2249ab),"good": 1, "addr": 0x2249ab, "bit": 0},329: { "levelId": 12, "mem": bit6(0x2249ab),"good": 1, "addr": 0x2249ab, "bit": 6},330: { "levelId": 12, "mem": bit7(0x2249ab),"good": 1, "addr": 0x2249ab, "bit": 7},331: { "levelId": 12, "mem": bit0(0x2249ac),"good": 1, "addr": 0x2249ac, "bit": 0},332: { "levelId": 12, "mem": bit1(0x2249ac),"good": 1, "addr": 0x2249ac, "bit": 1},333: { "levelId": 12, "mem": bit2(0x2249ac),"good": 1, "addr": 0x2249ac, "bit": 2},334: { "levelId": 12, "mem": bit3(0x2249ac),"good": 1, "addr": 0x2249ac, "bit": 3},335: { "levelId": 12, "mem": bit4(0x2249ac),"good": 1, "addr": 0x2249ac, "bit": 4},336: { "levelId": 12, "mem": bit5(0x2249ac),"good": 1, "addr": 0x2249ac, "bit": 5},337: { "levelId": 12, "mem": bit6(0x2249ac),"good": 1, "addr": 0x2249ac, "bit": 6},338: { "levelId": 12, "mem": bit7(0x2249ac),"good": 1, "addr": 0x2249ac, "bit": 7},339: { "levelId": 12, "mem": bit0(0x2249ad),"good": 1, "addr": 0x2249ad, "bit": 0},340: { "levelId": 12, "mem": bit1(0x2249ad),"good": 1, "addr": 0x2249ad, "bit": 1},341: { "levelId": 12, "mem": bit2(0x2249ad),"good": 1, "addr": 0x2249ad, "bit": 2},342: { "levelId": 12, "mem": bit3(0x2249ad),"good": 1, "addr": 0x2249ad, "bit": 3},343: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},344: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},345: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},346: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},347: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},348: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},349: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},350: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},351: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},352: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},353: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},354: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},355: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},356: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},357: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},358: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},359: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},360: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},361: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},362: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},363: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},364: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},365: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},366: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},367: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},368: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},369: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},370: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},371: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},372: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},373: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},374: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},375: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},376: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},377: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},378: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},379: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},380: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},381: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},382: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},383: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},384: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},385: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},386: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},387: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},388: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},389: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},390: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},391: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},392: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},393: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},394: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},395: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},396: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},397: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},398: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},399: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},400: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},401: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},402: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},403: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},404: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},405: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},406: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},407: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},408: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},409: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},410: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},411: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},412: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},413: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},414: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},415: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},416: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},417: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},418: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},419: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},420: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},421: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},422: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},423: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},424: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},425: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},426: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},427: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},428: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},429: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},430: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},431: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},432: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},433: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},434: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},435: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},436: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},437: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},438: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},439: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},440: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},441: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},442: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},443: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},444: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},445: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},446: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},447: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},448: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},449: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},450: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},451: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},452: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},453: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},454: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},455: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},456: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},457: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},458: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},459: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},460: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},461: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},462: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},463: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},464: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},465: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},466: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},467: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},468: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},469: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},470: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},471: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},472: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},473: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},474: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},475: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},476: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},477: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},478: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},479: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},480: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},481: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},482: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},483: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},484: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},485: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},486: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},487: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},488: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},489: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},490: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},491: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},492: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},493: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},494: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},495: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},496: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},497: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},498: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},499: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},500: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},501: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},502: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},503: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},504: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},505: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},506: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},507: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},508: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},509: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},510: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},511: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},512: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},513: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},514: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},515: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},516: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},517: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},518: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},519: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},520: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},521: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},522: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},523: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},524: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},525: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},526: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},527: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},528: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},529: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},530: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},531: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},532: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},533: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},534: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},535: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},536: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},537: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},538: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},539: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},540: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},541: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},542: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},543: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},544: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},545: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},546: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},547: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},548: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},549: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},550: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},551: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},552: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},553: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},554: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},555: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},556: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},557: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},558: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},559: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},560: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},561: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},562: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},563: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},564: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},565: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},566: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},567: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},568: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},569: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},570: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},571: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},572: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},573: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},574: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},575: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},576: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},577: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},578: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},579: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},580: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},581: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},582: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},583: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},584: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},585: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},586: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},587: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},588: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},589: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},590: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},591: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},592: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},593: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},594: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},595: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},596: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},597: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},598: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},599: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},600: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},601: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},602: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},603: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},604: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},605: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},606: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},607: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},608: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},609: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},610: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},611: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},612: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},613: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},614: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},615: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},616: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},617: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},618: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},619: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},620: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},621: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},622: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},623: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},624: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},625: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},626: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},627: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},628: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},629: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},630: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},631: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},632: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},633: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},634: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},635: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},636: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},637: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},638: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},639: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},640: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},641: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},642: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},643: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},644: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},645: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},646: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},647: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},648: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},649: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},650: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},651: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},652: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},653: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},654: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},655: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},656: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},657: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},658: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},659: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},660: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},661: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},662: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},663: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},664: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},665: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},666: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},667: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},668: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},669: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},670: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},671: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},672: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},673: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},674: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},675: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},676: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},677: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},678: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},679: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},680: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},681: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},682: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},683: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},684: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},685: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},686: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},687: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},688: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},689: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},690: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},691: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},692: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},693: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},694: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},695: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},696: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},697: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},698: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},699: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},700: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},701: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},702: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},703: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},704: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},705: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},706: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},707: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},708: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},709: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},710: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},711: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},712: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},713: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},714: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},715: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},716: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},717: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},718: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},719: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},720: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},721: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},722: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},723: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},724: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},725: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},726: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},727: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},728: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},729: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},730: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},731: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},732: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},733: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},734: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},735: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},736: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},737: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},738: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},739: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},740: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},741: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},742: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},743: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},744: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},745: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},746: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},747: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},748: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},749: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},750: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},751: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},752: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},753: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},754: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},755: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},756: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},757: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},758: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},759: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},760: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},761: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},762: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},763: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},764: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},765: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},766: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},767: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},768: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},769: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},770: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},771: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},772: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},773: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},774: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},775: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},776: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},777: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},778: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},779: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},780: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},781: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},782: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},783: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},784: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},785: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},786: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},787: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},788: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},789: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},790: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},791: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},792: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},793: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},794: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},795: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},796: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},797: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},798: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},799: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},800: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},801: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},802: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},803: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},804: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},805: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},806: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},807: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},808: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},809: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},810: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},811: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},812: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},813: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},814: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},815: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},816: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},817: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},818: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},819: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},820: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},821: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},822: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},823: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},824: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},825: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},826: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},827: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},828: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},829: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},830: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},831: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},832: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},833: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},834: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},835: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},836: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},837: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},838: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},839: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},840: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},841: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},842: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},843: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},844: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},845: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},846: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},847: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},848: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},849: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},850: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},851: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},852: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},853: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},854: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},855: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},856: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},857: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},858: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},859: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},860: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},861: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},862: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},863: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},864: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},865: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},866: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},867: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},868: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},869: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},870: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},871: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},872: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},873: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},874: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},875: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},876: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},877: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},878: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},879: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},880: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},881: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},882: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},883: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},884: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},885: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},886: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},887: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},888: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},889: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},890: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},891: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},892: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},893: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},894: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},895: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},896: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},897: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},898: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},899: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},900: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},901: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},902: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},903: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},904: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},905: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},906: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},907: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},908: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},909: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},910: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},911: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},912: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},913: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},914: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},915: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},916: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},917: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},918: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},919: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},920: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},921: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},922: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},923: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},924: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},925: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},926: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},927: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},928: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},929: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},930: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},931: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},932: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},933: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},934: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},935: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},936: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},937: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},938: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},939: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},940: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},941: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},942: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},943: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},944: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},945: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},946: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},947: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},948: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},949: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},950: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},951: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},952: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},953: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},954: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},955: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},956: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},957: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},958: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},959: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},960: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},961: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},962: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},963: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},964: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},965: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},966: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},967: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},968: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},969: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},970: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},971: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},972: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},973: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},974: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},975: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},976: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},977: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},978: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},979: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},980: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},981: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},982: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},983: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},984: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},985: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},986: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},987: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},988: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},989: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},990: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},991: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},992: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},993: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},994: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},995: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},996: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},997: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},998: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},999: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},1000: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>1: { "levelId": 2, "mem": bit0(0x224988),"good": 1, "addr": 0x224988, "bit": 0},2: { "levelId": 2, "mem": bit1(0x224988),"good": 1, "addr": 0x224988, "bit": 1},3: { "levelId": 2, "mem": bit2(0x224988),"good": 1, "addr": 0x224988, "bit": 2},4: { "levelId": 2, "mem": bit3(0x224988),"good": 1, "addr": 0x224988, "bit": 3},5: { "levelId": 2, "mem": bit4(0x224988),"good": 1, "addr": 0x224988, "bit": 4},6: { "levelId": 2, "mem": bit5(0x224988),"good": 1, "addr": 0x224988, "bit": 5},7: { "levelId": 2, "mem": bit6(0x224988),"good": 1, "addr": 0x224988, "bit": 6},8: { "levelId": 2, "mem": bit7(0x224988),"good": 1, "addr": 0x224988, "bit": 7},9: { "levelId": 2, "mem": bit2(0x224989),"good": 1, "addr": 0x224989, "bit": 2},10: { "levelId": 2, "mem": bit1(0x22498a),"good": 1, "addr": 0x22498a, "bit": 1},11: { "levelId": 2, "mem": bit2(0x22498a),"good": 1, "addr": 0x22498a, "bit": 2},12: { "levelId": 2, "mem": bit3(0x22498a),"good": 1, "addr": 0x22498a, "bit": 3},13: { "levelId": 2, "mem": bit4(0x22498a),"good": 1, "addr": 0x22498a, "bit": 4},14: { "levelId": 2, "mem": bit5(0x22498a),"good": 1, "addr": 0x22498a, "bit": 5},15: { "levelId": 2, "mem": bit6(0x22498a),"good": 1, "addr": 0x22498a, "bit": 6},16: { "levelId": 2, "mem": bit7(0x22498a),"good": 1, "addr": 0x22498a, "bit": 7},17: { "levelId": 2, "mem": bit5(0x22498b),"good": 1, "addr": 0x22498b, "bit": 5},18: { "levelId": 2, "mem": bit6(0x22498b),"good": 1, "addr": 0x22498b, "bit": 6},19: { "levelId": 2, "mem": bit7(0x22498b),"good": 1, "addr": 0x22498b, "bit": 7},20: { "levelId": 2, "mem": bit0(0x22498c),"good": 1, "addr": 0x22498c, "bit": 0},21: { "levelId": 2, "mem": bit1(0x22498c),"good": 1, "addr": 0x22498c, "bit": 1},22: { "levelId": 2, "mem": bit2(0x22498c),"good": 1, "addr": 0x22498c, "bit": 2},23: { "levelId": 2, "mem": bit3(0x22498c),"good": 1, "addr": 0x22498c, "bit": 3},24: { "levelId": 2, "mem": bit4(0x22498c),"good": 1, "addr": 0x22498c, "bit": 4},25: { "levelId": 2, "mem": bit5(0x22498c),"good": 1, "addr": 0x22498c, "bit": 5},26: { "levelId": 2, "mem": bit6(0x22498c),"good": 1, "addr": 0x22498c, "bit": 6},27: { "levelId": 2, "mem": bit7(0x22498c),"good": 1, "addr": 0x22498c, "bit": 7},28: { "levelId": 2, "mem": bit0(0x22498d),"good": 1, "addr": 0x22498d, "bit": 0},29: { "levelId": 2, "mem": bit1(0x22498d),"good": 1, "addr": 0x22498d, "bit": 1},30: { "levelId": 2, "mem": bit2(0x22498d),"good": 1, "addr": 0x22498d, "bit": 2},31: { "levelId": 2, "mem": bit3(0x22498d),"good": 1, "addr": 0x22498d, "bit": 3},32: { "levelId": 2, "mem": bit4(0x22498d),"good": 1, "addr": 0x22498d, "bit": 4},33: { "levelId": 2, "mem": bit5(0x22498d),"good": 1, "addr": 0x22498d, "bit": 5},34: { "levelId": 2, "mem": bit6(0x22498d),"good": 1, "addr": 0x22498d, "bit": 6},35: { "levelId": 2, "mem": bit7(0x22498d),"good": 1, "addr": 0x22498d, "bit": 7},36: { "levelId": 2, "mem": bit0(0x22498e),"good": 1, "addr": 0x22498e, "bit": 0},37: { "levelId": 2, "mem": bit1(0x22498e),"good": 1, "addr": 0x22498e, "bit": 1},38: { "levelId": 5, "mem": bit2(0x22498e),"good": 1, "addr": 0x22498e, "bit": 2},39: { "levelId": 5, "mem": bit3(0x22498e),"good": 1, "addr": 0x22498e, "bit": 3},40: { "levelId": 5, "mem": bit4(0x22498e),"good": 1, "addr": 0x22498e, "bit": 4},41: { "levelId": 5, "mem": bit5(0x22498e),"good": 1, "addr": 0x22498e, "bit": 5},42: { "levelId": 5, "mem": bit6(0x22498e),"good": 1, "addr": 0x22498e, "bit": 6},43: { "levelId": 5, "mem": bit7(0x22498e),"good": 1, "addr": 0x22498e, "bit": 7},44: { "levelId": 5, "mem": bit0(0x22498f),"good": 1, "addr": 0x22498f, "bit": 0},45: { "levelId": 5, "mem": bit1(0x22498f),"good": 1, "addr": 0x22498f, "bit": 1},46: { "levelId": 5, "mem": bit2(0x22498f),"good": 1, "addr": 0x22498f, "bit": 2},47: { "levelId": 5, "mem": bit3(0x22498f),"good": 1, "addr": 0x22498f, "bit": 3},48: { "levelId": 5, "mem": bit4(0x22498f),"good": 1, "addr": 0x22498f, "bit": 4},49: { "levelId": 5, "mem": bit5(0x22498f),"good": 1, "addr": 0x22498f, "bit": 5},50: { "levelId": 5, "mem": bit6(0x22498f),"good": 1, "addr": 0x22498f, "bit": 6},51: { "levelId": 5, "mem": bit7(0x22498f),"good": 1, "addr": 0x22498f, "bit": 7},52: { "levelId": 5, "mem": bit0(0x224990),"good": 1, "addr": 0x224990, "bit": 0},53: { "levelId": 5, "mem": bit1(0x224990),"good": 1, "addr": 0x224990, "bit": 1},54: { "levelId": 5, "mem": bit2(0x224990),"good": 1, "addr": 0x224990, "bit": 2},55: { "levelId": 5, "mem": bit3(0x224990),"good": 1, "addr": 0x224990, "bit": 3},56: { "levelId": 5, "mem": bit4(0x224990),"good": 1, "addr": 0x224990, "bit": 4},57: { "levelId": 5, "mem": bit5(0x224990),"good": 1, "addr": 0x224990, "bit": 5},58: { "levelId": 5, "mem": bit6(0x224990),"good": 1, "addr": 0x224990, "bit": 6},59: { "levelId": 5, "mem": bit7(0x224990),"good": 1, "addr": 0x224990, "bit": 7},60: { "levelId": 5, "mem": bit0(0x224991),"good": 1, "addr": 0x224991, "bit": 0},61: { "levelId": 5, "mem": bit1(0x224991),"good": 1, "addr": 0x224991, "bit": 1},62: { "levelId": 5, "mem": bit2(0x224991),"good": 1, "addr": 0x224991, "bit": 2},63: { "levelId": 5, "mem": bit3(0x224991),"good": 1, "addr": 0x224991, "bit": 3},64: { "levelId": 5, "mem": bit4(0x224991),"good": 1, "addr": 0x224991, "bit": 4},65: { "levelId": 5, "mem": bit5(0x224991),"good": 1, "addr": 0x224991, "bit": 5},66: { "levelId": 5, "mem": bit6(0x224991),"good": 1, "addr": 0x224991, "bit": 6},67: { "levelId": 5, "mem": bit7(0x224991),"good": 1, "addr": 0x224991, "bit": 7},68: { "levelId": 5, "mem": bit0(0x224992),"good": 1, "addr": 0x224992, "bit": 0},69: { "levelId": 5, "mem": bit1(0x224992),"good": 1, "addr": 0x224992, "bit": 1},70: { "levelId": 5, "mem": bit2(0x224992),"good": 1, "addr": 0x224992, "bit": 2},71: { "levelId": 5, "mem": bit3(0x224992),"good": 1, "addr": 0x224992, "bit": 3},72: { "levelId": 5, "mem": bit4(0x224992),"good": 1, "addr": 0x224992, "bit": 4},73: { "levelId": 5, "mem": bit5(0x224992),"good": 1, "addr": 0x224992, "bit": 5},74: { "levelId": 5, "mem": bit6(0x224992),"good": 1, "addr": 0x224992, "bit": 6},75: { "levelId": 5, "mem": bit7(0x224992),"good": 1, "addr": 0x224992, "bit": 7},76: { "levelId": 5, "mem": bit0(0x224993),"good": 1, "addr": 0x224993, "bit": 0},77: { "levelId": 5, "mem": bit1(0x224993),"good": 1, "addr": 0x224993, "bit": 1},78: { "levelId": 5, "mem": bit2(0x224993),"good": 1, "addr": 0x224993, "bit": 2},79: { "levelId": 5, "mem": bit3(0x224993),"good": 1, "addr": 0x224993, "bit": 3},80: { "levelId": 5, "mem": bit4(0x224993),"good": 1, "addr": 0x224993, "bit": 4},81: { "levelId": 5, "mem": bit5(0x224993),"good": 1, "addr": 0x224993, "bit": 5},82: { "levelId": 5, "mem": bit6(0x224993),"good": 1, "addr": 0x224993, "bit": 6},83: { "levelId": 5, "mem": bit7(0x224993),"good": 1, "addr": 0x224993, "bit": 7},84: { "levelId": 5, "mem": bit0(0x224994),"good": 1, "addr": 0x224994, "bit": 0},85: { "levelId": 5, "mem": bit1(0x224994),"good": 1, "addr": 0x224994, "bit": 1},86: { "levelId": 5, "mem": bit2(0x224994),"good": 1, "addr": 0x224994, "bit": 2},87: { "levelId": 5, "mem": bit3(0x224994),"good": 1, "addr": 0x224994, "bit": 3},88: { "levelId": 6, "mem": bit4(0x224994),"good": 1, "addr": 0x224994, "bit": 4},89: { "levelId": 6, "mem": bit5(0x224994),"good": 1, "addr": 0x224994, "bit": 5},90: { "levelId": 6, "mem": bit6(0x224994),"good": 1, "addr": 0x224994, "bit": 6},91: { "levelId": 6, "mem": bit7(0x224994),"good": 1, "addr": 0x224994, "bit": 7},92: { "levelId": 6, "mem": bit0(0x224995),"good": 1, "addr": 0x224995, "bit": 0},93: { "levelId": 6, "mem": bit1(0x224995),"good": 1, "addr": 0x224995, "bit": 1},94: { "levelId": 6, "mem": bit2(0x224995),"good": 1, "addr": 0x224995, "bit": 2},95: { "levelId": 6, "mem": bit3(0x224995),"good": 1, "addr": 0x224995, "bit": 3},96: { "levelId": 6, "mem": bit4(0x224995),"good": 1, "addr": 0x224995, "bit": 4},97: { "levelId": 6, "mem": bit5(0x224995),"good": 1, "addr": 0x224995, "bit": 5},98: { "levelId": 6, "mem": bit6(0x224995),"good": 1, "addr": 0x224995, "bit": 6},99: { "levelId": 6, "mem": bit7(0x224995),"good": 1, "addr": 0x224995, "bit": 7},100: { "levelId": 6, "mem": bit0(0x224996),"good": 1, "addr": 0x224996, "bit": 0},101: { "levelId": 6, "mem": bit1(0x224996),"good": 1, "addr": 0x224996, "bit": 1},102: { "levelId": 6, "mem": bit2(0x224996),"good": 1, "addr": 0x224996, "bit": 2},103: { "levelId": 6, "mem": bit3(0x224996),"good": 1, "addr": 0x224996, "bit": 3},104: { "levelId": 6, "mem": bit4(0x224996),"good": 1, "addr": 0x224996, "bit": 4},105: { "levelId": 6, "mem": bit5(0x224996),"good": 1, "addr": 0x224996, "bit": 5},106: { "levelId": 6, "mem": bit6(0x224996),"good": 1, "addr": 0x224996, "bit": 6},107: { "levelId": 6, "mem": bit7(0x224996),"good": 1, "addr": 0x224996, "bit": 7},108: { "levelId": 6, "mem": bit0(0x224997),"good": 1, "addr": 0x224997, "bit": 0},109: { "levelId": 6, "mem": bit1(0x224997),"good": 1, "addr": 0x224997, "bit": 1},110: { "levelId": 6, "mem": bit2(0x224997),"good": 1, "addr": 0x224997, "bit": 2},111: { "levelId": 6, "mem": bit3(0x224997),"good": 1, "addr": 0x224997, "bit": 3},112: { "levelId": 6, "mem": bit4(0x224997),"good": 1, "addr": 0x224997, "bit": 4},113: { "levelId": 6, "mem": bit5(0x224997),"good": 1, "addr": 0x224997, "bit": 5},114: { "levelId": 6, "mem": bit6(0x224997),"good": 1, "addr": 0x224997, "bit": 6},115: { "levelId": 6, "mem": bit7(0x224997),"good": 1, "addr": 0x224997, "bit": 7},116: { "levelId": 6, "mem": bit0(0x224998),"good": 1, "addr": 0x224998, "bit": 0},117: { "levelId": 6, "mem": bit1(0x224998),"good": 1, "addr": 0x224998, "bit": 1},118: { "levelId": 6, "mem": bit2(0x224998),"good": 1, "addr": 0x224998, "bit": 2},119: { "levelId": 6, "mem": bit3(0x224998),"good": 1, "addr": 0x224998, "bit": 3},120: { "levelId": 6, "mem": bit4(0x224998),"good": 1, "addr": 0x224998, "bit": 4},121: { "levelId": 6, "mem": bit5(0x224998),"good": 1, "addr": 0x224998, "bit": 5},122: { "levelId": 6, "mem": bit6(0x224998),"good": 1, "addr": 0x224998, "bit": 6},123: { "levelId": 6, "mem": bit0(0x224999),"good": 1, "addr": 0x224999, "bit": 0},124: { "levelId": 6, "mem": bit1(0x224999),"good": 1, "addr": 0x224999, "bit": 1},125: { "levelId": 6, "mem": bit2(0x224999),"good": 1, "addr": 0x224999, "bit": 2},126: { "levelId": 6, "mem": bit3(0x224999),"good": 1, "addr": 0x224999, "bit": 3},127: { "levelId": 6, "mem": bit4(0x224999),"good": 1, "addr": 0x224999, "bit": 4},128: { "levelId": 6, "mem": bit5(0x224999),"good": 1, "addr": 0x224999, "bit": 5},129: { "levelId": 6, "mem": bit6(0x224999),"good": 1, "addr": 0x224999, "bit": 6},130: { "levelId": 6, "mem": bit7(0x224999),"good": 1, "addr": 0x224999, "bit": 7},131: { "levelId": 6, "mem": bit0(0x22499a),"good": 1, "addr": 0x22499a, "bit": 0},132: { "levelId": 6, "mem": bit1(0x22499a),"good": 1, "addr": 0x22499a, "bit": 1},133: { "levelId": 6, "mem": bit2(0x22499a),"good": 1, "addr": 0x22499a, "bit": 2},134: { "levelId": 6, "mem": bit3(0x22499a),"good": 1, "addr": 0x22499a, "bit": 3},135: { "levelId": 6, "mem": bit4(0x22499a),"good": 1, "addr": 0x22499a, "bit": 4},136: { "levelId": 6, "mem": bit5(0x22499a),"good": 1, "addr": 0x22499a, "bit": 5},137: { "levelId": 1, "mem": bit3(0x224a36),"good": 1, "addr": 0x224a36, "bit": 3},138: { "levelId": 1, "mem": bit4(0x224a36),"good": 1, "addr": 0x224a36, "bit": 4},139: { "levelId": 1, "mem": bit5(0x224a36),"good": 1, "addr": 0x224a36, "bit": 5},140: { "levelId": 1, "mem": bit6(0x224a36),"good": 1, "addr": 0x224a36, "bit": 6},141: { "levelId": 1, "mem": bit7(0x224a36),"good": 1, "addr": 0x224a36, "bit": 7},142: { "levelId": 6, "mem": bit7(0x224998),"good": 1, "addr": 0x224998, "bit": 7},143: { "levelId": 8, "mem": bit3(0x22499b),"good": 1, "addr": 0x22499b, "bit": 3},144: { "levelId": 8, "mem": bit4(0x22499b),"good": 1, "addr": 0x22499b, "bit": 4},145: { "levelId": 8, "mem": bit5(0x22499b),"good": 1, "addr": 0x22499b, "bit": 5},146: { "levelId": 8, "mem": bit5(0x22499c),"good": 1, "addr": 0x22499c, "bit": 5},147: { "levelId": 8, "mem": bit6(0x22499c),"good": 1, "addr": 0x22499c, "bit": 6},148: { "levelId": 8, "mem": bit7(0x22499c),"good": 1, "addr": 0x22499c, "bit": 7},149: { "levelId": 8, "mem": bit0(0x22499d),"good": 1, "addr": 0x22499d, "bit": 0},150: { "levelId": 8, "mem": bit1(0x22499d),"good": 1, "addr": 0x22499d, "bit": 1},151: { "levelId": 8, "mem": bit2(0x22499d),"good": 1, "addr": 0x22499d, "bit": 2},152: { "levelId": 8, "mem": bit3(0x22499d),"good": 1, "addr": 0x22499d, "bit": 3},153: { "levelId": 8, "mem": bit4(0x22499d),"good": 1, "addr": 0x22499d, "bit": 4},154: { "levelId": 8, "mem": bit5(0x22499d),"good": 1, "addr": 0x22499d, "bit": 5},155: { "levelId": 8, "mem": bit6(0x22499d),"good": 1, "addr": 0x22499d, "bit": 6},156: { "levelId": 8, "mem": bit7(0x22499d),"good": 1, "addr": 0x22499d, "bit": 7},157: { "levelId": 8, "mem": bit0(0x22499e),"good": 1, "addr": 0x22499e, "bit": 0},158: { "levelId": 8, "mem": bit1(0x22499e),"good": 1, "addr": 0x22499e, "bit": 1},159: { "levelId": 8, "mem": bit6(0x22499a),"good": 1, "addr": 0x22499a, "bit": 6},160: { "levelId": 8, "mem": bit7(0x22499a),"good": 1, "addr": 0x22499a, "bit": 7},161: { "levelId": 8, "mem": bit0(0x22499b),"good": 1, "addr": 0x22499b, "bit": 0},162: { "levelId": 8, "mem": bit1(0x22499b),"good": 1, "addr": 0x22499b, "bit": 1},163: { "levelId": 8, "mem": bit2(0x22499b),"good": 1, "addr": 0x22499b, "bit": 2},164: { "levelId": 8, "mem": bit6(0x22499b),"good": 1, "addr": 0x22499b, "bit": 6},165: { "levelId": 8, "mem": bit7(0x22499b),"good": 1, "addr": 0x22499b, "bit": 7},166: { "levelId": 8, "mem": bit0(0x22499c),"good": 1, "addr": 0x22499c, "bit": 0},167: { "levelId": 8, "mem": bit1(0x22499c),"good": 1, "addr": 0x22499c, "bit": 1},168: { "levelId": 8, "mem": bit2(0x22499c),"good": 1, "addr": 0x22499c, "bit": 2},169: { "levelId": 8, "mem": bit3(0x22499c),"good": 1, "addr": 0x22499c, "bit": 3},170: { "levelId": 8, "mem": bit4(0x22499c),"good": 1, "addr": 0x22499c, "bit": 4},171: { "levelId": 8, "mem": bit2(0x22499e),"good": 1, "addr": 0x22499e, "bit": 2},172: { "levelId": 8, "mem": bit3(0x22499e),"good": 1, "addr": 0x22499e, "bit": 3},173: { "levelId": 8, "mem": bit4(0x22499e),"good": 1, "addr": 0x22499e, "bit": 4},174: { "levelId": 8, "mem": bit5(0x22499e),"good": 1, "addr": 0x22499e, "bit": 5},175: { "levelId": 8, "mem": bit6(0x22499e),"good": 1, "addr": 0x22499e, "bit": 6},176: { "levelId": 8, "mem": bit7(0x22499e),"good": 1, "addr": 0x22499e, "bit": 7},177: { "levelId": 8, "mem": bit0(0x22499f),"good": 1, "addr": 0x22499f, "bit": 0},178: { "levelId": 8, "mem": bit1(0x22499f),"good": 1, "addr": 0x22499f, "bit": 1},179: { "levelId": 8, "mem": bit2(0x22499f),"good": 1, "addr": 0x22499f, "bit": 2},180: { "levelId": 8, "mem": bit3(0x22499f),"good": 1, "addr": 0x22499f, "bit": 3},181: { "levelId": 8, "mem": bit4(0x22499f),"good": 1, "addr": 0x22499f, "bit": 4},182: { "levelId": 8, "mem": bit5(0x22499f),"good": 1, "addr": 0x22499f, "bit": 5},183: { "levelId": 8, "mem": bit6(0x22499f),"good": 1, "addr": 0x22499f, "bit": 6},184: { "levelId": 8, "mem": bit7(0x22499f),"good": 1, "addr": 0x22499f, "bit": 7},185: { "levelId": 8, "mem": bit0(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 0},186: { "levelId": 8, "mem": bit1(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 1},187: { "levelId": 8, "mem": bit2(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 2},188: { "levelId": 8, "mem": bit3(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 3},189: { "levelId": 8, "mem": bit4(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 4},190: { "levelId": 8, "mem": bit5(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 5},191: { "levelId": 8, "mem": bit6(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 6},192: { "levelId": 8, "mem": bit7(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 7},193: { "levelId": 10, "mem": bit0(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 0},194: { "levelId": 10, "mem": bit1(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 1},195: { "levelId": 10, "mem": bit2(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 2},196: { "levelId": 10, "mem": bit3(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 3},197: { "levelId": 10, "mem": bit4(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 4},198: { "levelId": 10, "mem": bit2(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 2},199: { "levelId": 10, "mem": bit3(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 3},200: { "levelId": 10, "mem": bit4(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 4},201: { "levelId": 10, "mem": bit5(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 5},202: { "levelId": 10, "mem": bit6(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 6},203: { "levelId": 10, "mem": bit1(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 1},204: { "levelId": 10, "mem": bit5(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 5},205: { "levelId": 10, "mem": bit6(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 6},206: { "levelId": 10, "mem": bit7(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 7},207: { "levelId": 10, "mem": bit0(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 0},208: { "levelId": 10, "mem": bit3(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 3},209: { "levelId": 10, "mem": bit5(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 5},210: { "levelId": 10, "mem": bit6(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 6},211: { "levelId": 10, "mem": bit7(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 7},212: { "levelId": 10, "mem": bit0(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 0},213: { "levelId": 10, "mem": bit1(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 1},214: { "levelId": 10, "mem": bit2(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 2},215: { "levelId": 10, "mem": bit4(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 4},216: { "levelId": 11, "mem": bit6(0x2249e5),"good": 1, "addr": 0x2249e5, "bit": 6},217: { "levelId": 11, "mem": bit7(0x2249e5),"good": 1, "addr": 0x2249e5, "bit": 7},218: { "levelId": 11, "mem": bit0(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 0},219: { "levelId": 11, "mem": bit1(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 1},220: { "levelId": 11, "mem": bit2(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 2},221: { "levelId": 11, "mem": bit3(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 3},222: { "levelId": 11, "mem": bit4(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 4},223: { "levelId": 11, "mem": bit5(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 5},224: { "levelId": 11, "mem": bit6(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 6},225: { "levelId": 11, "mem": bit7(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 7},226: { "levelId": 11, "mem": bit0(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 0},227: { "levelId": 11, "mem": bit1(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 1},228: { "levelId": 11, "mem": bit2(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 2},229: { "levelId": 11, "mem": bit3(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 3},230: { "levelId": 11, "mem": bit4(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 4},231: { "levelId": 11, "mem": bit5(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 5},232: { "levelId": 11, "mem": bit6(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 6},233: { "levelId": 11, "mem": bit7(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 7},234: { "levelId": 11, "mem": bit0(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 0},235: { "levelId": 11, "mem": bit1(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 1},236: { "levelId": 11, "mem": bit2(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 2},237: { "levelId": 11, "mem": bit3(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 3},238: { "levelId": 11, "mem": bit4(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 4},239: { "levelId": 11, "mem": bit5(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 5},240: { "levelId": 11, "mem": bit6(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 6},241: { "levelId": 11, "mem": bit7(0x2249e8),"good": 1, "addr": 0x2249e8, "bit": 7},242: { "levelId": 11, "mem": bit0(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 0},243: { "levelId": 11, "mem": bit1(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 1},244: { "levelId": 11, "mem": bit2(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 2},245: { "levelId": 11, "mem": bit3(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 3},246: { "levelId": 11, "mem": bit4(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 4},247: { "levelId": 11, "mem": bit5(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 5},248: { "levelId": 11, "mem": bit6(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 6},249: { "levelId": 11, "mem": bit7(0x2249e9),"good": 1, "addr": 0x2249e9, "bit": 7},250: { "levelId": 11, "mem": bit0(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 0},251: { "levelId": 11, "mem": bit1(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 1},252: { "levelId": 11, "mem": bit2(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 2},253: { "levelId": 11, "mem": bit3(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 3},254: { "levelId": 11, "mem": bit4(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 4},255: { "levelId": 11, "mem": bit5(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 5},256: { "levelId": 11, "mem": bit6(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 6},257: { "levelId": 11, "mem": bit7(0x2249ea),"good": 1, "addr": 0x2249ea, "bit": 7},258: { "levelId": 11, "mem": bit0(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 0},259: { "levelId": 11, "mem": bit1(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 1},260: { "levelId": 11, "mem": bit2(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 2},261: { "levelId": 11, "mem": bit3(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 3},262: { "levelId": 11, "mem": bit4(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 4},263: { "levelId": 11, "mem": bit5(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 5},264: { "levelId": 11, "mem": bit6(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 6},265: { "levelId": 11, "mem": bit7(0x2249eb),"good": 1, "addr": 0x2249eb, "bit": 7},266: { "levelId": 10, "mem": bit2(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 2},267: { "levelId": 10, "mem": bit2(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 2},268: { "levelId": 10, "mem": bit3(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 3},269: { "levelId": 10, "mem": bit4(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 4},270: { "levelId": 10, "mem": bit0(0x2249a6),"good": 1, "addr": 0x2249a6, "bit": 0},271: { "levelId": 10, "mem": bit1(0x2249a6),"good": 1, "addr": 0x2249a6, "bit": 1},272: { "levelId": 10, "mem": bit2(0x2249a6),"good": 1, "addr": 0x2249a6, "bit": 2},273: { "levelId": 10, "mem": bit3(0x2249a6),"good": 1, "addr": 0x2249a6, "bit": 3},274: { "levelId": 10, "mem": bit6(0x2249a6),"good": 1, "addr": 0x2249a6, "bit": 6},275: { "levelId": 10, "mem": bit7(0x2249a6),"good": 1, "addr": 0x2249a6, "bit": 7},276: { "levelId": 10, "mem": bit0(0x2249a7),"good": 1, "addr": 0x2249a7, "bit": 0},277: { "levelId": 10, "mem": bit1(0x2249a7),"good": 1, "addr": 0x2249a7, "bit": 1},278: { "levelId": 10, "mem": bit5(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 5},279: { "levelId": 10, "mem": bit6(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 6},280: { "levelId": 10, "mem": bit7(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 7},281: { "levelId": 10, "mem": bit0(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 0},282: { "levelId": 10, "mem": bit1(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 1},283: { "levelId": 10, "mem": bit7(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 7},284: { "levelId": 10, "mem": bit0(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 0},285: { "levelId": 10, "mem": bit1(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 1},286: { "levelId": 10, "mem": bit3(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 3},287: { "levelId": 10, "mem": bit4(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 4},288: { "levelId": 10, "mem": bit5(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 5},289: { "levelId": 10, "mem": bit6(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 6},290: { "levelId": 10, "mem": bit7(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 7},291: { "levelId": 10, "mem": bit4(0x2249a6),"good": 1, "addr": 0x2249a6, "bit": 4},292: { "levelId": 10, "mem": bit5(0x2249a6),"good": 1, "addr": 0x2249a6, "bit": 5},293: { "levelId": 12, "mem": bit2(0x2249a7),"good": 1, "addr": 0x2249a7, "bit": 2},294: { "levelId": 12, "mem": bit3(0x2249a7),"good": 1, "addr": 0x2249a7, "bit": 3},295: { "levelId": 12, "mem": bit4(0x2249a7),"good": 1, "addr": 0x2249a7, "bit": 4},296: { "levelId": 12, "mem": bit5(0x2249a7),"good": 1, "addr": 0x2249a7, "bit": 5},297: { "levelId": 12, "mem": bit6(0x2249a7),"good": 1, "addr": 0x2249a7, "bit": 6},298: { "levelId": 12, "mem": bit7(0x2249a7),"good": 1, "addr": 0x2249a7, "bit": 7},299: { "levelId": 12, "mem": bit0(0x2249a8),"good": 1, "addr": 0x2249a8, "bit": 0},300: { "levelId": 12, "mem": bit1(0x2249a8),"good": 1, "addr": 0x2249a8, "bit": 1},301: { "levelId": 12, "mem": bit2(0x2249a8),"good": 1, "addr": 0x2249a8, "bit": 2},302: { "levelId": 12, "mem": bit3(0x2249a8),"good": 1, "addr": 0x2249a8, "bit": 3},303: { "levelId": 12, "mem": bit4(0x2249a8),"good": 1, "addr": 0x2249a8, "bit": 4},304: { "levelId": 12, "mem": bit5(0x2249a8),"good": 1, "addr": 0x2249a8, "bit": 5},305: { "levelId": 12, "mem": bit6(0x2249a8),"good": 1, "addr": 0x2249a8, "bit": 6},306: { "levelId": 12, "mem": bit7(0x2249a8),"good": 1, "addr": 0x2249a8, "bit": 7},307: { "levelId": 12, "mem": bit0(0x2249a9),"good": 1, "addr": 0x2249a9, "bit": 0},308: { "levelId": 12, "mem": bit1(0x2249a9),"good": 1, "addr": 0x2249a9, "bit": 1},309: { "levelId": 12, "mem": bit2(0x2249a9),"good": 1, "addr": 0x2249a9, "bit": 2},310: { "levelId": 12, "mem": bit3(0x2249a9),"good": 1, "addr": 0x2249a9, "bit": 3},311: { "levelId": 12, "mem": bit4(0x2249a9),"good": 1, "addr": 0x2249a9, "bit": 4},312: { "levelId": 12, "mem": bit5(0x2249a9),"good": 1, "addr": 0x2249a9, "bit": 5},313: { "levelId": 12, "mem": bit6(0x2249a9),"good": 1, "addr": 0x2249a9, "bit": 6},314: { "levelId": 12, "mem": bit1(0x2249aa),"good": 1, "addr": 0x2249aa, "bit": 1},315: { "levelId": 12, "mem": bit2(0x2249aa),"good": 1, "addr": 0x2249aa, "bit": 2},316: { "levelId": 12, "mem": bit2(0x2249ab),"good": 1, "addr": 0x2249ab, "bit": 2},317: { "levelId": 12, "mem": bit3(0x2249aa),"good": 1, "addr": 0x2249aa, "bit": 3},318: { "levelId": 12, "mem": bit4(0x2249ab),"good": 1, "addr": 0x2249ab, "bit": 4},319: { "levelId": 12, "mem": bit7(0x2249a9),"good": 1, "addr": 0x2249a9, "bit": 7},320: { "levelId": 12, "mem": bit0(0x2249aa),"good": 1, "addr": 0x2249aa, "bit": 0},321: { "levelId": 12, "mem": bit4(0x2249aa),"good": 1, "addr": 0x2249aa, "bit": 4},322: { "levelId": 12, "mem": bit5(0x2249aa),"good": 1, "addr": 0x2249aa, "bit": 5},323: { "levelId": 12, "mem": bit6(0x2249aa),"good": 1, "addr": 0x2249aa, "bit": 6},324: { "levelId": 12, "mem": bit7(0x2249aa),"good": 1, "addr": 0x2249aa, "bit": 7},325: { "levelId": 12, "mem": bit1(0x2249ab),"good": 1, "addr": 0x2249ab, "bit": 1},326: { "levelId": 12, "mem": bit3(0x2249ab),"good": 1, "addr": 0x2249ab, "bit": 3},327: { "levelId": 12, "mem": bit5(0x2249ab),"good": 1, "addr": 0x2249ab, "bit": 5},328: { "levelId": 12, "mem": bit0(0x2249ab),"good": 1, "addr": 0x2249ab, "bit": 0},329: { "levelId": 12, "mem": bit6(0x2249ab),"good": 1, "addr": 0x2249ab, "bit": 6},330: { "levelId": 12, "mem": bit7(0x2249ab),"good": 1, "addr": 0x2249ab, "bit": 7},331: { "levelId": 12, "mem": bit0(0x2249ac),"good": 1, "addr": 0x2249ac, "bit": 0},332: { "levelId": 12, "mem": bit1(0x2249ac),"good": 1, "addr": 0x2249ac, "bit": 1},333: { "levelId": 12, "mem": bit2(0x2249ac),"good": 1, "addr": 0x2249ac, "bit": 2},334: { "levelId": 12, "mem": bit3(0x2249ac),"good": 1, "addr": 0x2249ac, "bit": 3},335: { "levelId": 12, "mem": bit4(0x2249ac),"good": 1, "addr": 0x2249ac, "bit": 4},336: { "levelId": 12, "mem": bit5(0x2249ac),"good": 1, "addr": 0x2249ac, "bit": 5},337: { "levelId": 12, "mem": bit6(0x2249ac),"good": 1, "addr": 0x2249ac, "bit": 6},338: { "levelId": 12, "mem": bit7(0x2249ac),"good": 1, "addr": 0x2249ac, "bit": 7},339: { "levelId": 12, "mem": bit0(0x2249ad),"good": 1, "addr": 0x2249ad, "bit": 0},340: { "levelId": 12, "mem": bit1(0x2249ad),"good": 1, "addr": 0x2249ad, "bit": 1},341: { "levelId": 12, "mem": bit2(0x2249ad),"good": 1, "addr": 0x2249ad, "bit": 2},342: { "levelId": 12, "mem": bit3(0x2249ad),"good": 1, "addr": 0x2249ad, "bit": 3},343: { "levelId": 13, "mem": bit4(0x2249ad),"good": 1, "addr": 0x2249ad, "bit": 4},344: { "levelId": 13, "mem": bit5(0x2249ad),"good": 1, "addr": 0x2249ad, "bit": 5},345: { "levelId": 13, "mem": bit6(0x2249ad),"good": 1, "addr": 0x2249ad, "bit": 6},346: { "levelId": 13, "mem": bit7(0x2249ad),"good": 1, "addr": 0x2249ad, "bit": 7},347: { "levelId": 13, "mem": bit0(0x2249ae),"good": 1, "addr": 0x2249ae, "bit": 0},348: { "levelId": 13, "mem": bit1(0x2249ae),"good": 1, "addr": 0x2249ae, "bit": 1},349: { "levelId": 13, "mem": bit2(0x2249ae),"good": 1, "addr": 0x2249ae, "bit": 2},350: { "levelId": 13, "mem": bit3(0x2249ae),"good": 1, "addr": 0x2249ae, "bit": 3},351: { "levelId": 13, "mem": bit4(0x2249ae),"good": 1, "addr": 0x2249ae, "bit": 4},352: { "levelId": 13, "mem": bit5(0x2249ae),"good": 1, "addr": 0x2249ae, "bit": 5},353: { "levelId": 13, "mem": bit6(0x2249ae),"good": 1, "addr": 0x2249ae, "bit": 6},354: { "levelId": 13, "mem": bit7(0x2249ae),"good": 1, "addr": 0x2249ae, "bit": 7},355: { "levelId": 13, "mem": bit0(0x2249af),"good": 1, "addr": 0x2249af, "bit": 0},356: { "levelId": 13, "mem": bit1(0x2249af),"good": 1, "addr": 0x2249af, "bit": 1},357: { "levelId": 13, "mem": bit2(0x2249af),"good": 1, "addr": 0x2249af, "bit": 2},358: { "levelId": 13, "mem": bit3(0x2249af),"good": 1, "addr": 0x2249af, "bit": 3},359: { "levelId": 13, "mem": bit4(0x2249af),"good": 1, "addr": 0x2249af, "bit": 4},360: { "levelId": 13, "mem": bit5(0x2249af),"good": 1, "addr": 0x2249af, "bit": 5},361: { "levelId": 13, "mem": bit6(0x2249af),"good": 1, "addr": 0x2249af, "bit": 6},362: { "levelId": 13, "mem": bit7(0x2249af),"good": 1, "addr": 0x2249af, "bit": 7},363: { "levelId": 13, "mem": bit0(0x2249b0),"good": 1, "addr": 0x2249b0, "bit": 0},364: { "levelId": 13, "mem": bit1(0x2249b0),"good": 1, "addr": 0x2249b0, "bit": 1},365: { "levelId": 13, "mem": bit2(0x2249b0),"good": 1, "addr": 0x2249b0, "bit": 2},366: { "levelId": 13, "mem": bit3(0x2249b0),"good": 1, "addr": 0x2249b0, "bit": 3},367: { "levelId": 13, "mem": bit4(0x2249b0),"good": 1, "addr": 0x2249b0, "bit": 4},368: { "levelId": 13, "mem": bit5(0x2249b0),"good": 1, "addr": 0x2249b0, "bit": 5},369: { "levelId": 13, "mem": bit6(0x2249b0),"good": 1, "addr": 0x2249b0, "bit": 6},370: { "levelId": 13, "mem": bit7(0x2249b0),"good": 1, "addr": 0x2249b0, "bit": 7},371: { "levelId": 13, "mem": bit0(0x2249b1),"good": 1, "addr": 0x2249b1, "bit": 0},372: { "levelId": 13, "mem": bit1(0x2249b1),"good": 1, "addr": 0x2249b1, "bit": 1},373: { "levelId": 13, "mem": bit2(0x2249b1),"good": 1, "addr": 0x2249b1, "bit": 2},374: { "levelId": 13, "mem": bit3(0x2249b1),"good": 1, "addr": 0x2249b1, "bit": 3},375: { "levelId": 13, "mem": bit4(0x2249b1),"good": 1, "addr": 0x2249b1, "bit": 4},376: { "levelId": 13, "mem": bit5(0x2249b1),"good": 1, "addr": 0x2249b1, "bit": 5},377: { "levelId": 13, "mem": bit6(0x2249b1),"good": 1, "addr": 0x2249b1, "bit": 6},378: { "levelId": 13, "mem": bit7(0x2249b1),"good": 1, "addr": 0x2249b1, "bit": 7},379: { "levelId": 13, "mem": bit0(0x2249b2),"good": 1, "addr": 0x2249b2, "bit": 0},380: { "levelId": 13, "mem": bit1(0x2249b2),"good": 1, "addr": 0x2249b2, "bit": 1},381: { "levelId": 13, "mem": bit2(0x2249b2),"good": 1, "addr": 0x2249b2, "bit": 2},382: { "levelId": 13, "mem": bit3(0x2249b2),"good": 1, "addr": 0x2249b2, "bit": 3},383: { "levelId": 13, "mem": bit4(0x2249b2),"good": 1, "addr": 0x2249b2, "bit": 4},384: { "levelId": 13, "mem": bit5(0x2249b2),"good": 1, "addr": 0x2249b2, "bit": 5},385: { "levelId": 13, "mem": bit6(0x2249b2),"good": 1, "addr": 0x2249b2, "bit": 6},386: { "levelId": 13, "mem": bit7(0x2249b2),"good": 1, "addr": 0x2249b2, "bit": 7},387: { "levelId": 13, "mem": bit0(0x2249b3),"good": 1, "addr": 0x2249b3, "bit": 0},388: { "levelId": 13, "mem": bit1(0x2249b3),"good": 1, "addr": 0x2249b3, "bit": 1},389: { "levelId": 13, "mem": bit2(0x2249b3),"good": 1, "addr": 0x2249b3, "bit": 2},390: { "levelId": 13, "mem": bit3(0x2249b3),"good": 1, "addr": 0x2249b3, "bit": 3},391: { "levelId": 13, "mem": bit4(0x2249b3),"good": 1, "addr": 0x2249b3, "bit": 4},392: { "levelId": 13, "mem": bit5(0x2249b3),"good": 1, "addr": 0x2249b3, "bit": 5},393: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},394: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},395: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},396: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},397: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},398: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},399: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},400: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},401: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},402: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},403: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},404: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},405: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},406: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},407: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},408: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},409: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},410: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},411: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},412: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},413: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},414: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},415: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},416: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},417: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},418: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},419: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},420: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},421: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},422: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},423: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},424: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},425: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},426: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},427: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},428: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},429: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},430: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},431: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},432: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},433: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},434: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},435: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},436: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},437: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},438: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},439: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},440: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},441: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},442: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},443: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},444: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},445: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},446: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},447: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},448: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},449: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},450: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},451: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},452: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},453: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},454: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},455: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},456: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},457: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},458: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},459: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},460: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},461: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},462: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},463: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},464: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},465: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},466: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},467: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},468: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},469: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},470: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},471: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},472: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},473: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},474: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},475: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},476: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},477: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},478: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},479: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},480: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},481: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},482: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},483: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},484: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},485: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},486: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},487: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},488: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},489: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},490: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},491: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},492: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},493: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},494: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},495: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},496: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},497: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},498: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},499: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},500: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},501: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},502: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},503: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},504: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},505: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},506: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},507: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},508: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},509: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},510: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},511: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},512: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},513: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},514: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},515: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},516: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},517: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},518: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},519: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},520: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},521: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},522: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},523: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},524: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},525: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},526: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},527: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},528: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},529: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},530: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},531: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},532: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},533: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},534: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},535: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},536: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},537: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},538: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},539: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},540: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},541: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},542: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},543: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},544: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},545: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},546: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},547: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},548: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},549: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},550: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},551: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},552: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},553: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},554: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},555: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},556: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},557: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},558: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},559: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},560: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},561: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},562: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},563: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},564: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},565: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},566: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},567: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},568: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},569: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},570: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},571: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},572: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},573: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},574: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},575: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},576: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},577: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},578: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},579: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},580: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},581: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},582: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},583: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},584: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},585: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},586: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},587: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},588: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},589: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},590: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},591: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},592: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},593: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},594: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},595: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},596: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},597: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},598: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},599: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},600: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},601: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},602: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},603: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},604: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},605: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},606: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},607: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},608: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},609: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},610: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},611: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},612: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},613: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},614: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},615: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},616: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},617: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},618: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},619: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},620: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},621: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},622: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},623: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},624: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},625: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},626: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},627: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},628: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},629: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},630: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},631: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},632: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},633: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},634: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},635: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},636: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},637: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},638: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},639: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},640: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},641: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},642: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},643: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},644: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},645: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},646: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},647: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},648: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},649: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},650: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},651: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},652: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},653: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},654: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},655: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},656: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},657: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},658: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},659: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},660: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},661: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},662: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},663: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},664: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},665: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},666: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},667: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},668: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},669: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},670: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},671: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},672: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},673: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},674: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},675: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},676: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},677: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},678: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},679: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},680: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},681: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},682: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},683: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},684: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},685: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},686: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},687: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},688: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},689: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},690: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},691: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},692: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},693: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},694: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},695: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},696: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},697: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},698: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},699: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},700: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},701: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},702: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},703: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},704: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},705: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},706: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},707: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},708: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},709: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},710: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},711: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},712: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},713: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},714: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},715: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},716: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},717: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},718: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},719: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},720: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},721: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},722: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},723: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},724: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},725: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},726: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},727: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},728: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},729: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},730: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},731: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},732: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},733: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},734: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},735: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},736: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},737: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},738: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},739: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},740: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},741: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},742: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},743: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},744: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},745: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},746: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},747: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},748: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},749: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},750: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},751: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},752: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},753: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},754: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},755: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},756: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},757: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},758: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},759: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},760: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},761: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},762: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},763: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},764: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},765: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},766: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},767: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},768: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},769: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},770: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},771: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},772: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},773: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},774: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},775: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},776: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},777: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},778: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},779: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},780: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},781: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},782: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},783: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},784: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},785: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},786: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},787: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},788: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},789: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},790: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},791: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},792: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},793: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},794: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},795: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},796: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},797: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},798: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},799: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},800: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},801: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},802: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},803: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},804: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},805: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},806: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},807: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},808: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},809: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},810: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},811: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},812: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},813: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},814: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},815: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},816: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},817: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},818: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},819: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},820: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},821: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},822: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},823: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},824: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},825: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},826: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},827: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},828: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},829: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},830: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},831: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},832: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},833: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},834: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},835: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},836: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},837: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},838: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},839: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},840: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},841: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},842: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},843: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},844: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},845: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},846: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},847: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},848: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},849: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},850: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},851: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},852: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},853: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},854: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},855: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},856: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},857: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},858: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},859: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},860: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},861: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},862: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},863: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},864: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},865: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},866: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},867: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},868: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},869: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},870: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},871: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},872: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},873: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},874: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},875: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},876: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},877: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},878: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},879: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},880: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},881: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},882: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},883: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},884: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},885: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},886: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},887: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},888: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},889: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},890: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},891: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},892: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},893: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},894: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},895: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},896: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},897: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},898: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},899: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},900: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},901: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},902: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},903: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},904: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},905: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},906: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},907: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},908: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},909: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},910: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},911: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},912: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},913: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},914: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},915: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},916: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},917: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},918: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},919: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},920: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},921: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},922: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},923: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},924: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},925: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},926: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},927: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},928: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},929: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},930: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},931: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},932: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},933: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},934: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},935: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},936: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},937: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},938: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},939: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},940: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},941: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},942: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},943: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},944: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},945: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},946: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},947: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},948: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},949: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},950: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},951: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},952: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},953: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},954: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},955: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},956: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},957: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},958: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},959: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},960: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},961: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},962: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},963: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},964: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},965: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},966: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},967: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},968: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},969: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},970: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},971: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},972: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},973: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},974: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},975: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},976: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},977: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},978: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},979: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},980: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},981: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},982: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},983: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},984: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},985: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},986: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},987: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},988: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},989: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},990: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},991: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},992: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},993: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},994: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},995: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},996: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},997: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},998: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},999: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},1000: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0</v>
@@ -8008,7 +8103,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1</v>
@@ -8024,7 +8119,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>2</v>
@@ -8040,7 +8135,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>3</v>
@@ -8056,7 +8151,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>4</v>
@@ -8072,7 +8167,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>5</v>
@@ -8088,7 +8183,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>6</v>
@@ -8104,7 +8199,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>7</v>
@@ -8120,7 +8215,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>2</v>
@@ -8135,7 +8230,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>1</v>
@@ -8150,7 +8245,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>2</v>
@@ -8165,7 +8260,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>3</v>
@@ -8180,7 +8275,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>4</v>
@@ -8195,7 +8290,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>5</v>
@@ -8210,7 +8305,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>6</v>
@@ -8225,7 +8320,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>7</v>
@@ -8240,7 +8335,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>5</v>
@@ -8255,7 +8350,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>6</v>
@@ -8270,7 +8365,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>7</v>
@@ -8285,7 +8380,7 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>0</v>
@@ -8300,7 +8395,7 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="6" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>1</v>
@@ -8315,7 +8410,7 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>2</v>
@@ -8330,7 +8425,7 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>3</v>
@@ -8345,7 +8440,7 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="6" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>4</v>
@@ -8360,7 +8455,7 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="6" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>5</v>
@@ -8375,7 +8470,7 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="6" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>6</v>
@@ -8390,7 +8485,7 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="6" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>7</v>
@@ -8405,7 +8500,7 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="6" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>0</v>
@@ -8420,7 +8515,7 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="6" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>1</v>
@@ -8435,7 +8530,7 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="6" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>2</v>
@@ -8450,7 +8545,7 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="6" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>3</v>
@@ -8465,7 +8560,7 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="6" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>4</v>
@@ -8480,7 +8575,7 @@
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="6" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>5</v>
@@ -8495,7 +8590,7 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="6" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>6</v>
@@ -8510,7 +8605,7 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="6" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>7</v>
@@ -8525,7 +8620,7 @@
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="6" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>0</v>
@@ -8540,7 +8635,7 @@
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="6" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>1</v>
@@ -8555,7 +8650,7 @@
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>2</v>
@@ -8570,7 +8665,7 @@
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>3</v>
@@ -8585,7 +8680,7 @@
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>4</v>
@@ -8600,7 +8695,7 @@
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>5</v>
@@ -8615,7 +8710,7 @@
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>6</v>
@@ -8630,7 +8725,7 @@
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="B44" s="0" t="n">
         <v>7</v>
@@ -8645,7 +8740,7 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="B45" s="0" t="n">
         <v>0</v>
@@ -8660,7 +8755,7 @@
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="B46" s="0" t="n">
         <v>1</v>
@@ -8675,7 +8770,7 @@
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="B47" s="0" t="n">
         <v>2</v>
@@ -8690,7 +8785,7 @@
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="B48" s="0" t="n">
         <v>3</v>
@@ -8705,7 +8800,7 @@
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="B49" s="0" t="n">
         <v>4</v>
@@ -8720,7 +8815,7 @@
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="B50" s="0" t="n">
         <v>5</v>
@@ -8735,7 +8830,7 @@
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="B51" s="0" t="n">
         <v>6</v>
@@ -8750,7 +8845,7 @@
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="B52" s="0" t="n">
         <v>7</v>
@@ -8765,7 +8860,7 @@
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="B53" s="0" t="n">
         <v>0</v>
@@ -8780,7 +8875,7 @@
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="B54" s="0" t="n">
         <v>1</v>
@@ -8795,7 +8890,7 @@
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="B55" s="0" t="n">
         <v>2</v>
@@ -8810,7 +8905,7 @@
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="B56" s="0" t="n">
         <v>3</v>
@@ -8825,7 +8920,7 @@
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="B57" s="0" t="n">
         <v>4</v>
@@ -8840,7 +8935,7 @@
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="B58" s="0" t="n">
         <v>5</v>
@@ -8855,7 +8950,7 @@
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="B59" s="0" t="n">
         <v>6</v>
@@ -8870,7 +8965,7 @@
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="B60" s="0" t="n">
         <v>7</v>
@@ -8885,7 +8980,7 @@
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="B61" s="0" t="n">
         <v>0</v>
@@ -8900,7 +8995,7 @@
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="B62" s="0" t="n">
         <v>1</v>
@@ -8915,7 +9010,7 @@
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="B63" s="0" t="n">
         <v>2</v>
@@ -8930,7 +9025,7 @@
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="B64" s="0" t="n">
         <v>3</v>
@@ -8945,7 +9040,7 @@
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="B65" s="0" t="n">
         <v>4</v>
@@ -8960,7 +9055,7 @@
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="B66" s="0" t="n">
         <v>5</v>
@@ -8975,7 +9070,7 @@
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="B67" s="0" t="n">
         <v>6</v>
@@ -8990,7 +9085,7 @@
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="B68" s="0" t="n">
         <v>7</v>
@@ -9005,7 +9100,7 @@
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="B69" s="0" t="n">
         <v>0</v>
@@ -9020,7 +9115,7 @@
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="B70" s="0" t="n">
         <v>1</v>
@@ -9035,7 +9130,7 @@
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="B71" s="0" t="n">
         <v>2</v>
@@ -9050,7 +9145,7 @@
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="B72" s="0" t="n">
         <v>3</v>
@@ -9065,7 +9160,7 @@
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="B73" s="0" t="n">
         <v>4</v>
@@ -9080,7 +9175,7 @@
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="B74" s="0" t="n">
         <v>5</v>
@@ -9095,7 +9190,7 @@
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="B75" s="0" t="n">
         <v>6</v>
@@ -9110,7 +9205,7 @@
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="B76" s="0" t="n">
         <v>7</v>
@@ -9125,7 +9220,7 @@
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="B77" s="0" t="n">
         <v>0</v>
@@ -9140,7 +9235,7 @@
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="B78" s="0" t="n">
         <v>1</v>
@@ -9155,7 +9250,7 @@
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="B79" s="0" t="n">
         <v>2</v>
@@ -9170,7 +9265,7 @@
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="B80" s="0" t="n">
         <v>3</v>
@@ -9185,7 +9280,7 @@
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="B81" s="0" t="n">
         <v>4</v>
@@ -9200,7 +9295,7 @@
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="B82" s="0" t="n">
         <v>5</v>
@@ -9215,7 +9310,7 @@
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="B83" s="0" t="n">
         <v>6</v>
@@ -9230,7 +9325,7 @@
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="B84" s="0" t="n">
         <v>7</v>
@@ -9245,7 +9340,7 @@
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="6" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="B85" s="0" t="n">
         <v>0</v>
@@ -9260,7 +9355,7 @@
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="6" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="B86" s="0" t="n">
         <v>1</v>
@@ -9275,7 +9370,7 @@
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="6" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="B87" s="0" t="n">
         <v>2</v>
@@ -9290,7 +9385,7 @@
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="6" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="B88" s="0" t="n">
         <v>3</v>
@@ -9305,7 +9400,7 @@
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="B89" s="0" t="n">
         <v>4</v>
@@ -9320,7 +9415,7 @@
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="B90" s="0" t="n">
         <v>5</v>
@@ -9335,7 +9430,7 @@
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="B91" s="0" t="n">
         <v>6</v>
@@ -9350,7 +9445,7 @@
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="B92" s="0" t="n">
         <v>7</v>
@@ -9365,7 +9460,7 @@
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="B93" s="0" t="n">
         <v>0</v>
@@ -9380,7 +9475,7 @@
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="B94" s="0" t="n">
         <v>1</v>
@@ -9395,7 +9490,7 @@
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="B95" s="0" t="n">
         <v>2</v>
@@ -9410,7 +9505,7 @@
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="B96" s="0" t="n">
         <v>3</v>
@@ -9425,7 +9520,7 @@
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="B97" s="0" t="n">
         <v>4</v>
@@ -9440,7 +9535,7 @@
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="B98" s="0" t="n">
         <v>5</v>
@@ -9455,7 +9550,7 @@
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="B99" s="0" t="n">
         <v>6</v>
@@ -9470,7 +9565,7 @@
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="B100" s="0" t="n">
         <v>7</v>
@@ -9485,7 +9580,7 @@
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="B101" s="0" t="n">
         <v>0</v>
@@ -9500,7 +9595,7 @@
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="B102" s="0" t="n">
         <v>1</v>
@@ -9515,7 +9610,7 @@
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="B103" s="0" t="n">
         <v>2</v>
@@ -9530,7 +9625,7 @@
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="B104" s="0" t="n">
         <v>3</v>
@@ -9545,7 +9640,7 @@
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="B105" s="0" t="n">
         <v>4</v>
@@ -9560,7 +9655,7 @@
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="B106" s="0" t="n">
         <v>5</v>
@@ -9575,7 +9670,7 @@
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="B107" s="0" t="n">
         <v>6</v>
@@ -9590,7 +9685,7 @@
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="B108" s="0" t="n">
         <v>7</v>
@@ -9605,7 +9700,7 @@
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="B109" s="0" t="n">
         <v>0</v>
@@ -9620,7 +9715,7 @@
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="B110" s="0" t="n">
         <v>1</v>
@@ -9635,7 +9730,7 @@
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="B111" s="0" t="n">
         <v>2</v>
@@ -9650,7 +9745,7 @@
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="B112" s="0" t="n">
         <v>3</v>
@@ -9665,7 +9760,7 @@
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="B113" s="0" t="n">
         <v>4</v>
@@ -9680,7 +9775,7 @@
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="B114" s="0" t="n">
         <v>5</v>
@@ -9695,7 +9790,7 @@
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="B115" s="0" t="n">
         <v>6</v>
@@ -9710,7 +9805,7 @@
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="B116" s="0" t="n">
         <v>7</v>
@@ -9725,7 +9820,7 @@
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="B117" s="0" t="n">
         <v>0</v>
@@ -9740,7 +9835,7 @@
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="B118" s="0" t="n">
         <v>1</v>
@@ -9755,7 +9850,7 @@
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="B119" s="0" t="n">
         <v>2</v>
@@ -9770,7 +9865,7 @@
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="B120" s="0" t="n">
         <v>3</v>
@@ -9785,7 +9880,7 @@
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="B121" s="0" t="n">
         <v>4</v>
@@ -9800,7 +9895,7 @@
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="B122" s="0" t="n">
         <v>5</v>
@@ -9815,7 +9910,7 @@
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="B123" s="0" t="n">
         <v>6</v>
@@ -9830,7 +9925,7 @@
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="B124" s="0" t="n">
         <v>0</v>
@@ -9845,7 +9940,7 @@
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="B125" s="0" t="n">
         <v>1</v>
@@ -9860,7 +9955,7 @@
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="B126" s="0" t="n">
         <v>2</v>
@@ -9875,7 +9970,7 @@
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="B127" s="0" t="n">
         <v>3</v>
@@ -9890,7 +9985,7 @@
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="B128" s="0" t="n">
         <v>4</v>
@@ -9905,7 +10000,7 @@
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="B129" s="0" t="n">
         <v>5</v>
@@ -9920,7 +10015,7 @@
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="B130" s="0" t="n">
         <v>6</v>
@@ -9935,7 +10030,7 @@
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="B131" s="0" t="n">
         <v>7</v>
@@ -9950,7 +10045,7 @@
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="B132" s="0" t="n">
         <v>0</v>
@@ -9965,7 +10060,7 @@
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="B133" s="0" t="n">
         <v>1</v>
@@ -9980,7 +10075,7 @@
     </row>
     <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="B134" s="0" t="n">
         <v>2</v>
@@ -9995,7 +10090,7 @@
     </row>
     <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="B135" s="0" t="n">
         <v>3</v>
@@ -10010,7 +10105,7 @@
     </row>
     <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="B136" s="0" t="n">
         <v>4</v>
@@ -10025,7 +10120,7 @@
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="B137" s="0" t="n">
         <v>5</v>
@@ -10040,7 +10135,7 @@
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="6" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="B138" s="0" t="n">
         <v>3</v>
@@ -10055,7 +10150,7 @@
     </row>
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="B139" s="0" t="n">
         <v>4</v>
@@ -10070,7 +10165,7 @@
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="B140" s="0" t="n">
         <v>5</v>
@@ -10085,7 +10180,7 @@
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="B141" s="0" t="n">
         <v>6</v>
@@ -10100,7 +10195,7 @@
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="B142" s="0" t="n">
         <v>7</v>
@@ -10115,7 +10210,7 @@
     </row>
     <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="B143" s="0" t="n">
         <v>7</v>
@@ -10130,7 +10225,7 @@
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="B144" s="0" t="n">
         <v>3</v>
@@ -10145,7 +10240,7 @@
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="B145" s="0" t="n">
         <v>4</v>
@@ -10160,7 +10255,7 @@
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="B146" s="0" t="n">
         <v>5</v>
@@ -10175,7 +10270,7 @@
     </row>
     <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="B147" s="0" t="n">
         <v>5</v>
@@ -10190,7 +10285,7 @@
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="B148" s="0" t="n">
         <v>6</v>
@@ -10205,7 +10300,7 @@
     </row>
     <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="B149" s="0" t="n">
         <v>7</v>
@@ -10220,7 +10315,7 @@
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="B150" s="0" t="n">
         <v>0</v>
@@ -10235,7 +10330,7 @@
     </row>
     <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="B151" s="0" t="n">
         <v>1</v>
@@ -10250,7 +10345,7 @@
     </row>
     <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="B152" s="0" t="n">
         <v>2</v>
@@ -10265,7 +10360,7 @@
     </row>
     <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="B153" s="0" t="n">
         <v>3</v>
@@ -10280,7 +10375,7 @@
     </row>
     <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="B154" s="0" t="n">
         <v>4</v>
@@ -10295,7 +10390,7 @@
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="B155" s="0" t="n">
         <v>5</v>
@@ -10310,7 +10405,7 @@
     </row>
     <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="B156" s="0" t="n">
         <v>6</v>
@@ -10325,7 +10420,7 @@
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="B157" s="0" t="n">
         <v>7</v>
@@ -10340,7 +10435,7 @@
     </row>
     <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="B158" s="0" t="n">
         <v>0</v>
@@ -10355,7 +10450,7 @@
     </row>
     <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="B159" s="0" t="n">
         <v>1</v>
@@ -10370,7 +10465,7 @@
     </row>
     <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="B160" s="0" t="n">
         <v>6</v>
@@ -10385,7 +10480,7 @@
     </row>
     <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="B161" s="0" t="n">
         <v>7</v>
@@ -10400,7 +10495,7 @@
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="B162" s="0" t="n">
         <v>0</v>
@@ -10415,7 +10510,7 @@
     </row>
     <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="B163" s="0" t="n">
         <v>1</v>
@@ -10430,7 +10525,7 @@
     </row>
     <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="B164" s="0" t="n">
         <v>2</v>
@@ -10445,7 +10540,7 @@
     </row>
     <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="B165" s="0" t="n">
         <v>6</v>
@@ -10460,7 +10555,7 @@
     </row>
     <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="B166" s="0" t="n">
         <v>7</v>
@@ -10475,7 +10570,7 @@
     </row>
     <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="B167" s="0" t="n">
         <v>0</v>
@@ -10490,7 +10585,7 @@
     </row>
     <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="B168" s="0" t="n">
         <v>1</v>
@@ -10505,7 +10600,7 @@
     </row>
     <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="B169" s="0" t="n">
         <v>2</v>
@@ -10520,7 +10615,7 @@
     </row>
     <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="B170" s="0" t="n">
         <v>3</v>
@@ -10535,7 +10630,7 @@
     </row>
     <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="B171" s="0" t="n">
         <v>4</v>
@@ -10550,7 +10645,7 @@
     </row>
     <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="B172" s="0" t="n">
         <v>2</v>
@@ -10565,7 +10660,7 @@
     </row>
     <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="B173" s="0" t="n">
         <v>3</v>
@@ -10580,7 +10675,7 @@
     </row>
     <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="B174" s="0" t="n">
         <v>4</v>
@@ -10595,7 +10690,7 @@
     </row>
     <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="B175" s="0" t="n">
         <v>5</v>
@@ -10610,7 +10705,7 @@
     </row>
     <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="B176" s="0" t="n">
         <v>6</v>
@@ -10625,7 +10720,7 @@
     </row>
     <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="B177" s="0" t="n">
         <v>7</v>
@@ -10640,7 +10735,7 @@
     </row>
     <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="B178" s="0" t="n">
         <v>0</v>
@@ -10655,7 +10750,7 @@
     </row>
     <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="B179" s="0" t="n">
         <v>1</v>
@@ -10670,7 +10765,7 @@
     </row>
     <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="B180" s="0" t="n">
         <v>2</v>
@@ -10685,7 +10780,7 @@
     </row>
     <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="B181" s="0" t="n">
         <v>3</v>
@@ -10700,7 +10795,7 @@
     </row>
     <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="B182" s="0" t="n">
         <v>4</v>
@@ -10715,7 +10810,7 @@
     </row>
     <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="0" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="B183" s="0" t="n">
         <v>5</v>
@@ -10730,7 +10825,7 @@
     </row>
     <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="0" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="B184" s="0" t="n">
         <v>6</v>
@@ -10745,7 +10840,7 @@
     </row>
     <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="B185" s="0" t="n">
         <v>7</v>
@@ -10760,7 +10855,7 @@
     </row>
     <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="B186" s="0" t="n">
         <v>0</v>
@@ -10775,7 +10870,7 @@
     </row>
     <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="0" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="B187" s="0" t="n">
         <v>1</v>
@@ -10790,7 +10885,7 @@
     </row>
     <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="0" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="B188" s="0" t="n">
         <v>2</v>
@@ -10805,7 +10900,7 @@
     </row>
     <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="0" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="B189" s="0" t="n">
         <v>3</v>
@@ -10820,7 +10915,7 @@
     </row>
     <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="0" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="B190" s="0" t="n">
         <v>4</v>
@@ -10835,7 +10930,7 @@
     </row>
     <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="0" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="B191" s="0" t="n">
         <v>5</v>
@@ -10850,7 +10945,7 @@
     </row>
     <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="0" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="B192" s="0" t="n">
         <v>6</v>
@@ -10865,7 +10960,7 @@
     </row>
     <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="0" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="B193" s="0" t="n">
         <v>7</v>
@@ -10880,7 +10975,7 @@
     </row>
     <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="0" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="B194" s="0" t="n">
         <v>0</v>
@@ -10895,7 +10990,7 @@
     </row>
     <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="0" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="B195" s="0" t="n">
         <v>1</v>
@@ -10910,7 +11005,7 @@
     </row>
     <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="0" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="B196" s="0" t="n">
         <v>2</v>
@@ -10925,7 +11020,7 @@
     </row>
     <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="0" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="B197" s="0" t="n">
         <v>3</v>
@@ -10940,7 +11035,7 @@
     </row>
     <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="0" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="B198" s="0" t="n">
         <v>4</v>
@@ -10955,7 +11050,7 @@
     </row>
     <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="0" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="B199" s="0" t="n">
         <v>2</v>
@@ -10970,7 +11065,7 @@
     </row>
     <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="B200" s="0" t="n">
         <v>3</v>
@@ -10985,7 +11080,7 @@
     </row>
     <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="0" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="B201" s="0" t="n">
         <v>4</v>
@@ -11000,7 +11095,7 @@
     </row>
     <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="0" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="B202" s="0" t="n">
         <v>5</v>
@@ -11015,7 +11110,7 @@
     </row>
     <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="0" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="B203" s="0" t="n">
         <v>6</v>
@@ -11030,7 +11125,7 @@
     </row>
     <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="0" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="B204" s="0" t="n">
         <v>1</v>
@@ -11045,7 +11140,7 @@
     </row>
     <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="0" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="B205" s="0" t="n">
         <v>5</v>
@@ -11060,7 +11155,7 @@
     </row>
     <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="0" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="B206" s="0" t="n">
         <v>6</v>
@@ -11075,7 +11170,7 @@
     </row>
     <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="0" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="B207" s="0" t="n">
         <v>7</v>
@@ -11090,7 +11185,7 @@
     </row>
     <row r="208" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="0" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="B208" s="0" t="n">
         <v>0</v>
@@ -11105,7 +11200,7 @@
     </row>
     <row r="209" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="0" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="B209" s="0" t="n">
         <v>3</v>
@@ -11120,7 +11215,7 @@
     </row>
     <row r="210" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="0" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="B210" s="0" t="n">
         <v>5</v>
@@ -11135,7 +11230,7 @@
     </row>
     <row r="211" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="0" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="B211" s="0" t="n">
         <v>6</v>
@@ -11150,7 +11245,7 @@
     </row>
     <row r="212" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="0" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="B212" s="0" t="n">
         <v>7</v>
@@ -11165,7 +11260,7 @@
     </row>
     <row r="213" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="0" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="B213" s="0" t="n">
         <v>0</v>
@@ -11180,7 +11275,7 @@
     </row>
     <row r="214" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="0" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="B214" s="0" t="n">
         <v>1</v>
@@ -11195,7 +11290,7 @@
     </row>
     <row r="215" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="0" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="B215" s="0" t="n">
         <v>2</v>
@@ -11210,7 +11305,7 @@
     </row>
     <row r="216" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="0" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="B216" s="0" t="n">
         <v>4</v>
@@ -11225,7 +11320,7 @@
     </row>
     <row r="217" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="0" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="B217" s="0" t="n">
         <v>6</v>
@@ -11240,7 +11335,7 @@
     </row>
     <row r="218" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="0" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="B218" s="0" t="n">
         <v>7</v>
@@ -11255,7 +11350,7 @@
     </row>
     <row r="219" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="0" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="B219" s="0" t="n">
         <v>0</v>
@@ -11270,7 +11365,7 @@
     </row>
     <row r="220" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="0" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="B220" s="0" t="n">
         <v>1</v>
@@ -11285,7 +11380,7 @@
     </row>
     <row r="221" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="0" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="B221" s="0" t="n">
         <v>2</v>
@@ -11300,7 +11395,7 @@
     </row>
     <row r="222" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="0" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="B222" s="0" t="n">
         <v>3</v>
@@ -11315,7 +11410,7 @@
     </row>
     <row r="223" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="0" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="B223" s="0" t="n">
         <v>4</v>
@@ -11330,7 +11425,7 @@
     </row>
     <row r="224" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="0" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="B224" s="0" t="n">
         <v>5</v>
@@ -11345,7 +11440,7 @@
     </row>
     <row r="225" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="0" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="B225" s="0" t="n">
         <v>6</v>
@@ -11360,7 +11455,7 @@
     </row>
     <row r="226" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="0" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="B226" s="0" t="n">
         <v>7</v>
@@ -11375,7 +11470,7 @@
     </row>
     <row r="227" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="0" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="B227" s="0" t="n">
         <v>0</v>
@@ -11390,7 +11485,7 @@
     </row>
     <row r="228" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="0" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="B228" s="0" t="n">
         <v>1</v>
@@ -11405,7 +11500,7 @@
     </row>
     <row r="229" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="0" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="B229" s="0" t="n">
         <v>2</v>
@@ -11420,7 +11515,7 @@
     </row>
     <row r="230" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="0" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="B230" s="0" t="n">
         <v>3</v>
@@ -11435,7 +11530,7 @@
     </row>
     <row r="231" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="0" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="B231" s="0" t="n">
         <v>4</v>
@@ -11450,7 +11545,7 @@
     </row>
     <row r="232" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="0" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="B232" s="0" t="n">
         <v>5</v>
@@ -11465,7 +11560,7 @@
     </row>
     <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="0" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="B233" s="0" t="n">
         <v>6</v>
@@ -11480,7 +11575,7 @@
     </row>
     <row r="234" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="0" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="B234" s="0" t="n">
         <v>7</v>
@@ -11495,7 +11590,7 @@
     </row>
     <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="0" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="B235" s="0" t="n">
         <v>0</v>
@@ -11510,7 +11605,7 @@
     </row>
     <row r="236" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="0" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="B236" s="0" t="n">
         <v>1</v>
@@ -11525,7 +11620,7 @@
     </row>
     <row r="237" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="0" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="B237" s="0" t="n">
         <v>2</v>
@@ -11540,7 +11635,7 @@
     </row>
     <row r="238" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="0" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="B238" s="0" t="n">
         <v>3</v>
@@ -11555,7 +11650,7 @@
     </row>
     <row r="239" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="0" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="B239" s="0" t="n">
         <v>4</v>
@@ -11570,7 +11665,7 @@
     </row>
     <row r="240" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="0" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="B240" s="0" t="n">
         <v>5</v>
@@ -11585,7 +11680,7 @@
     </row>
     <row r="241" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="0" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="B241" s="0" t="n">
         <v>6</v>
@@ -11600,7 +11695,7 @@
     </row>
     <row r="242" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="0" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="B242" s="0" t="n">
         <v>7</v>
@@ -11615,7 +11710,7 @@
     </row>
     <row r="243" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="0" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="B243" s="0" t="n">
         <v>0</v>
@@ -11630,7 +11725,7 @@
     </row>
     <row r="244" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="0" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="B244" s="0" t="n">
         <v>1</v>
@@ -11645,7 +11740,7 @@
     </row>
     <row r="245" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="0" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="B245" s="0" t="n">
         <v>2</v>
@@ -11660,7 +11755,7 @@
     </row>
     <row r="246" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="0" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="B246" s="0" t="n">
         <v>3</v>
@@ -11675,7 +11770,7 @@
     </row>
     <row r="247" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="0" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="B247" s="0" t="n">
         <v>4</v>
@@ -11690,7 +11785,7 @@
     </row>
     <row r="248" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="0" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="B248" s="0" t="n">
         <v>5</v>
@@ -11705,7 +11800,7 @@
     </row>
     <row r="249" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="0" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="B249" s="0" t="n">
         <v>6</v>
@@ -11720,7 +11815,7 @@
     </row>
     <row r="250" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="0" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="B250" s="0" t="n">
         <v>7</v>
@@ -11735,7 +11830,7 @@
     </row>
     <row r="251" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="0" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="B251" s="0" t="n">
         <v>0</v>
@@ -11750,7 +11845,7 @@
     </row>
     <row r="252" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="0" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="B252" s="0" t="n">
         <v>1</v>
@@ -11765,7 +11860,7 @@
     </row>
     <row r="253" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="0" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="B253" s="0" t="n">
         <v>2</v>
@@ -11780,7 +11875,7 @@
     </row>
     <row r="254" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="0" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="B254" s="0" t="n">
         <v>3</v>
@@ -11795,7 +11890,7 @@
     </row>
     <row r="255" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="0" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="B255" s="0" t="n">
         <v>4</v>
@@ -11810,7 +11905,7 @@
     </row>
     <row r="256" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="0" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="B256" s="0" t="n">
         <v>5</v>
@@ -11825,7 +11920,7 @@
     </row>
     <row r="257" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="0" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="B257" s="0" t="n">
         <v>6</v>
@@ -11840,7 +11935,7 @@
     </row>
     <row r="258" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="0" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="B258" s="0" t="n">
         <v>7</v>
@@ -11855,7 +11950,7 @@
     </row>
     <row r="259" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="0" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="B259" s="0" t="n">
         <v>0</v>
@@ -11870,7 +11965,7 @@
     </row>
     <row r="260" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="0" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="B260" s="0" t="n">
         <v>1</v>
@@ -11885,7 +11980,7 @@
     </row>
     <row r="261" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="0" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="B261" s="0" t="n">
         <v>2</v>
@@ -11900,7 +11995,7 @@
     </row>
     <row r="262" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="0" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="B262" s="0" t="n">
         <v>3</v>
@@ -11915,7 +12010,7 @@
     </row>
     <row r="263" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="0" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="B263" s="0" t="n">
         <v>4</v>
@@ -11930,7 +12025,7 @@
     </row>
     <row r="264" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="0" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="B264" s="0" t="n">
         <v>5</v>
@@ -11945,7 +12040,7 @@
     </row>
     <row r="265" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="0" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="B265" s="0" t="n">
         <v>6</v>
@@ -11960,7 +12055,7 @@
     </row>
     <row r="266" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="0" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="B266" s="0" t="n">
         <v>7</v>
@@ -11975,7 +12070,7 @@
     </row>
     <row r="267" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="0" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="B267" s="0" t="n">
         <v>2</v>
@@ -11990,7 +12085,7 @@
     </row>
     <row r="268" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="0" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="B268" s="0" t="n">
         <v>2</v>
@@ -12005,7 +12100,7 @@
     </row>
     <row r="269" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="0" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="B269" s="0" t="n">
         <v>3</v>
@@ -12020,7 +12115,7 @@
     </row>
     <row r="270" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="0" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="B270" s="0" t="n">
         <v>4</v>
@@ -12035,7 +12130,7 @@
     </row>
     <row r="271" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="0" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B271" s="0" t="n">
         <v>0</v>
@@ -12050,7 +12145,7 @@
     </row>
     <row r="272" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="0" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B272" s="0" t="n">
         <v>1</v>
@@ -12065,7 +12160,7 @@
     </row>
     <row r="273" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="0" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B273" s="0" t="n">
         <v>2</v>
@@ -12080,7 +12175,7 @@
     </row>
     <row r="274" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A274" s="0" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B274" s="0" t="n">
         <v>3</v>
@@ -12095,7 +12190,7 @@
     </row>
     <row r="275" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="0" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B275" s="0" t="n">
         <v>6</v>
@@ -12110,7 +12205,7 @@
     </row>
     <row r="276" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="0" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B276" s="0" t="n">
         <v>7</v>
@@ -12125,7 +12220,7 @@
     </row>
     <row r="277" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="0" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="B277" s="0" t="n">
         <v>0</v>
@@ -12140,7 +12235,7 @@
     </row>
     <row r="278" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="0" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="B278" s="0" t="n">
         <v>1</v>
@@ -12155,7 +12250,7 @@
     </row>
     <row r="279" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A279" s="0" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="B279" s="0" t="n">
         <v>5</v>
@@ -12170,7 +12265,7 @@
     </row>
     <row r="280" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="0" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="B280" s="0" t="n">
         <v>6</v>
@@ -12185,7 +12280,7 @@
     </row>
     <row r="281" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A281" s="0" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="B281" s="0" t="n">
         <v>7</v>
@@ -12200,7 +12295,7 @@
     </row>
     <row r="282" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="0" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="B282" s="0" t="n">
         <v>0</v>
@@ -12215,7 +12310,7 @@
     </row>
     <row r="283" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A283" s="0" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="B283" s="0" t="n">
         <v>1</v>
@@ -12230,7 +12325,7 @@
     </row>
     <row r="284" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="0" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="B284" s="0" t="n">
         <v>7</v>
@@ -12245,7 +12340,7 @@
     </row>
     <row r="285" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="0" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="B285" s="0" t="n">
         <v>0</v>
@@ -12260,7 +12355,7 @@
     </row>
     <row r="286" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="0" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="B286" s="0" t="n">
         <v>1</v>
@@ -12275,7 +12370,7 @@
     </row>
     <row r="287" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="0" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="B287" s="0" t="n">
         <v>3</v>
@@ -12290,7 +12385,7 @@
     </row>
     <row r="288" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A288" s="0" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="B288" s="0" t="n">
         <v>4</v>
@@ -12305,7 +12400,7 @@
     </row>
     <row r="289" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="0" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="B289" s="0" t="n">
         <v>5</v>
@@ -12320,7 +12415,7 @@
     </row>
     <row r="290" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="0" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="B290" s="0" t="n">
         <v>6</v>
@@ -12335,7 +12430,7 @@
     </row>
     <row r="291" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A291" s="0" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="B291" s="0" t="n">
         <v>7</v>
@@ -12350,7 +12445,7 @@
     </row>
     <row r="292" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="0" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B292" s="0" t="n">
         <v>4</v>
@@ -12365,7 +12460,7 @@
     </row>
     <row r="293" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A293" s="0" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B293" s="0" t="n">
         <v>5</v>
@@ -12380,7 +12475,7 @@
     </row>
     <row r="294" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A294" s="0" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="B294" s="0" t="n">
         <v>2</v>
@@ -12395,7 +12490,7 @@
     </row>
     <row r="295" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A295" s="0" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="B295" s="0" t="n">
         <v>3</v>
@@ -12410,7 +12505,7 @@
     </row>
     <row r="296" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A296" s="0" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="B296" s="0" t="n">
         <v>4</v>
@@ -12425,7 +12520,7 @@
     </row>
     <row r="297" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A297" s="0" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="B297" s="0" t="n">
         <v>5</v>
@@ -12440,7 +12535,7 @@
     </row>
     <row r="298" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A298" s="0" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="B298" s="0" t="n">
         <v>6</v>
@@ -12455,7 +12550,7 @@
     </row>
     <row r="299" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A299" s="0" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="B299" s="0" t="n">
         <v>7</v>
@@ -12470,7 +12565,7 @@
     </row>
     <row r="300" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="0" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="B300" s="0" t="n">
         <v>0</v>
@@ -12485,7 +12580,7 @@
     </row>
     <row r="301" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A301" s="0" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="B301" s="0" t="n">
         <v>1</v>
@@ -12500,7 +12595,7 @@
     </row>
     <row r="302" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A302" s="0" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="B302" s="0" t="n">
         <v>2</v>
@@ -12515,7 +12610,7 @@
     </row>
     <row r="303" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A303" s="0" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="B303" s="0" t="n">
         <v>3</v>
@@ -12530,7 +12625,7 @@
     </row>
     <row r="304" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A304" s="0" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="B304" s="0" t="n">
         <v>4</v>
@@ -12545,7 +12640,7 @@
     </row>
     <row r="305" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A305" s="0" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="B305" s="0" t="n">
         <v>5</v>
@@ -12560,7 +12655,7 @@
     </row>
     <row r="306" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A306" s="0" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="B306" s="0" t="n">
         <v>6</v>
@@ -12575,7 +12670,7 @@
     </row>
     <row r="307" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A307" s="0" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="B307" s="0" t="n">
         <v>7</v>
@@ -12590,7 +12685,7 @@
     </row>
     <row r="308" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A308" s="0" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="B308" s="0" t="n">
         <v>0</v>
@@ -12605,7 +12700,7 @@
     </row>
     <row r="309" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A309" s="0" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="B309" s="0" t="n">
         <v>1</v>
@@ -12620,7 +12715,7 @@
     </row>
     <row r="310" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A310" s="0" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="B310" s="0" t="n">
         <v>2</v>
@@ -12635,7 +12730,7 @@
     </row>
     <row r="311" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A311" s="0" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="B311" s="0" t="n">
         <v>3</v>
@@ -12650,7 +12745,7 @@
     </row>
     <row r="312" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="0" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="B312" s="0" t="n">
         <v>4</v>
@@ -12665,7 +12760,7 @@
     </row>
     <row r="313" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A313" s="0" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="B313" s="0" t="n">
         <v>5</v>
@@ -12680,7 +12775,7 @@
     </row>
     <row r="314" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A314" s="0" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="B314" s="0" t="n">
         <v>6</v>
@@ -12695,7 +12790,7 @@
     </row>
     <row r="315" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A315" s="0" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="B315" s="0" t="n">
         <v>1</v>
@@ -12710,7 +12805,7 @@
     </row>
     <row r="316" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A316" s="0" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="B316" s="0" t="n">
         <v>2</v>
@@ -12725,7 +12820,7 @@
     </row>
     <row r="317" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A317" s="0" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="B317" s="0" t="n">
         <v>2</v>
@@ -12740,7 +12835,7 @@
     </row>
     <row r="318" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A318" s="0" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="B318" s="0" t="n">
         <v>3</v>
@@ -12755,7 +12850,7 @@
     </row>
     <row r="319" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A319" s="0" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="B319" s="0" t="n">
         <v>4</v>
@@ -12770,7 +12865,7 @@
     </row>
     <row r="320" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A320" s="0" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="B320" s="0" t="n">
         <v>7</v>
@@ -12785,7 +12880,7 @@
     </row>
     <row r="321" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A321" s="0" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="B321" s="0" t="n">
         <v>0</v>
@@ -12800,7 +12895,7 @@
     </row>
     <row r="322" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A322" s="0" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="B322" s="0" t="n">
         <v>4</v>
@@ -12815,7 +12910,7 @@
     </row>
     <row r="323" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A323" s="0" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="B323" s="0" t="n">
         <v>5</v>
@@ -12830,7 +12925,7 @@
     </row>
     <row r="324" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A324" s="0" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="B324" s="0" t="n">
         <v>6</v>
@@ -12845,7 +12940,7 @@
     </row>
     <row r="325" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A325" s="0" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="B325" s="0" t="n">
         <v>7</v>
@@ -12860,7 +12955,7 @@
     </row>
     <row r="326" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A326" s="0" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="B326" s="0" t="n">
         <v>1</v>
@@ -12875,7 +12970,7 @@
     </row>
     <row r="327" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A327" s="0" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="B327" s="0" t="n">
         <v>3</v>
@@ -12890,7 +12985,7 @@
     </row>
     <row r="328" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A328" s="0" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="B328" s="0" t="n">
         <v>5</v>
@@ -12905,7 +13000,7 @@
     </row>
     <row r="329" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A329" s="0" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="B329" s="0" t="n">
         <v>0</v>
@@ -12920,7 +13015,7 @@
     </row>
     <row r="330" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A330" s="0" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="B330" s="0" t="n">
         <v>6</v>
@@ -12935,7 +13030,7 @@
     </row>
     <row r="331" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A331" s="0" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="B331" s="0" t="n">
         <v>7</v>
@@ -12950,7 +13045,7 @@
     </row>
     <row r="332" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A332" s="0" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="B332" s="0" t="n">
         <v>0</v>
@@ -12965,7 +13060,7 @@
     </row>
     <row r="333" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A333" s="0" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="B333" s="0" t="n">
         <v>1</v>
@@ -12980,7 +13075,7 @@
     </row>
     <row r="334" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A334" s="0" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="B334" s="0" t="n">
         <v>2</v>
@@ -12995,7 +13090,7 @@
     </row>
     <row r="335" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A335" s="0" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="B335" s="0" t="n">
         <v>3</v>
@@ -13010,7 +13105,7 @@
     </row>
     <row r="336" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A336" s="0" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="B336" s="0" t="n">
         <v>4</v>
@@ -13025,7 +13120,7 @@
     </row>
     <row r="337" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A337" s="0" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="B337" s="0" t="n">
         <v>5</v>
@@ -13040,7 +13135,7 @@
     </row>
     <row r="338" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A338" s="0" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="B338" s="0" t="n">
         <v>6</v>
@@ -13055,7 +13150,7 @@
     </row>
     <row r="339" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A339" s="0" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="B339" s="0" t="n">
         <v>7</v>
@@ -13070,7 +13165,7 @@
     </row>
     <row r="340" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A340" s="0" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="B340" s="0" t="n">
         <v>0</v>
@@ -13085,7 +13180,7 @@
     </row>
     <row r="341" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A341" s="0" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="B341" s="0" t="n">
         <v>1</v>
@@ -13100,7 +13195,7 @@
     </row>
     <row r="342" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A342" s="0" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="B342" s="0" t="n">
         <v>2</v>
@@ -13115,7 +13210,7 @@
     </row>
     <row r="343" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A343" s="0" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="B343" s="0" t="n">
         <v>3</v>
@@ -13129,453 +13224,753 @@
       </c>
     </row>
     <row r="344" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A344" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="B344" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="C344" s="4" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="D344" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C344, Levels!B:B, 0), 1, 1)),", ",IF(A344 &lt;&gt; "", """mem"": bit" &amp; B344 &amp; "(" &amp; A344 &amp; "),", ""),"""good"": ",IF(A344 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A344 &lt;&gt; "", A344, -1),", ""bit"": ",IF(B344 &lt;&gt; "", B344, -1),"},")</f>
-        <v>343: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>343: { "levelId": 13, "mem": bit4(0x2249ad),"good": 1, "addr": 0x2249ad, "bit": 4},</v>
       </c>
     </row>
     <row r="345" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A345" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="B345" s="0" t="n">
+        <v>5</v>
+      </c>
       <c r="C345" s="4" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="D345" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C345, Levels!B:B, 0), 1, 1)),", ",IF(A345 &lt;&gt; "", """mem"": bit" &amp; B345 &amp; "(" &amp; A345 &amp; "),", ""),"""good"": ",IF(A345 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A345 &lt;&gt; "", A345, -1),", ""bit"": ",IF(B345 &lt;&gt; "", B345, -1),"},")</f>
-        <v>344: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>344: { "levelId": 13, "mem": bit5(0x2249ad),"good": 1, "addr": 0x2249ad, "bit": 5},</v>
       </c>
     </row>
     <row r="346" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A346" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="B346" s="0" t="n">
+        <v>6</v>
+      </c>
       <c r="C346" s="4" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="D346" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C346, Levels!B:B, 0), 1, 1)),", ",IF(A346 &lt;&gt; "", """mem"": bit" &amp; B346 &amp; "(" &amp; A346 &amp; "),", ""),"""good"": ",IF(A346 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A346 &lt;&gt; "", A346, -1),", ""bit"": ",IF(B346 &lt;&gt; "", B346, -1),"},")</f>
-        <v>345: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>345: { "levelId": 13, "mem": bit6(0x2249ad),"good": 1, "addr": 0x2249ad, "bit": 6},</v>
       </c>
     </row>
     <row r="347" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A347" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="B347" s="0" t="n">
+        <v>7</v>
+      </c>
       <c r="C347" s="4" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="D347" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C347, Levels!B:B, 0), 1, 1)),", ",IF(A347 &lt;&gt; "", """mem"": bit" &amp; B347 &amp; "(" &amp; A347 &amp; "),", ""),"""good"": ",IF(A347 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A347 &lt;&gt; "", A347, -1),", ""bit"": ",IF(B347 &lt;&gt; "", B347, -1),"},")</f>
-        <v>346: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>346: { "levelId": 13, "mem": bit7(0x2249ad),"good": 1, "addr": 0x2249ad, "bit": 7},</v>
       </c>
     </row>
     <row r="348" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A348" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B348" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="C348" s="4" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="D348" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C348, Levels!B:B, 0), 1, 1)),", ",IF(A348 &lt;&gt; "", """mem"": bit" &amp; B348 &amp; "(" &amp; A348 &amp; "),", ""),"""good"": ",IF(A348 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A348 &lt;&gt; "", A348, -1),", ""bit"": ",IF(B348 &lt;&gt; "", B348, -1),"},")</f>
-        <v>347: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>347: { "levelId": 13, "mem": bit0(0x2249ae),"good": 1, "addr": 0x2249ae, "bit": 0},</v>
       </c>
     </row>
     <row r="349" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A349" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B349" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="C349" s="4" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="D349" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C349, Levels!B:B, 0), 1, 1)),", ",IF(A349 &lt;&gt; "", """mem"": bit" &amp; B349 &amp; "(" &amp; A349 &amp; "),", ""),"""good"": ",IF(A349 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A349 &lt;&gt; "", A349, -1),", ""bit"": ",IF(B349 &lt;&gt; "", B349, -1),"},")</f>
-        <v>348: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>348: { "levelId": 13, "mem": bit1(0x2249ae),"good": 1, "addr": 0x2249ae, "bit": 1},</v>
       </c>
     </row>
     <row r="350" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A350" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B350" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="C350" s="4" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="D350" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C350, Levels!B:B, 0), 1, 1)),", ",IF(A350 &lt;&gt; "", """mem"": bit" &amp; B350 &amp; "(" &amp; A350 &amp; "),", ""),"""good"": ",IF(A350 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A350 &lt;&gt; "", A350, -1),", ""bit"": ",IF(B350 &lt;&gt; "", B350, -1),"},")</f>
-        <v>349: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>349: { "levelId": 13, "mem": bit2(0x2249ae),"good": 1, "addr": 0x2249ae, "bit": 2},</v>
       </c>
     </row>
     <row r="351" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A351" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B351" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="C351" s="4" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="D351" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C351, Levels!B:B, 0), 1, 1)),", ",IF(A351 &lt;&gt; "", """mem"": bit" &amp; B351 &amp; "(" &amp; A351 &amp; "),", ""),"""good"": ",IF(A351 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A351 &lt;&gt; "", A351, -1),", ""bit"": ",IF(B351 &lt;&gt; "", B351, -1),"},")</f>
-        <v>350: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>350: { "levelId": 13, "mem": bit3(0x2249ae),"good": 1, "addr": 0x2249ae, "bit": 3},</v>
       </c>
     </row>
     <row r="352" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A352" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B352" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="C352" s="4" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="D352" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C352, Levels!B:B, 0), 1, 1)),", ",IF(A352 &lt;&gt; "", """mem"": bit" &amp; B352 &amp; "(" &amp; A352 &amp; "),", ""),"""good"": ",IF(A352 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A352 &lt;&gt; "", A352, -1),", ""bit"": ",IF(B352 &lt;&gt; "", B352, -1),"},")</f>
-        <v>351: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>351: { "levelId": 13, "mem": bit4(0x2249ae),"good": 1, "addr": 0x2249ae, "bit": 4},</v>
       </c>
     </row>
     <row r="353" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A353" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B353" s="0" t="n">
+        <v>5</v>
+      </c>
       <c r="C353" s="4" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="D353" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C353, Levels!B:B, 0), 1, 1)),", ",IF(A353 &lt;&gt; "", """mem"": bit" &amp; B353 &amp; "(" &amp; A353 &amp; "),", ""),"""good"": ",IF(A353 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A353 &lt;&gt; "", A353, -1),", ""bit"": ",IF(B353 &lt;&gt; "", B353, -1),"},")</f>
-        <v>352: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>352: { "levelId": 13, "mem": bit5(0x2249ae),"good": 1, "addr": 0x2249ae, "bit": 5},</v>
       </c>
     </row>
     <row r="354" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A354" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B354" s="0" t="n">
+        <v>6</v>
+      </c>
       <c r="C354" s="4" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="D354" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C354, Levels!B:B, 0), 1, 1)),", ",IF(A354 &lt;&gt; "", """mem"": bit" &amp; B354 &amp; "(" &amp; A354 &amp; "),", ""),"""good"": ",IF(A354 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A354 &lt;&gt; "", A354, -1),", ""bit"": ",IF(B354 &lt;&gt; "", B354, -1),"},")</f>
-        <v>353: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>353: { "levelId": 13, "mem": bit6(0x2249ae),"good": 1, "addr": 0x2249ae, "bit": 6},</v>
       </c>
     </row>
     <row r="355" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A355" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B355" s="0" t="n">
+        <v>7</v>
+      </c>
       <c r="C355" s="4" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="D355" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C355, Levels!B:B, 0), 1, 1)),", ",IF(A355 &lt;&gt; "", """mem"": bit" &amp; B355 &amp; "(" &amp; A355 &amp; "),", ""),"""good"": ",IF(A355 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A355 &lt;&gt; "", A355, -1),", ""bit"": ",IF(B355 &lt;&gt; "", B355, -1),"},")</f>
-        <v>354: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>354: { "levelId": 13, "mem": bit7(0x2249ae),"good": 1, "addr": 0x2249ae, "bit": 7},</v>
       </c>
     </row>
     <row r="356" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A356" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="B356" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="C356" s="4" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="D356" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C356, Levels!B:B, 0), 1, 1)),", ",IF(A356 &lt;&gt; "", """mem"": bit" &amp; B356 &amp; "(" &amp; A356 &amp; "),", ""),"""good"": ",IF(A356 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A356 &lt;&gt; "", A356, -1),", ""bit"": ",IF(B356 &lt;&gt; "", B356, -1),"},")</f>
-        <v>355: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>355: { "levelId": 13, "mem": bit0(0x2249af),"good": 1, "addr": 0x2249af, "bit": 0},</v>
       </c>
     </row>
     <row r="357" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A357" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="B357" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="C357" s="4" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="D357" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C357, Levels!B:B, 0), 1, 1)),", ",IF(A357 &lt;&gt; "", """mem"": bit" &amp; B357 &amp; "(" &amp; A357 &amp; "),", ""),"""good"": ",IF(A357 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A357 &lt;&gt; "", A357, -1),", ""bit"": ",IF(B357 &lt;&gt; "", B357, -1),"},")</f>
-        <v>356: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>356: { "levelId": 13, "mem": bit1(0x2249af),"good": 1, "addr": 0x2249af, "bit": 1},</v>
       </c>
     </row>
     <row r="358" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A358" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="B358" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="C358" s="4" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="D358" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C358, Levels!B:B, 0), 1, 1)),", ",IF(A358 &lt;&gt; "", """mem"": bit" &amp; B358 &amp; "(" &amp; A358 &amp; "),", ""),"""good"": ",IF(A358 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A358 &lt;&gt; "", A358, -1),", ""bit"": ",IF(B358 &lt;&gt; "", B358, -1),"},")</f>
-        <v>357: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>357: { "levelId": 13, "mem": bit2(0x2249af),"good": 1, "addr": 0x2249af, "bit": 2},</v>
       </c>
     </row>
     <row r="359" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A359" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="B359" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="C359" s="4" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="D359" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C359, Levels!B:B, 0), 1, 1)),", ",IF(A359 &lt;&gt; "", """mem"": bit" &amp; B359 &amp; "(" &amp; A359 &amp; "),", ""),"""good"": ",IF(A359 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A359 &lt;&gt; "", A359, -1),", ""bit"": ",IF(B359 &lt;&gt; "", B359, -1),"},")</f>
-        <v>358: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>358: { "levelId": 13, "mem": bit3(0x2249af),"good": 1, "addr": 0x2249af, "bit": 3},</v>
       </c>
     </row>
     <row r="360" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A360" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="B360" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="C360" s="4" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="D360" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C360, Levels!B:B, 0), 1, 1)),", ",IF(A360 &lt;&gt; "", """mem"": bit" &amp; B360 &amp; "(" &amp; A360 &amp; "),", ""),"""good"": ",IF(A360 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A360 &lt;&gt; "", A360, -1),", ""bit"": ",IF(B360 &lt;&gt; "", B360, -1),"},")</f>
-        <v>359: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>359: { "levelId": 13, "mem": bit4(0x2249af),"good": 1, "addr": 0x2249af, "bit": 4},</v>
       </c>
     </row>
     <row r="361" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A361" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="B361" s="0" t="n">
+        <v>5</v>
+      </c>
       <c r="C361" s="4" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="D361" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C361, Levels!B:B, 0), 1, 1)),", ",IF(A361 &lt;&gt; "", """mem"": bit" &amp; B361 &amp; "(" &amp; A361 &amp; "),", ""),"""good"": ",IF(A361 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A361 &lt;&gt; "", A361, -1),", ""bit"": ",IF(B361 &lt;&gt; "", B361, -1),"},")</f>
-        <v>360: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>360: { "levelId": 13, "mem": bit5(0x2249af),"good": 1, "addr": 0x2249af, "bit": 5},</v>
       </c>
     </row>
     <row r="362" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A362" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="B362" s="0" t="n">
+        <v>6</v>
+      </c>
       <c r="C362" s="4" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="D362" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C362, Levels!B:B, 0), 1, 1)),", ",IF(A362 &lt;&gt; "", """mem"": bit" &amp; B362 &amp; "(" &amp; A362 &amp; "),", ""),"""good"": ",IF(A362 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A362 &lt;&gt; "", A362, -1),", ""bit"": ",IF(B362 &lt;&gt; "", B362, -1),"},")</f>
-        <v>361: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>361: { "levelId": 13, "mem": bit6(0x2249af),"good": 1, "addr": 0x2249af, "bit": 6},</v>
       </c>
     </row>
     <row r="363" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A363" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="B363" s="0" t="n">
+        <v>7</v>
+      </c>
       <c r="C363" s="4" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="D363" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C363, Levels!B:B, 0), 1, 1)),", ",IF(A363 &lt;&gt; "", """mem"": bit" &amp; B363 &amp; "(" &amp; A363 &amp; "),", ""),"""good"": ",IF(A363 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A363 &lt;&gt; "", A363, -1),", ""bit"": ",IF(B363 &lt;&gt; "", B363, -1),"},")</f>
-        <v>362: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>362: { "levelId": 13, "mem": bit7(0x2249af),"good": 1, "addr": 0x2249af, "bit": 7},</v>
       </c>
     </row>
     <row r="364" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A364" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="B364" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="C364" s="4" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="D364" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C364, Levels!B:B, 0), 1, 1)),", ",IF(A364 &lt;&gt; "", """mem"": bit" &amp; B364 &amp; "(" &amp; A364 &amp; "),", ""),"""good"": ",IF(A364 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A364 &lt;&gt; "", A364, -1),", ""bit"": ",IF(B364 &lt;&gt; "", B364, -1),"},")</f>
-        <v>363: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>363: { "levelId": 13, "mem": bit0(0x2249b0),"good": 1, "addr": 0x2249b0, "bit": 0},</v>
       </c>
     </row>
     <row r="365" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A365" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="B365" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="C365" s="4" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="D365" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C365, Levels!B:B, 0), 1, 1)),", ",IF(A365 &lt;&gt; "", """mem"": bit" &amp; B365 &amp; "(" &amp; A365 &amp; "),", ""),"""good"": ",IF(A365 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A365 &lt;&gt; "", A365, -1),", ""bit"": ",IF(B365 &lt;&gt; "", B365, -1),"},")</f>
-        <v>364: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>364: { "levelId": 13, "mem": bit1(0x2249b0),"good": 1, "addr": 0x2249b0, "bit": 1},</v>
       </c>
     </row>
     <row r="366" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A366" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="B366" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="C366" s="4" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="D366" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C366, Levels!B:B, 0), 1, 1)),", ",IF(A366 &lt;&gt; "", """mem"": bit" &amp; B366 &amp; "(" &amp; A366 &amp; "),", ""),"""good"": ",IF(A366 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A366 &lt;&gt; "", A366, -1),", ""bit"": ",IF(B366 &lt;&gt; "", B366, -1),"},")</f>
-        <v>365: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>365: { "levelId": 13, "mem": bit2(0x2249b0),"good": 1, "addr": 0x2249b0, "bit": 2},</v>
       </c>
     </row>
     <row r="367" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A367" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="B367" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="C367" s="4" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="D367" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C367, Levels!B:B, 0), 1, 1)),", ",IF(A367 &lt;&gt; "", """mem"": bit" &amp; B367 &amp; "(" &amp; A367 &amp; "),", ""),"""good"": ",IF(A367 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A367 &lt;&gt; "", A367, -1),", ""bit"": ",IF(B367 &lt;&gt; "", B367, -1),"},")</f>
-        <v>366: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>366: { "levelId": 13, "mem": bit3(0x2249b0),"good": 1, "addr": 0x2249b0, "bit": 3},</v>
       </c>
     </row>
     <row r="368" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A368" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="B368" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="C368" s="4" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="D368" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C368, Levels!B:B, 0), 1, 1)),", ",IF(A368 &lt;&gt; "", """mem"": bit" &amp; B368 &amp; "(" &amp; A368 &amp; "),", ""),"""good"": ",IF(A368 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A368 &lt;&gt; "", A368, -1),", ""bit"": ",IF(B368 &lt;&gt; "", B368, -1),"},")</f>
-        <v>367: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>367: { "levelId": 13, "mem": bit4(0x2249b0),"good": 1, "addr": 0x2249b0, "bit": 4},</v>
       </c>
     </row>
     <row r="369" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A369" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="B369" s="0" t="n">
+        <v>5</v>
+      </c>
       <c r="C369" s="4" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="D369" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C369, Levels!B:B, 0), 1, 1)),", ",IF(A369 &lt;&gt; "", """mem"": bit" &amp; B369 &amp; "(" &amp; A369 &amp; "),", ""),"""good"": ",IF(A369 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A369 &lt;&gt; "", A369, -1),", ""bit"": ",IF(B369 &lt;&gt; "", B369, -1),"},")</f>
-        <v>368: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>368: { "levelId": 13, "mem": bit5(0x2249b0),"good": 1, "addr": 0x2249b0, "bit": 5},</v>
       </c>
     </row>
     <row r="370" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A370" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="B370" s="0" t="n">
+        <v>6</v>
+      </c>
       <c r="C370" s="4" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="D370" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C370, Levels!B:B, 0), 1, 1)),", ",IF(A370 &lt;&gt; "", """mem"": bit" &amp; B370 &amp; "(" &amp; A370 &amp; "),", ""),"""good"": ",IF(A370 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A370 &lt;&gt; "", A370, -1),", ""bit"": ",IF(B370 &lt;&gt; "", B370, -1),"},")</f>
-        <v>369: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>369: { "levelId": 13, "mem": bit6(0x2249b0),"good": 1, "addr": 0x2249b0, "bit": 6},</v>
       </c>
     </row>
     <row r="371" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A371" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="B371" s="0" t="n">
+        <v>7</v>
+      </c>
       <c r="C371" s="4" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="D371" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C371, Levels!B:B, 0), 1, 1)),", ",IF(A371 &lt;&gt; "", """mem"": bit" &amp; B371 &amp; "(" &amp; A371 &amp; "),", ""),"""good"": ",IF(A371 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A371 &lt;&gt; "", A371, -1),", ""bit"": ",IF(B371 &lt;&gt; "", B371, -1),"},")</f>
-        <v>370: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>370: { "levelId": 13, "mem": bit7(0x2249b0),"good": 1, "addr": 0x2249b0, "bit": 7},</v>
       </c>
     </row>
     <row r="372" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A372" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="B372" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="C372" s="4" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="D372" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C372, Levels!B:B, 0), 1, 1)),", ",IF(A372 &lt;&gt; "", """mem"": bit" &amp; B372 &amp; "(" &amp; A372 &amp; "),", ""),"""good"": ",IF(A372 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A372 &lt;&gt; "", A372, -1),", ""bit"": ",IF(B372 &lt;&gt; "", B372, -1),"},")</f>
-        <v>371: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>371: { "levelId": 13, "mem": bit0(0x2249b1),"good": 1, "addr": 0x2249b1, "bit": 0},</v>
       </c>
     </row>
     <row r="373" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A373" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="B373" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="C373" s="4" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="D373" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C373, Levels!B:B, 0), 1, 1)),", ",IF(A373 &lt;&gt; "", """mem"": bit" &amp; B373 &amp; "(" &amp; A373 &amp; "),", ""),"""good"": ",IF(A373 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A373 &lt;&gt; "", A373, -1),", ""bit"": ",IF(B373 &lt;&gt; "", B373, -1),"},")</f>
-        <v>372: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>372: { "levelId": 13, "mem": bit1(0x2249b1),"good": 1, "addr": 0x2249b1, "bit": 1},</v>
       </c>
     </row>
     <row r="374" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A374" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="B374" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="C374" s="4" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="D374" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C374, Levels!B:B, 0), 1, 1)),", ",IF(A374 &lt;&gt; "", """mem"": bit" &amp; B374 &amp; "(" &amp; A374 &amp; "),", ""),"""good"": ",IF(A374 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A374 &lt;&gt; "", A374, -1),", ""bit"": ",IF(B374 &lt;&gt; "", B374, -1),"},")</f>
-        <v>373: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>373: { "levelId": 13, "mem": bit2(0x2249b1),"good": 1, "addr": 0x2249b1, "bit": 2},</v>
       </c>
     </row>
     <row r="375" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A375" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="B375" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="C375" s="4" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="D375" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C375, Levels!B:B, 0), 1, 1)),", ",IF(A375 &lt;&gt; "", """mem"": bit" &amp; B375 &amp; "(" &amp; A375 &amp; "),", ""),"""good"": ",IF(A375 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A375 &lt;&gt; "", A375, -1),", ""bit"": ",IF(B375 &lt;&gt; "", B375, -1),"},")</f>
-        <v>374: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>374: { "levelId": 13, "mem": bit3(0x2249b1),"good": 1, "addr": 0x2249b1, "bit": 3},</v>
       </c>
     </row>
     <row r="376" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A376" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="B376" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="C376" s="4" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="D376" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C376, Levels!B:B, 0), 1, 1)),", ",IF(A376 &lt;&gt; "", """mem"": bit" &amp; B376 &amp; "(" &amp; A376 &amp; "),", ""),"""good"": ",IF(A376 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A376 &lt;&gt; "", A376, -1),", ""bit"": ",IF(B376 &lt;&gt; "", B376, -1),"},")</f>
-        <v>375: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>375: { "levelId": 13, "mem": bit4(0x2249b1),"good": 1, "addr": 0x2249b1, "bit": 4},</v>
       </c>
     </row>
     <row r="377" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A377" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="B377" s="0" t="n">
+        <v>5</v>
+      </c>
       <c r="C377" s="4" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="D377" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C377, Levels!B:B, 0), 1, 1)),", ",IF(A377 &lt;&gt; "", """mem"": bit" &amp; B377 &amp; "(" &amp; A377 &amp; "),", ""),"""good"": ",IF(A377 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A377 &lt;&gt; "", A377, -1),", ""bit"": ",IF(B377 &lt;&gt; "", B377, -1),"},")</f>
-        <v>376: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>376: { "levelId": 13, "mem": bit5(0x2249b1),"good": 1, "addr": 0x2249b1, "bit": 5},</v>
       </c>
     </row>
     <row r="378" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A378" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="B378" s="0" t="n">
+        <v>6</v>
+      </c>
       <c r="C378" s="4" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="D378" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C378, Levels!B:B, 0), 1, 1)),", ",IF(A378 &lt;&gt; "", """mem"": bit" &amp; B378 &amp; "(" &amp; A378 &amp; "),", ""),"""good"": ",IF(A378 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A378 &lt;&gt; "", A378, -1),", ""bit"": ",IF(B378 &lt;&gt; "", B378, -1),"},")</f>
-        <v>377: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>377: { "levelId": 13, "mem": bit6(0x2249b1),"good": 1, "addr": 0x2249b1, "bit": 6},</v>
       </c>
     </row>
     <row r="379" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A379" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="B379" s="0" t="n">
+        <v>7</v>
+      </c>
       <c r="C379" s="4" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="D379" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C379, Levels!B:B, 0), 1, 1)),", ",IF(A379 &lt;&gt; "", """mem"": bit" &amp; B379 &amp; "(" &amp; A379 &amp; "),", ""),"""good"": ",IF(A379 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A379 &lt;&gt; "", A379, -1),", ""bit"": ",IF(B379 &lt;&gt; "", B379, -1),"},")</f>
-        <v>378: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>378: { "levelId": 13, "mem": bit7(0x2249b1),"good": 1, "addr": 0x2249b1, "bit": 7},</v>
       </c>
     </row>
     <row r="380" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A380" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B380" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="C380" s="4" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="D380" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C380, Levels!B:B, 0), 1, 1)),", ",IF(A380 &lt;&gt; "", """mem"": bit" &amp; B380 &amp; "(" &amp; A380 &amp; "),", ""),"""good"": ",IF(A380 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A380 &lt;&gt; "", A380, -1),", ""bit"": ",IF(B380 &lt;&gt; "", B380, -1),"},")</f>
-        <v>379: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>379: { "levelId": 13, "mem": bit0(0x2249b2),"good": 1, "addr": 0x2249b2, "bit": 0},</v>
       </c>
     </row>
     <row r="381" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A381" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B381" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="C381" s="4" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="D381" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C381, Levels!B:B, 0), 1, 1)),", ",IF(A381 &lt;&gt; "", """mem"": bit" &amp; B381 &amp; "(" &amp; A381 &amp; "),", ""),"""good"": ",IF(A381 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A381 &lt;&gt; "", A381, -1),", ""bit"": ",IF(B381 &lt;&gt; "", B381, -1),"},")</f>
-        <v>380: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>380: { "levelId": 13, "mem": bit1(0x2249b2),"good": 1, "addr": 0x2249b2, "bit": 1},</v>
       </c>
     </row>
     <row r="382" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A382" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B382" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="C382" s="4" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="D382" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C382, Levels!B:B, 0), 1, 1)),", ",IF(A382 &lt;&gt; "", """mem"": bit" &amp; B382 &amp; "(" &amp; A382 &amp; "),", ""),"""good"": ",IF(A382 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A382 &lt;&gt; "", A382, -1),", ""bit"": ",IF(B382 &lt;&gt; "", B382, -1),"},")</f>
-        <v>381: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>381: { "levelId": 13, "mem": bit2(0x2249b2),"good": 1, "addr": 0x2249b2, "bit": 2},</v>
       </c>
     </row>
     <row r="383" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A383" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B383" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="C383" s="4" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="D383" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C383, Levels!B:B, 0), 1, 1)),", ",IF(A383 &lt;&gt; "", """mem"": bit" &amp; B383 &amp; "(" &amp; A383 &amp; "),", ""),"""good"": ",IF(A383 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A383 &lt;&gt; "", A383, -1),", ""bit"": ",IF(B383 &lt;&gt; "", B383, -1),"},")</f>
-        <v>382: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>382: { "levelId": 13, "mem": bit3(0x2249b2),"good": 1, "addr": 0x2249b2, "bit": 3},</v>
       </c>
     </row>
     <row r="384" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A384" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B384" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="C384" s="4" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="D384" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C384, Levels!B:B, 0), 1, 1)),", ",IF(A384 &lt;&gt; "", """mem"": bit" &amp; B384 &amp; "(" &amp; A384 &amp; "),", ""),"""good"": ",IF(A384 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A384 &lt;&gt; "", A384, -1),", ""bit"": ",IF(B384 &lt;&gt; "", B384, -1),"},")</f>
-        <v>383: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>383: { "levelId": 13, "mem": bit4(0x2249b2),"good": 1, "addr": 0x2249b2, "bit": 4},</v>
       </c>
     </row>
     <row r="385" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A385" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B385" s="0" t="n">
+        <v>5</v>
+      </c>
       <c r="C385" s="4" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="D385" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C385, Levels!B:B, 0), 1, 1)),", ",IF(A385 &lt;&gt; "", """mem"": bit" &amp; B385 &amp; "(" &amp; A385 &amp; "),", ""),"""good"": ",IF(A385 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A385 &lt;&gt; "", A385, -1),", ""bit"": ",IF(B385 &lt;&gt; "", B385, -1),"},")</f>
-        <v>384: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>384: { "levelId": 13, "mem": bit5(0x2249b2),"good": 1, "addr": 0x2249b2, "bit": 5},</v>
       </c>
     </row>
     <row r="386" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A386" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B386" s="0" t="n">
+        <v>6</v>
+      </c>
       <c r="C386" s="4" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="D386" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C386, Levels!B:B, 0), 1, 1)),", ",IF(A386 &lt;&gt; "", """mem"": bit" &amp; B386 &amp; "(" &amp; A386 &amp; "),", ""),"""good"": ",IF(A386 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A386 &lt;&gt; "", A386, -1),", ""bit"": ",IF(B386 &lt;&gt; "", B386, -1),"},")</f>
-        <v>385: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>385: { "levelId": 13, "mem": bit6(0x2249b2),"good": 1, "addr": 0x2249b2, "bit": 6},</v>
       </c>
     </row>
     <row r="387" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A387" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B387" s="0" t="n">
+        <v>7</v>
+      </c>
       <c r="C387" s="4" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="D387" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C387, Levels!B:B, 0), 1, 1)),", ",IF(A387 &lt;&gt; "", """mem"": bit" &amp; B387 &amp; "(" &amp; A387 &amp; "),", ""),"""good"": ",IF(A387 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A387 &lt;&gt; "", A387, -1),", ""bit"": ",IF(B387 &lt;&gt; "", B387, -1),"},")</f>
-        <v>386: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>386: { "levelId": 13, "mem": bit7(0x2249b2),"good": 1, "addr": 0x2249b2, "bit": 7},</v>
       </c>
     </row>
     <row r="388" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A388" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="B388" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="C388" s="4" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="D388" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C388, Levels!B:B, 0), 1, 1)),", ",IF(A388 &lt;&gt; "", """mem"": bit" &amp; B388 &amp; "(" &amp; A388 &amp; "),", ""),"""good"": ",IF(A388 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A388 &lt;&gt; "", A388, -1),", ""bit"": ",IF(B388 &lt;&gt; "", B388, -1),"},")</f>
-        <v>387: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>387: { "levelId": 13, "mem": bit0(0x2249b3),"good": 1, "addr": 0x2249b3, "bit": 0},</v>
       </c>
     </row>
     <row r="389" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A389" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="B389" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="C389" s="4" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="D389" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C389, Levels!B:B, 0), 1, 1)),", ",IF(A389 &lt;&gt; "", """mem"": bit" &amp; B389 &amp; "(" &amp; A389 &amp; "),", ""),"""good"": ",IF(A389 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A389 &lt;&gt; "", A389, -1),", ""bit"": ",IF(B389 &lt;&gt; "", B389, -1),"},")</f>
-        <v>388: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>388: { "levelId": 13, "mem": bit1(0x2249b3),"good": 1, "addr": 0x2249b3, "bit": 1},</v>
       </c>
     </row>
     <row r="390" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A390" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="B390" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="C390" s="4" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="D390" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C390, Levels!B:B, 0), 1, 1)),", ",IF(A390 &lt;&gt; "", """mem"": bit" &amp; B390 &amp; "(" &amp; A390 &amp; "),", ""),"""good"": ",IF(A390 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A390 &lt;&gt; "", A390, -1),", ""bit"": ",IF(B390 &lt;&gt; "", B390, -1),"},")</f>
-        <v>389: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>389: { "levelId": 13, "mem": bit2(0x2249b3),"good": 1, "addr": 0x2249b3, "bit": 2},</v>
       </c>
     </row>
     <row r="391" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A391" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="B391" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="C391" s="4" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="D391" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C391, Levels!B:B, 0), 1, 1)),", ",IF(A391 &lt;&gt; "", """mem"": bit" &amp; B391 &amp; "(" &amp; A391 &amp; "),", ""),"""good"": ",IF(A391 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A391 &lt;&gt; "", A391, -1),", ""bit"": ",IF(B391 &lt;&gt; "", B391, -1),"},")</f>
-        <v>390: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>390: { "levelId": 13, "mem": bit3(0x2249b3),"good": 1, "addr": 0x2249b3, "bit": 3},</v>
       </c>
     </row>
     <row r="392" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A392" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="B392" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="C392" s="4" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="D392" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C392, Levels!B:B, 0), 1, 1)),", ",IF(A392 &lt;&gt; "", """mem"": bit" &amp; B392 &amp; "(" &amp; A392 &amp; "),", ""),"""good"": ",IF(A392 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A392 &lt;&gt; "", A392, -1),", ""bit"": ",IF(B392 &lt;&gt; "", B392, -1),"},")</f>
-        <v>391: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>391: { "levelId": 13, "mem": bit4(0x2249b3),"good": 1, "addr": 0x2249b3, "bit": 4},</v>
       </c>
     </row>
     <row r="393" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A393" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="B393" s="0" t="n">
+        <v>5</v>
+      </c>
       <c r="C393" s="4" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="D393" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C393, Levels!B:B, 0), 1, 1)),", ",IF(A393 &lt;&gt; "", """mem"": bit" &amp; B393 &amp; "(" &amp; A393 &amp; "),", ""),"""good"": ",IF(A393 &lt;&gt; "", 1, 0),", ""addr"": ",IF(A393 &lt;&gt; "", A393, -1),", ""bit"": ",IF(B393 &lt;&gt; "", B393, -1),"},")</f>
-        <v>392: { "levelId": 3, "good": 0, "addr": -1, "bit": -1},</v>
+        <v>392: { "levelId": 13, "mem": bit5(0x2249b3),"good": 1, "addr": 0x2249b3, "bit": 5},</v>
       </c>
     </row>
     <row r="394" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19074,13 +19469,13 @@
   </sheetPr>
   <dimension ref="A1:H1081"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="B11" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
+      <selection pane="bottomLeft" activeCell="C38" activeCellId="0" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.93"/>
@@ -19090,13 +19485,13 @@
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>142</v>
+        <v>156</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>4</v>
@@ -19106,12 +19501,12 @@
       </c>
       <c r="H1" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(D2:D81)</f>
-        <v>1: { "levelId": 1, "mem": bit7(0x2249f0),"good": 1},2: { "levelId": 2, "mem": bit0(0x2249f1),"good": 1},3: { "levelId": 2, "mem": bit1(0x2249f1),"good": 1},4: { "levelId": 2, "mem": bit5(0x2249f1),"good": 1},5: { "levelId": 2, "mem": bit6(0x2249f1),"good": 1},6: { "levelId": 1, "mem": bit7(0x2249f1),"good": 1},7: { "levelId": 5, "mem": bit0(0x2249f2),"good": 1},8: { "levelId": 5, "mem": bit1(0x2249f2),"good": 1},9: { "levelId": 5, "mem": bit2(0x2249f2),"good": 1},10: { "levelId": 5, "mem": bit3(0x2249f2),"good": 1},11: { "levelId": 5, "mem": bit4(0x2249f2),"good": 1},12: { "levelId": 6, "mem": bit5(0x2249f2),"good": 1},13: { "levelId": 6, "mem": bit7(0x2249f2),"good": 1},14: { "levelId": 6, "mem": bit1(0x2249f3),"good": 1},15: { "levelId": 6, "mem": bit6(0x2249f2),"good": 1},16: { "levelId": 6, "mem": bit0(0x2249f3),"good": 1},17: { "levelId": 6, "mem": bit3(0x2249f3),"good": 1},18: { "levelId": 6, "mem": bit2(0x2249f3),"good": 1},19: { "levelId": 8, "mem": bit5(0x2249f3),"good": 1},20: { "levelId": 8, "mem": bit4(0x2249f3),"good": 1},21: { "levelId": 10, "mem": bit0(0x2249f4),"good": 1},22: { "levelId": 10, "mem": bit6(0x2249f3),"good": 1},23: { "levelId": 10, "mem": bit3(0x2249f4),"good": 1},24: { "levelId": 10, "mem": bit5(0x2249f4),"good": 1},25: { "levelId": 10, "mem": bit7(0x2249f3),"good": 1},26: { "levelId": 10, "mem": bit1(0x2249f4),"good": 1},27: { "levelId": 10, "mem": bit2(0x2249f4),"good": 1},28: { "levelId": 10, "mem": bit4(0x2249f4),"good": 1},29: { "levelId": 12, "mem": bit6(0x2249f4),"good": 1},30: { "levelId": 12, "mem": bit7(0x2249f4),"good": 1},31: { "levelId": 12, "mem": bit1(0x2249f5),"good": 1},32: { "levelId": 12, "mem": bit0(0x2249f5),"good": 1},33: { "levelId": 3, "good": 0},34: { "levelId": 3, "good": 0},35: { "levelId": 3, "good": 0},36: { "levelId": 3, "good": 0},37: { "levelId": 3, "good": 0},38: { "levelId": 3, "good": 0},39: { "levelId": 3, "good": 0},40: { "levelId": 3, "good": 0},41: { "levelId": 3, "good": 0},42: { "levelId": 3, "good": 0},43: { "levelId": 3, "good": 0},44: { "levelId": 3, "good": 0},45: { "levelId": 3, "good": 0},46: { "levelId": 3, "good": 0},47: { "levelId": 3, "good": 0},48: { "levelId": 3, "good": 0},49: { "levelId": 3, "good": 0},50: { "levelId": 3, "good": 0},51: { "levelId": 3, "good": 0},52: { "levelId": 3, "good": 0},53: { "levelId": 3, "good": 0},54: { "levelId": 3, "good": 0},55: { "levelId": 3, "good": 0},56: { "levelId": 3, "good": 0},57: { "levelId": 3, "good": 0},58: { "levelId": 3, "good": 0},59: { "levelId": 3, "good": 0},60: { "levelId": 3, "good": 0},61: { "levelId": 3, "good": 0},62: { "levelId": 3, "good": 0},63: { "levelId": 3, "good": 0},64: { "levelId": 3, "good": 0},65: { "levelId": 3, "good": 0},66: { "levelId": 3, "good": 0},67: { "levelId": 3, "good": 0},68: { "levelId": 3, "good": 0},69: { "levelId": 3, "good": 0},70: { "levelId": 3, "good": 0},71: { "levelId": 3, "good": 0},72: { "levelId": 3, "good": 0},73: { "levelId": 3, "good": 0},74: { "levelId": 3, "good": 0},75: { "levelId": 3, "good": 0},76: { "levelId": 3, "good": 0},77: { "levelId": 3, "good": 0},78: { "levelId": 3, "good": 0},79: { "levelId": 3, "good": 0},80: { "levelId": 3, "good": 0},</v>
+        <v>1: { "levelId": 1, "mem": bit7(0x2249f0),"good": 1},2: { "levelId": 2, "mem": bit0(0x2249f1),"good": 1},3: { "levelId": 2, "mem": bit1(0x2249f1),"good": 1},4: { "levelId": 2, "mem": bit5(0x2249f1),"good": 1},5: { "levelId": 2, "mem": bit6(0x2249f1),"good": 1},6: { "levelId": 1, "mem": bit7(0x2249f1),"good": 1},7: { "levelId": 5, "mem": bit0(0x2249f2),"good": 1},8: { "levelId": 5, "mem": bit1(0x2249f2),"good": 1},9: { "levelId": 5, "mem": bit2(0x2249f2),"good": 1},10: { "levelId": 5, "mem": bit3(0x2249f2),"good": 1},11: { "levelId": 5, "mem": bit4(0x2249f2),"good": 1},12: { "levelId": 6, "mem": bit5(0x2249f2),"good": 1},13: { "levelId": 6, "mem": bit7(0x2249f2),"good": 1},14: { "levelId": 6, "mem": bit1(0x2249f3),"good": 1},15: { "levelId": 6, "mem": bit6(0x2249f2),"good": 1},16: { "levelId": 6, "mem": bit0(0x2249f3),"good": 1},17: { "levelId": 6, "mem": bit3(0x2249f3),"good": 1},18: { "levelId": 6, "mem": bit2(0x2249f3),"good": 1},19: { "levelId": 8, "mem": bit5(0x2249f3),"good": 1},20: { "levelId": 8, "mem": bit4(0x2249f3),"good": 1},21: { "levelId": 10, "mem": bit0(0x2249f4),"good": 1},22: { "levelId": 10, "mem": bit6(0x2249f3),"good": 1},23: { "levelId": 10, "mem": bit3(0x2249f4),"good": 1},24: { "levelId": 10, "mem": bit5(0x2249f4),"good": 1},25: { "levelId": 10, "mem": bit7(0x2249f3),"good": 1},26: { "levelId": 10, "mem": bit1(0x2249f4),"good": 1},27: { "levelId": 10, "mem": bit2(0x2249f4),"good": 1},28: { "levelId": 10, "mem": bit4(0x2249f4),"good": 1},29: { "levelId": 12, "mem": bit6(0x2249f4),"good": 1},30: { "levelId": 12, "mem": bit7(0x2249f4),"good": 1},31: { "levelId": 12, "mem": bit1(0x2249f5),"good": 1},32: { "levelId": 12, "mem": bit0(0x2249f5),"good": 1},33: { "levelId": 13, "mem": bit2(0x2249f5),"good": 1},34: { "levelId": 13, "mem": bit3(0x2249f5),"good": 1},35: { "levelId": 13, "mem": bit4(0x2249f5),"good": 1},36: { "levelId": 13, "mem": bit5(0x2249f5),"good": 1},37: { "levelId": 3, "good": 0},38: { "levelId": 3, "good": 0},39: { "levelId": 3, "good": 0},40: { "levelId": 3, "good": 0},41: { "levelId": 3, "good": 0},42: { "levelId": 3, "good": 0},43: { "levelId": 3, "good": 0},44: { "levelId": 3, "good": 0},45: { "levelId": 3, "good": 0},46: { "levelId": 3, "good": 0},47: { "levelId": 3, "good": 0},48: { "levelId": 3, "good": 0},49: { "levelId": 3, "good": 0},50: { "levelId": 3, "good": 0},51: { "levelId": 3, "good": 0},52: { "levelId": 3, "good": 0},53: { "levelId": 3, "good": 0},54: { "levelId": 3, "good": 0},55: { "levelId": 3, "good": 0},56: { "levelId": 3, "good": 0},57: { "levelId": 3, "good": 0},58: { "levelId": 3, "good": 0},59: { "levelId": 3, "good": 0},60: { "levelId": 3, "good": 0},61: { "levelId": 3, "good": 0},62: { "levelId": 3, "good": 0},63: { "levelId": 3, "good": 0},64: { "levelId": 3, "good": 0},65: { "levelId": 3, "good": 0},66: { "levelId": 3, "good": 0},67: { "levelId": 3, "good": 0},68: { "levelId": 3, "good": 0},69: { "levelId": 3, "good": 0},70: { "levelId": 3, "good": 0},71: { "levelId": 3, "good": 0},72: { "levelId": 3, "good": 0},73: { "levelId": 3, "good": 0},74: { "levelId": 3, "good": 0},75: { "levelId": 3, "good": 0},76: { "levelId": 3, "good": 0},77: { "levelId": 3, "good": 0},78: { "levelId": 3, "good": 0},79: { "levelId": 3, "good": 0},80: { "levelId": 3, "good": 0},</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>7</v>
@@ -19126,7 +19521,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>144</v>
+        <v>158</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0</v>
@@ -19141,7 +19536,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>144</v>
+        <v>158</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>1</v>
@@ -19156,7 +19551,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>144</v>
+        <v>158</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>5</v>
@@ -19171,7 +19566,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>144</v>
+        <v>158</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>6</v>
@@ -19186,7 +19581,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>144</v>
+        <v>158</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>7</v>
@@ -19201,7 +19596,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>145</v>
+        <v>159</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>0</v>
@@ -19216,7 +19611,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>145</v>
+        <v>159</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>1</v>
@@ -19231,7 +19626,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>145</v>
+        <v>159</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>2</v>
@@ -19246,7 +19641,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>145</v>
+        <v>159</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>3</v>
@@ -19261,7 +19656,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>145</v>
+        <v>159</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>4</v>
@@ -19276,7 +19671,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>145</v>
+        <v>159</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>5</v>
@@ -19291,7 +19686,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>145</v>
+        <v>159</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>7</v>
@@ -19306,7 +19701,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>146</v>
+        <v>160</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>1</v>
@@ -19321,7 +19716,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>145</v>
+        <v>159</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>6</v>
@@ -19336,7 +19731,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>146</v>
+        <v>160</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>0</v>
@@ -19351,7 +19746,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>146</v>
+        <v>160</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>3</v>
@@ -19366,7 +19761,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>146</v>
+        <v>160</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>2</v>
@@ -19381,7 +19776,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>146</v>
+        <v>160</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>5</v>
@@ -19396,7 +19791,7 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>146</v>
+        <v>160</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>4</v>
@@ -19411,7 +19806,7 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>147</v>
+        <v>161</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>0</v>
@@ -19426,7 +19821,7 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>146</v>
+        <v>160</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>6</v>
@@ -19441,7 +19836,7 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>147</v>
+        <v>161</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>3</v>
@@ -19456,7 +19851,7 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>147</v>
+        <v>161</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>5</v>
@@ -19471,7 +19866,7 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>146</v>
+        <v>160</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>7</v>
@@ -19486,7 +19881,7 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>147</v>
+        <v>161</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>1</v>
@@ -19501,7 +19896,7 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>147</v>
+        <v>161</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>2</v>
@@ -19516,7 +19911,7 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>147</v>
+        <v>161</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>4</v>
@@ -19531,7 +19926,7 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>147</v>
+        <v>161</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>6</v>
@@ -19546,7 +19941,7 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>147</v>
+        <v>161</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>7</v>
@@ -19561,7 +19956,7 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>148</v>
+        <v>162</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>1</v>
@@ -19576,7 +19971,7 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>148</v>
+        <v>162</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>0</v>
@@ -19590,39 +19985,63 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="C34" s="4" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="D34" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C34, Levels!B:B, 0), 1, 1)),", ",IF(A34 &lt;&gt; "", """mem"": bit" &amp; B34 &amp; "(" &amp; A34 &amp; "),", ""),"""good"": ",IF(A34 &lt;&gt; "", 1, 0),"},")</f>
-        <v>33: { "levelId": 3, "good": 0},</v>
+        <v>33: { "levelId": 13, "mem": bit2(0x2249f5),"good": 1},</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="C35" s="4" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="D35" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C35, Levels!B:B, 0), 1, 1)),", ",IF(A35 &lt;&gt; "", """mem"": bit" &amp; B35 &amp; "(" &amp; A35 &amp; "),", ""),"""good"": ",IF(A35 &lt;&gt; "", 1, 0),"},")</f>
-        <v>34: { "levelId": 3, "good": 0},</v>
+        <v>34: { "levelId": 13, "mem": bit3(0x2249f5),"good": 1},</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="C36" s="4" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="D36" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C36, Levels!B:B, 0), 1, 1)),", ",IF(A36 &lt;&gt; "", """mem"": bit" &amp; B36 &amp; "(" &amp; A36 &amp; "),", ""),"""good"": ",IF(A36 &lt;&gt; "", 1, 0),"},")</f>
-        <v>35: { "levelId": 3, "good": 0},</v>
+        <v>35: { "levelId": 13, "mem": bit4(0x2249f5),"good": 1},</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <v>5</v>
+      </c>
       <c r="C37" s="4" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="D37" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(ROW()-1,": { ""levelId"": ",INDIRECT("'Levels'!" &amp; ADDRESS(MATCH(C37, Levels!B:B, 0), 1, 1)),", ",IF(A37 &lt;&gt; "", """mem"": bit" &amp; B37 &amp; "(" &amp; A37 &amp; "),", ""),"""good"": ",IF(A37 &lt;&gt; "", 1, 0),"},")</f>
-        <v>36: { "levelId": 3, "good": 0},</v>
+        <v>36: { "levelId": 13, "mem": bit5(0x2249f5),"good": 1},</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Fixed the achievement for the 1000th Lum
</commit_message>
<xml_diff>
--- a/Rayman 2.xlsx
+++ b/Rayman 2.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2495" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2496" uniqueCount="347">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -1029,6 +1029,9 @@
   </si>
   <si>
     <t xml:space="preserve">0x224a29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x224a06</t>
   </si>
   <si>
     <t xml:space="preserve">Level ID</t>
@@ -1283,7 +1286,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H1" activeCellId="1" sqref="B989:B996 H1"/>
+      <selection pane="bottomLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.9921875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5472,7 +5475,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G26" activeCellId="1" sqref="B989:B996 G26"/>
+      <selection pane="bottomLeft" activeCell="G26" activeCellId="0" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9364,7 +9367,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A966" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B989" activeCellId="0" sqref="B989:B996"/>
+      <selection pane="bottomLeft" activeCell="A1002" activeCellId="0" sqref="A1002"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9392,7 +9395,7 @@
       </c>
       <c r="H1" s="5" t="str">
         <f aca="false">_xlfn.CONCAT(D2:D1001)</f>
-        <v>1: { "levelId": 2, "mem": bit0(0x224988),"good": 1, "addr": 0x224988, "bit": 0},2: { "levelId": 2, "mem": bit1(0x224988),"good": 1, "addr": 0x224988, "bit": 1},3: { "levelId": 2, "mem": bit2(0x224988),"good": 1, "addr": 0x224988, "bit": 2},4: { "levelId": 2, "mem": bit3(0x224988),"good": 1, "addr": 0x224988, "bit": 3},5: { "levelId": 2, "mem": bit4(0x224988),"good": 1, "addr": 0x224988, "bit": 4},6: { "levelId": 2, "mem": bit5(0x224988),"good": 1, "addr": 0x224988, "bit": 5},7: { "levelId": 2, "mem": bit6(0x224988),"good": 1, "addr": 0x224988, "bit": 6},8: { "levelId": 2, "mem": bit7(0x224988),"good": 1, "addr": 0x224988, "bit": 7},9: { "levelId": 2, "mem": bit2(0x224989),"good": 1, "addr": 0x224989, "bit": 2},10: { "levelId": 2, "mem": bit1(0x22498a),"good": 1, "addr": 0x22498a, "bit": 1},11: { "levelId": 2, "mem": bit2(0x22498a),"good": 1, "addr": 0x22498a, "bit": 2},12: { "levelId": 2, "mem": bit3(0x22498a),"good": 1, "addr": 0x22498a, "bit": 3},13: { "levelId": 2, "mem": bit4(0x22498a),"good": 1, "addr": 0x22498a, "bit": 4},14: { "levelId": 2, "mem": bit5(0x22498a),"good": 1, "addr": 0x22498a, "bit": 5},15: { "levelId": 2, "mem": bit6(0x22498a),"good": 1, "addr": 0x22498a, "bit": 6},16: { "levelId": 2, "mem": bit7(0x22498a),"good": 1, "addr": 0x22498a, "bit": 7},17: { "levelId": 2, "mem": bit5(0x22498b),"good": 1, "addr": 0x22498b, "bit": 5},18: { "levelId": 2, "mem": bit6(0x22498b),"good": 1, "addr": 0x22498b, "bit": 6},19: { "levelId": 2, "mem": bit7(0x22498b),"good": 1, "addr": 0x22498b, "bit": 7},20: { "levelId": 2, "mem": bit0(0x22498c),"good": 1, "addr": 0x22498c, "bit": 0},21: { "levelId": 2, "mem": bit1(0x22498c),"good": 1, "addr": 0x22498c, "bit": 1},22: { "levelId": 2, "mem": bit2(0x22498c),"good": 1, "addr": 0x22498c, "bit": 2},23: { "levelId": 2, "mem": bit3(0x22498c),"good": 1, "addr": 0x22498c, "bit": 3},24: { "levelId": 2, "mem": bit4(0x22498c),"good": 1, "addr": 0x22498c, "bit": 4},25: { "levelId": 2, "mem": bit5(0x22498c),"good": 1, "addr": 0x22498c, "bit": 5},26: { "levelId": 2, "mem": bit6(0x22498c),"good": 1, "addr": 0x22498c, "bit": 6},27: { "levelId": 2, "mem": bit7(0x22498c),"good": 1, "addr": 0x22498c, "bit": 7},28: { "levelId": 2, "mem": bit0(0x22498d),"good": 1, "addr": 0x22498d, "bit": 0},29: { "levelId": 2, "mem": bit1(0x22498d),"good": 1, "addr": 0x22498d, "bit": 1},30: { "levelId": 2, "mem": bit2(0x22498d),"good": 1, "addr": 0x22498d, "bit": 2},31: { "levelId": 2, "mem": bit3(0x22498d),"good": 1, "addr": 0x22498d, "bit": 3},32: { "levelId": 2, "mem": bit4(0x22498d),"good": 1, "addr": 0x22498d, "bit": 4},33: { "levelId": 2, "mem": bit5(0x22498d),"good": 1, "addr": 0x22498d, "bit": 5},34: { "levelId": 2, "mem": bit6(0x22498d),"good": 1, "addr": 0x22498d, "bit": 6},35: { "levelId": 2, "mem": bit7(0x22498d),"good": 1, "addr": 0x22498d, "bit": 7},36: { "levelId": 2, "mem": bit0(0x22498e),"good": 1, "addr": 0x22498e, "bit": 0},37: { "levelId": 2, "mem": bit1(0x22498e),"good": 1, "addr": 0x22498e, "bit": 1},38: { "levelId": 5, "mem": bit2(0x22498e),"good": 1, "addr": 0x22498e, "bit": 2},39: { "levelId": 5, "mem": bit3(0x22498e),"good": 1, "addr": 0x22498e, "bit": 3},40: { "levelId": 5, "mem": bit4(0x22498e),"good": 1, "addr": 0x22498e, "bit": 4},41: { "levelId": 5, "mem": bit5(0x22498e),"good": 1, "addr": 0x22498e, "bit": 5},42: { "levelId": 5, "mem": bit6(0x22498e),"good": 1, "addr": 0x22498e, "bit": 6},43: { "levelId": 5, "mem": bit7(0x22498e),"good": 1, "addr": 0x22498e, "bit": 7},44: { "levelId": 5, "mem": bit0(0x22498f),"good": 1, "addr": 0x22498f, "bit": 0},45: { "levelId": 5, "mem": bit1(0x22498f),"good": 1, "addr": 0x22498f, "bit": 1},46: { "levelId": 5, "mem": bit2(0x22498f),"good": 1, "addr": 0x22498f, "bit": 2},47: { "levelId": 5, "mem": bit3(0x22498f),"good": 1, "addr": 0x22498f, "bit": 3},48: { "levelId": 5, "mem": bit4(0x22498f),"good": 1, "addr": 0x22498f, "bit": 4},49: { "levelId": 5, "mem": bit5(0x22498f),"good": 1, "addr": 0x22498f, "bit": 5},50: { "levelId": 5, "mem": bit6(0x22498f),"good": 1, "addr": 0x22498f, "bit": 6},51: { "levelId": 5, "mem": bit7(0x22498f),"good": 1, "addr": 0x22498f, "bit": 7},52: { "levelId": 5, "mem": bit0(0x224990),"good": 1, "addr": 0x224990, "bit": 0},53: { "levelId": 5, "mem": bit1(0x224990),"good": 1, "addr": 0x224990, "bit": 1},54: { "levelId": 5, "mem": bit2(0x224990),"good": 1, "addr": 0x224990, "bit": 2},55: { "levelId": 5, "mem": bit3(0x224990),"good": 1, "addr": 0x224990, "bit": 3},56: { "levelId": 5, "mem": bit4(0x224990),"good": 1, "addr": 0x224990, "bit": 4},57: { "levelId": 5, "mem": bit5(0x224990),"good": 1, "addr": 0x224990, "bit": 5},58: { "levelId": 5, "mem": bit6(0x224990),"good": 1, "addr": 0x224990, "bit": 6},59: { "levelId": 5, "mem": bit7(0x224990),"good": 1, "addr": 0x224990, "bit": 7},60: { "levelId": 5, "mem": bit0(0x224991),"good": 1, "addr": 0x224991, "bit": 0},61: { "levelId": 5, "mem": bit1(0x224991),"good": 1, "addr": 0x224991, "bit": 1},62: { "levelId": 5, "mem": bit2(0x224991),"good": 1, "addr": 0x224991, "bit": 2},63: { "levelId": 5, "mem": bit3(0x224991),"good": 1, "addr": 0x224991, "bit": 3},64: { "levelId": 5, "mem": bit4(0x224991),"good": 1, "addr": 0x224991, "bit": 4},65: { "levelId": 5, "mem": bit5(0x224991),"good": 1, "addr": 0x224991, "bit": 5},66: { "levelId": 5, "mem": bit6(0x224991),"good": 1, "addr": 0x224991, "bit": 6},67: { "levelId": 5, "mem": bit7(0x224991),"good": 1, "addr": 0x224991, "bit": 7},68: { "levelId": 5, "mem": bit0(0x224992),"good": 1, "addr": 0x224992, "bit": 0},69: { "levelId": 5, "mem": bit1(0x224992),"good": 1, "addr": 0x224992, "bit": 1},70: { "levelId": 5, "mem": bit2(0x224992),"good": 1, "addr": 0x224992, "bit": 2},71: { "levelId": 5, "mem": bit3(0x224992),"good": 1, "addr": 0x224992, "bit": 3},72: { "levelId": 5, "mem": bit4(0x224992),"good": 1, "addr": 0x224992, "bit": 4},73: { "levelId": 5, "mem": bit5(0x224992),"good": 1, "addr": 0x224992, "bit": 5},74: { "levelId": 5, "mem": bit6(0x224992),"good": 1, "addr": 0x224992, "bit": 6},75: { "levelId": 5, "mem": bit7(0x224992),"good": 1, "addr": 0x224992, "bit": 7},76: { "levelId": 5, "mem": bit0(0x224993),"good": 1, "addr": 0x224993, "bit": 0},77: { "levelId": 5, "mem": bit1(0x224993),"good": 1, "addr": 0x224993, "bit": 1},78: { "levelId": 5, "mem": bit2(0x224993),"good": 1, "addr": 0x224993, "bit": 2},79: { "levelId": 5, "mem": bit3(0x224993),"good": 1, "addr": 0x224993, "bit": 3},80: { "levelId": 5, "mem": bit4(0x224993),"good": 1, "addr": 0x224993, "bit": 4},81: { "levelId": 5, "mem": bit5(0x224993),"good": 1, "addr": 0x224993, "bit": 5},82: { "levelId": 5, "mem": bit6(0x224993),"good": 1, "addr": 0x224993, "bit": 6},83: { "levelId": 5, "mem": bit7(0x224993),"good": 1, "addr": 0x224993, "bit": 7},84: { "levelId": 5, "mem": bit0(0x224994),"good": 1, "addr": 0x224994, "bit": 0},85: { "levelId": 5, "mem": bit1(0x224994),"good": 1, "addr": 0x224994, "bit": 1},86: { "levelId": 5, "mem": bit2(0x224994),"good": 1, "addr": 0x224994, "bit": 2},87: { "levelId": 5, "mem": bit3(0x224994),"good": 1, "addr": 0x224994, "bit": 3},88: { "levelId": 6, "mem": bit4(0x224994),"good": 1, "addr": 0x224994, "bit": 4},89: { "levelId": 6, "mem": bit5(0x224994),"good": 1, "addr": 0x224994, "bit": 5},90: { "levelId": 6, "mem": bit6(0x224994),"good": 1, "addr": 0x224994, "bit": 6},91: { "levelId": 6, "mem": bit7(0x224994),"good": 1, "addr": 0x224994, "bit": 7},92: { "levelId": 6, "mem": bit0(0x224995),"good": 1, "addr": 0x224995, "bit": 0},93: { "levelId": 6, "mem": bit1(0x224995),"good": 1, "addr": 0x224995, "bit": 1},94: { "levelId": 6, "mem": bit2(0x224995),"good": 1, "addr": 0x224995, "bit": 2},95: { "levelId": 6, "mem": bit3(0x224995),"good": 1, "addr": 0x224995, "bit": 3},96: { "levelId": 6, "mem": bit4(0x224995),"good": 1, "addr": 0x224995, "bit": 4},97: { "levelId": 6, "mem": bit5(0x224995),"good": 1, "addr": 0x224995, "bit": 5},98: { "levelId": 6, "mem": bit6(0x224995),"good": 1, "addr": 0x224995, "bit": 6},99: { "levelId": 6, "mem": bit7(0x224995),"good": 1, "addr": 0x224995, "bit": 7},100: { "levelId": 6, "mem": bit0(0x224996),"good": 1, "addr": 0x224996, "bit": 0},101: { "levelId": 6, "mem": bit1(0x224996),"good": 1, "addr": 0x224996, "bit": 1},102: { "levelId": 6, "mem": bit2(0x224996),"good": 1, "addr": 0x224996, "bit": 2},103: { "levelId": 6, "mem": bit3(0x224996),"good": 1, "addr": 0x224996, "bit": 3},104: { "levelId": 6, "mem": bit4(0x224996),"good": 1, "addr": 0x224996, "bit": 4},105: { "levelId": 6, "mem": bit5(0x224996),"good": 1, "addr": 0x224996, "bit": 5},106: { "levelId": 6, "mem": bit6(0x224996),"good": 1, "addr": 0x224996, "bit": 6},107: { "levelId": 6, "mem": bit7(0x224996),"good": 1, "addr": 0x224996, "bit": 7},108: { "levelId": 6, "mem": bit0(0x224997),"good": 1, "addr": 0x224997, "bit": 0},109: { "levelId": 6, "mem": bit1(0x224997),"good": 1, "addr": 0x224997, "bit": 1},110: { "levelId": 6, "mem": bit2(0x224997),"good": 1, "addr": 0x224997, "bit": 2},111: { "levelId": 6, "mem": bit3(0x224997),"good": 1, "addr": 0x224997, "bit": 3},112: { "levelId": 6, "mem": bit4(0x224997),"good": 1, "addr": 0x224997, "bit": 4},113: { "levelId": 6, "mem": bit5(0x224997),"good": 1, "addr": 0x224997, "bit": 5},114: { "levelId": 6, "mem": bit6(0x224997),"good": 1, "addr": 0x224997, "bit": 6},115: { "levelId": 6, "mem": bit7(0x224997),"good": 1, "addr": 0x224997, "bit": 7},116: { "levelId": 6, "mem": bit0(0x224998),"good": 1, "addr": 0x224998, "bit": 0},117: { "levelId": 6, "mem": bit1(0x224998),"good": 1, "addr": 0x224998, "bit": 1},118: { "levelId": 6, "mem": bit2(0x224998),"good": 1, "addr": 0x224998, "bit": 2},119: { "levelId": 6, "mem": bit3(0x224998),"good": 1, "addr": 0x224998, "bit": 3},120: { "levelId": 6, "mem": bit4(0x224998),"good": 1, "addr": 0x224998, "bit": 4},121: { "levelId": 6, "mem": bit5(0x224998),"good": 1, "addr": 0x224998, "bit": 5},122: { "levelId": 6, "mem": bit6(0x224998),"good": 1, "addr": 0x224998, "bit": 6},123: { "levelId": 6, "mem": bit0(0x224999),"good": 1, "addr": 0x224999, "bit": 0},124: { "levelId": 6, "mem": bit1(0x224999),"good": 1, "addr": 0x224999, "bit": 1},125: { "levelId": 6, "mem": bit2(0x224999),"good": 1, "addr": 0x224999, "bit": 2},126: { "levelId": 6, "mem": bit3(0x224999),"good": 1, "addr": 0x224999, "bit": 3},127: { "levelId": 6, "mem": bit4(0x224999),"good": 1, "addr": 0x224999, "bit": 4},128: { "levelId": 6, "mem": bit5(0x224999),"good": 1, "addr": 0x224999, "bit": 5},129: { "levelId": 6, "mem": bit6(0x224999),"good": 1, "addr": 0x224999, "bit": 6},130: { "levelId": 6, "mem": bit7(0x224999),"good": 1, "addr": 0x224999, "bit": 7},131: { "levelId": 6, "mem": bit0(0x22499a),"good": 1, "addr": 0x22499a, "bit": 0},132: { "levelId": 6, "mem": bit1(0x22499a),"good": 1, "addr": 0x22499a, "bit": 1},133: { "levelId": 6, "mem": bit2(0x22499a),"good": 1, "addr": 0x22499a, "bit": 2},134: { "levelId": 6, "mem": bit3(0x22499a),"good": 1, "addr": 0x22499a, "bit": 3},135: { "levelId": 6, "mem": bit4(0x22499a),"good": 1, "addr": 0x22499a, "bit": 4},136: { "levelId": 6, "mem": bit5(0x22499a),"good": 1, "addr": 0x22499a, "bit": 5},137: { "levelId": 1, "mem": bit3(0x224a36),"good": 1, "addr": 0x224a36, "bit": 3},138: { "levelId": 1, "mem": bit4(0x224a36),"good": 1, "addr": 0x224a36, "bit": 4},139: { "levelId": 1, "mem": bit5(0x224a36),"good": 1, "addr": 0x224a36, "bit": 5},140: { "levelId": 1, "mem": bit6(0x224a36),"good": 1, "addr": 0x224a36, "bit": 6},141: { "levelId": 1, "mem": bit7(0x224a36),"good": 1, "addr": 0x224a36, "bit": 7},142: { "levelId": 6, "mem": bit7(0x224998),"good": 1, "addr": 0x224998, "bit": 7},143: { "levelId": 8, "mem": bit3(0x22499b),"good": 1, "addr": 0x22499b, "bit": 3},144: { "levelId": 8, "mem": bit4(0x22499b),"good": 1, "addr": 0x22499b, "bit": 4},145: { "levelId": 8, "mem": bit5(0x22499b),"good": 1, "addr": 0x22499b, "bit": 5},146: { "levelId": 8, "mem": bit5(0x22499c),"good": 1, "addr": 0x22499c, "bit": 5},147: { "levelId": 8, "mem": bit6(0x22499c),"good": 1, "addr": 0x22499c, "bit": 6},148: { "levelId": 8, "mem": bit7(0x22499c),"good": 1, "addr": 0x22499c, "bit": 7},149: { "levelId": 8, "mem": bit0(0x22499d),"good": 1, "addr": 0x22499d, "bit": 0},150: { "levelId": 8, "mem": bit1(0x22499d),"good": 1, "addr": 0x22499d, "bit": 1},151: { "levelId": 8, "mem": bit2(0x22499d),"good": 1, "addr": 0x22499d, "bit": 2},152: { "levelId": 8, "mem": bit3(0x22499d),"good": 1, "addr": 0x22499d, "bit": 3},153: { "levelId": 8, "mem": bit4(0x22499d),"good": 1, "addr": 0x22499d, "bit": 4},154: { "levelId": 8, "mem": bit5(0x22499d),"good": 1, "addr": 0x22499d, "bit": 5},155: { "levelId": 8, "mem": bit6(0x22499d),"good": 1, "addr": 0x22499d, "bit": 6},156: { "levelId": 8, "mem": bit7(0x22499d),"good": 1, "addr": 0x22499d, "bit": 7},157: { "levelId": 8, "mem": bit0(0x22499e),"good": 1, "addr": 0x22499e, "bit": 0},158: { "levelId": 8, "mem": bit1(0x22499e),"good": 1, "addr": 0x22499e, "bit": 1},159: { "levelId": 8, "mem": bit6(0x22499a),"good": 1, "addr": 0x22499a, "bit": 6},160: { "levelId": 8, "mem": bit7(0x22499a),"good": 1, "addr": 0x22499a, "bit": 7},161: { "levelId": 8, "mem": bit0(0x22499b),"good": 1, "addr": 0x22499b, "bit": 0},162: { "levelId": 8, "mem": bit1(0x22499b),"good": 1, "addr": 0x22499b, "bit": 1},163: { "levelId": 8, "mem": bit2(0x22499b),"good": 1, "addr": 0x22499b, "bit": 2},164: { "levelId": 8, "mem": bit6(0x22499b),"good": 1, "addr": 0x22499b, "bit": 6},165: { "levelId": 8, "mem": bit7(0x22499b),"good": 1, "addr": 0x22499b, "bit": 7},166: { "levelId": 8, "mem": bit0(0x22499c),"good": 1, "addr": 0x22499c, "bit": 0},167: { "levelId": 8, "mem": bit1(0x22499c),"good": 1, "addr": 0x22499c, "bit": 1},168: { "levelId": 8, "mem": bit2(0x22499c),"good": 1, "addr": 0x22499c, "bit": 2},169: { "levelId": 8, "mem": bit3(0x22499c),"good": 1, "addr": 0x22499c, "bit": 3},170: { "levelId": 8, "mem": bit4(0x22499c),"good": 1, "addr": 0x22499c, "bit": 4},171: { "levelId": 8, "mem": bit2(0x22499e),"good": 1, "addr": 0x22499e, "bit": 2},172: { "levelId": 8, "mem": bit3(0x22499e),"good": 1, "addr": 0x22499e, "bit": 3},173: { "levelId": 8, "mem": bit4(0x22499e),"good": 1, "addr": 0x22499e, "bit": 4},174: { "levelId": 8, "mem": bit5(0x22499e),"good": 1, "addr": 0x22499e, "bit": 5},175: { "levelId": 8, "mem": bit6(0x22499e),"good": 1, "addr": 0x22499e, "bit": 6},176: { "levelId": 8, "mem": bit7(0x22499e),"good": 1, "addr": 0x22499e, "bit": 7},177: { "levelId": 8, "mem": bit0(0x22499f),"good": 1, "addr": 0x22499f, "bit": 0},178: { "levelId": 8, "mem": bit1(0x22499f),"good": 1, "addr": 0x22499f, "bit": 1},179: { "levelId": 8, "mem": bit2(0x22499f),"good": 1, "addr": 0x22499f, "bit": 2},180: { "levelId": 8, "mem": bit3(0x22499f),"good": 1, "addr": 0x22499f, "bit": 3},181: { "levelId": 8, "mem": bit4(0x22499f),"good": 1, "addr": 0x22499f, "bit": 4},182: { "levelId": 8, "mem": bit5(0x22499f),"good": 1, "addr": 0x22499f, "bit": 5},183: { "levelId": 8, "mem": bit6(0x22499f),"good": 1, "addr": 0x22499f, "bit": 6},184: { "levelId": 8, "mem": bit7(0x22499f),"good": 1, "addr": 0x22499f, "bit": 7},185: { "levelId": 8, "mem": bit0(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 0},186: { "levelId": 8, "mem": bit1(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 1},187: { "levelId": 8, "mem": bit2(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 2},188: { "levelId": 8, "mem": bit3(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 3},189: { "levelId": 8, "mem": bit4(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 4},190: { "levelId": 8, "mem": bit5(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 5},191: { "levelId": 8, "mem": bit6(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 6},192: { "levelId": 8, "mem": bit7(0x2249a0),"good": 1, "addr": 0x2249a0, "bit": 7},193: { "levelId": 10, "mem": bit0(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 0},194: { "levelId": 10, "mem": bit1(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 1},195: { "levelId": 10, "mem": bit2(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 2},196: { "levelId": 10, "mem": bit3(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 3},197: { "levelId": 10, "mem": bit4(0x2249a1),"good": 1, "addr": 0x2249a1, "bit": 4},198: { "levelId": 10, "mem": bit2(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 2},199: { "levelId": 10, "mem": bit3(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 3},200: { "levelId": 10, "mem": bit4(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 4},201: { "levelId": 10, "mem": bit5(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 5},202: { "levelId": 10, "mem": bit6(0x2249a2),"good": 1, "addr": 0x2249a2, "bit": 6},203: { "levelId": 10, "mem": bit1(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 1},204: { "levelId": 10, "mem": bit5(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 5},205: { "levelId": 10, "mem": bit6(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 6},206: { "levelId": 10, "mem": bit7(0x2249a3),"good": 1, "addr": 0x2249a3, "bit": 7},207: { "levelId": 10, "mem": bit0(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 0},208: { "levelId": 10, "mem": bit3(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 3},209: { "levelId": 10, "mem": bit5(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 5},210: { "levelId": 10, "mem": bit6(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 6},211: { "levelId": 10, "mem": bit7(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 7},212: { "levelId": 10, "mem": bit0(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 0},213: { "levelId": 10, "mem": bit1(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 1},214: { "levelId": 10, "mem": bit2(0x2249a5),"good": 1, "addr": 0x2249a5, "bit": 2},215: { "levelId": 10, "mem": bit4(0x2249a4),"good": 1, "addr": 0x2249a4, "bit": 4},216: { "levelId": 11, "mem": bit6(0x2249e5),"good": 1, "addr": 0x2249e5, "bit": 6},217: { "levelId": 11, "mem": bit7(0x2249e5),"good": 1, "addr": 0x2249e5, "bit": 7},218: { "levelId": 11, "mem": bit0(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 0},219: { "levelId": 11, "mem": bit1(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 1},220: { "levelId": 11, "mem": bit2(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 2},221: { "levelId": 11, "mem": bit3(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 3},222: { "levelId": 11, "mem": bit4(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 4},223: { "levelId": 11, "mem": bit5(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 5},224: { "levelId": 11, "mem": bit6(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 6},225: { "levelId": 11, "mem": bit7(0x2249e6),"good": 1, "addr": 0x2249e6, "bit": 7},226: { "levelId": 11, "mem": bit0(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 0},227: { "levelId": 11, "mem": bit1(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 1},228: { "levelId": 11, "mem": bit2(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 2},229: { "levelId": 11, "mem": bit3(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 3},230: { "levelId": 11, "mem": bit4(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 4},231: { "levelId": 11, "mem": bit5(0x2249e7),"good": 1, "addr": 0x2249e7, "bit": 5},232: { "levelId": 11, "mem": bit6(0x2249e7),"good": 1, "addr": 0x2249e7, "bit":